<commit_message>
LIsää tilaajan laadunvalvojalle asiatarkastus-oikeus
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26812"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27211"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -17,6 +17,9 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="144">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -454,6 +457,9 @@
   </si>
   <si>
     <t>R*,W*,päätös</t>
+  </si>
+  <si>
+    <t>asiatarkastus</t>
   </si>
 </sst>
 </file>
@@ -1130,11 +1136,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
       <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D32" sqref="D32"/>
+      <selection pane="bottomRight" activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2643,7 +2649,9 @@
       <c r="F30" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="G30" s="21"/>
+      <c r="G30" s="21" t="s">
+        <v>143</v>
+      </c>
       <c r="H30" s="21" t="s">
         <v>134</v>
       </c>

</xml_diff>

<commit_message>
Lisää tilaajan laadunvalvojalle myös R*-oikeudet päällystysilmoituksiin, jotta voi tehdä asiatarkastuksen
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8780" yWindow="460" windowWidth="26580" windowHeight="27040" tabRatio="500"/>
+    <workbookView xWindow="8780" yWindow="460" windowWidth="37420" windowHeight="27040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -459,7 +459,7 @@
     <t>R*,W*,päätös</t>
   </si>
   <si>
-    <t>asiatarkastus</t>
+    <t>R*,asiatarkastus</t>
   </si>
 </sst>
 </file>
@@ -1137,7 +1137,7 @@
   <dimension ref="A1:X61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
       <selection pane="bottomRight" activeCell="G30" sqref="G30"/>

</xml_diff>

<commit_message>
Lisää roolit-exceliin uusi välitavoitteet-osio hallintaan
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="144">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -655,7 +655,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -715,6 +715,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1134,13 +1135,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X61"/>
+  <dimension ref="A1:X62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="G30" sqref="G30"/>
+      <selection pane="bottomRight" activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1175,38 +1176,38 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="40" t="s">
         <v>131</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
     </row>
     <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
     </row>
     <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
@@ -1227,30 +1228,30 @@
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="J5" s="38" t="s">
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="J5" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="37"/>
-      <c r="L5" s="37"/>
-      <c r="M5" s="37"/>
-      <c r="N5" s="37"/>
-      <c r="P5" s="38" t="s">
+      <c r="K5" s="38"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="38"/>
+      <c r="N5" s="38"/>
+      <c r="P5" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="Q5" s="37"/>
-      <c r="R5" s="37"/>
-      <c r="S5" s="37"/>
-      <c r="T5" s="37"/>
-      <c r="U5" s="37"/>
-      <c r="V5" s="37"/>
+      <c r="Q5" s="38"/>
+      <c r="R5" s="38"/>
+      <c r="S5" s="38"/>
+      <c r="T5" s="38"/>
+      <c r="U5" s="38"/>
+      <c r="V5" s="38"/>
       <c r="X5" s="5" t="s">
         <v>14</v>
       </c>
@@ -3922,7 +3923,7 @@
         <v>17</v>
       </c>
       <c r="W51" s="21"/>
-      <c r="X51" s="36" t="s">
+      <c r="X51" s="37" t="s">
         <v>60</v>
       </c>
     </row>
@@ -3992,7 +3993,7 @@
         <v>17</v>
       </c>
       <c r="W52" s="21"/>
-      <c r="X52" s="37"/>
+      <c r="X52" s="38"/>
     </row>
     <row r="53" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="26" t="s">
@@ -4230,12 +4231,12 @@
       <c r="V58" s="17"/>
       <c r="W58" s="17"/>
     </row>
-    <row r="59" spans="1:24" s="33" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:24" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="16" t="s">
         <v>63</v>
       </c>
       <c r="B59" s="16" t="s">
-        <v>129</v>
+        <v>33</v>
       </c>
       <c r="C59" s="17"/>
       <c r="D59" s="21" t="s">
@@ -4261,79 +4262,110 @@
       <c r="V59" s="17"/>
       <c r="W59" s="17"/>
     </row>
-    <row r="60" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:24" s="33" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="16" t="s">
-        <v>110</v>
+        <v>63</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="C60" s="20"/>
+        <v>129</v>
+      </c>
+      <c r="C60" s="17"/>
       <c r="D60" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="E60" s="20"/>
-      <c r="F60" s="20"/>
-      <c r="G60" s="20"/>
-      <c r="H60" s="20"/>
-      <c r="I60" s="20"/>
-      <c r="J60" s="20"/>
-      <c r="K60" s="20"/>
-      <c r="L60" s="20"/>
-      <c r="M60" s="20"/>
-      <c r="N60" s="20"/>
-      <c r="O60" s="20"/>
-      <c r="P60" s="20"/>
-      <c r="Q60" s="20"/>
-      <c r="R60" s="20"/>
-      <c r="S60" s="20"/>
-      <c r="T60" s="20"/>
-      <c r="U60" s="20"/>
-      <c r="V60" s="20"/>
-      <c r="W60" s="20"/>
+      <c r="E60" s="17"/>
+      <c r="F60" s="17"/>
+      <c r="G60" s="17"/>
+      <c r="H60" s="17"/>
+      <c r="I60" s="17"/>
+      <c r="J60" s="17"/>
+      <c r="K60" s="17"/>
+      <c r="L60" s="17"/>
+      <c r="M60" s="17"/>
+      <c r="N60" s="17"/>
+      <c r="O60" s="17"/>
+      <c r="P60" s="17"/>
+      <c r="Q60" s="17"/>
+      <c r="R60" s="17"/>
+      <c r="S60" s="17"/>
+      <c r="T60" s="17"/>
+      <c r="U60" s="17"/>
+      <c r="V60" s="17"/>
+      <c r="W60" s="17"/>
     </row>
     <row r="61" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="16" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="B61" s="16" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="C61" s="20"/>
       <c r="D61" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="E61" s="20"/>
+      <c r="F61" s="20"/>
+      <c r="G61" s="20"/>
+      <c r="H61" s="20"/>
+      <c r="I61" s="20"/>
+      <c r="J61" s="20"/>
+      <c r="K61" s="20"/>
+      <c r="L61" s="20"/>
+      <c r="M61" s="20"/>
+      <c r="N61" s="20"/>
+      <c r="O61" s="20"/>
+      <c r="P61" s="20"/>
+      <c r="Q61" s="20"/>
+      <c r="R61" s="20"/>
+      <c r="S61" s="20"/>
+      <c r="T61" s="20"/>
+      <c r="U61" s="20"/>
+      <c r="V61" s="20"/>
+      <c r="W61" s="20"/>
+    </row>
+    <row r="62" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A62" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B62" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="C62" s="20"/>
+      <c r="D62" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="E61" s="30" t="s">
+      <c r="E62" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="F61" s="30"/>
-      <c r="G61" s="30" t="s">
+      <c r="F62" s="30"/>
+      <c r="G62" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="H61" s="30"/>
-      <c r="I61" s="30"/>
-      <c r="J61" s="30" t="s">
+      <c r="H62" s="30"/>
+      <c r="I62" s="30"/>
+      <c r="J62" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="K61" s="30" t="s">
+      <c r="K62" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="L61" s="30" t="s">
+      <c r="L62" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="M61" s="30" t="s">
+      <c r="M62" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="N61" s="30"/>
-      <c r="O61" s="30"/>
-      <c r="P61" s="30"/>
-      <c r="Q61" s="30"/>
-      <c r="R61" s="30"/>
-      <c r="S61" s="30"/>
-      <c r="T61" s="30"/>
-      <c r="U61" s="30"/>
-      <c r="V61" s="30"/>
-      <c r="W61" s="30"/>
+      <c r="N62" s="30"/>
+      <c r="O62" s="30"/>
+      <c r="P62" s="30"/>
+      <c r="Q62" s="30"/>
+      <c r="R62" s="30"/>
+      <c r="S62" s="30"/>
+      <c r="T62" s="30"/>
+      <c r="U62" s="30"/>
+      <c r="V62" s="30"/>
+      <c r="W62" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Tee järjestelmävastaavan muu oikeuksista *
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27211"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarihan/Desktop/Harja/harja/resources/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8780" yWindow="460" windowWidth="37420" windowHeight="27040" tabRatio="500"/>
+    <workbookView xWindow="2560" yWindow="180" windowWidth="37420" windowHeight="27040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -17,11 +12,11 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -429,9 +424,6 @@
     <t>R*,W*</t>
   </si>
   <si>
-    <t>R*,W*,sido</t>
-  </si>
-  <si>
     <t>R*</t>
   </si>
   <si>
@@ -456,10 +448,13 @@
     <t>R*,W,sido</t>
   </si>
   <si>
-    <t>R*,W*,päätös</t>
-  </si>
-  <si>
     <t>R*,asiatarkastus</t>
+  </si>
+  <si>
+    <t>R*,W*,päätös*</t>
+  </si>
+  <si>
+    <t>R*,W*,sido*</t>
   </si>
 </sst>
 </file>
@@ -1138,13 +1133,13 @@
   <dimension ref="A1:X62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D60" sqref="D60"/>
+      <selection pane="bottomRight" activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.5" bestFit="1" customWidth="1"/>
@@ -1171,7 +1166,7 @@
     <col min="24" max="24" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:24" ht="15.75" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1191,7 +1186,7 @@
       <c r="M1" s="38"/>
       <c r="N1" s="38"/>
     </row>
-    <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:24" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="40" t="s">
@@ -1209,7 +1204,7 @@
       <c r="M2" s="38"/>
       <c r="N2" s="38"/>
     </row>
-    <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:24" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -1224,10 +1219,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:24" ht="15.75" customHeight="1">
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:24" ht="15.75" customHeight="1">
       <c r="C5" s="39" t="s">
         <v>6</v>
       </c>
@@ -1256,7 +1251,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:24" ht="15.75" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
@@ -1325,7 +1320,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:24" ht="15.75" customHeight="1">
       <c r="A7" s="16" t="s">
         <v>15</v>
       </c>
@@ -1337,52 +1332,52 @@
         <v>132</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I7" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J7" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="K7" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="K7" s="17" t="s">
-        <v>137</v>
-      </c>
       <c r="L7" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M7" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N7" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O7" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P7" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q7" s="17" t="s">
         <v>114</v>
       </c>
       <c r="R7" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="S7" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T7" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U7" s="17" t="s">
         <v>17</v>
@@ -1393,7 +1388,7 @@
       <c r="W7" s="17"/>
       <c r="X7" s="10"/>
     </row>
-    <row r="8" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:24" ht="15.75" customHeight="1">
       <c r="A8" s="16" t="s">
         <v>15</v>
       </c>
@@ -1405,28 +1400,28 @@
         <v>132</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G8" s="21"/>
       <c r="H8" s="21"/>
       <c r="I8" s="21"/>
       <c r="J8" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="K8" s="17" t="s">
         <v>136</v>
-      </c>
-      <c r="K8" s="17" t="s">
-        <v>137</v>
       </c>
       <c r="L8" s="21"/>
       <c r="M8" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N8" s="21"/>
       <c r="O8" s="17"/>
       <c r="P8" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q8" s="21" t="s">
         <v>17</v>
@@ -1434,7 +1429,7 @@
       <c r="R8" s="17"/>
       <c r="S8" s="17"/>
       <c r="T8" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U8" s="17" t="s">
         <v>19</v>
@@ -1447,7 +1442,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:24" ht="15.75" customHeight="1">
       <c r="A9" s="16" t="s">
         <v>15</v>
       </c>
@@ -1459,28 +1454,28 @@
         <v>132</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G9" s="21"/>
       <c r="H9" s="21"/>
       <c r="I9" s="21"/>
       <c r="J9" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="K9" s="17" t="s">
         <v>136</v>
-      </c>
-      <c r="K9" s="17" t="s">
-        <v>137</v>
       </c>
       <c r="L9" s="21"/>
       <c r="M9" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N9" s="21"/>
       <c r="O9" s="17"/>
       <c r="P9" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q9" s="21" t="s">
         <v>17</v>
@@ -1488,14 +1483,14 @@
       <c r="R9" s="17"/>
       <c r="S9" s="17"/>
       <c r="T9" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U9" s="17"/>
       <c r="V9" s="17"/>
       <c r="W9" s="17"/>
       <c r="X9" s="10"/>
     </row>
-    <row r="10" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:24" ht="15.75" customHeight="1">
       <c r="A10" s="16" t="s">
         <v>15</v>
       </c>
@@ -1507,28 +1502,28 @@
         <v>132</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G10" s="21"/>
       <c r="H10" s="21"/>
       <c r="I10" s="21"/>
       <c r="J10" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="K10" s="17" t="s">
         <v>136</v>
-      </c>
-      <c r="K10" s="17" t="s">
-        <v>137</v>
       </c>
       <c r="L10" s="21"/>
       <c r="M10" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N10" s="21"/>
       <c r="O10" s="17"/>
       <c r="P10" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q10" s="21" t="s">
         <v>17</v>
@@ -1536,14 +1531,14 @@
       <c r="R10" s="17"/>
       <c r="S10" s="17"/>
       <c r="T10" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U10" s="17"/>
       <c r="V10" s="17"/>
       <c r="W10" s="17"/>
       <c r="X10" s="10"/>
     </row>
-    <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:24" ht="15.75" customHeight="1">
       <c r="A11" s="16" t="s">
         <v>15</v>
       </c>
@@ -1555,57 +1550,57 @@
         <v>132</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H11" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I11" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J11" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="K11" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="K11" s="17" t="s">
-        <v>137</v>
-      </c>
       <c r="L11" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M11" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N11" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O11" s="17"/>
       <c r="P11" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q11" s="17" t="s">
         <v>17</v>
       </c>
       <c r="R11" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="S11" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T11" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U11" s="17"/>
       <c r="V11" s="17"/>
       <c r="W11" s="17"/>
       <c r="X11" s="10"/>
     </row>
-    <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:24" ht="15.75" customHeight="1">
       <c r="A12" s="16" t="s">
         <v>15</v>
       </c>
@@ -1617,57 +1612,57 @@
         <v>132</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I12" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J12" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="K12" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="K12" s="17" t="s">
-        <v>137</v>
-      </c>
       <c r="L12" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M12" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N12" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O12" s="17"/>
       <c r="P12" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q12" s="17" t="s">
         <v>17</v>
       </c>
       <c r="R12" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="S12" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T12" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U12" s="17"/>
       <c r="V12" s="17"/>
       <c r="W12" s="17"/>
       <c r="X12" s="10"/>
     </row>
-    <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:24" ht="15.75" customHeight="1">
       <c r="A13" s="16" t="s">
         <v>15</v>
       </c>
@@ -1679,28 +1674,28 @@
         <v>132</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G13" s="21"/>
       <c r="H13" s="21"/>
       <c r="I13" s="21"/>
       <c r="J13" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K13" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L13" s="17"/>
       <c r="M13" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N13" s="21"/>
       <c r="O13" s="17"/>
       <c r="P13" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q13" s="17" t="s">
         <v>114</v>
@@ -1708,14 +1703,14 @@
       <c r="R13" s="21"/>
       <c r="S13" s="17"/>
       <c r="T13" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U13" s="17"/>
       <c r="V13" s="17"/>
       <c r="W13" s="17"/>
       <c r="X13" s="10"/>
     </row>
-    <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:24" ht="15.75" customHeight="1">
       <c r="A14" s="16" t="s">
         <v>15</v>
       </c>
@@ -1727,28 +1722,28 @@
         <v>132</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
       <c r="I14" s="21"/>
       <c r="J14" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K14" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L14" s="17"/>
       <c r="M14" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N14" s="21"/>
       <c r="O14" s="17"/>
       <c r="P14" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q14" s="17" t="s">
         <v>114</v>
@@ -1756,14 +1751,14 @@
       <c r="R14" s="21"/>
       <c r="S14" s="17"/>
       <c r="T14" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U14" s="17"/>
       <c r="V14" s="17"/>
       <c r="W14" s="17"/>
       <c r="X14" s="10"/>
     </row>
-    <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:24" ht="15.75" customHeight="1">
       <c r="A15" s="16" t="s">
         <v>15</v>
       </c>
@@ -1775,28 +1770,28 @@
         <v>132</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G15" s="21"/>
       <c r="H15" s="21"/>
       <c r="I15" s="21"/>
       <c r="J15" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K15" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L15" s="17"/>
       <c r="M15" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N15" s="21"/>
       <c r="O15" s="17"/>
       <c r="P15" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q15" s="17" t="s">
         <v>114</v>
@@ -1804,14 +1799,14 @@
       <c r="R15" s="21"/>
       <c r="S15" s="17"/>
       <c r="T15" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U15" s="17"/>
       <c r="V15" s="17"/>
       <c r="W15" s="17"/>
       <c r="X15" s="10"/>
     </row>
-    <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:24" ht="15.75" customHeight="1">
       <c r="A16" s="16" t="s">
         <v>15</v>
       </c>
@@ -1823,57 +1818,57 @@
         <v>132</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I16" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J16" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K16" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L16" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M16" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N16" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O16" s="17"/>
       <c r="P16" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q16" s="17" t="s">
         <v>114</v>
       </c>
       <c r="R16" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="S16" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T16" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U16" s="17"/>
       <c r="V16" s="17"/>
       <c r="W16" s="17"/>
       <c r="X16" s="10"/>
     </row>
-    <row r="17" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:24" ht="15.75" customHeight="1">
       <c r="A17" s="16" t="s">
         <v>15</v>
       </c>
@@ -1885,57 +1880,57 @@
         <v>132</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I17" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J17" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K17" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L17" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M17" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N17" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O17" s="17"/>
       <c r="P17" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q17" s="17" t="s">
         <v>114</v>
       </c>
       <c r="R17" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="S17" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T17" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U17" s="17"/>
       <c r="V17" s="17"/>
       <c r="W17" s="17"/>
       <c r="X17" s="10"/>
     </row>
-    <row r="18" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:24" ht="15.75" customHeight="1">
       <c r="A18" s="16" t="s">
         <v>15</v>
       </c>
@@ -1947,28 +1942,28 @@
         <v>132</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G18" s="21"/>
       <c r="H18" s="21"/>
       <c r="I18" s="21"/>
       <c r="J18" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="K18" s="17" t="s">
         <v>136</v>
-      </c>
-      <c r="K18" s="17" t="s">
-        <v>137</v>
       </c>
       <c r="L18" s="17"/>
       <c r="M18" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N18" s="21"/>
       <c r="O18" s="17"/>
       <c r="P18" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q18" s="17" t="s">
         <v>17</v>
@@ -1976,14 +1971,14 @@
       <c r="R18" s="21"/>
       <c r="S18" s="21"/>
       <c r="T18" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U18" s="17"/>
       <c r="V18" s="17"/>
       <c r="W18" s="17"/>
       <c r="X18" s="10"/>
     </row>
-    <row r="19" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:24" ht="15.75" customHeight="1">
       <c r="A19" s="16" t="s">
         <v>15</v>
       </c>
@@ -1995,57 +1990,57 @@
         <v>132</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F19" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H19" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I19" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J19" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K19" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L19" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M19" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N19" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O19" s="17"/>
       <c r="P19" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q19" s="17" t="s">
         <v>114</v>
       </c>
       <c r="R19" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="S19" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T19" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U19" s="17"/>
       <c r="V19" s="17"/>
       <c r="W19" s="17"/>
       <c r="X19" s="10"/>
     </row>
-    <row r="20" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:24" ht="15.75" customHeight="1">
       <c r="A20" s="16" t="s">
         <v>15</v>
       </c>
@@ -2057,52 +2052,52 @@
         <v>132</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G20" s="17" t="s">
         <v>132</v>
       </c>
       <c r="H20" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I20" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J20" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="K20" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="K20" s="17" t="s">
-        <v>137</v>
-      </c>
       <c r="L20" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M20" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N20" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O20" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P20" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q20" s="17" t="s">
         <v>114</v>
       </c>
       <c r="R20" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="S20" s="21" t="s">
         <v>114</v>
       </c>
       <c r="T20" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U20" s="17"/>
       <c r="V20" s="21" t="s">
@@ -2111,7 +2106,7 @@
       <c r="W20" s="17"/>
       <c r="X20" s="10"/>
     </row>
-    <row r="21" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:24" ht="15.75" customHeight="1">
       <c r="A21" s="26" t="s">
         <v>15</v>
       </c>
@@ -2123,52 +2118,52 @@
         <v>132</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F21" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G21" s="17" t="s">
         <v>132</v>
       </c>
       <c r="H21" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I21" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J21" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="K21" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="K21" s="17" t="s">
-        <v>137</v>
-      </c>
       <c r="L21" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M21" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N21" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O21" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P21" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q21" s="21" t="s">
         <v>114</v>
       </c>
       <c r="R21" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="S21" s="21" t="s">
         <v>114</v>
       </c>
       <c r="T21" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U21" s="21" t="s">
         <v>17</v>
@@ -2179,7 +2174,7 @@
       <c r="W21" s="21"/>
       <c r="X21" s="10"/>
     </row>
-    <row r="22" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:24" ht="15.75" customHeight="1">
       <c r="A22" s="26" t="s">
         <v>15</v>
       </c>
@@ -2191,50 +2186,50 @@
         <v>132</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F22" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G22" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H22" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I22" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J22" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K22" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L22" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M22" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N22" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O22" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P22" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q22" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R22" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="S22" s="21"/>
       <c r="T22" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U22" s="21"/>
       <c r="V22" s="21" t="s">
@@ -2245,7 +2240,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="23" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:24" ht="15.75" customHeight="1">
       <c r="A23" s="26" t="s">
         <v>15</v>
       </c>
@@ -2257,52 +2252,52 @@
         <v>132</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F23" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G23" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H23" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I23" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J23" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="K23" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="K23" s="21" t="s">
-        <v>137</v>
-      </c>
       <c r="L23" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M23" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N23" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O23" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P23" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q23" s="21" t="s">
         <v>114</v>
       </c>
       <c r="R23" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="S23" s="21" t="s">
         <v>114</v>
       </c>
       <c r="T23" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U23" s="21"/>
       <c r="V23" s="21" t="s">
@@ -2311,7 +2306,7 @@
       <c r="W23" s="21"/>
       <c r="X23" s="10"/>
     </row>
-    <row r="24" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:24" ht="15.75" customHeight="1">
       <c r="A24" s="26" t="s">
         <v>15</v>
       </c>
@@ -2323,57 +2318,57 @@
         <v>132</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F24" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G24" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H24" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I24" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J24" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="K24" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="K24" s="21" t="s">
-        <v>137</v>
-      </c>
       <c r="L24" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M24" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N24" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O24" s="21"/>
       <c r="P24" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q24" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R24" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="S24" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T24" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U24" s="21"/>
       <c r="V24" s="21"/>
       <c r="W24" s="21"/>
       <c r="X24" s="10"/>
     </row>
-    <row r="25" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:24" ht="15.75" customHeight="1">
       <c r="A25" s="26" t="s">
         <v>15</v>
       </c>
@@ -2385,7 +2380,7 @@
         <v>132</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F25" s="21"/>
       <c r="G25" s="21"/>
@@ -2394,25 +2389,25 @@
         <v>132</v>
       </c>
       <c r="J25" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="K25" s="21" t="s">
         <v>136</v>
-      </c>
-      <c r="K25" s="21" t="s">
-        <v>137</v>
       </c>
       <c r="L25" s="21"/>
       <c r="M25" s="21"/>
       <c r="N25" s="21"/>
       <c r="O25" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="P25" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q25" s="21" t="s">
         <v>114</v>
       </c>
       <c r="R25" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="S25" s="27"/>
       <c r="T25" s="21"/>
@@ -2423,7 +2418,7 @@
       <c r="W25" s="21"/>
       <c r="X25" s="10"/>
     </row>
-    <row r="26" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:24" ht="15.75" customHeight="1">
       <c r="A26" s="26" t="s">
         <v>15</v>
       </c>
@@ -2432,31 +2427,31 @@
       </c>
       <c r="C26" s="21"/>
       <c r="D26" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F26" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G26" s="21"/>
       <c r="H26" s="21"/>
       <c r="I26" s="21"/>
       <c r="J26" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="K26" s="21" t="s">
         <v>136</v>
-      </c>
-      <c r="K26" s="21" t="s">
-        <v>137</v>
       </c>
       <c r="L26" s="21"/>
       <c r="M26" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N26" s="21"/>
       <c r="O26" s="21"/>
       <c r="P26" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q26" s="21" t="s">
         <v>17</v>
@@ -2469,7 +2464,7 @@
       <c r="W26" s="21"/>
       <c r="X26" s="10"/>
     </row>
-    <row r="27" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:24" ht="15.75" customHeight="1">
       <c r="A27" s="26" t="s">
         <v>15</v>
       </c>
@@ -2481,17 +2476,17 @@
         <v>132</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F27" s="21"/>
       <c r="G27" s="21"/>
       <c r="H27" s="21"/>
       <c r="I27" s="21"/>
       <c r="J27" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="K27" s="21" t="s">
         <v>136</v>
-      </c>
-      <c r="K27" s="21" t="s">
-        <v>137</v>
       </c>
       <c r="L27" s="21"/>
       <c r="M27" s="21"/>
@@ -2509,7 +2504,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:24" ht="15.75" customHeight="1">
       <c r="A28" s="26" t="s">
         <v>15</v>
       </c>
@@ -2521,50 +2516,50 @@
         <v>132</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F28" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G28" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H28" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I28" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J28" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="K28" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="K28" s="21" t="s">
-        <v>137</v>
-      </c>
       <c r="L28" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M28" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N28" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O28" s="21"/>
       <c r="P28" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q28" s="21" t="s">
         <v>114</v>
       </c>
       <c r="R28" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="S28" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T28" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U28" s="21"/>
       <c r="V28" s="21"/>
@@ -2575,7 +2570,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="29" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:24" ht="15.75" customHeight="1">
       <c r="A29" s="26" t="s">
         <v>15</v>
       </c>
@@ -2584,56 +2579,56 @@
       </c>
       <c r="C29" s="21"/>
       <c r="D29" s="21" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F29" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G29" s="21"/>
       <c r="H29" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I29" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J29" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="K29" s="21" t="s">
         <v>136</v>
-      </c>
-      <c r="K29" s="21" t="s">
-        <v>137</v>
       </c>
       <c r="L29" s="21"/>
       <c r="M29" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N29" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O29" s="21"/>
       <c r="P29" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q29" s="21" t="s">
         <v>114</v>
       </c>
       <c r="R29" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="S29" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T29" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U29" s="21"/>
       <c r="V29" s="21"/>
       <c r="W29" s="21"/>
       <c r="X29" s="10"/>
     </row>
-    <row r="30" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:24" ht="15.75" customHeight="1">
       <c r="A30" s="26" t="s">
         <v>15</v>
       </c>
@@ -2645,55 +2640,55 @@
         <v>142</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F30" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G30" s="21" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H30" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I30" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J30" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K30" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L30" s="21"/>
       <c r="M30" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N30" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O30" s="21"/>
       <c r="P30" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q30" s="21" t="s">
         <v>114</v>
       </c>
       <c r="R30" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="S30" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T30" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U30" s="21"/>
       <c r="V30" s="21"/>
       <c r="W30" s="21"/>
       <c r="X30" s="10"/>
     </row>
-    <row r="31" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:24" ht="15.75" customHeight="1">
       <c r="A31" s="26" t="s">
         <v>15</v>
       </c>
@@ -2702,56 +2697,56 @@
       </c>
       <c r="C31" s="21"/>
       <c r="D31" s="21" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F31" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G31" s="21"/>
       <c r="H31" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I31" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J31" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="K31" s="21" t="s">
         <v>136</v>
-      </c>
-      <c r="K31" s="21" t="s">
-        <v>137</v>
       </c>
       <c r="L31" s="21"/>
       <c r="M31" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N31" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O31" s="21"/>
       <c r="P31" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q31" s="21" t="s">
         <v>114</v>
       </c>
       <c r="R31" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="S31" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T31" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U31" s="21"/>
       <c r="V31" s="21"/>
       <c r="W31" s="21"/>
       <c r="X31" s="10"/>
     </row>
-    <row r="32" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:24" ht="15.75" customHeight="1">
       <c r="A32" s="26" t="s">
         <v>15</v>
       </c>
@@ -2763,53 +2758,53 @@
         <v>142</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F32" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G32" s="21"/>
       <c r="H32" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I32" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J32" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="K32" s="21" t="s">
         <v>136</v>
-      </c>
-      <c r="K32" s="21" t="s">
-        <v>137</v>
       </c>
       <c r="L32" s="21"/>
       <c r="M32" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N32" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O32" s="21"/>
       <c r="P32" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q32" s="21" t="s">
         <v>114</v>
       </c>
       <c r="R32" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="S32" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T32" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U32" s="21"/>
       <c r="V32" s="21"/>
       <c r="W32" s="21"/>
       <c r="X32" s="10"/>
     </row>
-    <row r="33" spans="1:24" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:24" s="13" customFormat="1" ht="15.75" customHeight="1">
       <c r="A33" s="26" t="s">
         <v>15</v>
       </c>
@@ -2821,52 +2816,52 @@
         <v>132</v>
       </c>
       <c r="E33" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F33" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G33" s="21" t="s">
         <v>132</v>
       </c>
       <c r="H33" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I33" s="21" t="s">
         <v>132</v>
       </c>
       <c r="J33" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K33" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L33" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M33" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N33" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O33" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P33" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q33" s="21" t="s">
         <v>114</v>
       </c>
       <c r="R33" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="S33" s="21" t="s">
         <v>114</v>
       </c>
       <c r="T33" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U33" s="21" t="s">
         <v>17</v>
@@ -2877,7 +2872,7 @@
       <c r="W33" s="21"/>
       <c r="X33" s="12"/>
     </row>
-    <row r="34" spans="1:24" s="32" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:24" s="32" customFormat="1" ht="15.75" customHeight="1">
       <c r="A34" s="26" t="s">
         <v>43</v>
       </c>
@@ -2886,31 +2881,31 @@
       </c>
       <c r="C34" s="21"/>
       <c r="D34" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F34" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G34" s="21"/>
       <c r="H34" s="21"/>
       <c r="I34" s="21"/>
       <c r="J34" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K34" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L34" s="21"/>
       <c r="M34" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N34" s="21"/>
       <c r="O34" s="21"/>
       <c r="P34" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q34" s="21" t="s">
         <v>17</v>
@@ -2923,7 +2918,7 @@
       <c r="W34" s="21"/>
       <c r="X34" s="31"/>
     </row>
-    <row r="35" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:24" ht="15.75" customHeight="1">
       <c r="A35" s="26" t="s">
         <v>43</v>
       </c>
@@ -2932,13 +2927,13 @@
       </c>
       <c r="C35" s="21"/>
       <c r="D35" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F35" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G35" s="21" t="s">
         <v>19</v>
@@ -2946,19 +2941,19 @@
       <c r="H35" s="21"/>
       <c r="I35" s="21"/>
       <c r="J35" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K35" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L35" s="21"/>
       <c r="M35" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N35" s="21"/>
       <c r="O35" s="21"/>
       <c r="P35" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q35" s="21" t="s">
         <v>17</v>
@@ -2966,14 +2961,14 @@
       <c r="R35" s="21"/>
       <c r="S35" s="21"/>
       <c r="T35" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U35" s="21"/>
       <c r="V35" s="21"/>
       <c r="W35" s="21"/>
       <c r="X35" s="10"/>
     </row>
-    <row r="36" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:24" ht="15.75" customHeight="1">
       <c r="A36" s="26" t="s">
         <v>43</v>
       </c>
@@ -2982,55 +2977,55 @@
       </c>
       <c r="C36" s="21"/>
       <c r="D36" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E36" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F36" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G36" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H36" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I36" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J36" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K36" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L36" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M36" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N36" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O36" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P36" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q36" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R36" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="S36" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T36" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U36" s="21"/>
       <c r="V36" s="21" t="s">
@@ -3039,7 +3034,7 @@
       <c r="W36" s="21"/>
       <c r="X36" s="10"/>
     </row>
-    <row r="37" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:24" ht="15.75" customHeight="1">
       <c r="A37" s="26" t="s">
         <v>43</v>
       </c>
@@ -3048,55 +3043,55 @@
       </c>
       <c r="C37" s="21"/>
       <c r="D37" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E37" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F37" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G37" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H37" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I37" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J37" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K37" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L37" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M37" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N37" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O37" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P37" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q37" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R37" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="S37" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T37" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U37" s="21"/>
       <c r="V37" s="21" t="s">
@@ -3105,7 +3100,7 @@
       <c r="W37" s="21"/>
       <c r="X37" s="10"/>
     </row>
-    <row r="38" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:24" ht="15.75" customHeight="1">
       <c r="A38" s="26" t="s">
         <v>43</v>
       </c>
@@ -3114,55 +3109,55 @@
       </c>
       <c r="C38" s="21"/>
       <c r="D38" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E38" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F38" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G38" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H38" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I38" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J38" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K38" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L38" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M38" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N38" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O38" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P38" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q38" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R38" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="S38" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T38" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U38" s="21"/>
       <c r="V38" s="21" t="s">
@@ -3171,7 +3166,7 @@
       <c r="W38" s="21"/>
       <c r="X38" s="10"/>
     </row>
-    <row r="39" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:24" ht="15.75" customHeight="1">
       <c r="A39" s="26" t="s">
         <v>43</v>
       </c>
@@ -3180,55 +3175,55 @@
       </c>
       <c r="C39" s="21"/>
       <c r="D39" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E39" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F39" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G39" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H39" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I39" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J39" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K39" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L39" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M39" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N39" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O39" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P39" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q39" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R39" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="S39" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T39" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U39" s="21"/>
       <c r="V39" s="21" t="s">
@@ -3237,7 +3232,7 @@
       <c r="W39" s="21"/>
       <c r="X39" s="10"/>
     </row>
-    <row r="40" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:24" ht="15.75" customHeight="1">
       <c r="A40" s="26" t="s">
         <v>43</v>
       </c>
@@ -3246,55 +3241,55 @@
       </c>
       <c r="C40" s="21"/>
       <c r="D40" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E40" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F40" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G40" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H40" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I40" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J40" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K40" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L40" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M40" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N40" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O40" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P40" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q40" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R40" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="S40" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T40" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U40" s="21"/>
       <c r="V40" s="21" t="s">
@@ -3303,7 +3298,7 @@
       <c r="W40" s="21"/>
       <c r="X40" s="10"/>
     </row>
-    <row r="41" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:24" ht="15.75" customHeight="1">
       <c r="A41" s="26" t="s">
         <v>43</v>
       </c>
@@ -3312,49 +3307,49 @@
       </c>
       <c r="C41" s="21"/>
       <c r="D41" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E41" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F41" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G41" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H41" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I41" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J41" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K41" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L41" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M41" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N41" s="21"/>
       <c r="O41" s="21"/>
       <c r="P41" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q41" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R41" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="S41" s="21"/>
       <c r="T41" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U41" s="21"/>
       <c r="V41" s="21" t="s">
@@ -3363,7 +3358,7 @@
       <c r="W41" s="21"/>
       <c r="X41" s="10"/>
     </row>
-    <row r="42" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:24" ht="15.75" customHeight="1">
       <c r="A42" s="26" t="s">
         <v>43</v>
       </c>
@@ -3372,55 +3367,55 @@
       </c>
       <c r="C42" s="21"/>
       <c r="D42" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E42" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F42" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G42" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H42" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I42" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J42" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K42" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L42" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M42" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N42" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O42" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P42" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q42" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R42" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="S42" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T42" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U42" s="21"/>
       <c r="V42" s="21" t="s">
@@ -3429,7 +3424,7 @@
       <c r="W42" s="21"/>
       <c r="X42" s="10"/>
     </row>
-    <row r="43" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:24" ht="15.75" customHeight="1">
       <c r="A43" s="26" t="s">
         <v>43</v>
       </c>
@@ -3438,31 +3433,31 @@
       </c>
       <c r="C43" s="21"/>
       <c r="D43" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E43" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F43" s="21"/>
       <c r="G43" s="21"/>
       <c r="H43" s="21"/>
       <c r="I43" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J43" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K43" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L43" s="21"/>
       <c r="M43" s="21"/>
       <c r="N43" s="21"/>
       <c r="O43" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P43" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q43" s="21" t="s">
         <v>17</v>
@@ -3470,7 +3465,7 @@
       <c r="R43" s="21"/>
       <c r="S43" s="21"/>
       <c r="T43" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U43" s="21"/>
       <c r="V43" s="21" t="s">
@@ -3479,7 +3474,7 @@
       <c r="W43" s="21"/>
       <c r="X43" s="10"/>
     </row>
-    <row r="44" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:24" ht="15.75" customHeight="1">
       <c r="A44" s="26" t="s">
         <v>43</v>
       </c>
@@ -3488,13 +3483,13 @@
       </c>
       <c r="C44" s="21"/>
       <c r="D44" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E44" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F44" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G44" s="21"/>
       <c r="H44" s="21" t="s">
@@ -3502,21 +3497,21 @@
       </c>
       <c r="I44" s="21"/>
       <c r="J44" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K44" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L44" s="21"/>
       <c r="M44" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N44" s="21" t="s">
         <v>19</v>
       </c>
       <c r="O44" s="21"/>
       <c r="P44" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q44" s="21" t="s">
         <v>17</v>
@@ -3529,7 +3524,7 @@
       <c r="W44" s="21"/>
       <c r="X44" s="10"/>
     </row>
-    <row r="45" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:24" ht="15.75" customHeight="1">
       <c r="A45" s="26" t="s">
         <v>43</v>
       </c>
@@ -3538,31 +3533,31 @@
       </c>
       <c r="C45" s="21"/>
       <c r="D45" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E45" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F45" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G45" s="21"/>
       <c r="H45" s="21"/>
       <c r="I45" s="21"/>
       <c r="J45" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K45" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L45" s="21"/>
       <c r="M45" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N45" s="21"/>
       <c r="O45" s="21"/>
       <c r="P45" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q45" s="21" t="s">
         <v>17</v>
@@ -3570,14 +3565,14 @@
       <c r="R45" s="21"/>
       <c r="S45" s="21"/>
       <c r="T45" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U45" s="21"/>
       <c r="V45" s="21"/>
       <c r="W45" s="21"/>
       <c r="X45" s="10"/>
     </row>
-    <row r="46" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:24" ht="15.75" customHeight="1">
       <c r="A46" s="26" t="s">
         <v>43</v>
       </c>
@@ -3586,31 +3581,31 @@
       </c>
       <c r="C46" s="21"/>
       <c r="D46" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E46" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F46" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G46" s="21"/>
       <c r="H46" s="21"/>
       <c r="I46" s="21"/>
       <c r="J46" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K46" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L46" s="21"/>
       <c r="M46" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N46" s="21"/>
       <c r="O46" s="21"/>
       <c r="P46" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q46" s="21" t="s">
         <v>17</v>
@@ -3618,14 +3613,14 @@
       <c r="R46" s="21"/>
       <c r="S46" s="21"/>
       <c r="T46" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U46" s="21"/>
       <c r="V46" s="21"/>
       <c r="W46" s="21"/>
       <c r="X46" s="10"/>
     </row>
-    <row r="47" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:24" ht="15.75" customHeight="1">
       <c r="A47" s="26" t="s">
         <v>43</v>
       </c>
@@ -3634,31 +3629,31 @@
       </c>
       <c r="C47" s="21"/>
       <c r="D47" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E47" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F47" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G47" s="21"/>
       <c r="H47" s="21"/>
       <c r="I47" s="21"/>
       <c r="J47" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K47" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L47" s="21"/>
       <c r="M47" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N47" s="21"/>
       <c r="O47" s="21"/>
       <c r="P47" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q47" s="21" t="s">
         <v>17</v>
@@ -3666,14 +3661,14 @@
       <c r="R47" s="21"/>
       <c r="S47" s="21"/>
       <c r="T47" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U47" s="21"/>
       <c r="V47" s="21"/>
       <c r="W47" s="21"/>
       <c r="X47" s="10"/>
     </row>
-    <row r="48" spans="1:24" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:24" s="29" customFormat="1" ht="15.75" customHeight="1">
       <c r="A48" s="26" t="s">
         <v>43</v>
       </c>
@@ -3682,45 +3677,45 @@
       </c>
       <c r="C48" s="21"/>
       <c r="D48" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E48" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F48" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G48" s="21"/>
       <c r="H48" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I48" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J48" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K48" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L48" s="21"/>
       <c r="M48" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N48" s="21"/>
       <c r="O48" s="21"/>
       <c r="P48" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q48" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R48" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="S48" s="21"/>
       <c r="T48" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U48" s="21"/>
       <c r="V48" s="21" t="s">
@@ -3729,7 +3724,7 @@
       <c r="W48" s="21"/>
       <c r="X48" s="28"/>
     </row>
-    <row r="49" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:24" ht="15.75" customHeight="1">
       <c r="A49" s="26" t="s">
         <v>43</v>
       </c>
@@ -3738,55 +3733,55 @@
       </c>
       <c r="C49" s="21"/>
       <c r="D49" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E49" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F49" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G49" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H49" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I49" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J49" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K49" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L49" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M49" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N49" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O49" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P49" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q49" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R49" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="S49" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T49" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U49" s="21"/>
       <c r="V49" s="21" t="s">
@@ -3795,7 +3790,7 @@
       <c r="W49" s="21"/>
       <c r="X49" s="10"/>
     </row>
-    <row r="50" spans="1:24" s="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:24" s="35" customFormat="1" ht="15.75" customHeight="1">
       <c r="A50" s="26" t="s">
         <v>43</v>
       </c>
@@ -3804,49 +3799,49 @@
       </c>
       <c r="C50" s="21"/>
       <c r="D50" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E50" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F50" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G50" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H50" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I50" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J50" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K50" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L50" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M50" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N50" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O50" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P50" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q50" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R50" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="S50" s="21" t="s">
         <v>17</v>
@@ -3857,7 +3852,7 @@
       <c r="W50" s="21"/>
       <c r="X50" s="34"/>
     </row>
-    <row r="51" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:24" ht="15.75" customHeight="1">
       <c r="A51" s="26" t="s">
         <v>58</v>
       </c>
@@ -3866,55 +3861,55 @@
       </c>
       <c r="C51" s="21"/>
       <c r="D51" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E51" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F51" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G51" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H51" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I51" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J51" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K51" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L51" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M51" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N51" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O51" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P51" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q51" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R51" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="S51" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T51" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U51" s="21" t="s">
         <v>17</v>
@@ -3927,7 +3922,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="52" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:24" ht="15.75" customHeight="1">
       <c r="A52" s="26" t="s">
         <v>58</v>
       </c>
@@ -3936,55 +3931,55 @@
       </c>
       <c r="C52" s="21"/>
       <c r="D52" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E52" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F52" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G52" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H52" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I52" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J52" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K52" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L52" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M52" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N52" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O52" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P52" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q52" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R52" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="S52" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T52" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U52" s="21" t="s">
         <v>17</v>
@@ -3995,7 +3990,7 @@
       <c r="W52" s="21"/>
       <c r="X52" s="38"/>
     </row>
-    <row r="53" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:24" ht="15.75" customHeight="1">
       <c r="A53" s="26" t="s">
         <v>62</v>
       </c>
@@ -4007,50 +4002,50 @@
         <v>132</v>
       </c>
       <c r="E53" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F53" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G53" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H53" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I53" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J53" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="K53" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="K53" s="21" t="s">
-        <v>137</v>
-      </c>
       <c r="L53" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M53" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N53" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O53" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P53" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q53" s="21" t="s">
         <v>114</v>
       </c>
       <c r="R53" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="S53" s="21"/>
       <c r="T53" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="U53" s="21" t="s">
         <v>114</v>
@@ -4061,7 +4056,7 @@
       <c r="W53" s="21"/>
       <c r="X53" s="10"/>
     </row>
-    <row r="54" spans="1:24" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:24" s="15" customFormat="1" ht="15.75" customHeight="1">
       <c r="A54" s="18" t="s">
         <v>63</v>
       </c>
@@ -4095,7 +4090,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="55" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:24" ht="15.75" customHeight="1">
       <c r="A55" s="16" t="s">
         <v>63</v>
       </c>
@@ -4138,7 +4133,7 @@
       <c r="V55" s="17"/>
       <c r="W55" s="17"/>
     </row>
-    <row r="56" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:24" ht="15.75" customHeight="1">
       <c r="A56" s="16" t="s">
         <v>63</v>
       </c>
@@ -4169,7 +4164,7 @@
       <c r="V56" s="17"/>
       <c r="W56" s="17"/>
     </row>
-    <row r="57" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:24" ht="15.75" customHeight="1">
       <c r="A57" s="16" t="s">
         <v>63</v>
       </c>
@@ -4200,7 +4195,7 @@
       <c r="V57" s="17"/>
       <c r="W57" s="17"/>
     </row>
-    <row r="58" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:24" ht="15.75" customHeight="1">
       <c r="A58" s="16" t="s">
         <v>63</v>
       </c>
@@ -4231,7 +4226,7 @@
       <c r="V58" s="17"/>
       <c r="W58" s="17"/>
     </row>
-    <row r="59" spans="1:24" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:24" s="36" customFormat="1" ht="15.75" customHeight="1">
       <c r="A59" s="16" t="s">
         <v>63</v>
       </c>
@@ -4262,7 +4257,7 @@
       <c r="V59" s="17"/>
       <c r="W59" s="17"/>
     </row>
-    <row r="60" spans="1:24" s="33" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:24" s="33" customFormat="1" ht="15.75" customHeight="1">
       <c r="A60" s="16" t="s">
         <v>63</v>
       </c>
@@ -4293,7 +4288,7 @@
       <c r="V60" s="17"/>
       <c r="W60" s="17"/>
     </row>
-    <row r="61" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:24" ht="15.75" customHeight="1">
       <c r="A61" s="16" t="s">
         <v>110</v>
       </c>
@@ -4324,7 +4319,7 @@
       <c r="V61" s="20"/>
       <c r="W61" s="20"/>
     </row>
-    <row r="62" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:24" ht="15.75" customHeight="1">
       <c r="A62" s="16" t="s">
         <v>124</v>
       </c>
@@ -4333,28 +4328,28 @@
       </c>
       <c r="C62" s="20"/>
       <c r="D62" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E62" s="30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F62" s="30"/>
       <c r="G62" s="30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H62" s="30"/>
       <c r="I62" s="30"/>
       <c r="J62" s="30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K62" s="30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L62" s="30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M62" s="30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N62" s="30"/>
       <c r="O62" s="30"/>
@@ -4378,6 +4373,11 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4389,7 +4389,7 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="29.6640625" customWidth="1"/>
     <col min="2" max="2" width="28.1640625" customWidth="1"/>
@@ -4397,7 +4397,7 @@
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="15">
       <c r="A1" s="22" t="s">
         <v>70</v>
       </c>
@@ -4414,7 +4414,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15">
       <c r="A2" s="23" t="s">
         <v>73</v>
       </c>
@@ -4427,7 +4427,7 @@
       <c r="D2" s="24"/>
       <c r="E2" s="24"/>
     </row>
-    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="15">
       <c r="A3" s="23" t="s">
         <v>75</v>
       </c>
@@ -4440,7 +4440,7 @@
       <c r="D3" s="24"/>
       <c r="E3" s="24"/>
     </row>
-    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="15">
       <c r="A4" s="23" t="s">
         <v>77</v>
       </c>
@@ -4453,7 +4453,7 @@
       <c r="D4" s="24"/>
       <c r="E4" s="24"/>
     </row>
-    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="15">
       <c r="A5" s="23" t="s">
         <v>97</v>
       </c>
@@ -4468,7 +4468,7 @@
       </c>
       <c r="E5" s="24"/>
     </row>
-    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="15">
       <c r="A6" s="23" t="s">
         <v>98</v>
       </c>
@@ -4483,7 +4483,7 @@
       </c>
       <c r="E6" s="24"/>
     </row>
-    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="15">
       <c r="A7" s="23" t="s">
         <v>99</v>
       </c>
@@ -4498,7 +4498,7 @@
       </c>
       <c r="E7" s="24"/>
     </row>
-    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="15">
       <c r="A8" s="23" t="s">
         <v>100</v>
       </c>
@@ -4513,7 +4513,7 @@
       </c>
       <c r="E8" s="24"/>
     </row>
-    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="15">
       <c r="A9" s="23" t="s">
         <v>109</v>
       </c>
@@ -4526,7 +4526,7 @@
       <c r="D9" s="24"/>
       <c r="E9" s="24"/>
     </row>
-    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="15">
       <c r="A10" s="23" t="s">
         <v>108</v>
       </c>
@@ -4539,7 +4539,7 @@
       <c r="D10" s="24"/>
       <c r="E10" s="24"/>
     </row>
-    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="15">
       <c r="A11" s="23" t="s">
         <v>107</v>
       </c>
@@ -4552,7 +4552,7 @@
       <c r="D11" s="24"/>
       <c r="E11" s="24"/>
     </row>
-    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="15">
       <c r="A12" s="23" t="s">
         <v>101</v>
       </c>
@@ -4567,7 +4567,7 @@
       </c>
       <c r="E12" s="24"/>
     </row>
-    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="15">
       <c r="A13" s="23" t="s">
         <v>106</v>
       </c>
@@ -4582,7 +4582,7 @@
       </c>
       <c r="E13" s="24"/>
     </row>
-    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="15">
       <c r="A14" s="23" t="s">
         <v>102</v>
       </c>
@@ -4597,7 +4597,7 @@
       </c>
       <c r="E14" s="24"/>
     </row>
-    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="15">
       <c r="A15" s="23" t="s">
         <v>103</v>
       </c>
@@ -4612,7 +4612,7 @@
       </c>
       <c r="E15" s="24"/>
     </row>
-    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="15">
       <c r="A16" s="23" t="s">
         <v>104</v>
       </c>
@@ -4627,7 +4627,7 @@
       </c>
       <c r="E16" s="24"/>
     </row>
-    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="15">
       <c r="A17" s="23" t="s">
         <v>127</v>
       </c>
@@ -4642,7 +4642,7 @@
       </c>
       <c r="E17" s="24"/>
     </row>
-    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="15">
       <c r="A18" s="23" t="s">
         <v>12</v>
       </c>
@@ -4657,7 +4657,7 @@
       </c>
       <c r="E18" s="24"/>
     </row>
-    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="15">
       <c r="A19" s="23" t="s">
         <v>13</v>
       </c>
@@ -4672,7 +4672,7 @@
       </c>
       <c r="E19" s="24"/>
     </row>
-    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="15">
       <c r="A20" s="23" t="s">
         <v>105</v>
       </c>
@@ -4687,7 +4687,7 @@
       </c>
       <c r="E20" s="24"/>
     </row>
-    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="15">
       <c r="A21" s="23" t="s">
         <v>117</v>
       </c>
@@ -4707,5 +4707,10 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Lisää "valmis" oikeus välitavoitteelle
Lisää uusi erikoisoikeus "valmis", joka annetaan myös
urakoitsijalle. Urakoitsija voi merkata valmiiksi, mutta ei muokata muuten.
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="180" windowWidth="37420" windowHeight="27040" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="150">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -455,6 +455,24 @@
   </si>
   <si>
     <t>R*,W*,sido*</t>
+  </si>
+  <si>
+    <t>R+,valmis+</t>
+  </si>
+  <si>
+    <t>R,valmis</t>
+  </si>
+  <si>
+    <t>valmis tarkoittaa välitavoitteen merkitsemistä valmiiksi</t>
+  </si>
+  <si>
+    <t>R*,W*,valmis*</t>
+  </si>
+  <si>
+    <t>R*,W,valmis</t>
+  </si>
+  <si>
+    <t>R*,W+,valmis+</t>
   </si>
 </sst>
 </file>
@@ -1133,10 +1151,10 @@
   <dimension ref="A1:X62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="O11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="F24" sqref="F24"/>
+      <selection pane="bottomRight" activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -2315,10 +2333,10 @@
       </c>
       <c r="C24" s="21"/>
       <c r="D24" s="17" t="s">
-        <v>132</v>
+        <v>147</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="F24" s="17" t="s">
         <v>133</v>
@@ -2333,10 +2351,10 @@
         <v>133</v>
       </c>
       <c r="J24" s="17" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="K24" s="21" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="L24" s="21" t="s">
         <v>133</v>
@@ -2349,16 +2367,16 @@
       </c>
       <c r="O24" s="21"/>
       <c r="P24" s="21" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="Q24" s="21" t="s">
-        <v>17</v>
+        <v>145</v>
       </c>
       <c r="R24" s="21" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="S24" s="21" t="s">
-        <v>17</v>
+        <v>145</v>
       </c>
       <c r="T24" s="17" t="s">
         <v>137</v>
@@ -2366,7 +2384,9 @@
       <c r="U24" s="21"/>
       <c r="V24" s="21"/>
       <c r="W24" s="21"/>
-      <c r="X24" s="10"/>
+      <c r="X24" s="10" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="25" spans="1:24" ht="15.75" customHeight="1">
       <c r="A25" s="26" t="s">

</xml_diff>

<commit_message>
Lisää JVH:lle puuttuva päätös-oikeus osioon: laadunseuranta / sanktiot
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27417"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarihan/Desktop/Harja/harja/resources/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="41500" windowHeight="24520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -12,11 +17,11 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
@@ -1154,13 +1159,13 @@
   <dimension ref="A1:X62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D30" sqref="D30"/>
+      <selection pane="bottomRight" activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.5" bestFit="1" customWidth="1"/>
@@ -1187,7 +1192,7 @@
     <col min="24" max="24" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" customHeight="1">
+    <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1207,7 +1212,7 @@
       <c r="M1" s="38"/>
       <c r="N1" s="38"/>
     </row>
-    <row r="2" spans="1:24" ht="15.75" customHeight="1">
+    <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="40" t="s">
@@ -1225,7 +1230,7 @@
       <c r="M2" s="38"/>
       <c r="N2" s="38"/>
     </row>
-    <row r="3" spans="1:24" ht="15.75" customHeight="1">
+    <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -1240,10 +1245,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="15.75" customHeight="1">
+    <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:24" ht="15.75" customHeight="1">
+    <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C5" s="39" t="s">
         <v>6</v>
       </c>
@@ -1272,7 +1277,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="15.75" customHeight="1">
+    <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
@@ -1341,7 +1346,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="15.75" customHeight="1">
+    <row r="7" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="16" t="s">
         <v>15</v>
       </c>
@@ -1409,7 +1414,7 @@
       <c r="W7" s="17"/>
       <c r="X7" s="10"/>
     </row>
-    <row r="8" spans="1:24" ht="15.75" customHeight="1">
+    <row r="8" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="16" t="s">
         <v>15</v>
       </c>
@@ -1463,7 +1468,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="15.75" customHeight="1">
+    <row r="9" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="16" t="s">
         <v>15</v>
       </c>
@@ -1511,7 +1516,7 @@
       <c r="W9" s="17"/>
       <c r="X9" s="10"/>
     </row>
-    <row r="10" spans="1:24" ht="15.75" customHeight="1">
+    <row r="10" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="16" t="s">
         <v>15</v>
       </c>
@@ -1559,7 +1564,7 @@
       <c r="W10" s="17"/>
       <c r="X10" s="10"/>
     </row>
-    <row r="11" spans="1:24" ht="15.75" customHeight="1">
+    <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="16" t="s">
         <v>15</v>
       </c>
@@ -1621,7 +1626,7 @@
       <c r="W11" s="17"/>
       <c r="X11" s="10"/>
     </row>
-    <row r="12" spans="1:24" ht="15.75" customHeight="1">
+    <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="16" t="s">
         <v>15</v>
       </c>
@@ -1683,7 +1688,7 @@
       <c r="W12" s="17"/>
       <c r="X12" s="10"/>
     </row>
-    <row r="13" spans="1:24" ht="15.75" customHeight="1">
+    <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="16" t="s">
         <v>15</v>
       </c>
@@ -1731,7 +1736,7 @@
       <c r="W13" s="17"/>
       <c r="X13" s="10"/>
     </row>
-    <row r="14" spans="1:24" ht="15.75" customHeight="1">
+    <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="16" t="s">
         <v>15</v>
       </c>
@@ -1779,7 +1784,7 @@
       <c r="W14" s="17"/>
       <c r="X14" s="10"/>
     </row>
-    <row r="15" spans="1:24" ht="15.75" customHeight="1">
+    <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="16" t="s">
         <v>15</v>
       </c>
@@ -1827,7 +1832,7 @@
       <c r="W15" s="17"/>
       <c r="X15" s="10"/>
     </row>
-    <row r="16" spans="1:24" ht="15.75" customHeight="1">
+    <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="16" t="s">
         <v>15</v>
       </c>
@@ -1889,7 +1894,7 @@
       <c r="W16" s="17"/>
       <c r="X16" s="10"/>
     </row>
-    <row r="17" spans="1:24" ht="15.75" customHeight="1">
+    <row r="17" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="16" t="s">
         <v>15</v>
       </c>
@@ -1951,7 +1956,7 @@
       <c r="W17" s="17"/>
       <c r="X17" s="10"/>
     </row>
-    <row r="18" spans="1:24" ht="15.75" customHeight="1">
+    <row r="18" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="16" t="s">
         <v>15</v>
       </c>
@@ -1999,7 +2004,7 @@
       <c r="W18" s="17"/>
       <c r="X18" s="10"/>
     </row>
-    <row r="19" spans="1:24" ht="15.75" customHeight="1">
+    <row r="19" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="16" t="s">
         <v>15</v>
       </c>
@@ -2061,7 +2066,7 @@
       <c r="W19" s="17"/>
       <c r="X19" s="10"/>
     </row>
-    <row r="20" spans="1:24" ht="15.75" customHeight="1">
+    <row r="20" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="16" t="s">
         <v>15</v>
       </c>
@@ -2127,7 +2132,7 @@
       <c r="W20" s="17"/>
       <c r="X20" s="10"/>
     </row>
-    <row r="21" spans="1:24" ht="15.75" customHeight="1">
+    <row r="21" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="26" t="s">
         <v>15</v>
       </c>
@@ -2195,7 +2200,7 @@
       <c r="W21" s="21"/>
       <c r="X21" s="10"/>
     </row>
-    <row r="22" spans="1:24" ht="15.75" customHeight="1">
+    <row r="22" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="26" t="s">
         <v>15</v>
       </c>
@@ -2204,7 +2209,7 @@
       </c>
       <c r="C22" s="21"/>
       <c r="D22" s="17" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="E22" s="17" t="s">
         <v>136</v>
@@ -2261,7 +2266,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="23" spans="1:24" ht="15.75" customHeight="1">
+    <row r="23" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="26" t="s">
         <v>15</v>
       </c>
@@ -2327,7 +2332,7 @@
       <c r="W23" s="21"/>
       <c r="X23" s="10"/>
     </row>
-    <row r="24" spans="1:24" ht="15.75" customHeight="1">
+    <row r="24" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="26" t="s">
         <v>15</v>
       </c>
@@ -2391,7 +2396,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="25" spans="1:24" ht="15.75" customHeight="1">
+    <row r="25" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="26" t="s">
         <v>15</v>
       </c>
@@ -2441,7 +2446,7 @@
       <c r="W25" s="21"/>
       <c r="X25" s="10"/>
     </row>
-    <row r="26" spans="1:24" ht="15.75" customHeight="1">
+    <row r="26" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="26" t="s">
         <v>15</v>
       </c>
@@ -2487,7 +2492,7 @@
       <c r="W26" s="21"/>
       <c r="X26" s="10"/>
     </row>
-    <row r="27" spans="1:24" ht="15.75" customHeight="1">
+    <row r="27" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="26" t="s">
         <v>15</v>
       </c>
@@ -2527,7 +2532,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:24" ht="15.75" customHeight="1">
+    <row r="28" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="26" t="s">
         <v>15</v>
       </c>
@@ -2593,7 +2598,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="29" spans="1:24" ht="15.75" customHeight="1">
+    <row r="29" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="26" t="s">
         <v>15</v>
       </c>
@@ -2651,7 +2656,7 @@
       <c r="W29" s="21"/>
       <c r="X29" s="10"/>
     </row>
-    <row r="30" spans="1:24" ht="15.75" customHeight="1">
+    <row r="30" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="26" t="s">
         <v>15</v>
       </c>
@@ -2711,7 +2716,7 @@
       <c r="W30" s="21"/>
       <c r="X30" s="10"/>
     </row>
-    <row r="31" spans="1:24" ht="15.75" customHeight="1">
+    <row r="31" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="26" t="s">
         <v>15</v>
       </c>
@@ -2769,7 +2774,7 @@
       <c r="W31" s="21"/>
       <c r="X31" s="10"/>
     </row>
-    <row r="32" spans="1:24" ht="15.75" customHeight="1">
+    <row r="32" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="26" t="s">
         <v>15</v>
       </c>
@@ -2827,7 +2832,7 @@
       <c r="W32" s="21"/>
       <c r="X32" s="10"/>
     </row>
-    <row r="33" spans="1:24" s="13" customFormat="1" ht="15.75" customHeight="1">
+    <row r="33" spans="1:24" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="26" t="s">
         <v>15</v>
       </c>
@@ -2895,7 +2900,7 @@
       <c r="W33" s="21"/>
       <c r="X33" s="12"/>
     </row>
-    <row r="34" spans="1:24" s="32" customFormat="1" ht="15.75" customHeight="1">
+    <row r="34" spans="1:24" s="32" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="26" t="s">
         <v>43</v>
       </c>
@@ -2941,7 +2946,7 @@
       <c r="W34" s="21"/>
       <c r="X34" s="31"/>
     </row>
-    <row r="35" spans="1:24" ht="15.75" customHeight="1">
+    <row r="35" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="26" t="s">
         <v>43</v>
       </c>
@@ -2991,7 +2996,7 @@
       <c r="W35" s="21"/>
       <c r="X35" s="10"/>
     </row>
-    <row r="36" spans="1:24" ht="15.75" customHeight="1">
+    <row r="36" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="26" t="s">
         <v>43</v>
       </c>
@@ -3057,7 +3062,7 @@
       <c r="W36" s="21"/>
       <c r="X36" s="10"/>
     </row>
-    <row r="37" spans="1:24" ht="15.75" customHeight="1">
+    <row r="37" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="26" t="s">
         <v>43</v>
       </c>
@@ -3123,7 +3128,7 @@
       <c r="W37" s="21"/>
       <c r="X37" s="10"/>
     </row>
-    <row r="38" spans="1:24" ht="15.75" customHeight="1">
+    <row r="38" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="26" t="s">
         <v>43</v>
       </c>
@@ -3189,7 +3194,7 @@
       <c r="W38" s="21"/>
       <c r="X38" s="10"/>
     </row>
-    <row r="39" spans="1:24" ht="15.75" customHeight="1">
+    <row r="39" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="26" t="s">
         <v>43</v>
       </c>
@@ -3255,7 +3260,7 @@
       <c r="W39" s="21"/>
       <c r="X39" s="10"/>
     </row>
-    <row r="40" spans="1:24" ht="15.75" customHeight="1">
+    <row r="40" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="26" t="s">
         <v>43</v>
       </c>
@@ -3321,7 +3326,7 @@
       <c r="W40" s="21"/>
       <c r="X40" s="10"/>
     </row>
-    <row r="41" spans="1:24" ht="15.75" customHeight="1">
+    <row r="41" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="26" t="s">
         <v>43</v>
       </c>
@@ -3381,7 +3386,7 @@
       <c r="W41" s="21"/>
       <c r="X41" s="10"/>
     </row>
-    <row r="42" spans="1:24" ht="15.75" customHeight="1">
+    <row r="42" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="26" t="s">
         <v>43</v>
       </c>
@@ -3447,7 +3452,7 @@
       <c r="W42" s="21"/>
       <c r="X42" s="10"/>
     </row>
-    <row r="43" spans="1:24" ht="15.75" customHeight="1">
+    <row r="43" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="26" t="s">
         <v>43</v>
       </c>
@@ -3497,7 +3502,7 @@
       <c r="W43" s="21"/>
       <c r="X43" s="10"/>
     </row>
-    <row r="44" spans="1:24" ht="15.75" customHeight="1">
+    <row r="44" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="26" t="s">
         <v>43</v>
       </c>
@@ -3547,7 +3552,7 @@
       <c r="W44" s="21"/>
       <c r="X44" s="10"/>
     </row>
-    <row r="45" spans="1:24" ht="15.75" customHeight="1">
+    <row r="45" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="26" t="s">
         <v>43</v>
       </c>
@@ -3595,7 +3600,7 @@
       <c r="W45" s="21"/>
       <c r="X45" s="10"/>
     </row>
-    <row r="46" spans="1:24" ht="15.75" customHeight="1">
+    <row r="46" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="26" t="s">
         <v>43</v>
       </c>
@@ -3643,7 +3648,7 @@
       <c r="W46" s="21"/>
       <c r="X46" s="10"/>
     </row>
-    <row r="47" spans="1:24" ht="15.75" customHeight="1">
+    <row r="47" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="26" t="s">
         <v>43</v>
       </c>
@@ -3691,7 +3696,7 @@
       <c r="W47" s="21"/>
       <c r="X47" s="10"/>
     </row>
-    <row r="48" spans="1:24" s="29" customFormat="1" ht="15.75" customHeight="1">
+    <row r="48" spans="1:24" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="26" t="s">
         <v>43</v>
       </c>
@@ -3747,7 +3752,7 @@
       <c r="W48" s="21"/>
       <c r="X48" s="28"/>
     </row>
-    <row r="49" spans="1:24" ht="15.75" customHeight="1">
+    <row r="49" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="26" t="s">
         <v>43</v>
       </c>
@@ -3813,7 +3818,7 @@
       <c r="W49" s="21"/>
       <c r="X49" s="10"/>
     </row>
-    <row r="50" spans="1:24" s="35" customFormat="1" ht="15.75" customHeight="1">
+    <row r="50" spans="1:24" s="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="26" t="s">
         <v>43</v>
       </c>
@@ -3875,7 +3880,7 @@
       <c r="W50" s="21"/>
       <c r="X50" s="34"/>
     </row>
-    <row r="51" spans="1:24" ht="15.75" customHeight="1">
+    <row r="51" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="26" t="s">
         <v>58</v>
       </c>
@@ -3945,7 +3950,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="52" spans="1:24" ht="15.75" customHeight="1">
+    <row r="52" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="26" t="s">
         <v>58</v>
       </c>
@@ -4013,7 +4018,7 @@
       <c r="W52" s="21"/>
       <c r="X52" s="38"/>
     </row>
-    <row r="53" spans="1:24" ht="15.75" customHeight="1">
+    <row r="53" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="26" t="s">
         <v>62</v>
       </c>
@@ -4079,7 +4084,7 @@
       <c r="W53" s="21"/>
       <c r="X53" s="10"/>
     </row>
-    <row r="54" spans="1:24" s="15" customFormat="1" ht="15.75" customHeight="1">
+    <row r="54" spans="1:24" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="18" t="s">
         <v>63</v>
       </c>
@@ -4113,7 +4118,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="55" spans="1:24" ht="15.75" customHeight="1">
+    <row r="55" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="16" t="s">
         <v>63</v>
       </c>
@@ -4156,7 +4161,7 @@
       <c r="V55" s="17"/>
       <c r="W55" s="17"/>
     </row>
-    <row r="56" spans="1:24" ht="15.75" customHeight="1">
+    <row r="56" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="16" t="s">
         <v>63</v>
       </c>
@@ -4187,7 +4192,7 @@
       <c r="V56" s="17"/>
       <c r="W56" s="17"/>
     </row>
-    <row r="57" spans="1:24" ht="15.75" customHeight="1">
+    <row r="57" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="16" t="s">
         <v>63</v>
       </c>
@@ -4218,7 +4223,7 @@
       <c r="V57" s="17"/>
       <c r="W57" s="17"/>
     </row>
-    <row r="58" spans="1:24" ht="15.75" customHeight="1">
+    <row r="58" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="16" t="s">
         <v>63</v>
       </c>
@@ -4249,7 +4254,7 @@
       <c r="V58" s="17"/>
       <c r="W58" s="17"/>
     </row>
-    <row r="59" spans="1:24" s="36" customFormat="1" ht="15.75" customHeight="1">
+    <row r="59" spans="1:24" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="16" t="s">
         <v>63</v>
       </c>
@@ -4280,7 +4285,7 @@
       <c r="V59" s="17"/>
       <c r="W59" s="17"/>
     </row>
-    <row r="60" spans="1:24" s="33" customFormat="1" ht="15.75" customHeight="1">
+    <row r="60" spans="1:24" s="33" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="16" t="s">
         <v>63</v>
       </c>
@@ -4311,7 +4316,7 @@
       <c r="V60" s="17"/>
       <c r="W60" s="17"/>
     </row>
-    <row r="61" spans="1:24" ht="15.75" customHeight="1">
+    <row r="61" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="16" t="s">
         <v>110</v>
       </c>
@@ -4342,7 +4347,7 @@
       <c r="V61" s="20"/>
       <c r="W61" s="20"/>
     </row>
-    <row r="62" spans="1:24" ht="15.75" customHeight="1">
+    <row r="62" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="16" t="s">
         <v>124</v>
       </c>
@@ -4396,11 +4401,6 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -4412,7 +4412,7 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="29.6640625" customWidth="1"/>
     <col min="2" max="2" width="28.1640625" customWidth="1"/>
@@ -4420,7 +4420,7 @@
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15">
+    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
         <v>70</v>
       </c>
@@ -4437,7 +4437,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15">
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
         <v>73</v>
       </c>
@@ -4450,7 +4450,7 @@
       <c r="D2" s="24"/>
       <c r="E2" s="24"/>
     </row>
-    <row r="3" spans="1:5" ht="15">
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
         <v>75</v>
       </c>
@@ -4463,7 +4463,7 @@
       <c r="D3" s="24"/>
       <c r="E3" s="24"/>
     </row>
-    <row r="4" spans="1:5" ht="15">
+    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
         <v>77</v>
       </c>
@@ -4476,7 +4476,7 @@
       <c r="D4" s="24"/>
       <c r="E4" s="24"/>
     </row>
-    <row r="5" spans="1:5" ht="15">
+    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
         <v>97</v>
       </c>
@@ -4491,7 +4491,7 @@
       </c>
       <c r="E5" s="24"/>
     </row>
-    <row r="6" spans="1:5" ht="15">
+    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
         <v>98</v>
       </c>
@@ -4506,7 +4506,7 @@
       </c>
       <c r="E6" s="24"/>
     </row>
-    <row r="7" spans="1:5" ht="15">
+    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
         <v>99</v>
       </c>
@@ -4521,7 +4521,7 @@
       </c>
       <c r="E7" s="24"/>
     </row>
-    <row r="8" spans="1:5" ht="15">
+    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
         <v>100</v>
       </c>
@@ -4536,7 +4536,7 @@
       </c>
       <c r="E8" s="24"/>
     </row>
-    <row r="9" spans="1:5" ht="15">
+    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
         <v>109</v>
       </c>
@@ -4549,7 +4549,7 @@
       <c r="D9" s="24"/>
       <c r="E9" s="24"/>
     </row>
-    <row r="10" spans="1:5" ht="15">
+    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
         <v>108</v>
       </c>
@@ -4562,7 +4562,7 @@
       <c r="D10" s="24"/>
       <c r="E10" s="24"/>
     </row>
-    <row r="11" spans="1:5" ht="15">
+    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
         <v>107</v>
       </c>
@@ -4575,7 +4575,7 @@
       <c r="D11" s="24"/>
       <c r="E11" s="24"/>
     </row>
-    <row r="12" spans="1:5" ht="15">
+    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
         <v>101</v>
       </c>
@@ -4590,7 +4590,7 @@
       </c>
       <c r="E12" s="24"/>
     </row>
-    <row r="13" spans="1:5" ht="15">
+    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="23" t="s">
         <v>106</v>
       </c>
@@ -4605,7 +4605,7 @@
       </c>
       <c r="E13" s="24"/>
     </row>
-    <row r="14" spans="1:5" ht="15">
+    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
         <v>102</v>
       </c>
@@ -4620,7 +4620,7 @@
       </c>
       <c r="E14" s="24"/>
     </row>
-    <row r="15" spans="1:5" ht="15">
+    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
         <v>103</v>
       </c>
@@ -4635,7 +4635,7 @@
       </c>
       <c r="E15" s="24"/>
     </row>
-    <row r="16" spans="1:5" ht="15">
+    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
         <v>104</v>
       </c>
@@ -4650,7 +4650,7 @@
       </c>
       <c r="E16" s="24"/>
     </row>
-    <row r="17" spans="1:5" ht="15">
+    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="23" t="s">
         <v>127</v>
       </c>
@@ -4665,7 +4665,7 @@
       </c>
       <c r="E17" s="24"/>
     </row>
-    <row r="18" spans="1:5" ht="15">
+    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
         <v>12</v>
       </c>
@@ -4680,7 +4680,7 @@
       </c>
       <c r="E18" s="24"/>
     </row>
-    <row r="19" spans="1:5" ht="15">
+    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="23" t="s">
         <v>13</v>
       </c>
@@ -4695,7 +4695,7 @@
       </c>
       <c r="E19" s="24"/>
     </row>
-    <row r="20" spans="1:5" ht="15">
+    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
         <v>105</v>
       </c>
@@ -4710,7 +4710,7 @@
       </c>
       <c r="E20" s="24"/>
     </row>
-    <row r="21" spans="1:5" ht="15">
+    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="23" t="s">
         <v>117</v>
       </c>
@@ -4730,10 +4730,5 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert roolit.xlsx suoraan developista
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -1159,10 +1159,10 @@
   <dimension ref="A1:X62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="J6" sqref="J6"/>
+      <selection pane="bottomRight" activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2209,7 +2209,7 @@
       </c>
       <c r="C22" s="21"/>
       <c r="D22" s="17" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="E22" s="17" t="s">
         <v>136</v>

</xml_diff>

<commit_message>
Lisää ELY Pääkäyttäjälle oikeus kaikkiin urakoihin
Sähköposti Anne L Wednesday 31 August 2016 at 15:07 mukaisesti
lisätään ELY Pääkäyttäjille kirj.oikeus kaikkiin urakoihin.
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27417"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarihan/Desktop/Harja/harja/resources/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="41500" windowHeight="24520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="49180" windowHeight="24520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -17,18 +12,18 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="150">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -475,9 +470,6 @@
   </si>
   <si>
     <t>R*,W,valmis</t>
-  </si>
-  <si>
-    <t>R*,W+,valmis+</t>
   </si>
   <si>
     <t>R*,W*,päätös*,asiatarkastus*</t>
@@ -597,8 +589,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="77">
+  <cellStyleXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -745,7 +741,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="77">
+  <cellStyles count="81">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -784,6 +780,8 @@
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -822,6 +820,8 @@
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1159,13 +1159,13 @@
   <dimension ref="A1:X62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="J25" sqref="J25"/>
+      <selection pane="bottomRight" activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.5" bestFit="1" customWidth="1"/>
@@ -1192,7 +1192,7 @@
     <col min="24" max="24" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:24" ht="15.75" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1212,7 +1212,7 @@
       <c r="M1" s="38"/>
       <c r="N1" s="38"/>
     </row>
-    <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:24" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="40" t="s">
@@ -1230,7 +1230,7 @@
       <c r="M2" s="38"/>
       <c r="N2" s="38"/>
     </row>
-    <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:24" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -1245,10 +1245,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:24" ht="15.75" customHeight="1">
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:24" ht="15.75" customHeight="1">
       <c r="C5" s="39" t="s">
         <v>6</v>
       </c>
@@ -1277,7 +1277,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:24" ht="15.75" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
@@ -1346,7 +1346,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:24" ht="15.75" customHeight="1">
       <c r="A7" s="16" t="s">
         <v>15</v>
       </c>
@@ -1373,7 +1373,7 @@
         <v>133</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="K7" s="17" t="s">
         <v>136</v>
@@ -1414,7 +1414,7 @@
       <c r="W7" s="17"/>
       <c r="X7" s="10"/>
     </row>
-    <row r="8" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:24" ht="15.75" customHeight="1">
       <c r="A8" s="16" t="s">
         <v>15</v>
       </c>
@@ -1435,7 +1435,7 @@
       <c r="H8" s="21"/>
       <c r="I8" s="21"/>
       <c r="J8" s="17" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="K8" s="17" t="s">
         <v>136</v>
@@ -1468,7 +1468,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:24" ht="15.75" customHeight="1">
       <c r="A9" s="16" t="s">
         <v>15</v>
       </c>
@@ -1489,7 +1489,7 @@
       <c r="H9" s="21"/>
       <c r="I9" s="21"/>
       <c r="J9" s="17" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="K9" s="17" t="s">
         <v>136</v>
@@ -1516,7 +1516,7 @@
       <c r="W9" s="17"/>
       <c r="X9" s="10"/>
     </row>
-    <row r="10" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:24" ht="15.75" customHeight="1">
       <c r="A10" s="16" t="s">
         <v>15</v>
       </c>
@@ -1537,7 +1537,7 @@
       <c r="H10" s="21"/>
       <c r="I10" s="21"/>
       <c r="J10" s="17" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="K10" s="17" t="s">
         <v>136</v>
@@ -1564,7 +1564,7 @@
       <c r="W10" s="17"/>
       <c r="X10" s="10"/>
     </row>
-    <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:24" ht="15.75" customHeight="1">
       <c r="A11" s="16" t="s">
         <v>15</v>
       </c>
@@ -1591,7 +1591,7 @@
         <v>133</v>
       </c>
       <c r="J11" s="17" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="K11" s="17" t="s">
         <v>136</v>
@@ -1626,7 +1626,7 @@
       <c r="W11" s="17"/>
       <c r="X11" s="10"/>
     </row>
-    <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:24" ht="15.75" customHeight="1">
       <c r="A12" s="16" t="s">
         <v>15</v>
       </c>
@@ -1653,7 +1653,7 @@
         <v>133</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="K12" s="17" t="s">
         <v>136</v>
@@ -1688,7 +1688,7 @@
       <c r="W12" s="17"/>
       <c r="X12" s="10"/>
     </row>
-    <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:24" ht="15.75" customHeight="1">
       <c r="A13" s="16" t="s">
         <v>15</v>
       </c>
@@ -1709,7 +1709,7 @@
       <c r="H13" s="21"/>
       <c r="I13" s="21"/>
       <c r="J13" s="17" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="K13" s="17" t="s">
         <v>133</v>
@@ -1736,7 +1736,7 @@
       <c r="W13" s="17"/>
       <c r="X13" s="10"/>
     </row>
-    <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:24" ht="15.75" customHeight="1">
       <c r="A14" s="16" t="s">
         <v>15</v>
       </c>
@@ -1757,7 +1757,7 @@
       <c r="H14" s="21"/>
       <c r="I14" s="21"/>
       <c r="J14" s="17" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="K14" s="17" t="s">
         <v>133</v>
@@ -1784,7 +1784,7 @@
       <c r="W14" s="17"/>
       <c r="X14" s="10"/>
     </row>
-    <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:24" ht="15.75" customHeight="1">
       <c r="A15" s="16" t="s">
         <v>15</v>
       </c>
@@ -1805,7 +1805,7 @@
       <c r="H15" s="21"/>
       <c r="I15" s="21"/>
       <c r="J15" s="17" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="K15" s="17" t="s">
         <v>133</v>
@@ -1832,7 +1832,7 @@
       <c r="W15" s="17"/>
       <c r="X15" s="10"/>
     </row>
-    <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:24" ht="15.75" customHeight="1">
       <c r="A16" s="16" t="s">
         <v>15</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>133</v>
       </c>
       <c r="J16" s="17" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="K16" s="17" t="s">
         <v>133</v>
@@ -1894,7 +1894,7 @@
       <c r="W16" s="17"/>
       <c r="X16" s="10"/>
     </row>
-    <row r="17" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:24" ht="15.75" customHeight="1">
       <c r="A17" s="16" t="s">
         <v>15</v>
       </c>
@@ -1921,7 +1921,7 @@
         <v>133</v>
       </c>
       <c r="J17" s="17" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="K17" s="17" t="s">
         <v>133</v>
@@ -1956,7 +1956,7 @@
       <c r="W17" s="17"/>
       <c r="X17" s="10"/>
     </row>
-    <row r="18" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:24" ht="15.75" customHeight="1">
       <c r="A18" s="16" t="s">
         <v>15</v>
       </c>
@@ -1977,7 +1977,7 @@
       <c r="H18" s="21"/>
       <c r="I18" s="21"/>
       <c r="J18" s="17" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="K18" s="17" t="s">
         <v>136</v>
@@ -2004,7 +2004,7 @@
       <c r="W18" s="17"/>
       <c r="X18" s="10"/>
     </row>
-    <row r="19" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:24" ht="15.75" customHeight="1">
       <c r="A19" s="16" t="s">
         <v>15</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>133</v>
       </c>
       <c r="J19" s="17" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="K19" s="17" t="s">
         <v>133</v>
@@ -2066,7 +2066,7 @@
       <c r="W19" s="17"/>
       <c r="X19" s="10"/>
     </row>
-    <row r="20" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:24" ht="15.75" customHeight="1">
       <c r="A20" s="16" t="s">
         <v>15</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>133</v>
       </c>
       <c r="J20" s="17" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="K20" s="17" t="s">
         <v>136</v>
@@ -2132,7 +2132,7 @@
       <c r="W20" s="17"/>
       <c r="X20" s="10"/>
     </row>
-    <row r="21" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:24" ht="15.75" customHeight="1">
       <c r="A21" s="26" t="s">
         <v>15</v>
       </c>
@@ -2159,7 +2159,7 @@
         <v>133</v>
       </c>
       <c r="J21" s="17" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="K21" s="17" t="s">
         <v>136</v>
@@ -2200,7 +2200,7 @@
       <c r="W21" s="21"/>
       <c r="X21" s="10"/>
     </row>
-    <row r="22" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:24" ht="15.75" customHeight="1">
       <c r="A22" s="26" t="s">
         <v>15</v>
       </c>
@@ -2227,7 +2227,7 @@
         <v>133</v>
       </c>
       <c r="J22" s="17" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="K22" s="21" t="s">
         <v>139</v>
@@ -2266,7 +2266,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="23" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:24" ht="15.75" customHeight="1">
       <c r="A23" s="26" t="s">
         <v>15</v>
       </c>
@@ -2293,7 +2293,7 @@
         <v>133</v>
       </c>
       <c r="J23" s="17" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="K23" s="21" t="s">
         <v>136</v>
@@ -2332,7 +2332,7 @@
       <c r="W23" s="21"/>
       <c r="X23" s="10"/>
     </row>
-    <row r="24" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:24" ht="15.75" customHeight="1">
       <c r="A24" s="26" t="s">
         <v>15</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>133</v>
       </c>
       <c r="J24" s="17" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="K24" s="21" t="s">
         <v>148</v>
@@ -2396,7 +2396,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="25" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:24" ht="15.75" customHeight="1">
       <c r="A25" s="26" t="s">
         <v>15</v>
       </c>
@@ -2417,7 +2417,7 @@
         <v>132</v>
       </c>
       <c r="J25" s="17" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="K25" s="21" t="s">
         <v>136</v>
@@ -2446,7 +2446,7 @@
       <c r="W25" s="21"/>
       <c r="X25" s="10"/>
     </row>
-    <row r="26" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:24" ht="15.75" customHeight="1">
       <c r="A26" s="26" t="s">
         <v>15</v>
       </c>
@@ -2467,7 +2467,7 @@
       <c r="H26" s="21"/>
       <c r="I26" s="21"/>
       <c r="J26" s="17" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="K26" s="21" t="s">
         <v>136</v>
@@ -2492,7 +2492,7 @@
       <c r="W26" s="21"/>
       <c r="X26" s="10"/>
     </row>
-    <row r="27" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:24" ht="15.75" customHeight="1">
       <c r="A27" s="26" t="s">
         <v>15</v>
       </c>
@@ -2511,7 +2511,7 @@
       <c r="H27" s="21"/>
       <c r="I27" s="21"/>
       <c r="J27" s="17" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="K27" s="21" t="s">
         <v>136</v>
@@ -2532,7 +2532,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:24" ht="15.75" customHeight="1">
       <c r="A28" s="26" t="s">
         <v>15</v>
       </c>
@@ -2559,7 +2559,7 @@
         <v>133</v>
       </c>
       <c r="J28" s="17" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="K28" s="21" t="s">
         <v>136</v>
@@ -2598,7 +2598,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="29" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:24" ht="15.75" customHeight="1">
       <c r="A29" s="26" t="s">
         <v>15</v>
       </c>
@@ -2623,7 +2623,7 @@
         <v>133</v>
       </c>
       <c r="J29" s="17" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="K29" s="21" t="s">
         <v>136</v>
@@ -2656,7 +2656,7 @@
       <c r="W29" s="21"/>
       <c r="X29" s="10"/>
     </row>
-    <row r="30" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:24" ht="15.75" customHeight="1">
       <c r="A30" s="26" t="s">
         <v>15</v>
       </c>
@@ -2665,7 +2665,7 @@
       </c>
       <c r="C30" s="21"/>
       <c r="D30" s="17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E30" s="17" t="s">
         <v>136</v>
@@ -2683,7 +2683,7 @@
         <v>133</v>
       </c>
       <c r="J30" s="17" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="K30" s="21" t="s">
         <v>139</v>
@@ -2716,7 +2716,7 @@
       <c r="W30" s="21"/>
       <c r="X30" s="10"/>
     </row>
-    <row r="31" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:24" ht="15.75" customHeight="1">
       <c r="A31" s="26" t="s">
         <v>15</v>
       </c>
@@ -2741,7 +2741,7 @@
         <v>133</v>
       </c>
       <c r="J31" s="17" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="K31" s="21" t="s">
         <v>136</v>
@@ -2774,7 +2774,7 @@
       <c r="W31" s="21"/>
       <c r="X31" s="10"/>
     </row>
-    <row r="32" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:24" ht="15.75" customHeight="1">
       <c r="A32" s="26" t="s">
         <v>15</v>
       </c>
@@ -2799,7 +2799,7 @@
         <v>133</v>
       </c>
       <c r="J32" s="17" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="K32" s="21" t="s">
         <v>136</v>
@@ -2832,7 +2832,7 @@
       <c r="W32" s="21"/>
       <c r="X32" s="10"/>
     </row>
-    <row r="33" spans="1:24" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:24" s="13" customFormat="1" ht="15.75" customHeight="1">
       <c r="A33" s="26" t="s">
         <v>15</v>
       </c>
@@ -2859,7 +2859,7 @@
         <v>132</v>
       </c>
       <c r="J33" s="17" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="K33" s="21" t="s">
         <v>139</v>
@@ -2900,7 +2900,7 @@
       <c r="W33" s="21"/>
       <c r="X33" s="12"/>
     </row>
-    <row r="34" spans="1:24" s="32" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:24" s="32" customFormat="1" ht="15.75" customHeight="1">
       <c r="A34" s="26" t="s">
         <v>43</v>
       </c>
@@ -2946,7 +2946,7 @@
       <c r="W34" s="21"/>
       <c r="X34" s="31"/>
     </row>
-    <row r="35" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:24" ht="15.75" customHeight="1">
       <c r="A35" s="26" t="s">
         <v>43</v>
       </c>
@@ -2996,7 +2996,7 @@
       <c r="W35" s="21"/>
       <c r="X35" s="10"/>
     </row>
-    <row r="36" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:24" ht="15.75" customHeight="1">
       <c r="A36" s="26" t="s">
         <v>43</v>
       </c>
@@ -3062,7 +3062,7 @@
       <c r="W36" s="21"/>
       <c r="X36" s="10"/>
     </row>
-    <row r="37" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:24" ht="15.75" customHeight="1">
       <c r="A37" s="26" t="s">
         <v>43</v>
       </c>
@@ -3128,7 +3128,7 @@
       <c r="W37" s="21"/>
       <c r="X37" s="10"/>
     </row>
-    <row r="38" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:24" ht="15.75" customHeight="1">
       <c r="A38" s="26" t="s">
         <v>43</v>
       </c>
@@ -3194,7 +3194,7 @@
       <c r="W38" s="21"/>
       <c r="X38" s="10"/>
     </row>
-    <row r="39" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:24" ht="15.75" customHeight="1">
       <c r="A39" s="26" t="s">
         <v>43</v>
       </c>
@@ -3260,7 +3260,7 @@
       <c r="W39" s="21"/>
       <c r="X39" s="10"/>
     </row>
-    <row r="40" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:24" ht="15.75" customHeight="1">
       <c r="A40" s="26" t="s">
         <v>43</v>
       </c>
@@ -3326,7 +3326,7 @@
       <c r="W40" s="21"/>
       <c r="X40" s="10"/>
     </row>
-    <row r="41" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:24" ht="15.75" customHeight="1">
       <c r="A41" s="26" t="s">
         <v>43</v>
       </c>
@@ -3386,7 +3386,7 @@
       <c r="W41" s="21"/>
       <c r="X41" s="10"/>
     </row>
-    <row r="42" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:24" ht="15.75" customHeight="1">
       <c r="A42" s="26" t="s">
         <v>43</v>
       </c>
@@ -3452,7 +3452,7 @@
       <c r="W42" s="21"/>
       <c r="X42" s="10"/>
     </row>
-    <row r="43" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:24" ht="15.75" customHeight="1">
       <c r="A43" s="26" t="s">
         <v>43</v>
       </c>
@@ -3502,7 +3502,7 @@
       <c r="W43" s="21"/>
       <c r="X43" s="10"/>
     </row>
-    <row r="44" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:24" ht="15.75" customHeight="1">
       <c r="A44" s="26" t="s">
         <v>43</v>
       </c>
@@ -3552,7 +3552,7 @@
       <c r="W44" s="21"/>
       <c r="X44" s="10"/>
     </row>
-    <row r="45" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:24" ht="15.75" customHeight="1">
       <c r="A45" s="26" t="s">
         <v>43</v>
       </c>
@@ -3600,7 +3600,7 @@
       <c r="W45" s="21"/>
       <c r="X45" s="10"/>
     </row>
-    <row r="46" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:24" ht="15.75" customHeight="1">
       <c r="A46" s="26" t="s">
         <v>43</v>
       </c>
@@ -3648,7 +3648,7 @@
       <c r="W46" s="21"/>
       <c r="X46" s="10"/>
     </row>
-    <row r="47" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:24" ht="15.75" customHeight="1">
       <c r="A47" s="26" t="s">
         <v>43</v>
       </c>
@@ -3696,7 +3696,7 @@
       <c r="W47" s="21"/>
       <c r="X47" s="10"/>
     </row>
-    <row r="48" spans="1:24" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:24" s="29" customFormat="1" ht="15.75" customHeight="1">
       <c r="A48" s="26" t="s">
         <v>43</v>
       </c>
@@ -3752,7 +3752,7 @@
       <c r="W48" s="21"/>
       <c r="X48" s="28"/>
     </row>
-    <row r="49" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:24" ht="15.75" customHeight="1">
       <c r="A49" s="26" t="s">
         <v>43</v>
       </c>
@@ -3818,7 +3818,7 @@
       <c r="W49" s="21"/>
       <c r="X49" s="10"/>
     </row>
-    <row r="50" spans="1:24" s="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:24" s="35" customFormat="1" ht="15.75" customHeight="1">
       <c r="A50" s="26" t="s">
         <v>43</v>
       </c>
@@ -3880,7 +3880,7 @@
       <c r="W50" s="21"/>
       <c r="X50" s="34"/>
     </row>
-    <row r="51" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:24" ht="15.75" customHeight="1">
       <c r="A51" s="26" t="s">
         <v>58</v>
       </c>
@@ -3950,7 +3950,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="52" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:24" ht="15.75" customHeight="1">
       <c r="A52" s="26" t="s">
         <v>58</v>
       </c>
@@ -4018,7 +4018,7 @@
       <c r="W52" s="21"/>
       <c r="X52" s="38"/>
     </row>
-    <row r="53" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:24" ht="15.75" customHeight="1">
       <c r="A53" s="26" t="s">
         <v>62</v>
       </c>
@@ -4045,7 +4045,7 @@
         <v>133</v>
       </c>
       <c r="J53" s="21" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="K53" s="21" t="s">
         <v>136</v>
@@ -4084,7 +4084,7 @@
       <c r="W53" s="21"/>
       <c r="X53" s="10"/>
     </row>
-    <row r="54" spans="1:24" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:24" s="15" customFormat="1" ht="15.75" customHeight="1">
       <c r="A54" s="18" t="s">
         <v>63</v>
       </c>
@@ -4118,7 +4118,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="55" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:24" ht="15.75" customHeight="1">
       <c r="A55" s="16" t="s">
         <v>63</v>
       </c>
@@ -4161,7 +4161,7 @@
       <c r="V55" s="17"/>
       <c r="W55" s="17"/>
     </row>
-    <row r="56" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:24" ht="15.75" customHeight="1">
       <c r="A56" s="16" t="s">
         <v>63</v>
       </c>
@@ -4192,7 +4192,7 @@
       <c r="V56" s="17"/>
       <c r="W56" s="17"/>
     </row>
-    <row r="57" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:24" ht="15.75" customHeight="1">
       <c r="A57" s="16" t="s">
         <v>63</v>
       </c>
@@ -4223,7 +4223,7 @@
       <c r="V57" s="17"/>
       <c r="W57" s="17"/>
     </row>
-    <row r="58" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:24" ht="15.75" customHeight="1">
       <c r="A58" s="16" t="s">
         <v>63</v>
       </c>
@@ -4254,7 +4254,7 @@
       <c r="V58" s="17"/>
       <c r="W58" s="17"/>
     </row>
-    <row r="59" spans="1:24" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:24" s="36" customFormat="1" ht="15.75" customHeight="1">
       <c r="A59" s="16" t="s">
         <v>63</v>
       </c>
@@ -4285,7 +4285,7 @@
       <c r="V59" s="17"/>
       <c r="W59" s="17"/>
     </row>
-    <row r="60" spans="1:24" s="33" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:24" s="33" customFormat="1" ht="15.75" customHeight="1">
       <c r="A60" s="16" t="s">
         <v>63</v>
       </c>
@@ -4316,7 +4316,7 @@
       <c r="V60" s="17"/>
       <c r="W60" s="17"/>
     </row>
-    <row r="61" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:24" ht="15.75" customHeight="1">
       <c r="A61" s="16" t="s">
         <v>110</v>
       </c>
@@ -4347,7 +4347,7 @@
       <c r="V61" s="20"/>
       <c r="W61" s="20"/>
     </row>
-    <row r="62" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:24" ht="15.75" customHeight="1">
       <c r="A62" s="16" t="s">
         <v>124</v>
       </c>
@@ -4401,6 +4401,11 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4412,7 +4417,7 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="29.6640625" customWidth="1"/>
     <col min="2" max="2" width="28.1640625" customWidth="1"/>
@@ -4420,7 +4425,7 @@
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="15">
       <c r="A1" s="22" t="s">
         <v>70</v>
       </c>
@@ -4437,7 +4442,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15">
       <c r="A2" s="23" t="s">
         <v>73</v>
       </c>
@@ -4450,7 +4455,7 @@
       <c r="D2" s="24"/>
       <c r="E2" s="24"/>
     </row>
-    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="15">
       <c r="A3" s="23" t="s">
         <v>75</v>
       </c>
@@ -4463,7 +4468,7 @@
       <c r="D3" s="24"/>
       <c r="E3" s="24"/>
     </row>
-    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="15">
       <c r="A4" s="23" t="s">
         <v>77</v>
       </c>
@@ -4476,7 +4481,7 @@
       <c r="D4" s="24"/>
       <c r="E4" s="24"/>
     </row>
-    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="15">
       <c r="A5" s="23" t="s">
         <v>97</v>
       </c>
@@ -4491,7 +4496,7 @@
       </c>
       <c r="E5" s="24"/>
     </row>
-    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="15">
       <c r="A6" s="23" t="s">
         <v>98</v>
       </c>
@@ -4506,7 +4511,7 @@
       </c>
       <c r="E6" s="24"/>
     </row>
-    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="15">
       <c r="A7" s="23" t="s">
         <v>99</v>
       </c>
@@ -4521,7 +4526,7 @@
       </c>
       <c r="E7" s="24"/>
     </row>
-    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="15">
       <c r="A8" s="23" t="s">
         <v>100</v>
       </c>
@@ -4536,7 +4541,7 @@
       </c>
       <c r="E8" s="24"/>
     </row>
-    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="15">
       <c r="A9" s="23" t="s">
         <v>109</v>
       </c>
@@ -4549,7 +4554,7 @@
       <c r="D9" s="24"/>
       <c r="E9" s="24"/>
     </row>
-    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="15">
       <c r="A10" s="23" t="s">
         <v>108</v>
       </c>
@@ -4562,7 +4567,7 @@
       <c r="D10" s="24"/>
       <c r="E10" s="24"/>
     </row>
-    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="15">
       <c r="A11" s="23" t="s">
         <v>107</v>
       </c>
@@ -4575,7 +4580,7 @@
       <c r="D11" s="24"/>
       <c r="E11" s="24"/>
     </row>
-    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="15">
       <c r="A12" s="23" t="s">
         <v>101</v>
       </c>
@@ -4590,7 +4595,7 @@
       </c>
       <c r="E12" s="24"/>
     </row>
-    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="15">
       <c r="A13" s="23" t="s">
         <v>106</v>
       </c>
@@ -4605,7 +4610,7 @@
       </c>
       <c r="E13" s="24"/>
     </row>
-    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="15">
       <c r="A14" s="23" t="s">
         <v>102</v>
       </c>
@@ -4620,7 +4625,7 @@
       </c>
       <c r="E14" s="24"/>
     </row>
-    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="15">
       <c r="A15" s="23" t="s">
         <v>103</v>
       </c>
@@ -4635,7 +4640,7 @@
       </c>
       <c r="E15" s="24"/>
     </row>
-    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="15">
       <c r="A16" s="23" t="s">
         <v>104</v>
       </c>
@@ -4650,7 +4655,7 @@
       </c>
       <c r="E16" s="24"/>
     </row>
-    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="15">
       <c r="A17" s="23" t="s">
         <v>127</v>
       </c>
@@ -4665,7 +4670,7 @@
       </c>
       <c r="E17" s="24"/>
     </row>
-    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="15">
       <c r="A18" s="23" t="s">
         <v>12</v>
       </c>
@@ -4680,7 +4685,7 @@
       </c>
       <c r="E18" s="24"/>
     </row>
-    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="15">
       <c r="A19" s="23" t="s">
         <v>13</v>
       </c>
@@ -4695,7 +4700,7 @@
       </c>
       <c r="E19" s="24"/>
     </row>
-    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="15">
       <c r="A20" s="23" t="s">
         <v>105</v>
       </c>
@@ -4710,7 +4715,7 @@
       </c>
       <c r="E20" s="24"/>
     </row>
-    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="15">
       <c r="A21" s="23" t="s">
         <v>117</v>
       </c>
@@ -4730,5 +4735,10 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Lisää puuttuneet raportit rooli-Exceliin
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="49180" windowHeight="24520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="49980" windowHeight="27800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="155">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -473,6 +473,21 @@
   </si>
   <si>
     <t>R*,W*,päätös*,asiatarkastus*</t>
+  </si>
+  <si>
+    <t>Toimenpidekilometrit</t>
+  </si>
+  <si>
+    <t>Toimenpidepäivät</t>
+  </si>
+  <si>
+    <t>Välitavoiteraportti</t>
+  </si>
+  <si>
+    <t>Siltatarkastusraportti</t>
+  </si>
+  <si>
+    <t>Indeksitarkistusraportti</t>
   </si>
 </sst>
 </file>
@@ -589,7 +604,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="81">
+  <cellStyleXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -671,8 +686,38 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -738,10 +783,14 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="81">
+  <cellStyles count="111">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -782,6 +831,21 @@
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -822,6 +886,21 @@
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1156,13 +1235,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X62"/>
+  <dimension ref="A1:X67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="J10" sqref="J10"/>
+      <selection pane="bottomRight" activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1197,38 +1276,38 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="42" t="s">
         <v>131</v>
       </c>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
     </row>
     <row r="2" spans="1:24" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
     </row>
     <row r="3" spans="1:24" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
@@ -1249,30 +1328,30 @@
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:24" ht="15.75" customHeight="1">
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="J5" s="39" t="s">
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="J5" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="38"/>
-      <c r="L5" s="38"/>
-      <c r="M5" s="38"/>
-      <c r="N5" s="38"/>
-      <c r="P5" s="39" t="s">
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
+      <c r="N5" s="40"/>
+      <c r="P5" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="Q5" s="38"/>
-      <c r="R5" s="38"/>
-      <c r="S5" s="38"/>
-      <c r="T5" s="38"/>
-      <c r="U5" s="38"/>
-      <c r="V5" s="38"/>
+      <c r="Q5" s="40"/>
+      <c r="R5" s="40"/>
+      <c r="S5" s="40"/>
+      <c r="T5" s="40"/>
+      <c r="U5" s="40"/>
+      <c r="V5" s="40"/>
       <c r="X5" s="5" t="s">
         <v>14</v>
       </c>
@@ -3818,7 +3897,7 @@
       <c r="W49" s="21"/>
       <c r="X49" s="10"/>
     </row>
-    <row r="50" spans="1:24" s="35" customFormat="1" ht="15.75" customHeight="1">
+    <row r="50" spans="1:24" s="38" customFormat="1" ht="15.75" customHeight="1">
       <c r="A50" s="26" t="s">
         <v>43</v>
       </c>
@@ -3878,14 +3957,14 @@
       <c r="U50" s="21"/>
       <c r="V50" s="21"/>
       <c r="W50" s="21"/>
-      <c r="X50" s="34"/>
-    </row>
-    <row r="51" spans="1:24" ht="15.75" customHeight="1">
+      <c r="X50" s="37"/>
+    </row>
+    <row r="51" spans="1:24" s="38" customFormat="1" ht="15.75" customHeight="1">
       <c r="A51" s="26" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="B51" s="26" t="s">
-        <v>59</v>
+        <v>150</v>
       </c>
       <c r="C51" s="21"/>
       <c r="D51" s="21" t="s">
@@ -3936,26 +4015,18 @@
       <c r="S51" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="T51" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="U51" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="V51" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="T51" s="21"/>
+      <c r="U51" s="21"/>
+      <c r="V51" s="21"/>
       <c r="W51" s="21"/>
-      <c r="X51" s="37" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="52" spans="1:24" ht="15.75" customHeight="1">
+      <c r="X51" s="37"/>
+    </row>
+    <row r="52" spans="1:24" s="38" customFormat="1" ht="15.75" customHeight="1">
       <c r="A52" s="26" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="B52" s="26" t="s">
-        <v>61</v>
+        <v>151</v>
       </c>
       <c r="C52" s="21"/>
       <c r="D52" s="21" t="s">
@@ -4006,306 +4077,457 @@
       <c r="S52" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="T52" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="U52" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="V52" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="T52" s="21"/>
+      <c r="U52" s="21"/>
+      <c r="V52" s="21"/>
       <c r="W52" s="21"/>
-      <c r="X52" s="38"/>
-    </row>
-    <row r="53" spans="1:24" ht="15.75" customHeight="1">
+      <c r="X52" s="37"/>
+    </row>
+    <row r="53" spans="1:24" s="38" customFormat="1" ht="15.75" customHeight="1">
       <c r="A53" s="26" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="B53" s="26" t="s">
-        <v>62</v>
+        <v>152</v>
       </c>
       <c r="C53" s="21"/>
       <c r="D53" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="E53" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E53" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="F53" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="G53" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="H53" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="I53" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="J53" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="K53" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="L53" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="M53" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="N53" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="O53" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="P53" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q53" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="R53" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="S53" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="T53" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="U53" s="21"/>
+      <c r="V53" s="21"/>
+      <c r="W53" s="21"/>
+      <c r="X53" s="37"/>
+    </row>
+    <row r="54" spans="1:24" s="38" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A54" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B54" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="C54" s="21"/>
+      <c r="D54" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="E54" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="F54" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="G54" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="H54" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="I54" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="J54" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="K54" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="L54" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="M54" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="N54" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="O54" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="P54" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q54" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="R54" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="S54" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="T54" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="U54" s="21"/>
+      <c r="V54" s="21"/>
+      <c r="W54" s="21"/>
+      <c r="X54" s="37"/>
+    </row>
+    <row r="55" spans="1:24" s="35" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A55" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B55" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="C55" s="21"/>
+      <c r="D55" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E55" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="F55" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="G55" s="21"/>
+      <c r="H55" s="21"/>
+      <c r="I55" s="21"/>
+      <c r="J55" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="K55" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="L55" s="21"/>
+      <c r="M55" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="N55" s="21"/>
+      <c r="O55" s="21"/>
+      <c r="P55" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q55" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="R55" s="21"/>
+      <c r="S55" s="21"/>
+      <c r="T55" s="21"/>
+      <c r="U55" s="21"/>
+      <c r="V55" s="21"/>
+      <c r="W55" s="21"/>
+      <c r="X55" s="34"/>
+    </row>
+    <row r="56" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A56" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B56" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C56" s="21"/>
+      <c r="D56" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="E56" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="F56" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="G56" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="H56" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="I56" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="J56" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="K56" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="L56" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="M56" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="N56" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="O56" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="P56" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q56" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="R56" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="S56" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="T56" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="U56" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="V56" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="W56" s="21"/>
+      <c r="X56" s="39" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A57" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B57" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C57" s="21"/>
+      <c r="D57" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="E57" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="F57" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="G57" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="H57" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="I57" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="J57" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="K57" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="L57" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="M57" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="N57" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="O57" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="P57" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q57" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="R57" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="S57" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="T57" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="U57" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="V57" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="W57" s="21"/>
+      <c r="X57" s="40"/>
+    </row>
+    <row r="58" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A58" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="B58" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C58" s="21"/>
+      <c r="D58" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="E58" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="F53" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="G53" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="H53" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="I53" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="J53" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="K53" s="21" t="s">
+      <c r="F58" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="G58" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="H58" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="I58" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="J58" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="K58" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="L53" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="M53" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="N53" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="O53" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="P53" s="21" t="s">
+      <c r="L58" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="M58" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="N58" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="O58" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="P58" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="Q53" s="21" t="s">
+      <c r="Q58" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="R53" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="S53" s="21"/>
-      <c r="T53" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="U53" s="21" t="s">
+      <c r="R58" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="S58" s="21"/>
+      <c r="T58" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="U58" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="V53" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="W53" s="21"/>
-      <c r="X53" s="10"/>
-    </row>
-    <row r="54" spans="1:24" s="15" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A54" s="18" t="s">
+      <c r="V58" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="W58" s="21"/>
+      <c r="X58" s="10"/>
+    </row>
+    <row r="59" spans="1:24" s="15" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A59" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="B54" s="18" t="s">
+      <c r="B59" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="C54" s="19"/>
-      <c r="D54" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="E54" s="19"/>
-      <c r="F54" s="19"/>
-      <c r="G54" s="19"/>
-      <c r="H54" s="19"/>
-      <c r="I54" s="19"/>
-      <c r="J54" s="19"/>
-      <c r="K54" s="19"/>
-      <c r="L54" s="19"/>
-      <c r="M54" s="19"/>
-      <c r="N54" s="19"/>
-      <c r="O54" s="19"/>
-      <c r="P54" s="19"/>
-      <c r="Q54" s="19"/>
-      <c r="R54" s="19"/>
-      <c r="S54" s="19"/>
-      <c r="T54" s="19"/>
-      <c r="U54" s="19"/>
-      <c r="V54" s="19"/>
-      <c r="W54" s="19"/>
-      <c r="X54" s="14" t="s">
+      <c r="C59" s="19"/>
+      <c r="D59" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="E59" s="19"/>
+      <c r="F59" s="19"/>
+      <c r="G59" s="19"/>
+      <c r="H59" s="19"/>
+      <c r="I59" s="19"/>
+      <c r="J59" s="19"/>
+      <c r="K59" s="19"/>
+      <c r="L59" s="19"/>
+      <c r="M59" s="19"/>
+      <c r="N59" s="19"/>
+      <c r="O59" s="19"/>
+      <c r="P59" s="19"/>
+      <c r="Q59" s="19"/>
+      <c r="R59" s="19"/>
+      <c r="S59" s="19"/>
+      <c r="T59" s="19"/>
+      <c r="U59" s="19"/>
+      <c r="V59" s="19"/>
+      <c r="W59" s="19"/>
+      <c r="X59" s="14" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="55" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A55" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="B55" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="C55" s="17"/>
-      <c r="D55" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="E55" s="17"/>
-      <c r="F55" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="G55" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="H55" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="I55" s="17"/>
-      <c r="J55" s="17"/>
-      <c r="K55" s="17"/>
-      <c r="L55" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="M55" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="N55" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="O55" s="17"/>
-      <c r="P55" s="17"/>
-      <c r="Q55" s="17"/>
-      <c r="R55" s="17"/>
-      <c r="S55" s="17"/>
-      <c r="T55" s="17"/>
-      <c r="U55" s="17"/>
-      <c r="V55" s="17"/>
-      <c r="W55" s="17"/>
-    </row>
-    <row r="56" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A56" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="B56" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="C56" s="17"/>
-      <c r="D56" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="E56" s="17"/>
-      <c r="F56" s="17"/>
-      <c r="G56" s="17"/>
-      <c r="H56" s="17"/>
-      <c r="I56" s="17"/>
-      <c r="J56" s="17"/>
-      <c r="K56" s="17"/>
-      <c r="L56" s="17"/>
-      <c r="M56" s="17"/>
-      <c r="N56" s="17"/>
-      <c r="O56" s="17"/>
-      <c r="P56" s="17"/>
-      <c r="Q56" s="17"/>
-      <c r="R56" s="17"/>
-      <c r="S56" s="17"/>
-      <c r="T56" s="17"/>
-      <c r="U56" s="17"/>
-      <c r="V56" s="17"/>
-      <c r="W56" s="17"/>
-    </row>
-    <row r="57" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A57" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="B57" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="C57" s="17"/>
-      <c r="D57" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="E57" s="17"/>
-      <c r="F57" s="17"/>
-      <c r="G57" s="17"/>
-      <c r="H57" s="17"/>
-      <c r="I57" s="17"/>
-      <c r="J57" s="17"/>
-      <c r="K57" s="17"/>
-      <c r="L57" s="17"/>
-      <c r="M57" s="17"/>
-      <c r="N57" s="17"/>
-      <c r="O57" s="17"/>
-      <c r="P57" s="17"/>
-      <c r="Q57" s="17"/>
-      <c r="R57" s="17"/>
-      <c r="S57" s="17"/>
-      <c r="T57" s="17"/>
-      <c r="U57" s="17"/>
-      <c r="V57" s="17"/>
-      <c r="W57" s="17"/>
-    </row>
-    <row r="58" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A58" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="B58" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="C58" s="17"/>
-      <c r="D58" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="E58" s="17"/>
-      <c r="F58" s="17"/>
-      <c r="G58" s="17"/>
-      <c r="H58" s="17"/>
-      <c r="I58" s="17"/>
-      <c r="J58" s="17"/>
-      <c r="K58" s="17"/>
-      <c r="L58" s="17"/>
-      <c r="M58" s="17"/>
-      <c r="N58" s="17"/>
-      <c r="O58" s="17"/>
-      <c r="P58" s="17"/>
-      <c r="Q58" s="17"/>
-      <c r="R58" s="17"/>
-      <c r="S58" s="17"/>
-      <c r="T58" s="17"/>
-      <c r="U58" s="17"/>
-      <c r="V58" s="17"/>
-      <c r="W58" s="17"/>
-    </row>
-    <row r="59" spans="1:24" s="36" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A59" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="B59" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="C59" s="17"/>
-      <c r="D59" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="E59" s="17"/>
-      <c r="F59" s="17"/>
-      <c r="G59" s="17"/>
-      <c r="H59" s="17"/>
-      <c r="I59" s="17"/>
-      <c r="J59" s="17"/>
-      <c r="K59" s="17"/>
-      <c r="L59" s="17"/>
-      <c r="M59" s="17"/>
-      <c r="N59" s="17"/>
-      <c r="O59" s="17"/>
-      <c r="P59" s="17"/>
-      <c r="Q59" s="17"/>
-      <c r="R59" s="17"/>
-      <c r="S59" s="17"/>
-      <c r="T59" s="17"/>
-      <c r="U59" s="17"/>
-      <c r="V59" s="17"/>
-      <c r="W59" s="17"/>
-    </row>
-    <row r="60" spans="1:24" s="33" customFormat="1" ht="15.75" customHeight="1">
+    <row r="60" spans="1:24" ht="15.75" customHeight="1">
       <c r="A60" s="16" t="s">
         <v>63</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>129</v>
+        <v>66</v>
       </c>
       <c r="C60" s="17"/>
       <c r="D60" s="21" t="s">
         <v>132</v>
       </c>
       <c r="E60" s="17"/>
-      <c r="F60" s="17"/>
-      <c r="G60" s="17"/>
-      <c r="H60" s="17"/>
+      <c r="F60" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G60" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H60" s="17" t="s">
+        <v>19</v>
+      </c>
       <c r="I60" s="17"/>
       <c r="J60" s="17"/>
       <c r="K60" s="17"/>
-      <c r="L60" s="17"/>
-      <c r="M60" s="17"/>
-      <c r="N60" s="17"/>
+      <c r="L60" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="M60" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="N60" s="17" t="s">
+        <v>19</v>
+      </c>
       <c r="O60" s="17"/>
       <c r="P60" s="17"/>
       <c r="Q60" s="17"/>
@@ -4318,81 +4540,236 @@
     </row>
     <row r="61" spans="1:24" ht="15.75" customHeight="1">
       <c r="A61" s="16" t="s">
-        <v>110</v>
+        <v>63</v>
       </c>
       <c r="B61" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="C61" s="20"/>
+        <v>67</v>
+      </c>
+      <c r="C61" s="17"/>
       <c r="D61" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="E61" s="20"/>
-      <c r="F61" s="20"/>
-      <c r="G61" s="20"/>
-      <c r="H61" s="20"/>
-      <c r="I61" s="20"/>
-      <c r="J61" s="20"/>
-      <c r="K61" s="20"/>
-      <c r="L61" s="20"/>
-      <c r="M61" s="20"/>
-      <c r="N61" s="20"/>
-      <c r="O61" s="20"/>
-      <c r="P61" s="20"/>
-      <c r="Q61" s="20"/>
-      <c r="R61" s="20"/>
-      <c r="S61" s="20"/>
-      <c r="T61" s="20"/>
-      <c r="U61" s="20"/>
-      <c r="V61" s="20"/>
-      <c r="W61" s="20"/>
+      <c r="E61" s="17"/>
+      <c r="F61" s="17"/>
+      <c r="G61" s="17"/>
+      <c r="H61" s="17"/>
+      <c r="I61" s="17"/>
+      <c r="J61" s="17"/>
+      <c r="K61" s="17"/>
+      <c r="L61" s="17"/>
+      <c r="M61" s="17"/>
+      <c r="N61" s="17"/>
+      <c r="O61" s="17"/>
+      <c r="P61" s="17"/>
+      <c r="Q61" s="17"/>
+      <c r="R61" s="17"/>
+      <c r="S61" s="17"/>
+      <c r="T61" s="17"/>
+      <c r="U61" s="17"/>
+      <c r="V61" s="17"/>
+      <c r="W61" s="17"/>
     </row>
     <row r="62" spans="1:24" ht="15.75" customHeight="1">
       <c r="A62" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B62" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C62" s="17"/>
+      <c r="D62" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="E62" s="17"/>
+      <c r="F62" s="17"/>
+      <c r="G62" s="17"/>
+      <c r="H62" s="17"/>
+      <c r="I62" s="17"/>
+      <c r="J62" s="17"/>
+      <c r="K62" s="17"/>
+      <c r="L62" s="17"/>
+      <c r="M62" s="17"/>
+      <c r="N62" s="17"/>
+      <c r="O62" s="17"/>
+      <c r="P62" s="17"/>
+      <c r="Q62" s="17"/>
+      <c r="R62" s="17"/>
+      <c r="S62" s="17"/>
+      <c r="T62" s="17"/>
+      <c r="U62" s="17"/>
+      <c r="V62" s="17"/>
+      <c r="W62" s="17"/>
+    </row>
+    <row r="63" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A63" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B63" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C63" s="17"/>
+      <c r="D63" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="E63" s="17"/>
+      <c r="F63" s="17"/>
+      <c r="G63" s="17"/>
+      <c r="H63" s="17"/>
+      <c r="I63" s="17"/>
+      <c r="J63" s="17"/>
+      <c r="K63" s="17"/>
+      <c r="L63" s="17"/>
+      <c r="M63" s="17"/>
+      <c r="N63" s="17"/>
+      <c r="O63" s="17"/>
+      <c r="P63" s="17"/>
+      <c r="Q63" s="17"/>
+      <c r="R63" s="17"/>
+      <c r="S63" s="17"/>
+      <c r="T63" s="17"/>
+      <c r="U63" s="17"/>
+      <c r="V63" s="17"/>
+      <c r="W63" s="17"/>
+    </row>
+    <row r="64" spans="1:24" s="36" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A64" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B64" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C64" s="17"/>
+      <c r="D64" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="E64" s="17"/>
+      <c r="F64" s="17"/>
+      <c r="G64" s="17"/>
+      <c r="H64" s="17"/>
+      <c r="I64" s="17"/>
+      <c r="J64" s="17"/>
+      <c r="K64" s="17"/>
+      <c r="L64" s="17"/>
+      <c r="M64" s="17"/>
+      <c r="N64" s="17"/>
+      <c r="O64" s="17"/>
+      <c r="P64" s="17"/>
+      <c r="Q64" s="17"/>
+      <c r="R64" s="17"/>
+      <c r="S64" s="17"/>
+      <c r="T64" s="17"/>
+      <c r="U64" s="17"/>
+      <c r="V64" s="17"/>
+      <c r="W64" s="17"/>
+    </row>
+    <row r="65" spans="1:23" s="33" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A65" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B65" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="C65" s="17"/>
+      <c r="D65" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="E65" s="17"/>
+      <c r="F65" s="17"/>
+      <c r="G65" s="17"/>
+      <c r="H65" s="17"/>
+      <c r="I65" s="17"/>
+      <c r="J65" s="17"/>
+      <c r="K65" s="17"/>
+      <c r="L65" s="17"/>
+      <c r="M65" s="17"/>
+      <c r="N65" s="17"/>
+      <c r="O65" s="17"/>
+      <c r="P65" s="17"/>
+      <c r="Q65" s="17"/>
+      <c r="R65" s="17"/>
+      <c r="S65" s="17"/>
+      <c r="T65" s="17"/>
+      <c r="U65" s="17"/>
+      <c r="V65" s="17"/>
+      <c r="W65" s="17"/>
+    </row>
+    <row r="66" spans="1:23" ht="15.75" customHeight="1">
+      <c r="A66" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B66" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="C66" s="20"/>
+      <c r="D66" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="E66" s="20"/>
+      <c r="F66" s="20"/>
+      <c r="G66" s="20"/>
+      <c r="H66" s="20"/>
+      <c r="I66" s="20"/>
+      <c r="J66" s="20"/>
+      <c r="K66" s="20"/>
+      <c r="L66" s="20"/>
+      <c r="M66" s="20"/>
+      <c r="N66" s="20"/>
+      <c r="O66" s="20"/>
+      <c r="P66" s="20"/>
+      <c r="Q66" s="20"/>
+      <c r="R66" s="20"/>
+      <c r="S66" s="20"/>
+      <c r="T66" s="20"/>
+      <c r="U66" s="20"/>
+      <c r="V66" s="20"/>
+      <c r="W66" s="20"/>
+    </row>
+    <row r="67" spans="1:23" ht="15.75" customHeight="1">
+      <c r="A67" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="B62" s="16" t="s">
+      <c r="B67" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="C62" s="20"/>
-      <c r="D62" s="21" t="s">
+      <c r="C67" s="20"/>
+      <c r="D67" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="E62" s="30" t="s">
+      <c r="E67" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="F62" s="30"/>
-      <c r="G62" s="30" t="s">
+      <c r="F67" s="30"/>
+      <c r="G67" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="H62" s="30"/>
-      <c r="I62" s="30"/>
-      <c r="J62" s="30" t="s">
+      <c r="H67" s="30"/>
+      <c r="I67" s="30"/>
+      <c r="J67" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="K62" s="30" t="s">
+      <c r="K67" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="L62" s="30" t="s">
+      <c r="L67" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="M62" s="30" t="s">
+      <c r="M67" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="N62" s="30"/>
-      <c r="O62" s="30"/>
-      <c r="P62" s="30"/>
-      <c r="Q62" s="30"/>
-      <c r="R62" s="30"/>
-      <c r="S62" s="30"/>
-      <c r="T62" s="30"/>
-      <c r="U62" s="30"/>
-      <c r="V62" s="30"/>
-      <c r="W62" s="30"/>
+      <c r="N67" s="30"/>
+      <c r="O67" s="30"/>
+      <c r="P67" s="30"/>
+      <c r="Q67" s="30"/>
+      <c r="R67" s="30"/>
+      <c r="S67" s="30"/>
+      <c r="T67" s="30"/>
+      <c r="U67" s="30"/>
+      <c r="V67" s="30"/>
+      <c r="W67" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="X51:X52"/>
+    <mergeCell ref="X56:X57"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="J5:N5"/>
     <mergeCell ref="P5:V5"/>

</xml_diff>

<commit_message>
Lisää urakoitsijalle oikeuksia välitavoitteisiin
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -1,16 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="49980" windowHeight="27880" tabRatio="500"/>
+    <workbookView xWindow="1100" yWindow="20" windowWidth="34900" windowHeight="17900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
     <sheet name="Roolit" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
+  <customWorkbookViews>
+    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
+  </customWorkbookViews>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -23,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="157">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -460,9 +463,6 @@
     <t>R+,valmis+</t>
   </si>
   <si>
-    <t>R,valmis</t>
-  </si>
-  <si>
     <t>valmis tarkoittaa välitavoitteen merkitsemistä valmiiksi</t>
   </si>
   <si>
@@ -491,6 +491,12 @@
   </si>
   <si>
     <t>Laaduntarkastusraportti</t>
+  </si>
+  <si>
+    <t>R+,W+,valmis+</t>
+  </si>
+  <si>
+    <t>R,W,valmis</t>
   </si>
 </sst>
 </file>
@@ -922,6 +928,74 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" diskRevisions="1" revisionId="3" version="2">
+  <header guid="{9913DD30-08DC-DF4C-B2D5-13B399C3569F}" dateTime="2016-09-06T09:10:23" maxSheetId="3" userName="Tatu Tarvainen" r:id="rId1">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" dateTime="2016-09-06T09:14:56" maxSheetId="3" userName="Tatu Tarvainen" r:id="rId2" minRId="1" maxRId="3">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+</headers>
+</file>
+
+<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
+</file>
+
+<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1" sId="1">
+    <oc r="P24" t="inlineStr">
+      <is>
+        <t>R+,valmis+</t>
+      </is>
+    </oc>
+    <nc r="P24" t="inlineStr">
+      <is>
+        <t>R+,W+,valmis+</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="2" sId="1">
+    <oc r="Q24" t="inlineStr">
+      <is>
+        <t>R,valmis</t>
+      </is>
+    </oc>
+    <nc r="Q24" t="inlineStr">
+      <is>
+        <t>R,W,valmis</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="3" sId="1">
+    <oc r="S24" t="inlineStr">
+      <is>
+        <t>R,valmis</t>
+      </is>
+    </oc>
+    <nc r="S24" t="inlineStr">
+      <is>
+        <t>R,W,valmis</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
+  <userInfo guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" name="Tatu Tarvainen" id="-130145201" dateTime="2016-09-06T09:10:23"/>
+</users>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1249,10 +1323,10 @@
   <dimension ref="A1:X68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="K16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B37" sqref="B37"/>
+      <selection pane="bottomRight" activeCell="S24" sqref="S24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -2431,11 +2505,11 @@
       </c>
       <c r="C24" s="21"/>
       <c r="D24" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="E24" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="E24" s="17" t="s">
-        <v>148</v>
-      </c>
       <c r="F24" s="17" t="s">
         <v>133</v>
       </c>
@@ -2449,10 +2523,10 @@
         <v>133</v>
       </c>
       <c r="J24" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="K24" s="21" t="s">
         <v>147</v>
-      </c>
-      <c r="K24" s="21" t="s">
-        <v>148</v>
       </c>
       <c r="L24" s="21" t="s">
         <v>133</v>
@@ -2465,16 +2539,16 @@
       </c>
       <c r="O24" s="21"/>
       <c r="P24" s="21" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
       <c r="Q24" s="21" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="R24" s="21" t="s">
         <v>144</v>
       </c>
       <c r="S24" s="21" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="T24" s="17" t="s">
         <v>137</v>
@@ -2483,7 +2557,7 @@
       <c r="V24" s="21"/>
       <c r="W24" s="21"/>
       <c r="X24" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="25" spans="1:24" ht="15.75" customHeight="1">
@@ -2755,7 +2829,7 @@
       </c>
       <c r="C30" s="21"/>
       <c r="D30" s="17" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E30" s="17" t="s">
         <v>136</v>
@@ -3223,7 +3297,7 @@
         <v>43</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C38" s="21"/>
       <c r="D38" s="21" t="s">
@@ -4041,7 +4115,7 @@
         <v>43</v>
       </c>
       <c r="B52" s="26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C52" s="21"/>
       <c r="D52" s="21" t="s">
@@ -4103,7 +4177,7 @@
         <v>43</v>
       </c>
       <c r="B53" s="26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C53" s="21"/>
       <c r="D53" s="21" t="s">
@@ -4165,7 +4239,7 @@
         <v>43</v>
       </c>
       <c r="B54" s="26" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C54" s="21"/>
       <c r="D54" s="21" t="s">
@@ -4229,7 +4303,7 @@
         <v>43</v>
       </c>
       <c r="B55" s="26" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C55" s="21"/>
       <c r="D55" s="21" t="s">
@@ -4293,7 +4367,7 @@
         <v>43</v>
       </c>
       <c r="B56" s="26" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C56" s="21"/>
       <c r="D56" s="17" t="s">
@@ -4845,6 +4919,13 @@
       <c r="W68" s="30"/>
     </row>
   </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
+      <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+  </customSheetViews>
   <mergeCells count="6">
     <mergeCell ref="X57:X58"/>
     <mergeCell ref="C5:H5"/>
@@ -5187,6 +5268,12 @@
       </c>
     </row>
   </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
+      <selection activeCell="C7" sqref="C7"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+  </customSheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
Salli urak. vastuuhlön syöttää erilliskustannuksia
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="20" windowWidth="34900" windowHeight="17900" tabRatio="500"/>
+    <workbookView xWindow="1100" yWindow="20" windowWidth="39220" windowHeight="24820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" xWindow="55" yWindow="55" windowWidth="1961" windowHeight="1187" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
     <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
@@ -730,7 +731,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -802,6 +803,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="115">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -931,7 +938,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" diskRevisions="1" revisionId="3" version="2">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{E0850D7E-A93F-EF44-B46A-3BEA4D7DBEDB}" diskRevisions="1" revisionId="6" version="4">
   <header guid="{9913DD30-08DC-DF4C-B2D5-13B399C3569F}" dateTime="2016-09-06T09:10:23" maxSheetId="3" userName="Tatu Tarvainen" r:id="rId1">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -939,6 +946,18 @@
     </sheetIdMap>
   </header>
   <header guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" dateTime="2016-09-06T09:14:56" maxSheetId="3" userName="Tatu Tarvainen" r:id="rId2" minRId="1" maxRId="3">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{771903DC-B093-EC43-82F7-AFD5957CF1ED}" dateTime="2016-09-06T13:03:01" maxSheetId="3" userName="Jarno Väyrynen" r:id="rId3" minRId="4">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{E0850D7E-A93F-EF44-B46A-3BEA4D7DBEDB}" dateTime="2016-09-06T13:07:55" maxSheetId="3" userName="Jarno Väyrynen" r:id="rId4" minRId="5" maxRId="6">
     <sheetIdMap count="2">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -992,9 +1011,86 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="4" sId="1">
+    <oc r="Q18" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </oc>
+    <nc r="Q18" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="5" sId="1" odxf="1" dxf="1">
+    <nc r="O1" t="inlineStr">
+      <is>
+        <t>R = lukuoikeus, R,W = luku- ja kirjoitusoikeus, tyhjä = ei näe osiota, muut erikoisoikeuksia, * R/W perässä tarkoittaa kaikkiin urakoihin, + tarkoittaa oman organisaation urakoihin</t>
+      </is>
+    </nc>
+    <odxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </odxf>
+    <ndxf>
+      <font>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </ndxf>
+  </rcc>
+  <rcc rId="6" sId="1" odxf="1" dxf="1">
+    <nc r="O1" t="inlineStr">
+      <is>
+        <t>R = lukuoikeus, R,W = luku- ja kirjoitusoikeus, tyhjä = ei näe osiota, muut erikoisoikeuksia, * R/W perässä tarkoittaa kaikkiin urakoihin, + tarkoittaa oman organisaation urakoihin</t>
+      </is>
+    </nc>
+    <odxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </odxf>
+    <ndxf>
+      <font>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </ndxf>
+  </rcc>
+  <rfmt sheetId="1" sqref="C1:N1">
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+  </rfmt>
+  <rcv guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" action="delete"/>
+  <rcv guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="2">
   <userInfo guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" name="Tatu Tarvainen" id="-130145201" dateTime="2016-09-06T09:10:23"/>
+  <userInfo guid="{E0850D7E-A93F-EF44-B46A-3BEA4D7DBEDB}" name="Jarno Väyrynen" id="-589116405" dateTime="2016-09-06T12:54:09"/>
 </users>
 </file>
 
@@ -1323,10 +1419,10 @@
   <dimension ref="A1:X68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="K16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="S24" sqref="S24"/>
+      <selection pane="bottomRight" activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1356,25 +1452,25 @@
     <col min="24" max="24" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" customHeight="1">
+    <row r="1" spans="1:24" ht="24" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="43" t="s">
         <v>131</v>
       </c>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
     </row>
     <row r="2" spans="1:24" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
@@ -2156,7 +2252,7 @@
         <v>137</v>
       </c>
       <c r="Q18" s="17" t="s">
-        <v>17</v>
+        <v>114</v>
       </c>
       <c r="R18" s="21"/>
       <c r="S18" s="21"/>
@@ -4920,6 +5016,11 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="170">
+      <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C16" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="O2" sqref="O2"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
     <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
       <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
@@ -5269,6 +5370,10 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
+      <selection activeCell="C7" sqref="C7"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
     <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
       <selection activeCell="C7" sqref="C7"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Excel: ELY Laadunvalvoja vain nimettyihin urakoihin
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="20" windowWidth="39220" windowHeight="24820" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="38400" windowHeight="21600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
-    <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" xWindow="55" yWindow="55" windowWidth="1961" windowHeight="1187" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
+    <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
     <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1029" uniqueCount="157">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -614,8 +614,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="115">
+  <cellStyleXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -802,15 +810,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="115">
+  <cellStyles count="123">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -868,6 +876,10 @@
     <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -925,6 +937,10 @@
     <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -938,7 +954,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{E0850D7E-A93F-EF44-B46A-3BEA4D7DBEDB}" diskRevisions="1" revisionId="6" version="4">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{0407E191-78DA-F349-B5E5-8AE1BC03A29E}" diskRevisions="1" revisionId="57" version="5">
   <header guid="{9913DD30-08DC-DF4C-B2D5-13B399C3569F}" dateTime="2016-09-06T09:10:23" maxSheetId="3" userName="Tatu Tarvainen" r:id="rId1">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -958,6 +974,12 @@
     </sheetIdMap>
   </header>
   <header guid="{E0850D7E-A93F-EF44-B46A-3BEA4D7DBEDB}" dateTime="2016-09-06T13:07:55" maxSheetId="3" userName="Jarno Väyrynen" r:id="rId4" minRId="5" maxRId="6">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{0407E191-78DA-F349-B5E5-8AE1BC03A29E}" dateTime="2016-09-08T16:15:41" maxSheetId="3" userName="Jarno Väyrynen" r:id="rId5" minRId="7" maxRId="57">
     <sheetIdMap count="2">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -1087,11 +1109,564 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog5.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="7" sId="1">
+    <oc r="E59" t="inlineStr">
+      <is>
+        <t>R*,W</t>
+      </is>
+    </oc>
+    <nc r="E59" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="8" sId="1">
+    <nc r="F44" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="9" sId="1" odxf="1" dxf="1">
+    <nc r="F25" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+    <odxf/>
+    <ndxf/>
+  </rcc>
+  <rcc rId="10" sId="1">
+    <oc r="G20" t="inlineStr">
+      <is>
+        <t>R*,W*</t>
+      </is>
+    </oc>
+    <nc r="G20" t="inlineStr">
+      <is>
+        <t>R*,W+</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="11" sId="1">
+    <oc r="G21" t="inlineStr">
+      <is>
+        <t>R*,W*</t>
+      </is>
+    </oc>
+    <nc r="G21" t="inlineStr">
+      <is>
+        <t>R*,W+</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="12" sId="1">
+    <oc r="G33" t="inlineStr">
+      <is>
+        <t>R*,W*</t>
+      </is>
+    </oc>
+    <nc r="G33" t="inlineStr">
+      <is>
+        <t>R*,W+</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="13" sId="1">
+    <nc r="G49" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="14" sId="1">
+    <oc r="J26" t="inlineStr">
+      <is>
+        <t>R*,W*</t>
+      </is>
+    </oc>
+    <nc r="J26" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="15" sId="1">
+    <oc r="K26" t="inlineStr">
+      <is>
+        <t>R*,W</t>
+      </is>
+    </oc>
+    <nc r="K26" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="16" sId="1">
+    <oc r="K59" t="inlineStr">
+      <is>
+        <t>R*,W</t>
+      </is>
+    </oc>
+    <nc r="K59" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="17" sId="1">
+    <nc r="M44" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="18" sId="1">
+    <nc r="M25" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="19" sId="1">
+    <nc r="O49" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="20" sId="1">
+    <nc r="O42" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="21" sId="1">
+    <nc r="R44" t="inlineStr">
+      <is>
+        <t>R+</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="22" sId="1" odxf="1" dxf="1">
+    <nc r="T26" t="inlineStr">
+      <is>
+        <t>R+</t>
+      </is>
+    </nc>
+    <odxf/>
+    <ndxf/>
+  </rcc>
+  <rcc rId="23" sId="1">
+    <nc r="T34" t="inlineStr">
+      <is>
+        <t>R+</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="24" sId="1">
+    <nc r="T51" t="inlineStr">
+      <is>
+        <t>R+</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="25" sId="1">
+    <nc r="T52" t="inlineStr">
+      <is>
+        <t>R+</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="26" sId="1">
+    <nc r="T53" t="inlineStr">
+      <is>
+        <t>R+</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="27" sId="1">
+    <oc r="L7" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </oc>
+    <nc r="L7" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="28" sId="1">
+    <oc r="L11" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </oc>
+    <nc r="L11" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="29" sId="1">
+    <oc r="L12" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </oc>
+    <nc r="L12" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="30" sId="1">
+    <oc r="L16" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </oc>
+    <nc r="L16" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="31" sId="1">
+    <oc r="L17" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </oc>
+    <nc r="L17" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="32" sId="1">
+    <oc r="L19" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </oc>
+    <nc r="L19" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="33" sId="1">
+    <oc r="L20" t="inlineStr">
+      <is>
+        <t>R*,W+</t>
+      </is>
+    </oc>
+    <nc r="L20" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="34" sId="1">
+    <oc r="L21" t="inlineStr">
+      <is>
+        <t>R*,W+</t>
+      </is>
+    </oc>
+    <nc r="L21" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="35" sId="1">
+    <oc r="L22" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </oc>
+    <nc r="L22" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="36" sId="1">
+    <oc r="L23" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </oc>
+    <nc r="L23" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="37" sId="1">
+    <oc r="L24" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </oc>
+    <nc r="L24" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="38" sId="1">
+    <oc r="L28" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </oc>
+    <nc r="L28" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="39" sId="1">
+    <oc r="L33" t="inlineStr">
+      <is>
+        <t>R*,W+</t>
+      </is>
+    </oc>
+    <nc r="L33" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="40" sId="1">
+    <oc r="L36" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </oc>
+    <nc r="L36" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="41" sId="1">
+    <oc r="L37" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </oc>
+    <nc r="L37" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="42" sId="1">
+    <oc r="L38" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </oc>
+    <nc r="L38" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="43" sId="1">
+    <oc r="L39" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </oc>
+    <nc r="L39" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="44" sId="1">
+    <oc r="L40" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </oc>
+    <nc r="L40" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="45" sId="1">
+    <oc r="L41" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </oc>
+    <nc r="L41" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="46" sId="1">
+    <oc r="L42" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </oc>
+    <nc r="L42" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="47" sId="1">
+    <oc r="L43" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </oc>
+    <nc r="L43" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="48" sId="1">
+    <nc r="L49" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="49" sId="1">
+    <oc r="L50" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </oc>
+    <nc r="L50" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="50" sId="1">
+    <oc r="L51" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </oc>
+    <nc r="L51" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="51" sId="1">
+    <oc r="L52" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </oc>
+    <nc r="L52" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="52" sId="1">
+    <oc r="L53" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </oc>
+    <nc r="L53" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="53" sId="1">
+    <oc r="L54" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </oc>
+    <nc r="L54" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="54" sId="1">
+    <oc r="L55" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </oc>
+    <nc r="L55" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="55" sId="1">
+    <oc r="L57" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </oc>
+    <nc r="L57" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="56" sId="1">
+    <oc r="L58" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </oc>
+    <nc r="L58" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="57" sId="1">
+    <oc r="L59" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </oc>
+    <nc r="L59" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" action="delete"/>
+  <rcv guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="3">
   <userInfo guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" name="Tatu Tarvainen" id="-130145201" dateTime="2016-09-06T09:10:23"/>
   <userInfo guid="{E0850D7E-A93F-EF44-B46A-3BEA4D7DBEDB}" name="Jarno Väyrynen" id="-589116405" dateTime="2016-09-06T12:54:09"/>
-  <userInfo guid="{E0850D7E-A93F-EF44-B46A-3BEA4D7DBEDB}" name="Jarno Väyrynen" id="-589108428" dateTime="2016-09-08T15:33:24"/>
+  <userInfo guid="{0407E191-78DA-F349-B5E5-8AE1BC03A29E}" name="Jarno Väyrynen" id="-589108428" dateTime="2016-09-08T15:33:24"/>
 </users>
 </file>
 
@@ -1419,11 +1994,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="2" ySplit="6" topLeftCell="E7" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="O2" sqref="O2"/>
+      <selection pane="bottomRight" activeCell="L57" sqref="L57:L59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1458,25 +2033,25 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="42" t="s">
         <v>131</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
     </row>
     <row r="2" spans="1:24" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="44" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="40"/>
@@ -1640,7 +2215,7 @@
         <v>136</v>
       </c>
       <c r="L7" s="17" t="s">
-        <v>133</v>
+        <v>17</v>
       </c>
       <c r="M7" s="21" t="s">
         <v>133</v>
@@ -1858,7 +2433,7 @@
         <v>136</v>
       </c>
       <c r="L11" s="17" t="s">
-        <v>133</v>
+        <v>17</v>
       </c>
       <c r="M11" s="21" t="s">
         <v>133</v>
@@ -1920,7 +2495,7 @@
         <v>136</v>
       </c>
       <c r="L12" s="17" t="s">
-        <v>133</v>
+        <v>17</v>
       </c>
       <c r="M12" s="21" t="s">
         <v>133</v>
@@ -2126,7 +2701,7 @@
         <v>133</v>
       </c>
       <c r="L16" s="17" t="s">
-        <v>133</v>
+        <v>17</v>
       </c>
       <c r="M16" s="21" t="s">
         <v>133</v>
@@ -2188,7 +2763,7 @@
         <v>133</v>
       </c>
       <c r="L17" s="17" t="s">
-        <v>133</v>
+        <v>17</v>
       </c>
       <c r="M17" s="21" t="s">
         <v>133</v>
@@ -2298,7 +2873,7 @@
         <v>133</v>
       </c>
       <c r="L19" s="17" t="s">
-        <v>133</v>
+        <v>17</v>
       </c>
       <c r="M19" s="21" t="s">
         <v>133</v>
@@ -2345,7 +2920,7 @@
         <v>133</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="H20" s="17" t="s">
         <v>133</v>
@@ -2360,7 +2935,7 @@
         <v>136</v>
       </c>
       <c r="L20" s="21" t="s">
-        <v>135</v>
+        <v>114</v>
       </c>
       <c r="M20" s="21" t="s">
         <v>133</v>
@@ -2411,7 +2986,7 @@
         <v>133</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="H21" s="17" t="s">
         <v>133</v>
@@ -2426,7 +3001,7 @@
         <v>136</v>
       </c>
       <c r="L21" s="21" t="s">
-        <v>135</v>
+        <v>114</v>
       </c>
       <c r="M21" s="21" t="s">
         <v>133</v>
@@ -2494,7 +3069,7 @@
         <v>139</v>
       </c>
       <c r="L22" s="21" t="s">
-        <v>133</v>
+        <v>17</v>
       </c>
       <c r="M22" s="21" t="s">
         <v>133</v>
@@ -2560,7 +3135,7 @@
         <v>136</v>
       </c>
       <c r="L23" s="21" t="s">
-        <v>133</v>
+        <v>17</v>
       </c>
       <c r="M23" s="21" t="s">
         <v>133</v>
@@ -2626,7 +3201,7 @@
         <v>147</v>
       </c>
       <c r="L24" s="21" t="s">
-        <v>133</v>
+        <v>17</v>
       </c>
       <c r="M24" s="21" t="s">
         <v>133</v>
@@ -2671,7 +3246,9 @@
       <c r="E25" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="F25" s="21"/>
+      <c r="F25" s="17" t="s">
+        <v>133</v>
+      </c>
       <c r="G25" s="21"/>
       <c r="H25" s="21"/>
       <c r="I25" s="21" t="s">
@@ -2684,7 +3261,9 @@
         <v>136</v>
       </c>
       <c r="L25" s="21"/>
-      <c r="M25" s="21"/>
+      <c r="M25" s="21" t="s">
+        <v>133</v>
+      </c>
       <c r="N25" s="21"/>
       <c r="O25" s="21" t="s">
         <v>135</v>
@@ -2728,10 +3307,10 @@
       <c r="H26" s="21"/>
       <c r="I26" s="21"/>
       <c r="J26" s="17" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K26" s="21" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="L26" s="21"/>
       <c r="M26" s="21" t="s">
@@ -2747,7 +3326,9 @@
       </c>
       <c r="R26" s="21"/>
       <c r="S26" s="21"/>
-      <c r="T26" s="21"/>
+      <c r="T26" s="17" t="s">
+        <v>137</v>
+      </c>
       <c r="U26" s="21"/>
       <c r="V26" s="21"/>
       <c r="W26" s="21"/>
@@ -2826,7 +3407,7 @@
         <v>136</v>
       </c>
       <c r="L28" s="21" t="s">
-        <v>133</v>
+        <v>17</v>
       </c>
       <c r="M28" s="21" t="s">
         <v>133</v>
@@ -3111,7 +3692,7 @@
         <v>133</v>
       </c>
       <c r="G33" s="21" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="H33" s="21" t="s">
         <v>133</v>
@@ -3126,7 +3707,7 @@
         <v>139</v>
       </c>
       <c r="L33" s="21" t="s">
-        <v>135</v>
+        <v>114</v>
       </c>
       <c r="M33" s="21" t="s">
         <v>133</v>
@@ -3201,7 +3782,9 @@
       </c>
       <c r="R34" s="21"/>
       <c r="S34" s="21"/>
-      <c r="T34" s="21"/>
+      <c r="T34" s="21" t="s">
+        <v>137</v>
+      </c>
       <c r="U34" s="21"/>
       <c r="V34" s="21"/>
       <c r="W34" s="21"/>
@@ -3290,7 +3873,7 @@
         <v>133</v>
       </c>
       <c r="L36" s="21" t="s">
-        <v>133</v>
+        <v>17</v>
       </c>
       <c r="M36" s="21" t="s">
         <v>133</v>
@@ -3356,7 +3939,7 @@
         <v>133</v>
       </c>
       <c r="L37" s="21" t="s">
-        <v>133</v>
+        <v>17</v>
       </c>
       <c r="M37" s="21" t="s">
         <v>133</v>
@@ -3422,7 +4005,7 @@
         <v>133</v>
       </c>
       <c r="L38" s="21" t="s">
-        <v>133</v>
+        <v>17</v>
       </c>
       <c r="M38" s="21" t="s">
         <v>133</v>
@@ -3488,7 +4071,7 @@
         <v>133</v>
       </c>
       <c r="L39" s="21" t="s">
-        <v>133</v>
+        <v>17</v>
       </c>
       <c r="M39" s="21" t="s">
         <v>133</v>
@@ -3554,7 +4137,7 @@
         <v>133</v>
       </c>
       <c r="L40" s="21" t="s">
-        <v>133</v>
+        <v>17</v>
       </c>
       <c r="M40" s="21" t="s">
         <v>133</v>
@@ -3620,7 +4203,7 @@
         <v>133</v>
       </c>
       <c r="L41" s="21" t="s">
-        <v>133</v>
+        <v>17</v>
       </c>
       <c r="M41" s="21" t="s">
         <v>133</v>
@@ -3686,13 +4269,15 @@
         <v>133</v>
       </c>
       <c r="L42" s="21" t="s">
-        <v>133</v>
+        <v>17</v>
       </c>
       <c r="M42" s="21" t="s">
         <v>133</v>
       </c>
       <c r="N42" s="21"/>
-      <c r="O42" s="21"/>
+      <c r="O42" s="21" t="s">
+        <v>133</v>
+      </c>
       <c r="P42" s="21" t="s">
         <v>137</v>
       </c>
@@ -3746,7 +4331,7 @@
         <v>133</v>
       </c>
       <c r="L43" s="21" t="s">
-        <v>133</v>
+        <v>17</v>
       </c>
       <c r="M43" s="21" t="s">
         <v>133</v>
@@ -3793,7 +4378,9 @@
       <c r="E44" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="F44" s="21"/>
+      <c r="F44" s="21" t="s">
+        <v>133</v>
+      </c>
       <c r="G44" s="21"/>
       <c r="H44" s="21"/>
       <c r="I44" s="21" t="s">
@@ -3806,7 +4393,9 @@
         <v>133</v>
       </c>
       <c r="L44" s="21"/>
-      <c r="M44" s="21"/>
+      <c r="M44" s="21" t="s">
+        <v>133</v>
+      </c>
       <c r="N44" s="21"/>
       <c r="O44" s="21" t="s">
         <v>133</v>
@@ -3817,7 +4406,9 @@
       <c r="Q44" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="R44" s="21"/>
+      <c r="R44" s="21" t="s">
+        <v>137</v>
+      </c>
       <c r="S44" s="21"/>
       <c r="T44" s="21" t="s">
         <v>137</v>
@@ -4040,7 +4631,9 @@
       <c r="F49" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="G49" s="21"/>
+      <c r="G49" s="21" t="s">
+        <v>133</v>
+      </c>
       <c r="H49" s="21" t="s">
         <v>133</v>
       </c>
@@ -4053,12 +4646,16 @@
       <c r="K49" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="L49" s="21"/>
+      <c r="L49" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="M49" s="21" t="s">
         <v>133</v>
       </c>
       <c r="N49" s="21"/>
-      <c r="O49" s="21"/>
+      <c r="O49" s="21" t="s">
+        <v>133</v>
+      </c>
       <c r="P49" s="21" t="s">
         <v>137</v>
       </c>
@@ -4112,7 +4709,7 @@
         <v>133</v>
       </c>
       <c r="L50" s="21" t="s">
-        <v>133</v>
+        <v>17</v>
       </c>
       <c r="M50" s="21" t="s">
         <v>133</v>
@@ -4178,7 +4775,7 @@
         <v>133</v>
       </c>
       <c r="L51" s="21" t="s">
-        <v>133</v>
+        <v>17</v>
       </c>
       <c r="M51" s="21" t="s">
         <v>133</v>
@@ -4201,7 +4798,9 @@
       <c r="S51" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="T51" s="21"/>
+      <c r="T51" s="21" t="s">
+        <v>137</v>
+      </c>
       <c r="U51" s="21"/>
       <c r="V51" s="21"/>
       <c r="W51" s="21"/>
@@ -4240,7 +4839,7 @@
         <v>133</v>
       </c>
       <c r="L52" s="21" t="s">
-        <v>133</v>
+        <v>17</v>
       </c>
       <c r="M52" s="21" t="s">
         <v>133</v>
@@ -4263,7 +4862,9 @@
       <c r="S52" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="T52" s="21"/>
+      <c r="T52" s="21" t="s">
+        <v>137</v>
+      </c>
       <c r="U52" s="21"/>
       <c r="V52" s="21"/>
       <c r="W52" s="21"/>
@@ -4302,7 +4903,7 @@
         <v>133</v>
       </c>
       <c r="L53" s="21" t="s">
-        <v>133</v>
+        <v>17</v>
       </c>
       <c r="M53" s="21" t="s">
         <v>133</v>
@@ -4325,7 +4926,9 @@
       <c r="S53" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="T53" s="21"/>
+      <c r="T53" s="21" t="s">
+        <v>137</v>
+      </c>
       <c r="U53" s="21"/>
       <c r="V53" s="21"/>
       <c r="W53" s="21"/>
@@ -4364,7 +4967,7 @@
         <v>133</v>
       </c>
       <c r="L54" s="21" t="s">
-        <v>133</v>
+        <v>17</v>
       </c>
       <c r="M54" s="21" t="s">
         <v>133</v>
@@ -4428,7 +5031,7 @@
         <v>133</v>
       </c>
       <c r="L55" s="21" t="s">
-        <v>133</v>
+        <v>17</v>
       </c>
       <c r="M55" s="21" t="s">
         <v>133</v>
@@ -4538,7 +5141,7 @@
         <v>133</v>
       </c>
       <c r="L57" s="21" t="s">
-        <v>133</v>
+        <v>17</v>
       </c>
       <c r="M57" s="21" t="s">
         <v>133</v>
@@ -4608,7 +5211,7 @@
         <v>133</v>
       </c>
       <c r="L58" s="21" t="s">
-        <v>133</v>
+        <v>17</v>
       </c>
       <c r="M58" s="21" t="s">
         <v>133</v>
@@ -4655,7 +5258,7 @@
         <v>132</v>
       </c>
       <c r="E59" s="17" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F59" s="21" t="s">
         <v>133</v>
@@ -4673,10 +5276,10 @@
         <v>132</v>
       </c>
       <c r="K59" s="21" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="L59" s="21" t="s">
-        <v>133</v>
+        <v>17</v>
       </c>
       <c r="M59" s="21" t="s">
         <v>133</v>
@@ -5017,9 +5620,9 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="170">
-      <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C16" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="O2" sqref="O2"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
+      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="E7" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="L57" sqref="L57:L59"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
     <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">

</xml_diff>

<commit_message>
HAR-3051 Lisää urakoitsijarooleille oikeuksia
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-900" windowWidth="38400" windowHeight="22040" tabRatio="500"/>
+    <workbookView xWindow="25640" yWindow="80" windowWidth="25540" windowHeight="28700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -12,8 +12,8 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
     <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1029" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="157">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -614,8 +614,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="123">
+  <cellStyleXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -818,7 +820,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="123">
+  <cellStyles count="125">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -880,6 +882,7 @@
     <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -941,6 +944,7 @@
     <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -954,7 +958,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{96A7966C-8B82-C646-99D9-18DB41B4F602}" diskRevisions="1" revisionId="59" version="7">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{F8907045-3B30-0A43-A905-F167D27F9989}" diskRevisions="1" revisionId="63" version="8">
   <header guid="{9913DD30-08DC-DF4C-B2D5-13B399C3569F}" dateTime="2016-09-06T09:10:23" maxSheetId="3" userName="Tatu Tarvainen" r:id="rId1">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -997,6 +1001,12 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{F8907045-3B30-0A43-A905-F167D27F9989}" dateTime="2016-09-27T15:32:39" maxSheetId="3" userName="Jarno Väyrynen" r:id="rId8" minRId="60" maxRId="63">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -1708,11 +1718,45 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog8.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="60" sId="1">
+    <nc r="U20" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="61" sId="1">
+    <nc r="T25" t="inlineStr">
+      <is>
+        <t>R+</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="62" sId="1">
+    <nc r="T45" t="inlineStr">
+      <is>
+        <t>R+</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="63" sId="1">
+    <nc r="U37" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="3">
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="4">
   <userInfo guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" name="Tatu Tarvainen" id="-130145201" dateTime="2016-09-06T09:10:23"/>
   <userInfo guid="{E0850D7E-A93F-EF44-B46A-3BEA4D7DBEDB}" name="Jarno Väyrynen" id="-589116405" dateTime="2016-09-06T12:54:09"/>
   <userInfo guid="{0407E191-78DA-F349-B5E5-8AE1BC03A29E}" name="Jarno Väyrynen" id="-589108428" dateTime="2016-09-08T15:33:24"/>
+  <userInfo guid="{F8907045-3B30-0A43-A905-F167D27F9989}" name="Jarno Väyrynen" id="-589157736" dateTime="2016-09-27T15:27:41"/>
 </users>
 </file>
 
@@ -2041,10 +2085,10 @@
   <dimension ref="A1:X68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C8" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="O8" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="M4" sqref="M4"/>
+      <selection pane="bottomRight" activeCell="U37" sqref="U37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -3007,7 +3051,9 @@
       <c r="T20" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="U20" s="17"/>
+      <c r="U20" s="17" t="s">
+        <v>17</v>
+      </c>
       <c r="V20" s="21" t="s">
         <v>17</v>
       </c>
@@ -3324,7 +3370,9 @@
         <v>136</v>
       </c>
       <c r="S25" s="27"/>
-      <c r="T25" s="21"/>
+      <c r="T25" s="21" t="s">
+        <v>136</v>
+      </c>
       <c r="U25" s="21"/>
       <c r="V25" s="21" t="s">
         <v>114</v>
@@ -4011,7 +4059,9 @@
       <c r="T37" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="U37" s="21"/>
+      <c r="U37" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="V37" s="21" t="s">
         <v>17</v>
       </c>
@@ -4510,7 +4560,9 @@
       </c>
       <c r="R45" s="21"/>
       <c r="S45" s="21"/>
-      <c r="T45" s="21"/>
+      <c r="T45" s="21" t="s">
+        <v>136</v>
+      </c>
       <c r="U45" s="21"/>
       <c r="V45" s="21"/>
       <c r="W45" s="21"/>
@@ -5666,14 +5718,14 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
+      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="E7" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="L57" sqref="L57:L59"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
     <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
       <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
-      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="E7" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="L57" sqref="L57:L59"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>
@@ -6020,11 +6072,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
       <selection activeCell="C7" sqref="C7"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
+    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
       <selection activeCell="C7" sqref="C7"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>

</xml_diff>

<commit_message>
Lisää JVH:lle uusi oikeus: TM-valmis
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarihan/Desktop/Harja/harja/resources/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="25640" yWindow="80" windowWidth="25540" windowHeight="28700" tabRatio="500"/>
+    <workbookView xWindow="25640" yWindow="460" windowWidth="25540" windowHeight="27200" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -12,22 +17,23 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="1277" windowHeight="1187" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
-    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="158">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -498,6 +504,9 @@
   </si>
   <si>
     <t>R = lukuoikeus nimettyihin urakoihin, R,W = luku- ja kirjoitusoikeus nimettyihin urakoihin, W+ kirjoitusoikeus oman organisaation urakoihin, W* kirjoitusoikeus kaikkiin urakoihin, tyhjä = ei näe osiota, muut erikoisoikeuksia</t>
+  </si>
+  <si>
+    <t>R*,W*,TM-valmis</t>
   </si>
 </sst>
 </file>
@@ -958,13 +967,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{F8907045-3B30-0A43-A905-F167D27F9989}" diskRevisions="1" revisionId="63" version="8">
-  <header guid="{9913DD30-08DC-DF4C-B2D5-13B399C3569F}" dateTime="2016-09-06T09:10:23" maxSheetId="3" userName="Tatu Tarvainen" r:id="rId1">
-    <sheetIdMap count="2">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-    </sheetIdMap>
-  </header>
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{FC69AAD3-0412-1847-89C5-E3EAD8A67C1F}" diskRevisions="1" revisionId="64" version="9">
   <header guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" dateTime="2016-09-06T09:14:56" maxSheetId="3" userName="Tatu Tarvainen" r:id="rId2" minRId="1" maxRId="3">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1007,11 +1010,13 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{FC69AAD3-0412-1847-89C5-E3EAD8A67C1F}" dateTime="2016-10-11T11:52:42" maxSheetId="3" userName="Microsoft Office User" r:id="rId9" minRId="64">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
-</file>
-
-<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
 </file>
 
 <file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1751,7 +1756,25 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/revisionLog9.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="64" sId="1">
+    <oc r="D28" t="inlineStr">
+      <is>
+        <t>R*,W*</t>
+      </is>
+    </oc>
+    <nc r="D28" t="inlineStr">
+      <is>
+        <t>R*,W*,TM-valmis</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="4">
   <userInfo guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" name="Tatu Tarvainen" id="-130145201" dateTime="2016-09-06T09:10:23"/>
   <userInfo guid="{E0850D7E-A93F-EF44-B46A-3BEA4D7DBEDB}" name="Jarno Väyrynen" id="-589116405" dateTime="2016-09-06T12:54:09"/>
@@ -2084,14 +2107,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="O8" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <pane xSplit="2" ySplit="6" topLeftCell="C12" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="U37" sqref="U37"/>
+      <selection pane="bottomRight" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.5" bestFit="1" customWidth="1"/>
@@ -2118,7 +2141,7 @@
     <col min="24" max="24" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="24" customHeight="1">
+    <row r="1" spans="1:24" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -2138,7 +2161,7 @@
       <c r="M1" s="43"/>
       <c r="N1" s="43"/>
     </row>
-    <row r="2" spans="1:24" ht="15.75" customHeight="1">
+    <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="44" t="s">
@@ -2156,7 +2179,7 @@
       <c r="M2" s="40"/>
       <c r="N2" s="40"/>
     </row>
-    <row r="3" spans="1:24" ht="15.75" customHeight="1">
+    <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -2171,10 +2194,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="15.75" customHeight="1">
+    <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:24" ht="15.75" customHeight="1">
+    <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C5" s="41" t="s">
         <v>6</v>
       </c>
@@ -2203,7 +2226,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="15.75" customHeight="1">
+    <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
@@ -2272,7 +2295,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="15.75" customHeight="1">
+    <row r="7" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="16" t="s">
         <v>15</v>
       </c>
@@ -2340,7 +2363,7 @@
       <c r="W7" s="17"/>
       <c r="X7" s="10"/>
     </row>
-    <row r="8" spans="1:24" ht="15.75" customHeight="1">
+    <row r="8" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="16" t="s">
         <v>15</v>
       </c>
@@ -2394,7 +2417,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="15.75" customHeight="1">
+    <row r="9" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="16" t="s">
         <v>15</v>
       </c>
@@ -2442,7 +2465,7 @@
       <c r="W9" s="17"/>
       <c r="X9" s="10"/>
     </row>
-    <row r="10" spans="1:24" ht="15.75" customHeight="1">
+    <row r="10" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="16" t="s">
         <v>15</v>
       </c>
@@ -2490,7 +2513,7 @@
       <c r="W10" s="17"/>
       <c r="X10" s="10"/>
     </row>
-    <row r="11" spans="1:24" ht="15.75" customHeight="1">
+    <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="16" t="s">
         <v>15</v>
       </c>
@@ -2552,7 +2575,7 @@
       <c r="W11" s="17"/>
       <c r="X11" s="10"/>
     </row>
-    <row r="12" spans="1:24" ht="15.75" customHeight="1">
+    <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="16" t="s">
         <v>15</v>
       </c>
@@ -2614,7 +2637,7 @@
       <c r="W12" s="17"/>
       <c r="X12" s="10"/>
     </row>
-    <row r="13" spans="1:24" ht="15.75" customHeight="1">
+    <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="16" t="s">
         <v>15</v>
       </c>
@@ -2662,7 +2685,7 @@
       <c r="W13" s="17"/>
       <c r="X13" s="10"/>
     </row>
-    <row r="14" spans="1:24" ht="15.75" customHeight="1">
+    <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="16" t="s">
         <v>15</v>
       </c>
@@ -2710,7 +2733,7 @@
       <c r="W14" s="17"/>
       <c r="X14" s="10"/>
     </row>
-    <row r="15" spans="1:24" ht="15.75" customHeight="1">
+    <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="16" t="s">
         <v>15</v>
       </c>
@@ -2758,7 +2781,7 @@
       <c r="W15" s="17"/>
       <c r="X15" s="10"/>
     </row>
-    <row r="16" spans="1:24" ht="15.75" customHeight="1">
+    <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="16" t="s">
         <v>15</v>
       </c>
@@ -2820,7 +2843,7 @@
       <c r="W16" s="17"/>
       <c r="X16" s="10"/>
     </row>
-    <row r="17" spans="1:24" ht="15.75" customHeight="1">
+    <row r="17" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="16" t="s">
         <v>15</v>
       </c>
@@ -2882,7 +2905,7 @@
       <c r="W17" s="17"/>
       <c r="X17" s="10"/>
     </row>
-    <row r="18" spans="1:24" ht="15.75" customHeight="1">
+    <row r="18" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="16" t="s">
         <v>15</v>
       </c>
@@ -2930,7 +2953,7 @@
       <c r="W18" s="17"/>
       <c r="X18" s="10"/>
     </row>
-    <row r="19" spans="1:24" ht="15.75" customHeight="1">
+    <row r="19" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="16" t="s">
         <v>15</v>
       </c>
@@ -2992,7 +3015,7 @@
       <c r="W19" s="17"/>
       <c r="X19" s="10"/>
     </row>
-    <row r="20" spans="1:24" ht="15.75" customHeight="1">
+    <row r="20" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="16" t="s">
         <v>15</v>
       </c>
@@ -3060,7 +3083,7 @@
       <c r="W20" s="17"/>
       <c r="X20" s="10"/>
     </row>
-    <row r="21" spans="1:24" ht="15.75" customHeight="1">
+    <row r="21" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="26" t="s">
         <v>15</v>
       </c>
@@ -3128,7 +3151,7 @@
       <c r="W21" s="21"/>
       <c r="X21" s="10"/>
     </row>
-    <row r="22" spans="1:24" ht="15.75" customHeight="1">
+    <row r="22" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="26" t="s">
         <v>15</v>
       </c>
@@ -3194,7 +3217,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="23" spans="1:24" ht="15.75" customHeight="1">
+    <row r="23" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="26" t="s">
         <v>15</v>
       </c>
@@ -3260,7 +3283,7 @@
       <c r="W23" s="21"/>
       <c r="X23" s="10"/>
     </row>
-    <row r="24" spans="1:24" ht="15.75" customHeight="1">
+    <row r="24" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="26" t="s">
         <v>15</v>
       </c>
@@ -3324,7 +3347,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="25" spans="1:24" ht="15.75" customHeight="1">
+    <row r="25" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="26" t="s">
         <v>15</v>
       </c>
@@ -3380,7 +3403,7 @@
       <c r="W25" s="21"/>
       <c r="X25" s="10"/>
     </row>
-    <row r="26" spans="1:24" ht="15.75" customHeight="1">
+    <row r="26" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="26" t="s">
         <v>15</v>
       </c>
@@ -3428,7 +3451,7 @@
       <c r="W26" s="21"/>
       <c r="X26" s="10"/>
     </row>
-    <row r="27" spans="1:24" ht="15.75" customHeight="1">
+    <row r="27" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="26" t="s">
         <v>15</v>
       </c>
@@ -3468,7 +3491,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:24" ht="15.75" customHeight="1">
+    <row r="28" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="26" t="s">
         <v>15</v>
       </c>
@@ -3477,7 +3500,7 @@
       </c>
       <c r="C28" s="21"/>
       <c r="D28" s="17" t="s">
-        <v>131</v>
+        <v>157</v>
       </c>
       <c r="E28" s="17" t="s">
         <v>135</v>
@@ -3534,7 +3557,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="29" spans="1:24" ht="15.75" customHeight="1">
+    <row r="29" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="26" t="s">
         <v>15</v>
       </c>
@@ -3592,7 +3615,7 @@
       <c r="W29" s="21"/>
       <c r="X29" s="10"/>
     </row>
-    <row r="30" spans="1:24" ht="15.75" customHeight="1">
+    <row r="30" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="26" t="s">
         <v>15</v>
       </c>
@@ -3652,7 +3675,7 @@
       <c r="W30" s="21"/>
       <c r="X30" s="10"/>
     </row>
-    <row r="31" spans="1:24" ht="15.75" customHeight="1">
+    <row r="31" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="26" t="s">
         <v>15</v>
       </c>
@@ -3710,7 +3733,7 @@
       <c r="W31" s="21"/>
       <c r="X31" s="10"/>
     </row>
-    <row r="32" spans="1:24" ht="15.75" customHeight="1">
+    <row r="32" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="26" t="s">
         <v>15</v>
       </c>
@@ -3768,7 +3791,7 @@
       <c r="W32" s="21"/>
       <c r="X32" s="10"/>
     </row>
-    <row r="33" spans="1:24" s="13" customFormat="1" ht="15.75" customHeight="1">
+    <row r="33" spans="1:24" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="26" t="s">
         <v>15</v>
       </c>
@@ -3836,7 +3859,7 @@
       <c r="W33" s="21"/>
       <c r="X33" s="12"/>
     </row>
-    <row r="34" spans="1:24" s="32" customFormat="1" ht="15.75" customHeight="1">
+    <row r="34" spans="1:24" s="32" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="26" t="s">
         <v>43</v>
       </c>
@@ -3884,7 +3907,7 @@
       <c r="W34" s="21"/>
       <c r="X34" s="31"/>
     </row>
-    <row r="35" spans="1:24" ht="15.75" customHeight="1">
+    <row r="35" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="26" t="s">
         <v>43</v>
       </c>
@@ -3934,7 +3957,7 @@
       <c r="W35" s="21"/>
       <c r="X35" s="10"/>
     </row>
-    <row r="36" spans="1:24" ht="15.75" customHeight="1">
+    <row r="36" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="26" t="s">
         <v>43</v>
       </c>
@@ -4000,7 +4023,7 @@
       <c r="W36" s="21"/>
       <c r="X36" s="10"/>
     </row>
-    <row r="37" spans="1:24" s="38" customFormat="1" ht="15.75" customHeight="1">
+    <row r="37" spans="1:24" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="26" t="s">
         <v>43</v>
       </c>
@@ -4068,7 +4091,7 @@
       <c r="W37" s="21"/>
       <c r="X37" s="37"/>
     </row>
-    <row r="38" spans="1:24" ht="15.75" customHeight="1">
+    <row r="38" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="26" t="s">
         <v>43</v>
       </c>
@@ -4134,7 +4157,7 @@
       <c r="W38" s="21"/>
       <c r="X38" s="10"/>
     </row>
-    <row r="39" spans="1:24" ht="15.75" customHeight="1">
+    <row r="39" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="26" t="s">
         <v>43</v>
       </c>
@@ -4200,7 +4223,7 @@
       <c r="W39" s="21"/>
       <c r="X39" s="10"/>
     </row>
-    <row r="40" spans="1:24" ht="15.75" customHeight="1">
+    <row r="40" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="26" t="s">
         <v>43</v>
       </c>
@@ -4266,7 +4289,7 @@
       <c r="W40" s="21"/>
       <c r="X40" s="10"/>
     </row>
-    <row r="41" spans="1:24" ht="15.75" customHeight="1">
+    <row r="41" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="26" t="s">
         <v>43</v>
       </c>
@@ -4332,7 +4355,7 @@
       <c r="W41" s="21"/>
       <c r="X41" s="10"/>
     </row>
-    <row r="42" spans="1:24" ht="15.75" customHeight="1">
+    <row r="42" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="26" t="s">
         <v>43</v>
       </c>
@@ -4394,7 +4417,7 @@
       <c r="W42" s="21"/>
       <c r="X42" s="10"/>
     </row>
-    <row r="43" spans="1:24" ht="15.75" customHeight="1">
+    <row r="43" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="26" t="s">
         <v>43</v>
       </c>
@@ -4460,7 +4483,7 @@
       <c r="W43" s="21"/>
       <c r="X43" s="10"/>
     </row>
-    <row r="44" spans="1:24" ht="15.75" customHeight="1">
+    <row r="44" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="26" t="s">
         <v>43</v>
       </c>
@@ -4516,7 +4539,7 @@
       <c r="W44" s="21"/>
       <c r="X44" s="10"/>
     </row>
-    <row r="45" spans="1:24" ht="15.75" customHeight="1">
+    <row r="45" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="26" t="s">
         <v>43</v>
       </c>
@@ -4568,7 +4591,7 @@
       <c r="W45" s="21"/>
       <c r="X45" s="10"/>
     </row>
-    <row r="46" spans="1:24" ht="15.75" customHeight="1">
+    <row r="46" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="26" t="s">
         <v>43</v>
       </c>
@@ -4616,7 +4639,7 @@
       <c r="W46" s="21"/>
       <c r="X46" s="10"/>
     </row>
-    <row r="47" spans="1:24" ht="15.75" customHeight="1">
+    <row r="47" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="26" t="s">
         <v>43</v>
       </c>
@@ -4664,7 +4687,7 @@
       <c r="W47" s="21"/>
       <c r="X47" s="10"/>
     </row>
-    <row r="48" spans="1:24" ht="15.75" customHeight="1">
+    <row r="48" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="26" t="s">
         <v>43</v>
       </c>
@@ -4712,7 +4735,7 @@
       <c r="W48" s="21"/>
       <c r="X48" s="10"/>
     </row>
-    <row r="49" spans="1:24" s="29" customFormat="1" ht="15.75" customHeight="1">
+    <row r="49" spans="1:24" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="26" t="s">
         <v>43</v>
       </c>
@@ -4774,7 +4797,7 @@
       <c r="W49" s="21"/>
       <c r="X49" s="28"/>
     </row>
-    <row r="50" spans="1:24" ht="15.75" customHeight="1">
+    <row r="50" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="26" t="s">
         <v>43</v>
       </c>
@@ -4840,7 +4863,7 @@
       <c r="W50" s="21"/>
       <c r="X50" s="10"/>
     </row>
-    <row r="51" spans="1:24" s="38" customFormat="1" ht="15.75" customHeight="1">
+    <row r="51" spans="1:24" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="26" t="s">
         <v>43</v>
       </c>
@@ -4904,7 +4927,7 @@
       <c r="W51" s="21"/>
       <c r="X51" s="37"/>
     </row>
-    <row r="52" spans="1:24" s="38" customFormat="1" ht="15.75" customHeight="1">
+    <row r="52" spans="1:24" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="26" t="s">
         <v>43</v>
       </c>
@@ -4968,7 +4991,7 @@
       <c r="W52" s="21"/>
       <c r="X52" s="37"/>
     </row>
-    <row r="53" spans="1:24" s="38" customFormat="1" ht="15.75" customHeight="1">
+    <row r="53" spans="1:24" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="26" t="s">
         <v>43</v>
       </c>
@@ -5032,7 +5055,7 @@
       <c r="W53" s="21"/>
       <c r="X53" s="37"/>
     </row>
-    <row r="54" spans="1:24" s="38" customFormat="1" ht="15.75" customHeight="1">
+    <row r="54" spans="1:24" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="26" t="s">
         <v>43</v>
       </c>
@@ -5096,7 +5119,7 @@
       <c r="W54" s="21"/>
       <c r="X54" s="37"/>
     </row>
-    <row r="55" spans="1:24" s="38" customFormat="1" ht="15.75" customHeight="1">
+    <row r="55" spans="1:24" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="26" t="s">
         <v>43</v>
       </c>
@@ -5160,7 +5183,7 @@
       <c r="W55" s="21"/>
       <c r="X55" s="37"/>
     </row>
-    <row r="56" spans="1:24" s="35" customFormat="1" ht="15.75" customHeight="1">
+    <row r="56" spans="1:24" s="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="26" t="s">
         <v>43</v>
       </c>
@@ -5206,7 +5229,7 @@
       <c r="W56" s="21"/>
       <c r="X56" s="34"/>
     </row>
-    <row r="57" spans="1:24" ht="15.75" customHeight="1">
+    <row r="57" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="26" t="s">
         <v>58</v>
       </c>
@@ -5276,7 +5299,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="58" spans="1:24" ht="15.75" customHeight="1">
+    <row r="58" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="26" t="s">
         <v>58</v>
       </c>
@@ -5344,7 +5367,7 @@
       <c r="W58" s="21"/>
       <c r="X58" s="40"/>
     </row>
-    <row r="59" spans="1:24" ht="15.75" customHeight="1">
+    <row r="59" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="26" t="s">
         <v>62</v>
       </c>
@@ -5410,7 +5433,7 @@
       <c r="W59" s="21"/>
       <c r="X59" s="10"/>
     </row>
-    <row r="60" spans="1:24" s="15" customFormat="1" ht="15.75" customHeight="1">
+    <row r="60" spans="1:24" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="18" t="s">
         <v>63</v>
       </c>
@@ -5444,7 +5467,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="61" spans="1:24" ht="15.75" customHeight="1">
+    <row r="61" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="16" t="s">
         <v>63</v>
       </c>
@@ -5487,7 +5510,7 @@
       <c r="V61" s="17"/>
       <c r="W61" s="17"/>
     </row>
-    <row r="62" spans="1:24" ht="15.75" customHeight="1">
+    <row r="62" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="16" t="s">
         <v>63</v>
       </c>
@@ -5518,7 +5541,7 @@
       <c r="V62" s="17"/>
       <c r="W62" s="17"/>
     </row>
-    <row r="63" spans="1:24" ht="15.75" customHeight="1">
+    <row r="63" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="16" t="s">
         <v>63</v>
       </c>
@@ -5549,7 +5572,7 @@
       <c r="V63" s="17"/>
       <c r="W63" s="17"/>
     </row>
-    <row r="64" spans="1:24" ht="15.75" customHeight="1">
+    <row r="64" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="16" t="s">
         <v>63</v>
       </c>
@@ -5580,7 +5603,7 @@
       <c r="V64" s="17"/>
       <c r="W64" s="17"/>
     </row>
-    <row r="65" spans="1:23" s="36" customFormat="1" ht="15.75" customHeight="1">
+    <row r="65" spans="1:23" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="16" t="s">
         <v>63</v>
       </c>
@@ -5611,7 +5634,7 @@
       <c r="V65" s="17"/>
       <c r="W65" s="17"/>
     </row>
-    <row r="66" spans="1:23" s="33" customFormat="1" ht="15.75" customHeight="1">
+    <row r="66" spans="1:23" s="33" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="16" t="s">
         <v>63</v>
       </c>
@@ -5642,7 +5665,7 @@
       <c r="V66" s="17"/>
       <c r="W66" s="17"/>
     </row>
-    <row r="67" spans="1:23" ht="15.75" customHeight="1">
+    <row r="67" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="16" t="s">
         <v>110</v>
       </c>
@@ -5673,7 +5696,7 @@
       <c r="V67" s="20"/>
       <c r="W67" s="20"/>
     </row>
-    <row r="68" spans="1:23" ht="15.75" customHeight="1">
+    <row r="68" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="16" t="s">
         <v>124</v>
       </c>
@@ -5718,14 +5741,22 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
-      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="E7" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="L57" sqref="L57:L59"/>
+    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="140">
+      <pane xSplit="2" ySplit="6" topLeftCell="C12" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="D28" sqref="D28"/>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
     <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
       <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
+      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="E7" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="L57" sqref="L57:L59"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>
@@ -5739,11 +5770,6 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5755,7 +5781,7 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="29.6640625" customWidth="1"/>
     <col min="2" max="2" width="28.1640625" customWidth="1"/>
@@ -5763,7 +5789,7 @@
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15">
+    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
         <v>70</v>
       </c>
@@ -5780,7 +5806,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15">
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
         <v>73</v>
       </c>
@@ -5793,7 +5819,7 @@
       <c r="D2" s="24"/>
       <c r="E2" s="24"/>
     </row>
-    <row r="3" spans="1:5" ht="15">
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
         <v>75</v>
       </c>
@@ -5806,7 +5832,7 @@
       <c r="D3" s="24"/>
       <c r="E3" s="24"/>
     </row>
-    <row r="4" spans="1:5" ht="15">
+    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
         <v>77</v>
       </c>
@@ -5819,7 +5845,7 @@
       <c r="D4" s="24"/>
       <c r="E4" s="24"/>
     </row>
-    <row r="5" spans="1:5" ht="15">
+    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
         <v>97</v>
       </c>
@@ -5834,7 +5860,7 @@
       </c>
       <c r="E5" s="24"/>
     </row>
-    <row r="6" spans="1:5" ht="15">
+    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
         <v>98</v>
       </c>
@@ -5849,7 +5875,7 @@
       </c>
       <c r="E6" s="24"/>
     </row>
-    <row r="7" spans="1:5" ht="15">
+    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
         <v>99</v>
       </c>
@@ -5864,7 +5890,7 @@
       </c>
       <c r="E7" s="24"/>
     </row>
-    <row r="8" spans="1:5" ht="15">
+    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
         <v>100</v>
       </c>
@@ -5879,7 +5905,7 @@
       </c>
       <c r="E8" s="24"/>
     </row>
-    <row r="9" spans="1:5" ht="15">
+    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
         <v>109</v>
       </c>
@@ -5892,7 +5918,7 @@
       <c r="D9" s="24"/>
       <c r="E9" s="24"/>
     </row>
-    <row r="10" spans="1:5" ht="15">
+    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
         <v>108</v>
       </c>
@@ -5905,7 +5931,7 @@
       <c r="D10" s="24"/>
       <c r="E10" s="24"/>
     </row>
-    <row r="11" spans="1:5" ht="15">
+    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
         <v>107</v>
       </c>
@@ -5918,7 +5944,7 @@
       <c r="D11" s="24"/>
       <c r="E11" s="24"/>
     </row>
-    <row r="12" spans="1:5" ht="15">
+    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
         <v>101</v>
       </c>
@@ -5933,7 +5959,7 @@
       </c>
       <c r="E12" s="24"/>
     </row>
-    <row r="13" spans="1:5" ht="15">
+    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="23" t="s">
         <v>106</v>
       </c>
@@ -5948,7 +5974,7 @@
       </c>
       <c r="E13" s="24"/>
     </row>
-    <row r="14" spans="1:5" ht="15">
+    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
         <v>102</v>
       </c>
@@ -5963,7 +5989,7 @@
       </c>
       <c r="E14" s="24"/>
     </row>
-    <row r="15" spans="1:5" ht="15">
+    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
         <v>103</v>
       </c>
@@ -5978,7 +6004,7 @@
       </c>
       <c r="E15" s="24"/>
     </row>
-    <row r="16" spans="1:5" ht="15">
+    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
         <v>104</v>
       </c>
@@ -5993,7 +6019,7 @@
       </c>
       <c r="E16" s="24"/>
     </row>
-    <row r="17" spans="1:5" ht="15">
+    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="23" t="s">
         <v>127</v>
       </c>
@@ -6008,7 +6034,7 @@
       </c>
       <c r="E17" s="24"/>
     </row>
-    <row r="18" spans="1:5" ht="15">
+    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
         <v>12</v>
       </c>
@@ -6023,7 +6049,7 @@
       </c>
       <c r="E18" s="24"/>
     </row>
-    <row r="19" spans="1:5" ht="15">
+    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="23" t="s">
         <v>13</v>
       </c>
@@ -6038,7 +6064,7 @@
       </c>
       <c r="E19" s="24"/>
     </row>
-    <row r="20" spans="1:5" ht="15">
+    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
         <v>105</v>
       </c>
@@ -6053,7 +6079,7 @@
       </c>
       <c r="E20" s="24"/>
     </row>
-    <row r="21" spans="1:5" ht="15">
+    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="23" t="s">
         <v>117</v>
       </c>
@@ -6072,21 +6098,23 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
+    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}">
       <selection activeCell="C7" sqref="C7"/>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
     <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
       <selection activeCell="C7" sqref="C7"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
+      <selection activeCell="C7" sqref="C7"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Lisää uusi erikoisoikeus TM-takaraja (JVH, ELY_Urakanvalvoja, tilaaja_Urakanvalvoja)
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="25640" yWindow="460" windowWidth="25540" windowHeight="27200" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38260" windowHeight="25060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -17,9 +17,9 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="1277" windowHeight="1187" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="1913" windowHeight="1080" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
     <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="159">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -506,7 +506,10 @@
     <t>R = lukuoikeus nimettyihin urakoihin, R,W = luku- ja kirjoitusoikeus nimettyihin urakoihin, W+ kirjoitusoikeus oman organisaation urakoihin, W* kirjoitusoikeus kaikkiin urakoihin, tyhjä = ei näe osiota, muut erikoisoikeuksia</t>
   </si>
   <si>
-    <t>R*,W*,TM-valmis</t>
+    <t>R*,W*,TM-valmis,TM-takaraja</t>
+  </si>
+  <si>
+    <t>R*,W,TM-takaraja</t>
   </si>
 </sst>
 </file>
@@ -967,7 +970,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{FC69AAD3-0412-1847-89C5-E3EAD8A67C1F}" diskRevisions="1" revisionId="64" version="9">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{3B00597B-4E8C-8B4F-BA72-B62F7DB2FF8A}" diskRevisions="1" revisionId="67" version="10">
   <header guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" dateTime="2016-09-06T09:14:56" maxSheetId="3" userName="Tatu Tarvainen" r:id="rId2" minRId="1" maxRId="3">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1016,7 +1019,56 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{3B00597B-4E8C-8B4F-BA72-B62F7DB2FF8A}" dateTime="2016-10-11T12:14:04" maxSheetId="3" userName="Microsoft Office User" r:id="rId10" minRId="65" maxRId="67">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
+</file>
+
+<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="65" sId="1">
+    <oc r="D28" t="inlineStr">
+      <is>
+        <t>R*,W*,TM-valmis</t>
+      </is>
+    </oc>
+    <nc r="D28" t="inlineStr">
+      <is>
+        <t>R*,W*,TM-valmis,TM-takaraja</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="66" sId="1">
+    <oc r="K28" t="inlineStr">
+      <is>
+        <t>R*,W</t>
+      </is>
+    </oc>
+    <nc r="K28" t="inlineStr">
+      <is>
+        <t>R*,W,TM-takaraja</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="67" sId="1">
+    <oc r="E28" t="inlineStr">
+      <is>
+        <t>R*,W</t>
+      </is>
+    </oc>
+    <nc r="E28" t="inlineStr">
+      <is>
+        <t>R*,W,TM-takaraja</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="delete"/>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="add"/>
+</revisions>
 </file>
 
 <file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1774,12 +1826,13 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="4">
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="5">
   <userInfo guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" name="Tatu Tarvainen" id="-130145201" dateTime="2016-09-06T09:10:23"/>
   <userInfo guid="{E0850D7E-A93F-EF44-B46A-3BEA4D7DBEDB}" name="Jarno Väyrynen" id="-589116405" dateTime="2016-09-06T12:54:09"/>
   <userInfo guid="{0407E191-78DA-F349-B5E5-8AE1BC03A29E}" name="Jarno Väyrynen" id="-589108428" dateTime="2016-09-08T15:33:24"/>
   <userInfo guid="{F8907045-3B30-0A43-A905-F167D27F9989}" name="Jarno Väyrynen" id="-589157736" dateTime="2016-09-27T15:27:41"/>
+  <userInfo guid="{3B00597B-4E8C-8B4F-BA72-B62F7DB2FF8A}" name="Microsoft Office User" id="-296969744" dateTime="2016-10-11T12:12:42"/>
 </users>
 </file>
 
@@ -2111,7 +2164,7 @@
       <pane xSplit="2" ySplit="6" topLeftCell="C12" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D26" sqref="D26"/>
+      <selection pane="bottomRight" activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3503,7 +3556,7 @@
         <v>157</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>135</v>
+        <v>158</v>
       </c>
       <c r="F28" s="21" t="s">
         <v>132</v>
@@ -3521,7 +3574,7 @@
         <v>131</v>
       </c>
       <c r="K28" s="21" t="s">
-        <v>135</v>
+        <v>158</v>
       </c>
       <c r="L28" s="21" t="s">
         <v>17</v>
@@ -5743,19 +5796,19 @@
   <customSheetViews>
     <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="140">
       <pane xSplit="2" ySplit="6" topLeftCell="C12" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="D28" sqref="D28"/>
+      <selection pane="bottomRight" activeCell="H26" sqref="H26"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
+      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="E7" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="L57" sqref="L57:L59"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
     <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
       <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
-      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="E7" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="L57" sqref="L57:L59"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -6103,12 +6156,12 @@
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
       <selection activeCell="C7" sqref="C7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
+    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
       <selection activeCell="C7" sqref="C7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Anna JVH:lle TM-valmis ja TM-takaraja oikeus kaikkiin urakoihin
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38260" windowHeight="25060" tabRatio="500"/>
+    <workbookView xWindow="5000" yWindow="1900" windowWidth="38260" windowHeight="23140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -17,9 +17,9 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="1913" windowHeight="1080" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="1913" windowHeight="984" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
-    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -506,10 +506,10 @@
     <t>R = lukuoikeus nimettyihin urakoihin, R,W = luku- ja kirjoitusoikeus nimettyihin urakoihin, W+ kirjoitusoikeus oman organisaation urakoihin, W* kirjoitusoikeus kaikkiin urakoihin, tyhjä = ei näe osiota, muut erikoisoikeuksia</t>
   </si>
   <si>
-    <t>R*,W*,TM-valmis,TM-takaraja</t>
-  </si>
-  <si>
     <t>R*,W,TM-takaraja</t>
+  </si>
+  <si>
+    <t>R*,W*,TM-valmis*,TM-takaraja*</t>
   </si>
 </sst>
 </file>
@@ -970,7 +970,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{3B00597B-4E8C-8B4F-BA72-B62F7DB2FF8A}" diskRevisions="1" revisionId="67" version="10">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{65E12868-01B4-8F43-907A-C749CC5006A6}" diskRevisions="1" revisionId="68" version="11">
   <header guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" dateTime="2016-09-06T09:14:56" maxSheetId="3" userName="Tatu Tarvainen" r:id="rId2" minRId="1" maxRId="3">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1025,6 +1025,12 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{65E12868-01B4-8F43-907A-C749CC5006A6}" dateTime="2016-10-11T12:52:46" maxSheetId="3" userName="Microsoft Office User" r:id="rId11" minRId="68">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -1063,6 +1069,25 @@
     <nc r="E28" t="inlineStr">
       <is>
         <t>R*,W,TM-takaraja</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="delete"/>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog10.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="68" sId="1">
+    <oc r="D28" t="inlineStr">
+      <is>
+        <t>R*,W*,TM-valmis,TM-takaraja</t>
+      </is>
+    </oc>
+    <nc r="D28" t="inlineStr">
+      <is>
+        <t>R*,W*,TM-valmis*,TM-takaraja*</t>
       </is>
     </nc>
   </rcc>
@@ -1826,13 +1851,12 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="5">
+<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="4">
   <userInfo guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" name="Tatu Tarvainen" id="-130145201" dateTime="2016-09-06T09:10:23"/>
   <userInfo guid="{E0850D7E-A93F-EF44-B46A-3BEA4D7DBEDB}" name="Jarno Väyrynen" id="-589116405" dateTime="2016-09-06T12:54:09"/>
   <userInfo guid="{0407E191-78DA-F349-B5E5-8AE1BC03A29E}" name="Jarno Väyrynen" id="-589108428" dateTime="2016-09-08T15:33:24"/>
   <userInfo guid="{F8907045-3B30-0A43-A905-F167D27F9989}" name="Jarno Väyrynen" id="-589157736" dateTime="2016-09-27T15:27:41"/>
-  <userInfo guid="{3B00597B-4E8C-8B4F-BA72-B62F7DB2FF8A}" name="Microsoft Office User" id="-296969744" dateTime="2016-10-11T12:12:42"/>
 </users>
 </file>
 
@@ -2160,11 +2184,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
       <pane xSplit="2" ySplit="6" topLeftCell="C12" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="H26" sqref="H26"/>
+      <selection pane="bottomRight" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3553,10 +3577,10 @@
       </c>
       <c r="C28" s="21"/>
       <c r="D28" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="E28" s="17" t="s">
         <v>157</v>
-      </c>
-      <c r="E28" s="17" t="s">
-        <v>158</v>
       </c>
       <c r="F28" s="21" t="s">
         <v>132</v>
@@ -3574,7 +3598,7 @@
         <v>131</v>
       </c>
       <c r="K28" s="21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L28" s="21" t="s">
         <v>17</v>
@@ -5794,21 +5818,21 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="140">
+    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
       <pane xSplit="2" ySplit="6" topLeftCell="C12" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="H26" sqref="H26"/>
+      <selection pane="bottomRight" activeCell="E28" sqref="E28"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
+      <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
     <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
       <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="E7" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="bottomRight" activeCell="L57" sqref="L57:L59"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
-      <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -6156,12 +6180,12 @@
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
+    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
       <selection activeCell="C7" sqref="C7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
       <selection activeCell="C7" sqref="C7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Lisää roolit-exceliin toteutus-välilehden rivit
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5000" yWindow="1900" windowWidth="38260" windowHeight="23140" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="1260" windowWidth="32960" windowHeight="13960" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="1913" windowHeight="984" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="1648" windowHeight="525" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
   </customWorkbookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="162">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -510,6 +510,15 @@
   </si>
   <si>
     <t>R*,W*,TM-valmis*,TM-takaraja*</t>
+  </si>
+  <si>
+    <t>Toteutus / Kokonaishintaiset työt</t>
+  </si>
+  <si>
+    <t>Toteutus / Yksikköhintaiset työt</t>
+  </si>
+  <si>
+    <t>Toteutus / Muut työt</t>
   </si>
 </sst>
 </file>
@@ -753,7 +762,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -814,6 +823,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -970,7 +983,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{65E12868-01B4-8F43-907A-C749CC5006A6}" diskRevisions="1" revisionId="68" version="11">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{570602AA-71A9-F341-BC7B-B09F7DB93788}" diskRevisions="1" revisionId="87" version="13">
   <header guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" dateTime="2016-09-06T09:14:56" maxSheetId="3" userName="Tatu Tarvainen" r:id="rId2" minRId="1" maxRId="3">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1031,6 +1044,18 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{38B11935-7ACB-8242-839C-AF964FC8C260}" dateTime="2016-10-25T13:53:22" maxSheetId="3" userName="Microsoft Office User" r:id="rId12" minRId="69" maxRId="87">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{570602AA-71A9-F341-BC7B-B09F7DB93788}" dateTime="2016-10-25T13:55:26" maxSheetId="3" userName="Microsoft Office User" r:id="rId13">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -1091,6 +1116,222 @@
       </is>
     </nc>
   </rcc>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="delete"/>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog11.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="69" sId="1" ref="A33:XFD35" action="insertRow"/>
+  <rcc rId="70" sId="1">
+    <nc r="A33" t="inlineStr">
+      <is>
+        <t>Urakat</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="71" sId="1">
+    <nc r="B33" t="inlineStr">
+      <is>
+        <t>Toteutus / Kokonaishintaiset työt</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="72" sId="1">
+    <nc r="J33" t="inlineStr">
+      <is>
+        <t>R*,W*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="73" sId="1">
+    <nc r="K33" t="inlineStr">
+      <is>
+        <t>R*,W</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="O33" start="0" length="0">
+    <dxf/>
+  </rfmt>
+  <rcc rId="74" sId="1">
+    <nc r="P33" t="inlineStr">
+      <is>
+        <t>R+,W+</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="75" sId="1">
+    <nc r="Q33" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="W33" start="0" length="0">
+    <dxf>
+      <alignment horizontal="general" vertical="center" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="X33" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment vertical="top" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rcc rId="76" sId="1">
+    <nc r="A34" t="inlineStr">
+      <is>
+        <t>Urakat</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="77" sId="1">
+    <nc r="B34" t="inlineStr">
+      <is>
+        <t>Toteutus / Yksikköhintaiset työt</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="78" sId="1">
+    <nc r="J34" t="inlineStr">
+      <is>
+        <t>R*,W*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="79" sId="1">
+    <nc r="K34" t="inlineStr">
+      <is>
+        <t>R*,W</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="O34" start="0" length="0">
+    <dxf/>
+  </rfmt>
+  <rcc rId="80" sId="1">
+    <nc r="P34" t="inlineStr">
+      <is>
+        <t>R+,W+</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="81" sId="1">
+    <nc r="Q34" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="W34" start="0" length="0">
+    <dxf>
+      <alignment horizontal="general" vertical="center" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="X34" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment vertical="top" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rcc rId="82" sId="1">
+    <nc r="A35" t="inlineStr">
+      <is>
+        <t>Urakat</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="83" sId="1">
+    <nc r="B35" t="inlineStr">
+      <is>
+        <t>Toteutus / Muut työt</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="84" sId="1">
+    <nc r="J35" t="inlineStr">
+      <is>
+        <t>R*,W*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="85" sId="1">
+    <nc r="K35" t="inlineStr">
+      <is>
+        <t>R*,W</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="O35" start="0" length="0">
+    <dxf/>
+  </rfmt>
+  <rcc rId="86" sId="1">
+    <nc r="P35" t="inlineStr">
+      <is>
+        <t>R+,W+</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="87" sId="1">
+    <nc r="Q35" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="W35" start="0" length="0">
+    <dxf>
+      <alignment horizontal="general" vertical="center" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="X35" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment vertical="top" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="delete"/>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog12.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="delete"/>
   <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="add"/>
 </revisions>
@@ -1851,7 +2092,7 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="4">
   <userInfo guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" name="Tatu Tarvainen" id="-130145201" dateTime="2016-09-06T09:10:23"/>
   <userInfo guid="{E0850D7E-A93F-EF44-B46A-3BEA4D7DBEDB}" name="Jarno Väyrynen" id="-589116405" dateTime="2016-09-06T12:54:09"/>
@@ -2182,20 +2423,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X68"/>
+  <dimension ref="A1:X71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C12" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C29" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E28" sqref="E28"/>
+      <selection pane="bottomRight" activeCell="W33" sqref="W33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" customWidth="1"/>
     <col min="4" max="4" width="12.5" customWidth="1"/>
     <col min="5" max="5" width="11.5" customWidth="1"/>
     <col min="6" max="6" width="10.1640625" customWidth="1"/>
@@ -2223,38 +2464,38 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="44" t="s">
         <v>156</v>
       </c>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
     </row>
     <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
     </row>
     <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
@@ -2275,30 +2516,30 @@
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="J5" s="41" t="s">
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="J5" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="40"/>
-      <c r="L5" s="40"/>
-      <c r="M5" s="40"/>
-      <c r="N5" s="40"/>
-      <c r="P5" s="41" t="s">
+      <c r="K5" s="42"/>
+      <c r="L5" s="42"/>
+      <c r="M5" s="42"/>
+      <c r="N5" s="42"/>
+      <c r="P5" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="Q5" s="40"/>
-      <c r="R5" s="40"/>
-      <c r="S5" s="40"/>
-      <c r="T5" s="40"/>
-      <c r="U5" s="40"/>
-      <c r="V5" s="40"/>
+      <c r="Q5" s="42"/>
+      <c r="R5" s="42"/>
+      <c r="S5" s="42"/>
+      <c r="T5" s="42"/>
+      <c r="U5" s="42"/>
+      <c r="V5" s="42"/>
       <c r="X5" s="5" t="s">
         <v>14</v>
       </c>
@@ -3868,312 +4109,239 @@
       <c r="W32" s="21"/>
       <c r="X32" s="10"/>
     </row>
-    <row r="33" spans="1:24" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:24" s="40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="26" t="s">
         <v>15</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>121</v>
+        <v>159</v>
       </c>
       <c r="C33" s="21"/>
-      <c r="D33" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="E33" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="F33" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="G33" s="21" t="s">
-        <v>134</v>
-      </c>
-      <c r="H33" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="I33" s="21" t="s">
-        <v>131</v>
-      </c>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
       <c r="J33" s="17" t="s">
         <v>131</v>
       </c>
       <c r="K33" s="21" t="s">
-        <v>138</v>
-      </c>
-      <c r="L33" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="M33" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="N33" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="O33" s="17" t="s">
-        <v>132</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="L33" s="21"/>
+      <c r="M33" s="21"/>
+      <c r="N33" s="17"/>
+      <c r="O33" s="17"/>
       <c r="P33" s="21" t="s">
         <v>137</v>
       </c>
       <c r="Q33" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="R33" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="S33" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="T33" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="U33" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="V33" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="W33" s="21"/>
-      <c r="X33" s="12"/>
-    </row>
-    <row r="34" spans="1:24" s="32" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="R33" s="21"/>
+      <c r="S33" s="21"/>
+      <c r="T33" s="17"/>
+      <c r="U33" s="21"/>
+      <c r="V33" s="21"/>
+      <c r="W33" s="39"/>
+    </row>
+    <row r="34" spans="1:24" s="40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="26" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>128</v>
+        <v>160</v>
       </c>
       <c r="C34" s="21"/>
-      <c r="D34" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="E34" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="F34" s="21" t="s">
-        <v>132</v>
-      </c>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="21"/>
       <c r="G34" s="21"/>
       <c r="H34" s="21"/>
       <c r="I34" s="21"/>
-      <c r="J34" s="21" t="s">
-        <v>132</v>
+      <c r="J34" s="17" t="s">
+        <v>131</v>
       </c>
       <c r="K34" s="21" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="L34" s="21"/>
-      <c r="M34" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="N34" s="21"/>
-      <c r="O34" s="21"/>
+      <c r="M34" s="21"/>
+      <c r="N34" s="17"/>
+      <c r="O34" s="17"/>
       <c r="P34" s="21" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="Q34" s="21" t="s">
-        <v>17</v>
+        <v>114</v>
       </c>
       <c r="R34" s="21"/>
       <c r="S34" s="21"/>
-      <c r="T34" s="21" t="s">
-        <v>136</v>
-      </c>
+      <c r="T34" s="17"/>
       <c r="U34" s="21"/>
       <c r="V34" s="21"/>
-      <c r="W34" s="21"/>
-      <c r="X34" s="31"/>
-    </row>
-    <row r="35" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="W34" s="39"/>
+    </row>
+    <row r="35" spans="1:24" s="40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="26" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>44</v>
+        <v>161</v>
       </c>
       <c r="C35" s="21"/>
-      <c r="D35" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="E35" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="F35" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="G35" s="21" t="s">
-        <v>19</v>
-      </c>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="21"/>
       <c r="H35" s="21"/>
       <c r="I35" s="21"/>
-      <c r="J35" s="21" t="s">
-        <v>132</v>
+      <c r="J35" s="17" t="s">
+        <v>131</v>
       </c>
       <c r="K35" s="21" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="L35" s="21"/>
-      <c r="M35" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="N35" s="21"/>
-      <c r="O35" s="21"/>
+      <c r="M35" s="21"/>
+      <c r="N35" s="17"/>
+      <c r="O35" s="17"/>
       <c r="P35" s="21" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="Q35" s="21" t="s">
-        <v>17</v>
+        <v>114</v>
       </c>
       <c r="R35" s="21"/>
       <c r="S35" s="21"/>
-      <c r="T35" s="21" t="s">
-        <v>136</v>
-      </c>
+      <c r="T35" s="17"/>
       <c r="U35" s="21"/>
       <c r="V35" s="21"/>
-      <c r="W35" s="21"/>
-      <c r="X35" s="10"/>
-    </row>
-    <row r="36" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="W35" s="39"/>
+    </row>
+    <row r="36" spans="1:24" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="26" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>45</v>
+        <v>121</v>
       </c>
       <c r="C36" s="21"/>
-      <c r="D36" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="E36" s="21" t="s">
-        <v>132</v>
+      <c r="D36" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="E36" s="17" t="s">
+        <v>135</v>
       </c>
       <c r="F36" s="21" t="s">
         <v>132</v>
       </c>
       <c r="G36" s="21" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="H36" s="21" t="s">
         <v>132</v>
       </c>
       <c r="I36" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="J36" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
+      </c>
+      <c r="J36" s="17" t="s">
+        <v>131</v>
       </c>
       <c r="K36" s="21" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="L36" s="21" t="s">
-        <v>17</v>
+        <v>114</v>
       </c>
       <c r="M36" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="N36" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="O36" s="21" t="s">
+      <c r="N36" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="O36" s="17" t="s">
         <v>132</v>
       </c>
       <c r="P36" s="21" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="Q36" s="21" t="s">
-        <v>17</v>
+        <v>114</v>
       </c>
       <c r="R36" s="21" t="s">
         <v>136</v>
       </c>
       <c r="S36" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="T36" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="U36" s="21"/>
+        <v>114</v>
+      </c>
+      <c r="T36" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="U36" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="V36" s="21" t="s">
         <v>17</v>
       </c>
       <c r="W36" s="21"/>
-      <c r="X36" s="10"/>
-    </row>
-    <row r="37" spans="1:24" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="X36" s="12"/>
+    </row>
+    <row r="37" spans="1:24" s="32" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>46</v>
+        <v>128</v>
       </c>
       <c r="C37" s="21"/>
-      <c r="D37" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="E37" s="21" t="s">
+      <c r="D37" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="E37" s="17" t="s">
         <v>132</v>
       </c>
       <c r="F37" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="G37" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="H37" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="I37" s="21" t="s">
-        <v>132</v>
-      </c>
+      <c r="G37" s="21"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="21"/>
       <c r="J37" s="21" t="s">
         <v>132</v>
       </c>
       <c r="K37" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="L37" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="L37" s="21"/>
       <c r="M37" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="N37" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="O37" s="21" t="s">
-        <v>132</v>
-      </c>
+      <c r="N37" s="21"/>
+      <c r="O37" s="21"/>
       <c r="P37" s="21" t="s">
         <v>136</v>
       </c>
       <c r="Q37" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="R37" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="S37" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="R37" s="21"/>
+      <c r="S37" s="21"/>
       <c r="T37" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="U37" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="V37" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="U37" s="21"/>
+      <c r="V37" s="21"/>
       <c r="W37" s="21"/>
-      <c r="X37" s="37"/>
+      <c r="X37" s="31"/>
     </row>
     <row r="38" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>153</v>
+        <v>44</v>
       </c>
       <c r="C38" s="21"/>
       <c r="D38" s="21" t="s">
@@ -4186,51 +4354,35 @@
         <v>132</v>
       </c>
       <c r="G38" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="H38" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="I38" s="21" t="s">
-        <v>132</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="H38" s="21"/>
+      <c r="I38" s="21"/>
       <c r="J38" s="21" t="s">
         <v>132</v>
       </c>
       <c r="K38" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="L38" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="L38" s="21"/>
       <c r="M38" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="N38" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="O38" s="21" t="s">
-        <v>132</v>
-      </c>
+      <c r="N38" s="21"/>
+      <c r="O38" s="21"/>
       <c r="P38" s="21" t="s">
         <v>136</v>
       </c>
       <c r="Q38" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="R38" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="S38" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="R38" s="21"/>
+      <c r="S38" s="21"/>
       <c r="T38" s="21" t="s">
         <v>136</v>
       </c>
       <c r="U38" s="21"/>
-      <c r="V38" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="V38" s="21"/>
       <c r="W38" s="21"/>
       <c r="X38" s="10"/>
     </row>
@@ -4239,7 +4391,7 @@
         <v>43</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C39" s="21"/>
       <c r="D39" s="21" t="s">
@@ -4300,12 +4452,12 @@
       <c r="W39" s="21"/>
       <c r="X39" s="10"/>
     </row>
-    <row r="40" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:24" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C40" s="21"/>
       <c r="D40" s="21" t="s">
@@ -4359,19 +4511,21 @@
       <c r="T40" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="U40" s="21"/>
+      <c r="U40" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="V40" s="21" t="s">
         <v>17</v>
       </c>
       <c r="W40" s="21"/>
-      <c r="X40" s="10"/>
+      <c r="X40" s="37"/>
     </row>
     <row r="41" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>49</v>
+        <v>153</v>
       </c>
       <c r="C41" s="21"/>
       <c r="D41" s="21" t="s">
@@ -4437,7 +4591,7 @@
         <v>43</v>
       </c>
       <c r="B42" s="26" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C42" s="21"/>
       <c r="D42" s="21" t="s">
@@ -4470,7 +4624,9 @@
       <c r="M42" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="N42" s="21"/>
+      <c r="N42" s="21" t="s">
+        <v>132</v>
+      </c>
       <c r="O42" s="21" t="s">
         <v>132</v>
       </c>
@@ -4483,7 +4639,9 @@
       <c r="R42" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="S42" s="21"/>
+      <c r="S42" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="T42" s="21" t="s">
         <v>136</v>
       </c>
@@ -4499,7 +4657,7 @@
         <v>43</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C43" s="21"/>
       <c r="D43" s="21" t="s">
@@ -4565,7 +4723,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="26" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C44" s="21"/>
       <c r="D44" s="21" t="s">
@@ -4577,8 +4735,12 @@
       <c r="F44" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="G44" s="21"/>
-      <c r="H44" s="21"/>
+      <c r="G44" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="H44" s="21" t="s">
+        <v>132</v>
+      </c>
       <c r="I44" s="21" t="s">
         <v>132</v>
       </c>
@@ -4588,11 +4750,15 @@
       <c r="K44" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="L44" s="21"/>
+      <c r="L44" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="M44" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="N44" s="21"/>
+      <c r="N44" s="21" t="s">
+        <v>132</v>
+      </c>
       <c r="O44" s="21" t="s">
         <v>132</v>
       </c>
@@ -4605,7 +4771,9 @@
       <c r="R44" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="S44" s="21"/>
+      <c r="S44" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="T44" s="21" t="s">
         <v>136</v>
       </c>
@@ -4621,7 +4789,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="26" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C45" s="21"/>
       <c r="D45" s="21" t="s">
@@ -4633,38 +4801,48 @@
       <c r="F45" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="G45" s="21"/>
+      <c r="G45" s="21" t="s">
+        <v>132</v>
+      </c>
       <c r="H45" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="I45" s="21"/>
+        <v>132</v>
+      </c>
+      <c r="I45" s="21" t="s">
+        <v>132</v>
+      </c>
       <c r="J45" s="21" t="s">
         <v>132</v>
       </c>
       <c r="K45" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="L45" s="21"/>
+      <c r="L45" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="M45" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="N45" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="O45" s="21"/>
+      <c r="N45" s="21"/>
+      <c r="O45" s="21" t="s">
+        <v>132</v>
+      </c>
       <c r="P45" s="21" t="s">
         <v>136</v>
       </c>
       <c r="Q45" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="R45" s="21"/>
+      <c r="R45" s="21" t="s">
+        <v>136</v>
+      </c>
       <c r="S45" s="21"/>
       <c r="T45" s="21" t="s">
         <v>136</v>
       </c>
       <c r="U45" s="21"/>
-      <c r="V45" s="21"/>
+      <c r="V45" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="W45" s="21"/>
       <c r="X45" s="10"/>
     </row>
@@ -4673,7 +4851,7 @@
         <v>43</v>
       </c>
       <c r="B46" s="26" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C46" s="21"/>
       <c r="D46" s="21" t="s">
@@ -4685,34 +4863,52 @@
       <c r="F46" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="G46" s="21"/>
-      <c r="H46" s="21"/>
-      <c r="I46" s="21"/>
+      <c r="G46" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="H46" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="I46" s="21" t="s">
+        <v>132</v>
+      </c>
       <c r="J46" s="21" t="s">
         <v>132</v>
       </c>
       <c r="K46" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="L46" s="21"/>
+      <c r="L46" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="M46" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="N46" s="21"/>
-      <c r="O46" s="21"/>
+      <c r="N46" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="O46" s="21" t="s">
+        <v>132</v>
+      </c>
       <c r="P46" s="21" t="s">
         <v>136</v>
       </c>
       <c r="Q46" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="R46" s="21"/>
-      <c r="S46" s="21"/>
+      <c r="R46" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="S46" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="T46" s="21" t="s">
         <v>136</v>
       </c>
       <c r="U46" s="21"/>
-      <c r="V46" s="21"/>
+      <c r="V46" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="W46" s="21"/>
       <c r="X46" s="10"/>
     </row>
@@ -4721,7 +4917,7 @@
         <v>43</v>
       </c>
       <c r="B47" s="26" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C47" s="21"/>
       <c r="D47" s="21" t="s">
@@ -4735,7 +4931,9 @@
       </c>
       <c r="G47" s="21"/>
       <c r="H47" s="21"/>
-      <c r="I47" s="21"/>
+      <c r="I47" s="21" t="s">
+        <v>132</v>
+      </c>
       <c r="J47" s="21" t="s">
         <v>132</v>
       </c>
@@ -4747,20 +4945,26 @@
         <v>132</v>
       </c>
       <c r="N47" s="21"/>
-      <c r="O47" s="21"/>
+      <c r="O47" s="21" t="s">
+        <v>132</v>
+      </c>
       <c r="P47" s="21" t="s">
         <v>136</v>
       </c>
       <c r="Q47" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="R47" s="21"/>
+      <c r="R47" s="21" t="s">
+        <v>136</v>
+      </c>
       <c r="S47" s="21"/>
       <c r="T47" s="21" t="s">
         <v>136</v>
       </c>
       <c r="U47" s="21"/>
-      <c r="V47" s="21"/>
+      <c r="V47" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="W47" s="21"/>
       <c r="X47" s="10"/>
     </row>
@@ -4769,7 +4973,7 @@
         <v>43</v>
       </c>
       <c r="B48" s="26" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C48" s="21"/>
       <c r="D48" s="21" t="s">
@@ -4782,7 +4986,9 @@
         <v>132</v>
       </c>
       <c r="G48" s="21"/>
-      <c r="H48" s="21"/>
+      <c r="H48" s="21" t="s">
+        <v>19</v>
+      </c>
       <c r="I48" s="21"/>
       <c r="J48" s="21" t="s">
         <v>132</v>
@@ -4794,7 +5000,9 @@
       <c r="M48" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="N48" s="21"/>
+      <c r="N48" s="21" t="s">
+        <v>19</v>
+      </c>
       <c r="O48" s="21"/>
       <c r="P48" s="21" t="s">
         <v>136</v>
@@ -4812,12 +5020,12 @@
       <c r="W48" s="21"/>
       <c r="X48" s="10"/>
     </row>
-    <row r="49" spans="1:24" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B49" s="26" t="s">
-        <v>126</v>
+        <v>54</v>
       </c>
       <c r="C49" s="21"/>
       <c r="D49" s="21" t="s">
@@ -4829,57 +5037,43 @@
       <c r="F49" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="G49" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="H49" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="I49" s="21" t="s">
-        <v>132</v>
-      </c>
+      <c r="G49" s="21"/>
+      <c r="H49" s="21"/>
+      <c r="I49" s="21"/>
       <c r="J49" s="21" t="s">
         <v>132</v>
       </c>
       <c r="K49" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="L49" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="L49" s="21"/>
       <c r="M49" s="21" t="s">
         <v>132</v>
       </c>
       <c r="N49" s="21"/>
-      <c r="O49" s="21" t="s">
-        <v>132</v>
-      </c>
+      <c r="O49" s="21"/>
       <c r="P49" s="21" t="s">
         <v>136</v>
       </c>
       <c r="Q49" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="R49" s="21" t="s">
-        <v>136</v>
-      </c>
+      <c r="R49" s="21"/>
       <c r="S49" s="21"/>
       <c r="T49" s="21" t="s">
         <v>136</v>
       </c>
       <c r="U49" s="21"/>
-      <c r="V49" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="V49" s="21"/>
       <c r="W49" s="21"/>
-      <c r="X49" s="28"/>
+      <c r="X49" s="10"/>
     </row>
     <row r="50" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B50" s="26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C50" s="21"/>
       <c r="D50" s="21" t="s">
@@ -4891,61 +5085,43 @@
       <c r="F50" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="G50" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="H50" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="I50" s="21" t="s">
-        <v>132</v>
-      </c>
+      <c r="G50" s="21"/>
+      <c r="H50" s="21"/>
+      <c r="I50" s="21"/>
       <c r="J50" s="21" t="s">
         <v>132</v>
       </c>
       <c r="K50" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="L50" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="L50" s="21"/>
       <c r="M50" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="N50" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="O50" s="21" t="s">
-        <v>132</v>
-      </c>
+      <c r="N50" s="21"/>
+      <c r="O50" s="21"/>
       <c r="P50" s="21" t="s">
         <v>136</v>
       </c>
       <c r="Q50" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="R50" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="S50" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="R50" s="21"/>
+      <c r="S50" s="21"/>
       <c r="T50" s="21" t="s">
         <v>136</v>
       </c>
       <c r="U50" s="21"/>
-      <c r="V50" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="V50" s="21"/>
       <c r="W50" s="21"/>
       <c r="X50" s="10"/>
     </row>
-    <row r="51" spans="1:24" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B51" s="26" t="s">
-        <v>130</v>
+        <v>56</v>
       </c>
       <c r="C51" s="21"/>
       <c r="D51" s="21" t="s">
@@ -4957,59 +5133,43 @@
       <c r="F51" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="G51" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="H51" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="I51" s="21" t="s">
-        <v>132</v>
-      </c>
+      <c r="G51" s="21"/>
+      <c r="H51" s="21"/>
+      <c r="I51" s="21"/>
       <c r="J51" s="21" t="s">
         <v>132</v>
       </c>
       <c r="K51" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="L51" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="L51" s="21"/>
       <c r="M51" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="N51" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="O51" s="21" t="s">
-        <v>132</v>
-      </c>
+      <c r="N51" s="21"/>
+      <c r="O51" s="21"/>
       <c r="P51" s="21" t="s">
         <v>136</v>
       </c>
       <c r="Q51" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="R51" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="S51" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="R51" s="21"/>
+      <c r="S51" s="21"/>
       <c r="T51" s="21" t="s">
         <v>136</v>
       </c>
       <c r="U51" s="21"/>
       <c r="V51" s="21"/>
       <c r="W51" s="21"/>
-      <c r="X51" s="37"/>
-    </row>
-    <row r="52" spans="1:24" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="X51" s="10"/>
+    </row>
+    <row r="52" spans="1:24" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B52" s="26" t="s">
-        <v>148</v>
+        <v>126</v>
       </c>
       <c r="C52" s="21"/>
       <c r="D52" s="21" t="s">
@@ -5042,9 +5202,7 @@
       <c r="M52" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="N52" s="21" t="s">
-        <v>132</v>
-      </c>
+      <c r="N52" s="21"/>
       <c r="O52" s="21" t="s">
         <v>132</v>
       </c>
@@ -5057,23 +5215,23 @@
       <c r="R52" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="S52" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="S52" s="21"/>
       <c r="T52" s="21" t="s">
         <v>136</v>
       </c>
       <c r="U52" s="21"/>
-      <c r="V52" s="21"/>
+      <c r="V52" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="W52" s="21"/>
-      <c r="X52" s="37"/>
-    </row>
-    <row r="53" spans="1:24" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="X52" s="28"/>
+    </row>
+    <row r="53" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B53" s="26" t="s">
-        <v>149</v>
+        <v>57</v>
       </c>
       <c r="C53" s="21"/>
       <c r="D53" s="21" t="s">
@@ -5128,16 +5286,18 @@
         <v>136</v>
       </c>
       <c r="U53" s="21"/>
-      <c r="V53" s="21"/>
+      <c r="V53" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="W53" s="21"/>
-      <c r="X53" s="37"/>
+      <c r="X53" s="10"/>
     </row>
     <row r="54" spans="1:24" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B54" s="26" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="C54" s="21"/>
       <c r="D54" s="21" t="s">
@@ -5201,7 +5361,7 @@
         <v>43</v>
       </c>
       <c r="B55" s="26" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C55" s="21"/>
       <c r="D55" s="21" t="s">
@@ -5260,58 +5420,76 @@
       <c r="W55" s="21"/>
       <c r="X55" s="37"/>
     </row>
-    <row r="56" spans="1:24" s="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:24" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B56" s="26" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C56" s="21"/>
-      <c r="D56" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="E56" s="17" t="s">
+      <c r="D56" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="E56" s="21" t="s">
         <v>132</v>
       </c>
       <c r="F56" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="G56" s="21"/>
-      <c r="H56" s="21"/>
-      <c r="I56" s="21"/>
+      <c r="G56" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="H56" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="I56" s="21" t="s">
+        <v>132</v>
+      </c>
       <c r="J56" s="21" t="s">
         <v>132</v>
       </c>
       <c r="K56" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="L56" s="21"/>
+      <c r="L56" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="M56" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="N56" s="21"/>
-      <c r="O56" s="21"/>
+      <c r="N56" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="O56" s="21" t="s">
+        <v>132</v>
+      </c>
       <c r="P56" s="21" t="s">
         <v>136</v>
       </c>
       <c r="Q56" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="R56" s="21"/>
-      <c r="S56" s="21"/>
-      <c r="T56" s="21"/>
+      <c r="R56" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="S56" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="T56" s="21" t="s">
+        <v>136</v>
+      </c>
       <c r="U56" s="21"/>
       <c r="V56" s="21"/>
       <c r="W56" s="21"/>
-      <c r="X56" s="34"/>
-    </row>
-    <row r="57" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="X56" s="37"/>
+    </row>
+    <row r="57" spans="1:24" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="26" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="B57" s="26" t="s">
-        <v>59</v>
+        <v>150</v>
       </c>
       <c r="C57" s="21"/>
       <c r="D57" s="21" t="s">
@@ -5365,23 +5543,17 @@
       <c r="T57" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="U57" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="V57" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="U57" s="21"/>
+      <c r="V57" s="21"/>
       <c r="W57" s="21"/>
-      <c r="X57" s="39" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="58" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="X57" s="37"/>
+    </row>
+    <row r="58" spans="1:24" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="26" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="B58" s="26" t="s">
-        <v>61</v>
+        <v>151</v>
       </c>
       <c r="C58" s="21"/>
       <c r="D58" s="21" t="s">
@@ -5435,241 +5607,328 @@
       <c r="T58" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="U58" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="V58" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="U58" s="21"/>
+      <c r="V58" s="21"/>
       <c r="W58" s="21"/>
-      <c r="X58" s="40"/>
-    </row>
-    <row r="59" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="X58" s="37"/>
+    </row>
+    <row r="59" spans="1:24" s="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B59" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="C59" s="21"/>
+      <c r="D59" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="E59" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="F59" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="G59" s="21"/>
+      <c r="H59" s="21"/>
+      <c r="I59" s="21"/>
+      <c r="J59" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="K59" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="L59" s="21"/>
+      <c r="M59" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="N59" s="21"/>
+      <c r="O59" s="21"/>
+      <c r="P59" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q59" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="R59" s="21"/>
+      <c r="S59" s="21"/>
+      <c r="T59" s="21"/>
+      <c r="U59" s="21"/>
+      <c r="V59" s="21"/>
+      <c r="W59" s="21"/>
+      <c r="X59" s="34"/>
+    </row>
+    <row r="60" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A60" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B60" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C60" s="21"/>
+      <c r="D60" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="E60" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="F60" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="G60" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="H60" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="I60" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="J60" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="K60" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="L60" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="M60" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="N60" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="O60" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="P60" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q60" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="R60" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="S60" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="T60" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="U60" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="V60" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="W60" s="21"/>
+      <c r="X60" s="41" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A61" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B61" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C61" s="21"/>
+      <c r="D61" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="E61" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="F61" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="G61" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="H61" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="I61" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="J61" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="K61" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="L61" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="M61" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="N61" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="O61" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="P61" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q61" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="R61" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="S61" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="T61" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="U61" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="V61" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="W61" s="21"/>
+      <c r="X61" s="42"/>
+    </row>
+    <row r="62" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A62" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="B59" s="26" t="s">
+      <c r="B62" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="C59" s="21"/>
-      <c r="D59" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="E59" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="F59" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="G59" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="H59" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="I59" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="J59" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="K59" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="L59" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="M59" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="N59" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="O59" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="P59" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="Q59" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="R59" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="S59" s="21"/>
-      <c r="T59" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="U59" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="V59" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="W59" s="21"/>
-      <c r="X59" s="10"/>
-    </row>
-    <row r="60" spans="1:24" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="B60" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="C60" s="19"/>
-      <c r="D60" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="E60" s="19"/>
-      <c r="F60" s="19"/>
-      <c r="G60" s="19"/>
-      <c r="H60" s="19"/>
-      <c r="I60" s="19"/>
-      <c r="J60" s="19"/>
-      <c r="K60" s="19"/>
-      <c r="L60" s="19"/>
-      <c r="M60" s="19"/>
-      <c r="N60" s="19"/>
-      <c r="O60" s="19"/>
-      <c r="P60" s="19"/>
-      <c r="Q60" s="19"/>
-      <c r="R60" s="19"/>
-      <c r="S60" s="19"/>
-      <c r="T60" s="19"/>
-      <c r="U60" s="19"/>
-      <c r="V60" s="19"/>
-      <c r="W60" s="19"/>
-      <c r="X60" s="14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="61" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A61" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="B61" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="C61" s="17"/>
-      <c r="D61" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="E61" s="17"/>
-      <c r="F61" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="G61" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="H61" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="I61" s="17"/>
-      <c r="J61" s="17"/>
-      <c r="K61" s="17"/>
-      <c r="L61" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="M61" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="N61" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="O61" s="17"/>
-      <c r="P61" s="17"/>
-      <c r="Q61" s="17"/>
-      <c r="R61" s="17"/>
-      <c r="S61" s="17"/>
-      <c r="T61" s="17"/>
-      <c r="U61" s="17"/>
-      <c r="V61" s="17"/>
-      <c r="W61" s="17"/>
-    </row>
-    <row r="62" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A62" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="B62" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="C62" s="17"/>
+      <c r="C62" s="21"/>
       <c r="D62" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="E62" s="17"/>
-      <c r="F62" s="17"/>
-      <c r="G62" s="17"/>
-      <c r="H62" s="17"/>
-      <c r="I62" s="17"/>
-      <c r="J62" s="17"/>
-      <c r="K62" s="17"/>
-      <c r="L62" s="17"/>
-      <c r="M62" s="17"/>
-      <c r="N62" s="17"/>
-      <c r="O62" s="17"/>
-      <c r="P62" s="17"/>
-      <c r="Q62" s="17"/>
-      <c r="R62" s="17"/>
-      <c r="S62" s="17"/>
-      <c r="T62" s="17"/>
-      <c r="U62" s="17"/>
-      <c r="V62" s="17"/>
-      <c r="W62" s="17"/>
-    </row>
-    <row r="63" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="16" t="s">
+      <c r="E62" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="F62" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="G62" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="H62" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="I62" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="J62" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="K62" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="L62" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="M62" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="N62" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="O62" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="P62" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q62" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="R62" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="S62" s="21"/>
+      <c r="T62" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="U62" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="V62" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="W62" s="21"/>
+      <c r="X62" s="10"/>
+    </row>
+    <row r="63" spans="1:24" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A63" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="B63" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="C63" s="17"/>
+      <c r="B63" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C63" s="19"/>
       <c r="D63" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="E63" s="17"/>
-      <c r="F63" s="17"/>
-      <c r="G63" s="17"/>
-      <c r="H63" s="17"/>
-      <c r="I63" s="17"/>
-      <c r="J63" s="17"/>
-      <c r="K63" s="17"/>
-      <c r="L63" s="17"/>
-      <c r="M63" s="17"/>
-      <c r="N63" s="17"/>
-      <c r="O63" s="17"/>
-      <c r="P63" s="17"/>
-      <c r="Q63" s="17"/>
-      <c r="R63" s="17"/>
-      <c r="S63" s="17"/>
-      <c r="T63" s="17"/>
-      <c r="U63" s="17"/>
-      <c r="V63" s="17"/>
-      <c r="W63" s="17"/>
+      <c r="E63" s="19"/>
+      <c r="F63" s="19"/>
+      <c r="G63" s="19"/>
+      <c r="H63" s="19"/>
+      <c r="I63" s="19"/>
+      <c r="J63" s="19"/>
+      <c r="K63" s="19"/>
+      <c r="L63" s="19"/>
+      <c r="M63" s="19"/>
+      <c r="N63" s="19"/>
+      <c r="O63" s="19"/>
+      <c r="P63" s="19"/>
+      <c r="Q63" s="19"/>
+      <c r="R63" s="19"/>
+      <c r="S63" s="19"/>
+      <c r="T63" s="19"/>
+      <c r="U63" s="19"/>
+      <c r="V63" s="19"/>
+      <c r="W63" s="19"/>
+      <c r="X63" s="14" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="64" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="16" t="s">
         <v>63</v>
       </c>
       <c r="B64" s="16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C64" s="17"/>
       <c r="D64" s="21" t="s">
         <v>131</v>
       </c>
       <c r="E64" s="17"/>
-      <c r="F64" s="17"/>
-      <c r="G64" s="17"/>
-      <c r="H64" s="17"/>
+      <c r="F64" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G64" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H64" s="17" t="s">
+        <v>19</v>
+      </c>
       <c r="I64" s="17"/>
       <c r="J64" s="17"/>
       <c r="K64" s="17"/>
-      <c r="L64" s="17"/>
-      <c r="M64" s="17"/>
-      <c r="N64" s="17"/>
+      <c r="L64" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="M64" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="N64" s="17" t="s">
+        <v>19</v>
+      </c>
       <c r="O64" s="17"/>
       <c r="P64" s="17"/>
       <c r="Q64" s="17"/>
@@ -5680,12 +5939,12 @@
       <c r="V64" s="17"/>
       <c r="W64" s="17"/>
     </row>
-    <row r="65" spans="1:23" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="16" t="s">
         <v>63</v>
       </c>
       <c r="B65" s="16" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="C65" s="17"/>
       <c r="D65" s="21" t="s">
@@ -5711,12 +5970,12 @@
       <c r="V65" s="17"/>
       <c r="W65" s="17"/>
     </row>
-    <row r="66" spans="1:23" s="33" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="16" t="s">
         <v>63</v>
       </c>
       <c r="B66" s="16" t="s">
-        <v>129</v>
+        <v>68</v>
       </c>
       <c r="C66" s="17"/>
       <c r="D66" s="21" t="s">
@@ -5744,83 +6003,176 @@
     </row>
     <row r="67" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="16" t="s">
-        <v>110</v>
+        <v>63</v>
       </c>
       <c r="B67" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="C67" s="20"/>
+        <v>69</v>
+      </c>
+      <c r="C67" s="17"/>
       <c r="D67" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="E67" s="20"/>
-      <c r="F67" s="20"/>
-      <c r="G67" s="20"/>
-      <c r="H67" s="20"/>
-      <c r="I67" s="20"/>
-      <c r="J67" s="20"/>
-      <c r="K67" s="20"/>
-      <c r="L67" s="20"/>
-      <c r="M67" s="20"/>
-      <c r="N67" s="20"/>
-      <c r="O67" s="20"/>
-      <c r="P67" s="20"/>
-      <c r="Q67" s="20"/>
-      <c r="R67" s="20"/>
-      <c r="S67" s="20"/>
-      <c r="T67" s="20"/>
-      <c r="U67" s="20"/>
-      <c r="V67" s="20"/>
-      <c r="W67" s="20"/>
-    </row>
-    <row r="68" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E67" s="17"/>
+      <c r="F67" s="17"/>
+      <c r="G67" s="17"/>
+      <c r="H67" s="17"/>
+      <c r="I67" s="17"/>
+      <c r="J67" s="17"/>
+      <c r="K67" s="17"/>
+      <c r="L67" s="17"/>
+      <c r="M67" s="17"/>
+      <c r="N67" s="17"/>
+      <c r="O67" s="17"/>
+      <c r="P67" s="17"/>
+      <c r="Q67" s="17"/>
+      <c r="R67" s="17"/>
+      <c r="S67" s="17"/>
+      <c r="T67" s="17"/>
+      <c r="U67" s="17"/>
+      <c r="V67" s="17"/>
+      <c r="W67" s="17"/>
+    </row>
+    <row r="68" spans="1:23" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B68" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C68" s="17"/>
+      <c r="D68" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="E68" s="17"/>
+      <c r="F68" s="17"/>
+      <c r="G68" s="17"/>
+      <c r="H68" s="17"/>
+      <c r="I68" s="17"/>
+      <c r="J68" s="17"/>
+      <c r="K68" s="17"/>
+      <c r="L68" s="17"/>
+      <c r="M68" s="17"/>
+      <c r="N68" s="17"/>
+      <c r="O68" s="17"/>
+      <c r="P68" s="17"/>
+      <c r="Q68" s="17"/>
+      <c r="R68" s="17"/>
+      <c r="S68" s="17"/>
+      <c r="T68" s="17"/>
+      <c r="U68" s="17"/>
+      <c r="V68" s="17"/>
+      <c r="W68" s="17"/>
+    </row>
+    <row r="69" spans="1:23" s="33" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A69" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B69" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="C69" s="17"/>
+      <c r="D69" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="E69" s="17"/>
+      <c r="F69" s="17"/>
+      <c r="G69" s="17"/>
+      <c r="H69" s="17"/>
+      <c r="I69" s="17"/>
+      <c r="J69" s="17"/>
+      <c r="K69" s="17"/>
+      <c r="L69" s="17"/>
+      <c r="M69" s="17"/>
+      <c r="N69" s="17"/>
+      <c r="O69" s="17"/>
+      <c r="P69" s="17"/>
+      <c r="Q69" s="17"/>
+      <c r="R69" s="17"/>
+      <c r="S69" s="17"/>
+      <c r="T69" s="17"/>
+      <c r="U69" s="17"/>
+      <c r="V69" s="17"/>
+      <c r="W69" s="17"/>
+    </row>
+    <row r="70" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A70" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B70" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="C70" s="20"/>
+      <c r="D70" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="E70" s="20"/>
+      <c r="F70" s="20"/>
+      <c r="G70" s="20"/>
+      <c r="H70" s="20"/>
+      <c r="I70" s="20"/>
+      <c r="J70" s="20"/>
+      <c r="K70" s="20"/>
+      <c r="L70" s="20"/>
+      <c r="M70" s="20"/>
+      <c r="N70" s="20"/>
+      <c r="O70" s="20"/>
+      <c r="P70" s="20"/>
+      <c r="Q70" s="20"/>
+      <c r="R70" s="20"/>
+      <c r="S70" s="20"/>
+      <c r="T70" s="20"/>
+      <c r="U70" s="20"/>
+      <c r="V70" s="20"/>
+      <c r="W70" s="20"/>
+    </row>
+    <row r="71" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A71" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="B68" s="16" t="s">
+      <c r="B71" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="C68" s="20"/>
-      <c r="D68" s="21" t="s">
+      <c r="C71" s="20"/>
+      <c r="D71" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="E68" s="30" t="s">
+      <c r="E71" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="F68" s="30"/>
-      <c r="G68" s="30" t="s">
+      <c r="F71" s="30"/>
+      <c r="G71" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="H68" s="30"/>
-      <c r="I68" s="30"/>
-      <c r="J68" s="30" t="s">
+      <c r="H71" s="30"/>
+      <c r="I71" s="30"/>
+      <c r="J71" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="K68" s="30" t="s">
+      <c r="K71" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="L68" s="30" t="s">
+      <c r="L71" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="M68" s="30" t="s">
+      <c r="M71" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="N68" s="30"/>
-      <c r="O68" s="30"/>
-      <c r="P68" s="30"/>
-      <c r="Q68" s="30"/>
-      <c r="R68" s="30"/>
-      <c r="S68" s="30"/>
-      <c r="T68" s="30"/>
-      <c r="U68" s="30"/>
-      <c r="V68" s="30"/>
-      <c r="W68" s="30"/>
+      <c r="N71" s="30"/>
+      <c r="O71" s="30"/>
+      <c r="P71" s="30"/>
+      <c r="Q71" s="30"/>
+      <c r="R71" s="30"/>
+      <c r="S71" s="30"/>
+      <c r="T71" s="30"/>
+      <c r="U71" s="30"/>
+      <c r="V71" s="30"/>
+      <c r="W71" s="30"/>
     </row>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C12" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="E28" sqref="E28"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C29" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="W33" sqref="W33"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -5838,7 +6190,7 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="6">
-    <mergeCell ref="X57:X58"/>
+    <mergeCell ref="X60:X61"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="J5:N5"/>
     <mergeCell ref="P5:V5"/>

</xml_diff>

<commit_message>
Lisää myös JVH:lle oikeudet toteutus-välilehdelle
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="32960" windowHeight="12040" tabRatio="500"/>
+    <workbookView xWindow="7420" yWindow="5600" windowWidth="38660" windowHeight="21040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -17,9 +17,9 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="1648" windowHeight="429" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="1933" windowHeight="879" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
-    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="158">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -968,7 +968,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{BF824A78-D4D3-104B-A2EF-6CDB88CD119F}" diskRevisions="1" revisionId="89" version="14">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{7E57EE25-C312-2947-AB26-89F9CE326DBC}" diskRevisions="1" revisionId="92" version="15">
   <header guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" dateTime="2016-09-06T09:14:56" maxSheetId="3" userName="Tatu Tarvainen" r:id="rId2" minRId="1" maxRId="3">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1047,6 +1047,12 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{7E57EE25-C312-2947-AB26-89F9CE326DBC}" dateTime="2016-10-26T11:00:39" maxSheetId="3" userName="Microsoft Office User" r:id="rId15" minRId="90" maxRId="92">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -3085,6 +3091,34 @@
       </ndxf>
     </rcc>
   </rrc>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="delete"/>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog14.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="90" sId="1">
+    <nc r="D33" t="inlineStr">
+      <is>
+        <t>R*,W*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="91" sId="1">
+    <nc r="D34" t="inlineStr">
+      <is>
+        <t>R*,W*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="92" sId="1">
+    <nc r="D35" t="inlineStr">
+      <is>
+        <t>R*,W*</t>
+      </is>
+    </nc>
+  </rcc>
   <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="delete"/>
   <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="add"/>
 </revisions>
@@ -4179,10 +4213,10 @@
   <dimension ref="A1:W71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="S33" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C22" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="W1" sqref="W1:W1048576"/>
+      <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5838,7 +5872,9 @@
         <v>155</v>
       </c>
       <c r="C33" s="21"/>
-      <c r="D33" s="17"/>
+      <c r="D33" s="17" t="s">
+        <v>127</v>
+      </c>
       <c r="E33" s="17"/>
       <c r="F33" s="21"/>
       <c r="G33" s="21"/>
@@ -5874,7 +5910,9 @@
         <v>156</v>
       </c>
       <c r="C34" s="21"/>
-      <c r="D34" s="17"/>
+      <c r="D34" s="17" t="s">
+        <v>127</v>
+      </c>
       <c r="E34" s="17"/>
       <c r="F34" s="21"/>
       <c r="G34" s="21"/>
@@ -5910,7 +5948,9 @@
         <v>157</v>
       </c>
       <c r="C35" s="21"/>
-      <c r="D35" s="17"/>
+      <c r="D35" s="17" t="s">
+        <v>127</v>
+      </c>
       <c r="E35" s="17"/>
       <c r="F35" s="21"/>
       <c r="G35" s="21"/>
@@ -7853,20 +7893,20 @@
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="S33" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="W1" sqref="W1:W1048576"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C22" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
+      <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
     <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
       <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="E7" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="bottomRight" activeCell="L57" sqref="L57:L59"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
-      <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -8197,12 +8237,12 @@
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
+    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
       <selection activeCell="C7" sqref="C7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
       <selection activeCell="C7" sqref="C7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Lisää oikeuksia rooli exceliin
Lisätty raportti Muutos- ja Lisätyöt

Lisätty oikeuksia Tiemerkinnän Toteutus-osioon kolmelle riville.
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarihan/Desktop/Harja/harja/resources/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7420" yWindow="5600" windowWidth="38660" windowHeight="21040" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-900" windowWidth="47580" windowHeight="26980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -17,23 +12,23 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="2379" windowHeight="1295" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
+    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="1933" windowHeight="879" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
   </customWorkbookViews>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="159">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -507,6 +502,9 @@
   </si>
   <si>
     <t>Toteutus / Muut työt</t>
+  </si>
+  <si>
+    <t>Muutos- ja lisätyöt</t>
   </si>
 </sst>
 </file>
@@ -623,7 +621,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="125">
+  <cellStyleXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -749,8 +747,30 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -821,6 +841,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -830,7 +854,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="125">
+  <cellStyles count="147">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -893,6 +917,17 @@
     <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -955,6 +990,17 @@
     <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -968,7 +1014,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{7E57EE25-C312-2947-AB26-89F9CE326DBC}" diskRevisions="1" revisionId="92" version="15">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{C606B059-99AC-3B47-8437-66D15B4E3D4B}" diskRevisions="1" revisionId="141" version="18">
   <header guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" dateTime="2016-09-06T09:14:56" maxSheetId="3" userName="Tatu Tarvainen" r:id="rId2" minRId="1" maxRId="3">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1053,6 +1099,24 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{2CE52D2A-1823-3948-9783-B30824F1800B}" dateTime="2016-10-27T09:36:14" maxSheetId="3" userName="Jarno Väyrynen" r:id="rId16" minRId="93" maxRId="119">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{7A420D3A-E414-F648-B986-850F97011CC0}" dateTime="2016-10-27T09:37:30" maxSheetId="3" userName="Jarno Väyrynen" r:id="rId17" minRId="120" maxRId="141">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{C606B059-99AC-3B47-8437-66D15B4E3D4B}" dateTime="2016-10-27T09:57:11" maxSheetId="3" userName="Jarno Väyrynen" r:id="rId18">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -3124,6 +3188,358 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog15.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="93" sId="1">
+    <nc r="E33" t="inlineStr">
+      <is>
+        <t>R*,W</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="94" sId="1">
+    <nc r="E34" t="inlineStr">
+      <is>
+        <t>R*,W</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="95" sId="1">
+    <nc r="E35" t="inlineStr">
+      <is>
+        <t>R*,W</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="96" sId="1">
+    <nc r="F33" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="97" sId="1">
+    <nc r="F34" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="98" sId="1">
+    <nc r="F35" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="99" sId="1">
+    <nc r="H33" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="100" sId="1">
+    <nc r="H34" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="101" sId="1">
+    <nc r="H35" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="102" sId="1">
+    <nc r="I33" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="103" sId="1">
+    <nc r="I34" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="104" sId="1">
+    <nc r="I35" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="105" sId="1">
+    <nc r="M33" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="106" sId="1">
+    <nc r="M34" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="107" sId="1">
+    <nc r="M35" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="108" sId="1">
+    <nc r="N33" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="109" sId="1">
+    <nc r="N34" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="110" sId="1">
+    <nc r="N35" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="111" sId="1">
+    <nc r="R33" t="inlineStr">
+      <is>
+        <t>R+</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="112" sId="1">
+    <nc r="R34" t="inlineStr">
+      <is>
+        <t>R+</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="113" sId="1">
+    <nc r="R35" t="inlineStr">
+      <is>
+        <t>R+</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="114" sId="1">
+    <nc r="S33" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="115" sId="1">
+    <nc r="S34" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="116" sId="1">
+    <nc r="S35" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="117" sId="1">
+    <nc r="T33" t="inlineStr">
+      <is>
+        <t>R+</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="118" sId="1">
+    <nc r="T34" t="inlineStr">
+      <is>
+        <t>R+</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="119" sId="1">
+    <nc r="T35" t="inlineStr">
+      <is>
+        <t>R+</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" action="delete"/>
+  <rcv guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog16.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="120" sId="1" ref="A43:XFD43" action="insertRow"/>
+  <rrc rId="121" sId="1" ref="A44:XFD44" action="insertRow"/>
+  <rcc rId="122" sId="1">
+    <nc r="A44" t="inlineStr">
+      <is>
+        <t>Raportit</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="123" sId="1">
+    <nc r="B44" t="inlineStr">
+      <is>
+        <t>Muutos- ja lisätyöt</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="124" sId="1">
+    <nc r="D44" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="125" sId="1">
+    <nc r="E44" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="126" sId="1">
+    <nc r="F44" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="127" sId="1">
+    <nc r="G44" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="128" sId="1">
+    <nc r="H44" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="129" sId="1">
+    <nc r="I44" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="130" sId="1">
+    <nc r="J44" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="131" sId="1">
+    <nc r="K44" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="132" sId="1">
+    <nc r="L44" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="133" sId="1">
+    <nc r="M44" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="134" sId="1">
+    <nc r="N44" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="135" sId="1">
+    <nc r="O44" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="136" sId="1">
+    <nc r="P44" t="inlineStr">
+      <is>
+        <t>R+</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="137" sId="1">
+    <nc r="Q44" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="138" sId="1">
+    <nc r="R44" t="inlineStr">
+      <is>
+        <t>R+</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="139" sId="1">
+    <nc r="S44" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="140" sId="1">
+    <nc r="T44" t="inlineStr">
+      <is>
+        <t>R+</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="141" sId="1">
+    <nc r="V44" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" action="delete"/>
+  <rcv guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog17.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcv guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" action="delete"/>
+  <rcv guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="1" sId="1">
@@ -3880,11 +4296,12 @@
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="4">
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="5">
   <userInfo guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" name="Tatu Tarvainen" id="-130145201" dateTime="2016-09-06T09:10:23"/>
   <userInfo guid="{E0850D7E-A93F-EF44-B46A-3BEA4D7DBEDB}" name="Jarno Väyrynen" id="-589116405" dateTime="2016-09-06T12:54:09"/>
   <userInfo guid="{0407E191-78DA-F349-B5E5-8AE1BC03A29E}" name="Jarno Väyrynen" id="-589108428" dateTime="2016-09-08T15:33:24"/>
   <userInfo guid="{F8907045-3B30-0A43-A905-F167D27F9989}" name="Jarno Väyrynen" id="-589157736" dateTime="2016-09-27T15:27:41"/>
+  <userInfo guid="{C606B059-99AC-3B47-8437-66D15B4E3D4B}" name="Jarno Väyrynen" id="-589137240" dateTime="2016-10-27T09:33:01"/>
 </users>
 </file>
 
@@ -4210,16 +4627,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W71"/>
+  <dimension ref="A1:W72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C22" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
+      <pane xSplit="2" ySplit="6" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
+      <selection pane="bottomRight" activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.5" bestFit="1" customWidth="1"/>
@@ -4245,45 +4662,45 @@
     <col min="23" max="23" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="24" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:23" ht="24" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="45" t="s">
         <v>152</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-    </row>
-    <row r="2" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+    </row>
+    <row r="2" spans="1:23" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="45" t="s">
+      <c r="C2" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-    </row>
-    <row r="3" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+    </row>
+    <row r="3" spans="1:23" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -4298,39 +4715,39 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:23" ht="15.75" customHeight="1">
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C5" s="42" t="s">
+    <row r="5" spans="1:23" ht="15.75" customHeight="1">
+      <c r="C5" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="J5" s="42" t="s">
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="J5" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="41"/>
-      <c r="L5" s="41"/>
-      <c r="M5" s="41"/>
-      <c r="N5" s="41"/>
-      <c r="P5" s="42" t="s">
+      <c r="K5" s="43"/>
+      <c r="L5" s="43"/>
+      <c r="M5" s="43"/>
+      <c r="N5" s="43"/>
+      <c r="P5" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="Q5" s="41"/>
-      <c r="R5" s="41"/>
-      <c r="S5" s="41"/>
-      <c r="T5" s="41"/>
-      <c r="U5" s="41"/>
-      <c r="V5" s="41"/>
+      <c r="Q5" s="43"/>
+      <c r="R5" s="43"/>
+      <c r="S5" s="43"/>
+      <c r="T5" s="43"/>
+      <c r="U5" s="43"/>
+      <c r="V5" s="43"/>
       <c r="W5" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:23" ht="15.75" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
@@ -4396,7 +4813,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:23" ht="15.75" customHeight="1">
       <c r="A7" s="16" t="s">
         <v>15</v>
       </c>
@@ -4463,7 +4880,7 @@
       </c>
       <c r="W7" s="10"/>
     </row>
-    <row r="8" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:23" ht="15.75" customHeight="1">
       <c r="A8" s="16" t="s">
         <v>15</v>
       </c>
@@ -4516,7 +4933,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:23" ht="15.75" customHeight="1">
       <c r="A9" s="16" t="s">
         <v>15</v>
       </c>
@@ -4563,7 +4980,7 @@
       <c r="V9" s="17"/>
       <c r="W9" s="10"/>
     </row>
-    <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:23" ht="15.75" customHeight="1">
       <c r="A10" s="16" t="s">
         <v>15</v>
       </c>
@@ -4610,7 +5027,7 @@
       <c r="V10" s="17"/>
       <c r="W10" s="10"/>
     </row>
-    <row r="11" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:23" ht="15.75" customHeight="1">
       <c r="A11" s="16" t="s">
         <v>15</v>
       </c>
@@ -4671,7 +5088,7 @@
       <c r="V11" s="17"/>
       <c r="W11" s="10"/>
     </row>
-    <row r="12" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:23" ht="15.75" customHeight="1">
       <c r="A12" s="16" t="s">
         <v>15</v>
       </c>
@@ -4732,7 +5149,7 @@
       <c r="V12" s="17"/>
       <c r="W12" s="10"/>
     </row>
-    <row r="13" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:23" ht="15.75" customHeight="1">
       <c r="A13" s="16" t="s">
         <v>15</v>
       </c>
@@ -4779,7 +5196,7 @@
       <c r="V13" s="17"/>
       <c r="W13" s="10"/>
     </row>
-    <row r="14" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:23" ht="15.75" customHeight="1">
       <c r="A14" s="16" t="s">
         <v>15</v>
       </c>
@@ -4826,7 +5243,7 @@
       <c r="V14" s="17"/>
       <c r="W14" s="10"/>
     </row>
-    <row r="15" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:23" ht="15.75" customHeight="1">
       <c r="A15" s="16" t="s">
         <v>15</v>
       </c>
@@ -4873,7 +5290,7 @@
       <c r="V15" s="17"/>
       <c r="W15" s="10"/>
     </row>
-    <row r="16" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:23" ht="15.75" customHeight="1">
       <c r="A16" s="16" t="s">
         <v>15</v>
       </c>
@@ -4934,7 +5351,7 @@
       <c r="V16" s="17"/>
       <c r="W16" s="10"/>
     </row>
-    <row r="17" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:23" ht="15.75" customHeight="1">
       <c r="A17" s="16" t="s">
         <v>15</v>
       </c>
@@ -4995,7 +5412,7 @@
       <c r="V17" s="17"/>
       <c r="W17" s="10"/>
     </row>
-    <row r="18" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:23" ht="15.75" customHeight="1">
       <c r="A18" s="16" t="s">
         <v>15</v>
       </c>
@@ -5042,7 +5459,7 @@
       <c r="V18" s="17"/>
       <c r="W18" s="10"/>
     </row>
-    <row r="19" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:23" ht="15.75" customHeight="1">
       <c r="A19" s="16" t="s">
         <v>15</v>
       </c>
@@ -5103,7 +5520,7 @@
       <c r="V19" s="17"/>
       <c r="W19" s="10"/>
     </row>
-    <row r="20" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:23" ht="15.75" customHeight="1">
       <c r="A20" s="16" t="s">
         <v>15</v>
       </c>
@@ -5170,7 +5587,7 @@
       </c>
       <c r="W20" s="10"/>
     </row>
-    <row r="21" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:23" ht="15.75" customHeight="1">
       <c r="A21" s="26" t="s">
         <v>15</v>
       </c>
@@ -5237,7 +5654,7 @@
       </c>
       <c r="W21" s="10"/>
     </row>
-    <row r="22" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:23" ht="15.75" customHeight="1">
       <c r="A22" s="26" t="s">
         <v>15</v>
       </c>
@@ -5302,7 +5719,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="23" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:23" ht="15.75" customHeight="1">
       <c r="A23" s="26" t="s">
         <v>15</v>
       </c>
@@ -5367,7 +5784,7 @@
       </c>
       <c r="W23" s="10"/>
     </row>
-    <row r="24" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:23" ht="15.75" customHeight="1">
       <c r="A24" s="26" t="s">
         <v>15</v>
       </c>
@@ -5430,7 +5847,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="25" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:23" ht="15.75" customHeight="1">
       <c r="A25" s="26" t="s">
         <v>15</v>
       </c>
@@ -5485,7 +5902,7 @@
       </c>
       <c r="W25" s="10"/>
     </row>
-    <row r="26" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:23" ht="15.75" customHeight="1">
       <c r="A26" s="26" t="s">
         <v>15</v>
       </c>
@@ -5532,7 +5949,7 @@
       <c r="V26" s="21"/>
       <c r="W26" s="10"/>
     </row>
-    <row r="27" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:23" ht="15.75" customHeight="1">
       <c r="A27" s="26" t="s">
         <v>15</v>
       </c>
@@ -5571,7 +5988,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:23" ht="15.75" customHeight="1">
       <c r="A28" s="26" t="s">
         <v>15</v>
       </c>
@@ -5634,7 +6051,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="29" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:23" ht="15.75" customHeight="1">
       <c r="A29" s="26" t="s">
         <v>15</v>
       </c>
@@ -5691,7 +6108,7 @@
       <c r="V29" s="21"/>
       <c r="W29" s="10"/>
     </row>
-    <row r="30" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:23" ht="15.75" customHeight="1">
       <c r="A30" s="26" t="s">
         <v>15</v>
       </c>
@@ -5750,7 +6167,7 @@
       <c r="V30" s="21"/>
       <c r="W30" s="10"/>
     </row>
-    <row r="31" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:23" ht="15.75" customHeight="1">
       <c r="A31" s="26" t="s">
         <v>15</v>
       </c>
@@ -5807,7 +6224,7 @@
       <c r="V31" s="21"/>
       <c r="W31" s="10"/>
     </row>
-    <row r="32" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:23" ht="15.75" customHeight="1">
       <c r="A32" s="26" t="s">
         <v>15</v>
       </c>
@@ -5864,7 +6281,7 @@
       <c r="V32" s="21"/>
       <c r="W32" s="10"/>
     </row>
-    <row r="33" spans="1:23" s="39" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:23" s="39" customFormat="1" ht="15.75" customHeight="1">
       <c r="A33" s="26" t="s">
         <v>15</v>
       </c>
@@ -5875,11 +6292,19 @@
       <c r="D33" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="E33" s="17"/>
-      <c r="F33" s="21"/>
+      <c r="E33" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="F33" s="21" t="s">
+        <v>128</v>
+      </c>
       <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="21"/>
+      <c r="H33" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="I33" s="21" t="s">
+        <v>128</v>
+      </c>
       <c r="J33" s="17" t="s">
         <v>127</v>
       </c>
@@ -5887,8 +6312,12 @@
         <v>131</v>
       </c>
       <c r="L33" s="21"/>
-      <c r="M33" s="21"/>
-      <c r="N33" s="17"/>
+      <c r="M33" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="N33" s="17" t="s">
+        <v>128</v>
+      </c>
       <c r="O33" s="17"/>
       <c r="P33" s="21" t="s">
         <v>133</v>
@@ -5896,13 +6325,19 @@
       <c r="Q33" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="R33" s="21"/>
-      <c r="S33" s="21"/>
-      <c r="T33" s="17"/>
+      <c r="R33" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="S33" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="T33" s="17" t="s">
+        <v>132</v>
+      </c>
       <c r="U33" s="21"/>
       <c r="V33" s="21"/>
     </row>
-    <row r="34" spans="1:23" s="39" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:23" s="39" customFormat="1" ht="15.75" customHeight="1">
       <c r="A34" s="26" t="s">
         <v>15</v>
       </c>
@@ -5913,11 +6348,19 @@
       <c r="D34" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="E34" s="17"/>
-      <c r="F34" s="21"/>
+      <c r="E34" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="F34" s="21" t="s">
+        <v>128</v>
+      </c>
       <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="21"/>
+      <c r="H34" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="I34" s="21" t="s">
+        <v>128</v>
+      </c>
       <c r="J34" s="17" t="s">
         <v>127</v>
       </c>
@@ -5925,8 +6368,12 @@
         <v>131</v>
       </c>
       <c r="L34" s="21"/>
-      <c r="M34" s="21"/>
-      <c r="N34" s="17"/>
+      <c r="M34" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="N34" s="17" t="s">
+        <v>128</v>
+      </c>
       <c r="O34" s="17"/>
       <c r="P34" s="21" t="s">
         <v>133</v>
@@ -5934,13 +6381,19 @@
       <c r="Q34" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="R34" s="21"/>
-      <c r="S34" s="21"/>
-      <c r="T34" s="17"/>
+      <c r="R34" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="S34" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="T34" s="17" t="s">
+        <v>132</v>
+      </c>
       <c r="U34" s="21"/>
       <c r="V34" s="21"/>
     </row>
-    <row r="35" spans="1:23" s="39" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:23" s="39" customFormat="1" ht="15.75" customHeight="1">
       <c r="A35" s="26" t="s">
         <v>15</v>
       </c>
@@ -5951,11 +6404,19 @@
       <c r="D35" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="E35" s="17"/>
-      <c r="F35" s="21"/>
+      <c r="E35" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="F35" s="21" t="s">
+        <v>128</v>
+      </c>
       <c r="G35" s="21"/>
-      <c r="H35" s="21"/>
-      <c r="I35" s="21"/>
+      <c r="H35" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="I35" s="21" t="s">
+        <v>128</v>
+      </c>
       <c r="J35" s="17" t="s">
         <v>127</v>
       </c>
@@ -5963,8 +6424,12 @@
         <v>131</v>
       </c>
       <c r="L35" s="21"/>
-      <c r="M35" s="21"/>
-      <c r="N35" s="17"/>
+      <c r="M35" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="N35" s="17" t="s">
+        <v>128</v>
+      </c>
       <c r="O35" s="17"/>
       <c r="P35" s="21" t="s">
         <v>133</v>
@@ -5972,13 +6437,19 @@
       <c r="Q35" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="R35" s="21"/>
-      <c r="S35" s="21"/>
-      <c r="T35" s="17"/>
+      <c r="R35" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="S35" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="T35" s="17" t="s">
+        <v>132</v>
+      </c>
       <c r="U35" s="21"/>
       <c r="V35" s="21"/>
     </row>
-    <row r="36" spans="1:23" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:23" s="13" customFormat="1" ht="15.75" customHeight="1">
       <c r="A36" s="26" t="s">
         <v>15</v>
       </c>
@@ -6045,7 +6516,7 @@
       </c>
       <c r="W36" s="12"/>
     </row>
-    <row r="37" spans="1:23" s="32" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:23" s="32" customFormat="1" ht="15.75" customHeight="1">
       <c r="A37" s="26" t="s">
         <v>43</v>
       </c>
@@ -6092,7 +6563,7 @@
       <c r="V37" s="21"/>
       <c r="W37" s="31"/>
     </row>
-    <row r="38" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:23" ht="15.75" customHeight="1">
       <c r="A38" s="26" t="s">
         <v>43</v>
       </c>
@@ -6141,7 +6612,7 @@
       <c r="V38" s="21"/>
       <c r="W38" s="10"/>
     </row>
-    <row r="39" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:23" ht="15.75" customHeight="1">
       <c r="A39" s="26" t="s">
         <v>43</v>
       </c>
@@ -6206,7 +6677,7 @@
       </c>
       <c r="W39" s="10"/>
     </row>
-    <row r="40" spans="1:23" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:23" s="38" customFormat="1" ht="15.75" customHeight="1">
       <c r="A40" s="26" t="s">
         <v>43</v>
       </c>
@@ -6273,7 +6744,7 @@
       </c>
       <c r="W40" s="37"/>
     </row>
-    <row r="41" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:23" ht="15.75" customHeight="1">
       <c r="A41" s="26" t="s">
         <v>43</v>
       </c>
@@ -6338,7 +6809,7 @@
       </c>
       <c r="W41" s="10"/>
     </row>
-    <row r="42" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:23" ht="15.75" customHeight="1">
       <c r="A42" s="26" t="s">
         <v>43</v>
       </c>
@@ -6403,7 +6874,7 @@
       </c>
       <c r="W42" s="10"/>
     </row>
-    <row r="43" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:23" ht="15.75" customHeight="1">
       <c r="A43" s="26" t="s">
         <v>43</v>
       </c>
@@ -6468,12 +6939,12 @@
       </c>
       <c r="W43" s="10"/>
     </row>
-    <row r="44" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:23" s="41" customFormat="1" ht="15.75" customHeight="1">
       <c r="A44" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B44" s="26" t="s">
-        <v>49</v>
+        <v>158</v>
       </c>
       <c r="C44" s="21"/>
       <c r="D44" s="21" t="s">
@@ -6531,14 +7002,14 @@
       <c r="V44" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="W44" s="10"/>
-    </row>
-    <row r="45" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="W44" s="40"/>
+    </row>
+    <row r="45" spans="1:23" ht="15.75" customHeight="1">
       <c r="A45" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B45" s="26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C45" s="21"/>
       <c r="D45" s="21" t="s">
@@ -6571,7 +7042,9 @@
       <c r="M45" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="N45" s="21"/>
+      <c r="N45" s="21" t="s">
+        <v>128</v>
+      </c>
       <c r="O45" s="21" t="s">
         <v>128</v>
       </c>
@@ -6584,7 +7057,9 @@
       <c r="R45" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="S45" s="21"/>
+      <c r="S45" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="T45" s="21" t="s">
         <v>132</v>
       </c>
@@ -6594,12 +7069,12 @@
       </c>
       <c r="W45" s="10"/>
     </row>
-    <row r="46" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:23" ht="15.75" customHeight="1">
       <c r="A46" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B46" s="26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C46" s="21"/>
       <c r="D46" s="21" t="s">
@@ -6632,9 +7107,7 @@
       <c r="M46" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="N46" s="21" t="s">
-        <v>128</v>
-      </c>
+      <c r="N46" s="21"/>
       <c r="O46" s="21" t="s">
         <v>128</v>
       </c>
@@ -6647,9 +7120,7 @@
       <c r="R46" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="S46" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="S46" s="21"/>
       <c r="T46" s="21" t="s">
         <v>132</v>
       </c>
@@ -6659,12 +7130,12 @@
       </c>
       <c r="W46" s="10"/>
     </row>
-    <row r="47" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:23" ht="15.75" customHeight="1">
       <c r="A47" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B47" s="26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C47" s="21"/>
       <c r="D47" s="21" t="s">
@@ -6676,8 +7147,12 @@
       <c r="F47" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="G47" s="21"/>
-      <c r="H47" s="21"/>
+      <c r="G47" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="H47" s="21" t="s">
+        <v>128</v>
+      </c>
       <c r="I47" s="21" t="s">
         <v>128</v>
       </c>
@@ -6687,11 +7162,15 @@
       <c r="K47" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="L47" s="21"/>
+      <c r="L47" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="M47" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="N47" s="21"/>
+      <c r="N47" s="21" t="s">
+        <v>128</v>
+      </c>
       <c r="O47" s="21" t="s">
         <v>128</v>
       </c>
@@ -6704,7 +7183,9 @@
       <c r="R47" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="S47" s="21"/>
+      <c r="S47" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="T47" s="21" t="s">
         <v>132</v>
       </c>
@@ -6714,12 +7195,12 @@
       </c>
       <c r="W47" s="10"/>
     </row>
-    <row r="48" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:23" ht="15.75" customHeight="1">
       <c r="A48" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B48" s="26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C48" s="21"/>
       <c r="D48" s="21" t="s">
@@ -6732,10 +7213,10 @@
         <v>128</v>
       </c>
       <c r="G48" s="21"/>
-      <c r="H48" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="I48" s="21"/>
+      <c r="H48" s="21"/>
+      <c r="I48" s="21" t="s">
+        <v>128</v>
+      </c>
       <c r="J48" s="21" t="s">
         <v>128</v>
       </c>
@@ -6746,31 +7227,35 @@
       <c r="M48" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="N48" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="O48" s="21"/>
+      <c r="N48" s="21"/>
+      <c r="O48" s="21" t="s">
+        <v>128</v>
+      </c>
       <c r="P48" s="21" t="s">
         <v>132</v>
       </c>
       <c r="Q48" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="R48" s="21"/>
+      <c r="R48" s="21" t="s">
+        <v>132</v>
+      </c>
       <c r="S48" s="21"/>
       <c r="T48" s="21" t="s">
         <v>132</v>
       </c>
       <c r="U48" s="21"/>
-      <c r="V48" s="21"/>
+      <c r="V48" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="W48" s="10"/>
     </row>
-    <row r="49" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:23" ht="15.75" customHeight="1">
       <c r="A49" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B49" s="26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C49" s="21"/>
       <c r="D49" s="21" t="s">
@@ -6783,7 +7268,9 @@
         <v>128</v>
       </c>
       <c r="G49" s="21"/>
-      <c r="H49" s="21"/>
+      <c r="H49" s="21" t="s">
+        <v>19</v>
+      </c>
       <c r="I49" s="21"/>
       <c r="J49" s="21" t="s">
         <v>128</v>
@@ -6795,7 +7282,9 @@
       <c r="M49" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="N49" s="21"/>
+      <c r="N49" s="21" t="s">
+        <v>19</v>
+      </c>
       <c r="O49" s="21"/>
       <c r="P49" s="21" t="s">
         <v>132</v>
@@ -6812,12 +7301,12 @@
       <c r="V49" s="21"/>
       <c r="W49" s="10"/>
     </row>
-    <row r="50" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:23" ht="15.75" customHeight="1">
       <c r="A50" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B50" s="26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C50" s="21"/>
       <c r="D50" s="21" t="s">
@@ -6859,12 +7348,12 @@
       <c r="V50" s="21"/>
       <c r="W50" s="10"/>
     </row>
-    <row r="51" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:23" ht="15.75" customHeight="1">
       <c r="A51" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B51" s="26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C51" s="21"/>
       <c r="D51" s="21" t="s">
@@ -6906,12 +7395,12 @@
       <c r="V51" s="21"/>
       <c r="W51" s="10"/>
     </row>
-    <row r="52" spans="1:23" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:23" ht="15.75" customHeight="1">
       <c r="A52" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B52" s="26" t="s">
-        <v>122</v>
+        <v>56</v>
       </c>
       <c r="C52" s="21"/>
       <c r="D52" s="21" t="s">
@@ -6923,56 +7412,42 @@
       <c r="F52" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="G52" s="21" t="s">
-        <v>128</v>
-      </c>
-      <c r="H52" s="21" t="s">
-        <v>128</v>
-      </c>
-      <c r="I52" s="21" t="s">
-        <v>128</v>
-      </c>
+      <c r="G52" s="21"/>
+      <c r="H52" s="21"/>
+      <c r="I52" s="21"/>
       <c r="J52" s="21" t="s">
         <v>128</v>
       </c>
       <c r="K52" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="L52" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="L52" s="21"/>
       <c r="M52" s="21" t="s">
         <v>128</v>
       </c>
       <c r="N52" s="21"/>
-      <c r="O52" s="21" t="s">
-        <v>128</v>
-      </c>
+      <c r="O52" s="21"/>
       <c r="P52" s="21" t="s">
         <v>132</v>
       </c>
       <c r="Q52" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="R52" s="21" t="s">
-        <v>132</v>
-      </c>
+      <c r="R52" s="21"/>
       <c r="S52" s="21"/>
       <c r="T52" s="21" t="s">
         <v>132</v>
       </c>
       <c r="U52" s="21"/>
-      <c r="V52" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="W52" s="28"/>
-    </row>
-    <row r="53" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="V52" s="21"/>
+      <c r="W52" s="10"/>
+    </row>
+    <row r="53" spans="1:23" s="29" customFormat="1" ht="15.75" customHeight="1">
       <c r="A53" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B53" s="26" t="s">
-        <v>57</v>
+        <v>122</v>
       </c>
       <c r="C53" s="21"/>
       <c r="D53" s="21" t="s">
@@ -7005,9 +7480,7 @@
       <c r="M53" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="N53" s="21" t="s">
-        <v>128</v>
-      </c>
+      <c r="N53" s="21"/>
       <c r="O53" s="21" t="s">
         <v>128</v>
       </c>
@@ -7020,9 +7493,7 @@
       <c r="R53" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="S53" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="S53" s="21"/>
       <c r="T53" s="21" t="s">
         <v>132</v>
       </c>
@@ -7030,14 +7501,14 @@
       <c r="V53" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="W53" s="10"/>
-    </row>
-    <row r="54" spans="1:23" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="W53" s="28"/>
+    </row>
+    <row r="54" spans="1:23" ht="15.75" customHeight="1">
       <c r="A54" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B54" s="26" t="s">
-        <v>126</v>
+        <v>57</v>
       </c>
       <c r="C54" s="21"/>
       <c r="D54" s="21" t="s">
@@ -7092,15 +7563,17 @@
         <v>132</v>
       </c>
       <c r="U54" s="21"/>
-      <c r="V54" s="21"/>
-      <c r="W54" s="37"/>
-    </row>
-    <row r="55" spans="1:23" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="V54" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="W54" s="10"/>
+    </row>
+    <row r="55" spans="1:23" s="38" customFormat="1" ht="15.75" customHeight="1">
       <c r="A55" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B55" s="26" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
       <c r="C55" s="21"/>
       <c r="D55" s="21" t="s">
@@ -7158,12 +7631,12 @@
       <c r="V55" s="21"/>
       <c r="W55" s="37"/>
     </row>
-    <row r="56" spans="1:23" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:23" s="38" customFormat="1" ht="15.75" customHeight="1">
       <c r="A56" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B56" s="26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C56" s="21"/>
       <c r="D56" s="21" t="s">
@@ -7221,12 +7694,12 @@
       <c r="V56" s="21"/>
       <c r="W56" s="37"/>
     </row>
-    <row r="57" spans="1:23" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:23" s="38" customFormat="1" ht="15.75" customHeight="1">
       <c r="A57" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B57" s="26" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C57" s="21"/>
       <c r="D57" s="21" t="s">
@@ -7284,12 +7757,12 @@
       <c r="V57" s="21"/>
       <c r="W57" s="37"/>
     </row>
-    <row r="58" spans="1:23" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:23" s="38" customFormat="1" ht="15.75" customHeight="1">
       <c r="A58" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B58" s="26" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C58" s="21"/>
       <c r="D58" s="21" t="s">
@@ -7347,126 +7820,120 @@
       <c r="V58" s="21"/>
       <c r="W58" s="37"/>
     </row>
-    <row r="59" spans="1:23" s="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:23" s="38" customFormat="1" ht="15.75" customHeight="1">
       <c r="A59" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B59" s="26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C59" s="21"/>
-      <c r="D59" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="E59" s="17" t="s">
+      <c r="D59" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="E59" s="21" t="s">
         <v>128</v>
       </c>
       <c r="F59" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="G59" s="21"/>
-      <c r="H59" s="21"/>
-      <c r="I59" s="21"/>
+      <c r="G59" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="H59" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="I59" s="21" t="s">
+        <v>128</v>
+      </c>
       <c r="J59" s="21" t="s">
         <v>128</v>
       </c>
       <c r="K59" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="L59" s="21"/>
+      <c r="L59" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="M59" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="N59" s="21"/>
-      <c r="O59" s="21"/>
+      <c r="N59" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="O59" s="21" t="s">
+        <v>128</v>
+      </c>
       <c r="P59" s="21" t="s">
         <v>132</v>
       </c>
       <c r="Q59" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="R59" s="21"/>
-      <c r="S59" s="21"/>
-      <c r="T59" s="21"/>
+      <c r="R59" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="S59" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="T59" s="21" t="s">
+        <v>132</v>
+      </c>
       <c r="U59" s="21"/>
       <c r="V59" s="21"/>
-      <c r="W59" s="34"/>
-    </row>
-    <row r="60" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="W59" s="37"/>
+    </row>
+    <row r="60" spans="1:23" s="35" customFormat="1" ht="15.75" customHeight="1">
       <c r="A60" s="26" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="B60" s="26" t="s">
-        <v>59</v>
+        <v>148</v>
       </c>
       <c r="C60" s="21"/>
-      <c r="D60" s="21" t="s">
-        <v>128</v>
-      </c>
-      <c r="E60" s="21" t="s">
+      <c r="D60" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="E60" s="17" t="s">
         <v>128</v>
       </c>
       <c r="F60" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="G60" s="21" t="s">
-        <v>128</v>
-      </c>
-      <c r="H60" s="21" t="s">
-        <v>128</v>
-      </c>
-      <c r="I60" s="21" t="s">
-        <v>128</v>
-      </c>
+      <c r="G60" s="21"/>
+      <c r="H60" s="21"/>
+      <c r="I60" s="21"/>
       <c r="J60" s="21" t="s">
         <v>128</v>
       </c>
       <c r="K60" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="L60" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="L60" s="21"/>
       <c r="M60" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="N60" s="21" t="s">
-        <v>128</v>
-      </c>
-      <c r="O60" s="21" t="s">
-        <v>128</v>
-      </c>
+      <c r="N60" s="21"/>
+      <c r="O60" s="21"/>
       <c r="P60" s="21" t="s">
         <v>132</v>
       </c>
       <c r="Q60" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="R60" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="S60" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="T60" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="U60" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="V60" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="W60" s="40" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="61" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="R60" s="21"/>
+      <c r="S60" s="21"/>
+      <c r="T60" s="21"/>
+      <c r="U60" s="21"/>
+      <c r="V60" s="21"/>
+      <c r="W60" s="34"/>
+    </row>
+    <row r="61" spans="1:23" ht="15.75" customHeight="1">
       <c r="A61" s="26" t="s">
         <v>58</v>
       </c>
       <c r="B61" s="26" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C61" s="21"/>
       <c r="D61" s="21" t="s">
@@ -7526,20 +7993,22 @@
       <c r="V61" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="W61" s="41"/>
-    </row>
-    <row r="62" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="W61" s="42" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:23" ht="15.75" customHeight="1">
       <c r="A62" s="26" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B62" s="26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C62" s="21"/>
       <c r="D62" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="E62" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="E62" s="21" t="s">
         <v>128</v>
       </c>
       <c r="F62" s="21" t="s">
@@ -7555,7 +8024,7 @@
         <v>128</v>
       </c>
       <c r="J62" s="21" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="K62" s="21" t="s">
         <v>128</v>
@@ -7573,122 +8042,159 @@
         <v>128</v>
       </c>
       <c r="P62" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q62" s="21" t="s">
-        <v>114</v>
+        <v>17</v>
       </c>
       <c r="R62" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="S62" s="21"/>
+      <c r="S62" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="T62" s="21" t="s">
         <v>132</v>
       </c>
       <c r="U62" s="21" t="s">
-        <v>114</v>
+        <v>17</v>
       </c>
       <c r="V62" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="W62" s="10"/>
-    </row>
-    <row r="63" spans="1:23" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="B63" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="C63" s="19"/>
+      <c r="W62" s="43"/>
+    </row>
+    <row r="63" spans="1:23" ht="15.75" customHeight="1">
+      <c r="A63" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="B63" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C63" s="21"/>
       <c r="D63" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="E63" s="19"/>
-      <c r="F63" s="19"/>
-      <c r="G63" s="19"/>
-      <c r="H63" s="19"/>
-      <c r="I63" s="19"/>
-      <c r="J63" s="19"/>
-      <c r="K63" s="19"/>
-      <c r="L63" s="19"/>
-      <c r="M63" s="19"/>
-      <c r="N63" s="19"/>
-      <c r="O63" s="19"/>
-      <c r="P63" s="19"/>
-      <c r="Q63" s="19"/>
-      <c r="R63" s="19"/>
-      <c r="S63" s="19"/>
-      <c r="T63" s="19"/>
-      <c r="U63" s="19"/>
-      <c r="V63" s="19"/>
-      <c r="W63" s="14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="64" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A64" s="16" t="s">
+      <c r="E63" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="F63" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="G63" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="H63" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="I63" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="J63" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="K63" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="L63" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="M63" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="N63" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="O63" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="P63" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q63" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="R63" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="S63" s="21"/>
+      <c r="T63" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="U63" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="V63" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="W63" s="10"/>
+    </row>
+    <row r="64" spans="1:23" s="15" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A64" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="B64" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="C64" s="17"/>
+      <c r="B64" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C64" s="19"/>
       <c r="D64" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="E64" s="17"/>
-      <c r="F64" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="G64" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="H64" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="I64" s="17"/>
-      <c r="J64" s="17"/>
-      <c r="K64" s="17"/>
-      <c r="L64" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="M64" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="N64" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="O64" s="17"/>
-      <c r="P64" s="17"/>
-      <c r="Q64" s="17"/>
-      <c r="R64" s="17"/>
-      <c r="S64" s="17"/>
-      <c r="T64" s="17"/>
-      <c r="U64" s="17"/>
-      <c r="V64" s="17"/>
-    </row>
-    <row r="65" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E64" s="19"/>
+      <c r="F64" s="19"/>
+      <c r="G64" s="19"/>
+      <c r="H64" s="19"/>
+      <c r="I64" s="19"/>
+      <c r="J64" s="19"/>
+      <c r="K64" s="19"/>
+      <c r="L64" s="19"/>
+      <c r="M64" s="19"/>
+      <c r="N64" s="19"/>
+      <c r="O64" s="19"/>
+      <c r="P64" s="19"/>
+      <c r="Q64" s="19"/>
+      <c r="R64" s="19"/>
+      <c r="S64" s="19"/>
+      <c r="T64" s="19"/>
+      <c r="U64" s="19"/>
+      <c r="V64" s="19"/>
+      <c r="W64" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="65" spans="1:22" ht="15.75" customHeight="1">
       <c r="A65" s="16" t="s">
         <v>63</v>
       </c>
       <c r="B65" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C65" s="17"/>
       <c r="D65" s="21" t="s">
         <v>127</v>
       </c>
       <c r="E65" s="17"/>
-      <c r="F65" s="17"/>
-      <c r="G65" s="17"/>
-      <c r="H65" s="17"/>
+      <c r="F65" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G65" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H65" s="17" t="s">
+        <v>19</v>
+      </c>
       <c r="I65" s="17"/>
       <c r="J65" s="17"/>
       <c r="K65" s="17"/>
-      <c r="L65" s="17"/>
-      <c r="M65" s="17"/>
-      <c r="N65" s="17"/>
+      <c r="L65" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="M65" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="N65" s="17" t="s">
+        <v>19</v>
+      </c>
       <c r="O65" s="17"/>
       <c r="P65" s="17"/>
       <c r="Q65" s="17"/>
@@ -7698,12 +8204,12 @@
       <c r="U65" s="17"/>
       <c r="V65" s="17"/>
     </row>
-    <row r="66" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:22" ht="15.75" customHeight="1">
       <c r="A66" s="16" t="s">
         <v>63</v>
       </c>
       <c r="B66" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C66" s="17"/>
       <c r="D66" s="21" t="s">
@@ -7728,12 +8234,12 @@
       <c r="U66" s="17"/>
       <c r="V66" s="17"/>
     </row>
-    <row r="67" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:22" ht="15.75" customHeight="1">
       <c r="A67" s="16" t="s">
         <v>63</v>
       </c>
       <c r="B67" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C67" s="17"/>
       <c r="D67" s="21" t="s">
@@ -7758,12 +8264,12 @@
       <c r="U67" s="17"/>
       <c r="V67" s="17"/>
     </row>
-    <row r="68" spans="1:22" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:22" ht="15.75" customHeight="1">
       <c r="A68" s="16" t="s">
         <v>63</v>
       </c>
       <c r="B68" s="16" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="C68" s="17"/>
       <c r="D68" s="21" t="s">
@@ -7788,12 +8294,12 @@
       <c r="U68" s="17"/>
       <c r="V68" s="17"/>
     </row>
-    <row r="69" spans="1:22" s="33" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:22" s="36" customFormat="1" ht="15.75" customHeight="1">
       <c r="A69" s="16" t="s">
         <v>63</v>
       </c>
       <c r="B69" s="16" t="s">
-        <v>125</v>
+        <v>33</v>
       </c>
       <c r="C69" s="17"/>
       <c r="D69" s="21" t="s">
@@ -7818,109 +8324,141 @@
       <c r="U69" s="17"/>
       <c r="V69" s="17"/>
     </row>
-    <row r="70" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:22" s="33" customFormat="1" ht="15.75" customHeight="1">
       <c r="A70" s="16" t="s">
-        <v>110</v>
+        <v>63</v>
       </c>
       <c r="B70" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="C70" s="20"/>
+        <v>125</v>
+      </c>
+      <c r="C70" s="17"/>
       <c r="D70" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="E70" s="20"/>
-      <c r="F70" s="20"/>
-      <c r="G70" s="20"/>
-      <c r="H70" s="20"/>
-      <c r="I70" s="20"/>
-      <c r="J70" s="20"/>
-      <c r="K70" s="20"/>
-      <c r="L70" s="20"/>
-      <c r="M70" s="20"/>
-      <c r="N70" s="20"/>
-      <c r="O70" s="20"/>
-      <c r="P70" s="20"/>
-      <c r="Q70" s="20"/>
-      <c r="R70" s="20"/>
-      <c r="S70" s="20"/>
-      <c r="T70" s="20"/>
-      <c r="U70" s="20"/>
-      <c r="V70" s="20"/>
-    </row>
-    <row r="71" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E70" s="17"/>
+      <c r="F70" s="17"/>
+      <c r="G70" s="17"/>
+      <c r="H70" s="17"/>
+      <c r="I70" s="17"/>
+      <c r="J70" s="17"/>
+      <c r="K70" s="17"/>
+      <c r="L70" s="17"/>
+      <c r="M70" s="17"/>
+      <c r="N70" s="17"/>
+      <c r="O70" s="17"/>
+      <c r="P70" s="17"/>
+      <c r="Q70" s="17"/>
+      <c r="R70" s="17"/>
+      <c r="S70" s="17"/>
+      <c r="T70" s="17"/>
+      <c r="U70" s="17"/>
+      <c r="V70" s="17"/>
+    </row>
+    <row r="71" spans="1:22" ht="15.75" customHeight="1">
       <c r="A71" s="16" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="B71" s="16" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="C71" s="20"/>
       <c r="D71" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="E71" s="20"/>
+      <c r="F71" s="20"/>
+      <c r="G71" s="20"/>
+      <c r="H71" s="20"/>
+      <c r="I71" s="20"/>
+      <c r="J71" s="20"/>
+      <c r="K71" s="20"/>
+      <c r="L71" s="20"/>
+      <c r="M71" s="20"/>
+      <c r="N71" s="20"/>
+      <c r="O71" s="20"/>
+      <c r="P71" s="20"/>
+      <c r="Q71" s="20"/>
+      <c r="R71" s="20"/>
+      <c r="S71" s="20"/>
+      <c r="T71" s="20"/>
+      <c r="U71" s="20"/>
+      <c r="V71" s="20"/>
+    </row>
+    <row r="72" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A72" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="B72" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="C72" s="20"/>
+      <c r="D72" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="E71" s="30" t="s">
+      <c r="E72" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="F71" s="30"/>
-      <c r="G71" s="30" t="s">
+      <c r="F72" s="30"/>
+      <c r="G72" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="H71" s="30"/>
-      <c r="I71" s="30"/>
-      <c r="J71" s="30" t="s">
+      <c r="H72" s="30"/>
+      <c r="I72" s="30"/>
+      <c r="J72" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="K71" s="30" t="s">
+      <c r="K72" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="L71" s="30" t="s">
+      <c r="L72" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="M71" s="30" t="s">
+      <c r="M72" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="N71" s="30"/>
-      <c r="O71" s="30"/>
-      <c r="P71" s="30"/>
-      <c r="Q71" s="30"/>
-      <c r="R71" s="30"/>
-      <c r="S71" s="30"/>
-      <c r="T71" s="30"/>
-      <c r="U71" s="30"/>
-      <c r="V71" s="30"/>
+      <c r="N72" s="30"/>
+      <c r="O72" s="30"/>
+      <c r="P72" s="30"/>
+      <c r="Q72" s="30"/>
+      <c r="R72" s="30"/>
+      <c r="S72" s="30"/>
+      <c r="T72" s="30"/>
+      <c r="U72" s="30"/>
+      <c r="V72" s="30"/>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C22" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
+      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="G49" sqref="G49"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
     <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
       <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
-      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="E7" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="L57" sqref="L57:L59"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="C22" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="6">
-    <mergeCell ref="W60:W61"/>
+    <mergeCell ref="W61:W62"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="J5:N5"/>
     <mergeCell ref="P5:V5"/>
     <mergeCell ref="C1:N1"/>
     <mergeCell ref="C2:N2"/>
   </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -7929,10 +8467,10 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="29.6640625" customWidth="1"/>
     <col min="2" max="2" width="28.1640625" customWidth="1"/>
@@ -7940,7 +8478,7 @@
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="15">
       <c r="A1" s="22" t="s">
         <v>70</v>
       </c>
@@ -7957,7 +8495,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15">
       <c r="A2" s="23" t="s">
         <v>73</v>
       </c>
@@ -7970,7 +8508,7 @@
       <c r="D2" s="24"/>
       <c r="E2" s="24"/>
     </row>
-    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="15">
       <c r="A3" s="23" t="s">
         <v>75</v>
       </c>
@@ -7983,7 +8521,7 @@
       <c r="D3" s="24"/>
       <c r="E3" s="24"/>
     </row>
-    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="15">
       <c r="A4" s="23" t="s">
         <v>77</v>
       </c>
@@ -7996,7 +8534,7 @@
       <c r="D4" s="24"/>
       <c r="E4" s="24"/>
     </row>
-    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="15">
       <c r="A5" s="23" t="s">
         <v>97</v>
       </c>
@@ -8011,7 +8549,7 @@
       </c>
       <c r="E5" s="24"/>
     </row>
-    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="15">
       <c r="A6" s="23" t="s">
         <v>98</v>
       </c>
@@ -8026,7 +8564,7 @@
       </c>
       <c r="E6" s="24"/>
     </row>
-    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="15">
       <c r="A7" s="23" t="s">
         <v>99</v>
       </c>
@@ -8041,7 +8579,7 @@
       </c>
       <c r="E7" s="24"/>
     </row>
-    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="15">
       <c r="A8" s="23" t="s">
         <v>100</v>
       </c>
@@ -8056,7 +8594,7 @@
       </c>
       <c r="E8" s="24"/>
     </row>
-    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="15">
       <c r="A9" s="23" t="s">
         <v>109</v>
       </c>
@@ -8069,7 +8607,7 @@
       <c r="D9" s="24"/>
       <c r="E9" s="24"/>
     </row>
-    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="15">
       <c r="A10" s="23" t="s">
         <v>108</v>
       </c>
@@ -8082,7 +8620,7 @@
       <c r="D10" s="24"/>
       <c r="E10" s="24"/>
     </row>
-    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="15">
       <c r="A11" s="23" t="s">
         <v>107</v>
       </c>
@@ -8095,7 +8633,7 @@
       <c r="D11" s="24"/>
       <c r="E11" s="24"/>
     </row>
-    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="15">
       <c r="A12" s="23" t="s">
         <v>101</v>
       </c>
@@ -8110,7 +8648,7 @@
       </c>
       <c r="E12" s="24"/>
     </row>
-    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="15">
       <c r="A13" s="23" t="s">
         <v>106</v>
       </c>
@@ -8125,7 +8663,7 @@
       </c>
       <c r="E13" s="24"/>
     </row>
-    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="15">
       <c r="A14" s="23" t="s">
         <v>102</v>
       </c>
@@ -8140,7 +8678,7 @@
       </c>
       <c r="E14" s="24"/>
     </row>
-    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="15">
       <c r="A15" s="23" t="s">
         <v>103</v>
       </c>
@@ -8155,7 +8693,7 @@
       </c>
       <c r="E15" s="24"/>
     </row>
-    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="15">
       <c r="A16" s="23" t="s">
         <v>104</v>
       </c>
@@ -8170,7 +8708,7 @@
       </c>
       <c r="E16" s="24"/>
     </row>
-    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="15">
       <c r="A17" s="23" t="s">
         <v>123</v>
       </c>
@@ -8185,7 +8723,7 @@
       </c>
       <c r="E17" s="24"/>
     </row>
-    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="15">
       <c r="A18" s="23" t="s">
         <v>12</v>
       </c>
@@ -8200,7 +8738,7 @@
       </c>
       <c r="E18" s="24"/>
     </row>
-    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="15">
       <c r="A19" s="23" t="s">
         <v>13</v>
       </c>
@@ -8215,7 +8753,7 @@
       </c>
       <c r="E19" s="24"/>
     </row>
-    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="15">
       <c r="A20" s="23" t="s">
         <v>105</v>
       </c>
@@ -8232,23 +8770,25 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
+      <selection activeCell="C7" sqref="C7"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
     <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
       <selection activeCell="C7" sqref="C7"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
-      <selection activeCell="C7" sqref="C7"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}">
+      <selection activeCell="A21" sqref="A21:XFD21"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Päivitä roolit.exceliin YIT+Destia+Lemminkäinen ehdotuksen mukaiset muutokset
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarihan/Desktop/Harja/harja/resources/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-900" windowWidth="47580" windowHeight="26980" tabRatio="500"/>
+    <workbookView xWindow="-1340" yWindow="2560" windowWidth="41260" windowHeight="21380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -12,23 +17,23 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="1933" windowHeight="783" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="2379" windowHeight="1295" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
-    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="1933" windowHeight="879" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1101" uniqueCount="160">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -505,6 +510,9 @@
   </si>
   <si>
     <t>Muutos- ja lisätyöt</t>
+  </si>
+  <si>
+    <t>Kelikeskus</t>
   </si>
 </sst>
 </file>
@@ -770,7 +778,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -814,7 +822,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1014,7 +1021,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{C606B059-99AC-3B47-8437-66D15B4E3D4B}" diskRevisions="1" revisionId="141" version="18">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{C0D8A1BF-1D13-2C41-BEFB-54E54F9CD4DD}" diskRevisions="1" revisionId="162" version="21">
   <header guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" dateTime="2016-09-06T09:14:56" maxSheetId="3" userName="Tatu Tarvainen" r:id="rId2" minRId="1" maxRId="3">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1117,6 +1124,24 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{10512BAD-3156-C24F-8776-86D565B99C8B}" dateTime="2016-10-28T10:40:25" maxSheetId="3" userName="Microsoft Office User" r:id="rId19" minRId="142" maxRId="156">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{35DE1F50-A040-2C4B-BA4C-69E94B44BD31}" dateTime="2016-10-28T10:44:36" maxSheetId="3" userName="Microsoft Office User" r:id="rId20" minRId="157">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{C0D8A1BF-1D13-2C41-BEFB-54E54F9CD4DD}" dateTime="2016-10-28T10:47:16" maxSheetId="3" userName="Microsoft Office User" r:id="rId21" minRId="158" maxRId="162">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -3540,6 +3565,212 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog18.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="142" sId="1" odxf="1" dxf="1">
+    <nc r="S25" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </nc>
+    <odxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </odxf>
+    <ndxf>
+      <font>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rcc rId="143" sId="1">
+    <oc r="V6" t="inlineStr">
+      <is>
+        <t>Urakan turvallisuusvastaava</t>
+      </is>
+    </oc>
+    <nc r="V6" t="inlineStr">
+      <is>
+        <t>Kelikeskus</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="144" sId="1">
+    <oc r="S7" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </oc>
+    <nc r="S7" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="145" sId="1" odxf="1" dxf="1">
+    <nc r="S13" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </nc>
+    <odxf/>
+    <ndxf/>
+  </rcc>
+  <rcc rId="146" sId="1" odxf="1" dxf="1">
+    <nc r="S14" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </nc>
+    <odxf/>
+    <ndxf/>
+  </rcc>
+  <rcc rId="147" sId="1" odxf="1" dxf="1">
+    <nc r="S15" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </nc>
+    <odxf/>
+    <ndxf/>
+  </rcc>
+  <rcc rId="148" sId="1">
+    <oc r="S16" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </oc>
+    <nc r="S16" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="149" sId="1">
+    <oc r="S17" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </oc>
+    <nc r="S17" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="150" sId="1">
+    <nc r="S18" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="151" sId="1">
+    <oc r="S19" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </oc>
+    <nc r="S19" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="152" sId="1">
+    <nc r="S22" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="153" sId="1">
+    <oc r="V7" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </oc>
+    <nc r="V7" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="154" sId="1">
+    <oc r="V25" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </oc>
+    <nc r="V25"/>
+  </rcc>
+  <rcc rId="155" sId="1">
+    <oc r="V23" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </oc>
+    <nc r="V23"/>
+  </rcc>
+  <rcc rId="156" sId="1">
+    <oc r="V22" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </oc>
+    <nc r="V22"/>
+  </rcc>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="delete"/>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog19.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="157" sId="1">
+    <oc r="S22" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </oc>
+    <nc r="S22" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="1" sId="1">
@@ -3575,6 +3806,46 @@
     <nc r="S24" t="inlineStr">
       <is>
         <t>R,W,valmis</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog20.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="158" sId="1">
+    <nc r="S63" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="159" sId="1">
+    <nc r="S53" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="160" sId="1">
+    <nc r="S48" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="161" sId="1">
+    <nc r="S46" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="162" sId="1">
+    <nc r="S46" t="inlineStr">
+      <is>
+        <t>R</t>
       </is>
     </nc>
   </rcc>
@@ -4629,14 +4900,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
+      <pane xSplit="2" ySplit="6" topLeftCell="M40" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="G49" sqref="G49"/>
+      <selection pane="bottomRight" activeCell="S55" sqref="S55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.5" bestFit="1" customWidth="1"/>
@@ -4662,45 +4933,45 @@
     <col min="23" max="23" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="24" customHeight="1">
+    <row r="1" spans="1:23" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="44" t="s">
         <v>152</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-    </row>
-    <row r="2" spans="1:23" ht="15.75" customHeight="1">
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+    </row>
+    <row r="2" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="43"/>
-    </row>
-    <row r="3" spans="1:23" ht="15.75" customHeight="1">
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+    </row>
+    <row r="3" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -4715,39 +4986,39 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="15.75" customHeight="1">
+    <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:23" ht="15.75" customHeight="1">
-      <c r="C5" s="44" t="s">
+    <row r="5" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C5" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
-      <c r="J5" s="44" t="s">
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="J5" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="43"/>
-      <c r="L5" s="43"/>
-      <c r="M5" s="43"/>
-      <c r="N5" s="43"/>
-      <c r="P5" s="44" t="s">
+      <c r="K5" s="42"/>
+      <c r="L5" s="42"/>
+      <c r="M5" s="42"/>
+      <c r="N5" s="42"/>
+      <c r="P5" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="Q5" s="43"/>
-      <c r="R5" s="43"/>
-      <c r="S5" s="43"/>
-      <c r="T5" s="43"/>
-      <c r="U5" s="43"/>
-      <c r="V5" s="43"/>
+      <c r="Q5" s="42"/>
+      <c r="R5" s="42"/>
+      <c r="S5" s="42"/>
+      <c r="T5" s="42"/>
+      <c r="U5" s="42"/>
+      <c r="V5" s="42"/>
       <c r="W5" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="15.75" customHeight="1">
+    <row r="6" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
@@ -4810,10 +5081,10 @@
         <v>93</v>
       </c>
       <c r="V6" s="9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" ht="15.75" customHeight="1">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="16" t="s">
         <v>15</v>
       </c>
@@ -4867,7 +5138,7 @@
         <v>132</v>
       </c>
       <c r="S7" s="21" t="s">
-        <v>17</v>
+        <v>114</v>
       </c>
       <c r="T7" s="17" t="s">
         <v>132</v>
@@ -4876,11 +5147,11 @@
         <v>17</v>
       </c>
       <c r="V7" s="17" t="s">
-        <v>17</v>
+        <v>114</v>
       </c>
       <c r="W7" s="10"/>
     </row>
-    <row r="8" spans="1:23" ht="15.75" customHeight="1">
+    <row r="8" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="16" t="s">
         <v>15</v>
       </c>
@@ -4933,7 +5204,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="15.75" customHeight="1">
+    <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="16" t="s">
         <v>15</v>
       </c>
@@ -4980,7 +5251,7 @@
       <c r="V9" s="17"/>
       <c r="W9" s="10"/>
     </row>
-    <row r="10" spans="1:23" ht="15.75" customHeight="1">
+    <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="16" t="s">
         <v>15</v>
       </c>
@@ -5027,7 +5298,7 @@
       <c r="V10" s="17"/>
       <c r="W10" s="10"/>
     </row>
-    <row r="11" spans="1:23" ht="15.75" customHeight="1">
+    <row r="11" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="16" t="s">
         <v>15</v>
       </c>
@@ -5088,7 +5359,7 @@
       <c r="V11" s="17"/>
       <c r="W11" s="10"/>
     </row>
-    <row r="12" spans="1:23" ht="15.75" customHeight="1">
+    <row r="12" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="16" t="s">
         <v>15</v>
       </c>
@@ -5149,7 +5420,7 @@
       <c r="V12" s="17"/>
       <c r="W12" s="10"/>
     </row>
-    <row r="13" spans="1:23" ht="15.75" customHeight="1">
+    <row r="13" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="16" t="s">
         <v>15</v>
       </c>
@@ -5188,7 +5459,9 @@
         <v>114</v>
       </c>
       <c r="R13" s="21"/>
-      <c r="S13" s="17"/>
+      <c r="S13" s="21" t="s">
+        <v>114</v>
+      </c>
       <c r="T13" s="17" t="s">
         <v>132</v>
       </c>
@@ -5196,7 +5469,7 @@
       <c r="V13" s="17"/>
       <c r="W13" s="10"/>
     </row>
-    <row r="14" spans="1:23" ht="15.75" customHeight="1">
+    <row r="14" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="16" t="s">
         <v>15</v>
       </c>
@@ -5235,7 +5508,9 @@
         <v>114</v>
       </c>
       <c r="R14" s="21"/>
-      <c r="S14" s="17"/>
+      <c r="S14" s="21" t="s">
+        <v>114</v>
+      </c>
       <c r="T14" s="17" t="s">
         <v>132</v>
       </c>
@@ -5243,7 +5518,7 @@
       <c r="V14" s="17"/>
       <c r="W14" s="10"/>
     </row>
-    <row r="15" spans="1:23" ht="15.75" customHeight="1">
+    <row r="15" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="16" t="s">
         <v>15</v>
       </c>
@@ -5282,7 +5557,9 @@
         <v>114</v>
       </c>
       <c r="R15" s="21"/>
-      <c r="S15" s="17"/>
+      <c r="S15" s="21" t="s">
+        <v>114</v>
+      </c>
       <c r="T15" s="17" t="s">
         <v>132</v>
       </c>
@@ -5290,7 +5567,7 @@
       <c r="V15" s="17"/>
       <c r="W15" s="10"/>
     </row>
-    <row r="16" spans="1:23" ht="15.75" customHeight="1">
+    <row r="16" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="16" t="s">
         <v>15</v>
       </c>
@@ -5342,7 +5619,7 @@
         <v>132</v>
       </c>
       <c r="S16" s="21" t="s">
-        <v>17</v>
+        <v>114</v>
       </c>
       <c r="T16" s="17" t="s">
         <v>132</v>
@@ -5351,7 +5628,7 @@
       <c r="V16" s="17"/>
       <c r="W16" s="10"/>
     </row>
-    <row r="17" spans="1:23" ht="15.75" customHeight="1">
+    <row r="17" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="16" t="s">
         <v>15</v>
       </c>
@@ -5403,7 +5680,7 @@
         <v>132</v>
       </c>
       <c r="S17" s="21" t="s">
-        <v>17</v>
+        <v>114</v>
       </c>
       <c r="T17" s="17" t="s">
         <v>132</v>
@@ -5412,7 +5689,7 @@
       <c r="V17" s="17"/>
       <c r="W17" s="10"/>
     </row>
-    <row r="18" spans="1:23" ht="15.75" customHeight="1">
+    <row r="18" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="16" t="s">
         <v>15</v>
       </c>
@@ -5451,7 +5728,9 @@
         <v>114</v>
       </c>
       <c r="R18" s="21"/>
-      <c r="S18" s="21"/>
+      <c r="S18" s="21" t="s">
+        <v>114</v>
+      </c>
       <c r="T18" s="17" t="s">
         <v>132</v>
       </c>
@@ -5459,7 +5738,7 @@
       <c r="V18" s="17"/>
       <c r="W18" s="10"/>
     </row>
-    <row r="19" spans="1:23" ht="15.75" customHeight="1">
+    <row r="19" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="16" t="s">
         <v>15</v>
       </c>
@@ -5511,7 +5790,7 @@
         <v>132</v>
       </c>
       <c r="S19" s="21" t="s">
-        <v>17</v>
+        <v>114</v>
       </c>
       <c r="T19" s="17" t="s">
         <v>132</v>
@@ -5520,7 +5799,7 @@
       <c r="V19" s="17"/>
       <c r="W19" s="10"/>
     </row>
-    <row r="20" spans="1:23" ht="15.75" customHeight="1">
+    <row r="20" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="16" t="s">
         <v>15</v>
       </c>
@@ -5587,7 +5866,7 @@
       </c>
       <c r="W20" s="10"/>
     </row>
-    <row r="21" spans="1:23" ht="15.75" customHeight="1">
+    <row r="21" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="26" t="s">
         <v>15</v>
       </c>
@@ -5654,7 +5933,7 @@
       </c>
       <c r="W21" s="10"/>
     </row>
-    <row r="22" spans="1:23" ht="15.75" customHeight="1">
+    <row r="22" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="26" t="s">
         <v>15</v>
       </c>
@@ -5707,19 +5986,19 @@
       <c r="R22" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="S22" s="21"/>
+      <c r="S22" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="T22" s="17" t="s">
         <v>132</v>
       </c>
       <c r="U22" s="21"/>
-      <c r="V22" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="V22" s="21"/>
       <c r="W22" s="10" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="23" spans="1:23" ht="15.75" customHeight="1">
+    <row r="23" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="26" t="s">
         <v>15</v>
       </c>
@@ -5779,12 +6058,10 @@
         <v>132</v>
       </c>
       <c r="U23" s="21"/>
-      <c r="V23" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="V23" s="21"/>
       <c r="W23" s="10"/>
     </row>
-    <row r="24" spans="1:23" ht="15.75" customHeight="1">
+    <row r="24" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="26" t="s">
         <v>15</v>
       </c>
@@ -5847,7 +6124,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="25" spans="1:23" ht="15.75" customHeight="1">
+    <row r="25" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="26" t="s">
         <v>15</v>
       </c>
@@ -5892,17 +6169,17 @@
       <c r="R25" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="S25" s="27"/>
+      <c r="S25" s="21" t="s">
+        <v>114</v>
+      </c>
       <c r="T25" s="21" t="s">
         <v>132</v>
       </c>
       <c r="U25" s="21"/>
-      <c r="V25" s="21" t="s">
-        <v>114</v>
-      </c>
+      <c r="V25" s="21"/>
       <c r="W25" s="10"/>
     </row>
-    <row r="26" spans="1:23" ht="15.75" customHeight="1">
+    <row r="26" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="26" t="s">
         <v>15</v>
       </c>
@@ -5949,7 +6226,7 @@
       <c r="V26" s="21"/>
       <c r="W26" s="10"/>
     </row>
-    <row r="27" spans="1:23" ht="15.75" customHeight="1">
+    <row r="27" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="26" t="s">
         <v>15</v>
       </c>
@@ -5988,7 +6265,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:23" ht="15.75" customHeight="1">
+    <row r="28" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="26" t="s">
         <v>15</v>
       </c>
@@ -6051,7 +6328,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="29" spans="1:23" ht="15.75" customHeight="1">
+    <row r="29" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="26" t="s">
         <v>15</v>
       </c>
@@ -6108,7 +6385,7 @@
       <c r="V29" s="21"/>
       <c r="W29" s="10"/>
     </row>
-    <row r="30" spans="1:23" ht="15.75" customHeight="1">
+    <row r="30" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="26" t="s">
         <v>15</v>
       </c>
@@ -6167,7 +6444,7 @@
       <c r="V30" s="21"/>
       <c r="W30" s="10"/>
     </row>
-    <row r="31" spans="1:23" ht="15.75" customHeight="1">
+    <row r="31" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="26" t="s">
         <v>15</v>
       </c>
@@ -6224,7 +6501,7 @@
       <c r="V31" s="21"/>
       <c r="W31" s="10"/>
     </row>
-    <row r="32" spans="1:23" ht="15.75" customHeight="1">
+    <row r="32" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="26" t="s">
         <v>15</v>
       </c>
@@ -6281,7 +6558,7 @@
       <c r="V32" s="21"/>
       <c r="W32" s="10"/>
     </row>
-    <row r="33" spans="1:23" s="39" customFormat="1" ht="15.75" customHeight="1">
+    <row r="33" spans="1:23" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="26" t="s">
         <v>15</v>
       </c>
@@ -6337,7 +6614,7 @@
       <c r="U33" s="21"/>
       <c r="V33" s="21"/>
     </row>
-    <row r="34" spans="1:23" s="39" customFormat="1" ht="15.75" customHeight="1">
+    <row r="34" spans="1:23" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="26" t="s">
         <v>15</v>
       </c>
@@ -6393,7 +6670,7 @@
       <c r="U34" s="21"/>
       <c r="V34" s="21"/>
     </row>
-    <row r="35" spans="1:23" s="39" customFormat="1" ht="15.75" customHeight="1">
+    <row r="35" spans="1:23" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="26" t="s">
         <v>15</v>
       </c>
@@ -6449,7 +6726,7 @@
       <c r="U35" s="21"/>
       <c r="V35" s="21"/>
     </row>
-    <row r="36" spans="1:23" s="13" customFormat="1" ht="15.75" customHeight="1">
+    <row r="36" spans="1:23" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="26" t="s">
         <v>15</v>
       </c>
@@ -6516,7 +6793,7 @@
       </c>
       <c r="W36" s="12"/>
     </row>
-    <row r="37" spans="1:23" s="32" customFormat="1" ht="15.75" customHeight="1">
+    <row r="37" spans="1:23" s="31" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="26" t="s">
         <v>43</v>
       </c>
@@ -6561,9 +6838,9 @@
       </c>
       <c r="U37" s="21"/>
       <c r="V37" s="21"/>
-      <c r="W37" s="31"/>
-    </row>
-    <row r="38" spans="1:23" ht="15.75" customHeight="1">
+      <c r="W37" s="30"/>
+    </row>
+    <row r="38" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="26" t="s">
         <v>43</v>
       </c>
@@ -6612,7 +6889,7 @@
       <c r="V38" s="21"/>
       <c r="W38" s="10"/>
     </row>
-    <row r="39" spans="1:23" ht="15.75" customHeight="1">
+    <row r="39" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="26" t="s">
         <v>43</v>
       </c>
@@ -6677,7 +6954,7 @@
       </c>
       <c r="W39" s="10"/>
     </row>
-    <row r="40" spans="1:23" s="38" customFormat="1" ht="15.75" customHeight="1">
+    <row r="40" spans="1:23" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="26" t="s">
         <v>43</v>
       </c>
@@ -6742,9 +7019,9 @@
       <c r="V40" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="W40" s="37"/>
-    </row>
-    <row r="41" spans="1:23" ht="15.75" customHeight="1">
+      <c r="W40" s="36"/>
+    </row>
+    <row r="41" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="26" t="s">
         <v>43</v>
       </c>
@@ -6809,7 +7086,7 @@
       </c>
       <c r="W41" s="10"/>
     </row>
-    <row r="42" spans="1:23" ht="15.75" customHeight="1">
+    <row r="42" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="26" t="s">
         <v>43</v>
       </c>
@@ -6874,7 +7151,7 @@
       </c>
       <c r="W42" s="10"/>
     </row>
-    <row r="43" spans="1:23" ht="15.75" customHeight="1">
+    <row r="43" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="26" t="s">
         <v>43</v>
       </c>
@@ -6939,7 +7216,7 @@
       </c>
       <c r="W43" s="10"/>
     </row>
-    <row r="44" spans="1:23" s="41" customFormat="1" ht="15.75" customHeight="1">
+    <row r="44" spans="1:23" s="40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="26" t="s">
         <v>43</v>
       </c>
@@ -7002,9 +7279,9 @@
       <c r="V44" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="W44" s="40"/>
-    </row>
-    <row r="45" spans="1:23" ht="15.75" customHeight="1">
+      <c r="W44" s="39"/>
+    </row>
+    <row r="45" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="26" t="s">
         <v>43</v>
       </c>
@@ -7069,7 +7346,7 @@
       </c>
       <c r="W45" s="10"/>
     </row>
-    <row r="46" spans="1:23" ht="15.75" customHeight="1">
+    <row r="46" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="26" t="s">
         <v>43</v>
       </c>
@@ -7120,7 +7397,9 @@
       <c r="R46" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="S46" s="21"/>
+      <c r="S46" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="T46" s="21" t="s">
         <v>132</v>
       </c>
@@ -7130,7 +7409,7 @@
       </c>
       <c r="W46" s="10"/>
     </row>
-    <row r="47" spans="1:23" ht="15.75" customHeight="1">
+    <row r="47" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="26" t="s">
         <v>43</v>
       </c>
@@ -7195,7 +7474,7 @@
       </c>
       <c r="W47" s="10"/>
     </row>
-    <row r="48" spans="1:23" ht="15.75" customHeight="1">
+    <row r="48" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="26" t="s">
         <v>43</v>
       </c>
@@ -7240,7 +7519,9 @@
       <c r="R48" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="S48" s="21"/>
+      <c r="S48" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="T48" s="21" t="s">
         <v>132</v>
       </c>
@@ -7250,7 +7531,7 @@
       </c>
       <c r="W48" s="10"/>
     </row>
-    <row r="49" spans="1:23" ht="15.75" customHeight="1">
+    <row r="49" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="26" t="s">
         <v>43</v>
       </c>
@@ -7301,7 +7582,7 @@
       <c r="V49" s="21"/>
       <c r="W49" s="10"/>
     </row>
-    <row r="50" spans="1:23" ht="15.75" customHeight="1">
+    <row r="50" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="26" t="s">
         <v>43</v>
       </c>
@@ -7348,7 +7629,7 @@
       <c r="V50" s="21"/>
       <c r="W50" s="10"/>
     </row>
-    <row r="51" spans="1:23" ht="15.75" customHeight="1">
+    <row r="51" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="26" t="s">
         <v>43</v>
       </c>
@@ -7395,7 +7676,7 @@
       <c r="V51" s="21"/>
       <c r="W51" s="10"/>
     </row>
-    <row r="52" spans="1:23" ht="15.75" customHeight="1">
+    <row r="52" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="26" t="s">
         <v>43</v>
       </c>
@@ -7442,7 +7723,7 @@
       <c r="V52" s="21"/>
       <c r="W52" s="10"/>
     </row>
-    <row r="53" spans="1:23" s="29" customFormat="1" ht="15.75" customHeight="1">
+    <row r="53" spans="1:23" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="26" t="s">
         <v>43</v>
       </c>
@@ -7493,7 +7774,9 @@
       <c r="R53" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="S53" s="21"/>
+      <c r="S53" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="T53" s="21" t="s">
         <v>132</v>
       </c>
@@ -7501,9 +7784,9 @@
       <c r="V53" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="W53" s="28"/>
-    </row>
-    <row r="54" spans="1:23" ht="15.75" customHeight="1">
+      <c r="W53" s="27"/>
+    </row>
+    <row r="54" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="26" t="s">
         <v>43</v>
       </c>
@@ -7568,7 +7851,7 @@
       </c>
       <c r="W54" s="10"/>
     </row>
-    <row r="55" spans="1:23" s="38" customFormat="1" ht="15.75" customHeight="1">
+    <row r="55" spans="1:23" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="26" t="s">
         <v>43</v>
       </c>
@@ -7629,9 +7912,9 @@
       </c>
       <c r="U55" s="21"/>
       <c r="V55" s="21"/>
-      <c r="W55" s="37"/>
-    </row>
-    <row r="56" spans="1:23" s="38" customFormat="1" ht="15.75" customHeight="1">
+      <c r="W55" s="36"/>
+    </row>
+    <row r="56" spans="1:23" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="26" t="s">
         <v>43</v>
       </c>
@@ -7692,9 +7975,9 @@
       </c>
       <c r="U56" s="21"/>
       <c r="V56" s="21"/>
-      <c r="W56" s="37"/>
-    </row>
-    <row r="57" spans="1:23" s="38" customFormat="1" ht="15.75" customHeight="1">
+      <c r="W56" s="36"/>
+    </row>
+    <row r="57" spans="1:23" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="26" t="s">
         <v>43</v>
       </c>
@@ -7755,9 +8038,9 @@
       </c>
       <c r="U57" s="21"/>
       <c r="V57" s="21"/>
-      <c r="W57" s="37"/>
-    </row>
-    <row r="58" spans="1:23" s="38" customFormat="1" ht="15.75" customHeight="1">
+      <c r="W57" s="36"/>
+    </row>
+    <row r="58" spans="1:23" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="26" t="s">
         <v>43</v>
       </c>
@@ -7818,9 +8101,9 @@
       </c>
       <c r="U58" s="21"/>
       <c r="V58" s="21"/>
-      <c r="W58" s="37"/>
-    </row>
-    <row r="59" spans="1:23" s="38" customFormat="1" ht="15.75" customHeight="1">
+      <c r="W58" s="36"/>
+    </row>
+    <row r="59" spans="1:23" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="26" t="s">
         <v>43</v>
       </c>
@@ -7881,9 +8164,9 @@
       </c>
       <c r="U59" s="21"/>
       <c r="V59" s="21"/>
-      <c r="W59" s="37"/>
-    </row>
-    <row r="60" spans="1:23" s="35" customFormat="1" ht="15.75" customHeight="1">
+      <c r="W59" s="36"/>
+    </row>
+    <row r="60" spans="1:23" s="34" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="26" t="s">
         <v>43</v>
       </c>
@@ -7926,9 +8209,9 @@
       <c r="T60" s="21"/>
       <c r="U60" s="21"/>
       <c r="V60" s="21"/>
-      <c r="W60" s="34"/>
-    </row>
-    <row r="61" spans="1:23" ht="15.75" customHeight="1">
+      <c r="W60" s="33"/>
+    </row>
+    <row r="61" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="26" t="s">
         <v>58</v>
       </c>
@@ -7993,11 +8276,11 @@
       <c r="V61" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="W61" s="42" t="s">
+      <c r="W61" s="41" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:23" ht="15.75" customHeight="1">
+    <row r="62" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="26" t="s">
         <v>58</v>
       </c>
@@ -8062,9 +8345,9 @@
       <c r="V62" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="W62" s="43"/>
-    </row>
-    <row r="63" spans="1:23" ht="15.75" customHeight="1">
+      <c r="W62" s="42"/>
+    </row>
+    <row r="63" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="26" t="s">
         <v>62</v>
       </c>
@@ -8117,7 +8400,9 @@
       <c r="R63" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="S63" s="21"/>
+      <c r="S63" s="21" t="s">
+        <v>114</v>
+      </c>
       <c r="T63" s="21" t="s">
         <v>132</v>
       </c>
@@ -8129,7 +8414,7 @@
       </c>
       <c r="W63" s="10"/>
     </row>
-    <row r="64" spans="1:23" s="15" customFormat="1" ht="15.75" customHeight="1">
+    <row r="64" spans="1:23" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="18" t="s">
         <v>63</v>
       </c>
@@ -8162,7 +8447,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="65" spans="1:22" ht="15.75" customHeight="1">
+    <row r="65" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="16" t="s">
         <v>63</v>
       </c>
@@ -8204,7 +8489,7 @@
       <c r="U65" s="17"/>
       <c r="V65" s="17"/>
     </row>
-    <row r="66" spans="1:22" ht="15.75" customHeight="1">
+    <row r="66" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="16" t="s">
         <v>63</v>
       </c>
@@ -8234,7 +8519,7 @@
       <c r="U66" s="17"/>
       <c r="V66" s="17"/>
     </row>
-    <row r="67" spans="1:22" ht="15.75" customHeight="1">
+    <row r="67" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="16" t="s">
         <v>63</v>
       </c>
@@ -8264,7 +8549,7 @@
       <c r="U67" s="17"/>
       <c r="V67" s="17"/>
     </row>
-    <row r="68" spans="1:22" ht="15.75" customHeight="1">
+    <row r="68" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="16" t="s">
         <v>63</v>
       </c>
@@ -8294,7 +8579,7 @@
       <c r="U68" s="17"/>
       <c r="V68" s="17"/>
     </row>
-    <row r="69" spans="1:22" s="36" customFormat="1" ht="15.75" customHeight="1">
+    <row r="69" spans="1:22" s="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="16" t="s">
         <v>63</v>
       </c>
@@ -8324,7 +8609,7 @@
       <c r="U69" s="17"/>
       <c r="V69" s="17"/>
     </row>
-    <row r="70" spans="1:22" s="33" customFormat="1" ht="15.75" customHeight="1">
+    <row r="70" spans="1:22" s="32" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="16" t="s">
         <v>63</v>
       </c>
@@ -8354,7 +8639,7 @@
       <c r="U70" s="17"/>
       <c r="V70" s="17"/>
     </row>
-    <row r="71" spans="1:22" ht="15.75" customHeight="1">
+    <row r="71" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="16" t="s">
         <v>110</v>
       </c>
@@ -8384,7 +8669,7 @@
       <c r="U71" s="20"/>
       <c r="V71" s="20"/>
     </row>
-    <row r="72" spans="1:22" ht="15.75" customHeight="1">
+    <row r="72" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="16" t="s">
         <v>120</v>
       </c>
@@ -8395,52 +8680,55 @@
       <c r="D72" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="E72" s="30" t="s">
+      <c r="E72" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="F72" s="30"/>
-      <c r="G72" s="30" t="s">
+      <c r="F72" s="29"/>
+      <c r="G72" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="H72" s="30"/>
-      <c r="I72" s="30"/>
-      <c r="J72" s="30" t="s">
+      <c r="H72" s="29"/>
+      <c r="I72" s="29"/>
+      <c r="J72" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="K72" s="30" t="s">
+      <c r="K72" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="L72" s="30" t="s">
+      <c r="L72" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="M72" s="30" t="s">
+      <c r="M72" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="N72" s="30"/>
-      <c r="O72" s="30"/>
-      <c r="P72" s="30"/>
-      <c r="Q72" s="30"/>
-      <c r="R72" s="30"/>
-      <c r="S72" s="30"/>
-      <c r="T72" s="30"/>
-      <c r="U72" s="30"/>
-      <c r="V72" s="30"/>
+      <c r="N72" s="29"/>
+      <c r="O72" s="29"/>
+      <c r="P72" s="29"/>
+      <c r="Q72" s="29"/>
+      <c r="R72" s="29"/>
+      <c r="S72" s="29"/>
+      <c r="T72" s="29"/>
+      <c r="U72" s="29"/>
+      <c r="V72" s="29"/>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
-      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="G49" sqref="G49"/>
+    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="M10" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="T19" sqref="T19"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
     <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
       <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C22" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
+      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="G49" sqref="G49"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>
@@ -8454,11 +8742,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -8467,10 +8750,10 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="29.6640625" customWidth="1"/>
     <col min="2" max="2" width="28.1640625" customWidth="1"/>
@@ -8478,7 +8761,7 @@
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15">
+    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
         <v>70</v>
       </c>
@@ -8495,7 +8778,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15">
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
         <v>73</v>
       </c>
@@ -8508,7 +8791,7 @@
       <c r="D2" s="24"/>
       <c r="E2" s="24"/>
     </row>
-    <row r="3" spans="1:5" ht="15">
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
         <v>75</v>
       </c>
@@ -8521,7 +8804,7 @@
       <c r="D3" s="24"/>
       <c r="E3" s="24"/>
     </row>
-    <row r="4" spans="1:5" ht="15">
+    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
         <v>77</v>
       </c>
@@ -8534,7 +8817,7 @@
       <c r="D4" s="24"/>
       <c r="E4" s="24"/>
     </row>
-    <row r="5" spans="1:5" ht="15">
+    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
         <v>97</v>
       </c>
@@ -8549,7 +8832,7 @@
       </c>
       <c r="E5" s="24"/>
     </row>
-    <row r="6" spans="1:5" ht="15">
+    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
         <v>98</v>
       </c>
@@ -8564,7 +8847,7 @@
       </c>
       <c r="E6" s="24"/>
     </row>
-    <row r="7" spans="1:5" ht="15">
+    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
         <v>99</v>
       </c>
@@ -8579,7 +8862,7 @@
       </c>
       <c r="E7" s="24"/>
     </row>
-    <row r="8" spans="1:5" ht="15">
+    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
         <v>100</v>
       </c>
@@ -8594,7 +8877,7 @@
       </c>
       <c r="E8" s="24"/>
     </row>
-    <row r="9" spans="1:5" ht="15">
+    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
         <v>109</v>
       </c>
@@ -8607,7 +8890,7 @@
       <c r="D9" s="24"/>
       <c r="E9" s="24"/>
     </row>
-    <row r="10" spans="1:5" ht="15">
+    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
         <v>108</v>
       </c>
@@ -8620,7 +8903,7 @@
       <c r="D10" s="24"/>
       <c r="E10" s="24"/>
     </row>
-    <row r="11" spans="1:5" ht="15">
+    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
         <v>107</v>
       </c>
@@ -8633,7 +8916,7 @@
       <c r="D11" s="24"/>
       <c r="E11" s="24"/>
     </row>
-    <row r="12" spans="1:5" ht="15">
+    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
         <v>101</v>
       </c>
@@ -8648,7 +8931,7 @@
       </c>
       <c r="E12" s="24"/>
     </row>
-    <row r="13" spans="1:5" ht="15">
+    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="23" t="s">
         <v>106</v>
       </c>
@@ -8663,7 +8946,7 @@
       </c>
       <c r="E13" s="24"/>
     </row>
-    <row r="14" spans="1:5" ht="15">
+    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
         <v>102</v>
       </c>
@@ -8678,7 +8961,7 @@
       </c>
       <c r="E14" s="24"/>
     </row>
-    <row r="15" spans="1:5" ht="15">
+    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
         <v>103</v>
       </c>
@@ -8693,7 +8976,7 @@
       </c>
       <c r="E15" s="24"/>
     </row>
-    <row r="16" spans="1:5" ht="15">
+    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
         <v>104</v>
       </c>
@@ -8708,7 +8991,7 @@
       </c>
       <c r="E16" s="24"/>
     </row>
-    <row r="17" spans="1:5" ht="15">
+    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="23" t="s">
         <v>123</v>
       </c>
@@ -8723,7 +9006,7 @@
       </c>
       <c r="E17" s="24"/>
     </row>
-    <row r="18" spans="1:5" ht="15">
+    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
         <v>12</v>
       </c>
@@ -8738,7 +9021,7 @@
       </c>
       <c r="E18" s="24"/>
     </row>
-    <row r="19" spans="1:5" ht="15">
+    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="23" t="s">
         <v>13</v>
       </c>
@@ -8753,7 +9036,7 @@
       </c>
       <c r="E19" s="24"/>
     </row>
-    <row r="20" spans="1:5" ht="15">
+    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
         <v>105</v>
       </c>
@@ -8770,25 +9053,23 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
-      <selection activeCell="C7" sqref="C7"/>
+    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}">
+      <selection activeCell="A21" sqref="A21:XFD21"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
     <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
       <selection activeCell="C7" sqref="C7"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
+      <selection activeCell="C7" sqref="C7"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Lisää tm-valmis oikeus urakanvalvojille (HAR-3282)
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-1340" yWindow="2560" windowWidth="41260" windowHeight="21380" tabRatio="500"/>
+    <workbookView xWindow="3360" yWindow="2020" windowWidth="43600" windowHeight="23700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -17,9 +17,9 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="1933" windowHeight="783" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="2180" windowHeight="1012" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="2379" windowHeight="1295" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
     <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="2379" windowHeight="1295" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -494,9 +494,6 @@
     <t>R = lukuoikeus nimettyihin urakoihin, R,W = luku- ja kirjoitusoikeus nimettyihin urakoihin, W+ kirjoitusoikeus oman organisaation urakoihin, W* kirjoitusoikeus kaikkiin urakoihin, tyhjä = ei näe osiota, muut erikoisoikeuksia</t>
   </si>
   <si>
-    <t>R*,W,TM-takaraja</t>
-  </si>
-  <si>
     <t>R*,W*,TM-valmis*,TM-takaraja*</t>
   </si>
   <si>
@@ -513,6 +510,9 @@
   </si>
   <si>
     <t>Kelikeskus</t>
+  </si>
+  <si>
+    <t>R*,W,TM-takaraja,TM-valmis</t>
   </si>
 </sst>
 </file>
@@ -1021,7 +1021,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{C0D8A1BF-1D13-2C41-BEFB-54E54F9CD4DD}" diskRevisions="1" revisionId="162" version="21">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{01C5CE6A-1AD5-8F40-B383-3FF2F2AC20C5}" diskRevisions="1" revisionId="164" version="22">
   <header guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" dateTime="2016-09-06T09:14:56" maxSheetId="3" userName="Tatu Tarvainen" r:id="rId2" minRId="1" maxRId="3">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1142,6 +1142,12 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{01C5CE6A-1AD5-8F40-B383-3FF2F2AC20C5}" dateTime="2016-11-01T08:45:04" maxSheetId="3" userName="Microsoft Office User" r:id="rId22" minRId="163" maxRId="164">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -3852,6 +3858,37 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog21.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="163" sId="1">
+    <oc r="E28" t="inlineStr">
+      <is>
+        <t>R*,W,TM-takaraja</t>
+      </is>
+    </oc>
+    <nc r="E28" t="inlineStr">
+      <is>
+        <t>R*,W,TM-takaraja,TM-valmis</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="164" sId="1">
+    <oc r="K28" t="inlineStr">
+      <is>
+        <t>R*,W,TM-takaraja</t>
+      </is>
+    </oc>
+    <nc r="K28" t="inlineStr">
+      <is>
+        <t>R*,W,TM-takaraja,TM-valmis</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="delete"/>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="4" sId="1">
@@ -4566,7 +4603,7 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="5">
   <userInfo guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" name="Tatu Tarvainen" id="-130145201" dateTime="2016-09-06T09:10:23"/>
   <userInfo guid="{E0850D7E-A93F-EF44-B46A-3BEA4D7DBEDB}" name="Jarno Väyrynen" id="-589116405" dateTime="2016-09-06T12:54:09"/>
@@ -4901,10 +4938,10 @@
   <dimension ref="A1:W72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="M40" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="G10" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="S55" sqref="S55"/>
+      <selection pane="bottomRight" activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5081,7 +5118,7 @@
         <v>93</v>
       </c>
       <c r="V6" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -6274,10 +6311,10 @@
       </c>
       <c r="C28" s="21"/>
       <c r="D28" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="F28" s="21" t="s">
         <v>128</v>
@@ -6295,7 +6332,7 @@
         <v>127</v>
       </c>
       <c r="K28" s="21" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="L28" s="21" t="s">
         <v>17</v>
@@ -6563,7 +6600,7 @@
         <v>15</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C33" s="21"/>
       <c r="D33" s="17" t="s">
@@ -6619,7 +6656,7 @@
         <v>15</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C34" s="21"/>
       <c r="D34" s="17" t="s">
@@ -6675,7 +6712,7 @@
         <v>15</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C35" s="21"/>
       <c r="D35" s="17" t="s">
@@ -7221,7 +7258,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="26" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C44" s="21"/>
       <c r="D44" s="21" t="s">
@@ -8714,20 +8751,20 @@
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="M10" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="T19" sqref="T19"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="G10" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="K28" sqref="K28"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
+      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="G49" sqref="G49"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
     <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
       <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
-      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="G49" sqref="G49"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -9058,12 +9095,12 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
       <selection activeCell="C7" sqref="C7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
+    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
       <selection activeCell="C7" sqref="C7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Muuta rooli "Urakan turvallisuusvastaava" -> "Kelikeskus" (HAR-3550)
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="2020" windowWidth="43600" windowHeight="23700" tabRatio="500"/>
+    <workbookView xWindow="14160" yWindow="3960" windowWidth="43600" windowHeight="21780" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -17,9 +17,9 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="2180" windowHeight="1012" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="2180" windowHeight="916" tabRatio="500" activeSheetId="2"/>
+    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="2379" windowHeight="1295" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
-    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1101" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1101" uniqueCount="159">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -279,9 +279,6 @@
   </si>
   <si>
     <t>Tilaajan turvallisuusvastaava</t>
-  </si>
-  <si>
-    <t>Urakan turvallisuusvastaava</t>
   </si>
   <si>
     <t>Yrityksen pääkäyttäjä</t>
@@ -1021,7 +1018,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{01C5CE6A-1AD5-8F40-B383-3FF2F2AC20C5}" diskRevisions="1" revisionId="164" version="22">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{C430F4B0-E87C-E742-803B-AF70E849AC88}" diskRevisions="1" revisionId="165" version="23">
   <header guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" dateTime="2016-09-06T09:14:56" maxSheetId="3" userName="Tatu Tarvainen" r:id="rId2" minRId="1" maxRId="3">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1148,6 +1145,12 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{C430F4B0-E87C-E742-803B-AF70E849AC88}" dateTime="2016-11-03T12:59:47" maxSheetId="3" userName="Microsoft Office User" r:id="rId23" minRId="165">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -3883,6 +3886,46 @@
         <t>R*,W,TM-takaraja,TM-valmis</t>
       </is>
     </nc>
+  </rcc>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="delete"/>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog22.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="165" sId="2" xfDxf="1" dxf="1">
+    <oc r="B19" t="inlineStr">
+      <is>
+        <t>Urakan turvallisuusvastaava</t>
+      </is>
+    </oc>
+    <nc r="B19" t="inlineStr">
+      <is>
+        <t>Kelikeskus</t>
+      </is>
+    </nc>
+    <ndxf>
+      <font>
+        <sz val="12"/>
+        <color theme="1"/>
+      </font>
+      <alignment vertical="center" wrapText="1" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
   </rcc>
   <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="delete"/>
   <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="add"/>
@@ -4937,11 +4980,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="G10" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
+      <pane xSplit="2" ySplit="6" topLeftCell="M10" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="K28" sqref="K28"/>
+      <selection pane="bottomRight" activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4976,7 +5019,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="44" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D1" s="45"/>
       <c r="E1" s="45"/>
@@ -5082,43 +5125,43 @@
         <v>81</v>
       </c>
       <c r="J6" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="M6" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="K6" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="L6" s="8" t="s">
+      <c r="N6" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="O6" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="M6" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="N6" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="O6" s="8" t="s">
-        <v>89</v>
-      </c>
       <c r="P6" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q6" s="9" t="s">
         <v>11</v>
       </c>
       <c r="R6" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="S6" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="T6" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="S6" s="9" t="s">
+      <c r="U6" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="T6" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="U6" s="9" t="s">
-        <v>93</v>
-      </c>
       <c r="V6" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5130,61 +5173,61 @@
       </c>
       <c r="C7" s="17"/>
       <c r="D7" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I7" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K7" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L7" s="17" t="s">
         <v>17</v>
       </c>
       <c r="M7" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N7" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O7" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P7" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q7" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="R7" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S7" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="T7" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U7" s="17" t="s">
         <v>17</v>
       </c>
       <c r="V7" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="W7" s="10"/>
     </row>
@@ -5197,31 +5240,31 @@
       </c>
       <c r="C8" s="17"/>
       <c r="D8" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G8" s="21"/>
       <c r="H8" s="21"/>
       <c r="I8" s="21"/>
       <c r="J8" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K8" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L8" s="21"/>
       <c r="M8" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N8" s="21"/>
       <c r="O8" s="17"/>
       <c r="P8" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q8" s="21" t="s">
         <v>17</v>
@@ -5229,7 +5272,7 @@
       <c r="R8" s="17"/>
       <c r="S8" s="17"/>
       <c r="T8" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U8" s="17" t="s">
         <v>19</v>
@@ -5238,7 +5281,7 @@
         <v>19</v>
       </c>
       <c r="W8" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5250,31 +5293,31 @@
       </c>
       <c r="C9" s="17"/>
       <c r="D9" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G9" s="21"/>
       <c r="H9" s="21"/>
       <c r="I9" s="21"/>
       <c r="J9" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K9" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L9" s="21"/>
       <c r="M9" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N9" s="21"/>
       <c r="O9" s="17"/>
       <c r="P9" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q9" s="21" t="s">
         <v>17</v>
@@ -5282,7 +5325,7 @@
       <c r="R9" s="17"/>
       <c r="S9" s="17"/>
       <c r="T9" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U9" s="17"/>
       <c r="V9" s="17"/>
@@ -5293,35 +5336,35 @@
         <v>15</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C10" s="17"/>
       <c r="D10" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G10" s="21"/>
       <c r="H10" s="21"/>
       <c r="I10" s="21"/>
       <c r="J10" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K10" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L10" s="21"/>
       <c r="M10" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N10" s="21"/>
       <c r="O10" s="17"/>
       <c r="P10" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q10" s="21" t="s">
         <v>17</v>
@@ -5329,7 +5372,7 @@
       <c r="R10" s="17"/>
       <c r="S10" s="17"/>
       <c r="T10" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U10" s="17"/>
       <c r="V10" s="17"/>
@@ -5344,53 +5387,53 @@
       </c>
       <c r="C11" s="17"/>
       <c r="D11" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H11" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I11" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J11" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K11" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L11" s="17" t="s">
         <v>17</v>
       </c>
       <c r="M11" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N11" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O11" s="17"/>
       <c r="P11" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q11" s="17" t="s">
         <v>17</v>
       </c>
       <c r="R11" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S11" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T11" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U11" s="17"/>
       <c r="V11" s="17"/>
@@ -5405,53 +5448,53 @@
       </c>
       <c r="C12" s="17"/>
       <c r="D12" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I12" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K12" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L12" s="17" t="s">
         <v>17</v>
       </c>
       <c r="M12" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N12" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O12" s="17"/>
       <c r="P12" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q12" s="17" t="s">
         <v>17</v>
       </c>
       <c r="R12" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S12" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T12" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U12" s="17"/>
       <c r="V12" s="17"/>
@@ -5466,41 +5509,41 @@
       </c>
       <c r="C13" s="17"/>
       <c r="D13" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G13" s="21"/>
       <c r="H13" s="21"/>
       <c r="I13" s="21"/>
       <c r="J13" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K13" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L13" s="17"/>
       <c r="M13" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N13" s="21"/>
       <c r="O13" s="17"/>
       <c r="P13" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q13" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="R13" s="21"/>
       <c r="S13" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="T13" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U13" s="17"/>
       <c r="V13" s="17"/>
@@ -5515,41 +5558,41 @@
       </c>
       <c r="C14" s="17"/>
       <c r="D14" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
       <c r="I14" s="21"/>
       <c r="J14" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K14" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L14" s="17"/>
       <c r="M14" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N14" s="21"/>
       <c r="O14" s="17"/>
       <c r="P14" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q14" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="R14" s="21"/>
       <c r="S14" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="T14" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U14" s="17"/>
       <c r="V14" s="17"/>
@@ -5560,45 +5603,45 @@
         <v>15</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C15" s="17"/>
       <c r="D15" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G15" s="21"/>
       <c r="H15" s="21"/>
       <c r="I15" s="21"/>
       <c r="J15" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K15" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L15" s="17"/>
       <c r="M15" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N15" s="21"/>
       <c r="O15" s="17"/>
       <c r="P15" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q15" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="R15" s="21"/>
       <c r="S15" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="T15" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U15" s="17"/>
       <c r="V15" s="17"/>
@@ -5613,53 +5656,53 @@
       </c>
       <c r="C16" s="17"/>
       <c r="D16" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I16" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J16" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K16" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L16" s="17" t="s">
         <v>17</v>
       </c>
       <c r="M16" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N16" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O16" s="17"/>
       <c r="P16" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q16" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="R16" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S16" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="T16" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U16" s="17"/>
       <c r="V16" s="17"/>
@@ -5674,53 +5717,53 @@
       </c>
       <c r="C17" s="17"/>
       <c r="D17" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I17" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J17" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K17" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L17" s="17" t="s">
         <v>17</v>
       </c>
       <c r="M17" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N17" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O17" s="17"/>
       <c r="P17" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q17" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="R17" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S17" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="T17" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U17" s="17"/>
       <c r="V17" s="17"/>
@@ -5735,41 +5778,41 @@
       </c>
       <c r="C18" s="17"/>
       <c r="D18" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G18" s="21"/>
       <c r="H18" s="21"/>
       <c r="I18" s="21"/>
       <c r="J18" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K18" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L18" s="17"/>
       <c r="M18" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N18" s="21"/>
       <c r="O18" s="17"/>
       <c r="P18" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q18" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="R18" s="21"/>
       <c r="S18" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="T18" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U18" s="17"/>
       <c r="V18" s="17"/>
@@ -5784,53 +5827,53 @@
       </c>
       <c r="C19" s="17"/>
       <c r="D19" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F19" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H19" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I19" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J19" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K19" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L19" s="17" t="s">
         <v>17</v>
       </c>
       <c r="M19" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N19" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O19" s="17"/>
       <c r="P19" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q19" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="R19" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S19" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="T19" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U19" s="17"/>
       <c r="V19" s="17"/>
@@ -5845,55 +5888,55 @@
       </c>
       <c r="C20" s="17"/>
       <c r="D20" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G20" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="H20" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="I20" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="J20" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="K20" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="H20" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="I20" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="J20" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="K20" s="17" t="s">
-        <v>131</v>
-      </c>
       <c r="L20" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M20" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N20" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O20" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P20" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q20" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="R20" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S20" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="T20" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U20" s="17" t="s">
         <v>17</v>
@@ -5912,55 +5955,55 @@
       </c>
       <c r="C21" s="21"/>
       <c r="D21" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F21" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G21" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="H21" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="I21" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="J21" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="K21" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="H21" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="I21" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="J21" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="K21" s="17" t="s">
-        <v>131</v>
-      </c>
       <c r="L21" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M21" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N21" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O21" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P21" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q21" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="R21" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S21" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="T21" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U21" s="21" t="s">
         <v>17</v>
@@ -5979,60 +6022,60 @@
       </c>
       <c r="C22" s="21"/>
       <c r="D22" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F22" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G22" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H22" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I22" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J22" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K22" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L22" s="21" t="s">
         <v>17</v>
       </c>
       <c r="M22" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N22" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O22" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P22" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q22" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R22" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S22" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T22" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U22" s="21"/>
       <c r="V22" s="21"/>
       <c r="W22" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -6044,55 +6087,55 @@
       </c>
       <c r="C23" s="21"/>
       <c r="D23" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F23" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G23" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H23" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I23" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J23" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K23" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="M23" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N23" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O23" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P23" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q23" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="R23" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S23" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="T23" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U23" s="21"/>
       <c r="V23" s="21"/>
@@ -6107,58 +6150,58 @@
       </c>
       <c r="C24" s="21"/>
       <c r="D24" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="E24" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="E24" s="17" t="s">
-        <v>142</v>
-      </c>
       <c r="F24" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G24" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H24" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I24" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J24" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="K24" s="21" t="s">
         <v>141</v>
       </c>
-      <c r="K24" s="21" t="s">
-        <v>142</v>
-      </c>
       <c r="L24" s="21" t="s">
         <v>17</v>
       </c>
       <c r="M24" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N24" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O24" s="21"/>
       <c r="P24" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q24" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="Q24" s="21" t="s">
-        <v>151</v>
-      </c>
       <c r="R24" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="S24" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="T24" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U24" s="21"/>
       <c r="V24" s="21"/>
       <c r="W24" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="25" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -6170,47 +6213,47 @@
       </c>
       <c r="C25" s="21"/>
       <c r="D25" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F25" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G25" s="21"/>
       <c r="H25" s="21"/>
       <c r="I25" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J25" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K25" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L25" s="21"/>
       <c r="M25" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N25" s="21"/>
       <c r="O25" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="P25" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q25" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="R25" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S25" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="T25" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U25" s="21"/>
       <c r="V25" s="21"/>
@@ -6225,31 +6268,31 @@
       </c>
       <c r="C26" s="21"/>
       <c r="D26" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F26" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G26" s="21"/>
       <c r="H26" s="21"/>
       <c r="I26" s="21"/>
       <c r="J26" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K26" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L26" s="21"/>
       <c r="M26" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N26" s="21"/>
       <c r="O26" s="21"/>
       <c r="P26" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q26" s="21" t="s">
         <v>17</v>
@@ -6257,7 +6300,7 @@
       <c r="R26" s="21"/>
       <c r="S26" s="21"/>
       <c r="T26" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U26" s="21"/>
       <c r="V26" s="21"/>
@@ -6272,20 +6315,20 @@
       </c>
       <c r="C27" s="21"/>
       <c r="D27" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F27" s="21"/>
       <c r="G27" s="21"/>
       <c r="H27" s="21"/>
       <c r="I27" s="21"/>
       <c r="J27" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K27" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L27" s="21"/>
       <c r="M27" s="21"/>
@@ -6311,58 +6354,58 @@
       </c>
       <c r="C28" s="21"/>
       <c r="D28" s="17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F28" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G28" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H28" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I28" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J28" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K28" s="21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L28" s="21" t="s">
         <v>17</v>
       </c>
       <c r="M28" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N28" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O28" s="21"/>
       <c r="P28" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q28" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="R28" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S28" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T28" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U28" s="21"/>
       <c r="V28" s="21"/>
       <c r="W28" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -6374,49 +6417,49 @@
       </c>
       <c r="C29" s="21"/>
       <c r="D29" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F29" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G29" s="21"/>
       <c r="H29" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I29" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J29" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K29" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L29" s="21"/>
       <c r="M29" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N29" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O29" s="21"/>
       <c r="P29" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q29" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="R29" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S29" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T29" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U29" s="21"/>
       <c r="V29" s="21"/>
@@ -6431,51 +6474,51 @@
       </c>
       <c r="C30" s="21"/>
       <c r="D30" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F30" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G30" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H30" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I30" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J30" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K30" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L30" s="21"/>
       <c r="M30" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N30" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O30" s="21"/>
       <c r="P30" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q30" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="R30" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S30" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T30" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U30" s="21"/>
       <c r="V30" s="21"/>
@@ -6490,49 +6533,49 @@
       </c>
       <c r="C31" s="21"/>
       <c r="D31" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F31" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G31" s="21"/>
       <c r="H31" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I31" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J31" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K31" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L31" s="21"/>
       <c r="M31" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N31" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O31" s="21"/>
       <c r="P31" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q31" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="R31" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S31" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T31" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U31" s="21"/>
       <c r="V31" s="21"/>
@@ -6547,49 +6590,49 @@
       </c>
       <c r="C32" s="21"/>
       <c r="D32" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F32" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G32" s="21"/>
       <c r="H32" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I32" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J32" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K32" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L32" s="21"/>
       <c r="M32" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N32" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O32" s="21"/>
       <c r="P32" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q32" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="R32" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S32" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T32" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U32" s="21"/>
       <c r="V32" s="21"/>
@@ -6600,53 +6643,53 @@
         <v>15</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C33" s="21"/>
       <c r="D33" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E33" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F33" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G33" s="21"/>
       <c r="H33" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I33" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J33" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K33" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L33" s="21"/>
       <c r="M33" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N33" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O33" s="17"/>
       <c r="P33" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q33" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="R33" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S33" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T33" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U33" s="21"/>
       <c r="V33" s="21"/>
@@ -6656,53 +6699,53 @@
         <v>15</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C34" s="21"/>
       <c r="D34" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F34" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G34" s="21"/>
       <c r="H34" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I34" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J34" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K34" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L34" s="21"/>
       <c r="M34" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N34" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O34" s="17"/>
       <c r="P34" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q34" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="R34" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S34" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T34" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U34" s="21"/>
       <c r="V34" s="21"/>
@@ -6712,53 +6755,53 @@
         <v>15</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C35" s="21"/>
       <c r="D35" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E35" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F35" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G35" s="21"/>
       <c r="H35" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I35" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J35" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K35" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L35" s="21"/>
       <c r="M35" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N35" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O35" s="17"/>
       <c r="P35" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q35" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="R35" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S35" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T35" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U35" s="21"/>
       <c r="V35" s="21"/>
@@ -6768,59 +6811,59 @@
         <v>15</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C36" s="21"/>
       <c r="D36" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E36" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F36" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G36" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H36" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I36" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J36" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K36" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L36" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M36" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N36" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O36" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P36" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q36" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="R36" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S36" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="T36" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U36" s="21" t="s">
         <v>17</v>
@@ -6835,35 +6878,35 @@
         <v>43</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C37" s="21"/>
       <c r="D37" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E37" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F37" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G37" s="21"/>
       <c r="H37" s="21"/>
       <c r="I37" s="21"/>
       <c r="J37" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K37" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L37" s="21"/>
       <c r="M37" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N37" s="21"/>
       <c r="O37" s="21"/>
       <c r="P37" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q37" s="21" t="s">
         <v>17</v>
@@ -6871,7 +6914,7 @@
       <c r="R37" s="21"/>
       <c r="S37" s="21"/>
       <c r="T37" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U37" s="21"/>
       <c r="V37" s="21"/>
@@ -6886,13 +6929,13 @@
       </c>
       <c r="C38" s="21"/>
       <c r="D38" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E38" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F38" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G38" s="21" t="s">
         <v>19</v>
@@ -6900,19 +6943,19 @@
       <c r="H38" s="21"/>
       <c r="I38" s="21"/>
       <c r="J38" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K38" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L38" s="21"/>
       <c r="M38" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N38" s="21"/>
       <c r="O38" s="21"/>
       <c r="P38" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q38" s="21" t="s">
         <v>17</v>
@@ -6920,7 +6963,7 @@
       <c r="R38" s="21"/>
       <c r="S38" s="21"/>
       <c r="T38" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U38" s="21"/>
       <c r="V38" s="21"/>
@@ -6935,55 +6978,55 @@
       </c>
       <c r="C39" s="21"/>
       <c r="D39" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E39" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F39" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G39" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H39" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I39" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J39" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K39" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L39" s="21" t="s">
         <v>17</v>
       </c>
       <c r="M39" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N39" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O39" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P39" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q39" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R39" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S39" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T39" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U39" s="21"/>
       <c r="V39" s="21" t="s">
@@ -7000,55 +7043,55 @@
       </c>
       <c r="C40" s="21"/>
       <c r="D40" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E40" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F40" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G40" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H40" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I40" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J40" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K40" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L40" s="21" t="s">
         <v>17</v>
       </c>
       <c r="M40" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N40" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O40" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P40" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q40" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R40" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S40" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T40" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U40" s="21" t="s">
         <v>17</v>
@@ -7063,59 +7106,59 @@
         <v>43</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C41" s="21"/>
       <c r="D41" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E41" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F41" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G41" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H41" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I41" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J41" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K41" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L41" s="21" t="s">
         <v>17</v>
       </c>
       <c r="M41" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N41" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O41" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P41" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q41" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R41" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S41" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T41" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U41" s="21"/>
       <c r="V41" s="21" t="s">
@@ -7132,55 +7175,55 @@
       </c>
       <c r="C42" s="21"/>
       <c r="D42" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E42" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F42" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G42" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H42" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I42" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J42" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K42" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L42" s="21" t="s">
         <v>17</v>
       </c>
       <c r="M42" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N42" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O42" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P42" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q42" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R42" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S42" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T42" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U42" s="21"/>
       <c r="V42" s="21" t="s">
@@ -7197,55 +7240,55 @@
       </c>
       <c r="C43" s="21"/>
       <c r="D43" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E43" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F43" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G43" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H43" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I43" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J43" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K43" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L43" s="21" t="s">
         <v>17</v>
       </c>
       <c r="M43" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N43" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O43" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P43" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q43" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R43" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S43" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T43" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U43" s="21"/>
       <c r="V43" s="21" t="s">
@@ -7258,59 +7301,59 @@
         <v>43</v>
       </c>
       <c r="B44" s="26" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C44" s="21"/>
       <c r="D44" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E44" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F44" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G44" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H44" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I44" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J44" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K44" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L44" s="21" t="s">
         <v>17</v>
       </c>
       <c r="M44" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N44" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O44" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P44" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q44" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R44" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S44" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T44" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U44" s="21"/>
       <c r="V44" s="21" t="s">
@@ -7327,55 +7370,55 @@
       </c>
       <c r="C45" s="21"/>
       <c r="D45" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E45" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F45" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G45" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H45" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I45" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J45" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K45" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L45" s="21" t="s">
         <v>17</v>
       </c>
       <c r="M45" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N45" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O45" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P45" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q45" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R45" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S45" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T45" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U45" s="21"/>
       <c r="V45" s="21" t="s">
@@ -7392,53 +7435,53 @@
       </c>
       <c r="C46" s="21"/>
       <c r="D46" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E46" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F46" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G46" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H46" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I46" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J46" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K46" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L46" s="21" t="s">
         <v>17</v>
       </c>
       <c r="M46" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N46" s="21"/>
       <c r="O46" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P46" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q46" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R46" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S46" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T46" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U46" s="21"/>
       <c r="V46" s="21" t="s">
@@ -7455,55 +7498,55 @@
       </c>
       <c r="C47" s="21"/>
       <c r="D47" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E47" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F47" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G47" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H47" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I47" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J47" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K47" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L47" s="21" t="s">
         <v>17</v>
       </c>
       <c r="M47" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N47" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O47" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P47" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q47" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R47" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S47" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T47" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U47" s="21"/>
       <c r="V47" s="21" t="s">
@@ -7520,47 +7563,47 @@
       </c>
       <c r="C48" s="21"/>
       <c r="D48" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E48" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F48" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G48" s="21"/>
       <c r="H48" s="21"/>
       <c r="I48" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J48" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K48" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L48" s="21"/>
       <c r="M48" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N48" s="21"/>
       <c r="O48" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P48" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q48" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R48" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S48" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T48" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U48" s="21"/>
       <c r="V48" s="21" t="s">
@@ -7577,13 +7620,13 @@
       </c>
       <c r="C49" s="21"/>
       <c r="D49" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E49" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F49" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G49" s="21"/>
       <c r="H49" s="21" t="s">
@@ -7591,21 +7634,21 @@
       </c>
       <c r="I49" s="21"/>
       <c r="J49" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K49" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L49" s="21"/>
       <c r="M49" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N49" s="21" t="s">
         <v>19</v>
       </c>
       <c r="O49" s="21"/>
       <c r="P49" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q49" s="21" t="s">
         <v>17</v>
@@ -7613,7 +7656,7 @@
       <c r="R49" s="21"/>
       <c r="S49" s="21"/>
       <c r="T49" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U49" s="21"/>
       <c r="V49" s="21"/>
@@ -7628,31 +7671,31 @@
       </c>
       <c r="C50" s="21"/>
       <c r="D50" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E50" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F50" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G50" s="21"/>
       <c r="H50" s="21"/>
       <c r="I50" s="21"/>
       <c r="J50" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K50" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L50" s="21"/>
       <c r="M50" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N50" s="21"/>
       <c r="O50" s="21"/>
       <c r="P50" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q50" s="21" t="s">
         <v>17</v>
@@ -7660,7 +7703,7 @@
       <c r="R50" s="21"/>
       <c r="S50" s="21"/>
       <c r="T50" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U50" s="21"/>
       <c r="V50" s="21"/>
@@ -7675,31 +7718,31 @@
       </c>
       <c r="C51" s="21"/>
       <c r="D51" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E51" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F51" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G51" s="21"/>
       <c r="H51" s="21"/>
       <c r="I51" s="21"/>
       <c r="J51" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K51" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L51" s="21"/>
       <c r="M51" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N51" s="21"/>
       <c r="O51" s="21"/>
       <c r="P51" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q51" s="21" t="s">
         <v>17</v>
@@ -7707,7 +7750,7 @@
       <c r="R51" s="21"/>
       <c r="S51" s="21"/>
       <c r="T51" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U51" s="21"/>
       <c r="V51" s="21"/>
@@ -7722,31 +7765,31 @@
       </c>
       <c r="C52" s="21"/>
       <c r="D52" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E52" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F52" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G52" s="21"/>
       <c r="H52" s="21"/>
       <c r="I52" s="21"/>
       <c r="J52" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K52" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L52" s="21"/>
       <c r="M52" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N52" s="21"/>
       <c r="O52" s="21"/>
       <c r="P52" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q52" s="21" t="s">
         <v>17</v>
@@ -7754,7 +7797,7 @@
       <c r="R52" s="21"/>
       <c r="S52" s="21"/>
       <c r="T52" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U52" s="21"/>
       <c r="V52" s="21"/>
@@ -7765,57 +7808,57 @@
         <v>43</v>
       </c>
       <c r="B53" s="26" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C53" s="21"/>
       <c r="D53" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E53" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F53" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G53" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H53" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I53" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J53" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K53" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L53" s="21" t="s">
         <v>17</v>
       </c>
       <c r="M53" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N53" s="21"/>
       <c r="O53" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P53" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q53" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R53" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S53" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T53" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U53" s="21"/>
       <c r="V53" s="21" t="s">
@@ -7832,55 +7875,55 @@
       </c>
       <c r="C54" s="21"/>
       <c r="D54" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E54" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F54" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G54" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H54" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I54" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J54" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K54" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L54" s="21" t="s">
         <v>17</v>
       </c>
       <c r="M54" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N54" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O54" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P54" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q54" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R54" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S54" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T54" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U54" s="21"/>
       <c r="V54" s="21" t="s">
@@ -7893,59 +7936,59 @@
         <v>43</v>
       </c>
       <c r="B55" s="26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C55" s="21"/>
       <c r="D55" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E55" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F55" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G55" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H55" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I55" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J55" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K55" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L55" s="21" t="s">
         <v>17</v>
       </c>
       <c r="M55" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N55" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O55" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P55" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q55" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R55" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S55" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T55" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U55" s="21"/>
       <c r="V55" s="21"/>
@@ -7956,59 +7999,59 @@
         <v>43</v>
       </c>
       <c r="B56" s="26" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C56" s="21"/>
       <c r="D56" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E56" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F56" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G56" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H56" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I56" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J56" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K56" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L56" s="21" t="s">
         <v>17</v>
       </c>
       <c r="M56" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N56" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O56" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P56" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q56" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R56" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S56" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T56" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U56" s="21"/>
       <c r="V56" s="21"/>
@@ -8019,59 +8062,59 @@
         <v>43</v>
       </c>
       <c r="B57" s="26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C57" s="21"/>
       <c r="D57" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E57" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F57" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G57" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H57" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I57" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J57" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K57" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L57" s="21" t="s">
         <v>17</v>
       </c>
       <c r="M57" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N57" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O57" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P57" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q57" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R57" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S57" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T57" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U57" s="21"/>
       <c r="V57" s="21"/>
@@ -8082,59 +8125,59 @@
         <v>43</v>
       </c>
       <c r="B58" s="26" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C58" s="21"/>
       <c r="D58" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E58" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F58" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G58" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H58" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I58" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J58" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K58" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L58" s="21" t="s">
         <v>17</v>
       </c>
       <c r="M58" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N58" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O58" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P58" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q58" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R58" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S58" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T58" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U58" s="21"/>
       <c r="V58" s="21"/>
@@ -8145,59 +8188,59 @@
         <v>43</v>
       </c>
       <c r="B59" s="26" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C59" s="21"/>
       <c r="D59" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E59" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F59" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G59" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H59" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I59" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J59" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K59" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L59" s="21" t="s">
         <v>17</v>
       </c>
       <c r="M59" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N59" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O59" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P59" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q59" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R59" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S59" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T59" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U59" s="21"/>
       <c r="V59" s="21"/>
@@ -8208,35 +8251,35 @@
         <v>43</v>
       </c>
       <c r="B60" s="26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C60" s="21"/>
       <c r="D60" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E60" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F60" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G60" s="21"/>
       <c r="H60" s="21"/>
       <c r="I60" s="21"/>
       <c r="J60" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K60" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L60" s="21"/>
       <c r="M60" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N60" s="21"/>
       <c r="O60" s="21"/>
       <c r="P60" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q60" s="21" t="s">
         <v>17</v>
@@ -8257,55 +8300,55 @@
       </c>
       <c r="C61" s="21"/>
       <c r="D61" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E61" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F61" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G61" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H61" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I61" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J61" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K61" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L61" s="21" t="s">
         <v>17</v>
       </c>
       <c r="M61" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N61" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O61" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P61" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q61" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R61" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S61" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T61" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U61" s="21" t="s">
         <v>17</v>
@@ -8326,55 +8369,55 @@
       </c>
       <c r="C62" s="21"/>
       <c r="D62" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E62" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F62" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G62" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H62" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I62" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J62" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K62" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L62" s="21" t="s">
         <v>17</v>
       </c>
       <c r="M62" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N62" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O62" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P62" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q62" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R62" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S62" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T62" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U62" s="21" t="s">
         <v>17</v>
@@ -8393,58 +8436,58 @@
       </c>
       <c r="C63" s="21"/>
       <c r="D63" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E63" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F63" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G63" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H63" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I63" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J63" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K63" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L63" s="21" t="s">
         <v>17</v>
       </c>
       <c r="M63" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N63" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O63" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P63" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q63" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="R63" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S63" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="T63" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U63" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="V63" s="21" t="s">
         <v>17</v>
@@ -8460,7 +8503,7 @@
       </c>
       <c r="C64" s="19"/>
       <c r="D64" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E64" s="19"/>
       <c r="F64" s="19"/>
@@ -8493,7 +8536,7 @@
       </c>
       <c r="C65" s="17"/>
       <c r="D65" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E65" s="17"/>
       <c r="F65" s="17" t="s">
@@ -8535,7 +8578,7 @@
       </c>
       <c r="C66" s="17"/>
       <c r="D66" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E66" s="17"/>
       <c r="F66" s="17"/>
@@ -8565,7 +8608,7 @@
       </c>
       <c r="C67" s="17"/>
       <c r="D67" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E67" s="17"/>
       <c r="F67" s="17"/>
@@ -8595,7 +8638,7 @@
       </c>
       <c r="C68" s="17"/>
       <c r="D68" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E68" s="17"/>
       <c r="F68" s="17"/>
@@ -8625,7 +8668,7 @@
       </c>
       <c r="C69" s="17"/>
       <c r="D69" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E69" s="17"/>
       <c r="F69" s="17"/>
@@ -8651,11 +8694,11 @@
         <v>63</v>
       </c>
       <c r="B70" s="16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C70" s="17"/>
       <c r="D70" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E70" s="17"/>
       <c r="F70" s="17"/>
@@ -8678,14 +8721,14 @@
     </row>
     <row r="71" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="B71" s="16" t="s">
         <v>110</v>
-      </c>
-      <c r="B71" s="16" t="s">
-        <v>111</v>
       </c>
       <c r="C71" s="20"/>
       <c r="D71" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E71" s="20"/>
       <c r="F71" s="20"/>
@@ -8708,35 +8751,35 @@
     </row>
     <row r="72" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="B72" s="16" t="s">
         <v>120</v>
-      </c>
-      <c r="B72" s="16" t="s">
-        <v>121</v>
       </c>
       <c r="C72" s="20"/>
       <c r="D72" s="21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E72" s="29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F72" s="29"/>
       <c r="G72" s="29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H72" s="29"/>
       <c r="I72" s="29"/>
       <c r="J72" s="29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K72" s="29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L72" s="29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="M72" s="29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N72" s="29"/>
       <c r="O72" s="29"/>
@@ -8751,20 +8794,20 @@
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="G10" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="K28" sqref="K28"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="M10" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="V6" sqref="V6"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
+      <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
     <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
       <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="bottomRight" activeCell="G49" sqref="G49"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
-      <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -8786,8 +8829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8809,10 +8852,10 @@
         <v>72</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -8856,7 +8899,7 @@
     </row>
     <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B5" s="23" t="s">
         <v>79</v>
@@ -8865,13 +8908,13 @@
         <v>3</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E5" s="24"/>
     </row>
     <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B6" s="23" t="s">
         <v>80</v>
@@ -8880,13 +8923,13 @@
         <v>3</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E6" s="24"/>
     </row>
     <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B7" s="23" t="s">
         <v>81</v>
@@ -8895,31 +8938,31 @@
         <v>3</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E7" s="24"/>
     </row>
     <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C8" s="23" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E8" s="24"/>
     </row>
     <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C9" s="23" t="s">
         <v>5</v>
@@ -8929,10 +8972,10 @@
     </row>
     <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C10" s="23" t="s">
         <v>5</v>
@@ -8942,10 +8985,10 @@
     </row>
     <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C11" s="23" t="s">
         <v>5</v>
@@ -8955,82 +8998,82 @@
     </row>
     <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C12" s="23" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E12" s="24"/>
     </row>
     <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C13" s="23" t="s">
         <v>5</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E13" s="24"/>
     </row>
     <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C14" s="23" t="s">
         <v>5</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E14" s="24"/>
     </row>
     <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C15" s="23" t="s">
         <v>4</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E15" s="24"/>
     </row>
     <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C16" s="23" t="s">
         <v>4</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E16" s="24"/>
     </row>
     <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B17" s="23" t="s">
         <v>11</v>
@@ -9039,7 +9082,7 @@
         <v>4</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E17" s="24"/>
     </row>
@@ -9048,13 +9091,13 @@
         <v>12</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C18" s="23" t="s">
         <v>4</v>
       </c>
       <c r="D18" s="24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E18" s="24"/>
     </row>
@@ -9063,44 +9106,44 @@
         <v>13</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>82</v>
+        <v>157</v>
       </c>
       <c r="C19" s="23" t="s">
         <v>4</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E19" s="24"/>
     </row>
     <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C20" s="23" t="s">
         <v>4</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E20" s="24"/>
     </row>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+      <selection activeCell="B19" sqref="B19"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
+      <selection activeCell="C7" sqref="C7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
     <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
-      <selection activeCell="C7" sqref="C7"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
       <selection activeCell="C7" sqref="C7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Lisää kelikeskukselle W oikeus
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarihan/Desktop/Harja/harja/resources/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14160" yWindow="3960" windowWidth="43600" windowHeight="21780" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="760" yWindow="0" windowWidth="50440" windowHeight="23560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -17,16 +12,16 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="2379" windowHeight="1295" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
+    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="2180" windowHeight="916" tabRatio="500" activeSheetId="2"/>
-    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="2379" windowHeight="1295" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
   </customWorkbookViews>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -1018,7 +1013,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{C430F4B0-E87C-E742-803B-AF70E849AC88}" diskRevisions="1" revisionId="165" version="23">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{C0B302B3-5097-3546-81CC-979DBA1FB813}" diskRevisions="1" revisionId="166" version="24">
   <header guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" dateTime="2016-09-06T09:14:56" maxSheetId="3" userName="Tatu Tarvainen" r:id="rId2" minRId="1" maxRId="3">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1151,6 +1146,12 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{C0B302B3-5097-3546-81CC-979DBA1FB813}" dateTime="2016-11-24T13:21:58" maxSheetId="3" userName="Tatu Tarvainen" r:id="rId24" minRId="166">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -3932,6 +3933,23 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog23.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="166" sId="1">
+    <oc r="V63" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </oc>
+    <nc r="V63" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="4" sId="1">
@@ -4646,7 +4664,7 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="5">
   <userInfo guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" name="Tatu Tarvainen" id="-130145201" dateTime="2016-09-06T09:10:23"/>
   <userInfo guid="{E0850D7E-A93F-EF44-B46A-3BEA4D7DBEDB}" name="Jarno Väyrynen" id="-589116405" dateTime="2016-09-06T12:54:09"/>
@@ -4980,14 +4998,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W72"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="M10" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
+      <pane xSplit="2" ySplit="6" topLeftCell="M51" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="V6" sqref="V6"/>
+      <selection pane="bottomRight" activeCell="V64" sqref="V64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.5" bestFit="1" customWidth="1"/>
@@ -5013,7 +5031,7 @@
     <col min="23" max="23" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="24" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:23" ht="24" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -5033,7 +5051,7 @@
       <c r="M1" s="45"/>
       <c r="N1" s="45"/>
     </row>
-    <row r="2" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:23" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="46" t="s">
@@ -5051,7 +5069,7 @@
       <c r="M2" s="42"/>
       <c r="N2" s="42"/>
     </row>
-    <row r="3" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:23" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -5066,10 +5084,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:23" ht="15.75" customHeight="1">
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:23" ht="15.75" customHeight="1">
       <c r="C5" s="43" t="s">
         <v>6</v>
       </c>
@@ -5098,7 +5116,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:23" ht="15.75" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
@@ -5164,7 +5182,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:23" ht="15.75" customHeight="1">
       <c r="A7" s="16" t="s">
         <v>15</v>
       </c>
@@ -5231,7 +5249,7 @@
       </c>
       <c r="W7" s="10"/>
     </row>
-    <row r="8" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:23" ht="15.75" customHeight="1">
       <c r="A8" s="16" t="s">
         <v>15</v>
       </c>
@@ -5284,7 +5302,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:23" ht="15.75" customHeight="1">
       <c r="A9" s="16" t="s">
         <v>15</v>
       </c>
@@ -5331,7 +5349,7 @@
       <c r="V9" s="17"/>
       <c r="W9" s="10"/>
     </row>
-    <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:23" ht="15.75" customHeight="1">
       <c r="A10" s="16" t="s">
         <v>15</v>
       </c>
@@ -5378,7 +5396,7 @@
       <c r="V10" s="17"/>
       <c r="W10" s="10"/>
     </row>
-    <row r="11" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:23" ht="15.75" customHeight="1">
       <c r="A11" s="16" t="s">
         <v>15</v>
       </c>
@@ -5439,7 +5457,7 @@
       <c r="V11" s="17"/>
       <c r="W11" s="10"/>
     </row>
-    <row r="12" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:23" ht="15.75" customHeight="1">
       <c r="A12" s="16" t="s">
         <v>15</v>
       </c>
@@ -5500,7 +5518,7 @@
       <c r="V12" s="17"/>
       <c r="W12" s="10"/>
     </row>
-    <row r="13" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:23" ht="15.75" customHeight="1">
       <c r="A13" s="16" t="s">
         <v>15</v>
       </c>
@@ -5549,7 +5567,7 @@
       <c r="V13" s="17"/>
       <c r="W13" s="10"/>
     </row>
-    <row r="14" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:23" ht="15.75" customHeight="1">
       <c r="A14" s="16" t="s">
         <v>15</v>
       </c>
@@ -5598,7 +5616,7 @@
       <c r="V14" s="17"/>
       <c r="W14" s="10"/>
     </row>
-    <row r="15" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:23" ht="15.75" customHeight="1">
       <c r="A15" s="16" t="s">
         <v>15</v>
       </c>
@@ -5647,7 +5665,7 @@
       <c r="V15" s="17"/>
       <c r="W15" s="10"/>
     </row>
-    <row r="16" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:23" ht="15.75" customHeight="1">
       <c r="A16" s="16" t="s">
         <v>15</v>
       </c>
@@ -5708,7 +5726,7 @@
       <c r="V16" s="17"/>
       <c r="W16" s="10"/>
     </row>
-    <row r="17" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:23" ht="15.75" customHeight="1">
       <c r="A17" s="16" t="s">
         <v>15</v>
       </c>
@@ -5769,7 +5787,7 @@
       <c r="V17" s="17"/>
       <c r="W17" s="10"/>
     </row>
-    <row r="18" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:23" ht="15.75" customHeight="1">
       <c r="A18" s="16" t="s">
         <v>15</v>
       </c>
@@ -5818,7 +5836,7 @@
       <c r="V18" s="17"/>
       <c r="W18" s="10"/>
     </row>
-    <row r="19" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:23" ht="15.75" customHeight="1">
       <c r="A19" s="16" t="s">
         <v>15</v>
       </c>
@@ -5879,7 +5897,7 @@
       <c r="V19" s="17"/>
       <c r="W19" s="10"/>
     </row>
-    <row r="20" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:23" ht="15.75" customHeight="1">
       <c r="A20" s="16" t="s">
         <v>15</v>
       </c>
@@ -5946,7 +5964,7 @@
       </c>
       <c r="W20" s="10"/>
     </row>
-    <row r="21" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:23" ht="15.75" customHeight="1">
       <c r="A21" s="26" t="s">
         <v>15</v>
       </c>
@@ -6013,7 +6031,7 @@
       </c>
       <c r="W21" s="10"/>
     </row>
-    <row r="22" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:23" ht="15.75" customHeight="1">
       <c r="A22" s="26" t="s">
         <v>15</v>
       </c>
@@ -6078,7 +6096,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="23" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:23" ht="15.75" customHeight="1">
       <c r="A23" s="26" t="s">
         <v>15</v>
       </c>
@@ -6141,7 +6159,7 @@
       <c r="V23" s="21"/>
       <c r="W23" s="10"/>
     </row>
-    <row r="24" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:23" ht="15.75" customHeight="1">
       <c r="A24" s="26" t="s">
         <v>15</v>
       </c>
@@ -6204,7 +6222,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="25" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:23" ht="15.75" customHeight="1">
       <c r="A25" s="26" t="s">
         <v>15</v>
       </c>
@@ -6259,7 +6277,7 @@
       <c r="V25" s="21"/>
       <c r="W25" s="10"/>
     </row>
-    <row r="26" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:23" ht="15.75" customHeight="1">
       <c r="A26" s="26" t="s">
         <v>15</v>
       </c>
@@ -6306,7 +6324,7 @@
       <c r="V26" s="21"/>
       <c r="W26" s="10"/>
     </row>
-    <row r="27" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:23" ht="15.75" customHeight="1">
       <c r="A27" s="26" t="s">
         <v>15</v>
       </c>
@@ -6345,7 +6363,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:23" ht="15.75" customHeight="1">
       <c r="A28" s="26" t="s">
         <v>15</v>
       </c>
@@ -6408,7 +6426,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="29" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:23" ht="15.75" customHeight="1">
       <c r="A29" s="26" t="s">
         <v>15</v>
       </c>
@@ -6465,7 +6483,7 @@
       <c r="V29" s="21"/>
       <c r="W29" s="10"/>
     </row>
-    <row r="30" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:23" ht="15.75" customHeight="1">
       <c r="A30" s="26" t="s">
         <v>15</v>
       </c>
@@ -6524,7 +6542,7 @@
       <c r="V30" s="21"/>
       <c r="W30" s="10"/>
     </row>
-    <row r="31" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:23" ht="15.75" customHeight="1">
       <c r="A31" s="26" t="s">
         <v>15</v>
       </c>
@@ -6581,7 +6599,7 @@
       <c r="V31" s="21"/>
       <c r="W31" s="10"/>
     </row>
-    <row r="32" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:23" ht="15.75" customHeight="1">
       <c r="A32" s="26" t="s">
         <v>15</v>
       </c>
@@ -6638,7 +6656,7 @@
       <c r="V32" s="21"/>
       <c r="W32" s="10"/>
     </row>
-    <row r="33" spans="1:23" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:23" s="38" customFormat="1" ht="15.75" customHeight="1">
       <c r="A33" s="26" t="s">
         <v>15</v>
       </c>
@@ -6694,7 +6712,7 @@
       <c r="U33" s="21"/>
       <c r="V33" s="21"/>
     </row>
-    <row r="34" spans="1:23" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:23" s="38" customFormat="1" ht="15.75" customHeight="1">
       <c r="A34" s="26" t="s">
         <v>15</v>
       </c>
@@ -6750,7 +6768,7 @@
       <c r="U34" s="21"/>
       <c r="V34" s="21"/>
     </row>
-    <row r="35" spans="1:23" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:23" s="38" customFormat="1" ht="15.75" customHeight="1">
       <c r="A35" s="26" t="s">
         <v>15</v>
       </c>
@@ -6806,7 +6824,7 @@
       <c r="U35" s="21"/>
       <c r="V35" s="21"/>
     </row>
-    <row r="36" spans="1:23" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:23" s="13" customFormat="1" ht="15.75" customHeight="1">
       <c r="A36" s="26" t="s">
         <v>15</v>
       </c>
@@ -6873,7 +6891,7 @@
       </c>
       <c r="W36" s="12"/>
     </row>
-    <row r="37" spans="1:23" s="31" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:23" s="31" customFormat="1" ht="15.75" customHeight="1">
       <c r="A37" s="26" t="s">
         <v>43</v>
       </c>
@@ -6920,7 +6938,7 @@
       <c r="V37" s="21"/>
       <c r="W37" s="30"/>
     </row>
-    <row r="38" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:23" ht="15.75" customHeight="1">
       <c r="A38" s="26" t="s">
         <v>43</v>
       </c>
@@ -6969,7 +6987,7 @@
       <c r="V38" s="21"/>
       <c r="W38" s="10"/>
     </row>
-    <row r="39" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:23" ht="15.75" customHeight="1">
       <c r="A39" s="26" t="s">
         <v>43</v>
       </c>
@@ -7034,7 +7052,7 @@
       </c>
       <c r="W39" s="10"/>
     </row>
-    <row r="40" spans="1:23" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:23" s="37" customFormat="1" ht="15.75" customHeight="1">
       <c r="A40" s="26" t="s">
         <v>43</v>
       </c>
@@ -7101,7 +7119,7 @@
       </c>
       <c r="W40" s="36"/>
     </row>
-    <row r="41" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:23" ht="15.75" customHeight="1">
       <c r="A41" s="26" t="s">
         <v>43</v>
       </c>
@@ -7166,7 +7184,7 @@
       </c>
       <c r="W41" s="10"/>
     </row>
-    <row r="42" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:23" ht="15.75" customHeight="1">
       <c r="A42" s="26" t="s">
         <v>43</v>
       </c>
@@ -7231,7 +7249,7 @@
       </c>
       <c r="W42" s="10"/>
     </row>
-    <row r="43" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:23" ht="15.75" customHeight="1">
       <c r="A43" s="26" t="s">
         <v>43</v>
       </c>
@@ -7296,7 +7314,7 @@
       </c>
       <c r="W43" s="10"/>
     </row>
-    <row r="44" spans="1:23" s="40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:23" s="40" customFormat="1" ht="15.75" customHeight="1">
       <c r="A44" s="26" t="s">
         <v>43</v>
       </c>
@@ -7361,7 +7379,7 @@
       </c>
       <c r="W44" s="39"/>
     </row>
-    <row r="45" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:23" ht="15.75" customHeight="1">
       <c r="A45" s="26" t="s">
         <v>43</v>
       </c>
@@ -7426,7 +7444,7 @@
       </c>
       <c r="W45" s="10"/>
     </row>
-    <row r="46" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:23" ht="15.75" customHeight="1">
       <c r="A46" s="26" t="s">
         <v>43</v>
       </c>
@@ -7489,7 +7507,7 @@
       </c>
       <c r="W46" s="10"/>
     </row>
-    <row r="47" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:23" ht="15.75" customHeight="1">
       <c r="A47" s="26" t="s">
         <v>43</v>
       </c>
@@ -7554,7 +7572,7 @@
       </c>
       <c r="W47" s="10"/>
     </row>
-    <row r="48" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:23" ht="15.75" customHeight="1">
       <c r="A48" s="26" t="s">
         <v>43</v>
       </c>
@@ -7611,7 +7629,7 @@
       </c>
       <c r="W48" s="10"/>
     </row>
-    <row r="49" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:23" ht="15.75" customHeight="1">
       <c r="A49" s="26" t="s">
         <v>43</v>
       </c>
@@ -7662,7 +7680,7 @@
       <c r="V49" s="21"/>
       <c r="W49" s="10"/>
     </row>
-    <row r="50" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:23" ht="15.75" customHeight="1">
       <c r="A50" s="26" t="s">
         <v>43</v>
       </c>
@@ -7709,7 +7727,7 @@
       <c r="V50" s="21"/>
       <c r="W50" s="10"/>
     </row>
-    <row r="51" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:23" ht="15.75" customHeight="1">
       <c r="A51" s="26" t="s">
         <v>43</v>
       </c>
@@ -7756,7 +7774,7 @@
       <c r="V51" s="21"/>
       <c r="W51" s="10"/>
     </row>
-    <row r="52" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:23" ht="15.75" customHeight="1">
       <c r="A52" s="26" t="s">
         <v>43</v>
       </c>
@@ -7803,7 +7821,7 @@
       <c r="V52" s="21"/>
       <c r="W52" s="10"/>
     </row>
-    <row r="53" spans="1:23" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:23" s="28" customFormat="1" ht="15.75" customHeight="1">
       <c r="A53" s="26" t="s">
         <v>43</v>
       </c>
@@ -7866,7 +7884,7 @@
       </c>
       <c r="W53" s="27"/>
     </row>
-    <row r="54" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:23" ht="15.75" customHeight="1">
       <c r="A54" s="26" t="s">
         <v>43</v>
       </c>
@@ -7931,7 +7949,7 @@
       </c>
       <c r="W54" s="10"/>
     </row>
-    <row r="55" spans="1:23" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:23" s="37" customFormat="1" ht="15.75" customHeight="1">
       <c r="A55" s="26" t="s">
         <v>43</v>
       </c>
@@ -7994,7 +8012,7 @@
       <c r="V55" s="21"/>
       <c r="W55" s="36"/>
     </row>
-    <row r="56" spans="1:23" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:23" s="37" customFormat="1" ht="15.75" customHeight="1">
       <c r="A56" s="26" t="s">
         <v>43</v>
       </c>
@@ -8057,7 +8075,7 @@
       <c r="V56" s="21"/>
       <c r="W56" s="36"/>
     </row>
-    <row r="57" spans="1:23" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:23" s="37" customFormat="1" ht="15.75" customHeight="1">
       <c r="A57" s="26" t="s">
         <v>43</v>
       </c>
@@ -8120,7 +8138,7 @@
       <c r="V57" s="21"/>
       <c r="W57" s="36"/>
     </row>
-    <row r="58" spans="1:23" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:23" s="37" customFormat="1" ht="15.75" customHeight="1">
       <c r="A58" s="26" t="s">
         <v>43</v>
       </c>
@@ -8183,7 +8201,7 @@
       <c r="V58" s="21"/>
       <c r="W58" s="36"/>
     </row>
-    <row r="59" spans="1:23" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:23" s="37" customFormat="1" ht="15.75" customHeight="1">
       <c r="A59" s="26" t="s">
         <v>43</v>
       </c>
@@ -8246,7 +8264,7 @@
       <c r="V59" s="21"/>
       <c r="W59" s="36"/>
     </row>
-    <row r="60" spans="1:23" s="34" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:23" s="34" customFormat="1" ht="15.75" customHeight="1">
       <c r="A60" s="26" t="s">
         <v>43</v>
       </c>
@@ -8291,7 +8309,7 @@
       <c r="V60" s="21"/>
       <c r="W60" s="33"/>
     </row>
-    <row r="61" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:23" ht="15.75" customHeight="1">
       <c r="A61" s="26" t="s">
         <v>58</v>
       </c>
@@ -8360,7 +8378,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:23" ht="15.75" customHeight="1">
       <c r="A62" s="26" t="s">
         <v>58</v>
       </c>
@@ -8427,7 +8445,7 @@
       </c>
       <c r="W62" s="42"/>
     </row>
-    <row r="63" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:23" ht="15.75" customHeight="1">
       <c r="A63" s="26" t="s">
         <v>62</v>
       </c>
@@ -8490,11 +8508,11 @@
         <v>113</v>
       </c>
       <c r="V63" s="21" t="s">
-        <v>17</v>
+        <v>113</v>
       </c>
       <c r="W63" s="10"/>
     </row>
-    <row r="64" spans="1:23" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:23" s="15" customFormat="1" ht="15.75" customHeight="1">
       <c r="A64" s="18" t="s">
         <v>63</v>
       </c>
@@ -8527,7 +8545,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="65" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:22" ht="15.75" customHeight="1">
       <c r="A65" s="16" t="s">
         <v>63</v>
       </c>
@@ -8569,7 +8587,7 @@
       <c r="U65" s="17"/>
       <c r="V65" s="17"/>
     </row>
-    <row r="66" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:22" ht="15.75" customHeight="1">
       <c r="A66" s="16" t="s">
         <v>63</v>
       </c>
@@ -8599,7 +8617,7 @@
       <c r="U66" s="17"/>
       <c r="V66" s="17"/>
     </row>
-    <row r="67" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:22" ht="15.75" customHeight="1">
       <c r="A67" s="16" t="s">
         <v>63</v>
       </c>
@@ -8629,7 +8647,7 @@
       <c r="U67" s="17"/>
       <c r="V67" s="17"/>
     </row>
-    <row r="68" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:22" ht="15.75" customHeight="1">
       <c r="A68" s="16" t="s">
         <v>63</v>
       </c>
@@ -8659,7 +8677,7 @@
       <c r="U68" s="17"/>
       <c r="V68" s="17"/>
     </row>
-    <row r="69" spans="1:22" s="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:22" s="35" customFormat="1" ht="15.75" customHeight="1">
       <c r="A69" s="16" t="s">
         <v>63</v>
       </c>
@@ -8689,7 +8707,7 @@
       <c r="U69" s="17"/>
       <c r="V69" s="17"/>
     </row>
-    <row r="70" spans="1:22" s="32" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:22" s="32" customFormat="1" ht="15.75" customHeight="1">
       <c r="A70" s="16" t="s">
         <v>63</v>
       </c>
@@ -8719,7 +8737,7 @@
       <c r="U70" s="17"/>
       <c r="V70" s="17"/>
     </row>
-    <row r="71" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:22" ht="15.75" customHeight="1">
       <c r="A71" s="16" t="s">
         <v>109</v>
       </c>
@@ -8749,7 +8767,7 @@
       <c r="U71" s="20"/>
       <c r="V71" s="20"/>
     </row>
-    <row r="72" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:22" ht="15.75" customHeight="1">
       <c r="A72" s="16" t="s">
         <v>119</v>
       </c>
@@ -8793,22 +8811,19 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="M10" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="V6" sqref="V6"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
+      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="G49" sqref="G49"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
     <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
       <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
-      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="G49" sqref="G49"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="M10" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="V6" sqref="V6"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>
@@ -8822,6 +8837,11 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -8829,11 +8849,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="29.6640625" customWidth="1"/>
     <col min="2" max="2" width="28.1640625" customWidth="1"/>
@@ -8841,7 +8861,7 @@
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="15">
       <c r="A1" s="22" t="s">
         <v>70</v>
       </c>
@@ -8858,7 +8878,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15">
       <c r="A2" s="23" t="s">
         <v>73</v>
       </c>
@@ -8871,7 +8891,7 @@
       <c r="D2" s="24"/>
       <c r="E2" s="24"/>
     </row>
-    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="15">
       <c r="A3" s="23" t="s">
         <v>75</v>
       </c>
@@ -8884,7 +8904,7 @@
       <c r="D3" s="24"/>
       <c r="E3" s="24"/>
     </row>
-    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="15">
       <c r="A4" s="23" t="s">
         <v>77</v>
       </c>
@@ -8897,7 +8917,7 @@
       <c r="D4" s="24"/>
       <c r="E4" s="24"/>
     </row>
-    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="15">
       <c r="A5" s="23" t="s">
         <v>96</v>
       </c>
@@ -8912,7 +8932,7 @@
       </c>
       <c r="E5" s="24"/>
     </row>
-    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="15">
       <c r="A6" s="23" t="s">
         <v>97</v>
       </c>
@@ -8927,7 +8947,7 @@
       </c>
       <c r="E6" s="24"/>
     </row>
-    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="15">
       <c r="A7" s="23" t="s">
         <v>98</v>
       </c>
@@ -8942,7 +8962,7 @@
       </c>
       <c r="E7" s="24"/>
     </row>
-    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="15">
       <c r="A8" s="23" t="s">
         <v>99</v>
       </c>
@@ -8957,7 +8977,7 @@
       </c>
       <c r="E8" s="24"/>
     </row>
-    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="15">
       <c r="A9" s="23" t="s">
         <v>108</v>
       </c>
@@ -8970,7 +8990,7 @@
       <c r="D9" s="24"/>
       <c r="E9" s="24"/>
     </row>
-    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="15">
       <c r="A10" s="23" t="s">
         <v>107</v>
       </c>
@@ -8983,7 +9003,7 @@
       <c r="D10" s="24"/>
       <c r="E10" s="24"/>
     </row>
-    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="15">
       <c r="A11" s="23" t="s">
         <v>106</v>
       </c>
@@ -8996,7 +9016,7 @@
       <c r="D11" s="24"/>
       <c r="E11" s="24"/>
     </row>
-    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="15">
       <c r="A12" s="23" t="s">
         <v>100</v>
       </c>
@@ -9011,7 +9031,7 @@
       </c>
       <c r="E12" s="24"/>
     </row>
-    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="15">
       <c r="A13" s="23" t="s">
         <v>105</v>
       </c>
@@ -9026,7 +9046,7 @@
       </c>
       <c r="E13" s="24"/>
     </row>
-    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="15">
       <c r="A14" s="23" t="s">
         <v>101</v>
       </c>
@@ -9041,7 +9061,7 @@
       </c>
       <c r="E14" s="24"/>
     </row>
-    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="15">
       <c r="A15" s="23" t="s">
         <v>102</v>
       </c>
@@ -9056,7 +9076,7 @@
       </c>
       <c r="E15" s="24"/>
     </row>
-    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="15">
       <c r="A16" s="23" t="s">
         <v>103</v>
       </c>
@@ -9071,7 +9091,7 @@
       </c>
       <c r="E16" s="24"/>
     </row>
-    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="15">
       <c r="A17" s="23" t="s">
         <v>122</v>
       </c>
@@ -9086,7 +9106,7 @@
       </c>
       <c r="E17" s="24"/>
     </row>
-    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="15">
       <c r="A18" s="23" t="s">
         <v>12</v>
       </c>
@@ -9101,7 +9121,7 @@
       </c>
       <c r="E18" s="24"/>
     </row>
-    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="15">
       <c r="A19" s="23" t="s">
         <v>13</v>
       </c>
@@ -9116,7 +9136,7 @@
       </c>
       <c r="E19" s="24"/>
     </row>
-    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="15">
       <c r="A20" s="23" t="s">
         <v>104</v>
       </c>
@@ -9133,23 +9153,25 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}">
-      <selection activeCell="B19" sqref="B19"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
+      <selection activeCell="C7" sqref="C7"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
     <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
       <selection activeCell="C7" sqref="C7"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
-      <selection activeCell="C7" sqref="C7"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}">
+      <selection activeCell="B19" sqref="B19"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Lisää ELY käyttäjälle maksueriin lukuoikeus
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="0" windowWidth="50440" windowHeight="23560" tabRatio="500"/>
+    <workbookView xWindow="760" yWindow="0" windowWidth="49640" windowHeight="24840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -12,9 +12,9 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="2180" windowHeight="916" tabRatio="500" activeSheetId="2"/>
+    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="2379" windowHeight="1295" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
-    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="2180" windowHeight="916" tabRatio="500" activeSheetId="2"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -27,8 +27,41 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Tatu Tarvainen</author>
+  </authors>
+  <commentList>
+    <comment ref="M27" authorId="0" guid="{DB5603A0-3291-7849-94B2-B86D15FBE193}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Tatu Tarvainen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+29.11.2016 Lisätty ELY käyttäjälle maksueriin oikeus
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1101" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1102" uniqueCount="159">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -511,7 +544,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -556,6 +589,17 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -1013,7 +1057,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{C0B302B3-5097-3546-81CC-979DBA1FB813}" diskRevisions="1" revisionId="166" version="24">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{B839B1D8-5356-624C-BB5E-17AF711C2B4C}" diskRevisions="1" revisionId="167" version="26">
   <header guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" dateTime="2016-09-06T09:14:56" maxSheetId="3" userName="Tatu Tarvainen" r:id="rId2" minRId="1" maxRId="3">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1152,6 +1196,18 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{C41E3471-0097-0441-97BD-2D3A7ED3036F}" dateTime="2016-11-29T16:12:11" maxSheetId="3" userName="Tatu Tarvainen" r:id="rId25" minRId="167">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{B839B1D8-5356-624C-BB5E-17AF711C2B4C}" dateTime="2016-11-29T16:12:48" maxSheetId="3" userName="Tatu Tarvainen" r:id="rId26">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -3947,6 +4003,24 @@
       </is>
     </nc>
   </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog24.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="167" sId="1">
+    <nc r="M27" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog25.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcmt sheetId="1" cell="M27" guid="{DB5603A0-3291-7849-94B2-B86D15FBE193}" author="Tatu Tarvainen" newLength="69"/>
 </revisions>
 </file>
 
@@ -4995,14 +5069,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="M51" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="V64" sqref="V64"/>
+      <selection pane="bottomRight" activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -6349,7 +6423,9 @@
         <v>130</v>
       </c>
       <c r="L27" s="21"/>
-      <c r="M27" s="21"/>
+      <c r="M27" s="21" t="s">
+        <v>127</v>
+      </c>
       <c r="N27" s="21"/>
       <c r="O27" s="21"/>
       <c r="P27" s="21"/>
@@ -8811,9 +8887,9 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
-      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="G49" sqref="G49"/>
+    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="M10" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="V6" sqref="V6"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
     <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
@@ -8821,9 +8897,9 @@
       <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="M10" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="V6" sqref="V6"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
+      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="G49" sqref="G49"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>
@@ -8835,8 +8911,9 @@
     <mergeCell ref="C1:N1"/>
     <mergeCell ref="C2:N2"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -9153,20 +9230,20 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
-      <selection activeCell="C7" sqref="C7"/>
+    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}">
+      <selection activeCell="B19" sqref="B19"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
     <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
       <selection activeCell="C7" sqref="C7"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}">
-      <selection activeCell="B19" sqref="B19"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
+      <selection activeCell="C7" sqref="C7"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Salli urakoitsijalle LS-työkalun käyttö
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="0" windowWidth="47580" windowHeight="26980" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-60" yWindow="0" windowWidth="47580" windowHeight="26980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -12,9 +12,9 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" xWindow="-3" yWindow="54" windowWidth="2379" windowHeight="1295" tabRatio="500" activeSheetId="2" showStatusbar="0"/>
+    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="2180" windowHeight="916" tabRatio="500" activeSheetId="2"/>
-    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" xWindow="-3" yWindow="54" windowWidth="2379" windowHeight="1295" tabRatio="500" activeSheetId="2" showStatusbar="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1228" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1230" uniqueCount="167">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -559,6 +559,9 @@
   </si>
   <si>
     <t>ELY rakennuttajakonsultti</t>
+  </si>
+  <si>
+    <t>W+</t>
   </si>
 </sst>
 </file>
@@ -691,7 +694,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="159">
+  <cellStyleXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -851,8 +854,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -942,8 +947,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="159">
+  <cellStyles count="161">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1023,6 +1031,7 @@
     <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1102,6 +1111,7 @@
     <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1115,7 +1125,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{181E8EC1-A181-2D44-895D-D640E4B6F248}" diskRevisions="1" revisionId="304" version="35">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{C8E2FDB6-435E-C040-B9F0-46C376A5EFB8}" diskRevisions="1" revisionId="306" version="36">
   <header guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" dateTime="2016-09-06T09:14:56" maxSheetId="3" userName="Tatu Tarvainen" r:id="rId2" minRId="1" maxRId="3">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1320,6 +1330,12 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{C8E2FDB6-435E-C040-B9F0-46C376A5EFB8}" dateTime="2017-02-01T12:42:09" maxSheetId="3" userName="Jarno Väyrynen" r:id="rId36" minRId="305" maxRId="306">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -7165,6 +7181,59 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog35.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="305" sId="1" odxf="1" dxf="1">
+    <nc r="S72" t="inlineStr">
+      <is>
+        <t>W</t>
+      </is>
+    </nc>
+    <odxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </odxf>
+    <ndxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </ndxf>
+  </rcc>
+  <rfmt sheetId="1" sqref="R72" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="306" sId="1" odxf="1" dxf="1">
+    <nc r="R72" t="inlineStr">
+      <is>
+        <t>W+</t>
+      </is>
+    </nc>
+    <ndxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </ndxf>
+  </rcc>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="5" sId="1" odxf="1" dxf="1">
@@ -7861,13 +7930,14 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="5">
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="6">
   <userInfo guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" name="Tatu Tarvainen" id="-130145201" dateTime="2016-09-06T09:10:23"/>
   <userInfo guid="{E0850D7E-A93F-EF44-B46A-3BEA4D7DBEDB}" name="Jarno Väyrynen" id="-589116405" dateTime="2016-09-06T12:54:09"/>
   <userInfo guid="{0407E191-78DA-F349-B5E5-8AE1BC03A29E}" name="Jarno Väyrynen" id="-589108428" dateTime="2016-09-08T15:33:24"/>
   <userInfo guid="{F8907045-3B30-0A43-A905-F167D27F9989}" name="Jarno Väyrynen" id="-589157736" dateTime="2016-09-27T15:27:41"/>
   <userInfo guid="{C606B059-99AC-3B47-8437-66D15B4E3D4B}" name="Jarno Väyrynen" id="-589137240" dateTime="2016-10-27T09:33:01"/>
+  <userInfo guid="{C8E2FDB6-435E-C040-B9F0-46C376A5EFB8}" name="Jarno Väyrynen" id="-589139215" dateTime="2017-02-01T12:41:16"/>
 </users>
 </file>
 
@@ -8195,11 +8265,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y72"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
       <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="Q7" sqref="Q7"/>
+      <selection pane="bottomRight" activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -12374,8 +12444,12 @@
       <c r="Q72" s="44" t="s">
         <v>161</v>
       </c>
-      <c r="R72" s="29"/>
-      <c r="S72" s="29"/>
+      <c r="R72" s="51" t="s">
+        <v>166</v>
+      </c>
+      <c r="S72" s="44" t="s">
+        <v>161</v>
+      </c>
       <c r="T72" s="29"/>
       <c r="U72" s="29"/>
       <c r="V72" s="29"/>
@@ -12384,9 +12458,9 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="M10" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="V6" sqref="V6"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
+      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="Q7" sqref="Q7"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
     <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
@@ -12394,9 +12468,9 @@
       <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
-      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="Q7" sqref="Q7"/>
+    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="M10" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="V6" sqref="V6"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>
@@ -12423,7 +12497,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -12757,16 +12831,16 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}">
-      <selection activeCell="B19" sqref="B19"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
+      <selection activeCell="B17" sqref="B17"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
     <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
       <selection activeCell="C7" sqref="C7"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
-      <selection activeCell="B17" sqref="B17"/>
+    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}">
+      <selection activeCell="B19" sqref="B19"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
Salli urak. laadunvalvojan käyttää LS työkalua
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1230" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1231" uniqueCount="167">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -1125,7 +1125,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{C8E2FDB6-435E-C040-B9F0-46C376A5EFB8}" diskRevisions="1" revisionId="306" version="36">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{73C5A3F1-D661-114E-91EF-0474461FB0FF}" diskRevisions="1" revisionId="307" version="37">
   <header guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" dateTime="2016-09-06T09:14:56" maxSheetId="3" userName="Tatu Tarvainen" r:id="rId2" minRId="1" maxRId="3">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1336,6 +1336,12 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{73C5A3F1-D661-114E-91EF-0474461FB0FF}" dateTime="2017-02-01T13:03:29" maxSheetId="3" userName="Jarno Väyrynen" r:id="rId37" minRId="307">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -7234,6 +7240,18 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog36.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="307" sId="1">
+    <nc r="U72" t="inlineStr">
+      <is>
+        <t>W</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="5" sId="1" odxf="1" dxf="1">
@@ -7930,14 +7948,14 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="6">
   <userInfo guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" name="Tatu Tarvainen" id="-130145201" dateTime="2016-09-06T09:10:23"/>
   <userInfo guid="{E0850D7E-A93F-EF44-B46A-3BEA4D7DBEDB}" name="Jarno Väyrynen" id="-589116405" dateTime="2016-09-06T12:54:09"/>
   <userInfo guid="{0407E191-78DA-F349-B5E5-8AE1BC03A29E}" name="Jarno Väyrynen" id="-589108428" dateTime="2016-09-08T15:33:24"/>
   <userInfo guid="{F8907045-3B30-0A43-A905-F167D27F9989}" name="Jarno Väyrynen" id="-589157736" dateTime="2016-09-27T15:27:41"/>
   <userInfo guid="{C606B059-99AC-3B47-8437-66D15B4E3D4B}" name="Jarno Väyrynen" id="-589137240" dateTime="2016-10-27T09:33:01"/>
-  <userInfo guid="{C8E2FDB6-435E-C040-B9F0-46C376A5EFB8}" name="Jarno Väyrynen" id="-589139215" dateTime="2017-02-01T12:41:16"/>
+  <userInfo guid="{73C5A3F1-D661-114E-91EF-0474461FB0FF}" name="Jarno Väyrynen" id="-589139215" dateTime="2017-02-01T12:41:16"/>
 </users>
 </file>
 
@@ -8266,10 +8284,10 @@
   <dimension ref="A1:Y72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C19" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A20" sqref="A20:XFD20"/>
+      <selection pane="bottomRight" activeCell="U72" sqref="U72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -12451,7 +12469,9 @@
         <v>161</v>
       </c>
       <c r="T72" s="29"/>
-      <c r="U72" s="29"/>
+      <c r="U72" s="29" t="s">
+        <v>161</v>
+      </c>
       <c r="V72" s="29"/>
       <c r="W72" s="29"/>
       <c r="X72" s="29"/>

</xml_diff>

<commit_message>
Päivitä Roolit.xlsx, lisää JVH:lle oikeudet Hallinta/Yhteydenpito-välilehdelle
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarihan/Jari/Projektit/Harja/harja/resources/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="0" windowWidth="47580" windowHeight="26980" tabRatio="500"/>
+    <workbookView xWindow="3420" yWindow="1940" windowWidth="43600" windowHeight="19860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -12,16 +17,16 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="2180" windowHeight="891" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" xWindow="-3" yWindow="54" windowWidth="2379" windowHeight="1295" tabRatio="500" activeSheetId="2" showStatusbar="0"/>
-    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="2180" windowHeight="916" tabRatio="500" activeSheetId="2"/>
   </customWorkbookViews>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
@@ -61,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1231" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1234" uniqueCount="168">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -562,6 +567,9 @@
   </si>
   <si>
     <t>W+</t>
+  </si>
+  <si>
+    <t>Yhteydenpito</t>
   </si>
 </sst>
 </file>
@@ -857,7 +865,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -935,6 +943,10 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -947,9 +959,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="161">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1125,7 +1134,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{73C5A3F1-D661-114E-91EF-0474461FB0FF}" diskRevisions="1" revisionId="307" version="37">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{C07F9140-3295-A14D-AED0-C4CE9E873F08}" diskRevisions="1" revisionId="311" version="38">
   <header guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" dateTime="2016-09-06T09:14:56" maxSheetId="3" userName="Tatu Tarvainen" r:id="rId2" minRId="1" maxRId="3">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1342,6 +1351,12 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{C07F9140-3295-A14D-AED0-C4CE9E873F08}" dateTime="2017-02-16T15:22:24" maxSheetId="3" userName="Microsoft Office User" r:id="rId38" minRId="308" maxRId="311">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -7252,6 +7267,35 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog37.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="308" sId="1" ref="A69:XFD69" action="insertRow"/>
+  <rcc rId="309" sId="1">
+    <nc r="A69" t="inlineStr">
+      <is>
+        <t>Hallinta</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="310" sId="1">
+    <nc r="B69" t="inlineStr">
+      <is>
+        <t>Yhteydenpito</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="311" sId="1">
+    <nc r="D69" t="inlineStr">
+      <is>
+        <t>R*,W*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="delete"/>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="5" sId="1" odxf="1" dxf="1">
@@ -7948,7 +7992,7 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="6">
   <userInfo guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" name="Tatu Tarvainen" id="-130145201" dateTime="2016-09-06T09:10:23"/>
   <userInfo guid="{E0850D7E-A93F-EF44-B46A-3BEA4D7DBEDB}" name="Jarno Väyrynen" id="-589116405" dateTime="2016-09-06T12:54:09"/>
@@ -8281,16 +8325,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y72"/>
+  <dimension ref="A1:Y73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C19" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
+      <pane xSplit="2" ySplit="6" topLeftCell="C50" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="U72" sqref="U72"/>
+      <selection pane="bottomRight" activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.5" bestFit="1" customWidth="1"/>
@@ -8318,47 +8362,47 @@
     <col min="25" max="25" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="24" customHeight="1">
+    <row r="1" spans="1:25" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="50" t="s">
         <v>151</v>
       </c>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
     </row>
-    <row r="2" spans="1:25" ht="15.75" customHeight="1">
+    <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="50" t="s">
+      <c r="C2" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
     </row>
-    <row r="3" spans="1:25" ht="15.75" customHeight="1">
+    <row r="3" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -8373,39 +8417,39 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="15.75" customHeight="1">
+    <row r="4" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:25" ht="15.75" customHeight="1">
-      <c r="C5" s="47" t="s">
+    <row r="5" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C5" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="K5" s="47" t="s">
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="K5" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="L5" s="46"/>
-      <c r="M5" s="46"/>
-      <c r="N5" s="46"/>
-      <c r="O5" s="46"/>
-      <c r="R5" s="47" t="s">
+      <c r="L5" s="48"/>
+      <c r="M5" s="48"/>
+      <c r="N5" s="48"/>
+      <c r="O5" s="48"/>
+      <c r="R5" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="S5" s="46"/>
-      <c r="T5" s="46"/>
-      <c r="U5" s="46"/>
-      <c r="V5" s="46"/>
-      <c r="W5" s="46"/>
-      <c r="X5" s="46"/>
+      <c r="S5" s="48"/>
+      <c r="T5" s="48"/>
+      <c r="U5" s="48"/>
+      <c r="V5" s="48"/>
+      <c r="W5" s="48"/>
+      <c r="X5" s="48"/>
       <c r="Y5" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="15.75" customHeight="1">
+    <row r="6" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
@@ -8477,7 +8521,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="15.75" customHeight="1">
+    <row r="7" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="16" t="s">
         <v>15</v>
       </c>
@@ -8550,7 +8594,7 @@
       </c>
       <c r="Y7" s="10"/>
     </row>
-    <row r="8" spans="1:25" ht="15.75" customHeight="1">
+    <row r="8" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="16" t="s">
         <v>15</v>
       </c>
@@ -8609,7 +8653,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="15.75" customHeight="1">
+    <row r="9" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="16" t="s">
         <v>15</v>
       </c>
@@ -8662,7 +8706,7 @@
       <c r="X9" s="17"/>
       <c r="Y9" s="10"/>
     </row>
-    <row r="10" spans="1:25" ht="15.75" customHeight="1">
+    <row r="10" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="16" t="s">
         <v>15</v>
       </c>
@@ -8715,7 +8759,7 @@
       <c r="X10" s="17"/>
       <c r="Y10" s="10"/>
     </row>
-    <row r="11" spans="1:25" ht="15.75" customHeight="1">
+    <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="16" t="s">
         <v>15</v>
       </c>
@@ -8782,7 +8826,7 @@
       <c r="X11" s="17"/>
       <c r="Y11" s="10"/>
     </row>
-    <row r="12" spans="1:25" ht="15.75" customHeight="1">
+    <row r="12" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="16" t="s">
         <v>15</v>
       </c>
@@ -8849,7 +8893,7 @@
       <c r="X12" s="17"/>
       <c r="Y12" s="10"/>
     </row>
-    <row r="13" spans="1:25" ht="15.75" customHeight="1">
+    <row r="13" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="16" t="s">
         <v>15</v>
       </c>
@@ -8904,7 +8948,7 @@
       <c r="X13" s="17"/>
       <c r="Y13" s="10"/>
     </row>
-    <row r="14" spans="1:25" ht="15.75" customHeight="1">
+    <row r="14" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="16" t="s">
         <v>15</v>
       </c>
@@ -8959,7 +9003,7 @@
       <c r="X14" s="17"/>
       <c r="Y14" s="10"/>
     </row>
-    <row r="15" spans="1:25" ht="15.75" customHeight="1">
+    <row r="15" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="16" t="s">
         <v>15</v>
       </c>
@@ -9014,7 +9058,7 @@
       <c r="X15" s="17"/>
       <c r="Y15" s="10"/>
     </row>
-    <row r="16" spans="1:25" ht="15.75" customHeight="1">
+    <row r="16" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="16" t="s">
         <v>15</v>
       </c>
@@ -9081,7 +9125,7 @@
       <c r="X16" s="17"/>
       <c r="Y16" s="10"/>
     </row>
-    <row r="17" spans="1:25" ht="15.75" customHeight="1">
+    <row r="17" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="16" t="s">
         <v>15</v>
       </c>
@@ -9148,7 +9192,7 @@
       <c r="X17" s="17"/>
       <c r="Y17" s="10"/>
     </row>
-    <row r="18" spans="1:25" ht="15.75" customHeight="1">
+    <row r="18" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="16" t="s">
         <v>15</v>
       </c>
@@ -9203,7 +9247,7 @@
       <c r="X18" s="17"/>
       <c r="Y18" s="10"/>
     </row>
-    <row r="19" spans="1:25" ht="15.75" customHeight="1">
+    <row r="19" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="16" t="s">
         <v>15</v>
       </c>
@@ -9270,7 +9314,7 @@
       <c r="X19" s="17"/>
       <c r="Y19" s="10"/>
     </row>
-    <row r="20" spans="1:25" ht="15.75" customHeight="1">
+    <row r="20" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="16" t="s">
         <v>15</v>
       </c>
@@ -9343,7 +9387,7 @@
       </c>
       <c r="Y20" s="10"/>
     </row>
-    <row r="21" spans="1:25" ht="15.75" customHeight="1">
+    <row r="21" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="26" t="s">
         <v>15</v>
       </c>
@@ -9416,7 +9460,7 @@
       </c>
       <c r="Y21" s="10"/>
     </row>
-    <row r="22" spans="1:25" ht="15.75" customHeight="1">
+    <row r="22" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="26" t="s">
         <v>15</v>
       </c>
@@ -9487,7 +9531,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="15.75" customHeight="1">
+    <row r="23" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="26" t="s">
         <v>15</v>
       </c>
@@ -9556,7 +9600,7 @@
       <c r="X23" s="21"/>
       <c r="Y23" s="10"/>
     </row>
-    <row r="24" spans="1:25" ht="15.75" customHeight="1">
+    <row r="24" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="26" t="s">
         <v>15</v>
       </c>
@@ -9625,7 +9669,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="15.75" customHeight="1">
+    <row r="25" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="26" t="s">
         <v>15</v>
       </c>
@@ -9686,7 +9730,7 @@
       <c r="X25" s="21"/>
       <c r="Y25" s="10"/>
     </row>
-    <row r="26" spans="1:25" ht="15.75" customHeight="1">
+    <row r="26" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="26" t="s">
         <v>15</v>
       </c>
@@ -9739,7 +9783,7 @@
       <c r="X26" s="21"/>
       <c r="Y26" s="10"/>
     </row>
-    <row r="27" spans="1:25" ht="15.75" customHeight="1">
+    <row r="27" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="26" t="s">
         <v>15</v>
       </c>
@@ -9786,7 +9830,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:25" ht="15.75" customHeight="1">
+    <row r="28" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="26" t="s">
         <v>15</v>
       </c>
@@ -9855,7 +9899,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="29" spans="1:25" ht="15.75" customHeight="1">
+    <row r="29" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="26" t="s">
         <v>15</v>
       </c>
@@ -9918,7 +9962,7 @@
       <c r="X29" s="21"/>
       <c r="Y29" s="10"/>
     </row>
-    <row r="30" spans="1:25" ht="15.75" customHeight="1">
+    <row r="30" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="26" t="s">
         <v>15</v>
       </c>
@@ -9983,7 +10027,7 @@
       <c r="X30" s="21"/>
       <c r="Y30" s="10"/>
     </row>
-    <row r="31" spans="1:25" ht="15.75" customHeight="1">
+    <row r="31" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="26" t="s">
         <v>15</v>
       </c>
@@ -10046,7 +10090,7 @@
       <c r="X31" s="21"/>
       <c r="Y31" s="10"/>
     </row>
-    <row r="32" spans="1:25" ht="15.75" customHeight="1">
+    <row r="32" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="26" t="s">
         <v>15</v>
       </c>
@@ -10109,7 +10153,7 @@
       <c r="X32" s="21"/>
       <c r="Y32" s="10"/>
     </row>
-    <row r="33" spans="1:25" s="38" customFormat="1" ht="15.75" customHeight="1">
+    <row r="33" spans="1:25" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="26" t="s">
         <v>15</v>
       </c>
@@ -10171,7 +10215,7 @@
       <c r="W33" s="21"/>
       <c r="X33" s="21"/>
     </row>
-    <row r="34" spans="1:25" s="38" customFormat="1" ht="15.75" customHeight="1">
+    <row r="34" spans="1:25" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="26" t="s">
         <v>15</v>
       </c>
@@ -10233,7 +10277,7 @@
       <c r="W34" s="21"/>
       <c r="X34" s="21"/>
     </row>
-    <row r="35" spans="1:25" s="38" customFormat="1" ht="15.75" customHeight="1">
+    <row r="35" spans="1:25" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="26" t="s">
         <v>15</v>
       </c>
@@ -10295,7 +10339,7 @@
       <c r="W35" s="21"/>
       <c r="X35" s="21"/>
     </row>
-    <row r="36" spans="1:25" s="13" customFormat="1" ht="15.75" customHeight="1">
+    <row r="36" spans="1:25" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="26" t="s">
         <v>15</v>
       </c>
@@ -10368,7 +10412,7 @@
       </c>
       <c r="Y36" s="12"/>
     </row>
-    <row r="37" spans="1:25" s="31" customFormat="1" ht="15.75" customHeight="1">
+    <row r="37" spans="1:25" s="31" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="26" t="s">
         <v>43</v>
       </c>
@@ -10421,7 +10465,7 @@
       <c r="X37" s="21"/>
       <c r="Y37" s="30"/>
     </row>
-    <row r="38" spans="1:25" ht="15.75" customHeight="1">
+    <row r="38" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="26" t="s">
         <v>43</v>
       </c>
@@ -10476,7 +10520,7 @@
       <c r="X38" s="21"/>
       <c r="Y38" s="10"/>
     </row>
-    <row r="39" spans="1:25" ht="15.75" customHeight="1">
+    <row r="39" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="26" t="s">
         <v>43</v>
       </c>
@@ -10547,7 +10591,7 @@
       </c>
       <c r="Y39" s="10"/>
     </row>
-    <row r="40" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1">
+    <row r="40" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="26" t="s">
         <v>43</v>
       </c>
@@ -10620,7 +10664,7 @@
       </c>
       <c r="Y40" s="36"/>
     </row>
-    <row r="41" spans="1:25" ht="15.75" customHeight="1">
+    <row r="41" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="26" t="s">
         <v>43</v>
       </c>
@@ -10691,7 +10735,7 @@
       </c>
       <c r="Y41" s="10"/>
     </row>
-    <row r="42" spans="1:25" ht="15.75" customHeight="1">
+    <row r="42" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="26" t="s">
         <v>43</v>
       </c>
@@ -10762,7 +10806,7 @@
       </c>
       <c r="Y42" s="10"/>
     </row>
-    <row r="43" spans="1:25" ht="15.75" customHeight="1">
+    <row r="43" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="26" t="s">
         <v>43</v>
       </c>
@@ -10833,7 +10877,7 @@
       </c>
       <c r="Y43" s="10"/>
     </row>
-    <row r="44" spans="1:25" s="40" customFormat="1" ht="15.75" customHeight="1">
+    <row r="44" spans="1:25" s="40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="26" t="s">
         <v>43</v>
       </c>
@@ -10904,7 +10948,7 @@
       </c>
       <c r="Y44" s="39"/>
     </row>
-    <row r="45" spans="1:25" ht="15.75" customHeight="1">
+    <row r="45" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="26" t="s">
         <v>43</v>
       </c>
@@ -10975,7 +11019,7 @@
       </c>
       <c r="Y45" s="10"/>
     </row>
-    <row r="46" spans="1:25" ht="15.75" customHeight="1">
+    <row r="46" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="26" t="s">
         <v>43</v>
       </c>
@@ -11044,7 +11088,7 @@
       </c>
       <c r="Y46" s="10"/>
     </row>
-    <row r="47" spans="1:25" ht="15.75" customHeight="1">
+    <row r="47" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="26" t="s">
         <v>43</v>
       </c>
@@ -11115,7 +11159,7 @@
       </c>
       <c r="Y47" s="10"/>
     </row>
-    <row r="48" spans="1:25" ht="15.75" customHeight="1">
+    <row r="48" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="26" t="s">
         <v>43</v>
       </c>
@@ -11178,7 +11222,7 @@
       </c>
       <c r="Y48" s="10"/>
     </row>
-    <row r="49" spans="1:25" ht="15.75" customHeight="1">
+    <row r="49" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="26" t="s">
         <v>43</v>
       </c>
@@ -11235,7 +11279,7 @@
       <c r="X49" s="21"/>
       <c r="Y49" s="10"/>
     </row>
-    <row r="50" spans="1:25" ht="15.75" customHeight="1">
+    <row r="50" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="26" t="s">
         <v>43</v>
       </c>
@@ -11288,7 +11332,7 @@
       <c r="X50" s="21"/>
       <c r="Y50" s="10"/>
     </row>
-    <row r="51" spans="1:25" ht="15.75" customHeight="1">
+    <row r="51" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="26" t="s">
         <v>43</v>
       </c>
@@ -11341,7 +11385,7 @@
       <c r="X51" s="21"/>
       <c r="Y51" s="10"/>
     </row>
-    <row r="52" spans="1:25" ht="15.75" customHeight="1">
+    <row r="52" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="26" t="s">
         <v>43</v>
       </c>
@@ -11394,7 +11438,7 @@
       <c r="X52" s="21"/>
       <c r="Y52" s="10"/>
     </row>
-    <row r="53" spans="1:25" s="28" customFormat="1" ht="15.75" customHeight="1">
+    <row r="53" spans="1:25" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="26" t="s">
         <v>43</v>
       </c>
@@ -11463,7 +11507,7 @@
       </c>
       <c r="Y53" s="27"/>
     </row>
-    <row r="54" spans="1:25" ht="15.75" customHeight="1">
+    <row r="54" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="26" t="s">
         <v>43</v>
       </c>
@@ -11534,7 +11578,7 @@
       </c>
       <c r="Y54" s="10"/>
     </row>
-    <row r="55" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1">
+    <row r="55" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="26" t="s">
         <v>43</v>
       </c>
@@ -11603,7 +11647,7 @@
       <c r="X55" s="21"/>
       <c r="Y55" s="36"/>
     </row>
-    <row r="56" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1">
+    <row r="56" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="26" t="s">
         <v>43</v>
       </c>
@@ -11672,7 +11716,7 @@
       <c r="X56" s="21"/>
       <c r="Y56" s="36"/>
     </row>
-    <row r="57" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1">
+    <row r="57" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="26" t="s">
         <v>43</v>
       </c>
@@ -11741,7 +11785,7 @@
       <c r="X57" s="21"/>
       <c r="Y57" s="36"/>
     </row>
-    <row r="58" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1">
+    <row r="58" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="26" t="s">
         <v>43</v>
       </c>
@@ -11810,7 +11854,7 @@
       <c r="X58" s="21"/>
       <c r="Y58" s="36"/>
     </row>
-    <row r="59" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1">
+    <row r="59" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="26" t="s">
         <v>43</v>
       </c>
@@ -11879,7 +11923,7 @@
       <c r="X59" s="21"/>
       <c r="Y59" s="36"/>
     </row>
-    <row r="60" spans="1:25" s="34" customFormat="1" ht="15.75" customHeight="1">
+    <row r="60" spans="1:25" s="34" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="26" t="s">
         <v>43</v>
       </c>
@@ -11930,7 +11974,7 @@
       <c r="X60" s="21"/>
       <c r="Y60" s="33"/>
     </row>
-    <row r="61" spans="1:25" ht="15.75" customHeight="1">
+    <row r="61" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="26" t="s">
         <v>58</v>
       </c>
@@ -12001,11 +12045,11 @@
       <c r="X61" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="Y61" s="45" t="s">
+      <c r="Y61" s="47" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:25" ht="15.75" customHeight="1">
+    <row r="62" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="26" t="s">
         <v>58</v>
       </c>
@@ -12076,9 +12120,9 @@
       <c r="X62" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="Y62" s="46"/>
+      <c r="Y62" s="48"/>
     </row>
-    <row r="63" spans="1:25" ht="15.75" customHeight="1">
+    <row r="63" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="26" t="s">
         <v>62</v>
       </c>
@@ -12151,7 +12195,7 @@
       </c>
       <c r="Y63" s="10"/>
     </row>
-    <row r="64" spans="1:25" s="15" customFormat="1" ht="15.75" customHeight="1">
+    <row r="64" spans="1:25" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="18" t="s">
         <v>63</v>
       </c>
@@ -12186,7 +12230,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="65" spans="1:24" ht="15.75" customHeight="1">
+    <row r="65" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="16" t="s">
         <v>63</v>
       </c>
@@ -12230,7 +12274,7 @@
       <c r="W65" s="17"/>
       <c r="X65" s="17"/>
     </row>
-    <row r="66" spans="1:24" ht="15.75" customHeight="1">
+    <row r="66" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="16" t="s">
         <v>63</v>
       </c>
@@ -12262,7 +12306,7 @@
       <c r="W66" s="17"/>
       <c r="X66" s="17"/>
     </row>
-    <row r="67" spans="1:24" ht="15.75" customHeight="1">
+    <row r="67" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="16" t="s">
         <v>63</v>
       </c>
@@ -12294,7 +12338,7 @@
       <c r="W67" s="17"/>
       <c r="X67" s="17"/>
     </row>
-    <row r="68" spans="1:24" ht="15.75" customHeight="1">
+    <row r="68" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="16" t="s">
         <v>63</v>
       </c>
@@ -12326,12 +12370,12 @@
       <c r="W68" s="17"/>
       <c r="X68" s="17"/>
     </row>
-    <row r="69" spans="1:24" s="35" customFormat="1" ht="15.75" customHeight="1">
+    <row r="69" spans="1:24" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="16" t="s">
         <v>63</v>
       </c>
       <c r="B69" s="16" t="s">
-        <v>33</v>
+        <v>167</v>
       </c>
       <c r="C69" s="17"/>
       <c r="D69" s="21" t="s">
@@ -12358,12 +12402,12 @@
       <c r="W69" s="17"/>
       <c r="X69" s="17"/>
     </row>
-    <row r="70" spans="1:24" s="32" customFormat="1" ht="15.75" customHeight="1">
+    <row r="70" spans="1:24" s="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="16" t="s">
         <v>63</v>
       </c>
       <c r="B70" s="16" t="s">
-        <v>124</v>
+        <v>33</v>
       </c>
       <c r="C70" s="17"/>
       <c r="D70" s="21" t="s">
@@ -12390,107 +12434,142 @@
       <c r="W70" s="17"/>
       <c r="X70" s="17"/>
     </row>
-    <row r="71" spans="1:24" ht="15.75" customHeight="1">
+    <row r="71" spans="1:24" s="32" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="16" t="s">
-        <v>109</v>
+        <v>63</v>
       </c>
       <c r="B71" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="C71" s="20"/>
+        <v>124</v>
+      </c>
+      <c r="C71" s="17"/>
       <c r="D71" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="E71" s="20"/>
-      <c r="F71" s="20"/>
-      <c r="G71" s="20"/>
-      <c r="H71" s="20"/>
-      <c r="I71" s="20"/>
-      <c r="J71" s="43"/>
-      <c r="K71" s="20"/>
-      <c r="L71" s="20"/>
-      <c r="M71" s="20"/>
-      <c r="N71" s="20"/>
-      <c r="O71" s="20"/>
-      <c r="P71" s="20"/>
-      <c r="Q71" s="43"/>
-      <c r="R71" s="20"/>
-      <c r="S71" s="20"/>
-      <c r="T71" s="20"/>
-      <c r="U71" s="20"/>
-      <c r="V71" s="20"/>
-      <c r="W71" s="20"/>
-      <c r="X71" s="20"/>
+      <c r="E71" s="17"/>
+      <c r="F71" s="17"/>
+      <c r="G71" s="17"/>
+      <c r="H71" s="17"/>
+      <c r="I71" s="17"/>
+      <c r="J71" s="21"/>
+      <c r="K71" s="17"/>
+      <c r="L71" s="17"/>
+      <c r="M71" s="17"/>
+      <c r="N71" s="17"/>
+      <c r="O71" s="17"/>
+      <c r="P71" s="17"/>
+      <c r="Q71" s="21"/>
+      <c r="R71" s="17"/>
+      <c r="S71" s="17"/>
+      <c r="T71" s="17"/>
+      <c r="U71" s="17"/>
+      <c r="V71" s="17"/>
+      <c r="W71" s="17"/>
+      <c r="X71" s="17"/>
     </row>
-    <row r="72" spans="1:24" ht="15.75" customHeight="1">
+    <row r="72" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="16" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="B72" s="16" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="C72" s="20"/>
       <c r="D72" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="E72" s="20"/>
+      <c r="F72" s="20"/>
+      <c r="G72" s="20"/>
+      <c r="H72" s="20"/>
+      <c r="I72" s="20"/>
+      <c r="J72" s="43"/>
+      <c r="K72" s="20"/>
+      <c r="L72" s="20"/>
+      <c r="M72" s="20"/>
+      <c r="N72" s="20"/>
+      <c r="O72" s="20"/>
+      <c r="P72" s="20"/>
+      <c r="Q72" s="43"/>
+      <c r="R72" s="20"/>
+      <c r="S72" s="20"/>
+      <c r="T72" s="20"/>
+      <c r="U72" s="20"/>
+      <c r="V72" s="20"/>
+      <c r="W72" s="20"/>
+      <c r="X72" s="20"/>
+    </row>
+    <row r="73" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A73" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="B73" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C73" s="20"/>
+      <c r="D73" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="E72" s="29" t="s">
+      <c r="E73" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="F72" s="29"/>
-      <c r="G72" s="29" t="s">
+      <c r="F73" s="29"/>
+      <c r="G73" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="H72" s="29"/>
-      <c r="I72" s="29"/>
-      <c r="J72" s="44" t="s">
+      <c r="H73" s="29"/>
+      <c r="I73" s="29"/>
+      <c r="J73" s="44" t="s">
         <v>161</v>
       </c>
-      <c r="K72" s="29" t="s">
+      <c r="K73" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="L72" s="29" t="s">
+      <c r="L73" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="M72" s="29" t="s">
+      <c r="M73" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="N72" s="29" t="s">
+      <c r="N73" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="O72" s="29"/>
-      <c r="P72" s="29"/>
-      <c r="Q72" s="44" t="s">
+      <c r="O73" s="29"/>
+      <c r="P73" s="29"/>
+      <c r="Q73" s="44" t="s">
         <v>161</v>
       </c>
-      <c r="R72" s="51" t="s">
+      <c r="R73" s="46" t="s">
         <v>166</v>
       </c>
-      <c r="S72" s="44" t="s">
+      <c r="S73" s="44" t="s">
         <v>161</v>
       </c>
-      <c r="T72" s="29"/>
-      <c r="U72" s="29" t="s">
+      <c r="T73" s="29"/>
+      <c r="U73" s="29" t="s">
         <v>161</v>
       </c>
-      <c r="V72" s="29"/>
-      <c r="W72" s="29"/>
-      <c r="X72" s="29"/>
+      <c r="V73" s="29"/>
+      <c r="W73" s="29"/>
+      <c r="X73" s="29"/>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
-      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="Q7" sqref="Q7"/>
+    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="C50" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="D69" sqref="D69"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
     <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
       <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="M10" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="V6" sqref="V6"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
+      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="Q7" sqref="Q7"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>
@@ -12502,14 +12581,9 @@
     <mergeCell ref="C1:O1"/>
     <mergeCell ref="C2:O2"/>
   </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -12518,10 +12592,10 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="29.6640625" customWidth="1"/>
     <col min="2" max="2" width="28.1640625" customWidth="1"/>
@@ -12529,7 +12603,7 @@
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15">
+    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
         <v>70</v>
       </c>
@@ -12546,7 +12620,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15">
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
         <v>73</v>
       </c>
@@ -12559,7 +12633,7 @@
       <c r="D2" s="24"/>
       <c r="E2" s="24"/>
     </row>
-    <row r="3" spans="1:5" ht="15">
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
         <v>75</v>
       </c>
@@ -12572,7 +12646,7 @@
       <c r="D3" s="24"/>
       <c r="E3" s="24"/>
     </row>
-    <row r="4" spans="1:5" ht="15">
+    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
         <v>77</v>
       </c>
@@ -12585,7 +12659,7 @@
       <c r="D4" s="24"/>
       <c r="E4" s="24"/>
     </row>
-    <row r="5" spans="1:5" ht="15">
+    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
         <v>96</v>
       </c>
@@ -12600,7 +12674,7 @@
       </c>
       <c r="E5" s="24"/>
     </row>
-    <row r="6" spans="1:5" ht="15">
+    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
         <v>97</v>
       </c>
@@ -12615,7 +12689,7 @@
       </c>
       <c r="E6" s="24"/>
     </row>
-    <row r="7" spans="1:5" ht="15">
+    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
         <v>98</v>
       </c>
@@ -12630,7 +12704,7 @@
       </c>
       <c r="E7" s="24"/>
     </row>
-    <row r="8" spans="1:5" s="41" customFormat="1" ht="15">
+    <row r="8" spans="1:5" s="41" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
         <v>163</v>
       </c>
@@ -12645,7 +12719,7 @@
       </c>
       <c r="E8" s="24"/>
     </row>
-    <row r="9" spans="1:5" ht="15">
+    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
         <v>99</v>
       </c>
@@ -12660,7 +12734,7 @@
       </c>
       <c r="E9" s="24"/>
     </row>
-    <row r="10" spans="1:5" ht="15">
+    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
         <v>108</v>
       </c>
@@ -12673,7 +12747,7 @@
       <c r="D10" s="24"/>
       <c r="E10" s="24"/>
     </row>
-    <row r="11" spans="1:5" ht="15">
+    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
         <v>107</v>
       </c>
@@ -12686,7 +12760,7 @@
       <c r="D11" s="24"/>
       <c r="E11" s="24"/>
     </row>
-    <row r="12" spans="1:5" ht="15">
+    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
         <v>106</v>
       </c>
@@ -12699,7 +12773,7 @@
       <c r="D12" s="24"/>
       <c r="E12" s="24"/>
     </row>
-    <row r="13" spans="1:5" ht="15">
+    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="23" t="s">
         <v>100</v>
       </c>
@@ -12714,7 +12788,7 @@
       </c>
       <c r="E13" s="24"/>
     </row>
-    <row r="14" spans="1:5" ht="15">
+    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
         <v>105</v>
       </c>
@@ -12729,7 +12803,7 @@
       </c>
       <c r="E14" s="24"/>
     </row>
-    <row r="15" spans="1:5" ht="15">
+    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
         <v>101</v>
       </c>
@@ -12744,7 +12818,7 @@
       </c>
       <c r="E15" s="24"/>
     </row>
-    <row r="16" spans="1:5" s="41" customFormat="1" ht="15">
+    <row r="16" spans="1:5" s="41" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
         <v>162</v>
       </c>
@@ -12759,7 +12833,7 @@
       </c>
       <c r="E16" s="24"/>
     </row>
-    <row r="17" spans="1:5" ht="15">
+    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="23" t="s">
         <v>102</v>
       </c>
@@ -12774,7 +12848,7 @@
       </c>
       <c r="E17" s="24"/>
     </row>
-    <row r="18" spans="1:5" ht="15">
+    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
         <v>103</v>
       </c>
@@ -12789,7 +12863,7 @@
       </c>
       <c r="E18" s="24"/>
     </row>
-    <row r="19" spans="1:5" ht="15">
+    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="23" t="s">
         <v>122</v>
       </c>
@@ -12804,7 +12878,7 @@
       </c>
       <c r="E19" s="24"/>
     </row>
-    <row r="20" spans="1:5" ht="15">
+    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
         <v>12</v>
       </c>
@@ -12819,7 +12893,7 @@
       </c>
       <c r="E20" s="24"/>
     </row>
-    <row r="21" spans="1:5" ht="15">
+    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="23" t="s">
         <v>13</v>
       </c>
@@ -12834,7 +12908,7 @@
       </c>
       <c r="E21" s="24"/>
     </row>
-    <row r="22" spans="1:5" ht="15">
+    <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="23" t="s">
         <v>104</v>
       </c>
@@ -12851,25 +12925,23 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
-      <selection activeCell="B17" sqref="B17"/>
+    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}">
+      <selection activeCell="G36" sqref="G36"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
     <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
       <selection activeCell="C7" sqref="C7"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}">
-      <selection activeCell="B19" sqref="B19"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
+      <selection activeCell="B17" sqref="B17"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Salli urakoitsijan merkitä tiemerkintä valmiiksi
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarihan/Jari/Projektit/Harja/harja/resources/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="1940" windowWidth="43600" windowHeight="19860" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="38400" windowHeight="21600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -17,16 +12,16 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
+    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="2180" windowHeight="891" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" xWindow="-3" yWindow="54" windowWidth="2379" windowHeight="1295" tabRatio="500" activeSheetId="2" showStatusbar="0"/>
   </customWorkbookViews>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -66,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1234" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1234" uniqueCount="170">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -570,6 +565,12 @@
   </si>
   <si>
     <t>Yhteydenpito</t>
+  </si>
+  <si>
+    <t>R,W,TM-valmis</t>
+  </si>
+  <si>
+    <t>R+,W+,TM-valmis</t>
   </si>
 </sst>
 </file>
@@ -1134,7 +1135,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{C07F9140-3295-A14D-AED0-C4CE9E873F08}" diskRevisions="1" revisionId="311" version="38">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{20D72FDE-B37A-954B-96C9-CC76E718E9F1}" diskRevisions="1" revisionId="313" version="39">
   <header guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" dateTime="2016-09-06T09:14:56" maxSheetId="3" userName="Tatu Tarvainen" r:id="rId2" minRId="1" maxRId="3">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1357,6 +1358,12 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{20D72FDE-B37A-954B-96C9-CC76E718E9F1}" dateTime="2017-03-02T10:37:41" maxSheetId="3" userName="Jarno Väyrynen" r:id="rId39" minRId="312" maxRId="313">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -7296,6 +7303,37 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog38.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="312" sId="1">
+    <oc r="S28" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </oc>
+    <nc r="S28" t="inlineStr">
+      <is>
+        <t>R,W,TM-valmis</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="313" sId="1">
+    <oc r="R28" t="inlineStr">
+      <is>
+        <t>R+,W+</t>
+      </is>
+    </oc>
+    <nc r="R28" t="inlineStr">
+      <is>
+        <t>R+,W+,TM-valmis</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" action="delete"/>
+  <rcv guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="5" sId="1" odxf="1" dxf="1">
@@ -7993,13 +8031,14 @@
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="6">
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="7">
   <userInfo guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" name="Tatu Tarvainen" id="-130145201" dateTime="2016-09-06T09:10:23"/>
   <userInfo guid="{E0850D7E-A93F-EF44-B46A-3BEA4D7DBEDB}" name="Jarno Väyrynen" id="-589116405" dateTime="2016-09-06T12:54:09"/>
   <userInfo guid="{0407E191-78DA-F349-B5E5-8AE1BC03A29E}" name="Jarno Väyrynen" id="-589108428" dateTime="2016-09-08T15:33:24"/>
   <userInfo guid="{F8907045-3B30-0A43-A905-F167D27F9989}" name="Jarno Väyrynen" id="-589157736" dateTime="2016-09-27T15:27:41"/>
   <userInfo guid="{C606B059-99AC-3B47-8437-66D15B4E3D4B}" name="Jarno Väyrynen" id="-589137240" dateTime="2016-10-27T09:33:01"/>
   <userInfo guid="{73C5A3F1-D661-114E-91EF-0474461FB0FF}" name="Jarno Väyrynen" id="-589139215" dateTime="2017-02-01T12:41:16"/>
+  <userInfo guid="{20D72FDE-B37A-954B-96C9-CC76E718E9F1}" name="Jarno Väyrynen" id="-589140570" dateTime="2017-03-02T10:49:07"/>
 </users>
 </file>
 
@@ -8327,14 +8366,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C50" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
+      <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D63" sqref="D63"/>
+      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.5" bestFit="1" customWidth="1"/>
@@ -8362,7 +8401,7 @@
     <col min="25" max="25" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="24" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:25" ht="24" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -8383,7 +8422,7 @@
       <c r="N1" s="51"/>
       <c r="O1" s="51"/>
     </row>
-    <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:25" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="52" t="s">
@@ -8402,7 +8441,7 @@
       <c r="N2" s="48"/>
       <c r="O2" s="48"/>
     </row>
-    <row r="3" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:25" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -8417,10 +8456,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:25" ht="15.75" customHeight="1">
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:25" ht="15.75" customHeight="1">
       <c r="C5" s="49" t="s">
         <v>6</v>
       </c>
@@ -8449,7 +8488,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:25" ht="15.75" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
@@ -8521,7 +8560,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:25" ht="15.75" customHeight="1">
       <c r="A7" s="16" t="s">
         <v>15</v>
       </c>
@@ -8594,7 +8633,7 @@
       </c>
       <c r="Y7" s="10"/>
     </row>
-    <row r="8" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:25" ht="15.75" customHeight="1">
       <c r="A8" s="16" t="s">
         <v>15</v>
       </c>
@@ -8653,7 +8692,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:25" ht="15.75" customHeight="1">
       <c r="A9" s="16" t="s">
         <v>15</v>
       </c>
@@ -8706,7 +8745,7 @@
       <c r="X9" s="17"/>
       <c r="Y9" s="10"/>
     </row>
-    <row r="10" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:25" ht="15.75" customHeight="1">
       <c r="A10" s="16" t="s">
         <v>15</v>
       </c>
@@ -8759,7 +8798,7 @@
       <c r="X10" s="17"/>
       <c r="Y10" s="10"/>
     </row>
-    <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:25" ht="15.75" customHeight="1">
       <c r="A11" s="16" t="s">
         <v>15</v>
       </c>
@@ -8826,7 +8865,7 @@
       <c r="X11" s="17"/>
       <c r="Y11" s="10"/>
     </row>
-    <row r="12" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:25" ht="15.75" customHeight="1">
       <c r="A12" s="16" t="s">
         <v>15</v>
       </c>
@@ -8893,7 +8932,7 @@
       <c r="X12" s="17"/>
       <c r="Y12" s="10"/>
     </row>
-    <row r="13" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:25" ht="15.75" customHeight="1">
       <c r="A13" s="16" t="s">
         <v>15</v>
       </c>
@@ -8948,7 +8987,7 @@
       <c r="X13" s="17"/>
       <c r="Y13" s="10"/>
     </row>
-    <row r="14" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:25" ht="15.75" customHeight="1">
       <c r="A14" s="16" t="s">
         <v>15</v>
       </c>
@@ -9003,7 +9042,7 @@
       <c r="X14" s="17"/>
       <c r="Y14" s="10"/>
     </row>
-    <row r="15" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:25" ht="15.75" customHeight="1">
       <c r="A15" s="16" t="s">
         <v>15</v>
       </c>
@@ -9058,7 +9097,7 @@
       <c r="X15" s="17"/>
       <c r="Y15" s="10"/>
     </row>
-    <row r="16" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:25" ht="15.75" customHeight="1">
       <c r="A16" s="16" t="s">
         <v>15</v>
       </c>
@@ -9125,7 +9164,7 @@
       <c r="X16" s="17"/>
       <c r="Y16" s="10"/>
     </row>
-    <row r="17" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:25" ht="15.75" customHeight="1">
       <c r="A17" s="16" t="s">
         <v>15</v>
       </c>
@@ -9192,7 +9231,7 @@
       <c r="X17" s="17"/>
       <c r="Y17" s="10"/>
     </row>
-    <row r="18" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:25" ht="15.75" customHeight="1">
       <c r="A18" s="16" t="s">
         <v>15</v>
       </c>
@@ -9247,7 +9286,7 @@
       <c r="X18" s="17"/>
       <c r="Y18" s="10"/>
     </row>
-    <row r="19" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:25" ht="15.75" customHeight="1">
       <c r="A19" s="16" t="s">
         <v>15</v>
       </c>
@@ -9314,7 +9353,7 @@
       <c r="X19" s="17"/>
       <c r="Y19" s="10"/>
     </row>
-    <row r="20" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:25" ht="15.75" customHeight="1">
       <c r="A20" s="16" t="s">
         <v>15</v>
       </c>
@@ -9387,7 +9426,7 @@
       </c>
       <c r="Y20" s="10"/>
     </row>
-    <row r="21" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:25" ht="15.75" customHeight="1">
       <c r="A21" s="26" t="s">
         <v>15</v>
       </c>
@@ -9460,7 +9499,7 @@
       </c>
       <c r="Y21" s="10"/>
     </row>
-    <row r="22" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:25" ht="15.75" customHeight="1">
       <c r="A22" s="26" t="s">
         <v>15</v>
       </c>
@@ -9531,7 +9570,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:25" ht="15.75" customHeight="1">
       <c r="A23" s="26" t="s">
         <v>15</v>
       </c>
@@ -9600,7 +9639,7 @@
       <c r="X23" s="21"/>
       <c r="Y23" s="10"/>
     </row>
-    <row r="24" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:25" ht="15.75" customHeight="1">
       <c r="A24" s="26" t="s">
         <v>15</v>
       </c>
@@ -9669,7 +9708,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:25" ht="15.75" customHeight="1">
       <c r="A25" s="26" t="s">
         <v>15</v>
       </c>
@@ -9730,7 +9769,7 @@
       <c r="X25" s="21"/>
       <c r="Y25" s="10"/>
     </row>
-    <row r="26" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:25" ht="15.75" customHeight="1">
       <c r="A26" s="26" t="s">
         <v>15</v>
       </c>
@@ -9783,7 +9822,7 @@
       <c r="X26" s="21"/>
       <c r="Y26" s="10"/>
     </row>
-    <row r="27" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:25" ht="15.75" customHeight="1">
       <c r="A27" s="26" t="s">
         <v>15</v>
       </c>
@@ -9830,7 +9869,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:25" ht="15.75" customHeight="1">
       <c r="A28" s="26" t="s">
         <v>15</v>
       </c>
@@ -9879,10 +9918,10 @@
         <v>160</v>
       </c>
       <c r="R28" s="21" t="s">
-        <v>132</v>
+        <v>169</v>
       </c>
       <c r="S28" s="21" t="s">
-        <v>113</v>
+        <v>168</v>
       </c>
       <c r="T28" s="21" t="s">
         <v>131</v>
@@ -9899,7 +9938,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="29" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:25" ht="15.75" customHeight="1">
       <c r="A29" s="26" t="s">
         <v>15</v>
       </c>
@@ -9962,7 +10001,7 @@
       <c r="X29" s="21"/>
       <c r="Y29" s="10"/>
     </row>
-    <row r="30" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:25" ht="15.75" customHeight="1">
       <c r="A30" s="26" t="s">
         <v>15</v>
       </c>
@@ -10027,7 +10066,7 @@
       <c r="X30" s="21"/>
       <c r="Y30" s="10"/>
     </row>
-    <row r="31" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:25" ht="15.75" customHeight="1">
       <c r="A31" s="26" t="s">
         <v>15</v>
       </c>
@@ -10090,7 +10129,7 @@
       <c r="X31" s="21"/>
       <c r="Y31" s="10"/>
     </row>
-    <row r="32" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:25" ht="15.75" customHeight="1">
       <c r="A32" s="26" t="s">
         <v>15</v>
       </c>
@@ -10153,7 +10192,7 @@
       <c r="X32" s="21"/>
       <c r="Y32" s="10"/>
     </row>
-    <row r="33" spans="1:25" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:25" s="38" customFormat="1" ht="15.75" customHeight="1">
       <c r="A33" s="26" t="s">
         <v>15</v>
       </c>
@@ -10215,7 +10254,7 @@
       <c r="W33" s="21"/>
       <c r="X33" s="21"/>
     </row>
-    <row r="34" spans="1:25" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:25" s="38" customFormat="1" ht="15.75" customHeight="1">
       <c r="A34" s="26" t="s">
         <v>15</v>
       </c>
@@ -10277,7 +10316,7 @@
       <c r="W34" s="21"/>
       <c r="X34" s="21"/>
     </row>
-    <row r="35" spans="1:25" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:25" s="38" customFormat="1" ht="15.75" customHeight="1">
       <c r="A35" s="26" t="s">
         <v>15</v>
       </c>
@@ -10339,7 +10378,7 @@
       <c r="W35" s="21"/>
       <c r="X35" s="21"/>
     </row>
-    <row r="36" spans="1:25" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:25" s="13" customFormat="1" ht="15.75" customHeight="1">
       <c r="A36" s="26" t="s">
         <v>15</v>
       </c>
@@ -10412,7 +10451,7 @@
       </c>
       <c r="Y36" s="12"/>
     </row>
-    <row r="37" spans="1:25" s="31" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:25" s="31" customFormat="1" ht="15.75" customHeight="1">
       <c r="A37" s="26" t="s">
         <v>43</v>
       </c>
@@ -10465,7 +10504,7 @@
       <c r="X37" s="21"/>
       <c r="Y37" s="30"/>
     </row>
-    <row r="38" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:25" ht="15.75" customHeight="1">
       <c r="A38" s="26" t="s">
         <v>43</v>
       </c>
@@ -10520,7 +10559,7 @@
       <c r="X38" s="21"/>
       <c r="Y38" s="10"/>
     </row>
-    <row r="39" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:25" ht="15.75" customHeight="1">
       <c r="A39" s="26" t="s">
         <v>43</v>
       </c>
@@ -10591,7 +10630,7 @@
       </c>
       <c r="Y39" s="10"/>
     </row>
-    <row r="40" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1">
       <c r="A40" s="26" t="s">
         <v>43</v>
       </c>
@@ -10664,7 +10703,7 @@
       </c>
       <c r="Y40" s="36"/>
     </row>
-    <row r="41" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:25" ht="15.75" customHeight="1">
       <c r="A41" s="26" t="s">
         <v>43</v>
       </c>
@@ -10735,7 +10774,7 @@
       </c>
       <c r="Y41" s="10"/>
     </row>
-    <row r="42" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:25" ht="15.75" customHeight="1">
       <c r="A42" s="26" t="s">
         <v>43</v>
       </c>
@@ -10806,7 +10845,7 @@
       </c>
       <c r="Y42" s="10"/>
     </row>
-    <row r="43" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:25" ht="15.75" customHeight="1">
       <c r="A43" s="26" t="s">
         <v>43</v>
       </c>
@@ -10877,7 +10916,7 @@
       </c>
       <c r="Y43" s="10"/>
     </row>
-    <row r="44" spans="1:25" s="40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:25" s="40" customFormat="1" ht="15.75" customHeight="1">
       <c r="A44" s="26" t="s">
         <v>43</v>
       </c>
@@ -10948,7 +10987,7 @@
       </c>
       <c r="Y44" s="39"/>
     </row>
-    <row r="45" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:25" ht="15.75" customHeight="1">
       <c r="A45" s="26" t="s">
         <v>43</v>
       </c>
@@ -11019,7 +11058,7 @@
       </c>
       <c r="Y45" s="10"/>
     </row>
-    <row r="46" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:25" ht="15.75" customHeight="1">
       <c r="A46" s="26" t="s">
         <v>43</v>
       </c>
@@ -11088,7 +11127,7 @@
       </c>
       <c r="Y46" s="10"/>
     </row>
-    <row r="47" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:25" ht="15.75" customHeight="1">
       <c r="A47" s="26" t="s">
         <v>43</v>
       </c>
@@ -11159,7 +11198,7 @@
       </c>
       <c r="Y47" s="10"/>
     </row>
-    <row r="48" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:25" ht="15.75" customHeight="1">
       <c r="A48" s="26" t="s">
         <v>43</v>
       </c>
@@ -11222,7 +11261,7 @@
       </c>
       <c r="Y48" s="10"/>
     </row>
-    <row r="49" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:25" ht="15.75" customHeight="1">
       <c r="A49" s="26" t="s">
         <v>43</v>
       </c>
@@ -11279,7 +11318,7 @@
       <c r="X49" s="21"/>
       <c r="Y49" s="10"/>
     </row>
-    <row r="50" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:25" ht="15.75" customHeight="1">
       <c r="A50" s="26" t="s">
         <v>43</v>
       </c>
@@ -11332,7 +11371,7 @@
       <c r="X50" s="21"/>
       <c r="Y50" s="10"/>
     </row>
-    <row r="51" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:25" ht="15.75" customHeight="1">
       <c r="A51" s="26" t="s">
         <v>43</v>
       </c>
@@ -11385,7 +11424,7 @@
       <c r="X51" s="21"/>
       <c r="Y51" s="10"/>
     </row>
-    <row r="52" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:25" ht="15.75" customHeight="1">
       <c r="A52" s="26" t="s">
         <v>43</v>
       </c>
@@ -11438,7 +11477,7 @@
       <c r="X52" s="21"/>
       <c r="Y52" s="10"/>
     </row>
-    <row r="53" spans="1:25" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:25" s="28" customFormat="1" ht="15.75" customHeight="1">
       <c r="A53" s="26" t="s">
         <v>43</v>
       </c>
@@ -11507,7 +11546,7 @@
       </c>
       <c r="Y53" s="27"/>
     </row>
-    <row r="54" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:25" ht="15.75" customHeight="1">
       <c r="A54" s="26" t="s">
         <v>43</v>
       </c>
@@ -11578,7 +11617,7 @@
       </c>
       <c r="Y54" s="10"/>
     </row>
-    <row r="55" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1">
       <c r="A55" s="26" t="s">
         <v>43</v>
       </c>
@@ -11647,7 +11686,7 @@
       <c r="X55" s="21"/>
       <c r="Y55" s="36"/>
     </row>
-    <row r="56" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1">
       <c r="A56" s="26" t="s">
         <v>43</v>
       </c>
@@ -11716,7 +11755,7 @@
       <c r="X56" s="21"/>
       <c r="Y56" s="36"/>
     </row>
-    <row r="57" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1">
       <c r="A57" s="26" t="s">
         <v>43</v>
       </c>
@@ -11785,7 +11824,7 @@
       <c r="X57" s="21"/>
       <c r="Y57" s="36"/>
     </row>
-    <row r="58" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1">
       <c r="A58" s="26" t="s">
         <v>43</v>
       </c>
@@ -11854,7 +11893,7 @@
       <c r="X58" s="21"/>
       <c r="Y58" s="36"/>
     </row>
-    <row r="59" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1">
       <c r="A59" s="26" t="s">
         <v>43</v>
       </c>
@@ -11923,7 +11962,7 @@
       <c r="X59" s="21"/>
       <c r="Y59" s="36"/>
     </row>
-    <row r="60" spans="1:25" s="34" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:25" s="34" customFormat="1" ht="15.75" customHeight="1">
       <c r="A60" s="26" t="s">
         <v>43</v>
       </c>
@@ -11974,7 +12013,7 @@
       <c r="X60" s="21"/>
       <c r="Y60" s="33"/>
     </row>
-    <row r="61" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:25" ht="15.75" customHeight="1">
       <c r="A61" s="26" t="s">
         <v>58</v>
       </c>
@@ -12049,7 +12088,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:25" ht="15.75" customHeight="1">
       <c r="A62" s="26" t="s">
         <v>58</v>
       </c>
@@ -12122,7 +12161,7 @@
       </c>
       <c r="Y62" s="48"/>
     </row>
-    <row r="63" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:25" ht="15.75" customHeight="1">
       <c r="A63" s="26" t="s">
         <v>62</v>
       </c>
@@ -12195,7 +12234,7 @@
       </c>
       <c r="Y63" s="10"/>
     </row>
-    <row r="64" spans="1:25" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:25" s="15" customFormat="1" ht="15.75" customHeight="1">
       <c r="A64" s="18" t="s">
         <v>63</v>
       </c>
@@ -12230,7 +12269,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="65" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:24" ht="15.75" customHeight="1">
       <c r="A65" s="16" t="s">
         <v>63</v>
       </c>
@@ -12274,7 +12313,7 @@
       <c r="W65" s="17"/>
       <c r="X65" s="17"/>
     </row>
-    <row r="66" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:24" ht="15.75" customHeight="1">
       <c r="A66" s="16" t="s">
         <v>63</v>
       </c>
@@ -12306,7 +12345,7 @@
       <c r="W66" s="17"/>
       <c r="X66" s="17"/>
     </row>
-    <row r="67" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:24" ht="15.75" customHeight="1">
       <c r="A67" s="16" t="s">
         <v>63</v>
       </c>
@@ -12338,7 +12377,7 @@
       <c r="W67" s="17"/>
       <c r="X67" s="17"/>
     </row>
-    <row r="68" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:24" ht="15.75" customHeight="1">
       <c r="A68" s="16" t="s">
         <v>63</v>
       </c>
@@ -12370,7 +12409,7 @@
       <c r="W68" s="17"/>
       <c r="X68" s="17"/>
     </row>
-    <row r="69" spans="1:24" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:24" s="45" customFormat="1" ht="15.75" customHeight="1">
       <c r="A69" s="16" t="s">
         <v>63</v>
       </c>
@@ -12402,7 +12441,7 @@
       <c r="W69" s="17"/>
       <c r="X69" s="17"/>
     </row>
-    <row r="70" spans="1:24" s="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:24" s="35" customFormat="1" ht="15.75" customHeight="1">
       <c r="A70" s="16" t="s">
         <v>63</v>
       </c>
@@ -12434,7 +12473,7 @@
       <c r="W70" s="17"/>
       <c r="X70" s="17"/>
     </row>
-    <row r="71" spans="1:24" s="32" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:24" s="32" customFormat="1" ht="15.75" customHeight="1">
       <c r="A71" s="16" t="s">
         <v>63</v>
       </c>
@@ -12466,7 +12505,7 @@
       <c r="W71" s="17"/>
       <c r="X71" s="17"/>
     </row>
-    <row r="72" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:24" ht="15.75" customHeight="1">
       <c r="A72" s="16" t="s">
         <v>109</v>
       </c>
@@ -12498,7 +12537,7 @@
       <c r="W72" s="20"/>
       <c r="X72" s="20"/>
     </row>
-    <row r="73" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:24" ht="15.75" customHeight="1">
       <c r="A73" s="16" t="s">
         <v>119</v>
       </c>
@@ -12554,22 +12593,19 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C50" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="D69" sqref="D69"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
+      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
     <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
       <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
-      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="Q7" sqref="Q7"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="C50" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="D69" sqref="D69"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>
@@ -12584,6 +12620,11 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -12592,10 +12633,10 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="29.6640625" customWidth="1"/>
     <col min="2" max="2" width="28.1640625" customWidth="1"/>
@@ -12603,7 +12644,7 @@
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="15">
       <c r="A1" s="22" t="s">
         <v>70</v>
       </c>
@@ -12620,7 +12661,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15">
       <c r="A2" s="23" t="s">
         <v>73</v>
       </c>
@@ -12633,7 +12674,7 @@
       <c r="D2" s="24"/>
       <c r="E2" s="24"/>
     </row>
-    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="15">
       <c r="A3" s="23" t="s">
         <v>75</v>
       </c>
@@ -12646,7 +12687,7 @@
       <c r="D3" s="24"/>
       <c r="E3" s="24"/>
     </row>
-    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="15">
       <c r="A4" s="23" t="s">
         <v>77</v>
       </c>
@@ -12659,7 +12700,7 @@
       <c r="D4" s="24"/>
       <c r="E4" s="24"/>
     </row>
-    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="15">
       <c r="A5" s="23" t="s">
         <v>96</v>
       </c>
@@ -12674,7 +12715,7 @@
       </c>
       <c r="E5" s="24"/>
     </row>
-    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="15">
       <c r="A6" s="23" t="s">
         <v>97</v>
       </c>
@@ -12689,7 +12730,7 @@
       </c>
       <c r="E6" s="24"/>
     </row>
-    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="15">
       <c r="A7" s="23" t="s">
         <v>98</v>
       </c>
@@ -12704,7 +12745,7 @@
       </c>
       <c r="E7" s="24"/>
     </row>
-    <row r="8" spans="1:5" s="41" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" s="41" customFormat="1" ht="15">
       <c r="A8" s="23" t="s">
         <v>163</v>
       </c>
@@ -12719,7 +12760,7 @@
       </c>
       <c r="E8" s="24"/>
     </row>
-    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="15">
       <c r="A9" s="23" t="s">
         <v>99</v>
       </c>
@@ -12734,7 +12775,7 @@
       </c>
       <c r="E9" s="24"/>
     </row>
-    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="15">
       <c r="A10" s="23" t="s">
         <v>108</v>
       </c>
@@ -12747,7 +12788,7 @@
       <c r="D10" s="24"/>
       <c r="E10" s="24"/>
     </row>
-    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="15">
       <c r="A11" s="23" t="s">
         <v>107</v>
       </c>
@@ -12760,7 +12801,7 @@
       <c r="D11" s="24"/>
       <c r="E11" s="24"/>
     </row>
-    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="15">
       <c r="A12" s="23" t="s">
         <v>106</v>
       </c>
@@ -12773,7 +12814,7 @@
       <c r="D12" s="24"/>
       <c r="E12" s="24"/>
     </row>
-    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="15">
       <c r="A13" s="23" t="s">
         <v>100</v>
       </c>
@@ -12788,7 +12829,7 @@
       </c>
       <c r="E13" s="24"/>
     </row>
-    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="15">
       <c r="A14" s="23" t="s">
         <v>105</v>
       </c>
@@ -12803,7 +12844,7 @@
       </c>
       <c r="E14" s="24"/>
     </row>
-    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="15">
       <c r="A15" s="23" t="s">
         <v>101</v>
       </c>
@@ -12818,7 +12859,7 @@
       </c>
       <c r="E15" s="24"/>
     </row>
-    <row r="16" spans="1:5" s="41" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" s="41" customFormat="1" ht="15">
       <c r="A16" s="23" t="s">
         <v>162</v>
       </c>
@@ -12833,7 +12874,7 @@
       </c>
       <c r="E16" s="24"/>
     </row>
-    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="15">
       <c r="A17" s="23" t="s">
         <v>102</v>
       </c>
@@ -12848,7 +12889,7 @@
       </c>
       <c r="E17" s="24"/>
     </row>
-    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="15">
       <c r="A18" s="23" t="s">
         <v>103</v>
       </c>
@@ -12863,7 +12904,7 @@
       </c>
       <c r="E18" s="24"/>
     </row>
-    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="15">
       <c r="A19" s="23" t="s">
         <v>122</v>
       </c>
@@ -12878,7 +12919,7 @@
       </c>
       <c r="E19" s="24"/>
     </row>
-    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="15">
       <c r="A20" s="23" t="s">
         <v>12</v>
       </c>
@@ -12893,7 +12934,7 @@
       </c>
       <c r="E20" s="24"/>
     </row>
-    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="15">
       <c r="A21" s="23" t="s">
         <v>13</v>
       </c>
@@ -12908,7 +12949,7 @@
       </c>
       <c r="E21" s="24"/>
     </row>
-    <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="15">
       <c r="A22" s="23" t="s">
         <v>104</v>
       </c>
@@ -12925,23 +12966,25 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}">
-      <selection activeCell="G36" sqref="G36"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
+      <selection activeCell="B17" sqref="B17"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
     <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
       <selection activeCell="C7" sqref="C7"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
-      <selection activeCell="B17" sqref="B17"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}">
+      <selection activeCell="G36" sqref="G36"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
HAR-4745 Salli urakanvalvojalle yha-kohteiden tuonti
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="38400" windowHeight="21600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-900" windowWidth="38400" windowHeight="22040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -12,9 +12,9 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="2180" windowHeight="891" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
-    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="2180" windowHeight="891" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1234" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1234" uniqueCount="172">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -571,6 +571,12 @@
   </si>
   <si>
     <t>R+,W+,TM-valmis</t>
+  </si>
+  <si>
+    <t>R*,W*,sido</t>
+  </si>
+  <si>
+    <t>R,W,sido</t>
   </si>
 </sst>
 </file>
@@ -703,8 +709,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="161">
+  <cellStyleXfs count="167">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -961,7 +973,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="161">
+  <cellStyles count="167">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1042,6 +1054,9 @@
     <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1122,6 +1137,9 @@
     <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1135,7 +1153,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{20D72FDE-B37A-954B-96C9-CC76E718E9F1}" diskRevisions="1" revisionId="313" version="39">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{B41A3796-87BE-7844-B985-10174BA79182}" diskRevisions="1" revisionId="319" version="40">
   <header guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" dateTime="2016-09-06T09:14:56" maxSheetId="3" userName="Tatu Tarvainen" r:id="rId2" minRId="1" maxRId="3">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1364,6 +1382,12 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{B41A3796-87BE-7844-B985-10174BA79182}" dateTime="2017-03-13T12:47:10" maxSheetId="3" userName="Jarno Väyrynen" r:id="rId40" minRId="314" maxRId="319">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -7334,6 +7358,83 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog39.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="314" sId="1">
+    <oc r="L29" t="inlineStr">
+      <is>
+        <t>R*,W</t>
+      </is>
+    </oc>
+    <nc r="L29" t="inlineStr">
+      <is>
+        <t>R*,W,sido</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="315" sId="1">
+    <oc r="K29" t="inlineStr">
+      <is>
+        <t>R*,W*</t>
+      </is>
+    </oc>
+    <nc r="K29" t="inlineStr">
+      <is>
+        <t>R*,W*,sido</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="316" sId="1">
+    <oc r="Q29" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </oc>
+    <nc r="Q29" t="inlineStr">
+      <is>
+        <t>R,W,sido</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="317" sId="1">
+    <oc r="Q31" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </oc>
+    <nc r="Q31" t="inlineStr">
+      <is>
+        <t>R,W,sido</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="318" sId="1">
+    <oc r="L31" t="inlineStr">
+      <is>
+        <t>R*,W</t>
+      </is>
+    </oc>
+    <nc r="L31" t="inlineStr">
+      <is>
+        <t>R*,W,sido</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="319" sId="1">
+    <oc r="K31" t="inlineStr">
+      <is>
+        <t>R*,W*</t>
+      </is>
+    </oc>
+    <nc r="K31" t="inlineStr">
+      <is>
+        <t>R*,W*,sido</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="5" sId="1" odxf="1" dxf="1">
@@ -8030,8 +8131,8 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="7">
+<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="8">
   <userInfo guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" name="Tatu Tarvainen" id="-130145201" dateTime="2016-09-06T09:10:23"/>
   <userInfo guid="{E0850D7E-A93F-EF44-B46A-3BEA4D7DBEDB}" name="Jarno Väyrynen" id="-589116405" dateTime="2016-09-06T12:54:09"/>
   <userInfo guid="{0407E191-78DA-F349-B5E5-8AE1BC03A29E}" name="Jarno Väyrynen" id="-589108428" dateTime="2016-09-08T15:33:24"/>
@@ -8039,6 +8140,7 @@
   <userInfo guid="{C606B059-99AC-3B47-8437-66D15B4E3D4B}" name="Jarno Väyrynen" id="-589137240" dateTime="2016-10-27T09:33:01"/>
   <userInfo guid="{73C5A3F1-D661-114E-91EF-0474461FB0FF}" name="Jarno Väyrynen" id="-589139215" dateTime="2017-02-01T12:41:16"/>
   <userInfo guid="{20D72FDE-B37A-954B-96C9-CC76E718E9F1}" name="Jarno Väyrynen" id="-589140570" dateTime="2017-03-02T10:49:07"/>
+  <userInfo guid="{B41A3796-87BE-7844-B985-10174BA79182}" name="Jarno Väyrynen" id="-589147330" dateTime="2017-03-13T12:30:30"/>
 </users>
 </file>
 
@@ -8367,10 +8469,10 @@
   <dimension ref="A1:Y73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="E8" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
+      <selection pane="bottomRight" activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -9966,10 +10068,10 @@
         <v>113</v>
       </c>
       <c r="K29" s="17" t="s">
-        <v>126</v>
+        <v>170</v>
       </c>
       <c r="L29" s="21" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="M29" s="21"/>
       <c r="N29" s="21" t="s">
@@ -9980,7 +10082,7 @@
       </c>
       <c r="P29" s="21"/>
       <c r="Q29" s="21" t="s">
-        <v>113</v>
+        <v>171</v>
       </c>
       <c r="R29" s="21" t="s">
         <v>132</v>
@@ -10094,10 +10196,10 @@
         <v>113</v>
       </c>
       <c r="K31" s="17" t="s">
-        <v>126</v>
+        <v>170</v>
       </c>
       <c r="L31" s="21" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="M31" s="21"/>
       <c r="N31" s="21" t="s">
@@ -10108,7 +10210,7 @@
       </c>
       <c r="P31" s="21"/>
       <c r="Q31" s="21" t="s">
-        <v>113</v>
+        <v>171</v>
       </c>
       <c r="R31" s="21" t="s">
         <v>132</v>
@@ -12593,9 +12695,9 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
-      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
+    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="C50" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="D69" sqref="D69"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
     <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
@@ -12603,9 +12705,9 @@
       <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C50" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="D69" sqref="D69"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
+      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>
@@ -12617,7 +12719,7 @@
     <mergeCell ref="C1:O1"/>
     <mergeCell ref="C2:O2"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
@@ -12966,20 +13068,20 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
-      <selection activeCell="B17" sqref="B17"/>
+    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}">
+      <selection activeCell="G36" sqref="G36"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
     <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
       <selection activeCell="C7" sqref="C7"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}">
-      <selection activeCell="G36" sqref="G36"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
+      <selection activeCell="B17" sqref="B17"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
HAR-4882 Muuta rooliexceliin muuttyot -> muutkustannukset
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-900" windowWidth="51160" windowHeight="28560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-900" windowWidth="47320" windowHeight="28320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -12,9 +12,9 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="2180" windowHeight="891" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
-    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="2180" windowHeight="891" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -528,9 +528,6 @@
     <t>Toteutus / Yksikköhintaiset työt</t>
   </si>
   <si>
-    <t>Toteutus / Muut työt</t>
-  </si>
-  <si>
     <t>Muutos- ja lisätyöt</t>
   </si>
   <si>
@@ -586,6 +583,9 @@
   </si>
   <si>
     <t>Sakko- ja bonusraportti</t>
+  </si>
+  <si>
+    <t>Toteutus / Muut kustannukset</t>
   </si>
 </sst>
 </file>
@@ -1182,7 +1182,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{AB1578F0-267B-E24D-9EF4-EAE2A9AEBDC8}" diskRevisions="1" revisionId="369" version="44">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{5E865E05-EE6E-304C-806E-707B869C773E}" diskRevisions="1" revisionId="370" version="45">
   <header guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" dateTime="2016-09-06T09:14:56" maxSheetId="3" userName="Tatu Tarvainen" r:id="rId2" minRId="1" maxRId="3">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1441,6 +1441,12 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{5E865E05-EE6E-304C-806E-707B869C773E}" dateTime="2017-03-27T13:19:01" maxSheetId="3" userName="Jarno Väyrynen" r:id="rId45" minRId="370">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -7900,6 +7906,23 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog44.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="370" sId="1">
+    <oc r="B36" t="inlineStr">
+      <is>
+        <t>Toteutus / Muut työt</t>
+      </is>
+    </oc>
+    <nc r="B36" t="inlineStr">
+      <is>
+        <t>Toteutus / Muut kustannukset</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog5.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="7" sId="1">
@@ -8539,7 +8562,7 @@
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="9">
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="10">
   <userInfo guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" name="Tatu Tarvainen" id="-130145201" dateTime="2016-09-06T09:10:23"/>
   <userInfo guid="{E0850D7E-A93F-EF44-B46A-3BEA4D7DBEDB}" name="Jarno Väyrynen" id="-589116405" dateTime="2016-09-06T12:54:09"/>
   <userInfo guid="{0407E191-78DA-F349-B5E5-8AE1BC03A29E}" name="Jarno Väyrynen" id="-589108428" dateTime="2016-09-08T15:33:24"/>
@@ -8549,6 +8572,7 @@
   <userInfo guid="{20D72FDE-B37A-954B-96C9-CC76E718E9F1}" name="Jarno Väyrynen" id="-589140570" dateTime="2017-03-02T10:49:07"/>
   <userInfo guid="{B41A3796-87BE-7844-B985-10174BA79182}" name="Jarno Väyrynen" id="-589147330" dateTime="2017-03-13T12:30:30"/>
   <userInfo guid="{AB1578F0-267B-E24D-9EF4-EAE2A9AEBDC8}" name="Jarno Väyrynen" id="-589122421" dateTime="2017-03-17T14:40:01"/>
+  <userInfo guid="{5E865E05-EE6E-304C-806E-707B869C773E}" name="Jarno Väyrynen" id="-589107713" dateTime="2017-03-27T13:18:35"/>
 </users>
 </file>
 
@@ -8877,10 +8901,10 @@
   <dimension ref="A1:Y76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="D23" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B57" sqref="B57"/>
+      <selection pane="bottomRight" activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -9025,7 +9049,7 @@
         <v>81</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K6" s="8" t="s">
         <v>83</v>
@@ -9046,7 +9070,7 @@
         <v>88</v>
       </c>
       <c r="Q6" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="R6" s="9" t="s">
         <v>82</v>
@@ -9067,7 +9091,7 @@
         <v>92</v>
       </c>
       <c r="X6" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="15.75" customHeight="1">
@@ -10036,7 +10060,7 @@
         <v>127</v>
       </c>
       <c r="J22" s="21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K22" s="17" t="s">
         <v>126</v>
@@ -10057,7 +10081,7 @@
         <v>127</v>
       </c>
       <c r="Q22" s="21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="R22" s="21" t="s">
         <v>131</v>
@@ -10384,7 +10408,7 @@
         <v>15</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C28" s="21"/>
       <c r="D28" s="17" t="s">
@@ -10444,7 +10468,7 @@
         <v>152</v>
       </c>
       <c r="E29" s="17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F29" s="21" t="s">
         <v>127</v>
@@ -10459,13 +10483,13 @@
         <v>127</v>
       </c>
       <c r="J29" s="42" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K29" s="17" t="s">
         <v>126</v>
       </c>
       <c r="L29" s="21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M29" s="21" t="s">
         <v>17</v>
@@ -10478,13 +10502,13 @@
       </c>
       <c r="P29" s="21"/>
       <c r="Q29" s="42" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="R29" s="21" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="S29" s="21" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="T29" s="21" t="s">
         <v>131</v>
@@ -10529,7 +10553,7 @@
         <v>113</v>
       </c>
       <c r="K30" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L30" s="21" t="s">
         <v>134</v>
@@ -10543,7 +10567,7 @@
       </c>
       <c r="P30" s="21"/>
       <c r="Q30" s="21" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="R30" s="21" t="s">
         <v>132</v>
@@ -10591,7 +10615,7 @@
         <v>127</v>
       </c>
       <c r="J31" s="21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K31" s="17" t="s">
         <v>126</v>
@@ -10608,7 +10632,7 @@
       </c>
       <c r="P31" s="21"/>
       <c r="Q31" s="21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="R31" s="21" t="s">
         <v>132</v>
@@ -10657,7 +10681,7 @@
         <v>113</v>
       </c>
       <c r="K32" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L32" s="21" t="s">
         <v>134</v>
@@ -10671,7 +10695,7 @@
       </c>
       <c r="P32" s="21"/>
       <c r="Q32" s="21" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="R32" s="21" t="s">
         <v>132</v>
@@ -10884,7 +10908,7 @@
         <v>15</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>155</v>
+        <v>174</v>
       </c>
       <c r="C36" s="21"/>
       <c r="D36" s="17" t="s">
@@ -11072,7 +11096,7 @@
         <v>43</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C39" s="21"/>
       <c r="D39" s="17" t="s">
@@ -11537,7 +11561,7 @@
         <v>43</v>
       </c>
       <c r="B46" s="26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C46" s="21"/>
       <c r="D46" s="21" t="s">
@@ -12167,7 +12191,7 @@
         <v>43</v>
       </c>
       <c r="B56" s="26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C56" s="21"/>
       <c r="D56" s="21" t="s">
@@ -13099,7 +13123,7 @@
         <v>63</v>
       </c>
       <c r="B72" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C72" s="17"/>
       <c r="D72" s="21" t="s">
@@ -13243,7 +13267,7 @@
       <c r="H76" s="29"/>
       <c r="I76" s="29"/>
       <c r="J76" s="44" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K76" s="29" t="s">
         <v>128</v>
@@ -13260,17 +13284,17 @@
       <c r="O76" s="29"/>
       <c r="P76" s="29"/>
       <c r="Q76" s="44" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="R76" s="46" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="S76" s="44" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="T76" s="29"/>
       <c r="U76" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="V76" s="29"/>
       <c r="W76" s="29"/>
@@ -13278,9 +13302,9 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
-      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
+    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="C50" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="D69" sqref="D69"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
     <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
@@ -13288,9 +13312,9 @@
       <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C50" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="D69" sqref="D69"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
+      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>
@@ -13432,10 +13456,10 @@
     </row>
     <row r="8" spans="1:5" s="41" customFormat="1" ht="15">
       <c r="A8" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="B8" s="23" t="s">
         <v>163</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>164</v>
       </c>
       <c r="C8" s="23" t="s">
         <v>3</v>
@@ -13546,10 +13570,10 @@
     </row>
     <row r="16" spans="1:5" s="41" customFormat="1" ht="15">
       <c r="A16" s="23" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C16" s="23" t="s">
         <v>5</v>
@@ -13624,7 +13648,7 @@
         <v>13</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C21" s="23" t="s">
         <v>4</v>
@@ -13651,16 +13675,16 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
-      <selection activeCell="B17" sqref="B17"/>
+    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}">
+      <selection activeCell="G36" sqref="G36"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
     <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
       <selection activeCell="C7" sqref="C7"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}">
-      <selection activeCell="G36" sqref="G36"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
+      <selection activeCell="B17" sqref="B17"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
Lisää JVH:lle "maksuerat" erikoisoikeus päällystyksen maksueränäkymään
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarihan/Jari/Projektit/Harja/harja/resources/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-900" windowWidth="32880" windowHeight="29160" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="43600" windowHeight="19360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -12,16 +17,16 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="2180" windowHeight="866" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
-    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="2180" windowHeight="891" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
@@ -61,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1299" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1299" uniqueCount="181">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -601,6 +606,9 @@
   </si>
   <si>
     <t>R*,W*,maksueratunnus</t>
+  </si>
+  <si>
+    <t>R*,W*,maksuerat,maksueratunnus</t>
   </si>
 </sst>
 </file>
@@ -1205,7 +1213,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{ED78840A-3509-BB4A-BA89-075EA96D3AEC}" diskRevisions="1" revisionId="389" version="46">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{EA67C2AA-D5C4-9A49-8DF5-86A96AD16ED9}" diskRevisions="1" revisionId="390" version="47">
   <header guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" dateTime="2016-09-06T09:14:56" maxSheetId="3" userName="Tatu Tarvainen" r:id="rId2" minRId="1" maxRId="3">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1476,6 +1484,12 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{EA67C2AA-D5C4-9A49-8DF5-86A96AD16ED9}" dateTime="2017-04-04T12:26:09" maxSheetId="3" userName="Microsoft Office User" r:id="rId47" minRId="390">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -8084,6 +8098,25 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog46.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="390" sId="1">
+    <oc r="D34" t="inlineStr">
+      <is>
+        <t>R*,W*,maksueratunnus</t>
+      </is>
+    </oc>
+    <nc r="D34" t="inlineStr">
+      <is>
+        <t>R*,W*,maksuerat,maksueratunnus</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="delete"/>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog5.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="7" sId="1">
@@ -8722,7 +8755,7 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="11">
   <userInfo guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" name="Tatu Tarvainen" id="-130145201" dateTime="2016-09-06T09:10:23"/>
   <userInfo guid="{E0850D7E-A93F-EF44-B46A-3BEA4D7DBEDB}" name="Jarno Väyrynen" id="-589116405" dateTime="2016-09-06T12:54:09"/>
@@ -9062,14 +9095,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
+      <pane xSplit="2" ySplit="6" topLeftCell="C14" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D34" sqref="D34"/>
+      <selection pane="bottomRight" activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.5" bestFit="1" customWidth="1"/>
@@ -9097,7 +9130,7 @@
     <col min="25" max="25" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="24" customHeight="1">
+    <row r="1" spans="1:25" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -9118,7 +9151,7 @@
       <c r="N1" s="55"/>
       <c r="O1" s="55"/>
     </row>
-    <row r="2" spans="1:25" ht="15.75" customHeight="1">
+    <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="56" t="s">
@@ -9137,7 +9170,7 @@
       <c r="N2" s="52"/>
       <c r="O2" s="52"/>
     </row>
-    <row r="3" spans="1:25" ht="15.75" customHeight="1">
+    <row r="3" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -9152,10 +9185,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="15.75" customHeight="1">
+    <row r="4" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:25" ht="15.75" customHeight="1">
+    <row r="5" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C5" s="53" t="s">
         <v>6</v>
       </c>
@@ -9184,7 +9217,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="15.75" customHeight="1">
+    <row r="6" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
@@ -9256,7 +9289,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="15.75" customHeight="1">
+    <row r="7" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="16" t="s">
         <v>15</v>
       </c>
@@ -9329,7 +9362,7 @@
       </c>
       <c r="Y7" s="10"/>
     </row>
-    <row r="8" spans="1:25" ht="15.75" customHeight="1">
+    <row r="8" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="16" t="s">
         <v>15</v>
       </c>
@@ -9388,7 +9421,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="15.75" customHeight="1">
+    <row r="9" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="16" t="s">
         <v>15</v>
       </c>
@@ -9441,7 +9474,7 @@
       <c r="X9" s="17"/>
       <c r="Y9" s="10"/>
     </row>
-    <row r="10" spans="1:25" ht="15.75" customHeight="1">
+    <row r="10" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="16" t="s">
         <v>15</v>
       </c>
@@ -9494,7 +9527,7 @@
       <c r="X10" s="17"/>
       <c r="Y10" s="10"/>
     </row>
-    <row r="11" spans="1:25" ht="15.75" customHeight="1">
+    <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="16" t="s">
         <v>15</v>
       </c>
@@ -9561,7 +9594,7 @@
       <c r="X11" s="17"/>
       <c r="Y11" s="10"/>
     </row>
-    <row r="12" spans="1:25" ht="15.75" customHeight="1">
+    <row r="12" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="16" t="s">
         <v>15</v>
       </c>
@@ -9628,7 +9661,7 @@
       <c r="X12" s="17"/>
       <c r="Y12" s="10"/>
     </row>
-    <row r="13" spans="1:25" ht="15.75" customHeight="1">
+    <row r="13" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="16" t="s">
         <v>15</v>
       </c>
@@ -9683,7 +9716,7 @@
       <c r="X13" s="17"/>
       <c r="Y13" s="10"/>
     </row>
-    <row r="14" spans="1:25" ht="15.75" customHeight="1">
+    <row r="14" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="16" t="s">
         <v>15</v>
       </c>
@@ -9738,7 +9771,7 @@
       <c r="X14" s="17"/>
       <c r="Y14" s="10"/>
     </row>
-    <row r="15" spans="1:25" ht="15.75" customHeight="1">
+    <row r="15" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="16" t="s">
         <v>15</v>
       </c>
@@ -9793,7 +9826,7 @@
       <c r="X15" s="17"/>
       <c r="Y15" s="10"/>
     </row>
-    <row r="16" spans="1:25" ht="15.75" customHeight="1">
+    <row r="16" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="16" t="s">
         <v>15</v>
       </c>
@@ -9860,7 +9893,7 @@
       <c r="X16" s="17"/>
       <c r="Y16" s="10"/>
     </row>
-    <row r="17" spans="1:25" ht="15.75" customHeight="1">
+    <row r="17" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="16" t="s">
         <v>15</v>
       </c>
@@ -9927,7 +9960,7 @@
       <c r="X17" s="17"/>
       <c r="Y17" s="10"/>
     </row>
-    <row r="18" spans="1:25" ht="15.75" customHeight="1">
+    <row r="18" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="16" t="s">
         <v>15</v>
       </c>
@@ -9982,7 +10015,7 @@
       <c r="X18" s="17"/>
       <c r="Y18" s="10"/>
     </row>
-    <row r="19" spans="1:25" ht="15.75" customHeight="1">
+    <row r="19" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="16" t="s">
         <v>15</v>
       </c>
@@ -10049,7 +10082,7 @@
       <c r="X19" s="17"/>
       <c r="Y19" s="10"/>
     </row>
-    <row r="20" spans="1:25" ht="15.75" customHeight="1">
+    <row r="20" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="16" t="s">
         <v>15</v>
       </c>
@@ -10122,7 +10155,7 @@
       </c>
       <c r="Y20" s="10"/>
     </row>
-    <row r="21" spans="1:25" ht="15.75" customHeight="1">
+    <row r="21" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="26" t="s">
         <v>15</v>
       </c>
@@ -10195,7 +10228,7 @@
       </c>
       <c r="Y21" s="10"/>
     </row>
-    <row r="22" spans="1:25" ht="15.75" customHeight="1">
+    <row r="22" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="26" t="s">
         <v>15</v>
       </c>
@@ -10266,7 +10299,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="15.75" customHeight="1">
+    <row r="23" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="26" t="s">
         <v>15</v>
       </c>
@@ -10335,7 +10368,7 @@
       <c r="X23" s="21"/>
       <c r="Y23" s="10"/>
     </row>
-    <row r="24" spans="1:25" ht="15.75" customHeight="1">
+    <row r="24" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="26" t="s">
         <v>15</v>
       </c>
@@ -10404,7 +10437,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="15.75" customHeight="1">
+    <row r="25" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="26" t="s">
         <v>15</v>
       </c>
@@ -10465,7 +10498,7 @@
       <c r="X25" s="21"/>
       <c r="Y25" s="10"/>
     </row>
-    <row r="26" spans="1:25" ht="15.75" customHeight="1">
+    <row r="26" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="26" t="s">
         <v>15</v>
       </c>
@@ -10518,7 +10551,7 @@
       <c r="X26" s="21"/>
       <c r="Y26" s="10"/>
     </row>
-    <row r="27" spans="1:25" ht="15.75" customHeight="1">
+    <row r="27" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="26" t="s">
         <v>15</v>
       </c>
@@ -10565,7 +10598,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:25" s="48" customFormat="1" ht="15.75" customHeight="1">
+    <row r="28" spans="1:25" s="48" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="26" t="s">
         <v>15</v>
       </c>
@@ -10618,7 +10651,7 @@
       <c r="X28" s="21"/>
       <c r="Y28" s="47"/>
     </row>
-    <row r="29" spans="1:25" ht="15.75" customHeight="1">
+    <row r="29" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="26" t="s">
         <v>15</v>
       </c>
@@ -10687,7 +10720,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="30" spans="1:25" ht="15.75" customHeight="1">
+    <row r="30" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="26" t="s">
         <v>15</v>
       </c>
@@ -10750,7 +10783,7 @@
       <c r="X30" s="21"/>
       <c r="Y30" s="10"/>
     </row>
-    <row r="31" spans="1:25" ht="15.75" customHeight="1">
+    <row r="31" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="26" t="s">
         <v>15</v>
       </c>
@@ -10815,7 +10848,7 @@
       <c r="X31" s="21"/>
       <c r="Y31" s="10"/>
     </row>
-    <row r="32" spans="1:25" ht="15.75" customHeight="1">
+    <row r="32" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="26" t="s">
         <v>15</v>
       </c>
@@ -10878,7 +10911,7 @@
       <c r="X32" s="21"/>
       <c r="Y32" s="10"/>
     </row>
-    <row r="33" spans="1:25" ht="15.75" customHeight="1">
+    <row r="33" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="26" t="s">
         <v>15</v>
       </c>
@@ -10941,7 +10974,7 @@
       <c r="X33" s="21"/>
       <c r="Y33" s="10"/>
     </row>
-    <row r="34" spans="1:25" s="50" customFormat="1" ht="15.75" customHeight="1">
+    <row r="34" spans="1:25" s="50" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="26" t="s">
         <v>15</v>
       </c>
@@ -10950,7 +10983,7 @@
       </c>
       <c r="C34" s="21"/>
       <c r="D34" s="17" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E34" s="17" t="s">
         <v>177</v>
@@ -11004,7 +11037,7 @@
       <c r="X34" s="21"/>
       <c r="Y34" s="49"/>
     </row>
-    <row r="35" spans="1:25" s="38" customFormat="1" ht="15.75" customHeight="1">
+    <row r="35" spans="1:25" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="26" t="s">
         <v>15</v>
       </c>
@@ -11066,7 +11099,7 @@
       <c r="W35" s="21"/>
       <c r="X35" s="21"/>
     </row>
-    <row r="36" spans="1:25" s="38" customFormat="1" ht="15.75" customHeight="1">
+    <row r="36" spans="1:25" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="26" t="s">
         <v>15</v>
       </c>
@@ -11128,7 +11161,7 @@
       <c r="W36" s="21"/>
       <c r="X36" s="21"/>
     </row>
-    <row r="37" spans="1:25" s="38" customFormat="1" ht="15.75" customHeight="1">
+    <row r="37" spans="1:25" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="26" t="s">
         <v>15</v>
       </c>
@@ -11190,7 +11223,7 @@
       <c r="W37" s="21"/>
       <c r="X37" s="21"/>
     </row>
-    <row r="38" spans="1:25" s="13" customFormat="1" ht="15.75" customHeight="1">
+    <row r="38" spans="1:25" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="26" t="s">
         <v>15</v>
       </c>
@@ -11263,7 +11296,7 @@
       </c>
       <c r="Y38" s="12"/>
     </row>
-    <row r="39" spans="1:25" s="31" customFormat="1" ht="15.75" customHeight="1">
+    <row r="39" spans="1:25" s="31" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="26" t="s">
         <v>43</v>
       </c>
@@ -11316,7 +11349,7 @@
       <c r="X39" s="21"/>
       <c r="Y39" s="30"/>
     </row>
-    <row r="40" spans="1:25" s="48" customFormat="1" ht="15.75" customHeight="1">
+    <row r="40" spans="1:25" s="48" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="26" t="s">
         <v>43</v>
       </c>
@@ -11369,7 +11402,7 @@
       <c r="X40" s="21"/>
       <c r="Y40" s="47"/>
     </row>
-    <row r="41" spans="1:25" ht="15.75" customHeight="1">
+    <row r="41" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="26" t="s">
         <v>43</v>
       </c>
@@ -11424,7 +11457,7 @@
       <c r="X41" s="21"/>
       <c r="Y41" s="10"/>
     </row>
-    <row r="42" spans="1:25" ht="15.75" customHeight="1">
+    <row r="42" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="26" t="s">
         <v>43</v>
       </c>
@@ -11495,7 +11528,7 @@
       </c>
       <c r="Y42" s="10"/>
     </row>
-    <row r="43" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1">
+    <row r="43" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="26" t="s">
         <v>43</v>
       </c>
@@ -11568,7 +11601,7 @@
       </c>
       <c r="Y43" s="36"/>
     </row>
-    <row r="44" spans="1:25" ht="15.75" customHeight="1">
+    <row r="44" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="26" t="s">
         <v>43</v>
       </c>
@@ -11639,7 +11672,7 @@
       </c>
       <c r="Y44" s="10"/>
     </row>
-    <row r="45" spans="1:25" ht="15.75" customHeight="1">
+    <row r="45" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="26" t="s">
         <v>43</v>
       </c>
@@ -11710,7 +11743,7 @@
       </c>
       <c r="Y45" s="10"/>
     </row>
-    <row r="46" spans="1:25" ht="15.75" customHeight="1">
+    <row r="46" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="26" t="s">
         <v>43</v>
       </c>
@@ -11781,7 +11814,7 @@
       </c>
       <c r="Y46" s="10"/>
     </row>
-    <row r="47" spans="1:25" s="40" customFormat="1" ht="15.75" customHeight="1">
+    <row r="47" spans="1:25" s="40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="26" t="s">
         <v>43</v>
       </c>
@@ -11852,7 +11885,7 @@
       </c>
       <c r="Y47" s="39"/>
     </row>
-    <row r="48" spans="1:25" ht="15.75" customHeight="1">
+    <row r="48" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="26" t="s">
         <v>43</v>
       </c>
@@ -11923,7 +11956,7 @@
       </c>
       <c r="Y48" s="10"/>
     </row>
-    <row r="49" spans="1:25" ht="15.75" customHeight="1">
+    <row r="49" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="26" t="s">
         <v>43</v>
       </c>
@@ -11992,7 +12025,7 @@
       </c>
       <c r="Y49" s="10"/>
     </row>
-    <row r="50" spans="1:25" ht="15.75" customHeight="1">
+    <row r="50" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="26" t="s">
         <v>43</v>
       </c>
@@ -12063,7 +12096,7 @@
       </c>
       <c r="Y50" s="10"/>
     </row>
-    <row r="51" spans="1:25" ht="15.75" customHeight="1">
+    <row r="51" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="26" t="s">
         <v>43</v>
       </c>
@@ -12126,7 +12159,7 @@
       </c>
       <c r="Y51" s="10"/>
     </row>
-    <row r="52" spans="1:25" ht="15.75" customHeight="1">
+    <row r="52" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="26" t="s">
         <v>43</v>
       </c>
@@ -12183,7 +12216,7 @@
       <c r="X52" s="21"/>
       <c r="Y52" s="10"/>
     </row>
-    <row r="53" spans="1:25" ht="15.75" customHeight="1">
+    <row r="53" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="26" t="s">
         <v>43</v>
       </c>
@@ -12236,7 +12269,7 @@
       <c r="X53" s="21"/>
       <c r="Y53" s="10"/>
     </row>
-    <row r="54" spans="1:25" ht="15.75" customHeight="1">
+    <row r="54" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="26" t="s">
         <v>43</v>
       </c>
@@ -12289,7 +12322,7 @@
       <c r="X54" s="21"/>
       <c r="Y54" s="10"/>
     </row>
-    <row r="55" spans="1:25" ht="15.75" customHeight="1">
+    <row r="55" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="26" t="s">
         <v>43</v>
       </c>
@@ -12342,7 +12375,7 @@
       <c r="X55" s="21"/>
       <c r="Y55" s="10"/>
     </row>
-    <row r="56" spans="1:25" s="28" customFormat="1" ht="15.75" customHeight="1">
+    <row r="56" spans="1:25" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="26" t="s">
         <v>43</v>
       </c>
@@ -12411,7 +12444,7 @@
       </c>
       <c r="Y56" s="27"/>
     </row>
-    <row r="57" spans="1:25" s="48" customFormat="1" ht="15.75" customHeight="1">
+    <row r="57" spans="1:25" s="48" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="26" t="s">
         <v>43</v>
       </c>
@@ -12480,7 +12513,7 @@
       </c>
       <c r="Y57" s="47"/>
     </row>
-    <row r="58" spans="1:25" ht="15.75" customHeight="1">
+    <row r="58" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="26" t="s">
         <v>43</v>
       </c>
@@ -12551,7 +12584,7 @@
       </c>
       <c r="Y58" s="10"/>
     </row>
-    <row r="59" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1">
+    <row r="59" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="26" t="s">
         <v>43</v>
       </c>
@@ -12620,7 +12653,7 @@
       <c r="X59" s="21"/>
       <c r="Y59" s="36"/>
     </row>
-    <row r="60" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1">
+    <row r="60" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="26" t="s">
         <v>43</v>
       </c>
@@ -12689,7 +12722,7 @@
       <c r="X60" s="21"/>
       <c r="Y60" s="36"/>
     </row>
-    <row r="61" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1">
+    <row r="61" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="26" t="s">
         <v>43</v>
       </c>
@@ -12758,7 +12791,7 @@
       <c r="X61" s="21"/>
       <c r="Y61" s="36"/>
     </row>
-    <row r="62" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1">
+    <row r="62" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="26" t="s">
         <v>43</v>
       </c>
@@ -12827,7 +12860,7 @@
       <c r="X62" s="21"/>
       <c r="Y62" s="36"/>
     </row>
-    <row r="63" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1">
+    <row r="63" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="26" t="s">
         <v>43</v>
       </c>
@@ -12896,7 +12929,7 @@
       <c r="X63" s="21"/>
       <c r="Y63" s="36"/>
     </row>
-    <row r="64" spans="1:25" s="34" customFormat="1" ht="15.75" customHeight="1">
+    <row r="64" spans="1:25" s="34" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="26" t="s">
         <v>43</v>
       </c>
@@ -12947,7 +12980,7 @@
       <c r="X64" s="21"/>
       <c r="Y64" s="33"/>
     </row>
-    <row r="65" spans="1:25" ht="15.75" customHeight="1">
+    <row r="65" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="26" t="s">
         <v>58</v>
       </c>
@@ -13022,7 +13055,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="66" spans="1:25" ht="15.75" customHeight="1">
+    <row r="66" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="26" t="s">
         <v>58</v>
       </c>
@@ -13095,7 +13128,7 @@
       </c>
       <c r="Y66" s="52"/>
     </row>
-    <row r="67" spans="1:25" ht="15.75" customHeight="1">
+    <row r="67" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="26" t="s">
         <v>62</v>
       </c>
@@ -13168,7 +13201,7 @@
       </c>
       <c r="Y67" s="10"/>
     </row>
-    <row r="68" spans="1:25" s="15" customFormat="1" ht="15.75" customHeight="1">
+    <row r="68" spans="1:25" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="18" t="s">
         <v>63</v>
       </c>
@@ -13203,7 +13236,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="69" spans="1:25" ht="15.75" customHeight="1">
+    <row r="69" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="16" t="s">
         <v>63</v>
       </c>
@@ -13247,7 +13280,7 @@
       <c r="W69" s="17"/>
       <c r="X69" s="17"/>
     </row>
-    <row r="70" spans="1:25" ht="15.75" customHeight="1">
+    <row r="70" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="16" t="s">
         <v>63</v>
       </c>
@@ -13279,7 +13312,7 @@
       <c r="W70" s="17"/>
       <c r="X70" s="17"/>
     </row>
-    <row r="71" spans="1:25" ht="15.75" customHeight="1">
+    <row r="71" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="16" t="s">
         <v>63</v>
       </c>
@@ -13311,7 +13344,7 @@
       <c r="W71" s="17"/>
       <c r="X71" s="17"/>
     </row>
-    <row r="72" spans="1:25" ht="15.75" customHeight="1">
+    <row r="72" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="16" t="s">
         <v>63</v>
       </c>
@@ -13343,7 +13376,7 @@
       <c r="W72" s="17"/>
       <c r="X72" s="17"/>
     </row>
-    <row r="73" spans="1:25" s="45" customFormat="1" ht="15.75" customHeight="1">
+    <row r="73" spans="1:25" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="16" t="s">
         <v>63</v>
       </c>
@@ -13375,7 +13408,7 @@
       <c r="W73" s="17"/>
       <c r="X73" s="17"/>
     </row>
-    <row r="74" spans="1:25" s="35" customFormat="1" ht="15.75" customHeight="1">
+    <row r="74" spans="1:25" s="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="16" t="s">
         <v>63</v>
       </c>
@@ -13407,7 +13440,7 @@
       <c r="W74" s="17"/>
       <c r="X74" s="17"/>
     </row>
-    <row r="75" spans="1:25" s="32" customFormat="1" ht="15.75" customHeight="1">
+    <row r="75" spans="1:25" s="32" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="16" t="s">
         <v>63</v>
       </c>
@@ -13439,7 +13472,7 @@
       <c r="W75" s="17"/>
       <c r="X75" s="17"/>
     </row>
-    <row r="76" spans="1:25" ht="15.75" customHeight="1">
+    <row r="76" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="16" t="s">
         <v>109</v>
       </c>
@@ -13471,7 +13504,7 @@
       <c r="W76" s="20"/>
       <c r="X76" s="20"/>
     </row>
-    <row r="77" spans="1:25" ht="15.75" customHeight="1">
+    <row r="77" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77" s="16" t="s">
         <v>119</v>
       </c>
@@ -13527,19 +13560,22 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
-      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
+    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="C14" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="D35" sqref="D35"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
     <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
       <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C50" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="D69" sqref="D69"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
+      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>
@@ -13551,14 +13587,9 @@
     <mergeCell ref="C1:O1"/>
     <mergeCell ref="C2:O2"/>
   </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -13567,10 +13598,10 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="29.6640625" customWidth="1"/>
     <col min="2" max="2" width="28.1640625" customWidth="1"/>
@@ -13578,7 +13609,7 @@
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15">
+    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
         <v>70</v>
       </c>
@@ -13595,7 +13626,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15">
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
         <v>73</v>
       </c>
@@ -13608,7 +13639,7 @@
       <c r="D2" s="24"/>
       <c r="E2" s="24"/>
     </row>
-    <row r="3" spans="1:5" ht="15">
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
         <v>75</v>
       </c>
@@ -13621,7 +13652,7 @@
       <c r="D3" s="24"/>
       <c r="E3" s="24"/>
     </row>
-    <row r="4" spans="1:5" ht="15">
+    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
         <v>77</v>
       </c>
@@ -13634,7 +13665,7 @@
       <c r="D4" s="24"/>
       <c r="E4" s="24"/>
     </row>
-    <row r="5" spans="1:5" ht="15">
+    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
         <v>96</v>
       </c>
@@ -13649,7 +13680,7 @@
       </c>
       <c r="E5" s="24"/>
     </row>
-    <row r="6" spans="1:5" ht="15">
+    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
         <v>97</v>
       </c>
@@ -13664,7 +13695,7 @@
       </c>
       <c r="E6" s="24"/>
     </row>
-    <row r="7" spans="1:5" ht="15">
+    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
         <v>98</v>
       </c>
@@ -13679,7 +13710,7 @@
       </c>
       <c r="E7" s="24"/>
     </row>
-    <row r="8" spans="1:5" s="41" customFormat="1" ht="15">
+    <row r="8" spans="1:5" s="41" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
         <v>162</v>
       </c>
@@ -13694,7 +13725,7 @@
       </c>
       <c r="E8" s="24"/>
     </row>
-    <row r="9" spans="1:5" ht="15">
+    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
         <v>99</v>
       </c>
@@ -13709,7 +13740,7 @@
       </c>
       <c r="E9" s="24"/>
     </row>
-    <row r="10" spans="1:5" ht="15">
+    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
         <v>108</v>
       </c>
@@ -13722,7 +13753,7 @@
       <c r="D10" s="24"/>
       <c r="E10" s="24"/>
     </row>
-    <row r="11" spans="1:5" ht="15">
+    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
         <v>107</v>
       </c>
@@ -13735,7 +13766,7 @@
       <c r="D11" s="24"/>
       <c r="E11" s="24"/>
     </row>
-    <row r="12" spans="1:5" ht="15">
+    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
         <v>106</v>
       </c>
@@ -13748,7 +13779,7 @@
       <c r="D12" s="24"/>
       <c r="E12" s="24"/>
     </row>
-    <row r="13" spans="1:5" ht="15">
+    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="23" t="s">
         <v>100</v>
       </c>
@@ -13763,7 +13794,7 @@
       </c>
       <c r="E13" s="24"/>
     </row>
-    <row r="14" spans="1:5" ht="15">
+    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
         <v>105</v>
       </c>
@@ -13778,7 +13809,7 @@
       </c>
       <c r="E14" s="24"/>
     </row>
-    <row r="15" spans="1:5" ht="15">
+    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
         <v>101</v>
       </c>
@@ -13793,7 +13824,7 @@
       </c>
       <c r="E15" s="24"/>
     </row>
-    <row r="16" spans="1:5" s="41" customFormat="1" ht="15">
+    <row r="16" spans="1:5" s="41" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
         <v>161</v>
       </c>
@@ -13808,7 +13839,7 @@
       </c>
       <c r="E16" s="24"/>
     </row>
-    <row r="17" spans="1:5" ht="15">
+    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="23" t="s">
         <v>102</v>
       </c>
@@ -13823,7 +13854,7 @@
       </c>
       <c r="E17" s="24"/>
     </row>
-    <row r="18" spans="1:5" ht="15">
+    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
         <v>103</v>
       </c>
@@ -13838,7 +13869,7 @@
       </c>
       <c r="E18" s="24"/>
     </row>
-    <row r="19" spans="1:5" ht="15">
+    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="23" t="s">
         <v>122</v>
       </c>
@@ -13853,7 +13884,7 @@
       </c>
       <c r="E19" s="24"/>
     </row>
-    <row r="20" spans="1:5" ht="15">
+    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
         <v>12</v>
       </c>
@@ -13868,7 +13899,7 @@
       </c>
       <c r="E20" s="24"/>
     </row>
-    <row r="21" spans="1:5" ht="15">
+    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="23" t="s">
         <v>13</v>
       </c>
@@ -13883,7 +13914,7 @@
       </c>
       <c r="E21" s="24"/>
     </row>
-    <row r="22" spans="1:5" ht="15">
+    <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="23" t="s">
         <v>104</v>
       </c>
@@ -13900,25 +13931,23 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
-      <selection activeCell="B17" sqref="B17"/>
+    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}">
+      <selection activeCell="G36" sqref="G36"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
     <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
       <selection activeCell="C7" sqref="C7"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}">
-      <selection activeCell="G36" sqref="G36"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
+      <selection activeCell="B17" sqref="B17"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Käytä ääkkösiä maksuerien erikoisoikeuksissa
Koska yhteinen nimeämiskäytöntä
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="43600" windowHeight="19360" tabRatio="500"/>
+    <workbookView xWindow="1780" yWindow="1520" windowWidth="43600" windowHeight="18860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -17,9 +17,9 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="2180" windowHeight="866" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="2180" windowHeight="770" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
     <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -596,19 +596,19 @@
     <t>Kohdeluettelo / Maksuerät</t>
   </si>
   <si>
-    <t>R,W,maksuerat</t>
-  </si>
-  <si>
-    <t>R*,W,maksueratunnus</t>
-  </si>
-  <si>
-    <t>R+,W+,maksuerat</t>
-  </si>
-  <si>
-    <t>R*,W*,maksueratunnus</t>
-  </si>
-  <si>
-    <t>R*,W*,maksuerat,maksueratunnus</t>
+    <t>R*,W*,maksuerät,maksuerätunnus</t>
+  </si>
+  <si>
+    <t>R*,W,maksuerätunnus</t>
+  </si>
+  <si>
+    <t>R*,W*,maksuerätunnus</t>
+  </si>
+  <si>
+    <t>R+,W+,maksuerät</t>
+  </si>
+  <si>
+    <t>R,W,maksuerät</t>
   </si>
 </sst>
 </file>
@@ -1213,7 +1213,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{EA67C2AA-D5C4-9A49-8DF5-86A96AD16ED9}" diskRevisions="1" revisionId="390" version="47">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{CF2EB214-A1D0-0A48-BB84-067F19F3C965}" diskRevisions="1" revisionId="396" version="48">
   <header guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" dateTime="2016-09-06T09:14:56" maxSheetId="3" userName="Tatu Tarvainen" r:id="rId2" minRId="1" maxRId="3">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1490,6 +1490,12 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{CF2EB214-A1D0-0A48-BB84-067F19F3C965}" dateTime="2017-04-04T13:01:58" maxSheetId="3" userName="Microsoft Office User" r:id="rId48" minRId="391" maxRId="396">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -8109,6 +8115,85 @@
     <nc r="D34" t="inlineStr">
       <is>
         <t>R*,W*,maksuerat,maksueratunnus</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="delete"/>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog47.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="391" sId="1">
+    <oc r="D34" t="inlineStr">
+      <is>
+        <t>R*,W*,maksuerat,maksueratunnus</t>
+      </is>
+    </oc>
+    <nc r="D34" t="inlineStr">
+      <is>
+        <t>R*,W*,maksuerät,maksuerätunnus</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="392" sId="1">
+    <oc r="E34" t="inlineStr">
+      <is>
+        <t>R*,W,maksueratunnus</t>
+      </is>
+    </oc>
+    <nc r="E34" t="inlineStr">
+      <is>
+        <t>R*,W,maksuerätunnus</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="393" sId="1">
+    <oc r="K34" t="inlineStr">
+      <is>
+        <t>R*,W*,maksueratunnus</t>
+      </is>
+    </oc>
+    <nc r="K34" t="inlineStr">
+      <is>
+        <t>R*,W*,maksuerätunnus</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="394" sId="1">
+    <oc r="L34" t="inlineStr">
+      <is>
+        <t>R*,W,maksueratunnus</t>
+      </is>
+    </oc>
+    <nc r="L34" t="inlineStr">
+      <is>
+        <t>R*,W,maksuerätunnus</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="395" sId="1">
+    <oc r="R34" t="inlineStr">
+      <is>
+        <t>R+,W+,maksuerat</t>
+      </is>
+    </oc>
+    <nc r="R34" t="inlineStr">
+      <is>
+        <t>R+,W+,maksuerät</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="396" sId="1">
+    <oc r="S34" t="inlineStr">
+      <is>
+        <t>R,W,maksuerat</t>
+      </is>
+    </oc>
+    <nc r="S34" t="inlineStr">
+      <is>
+        <t>R,W,maksuerät</t>
       </is>
     </nc>
   </rcc>
@@ -9096,10 +9181,10 @@
   <dimension ref="A1:Y77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C14" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C19" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D35" sqref="D35"/>
+      <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -10983,7 +11068,7 @@
       </c>
       <c r="C34" s="21"/>
       <c r="D34" s="17" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E34" s="17" t="s">
         <v>177</v>
@@ -11002,7 +11087,7 @@
         <v>113</v>
       </c>
       <c r="K34" s="17" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L34" s="21" t="s">
         <v>177</v>
@@ -11019,10 +11104,10 @@
         <v>113</v>
       </c>
       <c r="R34" s="21" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="S34" s="21" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="T34" s="21" t="s">
         <v>131</v>
@@ -13561,20 +13646,20 @@
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C14" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="D35" sqref="D35"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C19" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
+      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
     <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
       <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
-      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -13936,13 +14021,13 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
-      <selection activeCell="C7" sqref="C7"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
+      <selection activeCell="B17" sqref="B17"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
-      <selection activeCell="B17" sqref="B17"/>
+    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
+      <selection activeCell="C7" sqref="C7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>

</xml_diff>

<commit_message>
Anna JVH:lle maksueränäkymään erikoisoikeus kaikkiin urakoihin
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1780" yWindow="1520" windowWidth="43600" windowHeight="18860" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="800" windowWidth="43600" windowHeight="16940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -17,9 +17,9 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="2180" windowHeight="770" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="2180" windowHeight="674" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
-    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -596,9 +596,6 @@
     <t>Kohdeluettelo / Maksuerät</t>
   </si>
   <si>
-    <t>R*,W*,maksuerät,maksuerätunnus</t>
-  </si>
-  <si>
     <t>R*,W,maksuerätunnus</t>
   </si>
   <si>
@@ -609,6 +606,9 @@
   </si>
   <si>
     <t>R,W,maksuerät</t>
+  </si>
+  <si>
+    <t>R*,W*,maksuerät*,maksuerätunnus*</t>
   </si>
 </sst>
 </file>
@@ -1213,7 +1213,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{CF2EB214-A1D0-0A48-BB84-067F19F3C965}" diskRevisions="1" revisionId="396" version="48">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{BB78E6C2-81A3-BD4F-8C39-7DD20054638D}" diskRevisions="1" revisionId="397" version="49">
   <header guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" dateTime="2016-09-06T09:14:56" maxSheetId="3" userName="Tatu Tarvainen" r:id="rId2" minRId="1" maxRId="3">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1496,6 +1496,12 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{BB78E6C2-81A3-BD4F-8C39-7DD20054638D}" dateTime="2017-04-04T13:32:43" maxSheetId="3" userName="Microsoft Office User" r:id="rId49" minRId="397">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -8194,6 +8200,25 @@
     <nc r="S34" t="inlineStr">
       <is>
         <t>R,W,maksuerät</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="delete"/>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog48.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="397" sId="1">
+    <oc r="D34" t="inlineStr">
+      <is>
+        <t>R*,W*,maksuerät,maksuerätunnus</t>
+      </is>
+    </oc>
+    <nc r="D34" t="inlineStr">
+      <is>
+        <t>R*,W*,maksuerät*,maksuerätunnus*</t>
       </is>
     </nc>
   </rcc>
@@ -9181,10 +9206,10 @@
   <dimension ref="A1:Y77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C19" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C20" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
+      <selection pane="bottomRight" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -11068,10 +11093,10 @@
       </c>
       <c r="C34" s="21"/>
       <c r="D34" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="E34" s="17" t="s">
         <v>176</v>
-      </c>
-      <c r="E34" s="17" t="s">
-        <v>177</v>
       </c>
       <c r="F34" s="21" t="s">
         <v>127</v>
@@ -11087,10 +11112,10 @@
         <v>113</v>
       </c>
       <c r="K34" s="17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L34" s="21" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M34" s="21"/>
       <c r="N34" s="21" t="s">
@@ -11104,10 +11129,10 @@
         <v>113</v>
       </c>
       <c r="R34" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="S34" s="21" t="s">
         <v>179</v>
-      </c>
-      <c r="S34" s="21" t="s">
-        <v>180</v>
       </c>
       <c r="T34" s="21" t="s">
         <v>131</v>
@@ -13646,20 +13671,20 @@
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C19" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C20" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="D26" sqref="D26"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
+      <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
     <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
       <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
-      <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -14021,13 +14046,13 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
-      <selection activeCell="B17" sqref="B17"/>
+    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
+      <selection activeCell="C7" sqref="C7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
-      <selection activeCell="C7" sqref="C7"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
+      <selection activeCell="B17" sqref="B17"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>

</xml_diff>

<commit_message>
Oikeudet eivät voi olla kolmessa tasossa
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -9,17 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="43600" windowHeight="15020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="15380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
     <sheet name="Roolit" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$83</definedName>
+    <definedName name="Z_7A9649F2_657F_9445_B6E6_FE94C6A09957_.wvu.FilterData" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$83</definedName>
+  </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="2180" windowHeight="578" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="596" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
-    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -66,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1302" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1317" uniqueCount="187">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -612,6 +616,21 @@
   </si>
   <si>
     <t>Vesiväylät</t>
+  </si>
+  <si>
+    <t>Vesiväylätoimenpiteet / Kokonaishintaiset</t>
+  </si>
+  <si>
+    <t>Vesiväylätoimenpiteet / Yksikköhintaiset</t>
+  </si>
+  <si>
+    <t>Vesiväylälaadunseuranta / Sanktiot</t>
+  </si>
+  <si>
+    <t>Vesiväylä / Turvalaitteet</t>
+  </si>
+  <si>
+    <t>Vesiväylälaadunseuranta / Viat</t>
   </si>
 </sst>
 </file>
@@ -923,7 +942,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -1013,6 +1032,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1217,7 +1240,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{88D4547C-A4BB-3843-ABD6-020023F84CCA}" diskRevisions="1" revisionId="401" version="50">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{084BE7CF-27AE-7F41-8749-56DF6A95DCBA}" diskRevisions="1" revisionId="437" version="56">
   <header guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" dateTime="2016-09-06T09:14:56" maxSheetId="3" userName="Tatu Tarvainen" r:id="rId2" minRId="1" maxRId="3">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1512,6 +1535,42 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{2A3C1768-5A6C-F54A-9706-235E6C37C69A}" dateTime="2017-05-08T12:22:39" maxSheetId="3" userName="Microsoft Office User" r:id="rId51" minRId="402" maxRId="417">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{F5607BA9-8194-A34F-8708-244DCBB6E78D}" dateTime="2017-05-08T12:30:36" maxSheetId="3" userName="Microsoft Office User" r:id="rId52" minRId="419" maxRId="423">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{49EFA7EF-02CD-D544-BC84-4A84D4318CBC}" dateTime="2017-05-08T12:31:27" maxSheetId="3" userName="Microsoft Office User" r:id="rId53" minRId="425">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{29D41E1A-269D-AF4B-AFC8-7844773F57C6}" dateTime="2017-05-08T13:07:40" maxSheetId="3" userName="Microsoft Office User" r:id="rId54" minRId="426" maxRId="427">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{06DC6EEF-37B9-1D49-8D4D-C0FD1057F30B}" dateTime="2017-05-08T13:15:50" maxSheetId="3" userName="Microsoft Office User" r:id="rId55" minRId="428" maxRId="430">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{084BE7CF-27AE-7F41-8749-56DF6A95DCBA}" dateTime="2017-05-08T13:37:31" maxSheetId="3" userName="Microsoft Office User" r:id="rId56" minRId="432" maxRId="436">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -8816,6 +8875,357 @@
   </rcc>
   <rcv guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" action="delete"/>
   <rcv guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog50.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="402" sId="1" ref="A39:XFD43" action="insertRow"/>
+  <rcc rId="403" sId="1">
+    <nc r="A39" t="inlineStr">
+      <is>
+        <t>Urakat</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="404" sId="1">
+    <nc r="B39" t="inlineStr">
+      <is>
+        <t>Vesivaylat / Toimenpiteet / Kokonaishintaiset</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="405" sId="1">
+    <nc r="D39" t="inlineStr">
+      <is>
+        <t>R*,W*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="406" sId="1">
+    <nc r="A40" t="inlineStr">
+      <is>
+        <t>Urakat</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="407" sId="1">
+    <nc r="B40" t="inlineStr">
+      <is>
+        <t>Vesivaylat / Toimenpiteet / Yksikköhintaiset</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="408" sId="1">
+    <nc r="D40" t="inlineStr">
+      <is>
+        <t>R*,W*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="409" sId="1">
+    <nc r="A41" t="inlineStr">
+      <is>
+        <t>Urakat</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="410" sId="1">
+    <nc r="B41" t="inlineStr">
+      <is>
+        <t>Vesivaylat / Laadunseuranta / Viat</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="411" sId="1">
+    <nc r="D41" t="inlineStr">
+      <is>
+        <t>R*,W*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="412" sId="1">
+    <nc r="A42" t="inlineStr">
+      <is>
+        <t>Urakat</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="413" sId="1">
+    <nc r="B42" t="inlineStr">
+      <is>
+        <t>Vesivaylat / Laadunseuranta / Sanktiot</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="414" sId="1">
+    <nc r="D42" t="inlineStr">
+      <is>
+        <t>R*,W*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="415" sId="1">
+    <nc r="A43" t="inlineStr">
+      <is>
+        <t>Urakat</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="416" sId="1">
+    <nc r="B43" t="inlineStr">
+      <is>
+        <t>Vesivaylat / Turvalaitteet</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="417" sId="1">
+    <nc r="D43" t="inlineStr">
+      <is>
+        <t>R*,W*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="delete"/>
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_7A9649F2_657F_9445_B6E6_FE94C6A09957_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Oikeudet!$A$5:$Y$83</formula>
+  </rdn>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog51.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="419" sId="1">
+    <oc r="B41" t="inlineStr">
+      <is>
+        <t>Vesivaylat / Laadunseuranta / Viat</t>
+      </is>
+    </oc>
+    <nc r="B41" t="inlineStr">
+      <is>
+        <t>Vesiväylälaadunseuranta / Viat</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="420" sId="1">
+    <oc r="B39" t="inlineStr">
+      <is>
+        <t>Vesivaylat / Toimenpiteet / Kokonaishintaiset</t>
+      </is>
+    </oc>
+    <nc r="B39" t="inlineStr">
+      <is>
+        <t>Vesiväylätoimenpiteet / Kokonaishintaiset</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="421" sId="1">
+    <oc r="B40" t="inlineStr">
+      <is>
+        <t>Vesivaylat / Toimenpiteet / Yksikköhintaiset</t>
+      </is>
+    </oc>
+    <nc r="B40" t="inlineStr">
+      <is>
+        <t>Vesiväylätoimenpiteet / Yksikköhintaiset</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="422" sId="1">
+    <oc r="B42" t="inlineStr">
+      <is>
+        <t>Vesivaylat / Laadunseuranta / Sanktiot</t>
+      </is>
+    </oc>
+    <nc r="B42" t="inlineStr">
+      <is>
+        <t>Vesiväylälaadunseuranta / Sanktiot</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="423" sId="1">
+    <oc r="B43" t="inlineStr">
+      <is>
+        <t>Vesivaylat / Turvalaitteet</t>
+      </is>
+    </oc>
+    <nc r="B43" t="inlineStr">
+      <is>
+        <t>Vesiväylät / Turvalaitteet</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="delete"/>
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_7A9649F2_657F_9445_B6E6_FE94C6A09957_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Oikeudet!$A$5:$Y$83</formula>
+    <oldFormula>Oikeudet!$A$5:$Y$83</oldFormula>
+  </rdn>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog52.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="425" sId="1">
+    <oc r="B43" t="inlineStr">
+      <is>
+        <t>Vesiväylät / Turvalaitteet</t>
+      </is>
+    </oc>
+    <nc r="B43" t="inlineStr">
+      <is>
+        <t>Vesiväylä / Turvalaitteet</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog53.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="426" sId="1">
+    <oc r="B39" t="inlineStr">
+      <is>
+        <t>Vesiväylätoimenpiteet / Kokonaishintaiset</t>
+      </is>
+    </oc>
+    <nc r="B39" t="inlineStr">
+      <is>
+        <t>Vesiväylät / Toimenpiteet / Kokonaishintaiset</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="427" sId="1">
+    <oc r="B40" t="inlineStr">
+      <is>
+        <t>Vesiväylätoimenpiteet / Yksikköhintaiset</t>
+      </is>
+    </oc>
+    <nc r="B40" t="inlineStr">
+      <is>
+        <t>Vesiväylät / Toimenpiteet / Yksikköhintaiset</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog54.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="428" sId="1">
+    <oc r="B41" t="inlineStr">
+      <is>
+        <t>Vesiväylälaadunseuranta / Viat</t>
+      </is>
+    </oc>
+    <nc r="B41" t="inlineStr">
+      <is>
+        <t>Vesiväylät / Laadunseuranta / Viat</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="429" sId="1">
+    <oc r="B42" t="inlineStr">
+      <is>
+        <t>Vesiväylälaadunseuranta / Sanktiot</t>
+      </is>
+    </oc>
+    <nc r="B42" t="inlineStr">
+      <is>
+        <t>Vesiväylät / Laadunseuranta / Sanktiot</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="430" sId="1">
+    <oc r="B43" t="inlineStr">
+      <is>
+        <t>Vesiväylä / Turvalaitteet</t>
+      </is>
+    </oc>
+    <nc r="B43" t="inlineStr">
+      <is>
+        <t>Vesiväylät / Turvalaitteet</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="delete"/>
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_7A9649F2_657F_9445_B6E6_FE94C6A09957_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Oikeudet!$A$5:$Y$83</formula>
+    <oldFormula>Oikeudet!$A$5:$Y$83</oldFormula>
+  </rdn>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog55.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="432" sId="1">
+    <oc r="B39" t="inlineStr">
+      <is>
+        <t>Vesiväylät / Toimenpiteet / Kokonaishintaiset</t>
+      </is>
+    </oc>
+    <nc r="B39" t="inlineStr">
+      <is>
+        <t>Vesiväylätoimenpiteet / Kokonaishintaiset</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="433" sId="1">
+    <oc r="B40" t="inlineStr">
+      <is>
+        <t>Vesiväylät / Toimenpiteet / Yksikköhintaiset</t>
+      </is>
+    </oc>
+    <nc r="B40" t="inlineStr">
+      <is>
+        <t>Vesiväylätoimenpiteet / Yksikköhintaiset</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="434" sId="1">
+    <oc r="B42" t="inlineStr">
+      <is>
+        <t>Vesiväylät / Laadunseuranta / Sanktiot</t>
+      </is>
+    </oc>
+    <nc r="B42" t="inlineStr">
+      <is>
+        <t>Vesiväylälaadunseuranta / Sanktiot</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="435" sId="1">
+    <oc r="B43" t="inlineStr">
+      <is>
+        <t>Vesiväylät / Turvalaitteet</t>
+      </is>
+    </oc>
+    <nc r="B43" t="inlineStr">
+      <is>
+        <t>Vesiväylä / Turvalaitteet</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="436" sId="1">
+    <oc r="B41" t="inlineStr">
+      <is>
+        <t>Vesiväylät / Laadunseuranta / Viat</t>
+      </is>
+    </oc>
+    <nc r="B41" t="inlineStr">
+      <is>
+        <t>Vesiväylälaadunseuranta / Viat</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="delete"/>
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_7A9649F2_657F_9445_B6E6_FE94C6A09957_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Oikeudet!$A$5:$Y$83</formula>
+    <oldFormula>Oikeudet!$A$5:$Y$83</oldFormula>
+  </rdn>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="add"/>
 </revisions>
 </file>
 
@@ -9244,13 +9654,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y78"/>
+  <dimension ref="A1:Y83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C67" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C33" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D75" sqref="D75"/>
+      <selection pane="bottomRight" activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9286,40 +9696,40 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="55" t="s">
+      <c r="C1" s="57" t="s">
         <v>151</v>
       </c>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
     </row>
     <row r="3" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
@@ -9340,30 +9750,30 @@
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C5" s="54" t="s">
+      <c r="C5" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="53"/>
-      <c r="K5" s="54" t="s">
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="55"/>
+      <c r="K5" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="L5" s="53"/>
-      <c r="M5" s="53"/>
-      <c r="N5" s="53"/>
-      <c r="O5" s="53"/>
-      <c r="R5" s="54" t="s">
+      <c r="L5" s="55"/>
+      <c r="M5" s="55"/>
+      <c r="N5" s="55"/>
+      <c r="O5" s="55"/>
+      <c r="R5" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="S5" s="53"/>
-      <c r="T5" s="53"/>
-      <c r="U5" s="53"/>
-      <c r="V5" s="53"/>
-      <c r="W5" s="53"/>
-      <c r="X5" s="53"/>
+      <c r="S5" s="55"/>
+      <c r="T5" s="55"/>
+      <c r="U5" s="55"/>
+      <c r="V5" s="55"/>
+      <c r="W5" s="55"/>
+      <c r="X5" s="55"/>
       <c r="Y5" s="5" t="s">
         <v>14</v>
       </c>
@@ -11447,337 +11857,191 @@
       </c>
       <c r="Y38" s="12"/>
     </row>
-    <row r="39" spans="1:25" s="31" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:25" s="53" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="26" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>123</v>
+        <v>182</v>
       </c>
       <c r="C39" s="21"/>
       <c r="D39" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="E39" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="F39" s="21" t="s">
-        <v>127</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="E39" s="17"/>
+      <c r="F39" s="21"/>
       <c r="G39" s="21"/>
       <c r="H39" s="21"/>
       <c r="I39" s="21"/>
-      <c r="J39" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="K39" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="L39" s="21" t="s">
-        <v>127</v>
-      </c>
+      <c r="J39" s="21"/>
+      <c r="K39" s="17"/>
+      <c r="L39" s="21"/>
       <c r="M39" s="21"/>
-      <c r="N39" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="O39" s="21"/>
-      <c r="P39" s="21"/>
-      <c r="Q39" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="R39" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="S39" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="N39" s="21"/>
+      <c r="O39" s="17"/>
+      <c r="P39" s="17"/>
+      <c r="Q39" s="21"/>
+      <c r="R39" s="21"/>
+      <c r="S39" s="21"/>
       <c r="T39" s="21"/>
       <c r="U39" s="21"/>
-      <c r="V39" s="21" t="s">
-        <v>131</v>
-      </c>
+      <c r="V39" s="17"/>
       <c r="W39" s="21"/>
       <c r="X39" s="21"/>
-      <c r="Y39" s="30"/>
+      <c r="Y39" s="52"/>
     </row>
-    <row r="40" spans="1:25" s="48" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:25" s="53" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="26" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="C40" s="21"/>
       <c r="D40" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="E40" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="F40" s="21" t="s">
-        <v>127</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="E40" s="17"/>
+      <c r="F40" s="21"/>
       <c r="G40" s="21"/>
       <c r="H40" s="21"/>
       <c r="I40" s="21"/>
-      <c r="J40" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="K40" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="L40" s="21" t="s">
-        <v>127</v>
-      </c>
+      <c r="J40" s="21"/>
+      <c r="K40" s="17"/>
+      <c r="L40" s="21"/>
       <c r="M40" s="21"/>
-      <c r="N40" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="O40" s="21"/>
-      <c r="P40" s="21"/>
-      <c r="Q40" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="R40" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="S40" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="N40" s="21"/>
+      <c r="O40" s="17"/>
+      <c r="P40" s="17"/>
+      <c r="Q40" s="21"/>
+      <c r="R40" s="21"/>
+      <c r="S40" s="21"/>
       <c r="T40" s="21"/>
       <c r="U40" s="21"/>
-      <c r="V40" s="21" t="s">
-        <v>131</v>
-      </c>
+      <c r="V40" s="17"/>
       <c r="W40" s="21"/>
       <c r="X40" s="21"/>
-      <c r="Y40" s="47"/>
+      <c r="Y40" s="52"/>
     </row>
-    <row r="41" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:25" s="53" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="26" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>44</v>
+        <v>186</v>
       </c>
       <c r="C41" s="21"/>
-      <c r="D41" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="E41" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="F41" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="G41" s="21" t="s">
-        <v>19</v>
-      </c>
+      <c r="D41" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="E41" s="17"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="21"/>
       <c r="H41" s="21"/>
       <c r="I41" s="21"/>
-      <c r="J41" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="K41" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="L41" s="21" t="s">
-        <v>127</v>
-      </c>
+      <c r="J41" s="21"/>
+      <c r="K41" s="17"/>
+      <c r="L41" s="21"/>
       <c r="M41" s="21"/>
-      <c r="N41" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="O41" s="21"/>
-      <c r="P41" s="21"/>
-      <c r="Q41" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="R41" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="S41" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="N41" s="21"/>
+      <c r="O41" s="17"/>
+      <c r="P41" s="17"/>
+      <c r="Q41" s="21"/>
+      <c r="R41" s="21"/>
+      <c r="S41" s="21"/>
       <c r="T41" s="21"/>
       <c r="U41" s="21"/>
-      <c r="V41" s="21" t="s">
-        <v>131</v>
-      </c>
+      <c r="V41" s="17"/>
       <c r="W41" s="21"/>
       <c r="X41" s="21"/>
-      <c r="Y41" s="10"/>
+      <c r="Y41" s="52"/>
     </row>
-    <row r="42" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:25" s="53" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="26" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="B42" s="26" t="s">
-        <v>45</v>
+        <v>184</v>
       </c>
       <c r="C42" s="21"/>
-      <c r="D42" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="E42" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="F42" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="G42" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="H42" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="I42" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="J42" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="K42" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="L42" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="M42" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="N42" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="O42" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="P42" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q42" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="R42" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="S42" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="T42" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="U42" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="V42" s="21" t="s">
-        <v>131</v>
-      </c>
+      <c r="D42" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="E42" s="17"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="21"/>
+      <c r="H42" s="21"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
+      <c r="K42" s="17"/>
+      <c r="L42" s="21"/>
+      <c r="M42" s="21"/>
+      <c r="N42" s="21"/>
+      <c r="O42" s="17"/>
+      <c r="P42" s="17"/>
+      <c r="Q42" s="21"/>
+      <c r="R42" s="21"/>
+      <c r="S42" s="21"/>
+      <c r="T42" s="21"/>
+      <c r="U42" s="21"/>
+      <c r="V42" s="17"/>
       <c r="W42" s="21"/>
-      <c r="X42" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y42" s="10"/>
+      <c r="X42" s="21"/>
+      <c r="Y42" s="52"/>
     </row>
-    <row r="43" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:25" s="53" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="26" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>46</v>
+        <v>185</v>
       </c>
       <c r="C43" s="21"/>
-      <c r="D43" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="E43" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="F43" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="G43" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="H43" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="I43" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="J43" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="K43" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="L43" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="M43" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="N43" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="O43" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="P43" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q43" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="R43" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="S43" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="T43" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="U43" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="V43" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="W43" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="X43" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y43" s="36"/>
+      <c r="D43" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="E43" s="17"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="21"/>
+      <c r="H43" s="21"/>
+      <c r="I43" s="21"/>
+      <c r="J43" s="21"/>
+      <c r="K43" s="17"/>
+      <c r="L43" s="21"/>
+      <c r="M43" s="21"/>
+      <c r="N43" s="21"/>
+      <c r="O43" s="17"/>
+      <c r="P43" s="17"/>
+      <c r="Q43" s="21"/>
+      <c r="R43" s="21"/>
+      <c r="S43" s="21"/>
+      <c r="T43" s="21"/>
+      <c r="U43" s="21"/>
+      <c r="V43" s="17"/>
+      <c r="W43" s="21"/>
+      <c r="X43" s="21"/>
+      <c r="Y43" s="52"/>
     </row>
-    <row r="44" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:25" s="31" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B44" s="26" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="C44" s="21"/>
-      <c r="D44" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="E44" s="21" t="s">
+      <c r="D44" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="E44" s="17" t="s">
         <v>127</v>
       </c>
       <c r="F44" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="G44" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="H44" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="I44" s="21" t="s">
-        <v>127</v>
-      </c>
+      <c r="G44" s="21"/>
+      <c r="H44" s="21"/>
+      <c r="I44" s="21"/>
       <c r="J44" s="21" t="s">
         <v>17</v>
       </c>
@@ -11787,18 +12051,12 @@
       <c r="L44" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="M44" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="M44" s="21"/>
       <c r="N44" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="O44" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="P44" s="21" t="s">
-        <v>127</v>
-      </c>
+      <c r="O44" s="21"/>
+      <c r="P44" s="21"/>
       <c r="Q44" s="21" t="s">
         <v>17</v>
       </c>
@@ -11808,47 +12066,35 @@
       <c r="S44" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="T44" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="U44" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="T44" s="21"/>
+      <c r="U44" s="21"/>
       <c r="V44" s="21" t="s">
         <v>131</v>
       </c>
       <c r="W44" s="21"/>
-      <c r="X44" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y44" s="10"/>
+      <c r="X44" s="21"/>
+      <c r="Y44" s="30"/>
     </row>
-    <row r="45" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:25" s="48" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B45" s="26" t="s">
-        <v>47</v>
+        <v>172</v>
       </c>
       <c r="C45" s="21"/>
-      <c r="D45" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="E45" s="21" t="s">
+      <c r="D45" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="E45" s="17" t="s">
         <v>127</v>
       </c>
       <c r="F45" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="G45" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="H45" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="I45" s="21" t="s">
-        <v>127</v>
-      </c>
+      <c r="G45" s="21"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="21"/>
       <c r="J45" s="21" t="s">
         <v>17</v>
       </c>
@@ -11858,18 +12104,12 @@
       <c r="L45" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="M45" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="M45" s="21"/>
       <c r="N45" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="O45" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="P45" s="21" t="s">
-        <v>127</v>
-      </c>
+      <c r="O45" s="21"/>
+      <c r="P45" s="21"/>
       <c r="Q45" s="21" t="s">
         <v>17</v>
       </c>
@@ -11879,27 +12119,21 @@
       <c r="S45" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="T45" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="U45" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="T45" s="21"/>
+      <c r="U45" s="21"/>
       <c r="V45" s="21" t="s">
         <v>131</v>
       </c>
       <c r="W45" s="21"/>
-      <c r="X45" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y45" s="10"/>
+      <c r="X45" s="21"/>
+      <c r="Y45" s="47"/>
     </row>
     <row r="46" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B46" s="26" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C46" s="21"/>
       <c r="D46" s="21" t="s">
@@ -11912,14 +12146,10 @@
         <v>127</v>
       </c>
       <c r="G46" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="H46" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="I46" s="21" t="s">
-        <v>127</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="H46" s="21"/>
+      <c r="I46" s="21"/>
       <c r="J46" s="21" t="s">
         <v>17</v>
       </c>
@@ -11929,18 +12159,12 @@
       <c r="L46" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="M46" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="M46" s="21"/>
       <c r="N46" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="O46" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="P46" s="21" t="s">
-        <v>127</v>
-      </c>
+      <c r="O46" s="21"/>
+      <c r="P46" s="21"/>
       <c r="Q46" s="21" t="s">
         <v>17</v>
       </c>
@@ -11950,27 +12174,21 @@
       <c r="S46" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="T46" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="U46" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="T46" s="21"/>
+      <c r="U46" s="21"/>
       <c r="V46" s="21" t="s">
         <v>131</v>
       </c>
       <c r="W46" s="21"/>
-      <c r="X46" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="X46" s="21"/>
       <c r="Y46" s="10"/>
     </row>
-    <row r="47" spans="1:25" s="40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B47" s="26" t="s">
-        <v>155</v>
+        <v>45</v>
       </c>
       <c r="C47" s="21"/>
       <c r="D47" s="21" t="s">
@@ -12034,14 +12252,14 @@
       <c r="X47" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="Y47" s="39"/>
+      <c r="Y47" s="10"/>
     </row>
-    <row r="48" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B48" s="26" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C48" s="21"/>
       <c r="D48" s="21" t="s">
@@ -12101,18 +12319,20 @@
       <c r="V48" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="W48" s="21"/>
+      <c r="W48" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="X48" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="Y48" s="10"/>
+      <c r="Y48" s="36"/>
     </row>
     <row r="49" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B49" s="26" t="s">
-        <v>50</v>
+        <v>148</v>
       </c>
       <c r="C49" s="21"/>
       <c r="D49" s="21" t="s">
@@ -12148,7 +12368,9 @@
       <c r="N49" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="O49" s="21"/>
+      <c r="O49" s="21" t="s">
+        <v>127</v>
+      </c>
       <c r="P49" s="21" t="s">
         <v>127</v>
       </c>
@@ -12181,7 +12403,7 @@
         <v>43</v>
       </c>
       <c r="B50" s="26" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C50" s="21"/>
       <c r="D50" s="21" t="s">
@@ -12252,7 +12474,7 @@
         <v>43</v>
       </c>
       <c r="B51" s="26" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C51" s="21"/>
       <c r="D51" s="21" t="s">
@@ -12264,8 +12486,12 @@
       <c r="F51" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="G51" s="21"/>
-      <c r="H51" s="21"/>
+      <c r="G51" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="H51" s="21" t="s">
+        <v>127</v>
+      </c>
       <c r="I51" s="21" t="s">
         <v>127</v>
       </c>
@@ -12278,11 +12504,15 @@
       <c r="L51" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="M51" s="21"/>
+      <c r="M51" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="N51" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="O51" s="21"/>
+      <c r="O51" s="21" t="s">
+        <v>127</v>
+      </c>
       <c r="P51" s="21" t="s">
         <v>127</v>
       </c>
@@ -12310,12 +12540,12 @@
       </c>
       <c r="Y51" s="10"/>
     </row>
-    <row r="52" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:25" s="40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B52" s="26" t="s">
-        <v>53</v>
+        <v>155</v>
       </c>
       <c r="C52" s="21"/>
       <c r="D52" s="21" t="s">
@@ -12327,11 +12557,15 @@
       <c r="F52" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="G52" s="21"/>
+      <c r="G52" s="21" t="s">
+        <v>127</v>
+      </c>
       <c r="H52" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="I52" s="21"/>
+        <v>127</v>
+      </c>
+      <c r="I52" s="21" t="s">
+        <v>127</v>
+      </c>
       <c r="J52" s="21" t="s">
         <v>17</v>
       </c>
@@ -12341,14 +12575,18 @@
       <c r="L52" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="M52" s="21"/>
+      <c r="M52" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="N52" s="21" t="s">
         <v>127</v>
       </c>
       <c r="O52" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="P52" s="21"/>
+        <v>127</v>
+      </c>
+      <c r="P52" s="21" t="s">
+        <v>127</v>
+      </c>
       <c r="Q52" s="21" t="s">
         <v>17</v>
       </c>
@@ -12358,21 +12596,27 @@
       <c r="S52" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="T52" s="21"/>
-      <c r="U52" s="21"/>
+      <c r="T52" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="U52" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="V52" s="21" t="s">
         <v>131</v>
       </c>
       <c r="W52" s="21"/>
-      <c r="X52" s="21"/>
-      <c r="Y52" s="10"/>
+      <c r="X52" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y52" s="39"/>
     </row>
     <row r="53" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B53" s="26" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C53" s="21"/>
       <c r="D53" s="21" t="s">
@@ -12384,9 +12628,15 @@
       <c r="F53" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="G53" s="21"/>
-      <c r="H53" s="21"/>
-      <c r="I53" s="21"/>
+      <c r="G53" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="H53" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="I53" s="21" t="s">
+        <v>127</v>
+      </c>
       <c r="J53" s="21" t="s">
         <v>17</v>
       </c>
@@ -12396,12 +12646,18 @@
       <c r="L53" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="M53" s="21"/>
+      <c r="M53" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="N53" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="O53" s="21"/>
-      <c r="P53" s="21"/>
+      <c r="O53" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="P53" s="21" t="s">
+        <v>127</v>
+      </c>
       <c r="Q53" s="21" t="s">
         <v>17</v>
       </c>
@@ -12411,13 +12667,19 @@
       <c r="S53" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="T53" s="21"/>
-      <c r="U53" s="21"/>
+      <c r="T53" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="U53" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="V53" s="21" t="s">
         <v>131</v>
       </c>
       <c r="W53" s="21"/>
-      <c r="X53" s="21"/>
+      <c r="X53" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="Y53" s="10"/>
     </row>
     <row r="54" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -12425,7 +12687,7 @@
         <v>43</v>
       </c>
       <c r="B54" s="26" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C54" s="21"/>
       <c r="D54" s="21" t="s">
@@ -12437,9 +12699,15 @@
       <c r="F54" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="G54" s="21"/>
-      <c r="H54" s="21"/>
-      <c r="I54" s="21"/>
+      <c r="G54" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="H54" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="I54" s="21" t="s">
+        <v>127</v>
+      </c>
       <c r="J54" s="21" t="s">
         <v>17</v>
       </c>
@@ -12449,12 +12717,16 @@
       <c r="L54" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="M54" s="21"/>
+      <c r="M54" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="N54" s="21" t="s">
         <v>127</v>
       </c>
       <c r="O54" s="21"/>
-      <c r="P54" s="21"/>
+      <c r="P54" s="21" t="s">
+        <v>127</v>
+      </c>
       <c r="Q54" s="21" t="s">
         <v>17</v>
       </c>
@@ -12464,13 +12736,19 @@
       <c r="S54" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="T54" s="21"/>
-      <c r="U54" s="21"/>
+      <c r="T54" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="U54" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="V54" s="21" t="s">
         <v>131</v>
       </c>
       <c r="W54" s="21"/>
-      <c r="X54" s="21"/>
+      <c r="X54" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="Y54" s="10"/>
     </row>
     <row r="55" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -12478,7 +12756,7 @@
         <v>43</v>
       </c>
       <c r="B55" s="26" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C55" s="21"/>
       <c r="D55" s="21" t="s">
@@ -12490,9 +12768,15 @@
       <c r="F55" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="G55" s="21"/>
-      <c r="H55" s="21"/>
-      <c r="I55" s="21"/>
+      <c r="G55" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="H55" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="I55" s="21" t="s">
+        <v>127</v>
+      </c>
       <c r="J55" s="21" t="s">
         <v>17</v>
       </c>
@@ -12502,12 +12786,18 @@
       <c r="L55" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="M55" s="21"/>
+      <c r="M55" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="N55" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="O55" s="21"/>
-      <c r="P55" s="21"/>
+      <c r="O55" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="P55" s="21" t="s">
+        <v>127</v>
+      </c>
       <c r="Q55" s="21" t="s">
         <v>17</v>
       </c>
@@ -12517,21 +12807,27 @@
       <c r="S55" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="T55" s="21"/>
-      <c r="U55" s="21"/>
+      <c r="T55" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="U55" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="V55" s="21" t="s">
         <v>131</v>
       </c>
       <c r="W55" s="21"/>
-      <c r="X55" s="21"/>
+      <c r="X55" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="Y55" s="10"/>
     </row>
-    <row r="56" spans="1:25" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B56" s="26" t="s">
-        <v>121</v>
+        <v>52</v>
       </c>
       <c r="C56" s="21"/>
       <c r="D56" s="21" t="s">
@@ -12543,12 +12839,8 @@
       <c r="F56" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="G56" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="H56" s="21" t="s">
-        <v>127</v>
-      </c>
+      <c r="G56" s="21"/>
+      <c r="H56" s="21"/>
       <c r="I56" s="21" t="s">
         <v>127</v>
       </c>
@@ -12561,9 +12853,7 @@
       <c r="L56" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="M56" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="M56" s="21"/>
       <c r="N56" s="21" t="s">
         <v>127</v>
       </c>
@@ -12593,14 +12883,14 @@
       <c r="X56" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="Y56" s="27"/>
+      <c r="Y56" s="10"/>
     </row>
-    <row r="57" spans="1:25" s="48" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B57" s="26" t="s">
-        <v>173</v>
+        <v>53</v>
       </c>
       <c r="C57" s="21"/>
       <c r="D57" s="21" t="s">
@@ -12612,15 +12902,11 @@
       <c r="F57" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="G57" s="21" t="s">
-        <v>127</v>
-      </c>
+      <c r="G57" s="21"/>
       <c r="H57" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="I57" s="21" t="s">
-        <v>127</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="I57" s="21"/>
       <c r="J57" s="21" t="s">
         <v>17</v>
       </c>
@@ -12630,16 +12916,14 @@
       <c r="L57" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="M57" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="M57" s="21"/>
       <c r="N57" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="O57" s="21"/>
-      <c r="P57" s="21" t="s">
-        <v>127</v>
-      </c>
+      <c r="O57" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="P57" s="21"/>
       <c r="Q57" s="21" t="s">
         <v>17</v>
       </c>
@@ -12649,27 +12933,21 @@
       <c r="S57" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="T57" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="U57" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="T57" s="21"/>
+      <c r="U57" s="21"/>
       <c r="V57" s="21" t="s">
         <v>131</v>
       </c>
       <c r="W57" s="21"/>
-      <c r="X57" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y57" s="47"/>
+      <c r="X57" s="21"/>
+      <c r="Y57" s="10"/>
     </row>
     <row r="58" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B58" s="26" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C58" s="21"/>
       <c r="D58" s="21" t="s">
@@ -12681,15 +12959,9 @@
       <c r="F58" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="G58" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="H58" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="I58" s="21" t="s">
-        <v>127</v>
-      </c>
+      <c r="G58" s="21"/>
+      <c r="H58" s="21"/>
+      <c r="I58" s="21"/>
       <c r="J58" s="21" t="s">
         <v>17</v>
       </c>
@@ -12699,18 +12971,12 @@
       <c r="L58" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="M58" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="M58" s="21"/>
       <c r="N58" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="O58" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="P58" s="21" t="s">
-        <v>127</v>
-      </c>
+      <c r="O58" s="21"/>
+      <c r="P58" s="21"/>
       <c r="Q58" s="21" t="s">
         <v>17</v>
       </c>
@@ -12720,27 +12986,21 @@
       <c r="S58" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="T58" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="U58" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="T58" s="21"/>
+      <c r="U58" s="21"/>
       <c r="V58" s="21" t="s">
         <v>131</v>
       </c>
       <c r="W58" s="21"/>
-      <c r="X58" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="X58" s="21"/>
       <c r="Y58" s="10"/>
     </row>
-    <row r="59" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B59" s="26" t="s">
-        <v>125</v>
+        <v>55</v>
       </c>
       <c r="C59" s="21"/>
       <c r="D59" s="21" t="s">
@@ -12752,15 +13012,9 @@
       <c r="F59" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="G59" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="H59" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="I59" s="21" t="s">
-        <v>127</v>
-      </c>
+      <c r="G59" s="21"/>
+      <c r="H59" s="21"/>
+      <c r="I59" s="21"/>
       <c r="J59" s="21" t="s">
         <v>17</v>
       </c>
@@ -12770,18 +13024,12 @@
       <c r="L59" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="M59" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="M59" s="21"/>
       <c r="N59" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="O59" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="P59" s="21" t="s">
-        <v>127</v>
-      </c>
+      <c r="O59" s="21"/>
+      <c r="P59" s="21"/>
       <c r="Q59" s="21" t="s">
         <v>17</v>
       </c>
@@ -12791,25 +13039,21 @@
       <c r="S59" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="T59" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="U59" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="T59" s="21"/>
+      <c r="U59" s="21"/>
       <c r="V59" s="21" t="s">
         <v>131</v>
       </c>
       <c r="W59" s="21"/>
       <c r="X59" s="21"/>
-      <c r="Y59" s="36"/>
+      <c r="Y59" s="10"/>
     </row>
-    <row r="60" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B60" s="26" t="s">
-        <v>143</v>
+        <v>56</v>
       </c>
       <c r="C60" s="21"/>
       <c r="D60" s="21" t="s">
@@ -12821,15 +13065,9 @@
       <c r="F60" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="G60" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="H60" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="I60" s="21" t="s">
-        <v>127</v>
-      </c>
+      <c r="G60" s="21"/>
+      <c r="H60" s="21"/>
+      <c r="I60" s="21"/>
       <c r="J60" s="21" t="s">
         <v>17</v>
       </c>
@@ -12839,18 +13077,12 @@
       <c r="L60" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="M60" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="M60" s="21"/>
       <c r="N60" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="O60" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="P60" s="21" t="s">
-        <v>127</v>
-      </c>
+      <c r="O60" s="21"/>
+      <c r="P60" s="21"/>
       <c r="Q60" s="21" t="s">
         <v>17</v>
       </c>
@@ -12860,25 +13092,21 @@
       <c r="S60" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="T60" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="U60" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="T60" s="21"/>
+      <c r="U60" s="21"/>
       <c r="V60" s="21" t="s">
         <v>131</v>
       </c>
       <c r="W60" s="21"/>
       <c r="X60" s="21"/>
-      <c r="Y60" s="36"/>
+      <c r="Y60" s="10"/>
     </row>
-    <row r="61" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:25" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B61" s="26" t="s">
-        <v>144</v>
+        <v>121</v>
       </c>
       <c r="C61" s="21"/>
       <c r="D61" s="21" t="s">
@@ -12914,9 +13142,7 @@
       <c r="N61" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="O61" s="21" t="s">
-        <v>127</v>
-      </c>
+      <c r="O61" s="21"/>
       <c r="P61" s="21" t="s">
         <v>127</v>
       </c>
@@ -12939,15 +13165,17 @@
         <v>131</v>
       </c>
       <c r="W61" s="21"/>
-      <c r="X61" s="21"/>
-      <c r="Y61" s="36"/>
+      <c r="X61" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y61" s="27"/>
     </row>
-    <row r="62" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:25" s="48" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B62" s="26" t="s">
-        <v>145</v>
+        <v>173</v>
       </c>
       <c r="C62" s="21"/>
       <c r="D62" s="21" t="s">
@@ -12983,9 +13211,7 @@
       <c r="N62" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="O62" s="21" t="s">
-        <v>127</v>
-      </c>
+      <c r="O62" s="21"/>
       <c r="P62" s="21" t="s">
         <v>127</v>
       </c>
@@ -13008,15 +13234,17 @@
         <v>131</v>
       </c>
       <c r="W62" s="21"/>
-      <c r="X62" s="21"/>
-      <c r="Y62" s="36"/>
+      <c r="X62" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y62" s="47"/>
     </row>
-    <row r="63" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B63" s="26" t="s">
-        <v>146</v>
+        <v>57</v>
       </c>
       <c r="C63" s="21"/>
       <c r="D63" s="21" t="s">
@@ -13077,29 +13305,37 @@
         <v>131</v>
       </c>
       <c r="W63" s="21"/>
-      <c r="X63" s="21"/>
-      <c r="Y63" s="36"/>
+      <c r="X63" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y63" s="10"/>
     </row>
-    <row r="64" spans="1:25" s="34" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B64" s="26" t="s">
-        <v>147</v>
+        <v>125</v>
       </c>
       <c r="C64" s="21"/>
-      <c r="D64" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="E64" s="17" t="s">
+      <c r="D64" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="E64" s="21" t="s">
         <v>127</v>
       </c>
       <c r="F64" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="G64" s="21"/>
-      <c r="H64" s="21"/>
-      <c r="I64" s="21"/>
+      <c r="G64" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="H64" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="I64" s="21" t="s">
+        <v>127</v>
+      </c>
       <c r="J64" s="21" t="s">
         <v>17</v>
       </c>
@@ -13109,12 +13345,18 @@
       <c r="L64" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="M64" s="21"/>
+      <c r="M64" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="N64" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="O64" s="21"/>
-      <c r="P64" s="21"/>
+      <c r="O64" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="P64" s="21" t="s">
+        <v>127</v>
+      </c>
       <c r="Q64" s="21" t="s">
         <v>17</v>
       </c>
@@ -13124,19 +13366,25 @@
       <c r="S64" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="T64" s="21"/>
-      <c r="U64" s="21"/>
-      <c r="V64" s="21"/>
+      <c r="T64" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="U64" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="V64" s="21" t="s">
+        <v>131</v>
+      </c>
       <c r="W64" s="21"/>
       <c r="X64" s="21"/>
-      <c r="Y64" s="33"/>
+      <c r="Y64" s="36"/>
     </row>
-    <row r="65" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="26" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="B65" s="26" t="s">
-        <v>59</v>
+        <v>143</v>
       </c>
       <c r="C65" s="21"/>
       <c r="D65" s="21" t="s">
@@ -13196,22 +13444,16 @@
       <c r="V65" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="W65" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="X65" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y65" s="52" t="s">
-        <v>60</v>
-      </c>
+      <c r="W65" s="21"/>
+      <c r="X65" s="21"/>
+      <c r="Y65" s="36"/>
     </row>
-    <row r="66" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="26" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="B66" s="26" t="s">
-        <v>61</v>
+        <v>144</v>
       </c>
       <c r="C66" s="21"/>
       <c r="D66" s="21" t="s">
@@ -13271,26 +13513,22 @@
       <c r="V66" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="W66" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="X66" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y66" s="53"/>
+      <c r="W66" s="21"/>
+      <c r="X66" s="21"/>
+      <c r="Y66" s="36"/>
     </row>
-    <row r="67" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="26" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="B67" s="26" t="s">
-        <v>62</v>
+        <v>145</v>
       </c>
       <c r="C67" s="21"/>
       <c r="D67" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="E67" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="E67" s="21" t="s">
         <v>127</v>
       </c>
       <c r="F67" s="21" t="s">
@@ -13309,7 +13547,7 @@
         <v>17</v>
       </c>
       <c r="K67" s="21" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="L67" s="21" t="s">
         <v>127</v>
@@ -13330,257 +13568,434 @@
         <v>17</v>
       </c>
       <c r="R67" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S67" s="21" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="T67" s="21" t="s">
         <v>131</v>
       </c>
       <c r="U67" s="21" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="V67" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="W67" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="X67" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="Y67" s="10"/>
+      <c r="W67" s="21"/>
+      <c r="X67" s="21"/>
+      <c r="Y67" s="36"/>
     </row>
-    <row r="68" spans="1:25" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A68" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="B68" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="C68" s="19"/>
+    <row r="68" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A68" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B68" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="C68" s="21"/>
       <c r="D68" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="E68" s="19"/>
-      <c r="F68" s="19"/>
-      <c r="G68" s="19"/>
-      <c r="H68" s="19"/>
-      <c r="I68" s="19"/>
-      <c r="J68" s="19"/>
-      <c r="K68" s="19"/>
-      <c r="L68" s="19"/>
-      <c r="M68" s="19"/>
-      <c r="N68" s="19"/>
-      <c r="O68" s="19"/>
-      <c r="P68" s="19"/>
-      <c r="Q68" s="19"/>
-      <c r="R68" s="19"/>
-      <c r="S68" s="19"/>
-      <c r="T68" s="19"/>
-      <c r="U68" s="19"/>
-      <c r="V68" s="19"/>
-      <c r="W68" s="19"/>
-      <c r="X68" s="19"/>
-      <c r="Y68" s="14" t="s">
-        <v>65</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="E68" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="F68" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="G68" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="H68" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="I68" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="J68" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="K68" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="L68" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="M68" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="N68" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="O68" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="P68" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q68" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="R68" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="S68" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="T68" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="U68" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="V68" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="W68" s="21"/>
+      <c r="X68" s="21"/>
+      <c r="Y68" s="36"/>
     </row>
-    <row r="69" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A69" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="B69" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="C69" s="17"/>
-      <c r="D69" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="E69" s="17"/>
-      <c r="F69" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="G69" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="H69" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="I69" s="17"/>
-      <c r="J69" s="21"/>
-      <c r="K69" s="17"/>
-      <c r="L69" s="17"/>
-      <c r="M69" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="N69" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="O69" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="P69" s="17"/>
-      <c r="Q69" s="21"/>
-      <c r="R69" s="17"/>
-      <c r="S69" s="17"/>
-      <c r="T69" s="17"/>
-      <c r="U69" s="17"/>
-      <c r="V69" s="17"/>
-      <c r="W69" s="17"/>
-      <c r="X69" s="17"/>
+    <row r="69" spans="1:25" s="34" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A69" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B69" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="C69" s="21"/>
+      <c r="D69" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="E69" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="F69" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="G69" s="21"/>
+      <c r="H69" s="21"/>
+      <c r="I69" s="21"/>
+      <c r="J69" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="K69" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="L69" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="M69" s="21"/>
+      <c r="N69" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="O69" s="21"/>
+      <c r="P69" s="21"/>
+      <c r="Q69" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="R69" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="S69" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="T69" s="21"/>
+      <c r="U69" s="21"/>
+      <c r="V69" s="21"/>
+      <c r="W69" s="21"/>
+      <c r="X69" s="21"/>
+      <c r="Y69" s="33"/>
     </row>
     <row r="70" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A70" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="B70" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="C70" s="17"/>
+      <c r="A70" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B70" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C70" s="21"/>
       <c r="D70" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="E70" s="17"/>
-      <c r="F70" s="17"/>
-      <c r="G70" s="17"/>
-      <c r="H70" s="17"/>
-      <c r="I70" s="17"/>
-      <c r="J70" s="21"/>
-      <c r="K70" s="17"/>
-      <c r="L70" s="17"/>
-      <c r="M70" s="17"/>
-      <c r="N70" s="17"/>
-      <c r="O70" s="17"/>
-      <c r="P70" s="17"/>
-      <c r="Q70" s="21"/>
-      <c r="R70" s="17"/>
-      <c r="S70" s="17"/>
-      <c r="T70" s="17"/>
-      <c r="U70" s="17"/>
-      <c r="V70" s="17"/>
-      <c r="W70" s="17"/>
-      <c r="X70" s="17"/>
+        <v>127</v>
+      </c>
+      <c r="E70" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="F70" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="G70" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="H70" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="I70" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="J70" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="K70" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="L70" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="M70" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="N70" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="O70" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="P70" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q70" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="R70" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="S70" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="T70" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="U70" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="V70" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="W70" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="X70" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y70" s="54" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="71" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A71" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="B71" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="C71" s="17"/>
+      <c r="A71" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B71" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C71" s="21"/>
       <c r="D71" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="E71" s="17"/>
-      <c r="F71" s="17"/>
-      <c r="G71" s="17"/>
-      <c r="H71" s="17"/>
-      <c r="I71" s="17"/>
-      <c r="J71" s="21"/>
-      <c r="K71" s="17"/>
-      <c r="L71" s="17"/>
-      <c r="M71" s="17"/>
-      <c r="N71" s="17"/>
-      <c r="O71" s="17"/>
-      <c r="P71" s="17"/>
-      <c r="Q71" s="21"/>
-      <c r="R71" s="17"/>
-      <c r="S71" s="17"/>
-      <c r="T71" s="17"/>
-      <c r="U71" s="17"/>
-      <c r="V71" s="17"/>
-      <c r="W71" s="17"/>
-      <c r="X71" s="17"/>
+        <v>127</v>
+      </c>
+      <c r="E71" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="F71" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="G71" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="H71" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="I71" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="J71" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="K71" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="L71" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="M71" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="N71" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="O71" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="P71" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q71" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="R71" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="S71" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="T71" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="U71" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="V71" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="W71" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="X71" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y71" s="55"/>
     </row>
     <row r="72" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A72" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="B72" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="C72" s="17"/>
+      <c r="A72" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="B72" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C72" s="21"/>
       <c r="D72" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="E72" s="17"/>
-      <c r="F72" s="17"/>
-      <c r="G72" s="17"/>
-      <c r="H72" s="17"/>
-      <c r="I72" s="17"/>
-      <c r="J72" s="21"/>
-      <c r="K72" s="17"/>
-      <c r="L72" s="17"/>
-      <c r="M72" s="17"/>
-      <c r="N72" s="17"/>
-      <c r="O72" s="17"/>
-      <c r="P72" s="17"/>
-      <c r="Q72" s="21"/>
-      <c r="R72" s="17"/>
-      <c r="S72" s="17"/>
-      <c r="T72" s="17"/>
-      <c r="U72" s="17"/>
-      <c r="V72" s="17"/>
-      <c r="W72" s="17"/>
-      <c r="X72" s="17"/>
+      <c r="E72" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="F72" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="G72" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="H72" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="I72" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="J72" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="K72" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="L72" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="M72" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="N72" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="O72" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="P72" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q72" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="R72" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="S72" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="T72" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="U72" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="V72" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="W72" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="X72" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y72" s="10"/>
     </row>
-    <row r="73" spans="1:25" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A73" s="16" t="s">
+    <row r="73" spans="1:25" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A73" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="B73" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="C73" s="17"/>
+      <c r="B73" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C73" s="19"/>
       <c r="D73" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="E73" s="17"/>
-      <c r="F73" s="17"/>
-      <c r="G73" s="17"/>
-      <c r="H73" s="17"/>
-      <c r="I73" s="17"/>
-      <c r="J73" s="21"/>
-      <c r="K73" s="17"/>
-      <c r="L73" s="17"/>
-      <c r="M73" s="17"/>
-      <c r="N73" s="17"/>
-      <c r="O73" s="17"/>
-      <c r="P73" s="17"/>
-      <c r="Q73" s="21"/>
-      <c r="R73" s="17"/>
-      <c r="S73" s="17"/>
-      <c r="T73" s="17"/>
-      <c r="U73" s="17"/>
-      <c r="V73" s="17"/>
-      <c r="W73" s="17"/>
-      <c r="X73" s="17"/>
+      <c r="E73" s="19"/>
+      <c r="F73" s="19"/>
+      <c r="G73" s="19"/>
+      <c r="H73" s="19"/>
+      <c r="I73" s="19"/>
+      <c r="J73" s="19"/>
+      <c r="K73" s="19"/>
+      <c r="L73" s="19"/>
+      <c r="M73" s="19"/>
+      <c r="N73" s="19"/>
+      <c r="O73" s="19"/>
+      <c r="P73" s="19"/>
+      <c r="Q73" s="19"/>
+      <c r="R73" s="19"/>
+      <c r="S73" s="19"/>
+      <c r="T73" s="19"/>
+      <c r="U73" s="19"/>
+      <c r="V73" s="19"/>
+      <c r="W73" s="19"/>
+      <c r="X73" s="19"/>
+      <c r="Y73" s="14" t="s">
+        <v>65</v>
+      </c>
     </row>
-    <row r="74" spans="1:25" s="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="16" t="s">
         <v>63</v>
       </c>
       <c r="B74" s="16" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="C74" s="17"/>
       <c r="D74" s="21" t="s">
         <v>126</v>
       </c>
       <c r="E74" s="17"/>
-      <c r="F74" s="17"/>
-      <c r="G74" s="17"/>
-      <c r="H74" s="17"/>
+      <c r="F74" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G74" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H74" s="17" t="s">
+        <v>19</v>
+      </c>
       <c r="I74" s="17"/>
       <c r="J74" s="21"/>
       <c r="K74" s="17"/>
       <c r="L74" s="17"/>
-      <c r="M74" s="17"/>
-      <c r="N74" s="17"/>
-      <c r="O74" s="17"/>
+      <c r="M74" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="N74" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="O74" s="17" t="s">
+        <v>19</v>
+      </c>
       <c r="P74" s="17"/>
       <c r="Q74" s="21"/>
       <c r="R74" s="17"/>
@@ -13591,12 +14006,12 @@
       <c r="W74" s="17"/>
       <c r="X74" s="17"/>
     </row>
-    <row r="75" spans="1:25" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="16" t="s">
         <v>63</v>
       </c>
       <c r="B75" s="16" t="s">
-        <v>181</v>
+        <v>67</v>
       </c>
       <c r="C75" s="17"/>
       <c r="D75" s="21" t="s">
@@ -13623,12 +14038,12 @@
       <c r="W75" s="17"/>
       <c r="X75" s="17"/>
     </row>
-    <row r="76" spans="1:25" s="32" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="16" t="s">
         <v>63</v>
       </c>
       <c r="B76" s="16" t="s">
-        <v>124</v>
+        <v>68</v>
       </c>
       <c r="C76" s="17"/>
       <c r="D76" s="21" t="s">
@@ -13657,95 +14072,261 @@
     </row>
     <row r="77" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77" s="16" t="s">
-        <v>109</v>
+        <v>63</v>
       </c>
       <c r="B77" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="C77" s="20"/>
+        <v>69</v>
+      </c>
+      <c r="C77" s="17"/>
       <c r="D77" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="E77" s="20"/>
-      <c r="F77" s="20"/>
-      <c r="G77" s="20"/>
-      <c r="H77" s="20"/>
-      <c r="I77" s="20"/>
-      <c r="J77" s="43"/>
-      <c r="K77" s="20"/>
-      <c r="L77" s="20"/>
-      <c r="M77" s="20"/>
-      <c r="N77" s="20"/>
-      <c r="O77" s="20"/>
-      <c r="P77" s="20"/>
-      <c r="Q77" s="43"/>
-      <c r="R77" s="20"/>
-      <c r="S77" s="20"/>
-      <c r="T77" s="20"/>
-      <c r="U77" s="20"/>
-      <c r="V77" s="20"/>
-      <c r="W77" s="20"/>
-      <c r="X77" s="20"/>
+      <c r="E77" s="17"/>
+      <c r="F77" s="17"/>
+      <c r="G77" s="17"/>
+      <c r="H77" s="17"/>
+      <c r="I77" s="17"/>
+      <c r="J77" s="21"/>
+      <c r="K77" s="17"/>
+      <c r="L77" s="17"/>
+      <c r="M77" s="17"/>
+      <c r="N77" s="17"/>
+      <c r="O77" s="17"/>
+      <c r="P77" s="17"/>
+      <c r="Q77" s="21"/>
+      <c r="R77" s="17"/>
+      <c r="S77" s="17"/>
+      <c r="T77" s="17"/>
+      <c r="U77" s="17"/>
+      <c r="V77" s="17"/>
+      <c r="W77" s="17"/>
+      <c r="X77" s="17"/>
     </row>
-    <row r="78" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:25" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B78" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="C78" s="17"/>
+      <c r="D78" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="E78" s="17"/>
+      <c r="F78" s="17"/>
+      <c r="G78" s="17"/>
+      <c r="H78" s="17"/>
+      <c r="I78" s="17"/>
+      <c r="J78" s="21"/>
+      <c r="K78" s="17"/>
+      <c r="L78" s="17"/>
+      <c r="M78" s="17"/>
+      <c r="N78" s="17"/>
+      <c r="O78" s="17"/>
+      <c r="P78" s="17"/>
+      <c r="Q78" s="21"/>
+      <c r="R78" s="17"/>
+      <c r="S78" s="17"/>
+      <c r="T78" s="17"/>
+      <c r="U78" s="17"/>
+      <c r="V78" s="17"/>
+      <c r="W78" s="17"/>
+      <c r="X78" s="17"/>
+    </row>
+    <row r="79" spans="1:25" s="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A79" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B79" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C79" s="17"/>
+      <c r="D79" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="E79" s="17"/>
+      <c r="F79" s="17"/>
+      <c r="G79" s="17"/>
+      <c r="H79" s="17"/>
+      <c r="I79" s="17"/>
+      <c r="J79" s="21"/>
+      <c r="K79" s="17"/>
+      <c r="L79" s="17"/>
+      <c r="M79" s="17"/>
+      <c r="N79" s="17"/>
+      <c r="O79" s="17"/>
+      <c r="P79" s="17"/>
+      <c r="Q79" s="21"/>
+      <c r="R79" s="17"/>
+      <c r="S79" s="17"/>
+      <c r="T79" s="17"/>
+      <c r="U79" s="17"/>
+      <c r="V79" s="17"/>
+      <c r="W79" s="17"/>
+      <c r="X79" s="17"/>
+    </row>
+    <row r="80" spans="1:25" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A80" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B80" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="C80" s="17"/>
+      <c r="D80" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="E80" s="17"/>
+      <c r="F80" s="17"/>
+      <c r="G80" s="17"/>
+      <c r="H80" s="17"/>
+      <c r="I80" s="17"/>
+      <c r="J80" s="21"/>
+      <c r="K80" s="17"/>
+      <c r="L80" s="17"/>
+      <c r="M80" s="17"/>
+      <c r="N80" s="17"/>
+      <c r="O80" s="17"/>
+      <c r="P80" s="17"/>
+      <c r="Q80" s="21"/>
+      <c r="R80" s="17"/>
+      <c r="S80" s="17"/>
+      <c r="T80" s="17"/>
+      <c r="U80" s="17"/>
+      <c r="V80" s="17"/>
+      <c r="W80" s="17"/>
+      <c r="X80" s="17"/>
+    </row>
+    <row r="81" spans="1:24" s="32" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A81" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B81" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="C81" s="17"/>
+      <c r="D81" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="E81" s="17"/>
+      <c r="F81" s="17"/>
+      <c r="G81" s="17"/>
+      <c r="H81" s="17"/>
+      <c r="I81" s="17"/>
+      <c r="J81" s="21"/>
+      <c r="K81" s="17"/>
+      <c r="L81" s="17"/>
+      <c r="M81" s="17"/>
+      <c r="N81" s="17"/>
+      <c r="O81" s="17"/>
+      <c r="P81" s="17"/>
+      <c r="Q81" s="21"/>
+      <c r="R81" s="17"/>
+      <c r="S81" s="17"/>
+      <c r="T81" s="17"/>
+      <c r="U81" s="17"/>
+      <c r="V81" s="17"/>
+      <c r="W81" s="17"/>
+      <c r="X81" s="17"/>
+    </row>
+    <row r="82" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A82" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="B82" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C82" s="20"/>
+      <c r="D82" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="E82" s="20"/>
+      <c r="F82" s="20"/>
+      <c r="G82" s="20"/>
+      <c r="H82" s="20"/>
+      <c r="I82" s="20"/>
+      <c r="J82" s="43"/>
+      <c r="K82" s="20"/>
+      <c r="L82" s="20"/>
+      <c r="M82" s="20"/>
+      <c r="N82" s="20"/>
+      <c r="O82" s="20"/>
+      <c r="P82" s="20"/>
+      <c r="Q82" s="43"/>
+      <c r="R82" s="20"/>
+      <c r="S82" s="20"/>
+      <c r="T82" s="20"/>
+      <c r="U82" s="20"/>
+      <c r="V82" s="20"/>
+      <c r="W82" s="20"/>
+      <c r="X82" s="20"/>
+    </row>
+    <row r="83" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A83" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="B78" s="16" t="s">
+      <c r="B83" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="C78" s="20"/>
-      <c r="D78" s="21" t="s">
+      <c r="C83" s="20"/>
+      <c r="D83" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="E78" s="29" t="s">
+      <c r="E83" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="F78" s="29"/>
-      <c r="G78" s="29" t="s">
+      <c r="F83" s="29"/>
+      <c r="G83" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="H78" s="29"/>
-      <c r="I78" s="29"/>
-      <c r="J78" s="44" t="s">
+      <c r="H83" s="29"/>
+      <c r="I83" s="29"/>
+      <c r="J83" s="44" t="s">
         <v>160</v>
       </c>
-      <c r="K78" s="29" t="s">
+      <c r="K83" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="L78" s="29" t="s">
+      <c r="L83" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="M78" s="29" t="s">
+      <c r="M83" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="N78" s="29" t="s">
+      <c r="N83" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="O78" s="29"/>
-      <c r="P78" s="29"/>
-      <c r="Q78" s="44" t="s">
+      <c r="O83" s="29"/>
+      <c r="P83" s="29"/>
+      <c r="Q83" s="44" t="s">
         <v>160</v>
       </c>
-      <c r="R78" s="46" t="s">
+      <c r="R83" s="46" t="s">
         <v>165</v>
       </c>
-      <c r="S78" s="44" t="s">
+      <c r="S83" s="44" t="s">
         <v>160</v>
       </c>
-      <c r="T78" s="29"/>
-      <c r="U78" s="29" t="s">
+      <c r="T83" s="29"/>
+      <c r="U83" s="29" t="s">
         <v>160</v>
       </c>
-      <c r="V78" s="29"/>
-      <c r="W78" s="29"/>
-      <c r="X78" s="29"/>
+      <c r="V83" s="29"/>
+      <c r="W83" s="29"/>
+      <c r="X83" s="29"/>
     </row>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C67" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="D75" sqref="D75"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C33" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="F37" sqref="F37"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
+      <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -13755,15 +14336,9 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
-      <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
   </customSheetViews>
   <mergeCells count="6">
-    <mergeCell ref="Y65:Y66"/>
+    <mergeCell ref="Y70:Y71"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="K5:O5"/>
     <mergeCell ref="R5:X5"/>
@@ -14119,13 +14694,13 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
-      <selection activeCell="B17" sqref="B17"/>
+    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
+      <selection activeCell="C7" sqref="C7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
-      <selection activeCell="C7" sqref="C7"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
+      <selection activeCell="B17" sqref="B17"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>

</xml_diff>

<commit_message>
HAR-5113 Laadunvalvojalle kirjoitusoikeus aikatauluun
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikkoro/Desktop/Sources/harja/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarnova/projects/harja/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28720" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="13460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -22,10 +22,10 @@
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="571" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
     <customWorkbookView name="Mikko Rönkkömäki - Personal View" guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" mergeInterval="0" personalView="1" windowWidth="2560" windowHeight="1263" tabRatio="500" activeSheetId="2"/>
-    <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
-    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="596" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -1239,7 +1239,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{FEE05AE3-8182-DC45-9C12-C837CD9BAE99}" diskRevisions="1" revisionId="439" version="57">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{18D528AF-50AD-3744-BF7B-4E3B5E8C50B3}" diskRevisions="1" revisionId="442" version="58">
   <header guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" dateTime="2016-09-06T09:14:56" maxSheetId="3" userName="Tatu Tarvainen" r:id="rId2" minRId="1" maxRId="3">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1576,6 +1576,12 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{18D528AF-50AD-3744-BF7B-4E3B5E8C50B3}" dateTime="2017-06-15T14:58:33" maxSheetId="3" userName="Microsoft Office User" r:id="rId58" minRId="440" maxRId="441">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -9255,6 +9261,43 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog57.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="440" sId="1" odxf="1" dxf="1">
+    <oc r="G29" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </oc>
+    <nc r="G29" t="inlineStr">
+      <is>
+        <t>R*,W</t>
+      </is>
+    </nc>
+    <odxf/>
+    <ndxf/>
+  </rcc>
+  <rcc rId="441" sId="1">
+    <oc r="M29" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </oc>
+    <nc r="M29" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="delete"/>
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_7A9649F2_657F_9445_B6E6_FE94C6A09957_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Oikeudet!$A$5:$Y$83</formula>
+    <oldFormula>Oikeudet!$A$5:$Y$83</oldFormula>
+  </rdn>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog6.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="58" sId="1">
@@ -9341,7 +9384,7 @@
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="14">
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="15">
   <userInfo guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" name="Tatu Tarvainen" id="-130145201" dateTime="2016-09-06T09:10:23"/>
   <userInfo guid="{E0850D7E-A93F-EF44-B46A-3BEA4D7DBEDB}" name="Jarno Väyrynen" id="-589116405" dateTime="2016-09-06T12:54:09"/>
   <userInfo guid="{0407E191-78DA-F349-B5E5-8AE1BC03A29E}" name="Jarno Väyrynen" id="-589108428" dateTime="2016-09-08T15:33:24"/>
@@ -9356,6 +9399,7 @@
   <userInfo guid="{88D4547C-A4BB-3843-ABD6-020023F84CCA}" name="Microsoft Office User" id="-297001900" dateTime="2017-04-07T14:47:26"/>
   <userInfo guid="{88D4547C-A4BB-3843-ABD6-020023F84CCA}" name="Microsoft Office User" id="-296969784" dateTime="2017-05-08T10:00:09"/>
   <userInfo guid="{FEE05AE3-8182-DC45-9C12-C837CD9BAE99}" name="Mikko Rönkkömäki" id="-727915884" dateTime="2017-05-18T10:22:30"/>
+  <userInfo guid="{18D528AF-50AD-3744-BF7B-4E3B5E8C50B3}" name="Microsoft Office User" id="-297007836" dateTime="2017-06-15T12:29:16"/>
 </users>
 </file>
 
@@ -9683,11 +9727,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y83"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C29" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
+      <pane xSplit="2" ySplit="6" topLeftCell="H25" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B48" sqref="B48"/>
+      <selection pane="bottomRight" activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -11256,8 +11300,8 @@
       <c r="F29" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="G29" s="21" t="s">
-        <v>126</v>
+      <c r="G29" s="17" t="s">
+        <v>129</v>
       </c>
       <c r="H29" s="21" t="s">
         <v>126</v>
@@ -11275,7 +11319,7 @@
         <v>156</v>
       </c>
       <c r="M29" s="21" t="s">
-        <v>16</v>
+        <v>112</v>
       </c>
       <c r="N29" s="21" t="s">
         <v>126</v>
@@ -14345,9 +14389,15 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C29" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="B48" sqref="B48"/>
+    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="H25" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="N31" sqref="N31"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
+      <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -14357,15 +14407,9 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
-      <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C33" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="F37" sqref="F37"/>
+    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="C29" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="B48" sqref="B48"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -14388,8 +14432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -14722,8 +14766,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}">
-      <selection activeCell="A22" sqref="A22"/>
+    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}">
+      <selection activeCell="G36" sqref="G36"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
+      <selection activeCell="C7" sqref="C7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -14732,13 +14781,8 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
-      <selection activeCell="C7" sqref="C7"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}">
-      <selection activeCell="G36" sqref="G36"/>
+    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}">
+      <selection activeCell="A22" sqref="A22"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>

</xml_diff>

<commit_message>
Lisää vesiväylä materiaalit oikeus
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -5,27 +5,29 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarnova/projects/harja/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tatuta/projects/harja/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="13460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19420" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
     <sheet name="Roolit" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$83</definedName>
-    <definedName name="Z_1DD617EE_F308_3E45_A8EF_4713F47FA0DD_.wvu.FilterData" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$83</definedName>
-    <definedName name="Z_7A9649F2_657F_9445_B6E6_FE94C6A09957_.wvu.FilterData" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$83</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$84</definedName>
+    <definedName name="Z_1DD617EE_F308_3E45_A8EF_4713F47FA0DD_.wvu.FilterData" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$84</definedName>
+    <definedName name="Z_7A9649F2_657F_9445_B6E6_FE94C6A09957_.wvu.FilterData" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$84</definedName>
+    <definedName name="Z_E88E7AA2_EE96_CA4C_AB2A_FE73CCE938AC_.wvu.FilterData" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$84</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Microsoft Office -käyttäjä - Oma näkymä" guid="{E88E7AA2-EE96-CA4C-AB2A-FE73CCE938AC}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="798" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Mikko Rönkkömäki - Personal View" guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" mergeInterval="0" personalView="1" windowWidth="2560" windowHeight="1263" tabRatio="500" activeSheetId="2"/>
+    <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
+    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="571" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
-    <customWorkbookView name="Mikko Rönkkömäki - Personal View" guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" mergeInterval="0" personalView="1" windowWidth="2560" windowHeight="1263" tabRatio="500" activeSheetId="2"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -72,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1317" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="187">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -630,6 +632,9 @@
   </si>
   <si>
     <t>Vesiväylälaadunseuranta / Viat</t>
+  </si>
+  <si>
+    <t>Vesiväylä / Materiaalit</t>
   </si>
 </sst>
 </file>
@@ -941,7 +946,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -1040,6 +1045,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1050,183 +1059,183 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="177">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Norm." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1239,7 +1248,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{18D528AF-50AD-3744-BF7B-4E3B5E8C50B3}" diskRevisions="1" revisionId="442" version="58">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{FED76948-6277-1647-9EFC-6DA116A5279E}" diskRevisions="1" revisionId="460" version="59">
   <header guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" dateTime="2016-09-06T09:14:56" maxSheetId="3" userName="Tatu Tarvainen" r:id="rId2" minRId="1" maxRId="3">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1582,6 +1591,12 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{FED76948-6277-1647-9EFC-6DA116A5279E}" dateTime="2017-06-19T20:29:12" maxSheetId="3" userName="Microsoft Office -käyttäjä" r:id="rId59" minRId="443" maxRId="459">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -9298,6 +9313,128 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog58.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="443" sId="1" ref="A44:XFD44" action="insertRow"/>
+  <rcc rId="444" sId="1">
+    <nc r="A44" t="inlineStr">
+      <is>
+        <t>Urakat</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="445" sId="1">
+    <nc r="B44" t="inlineStr">
+      <is>
+        <t>Vesiväylä / Materiaalit</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="446" sId="1">
+    <nc r="D44" t="inlineStr">
+      <is>
+        <t>R*,W*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="447" sId="1">
+    <nc r="E44" t="inlineStr">
+      <is>
+        <t>R*,W</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="448" sId="1">
+    <nc r="F44" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="449" sId="1">
+    <nc r="G44" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="450" sId="1">
+    <nc r="K44" t="inlineStr">
+      <is>
+        <t>R*,W*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="451" sId="1">
+    <nc r="L44" t="inlineStr">
+      <is>
+        <t>R*,W*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="452" sId="1">
+    <nc r="M44" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="453" sId="1">
+    <nc r="N44" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="454" sId="1">
+    <nc r="O44" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="455" sId="1">
+    <nc r="S44" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="456" sId="1">
+    <nc r="R44" t="inlineStr">
+      <is>
+        <t>R+,W+</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="457" sId="1">
+    <nc r="T44" t="inlineStr">
+      <is>
+        <t>R+</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="458" sId="1">
+    <nc r="U44" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="459" sId="1">
+    <nc r="V44" t="inlineStr">
+      <is>
+        <t>R+</t>
+      </is>
+    </nc>
+  </rcc>
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_E88E7AA2_EE96_CA4C_AB2A_FE73CCE938AC_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Oikeudet!$A$5:$Y$84</formula>
+  </rdn>
+  <rcv guid="{E88E7AA2-EE96-CA4C-AB2A-FE73CCE938AC}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog6.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="58" sId="1">
@@ -9384,7 +9521,7 @@
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="15">
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="16">
   <userInfo guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" name="Tatu Tarvainen" id="-130145201" dateTime="2016-09-06T09:10:23"/>
   <userInfo guid="{E0850D7E-A93F-EF44-B46A-3BEA4D7DBEDB}" name="Jarno Väyrynen" id="-589116405" dateTime="2016-09-06T12:54:09"/>
   <userInfo guid="{0407E191-78DA-F349-B5E5-8AE1BC03A29E}" name="Jarno Väyrynen" id="-589108428" dateTime="2016-09-08T15:33:24"/>
@@ -9400,6 +9537,7 @@
   <userInfo guid="{88D4547C-A4BB-3843-ABD6-020023F84CCA}" name="Microsoft Office User" id="-296969784" dateTime="2017-05-08T10:00:09"/>
   <userInfo guid="{FEE05AE3-8182-DC45-9C12-C837CD9BAE99}" name="Mikko Rönkkömäki" id="-727915884" dateTime="2017-05-18T10:22:30"/>
   <userInfo guid="{18D528AF-50AD-3744-BF7B-4E3B5E8C50B3}" name="Microsoft Office User" id="-297007836" dateTime="2017-06-15T12:29:16"/>
+  <userInfo guid="{FED76948-6277-1647-9EFC-6DA116A5279E}" name="Microsoft Office -käyttäjä" id="-785734380" dateTime="2017-06-19T20:24:56"/>
 </users>
 </file>
 
@@ -9725,13 +9863,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y83"/>
+  <dimension ref="A1:Y84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="H25" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C32" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="N31" sqref="N31"/>
+      <selection pane="bottomRight" activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9767,40 +9905,40 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="59" t="s">
         <v>150</v>
       </c>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="59" t="s">
+      <c r="C2" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
     </row>
     <row r="3" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
@@ -9821,30 +9959,30 @@
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="55"/>
-      <c r="K5" s="56" t="s">
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="K5" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="L5" s="55"/>
-      <c r="M5" s="55"/>
-      <c r="N5" s="55"/>
-      <c r="O5" s="55"/>
-      <c r="R5" s="56" t="s">
+      <c r="L5" s="57"/>
+      <c r="M5" s="57"/>
+      <c r="N5" s="57"/>
+      <c r="O5" s="57"/>
+      <c r="R5" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="S5" s="55"/>
-      <c r="T5" s="55"/>
-      <c r="U5" s="55"/>
-      <c r="V5" s="55"/>
-      <c r="W5" s="55"/>
-      <c r="X5" s="55"/>
+      <c r="S5" s="57"/>
+      <c r="T5" s="57"/>
+      <c r="U5" s="57"/>
+      <c r="V5" s="57"/>
+      <c r="W5" s="57"/>
+      <c r="X5" s="57"/>
       <c r="Y5" s="5" t="s">
         <v>13</v>
       </c>
@@ -12093,65 +12231,71 @@
       <c r="X43" s="21"/>
       <c r="Y43" s="52"/>
     </row>
-    <row r="44" spans="1:25" s="31" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:25" s="55" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="26" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="B44" s="26" t="s">
-        <v>122</v>
+        <v>186</v>
       </c>
       <c r="C44" s="21"/>
       <c r="D44" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E44" s="17" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="F44" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="G44" s="21"/>
+      <c r="G44" s="21" t="s">
+        <v>126</v>
+      </c>
       <c r="H44" s="21"/>
       <c r="I44" s="21"/>
-      <c r="J44" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="K44" s="21" t="s">
-        <v>126</v>
+      <c r="J44" s="21"/>
+      <c r="K44" s="17" t="s">
+        <v>125</v>
       </c>
       <c r="L44" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="M44" s="21"/>
+        <v>125</v>
+      </c>
+      <c r="M44" s="21" t="s">
+        <v>112</v>
+      </c>
       <c r="N44" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="O44" s="21"/>
-      <c r="P44" s="21"/>
-      <c r="Q44" s="21" t="s">
-        <v>16</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="O44" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="P44" s="17"/>
+      <c r="Q44" s="21"/>
       <c r="R44" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="S44" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="T44" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="S44" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="T44" s="21"/>
-      <c r="U44" s="21"/>
-      <c r="V44" s="21" t="s">
+      <c r="U44" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="V44" s="17" t="s">
         <v>130</v>
       </c>
       <c r="W44" s="21"/>
       <c r="X44" s="21"/>
-      <c r="Y44" s="30"/>
+      <c r="Y44" s="54"/>
     </row>
-    <row r="45" spans="1:25" s="48" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:25" s="31" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="26" t="s">
         <v>42</v>
       </c>
       <c r="B45" s="26" t="s">
-        <v>171</v>
+        <v>122</v>
       </c>
       <c r="C45" s="21"/>
       <c r="D45" s="17" t="s">
@@ -12197,28 +12341,26 @@
       </c>
       <c r="W45" s="21"/>
       <c r="X45" s="21"/>
-      <c r="Y45" s="47"/>
+      <c r="Y45" s="30"/>
     </row>
-    <row r="46" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:25" s="48" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="26" t="s">
         <v>42</v>
       </c>
       <c r="B46" s="26" t="s">
-        <v>43</v>
+        <v>171</v>
       </c>
       <c r="C46" s="21"/>
-      <c r="D46" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="E46" s="21" t="s">
+      <c r="D46" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="E46" s="17" t="s">
         <v>126</v>
       </c>
       <c r="F46" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="G46" s="21" t="s">
-        <v>18</v>
-      </c>
+      <c r="G46" s="21"/>
       <c r="H46" s="21"/>
       <c r="I46" s="21"/>
       <c r="J46" s="21" t="s">
@@ -12252,14 +12394,14 @@
       </c>
       <c r="W46" s="21"/>
       <c r="X46" s="21"/>
-      <c r="Y46" s="10"/>
+      <c r="Y46" s="47"/>
     </row>
     <row r="47" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="26" t="s">
         <v>42</v>
       </c>
       <c r="B47" s="26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C47" s="21"/>
       <c r="D47" s="21" t="s">
@@ -12272,14 +12414,10 @@
         <v>126</v>
       </c>
       <c r="G47" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="H47" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="I47" s="21" t="s">
-        <v>126</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="H47" s="21"/>
+      <c r="I47" s="21"/>
       <c r="J47" s="21" t="s">
         <v>16</v>
       </c>
@@ -12289,18 +12427,12 @@
       <c r="L47" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="M47" s="21" t="s">
-        <v>16</v>
-      </c>
+      <c r="M47" s="21"/>
       <c r="N47" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="O47" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="P47" s="21" t="s">
-        <v>126</v>
-      </c>
+      <c r="O47" s="21"/>
+      <c r="P47" s="21"/>
       <c r="Q47" s="21" t="s">
         <v>16</v>
       </c>
@@ -12310,27 +12442,21 @@
       <c r="S47" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="T47" s="21" t="s">
-        <v>130</v>
-      </c>
-      <c r="U47" s="21" t="s">
-        <v>16</v>
-      </c>
+      <c r="T47" s="21"/>
+      <c r="U47" s="21"/>
       <c r="V47" s="21" t="s">
         <v>130</v>
       </c>
       <c r="W47" s="21"/>
-      <c r="X47" s="21" t="s">
-        <v>16</v>
-      </c>
+      <c r="X47" s="21"/>
       <c r="Y47" s="10"/>
     </row>
-    <row r="48" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="26" t="s">
         <v>42</v>
       </c>
       <c r="B48" s="26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C48" s="21"/>
       <c r="D48" s="21" t="s">
@@ -12390,20 +12516,18 @@
       <c r="V48" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="W48" s="21" t="s">
-        <v>16</v>
-      </c>
+      <c r="W48" s="21"/>
       <c r="X48" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="Y48" s="36"/>
+      <c r="Y48" s="10"/>
     </row>
-    <row r="49" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="26" t="s">
         <v>42</v>
       </c>
       <c r="B49" s="26" t="s">
-        <v>147</v>
+        <v>45</v>
       </c>
       <c r="C49" s="21"/>
       <c r="D49" s="21" t="s">
@@ -12463,18 +12587,20 @@
       <c r="V49" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="W49" s="21"/>
+      <c r="W49" s="21" t="s">
+        <v>16</v>
+      </c>
       <c r="X49" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="Y49" s="10"/>
+      <c r="Y49" s="36"/>
     </row>
     <row r="50" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="26" t="s">
         <v>42</v>
       </c>
       <c r="B50" s="26" t="s">
-        <v>46</v>
+        <v>147</v>
       </c>
       <c r="C50" s="21"/>
       <c r="D50" s="21" t="s">
@@ -12545,7 +12671,7 @@
         <v>42</v>
       </c>
       <c r="B51" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C51" s="21"/>
       <c r="D51" s="21" t="s">
@@ -12611,12 +12737,12 @@
       </c>
       <c r="Y51" s="10"/>
     </row>
-    <row r="52" spans="1:25" s="40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="26" t="s">
         <v>42</v>
       </c>
       <c r="B52" s="26" t="s">
-        <v>154</v>
+        <v>47</v>
       </c>
       <c r="C52" s="21"/>
       <c r="D52" s="21" t="s">
@@ -12680,14 +12806,14 @@
       <c r="X52" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="Y52" s="39"/>
+      <c r="Y52" s="10"/>
     </row>
-    <row r="53" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:25" s="40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="26" t="s">
         <v>42</v>
       </c>
       <c r="B53" s="26" t="s">
-        <v>48</v>
+        <v>154</v>
       </c>
       <c r="C53" s="21"/>
       <c r="D53" s="21" t="s">
@@ -12751,14 +12877,14 @@
       <c r="X53" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="Y53" s="10"/>
+      <c r="Y53" s="39"/>
     </row>
     <row r="54" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="26" t="s">
         <v>42</v>
       </c>
       <c r="B54" s="26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C54" s="21"/>
       <c r="D54" s="21" t="s">
@@ -12794,7 +12920,9 @@
       <c r="N54" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="O54" s="21"/>
+      <c r="O54" s="21" t="s">
+        <v>126</v>
+      </c>
       <c r="P54" s="21" t="s">
         <v>126</v>
       </c>
@@ -12827,7 +12955,7 @@
         <v>42</v>
       </c>
       <c r="B55" s="26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C55" s="21"/>
       <c r="D55" s="21" t="s">
@@ -12863,9 +12991,7 @@
       <c r="N55" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="O55" s="21" t="s">
-        <v>126</v>
-      </c>
+      <c r="O55" s="21"/>
       <c r="P55" s="21" t="s">
         <v>126</v>
       </c>
@@ -12898,7 +13024,7 @@
         <v>42</v>
       </c>
       <c r="B56" s="26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C56" s="21"/>
       <c r="D56" s="21" t="s">
@@ -12910,8 +13036,12 @@
       <c r="F56" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="G56" s="21"/>
-      <c r="H56" s="21"/>
+      <c r="G56" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="H56" s="21" t="s">
+        <v>126</v>
+      </c>
       <c r="I56" s="21" t="s">
         <v>126</v>
       </c>
@@ -12924,11 +13054,15 @@
       <c r="L56" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="M56" s="21"/>
+      <c r="M56" s="21" t="s">
+        <v>16</v>
+      </c>
       <c r="N56" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="O56" s="21"/>
+      <c r="O56" s="21" t="s">
+        <v>126</v>
+      </c>
       <c r="P56" s="21" t="s">
         <v>126</v>
       </c>
@@ -12961,7 +13095,7 @@
         <v>42</v>
       </c>
       <c r="B57" s="26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C57" s="21"/>
       <c r="D57" s="21" t="s">
@@ -12974,10 +13108,10 @@
         <v>126</v>
       </c>
       <c r="G57" s="21"/>
-      <c r="H57" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="I57" s="21"/>
+      <c r="H57" s="21"/>
+      <c r="I57" s="21" t="s">
+        <v>126</v>
+      </c>
       <c r="J57" s="21" t="s">
         <v>16</v>
       </c>
@@ -12991,10 +13125,10 @@
       <c r="N57" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="O57" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="P57" s="21"/>
+      <c r="O57" s="21"/>
+      <c r="P57" s="21" t="s">
+        <v>126</v>
+      </c>
       <c r="Q57" s="21" t="s">
         <v>16</v>
       </c>
@@ -13004,13 +13138,19 @@
       <c r="S57" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="T57" s="21"/>
-      <c r="U57" s="21"/>
+      <c r="T57" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="U57" s="21" t="s">
+        <v>16</v>
+      </c>
       <c r="V57" s="21" t="s">
         <v>130</v>
       </c>
       <c r="W57" s="21"/>
-      <c r="X57" s="21"/>
+      <c r="X57" s="21" t="s">
+        <v>16</v>
+      </c>
       <c r="Y57" s="10"/>
     </row>
     <row r="58" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -13018,7 +13158,7 @@
         <v>42</v>
       </c>
       <c r="B58" s="26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C58" s="21"/>
       <c r="D58" s="21" t="s">
@@ -13031,7 +13171,9 @@
         <v>126</v>
       </c>
       <c r="G58" s="21"/>
-      <c r="H58" s="21"/>
+      <c r="H58" s="21" t="s">
+        <v>18</v>
+      </c>
       <c r="I58" s="21"/>
       <c r="J58" s="21" t="s">
         <v>16</v>
@@ -13046,7 +13188,9 @@
       <c r="N58" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="O58" s="21"/>
+      <c r="O58" s="21" t="s">
+        <v>18</v>
+      </c>
       <c r="P58" s="21"/>
       <c r="Q58" s="21" t="s">
         <v>16</v>
@@ -13071,7 +13215,7 @@
         <v>42</v>
       </c>
       <c r="B59" s="26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C59" s="21"/>
       <c r="D59" s="21" t="s">
@@ -13124,7 +13268,7 @@
         <v>42</v>
       </c>
       <c r="B60" s="26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C60" s="21"/>
       <c r="D60" s="21" t="s">
@@ -13172,12 +13316,12 @@
       <c r="X60" s="21"/>
       <c r="Y60" s="10"/>
     </row>
-    <row r="61" spans="1:25" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="26" t="s">
         <v>42</v>
       </c>
       <c r="B61" s="26" t="s">
-        <v>120</v>
+        <v>55</v>
       </c>
       <c r="C61" s="21"/>
       <c r="D61" s="21" t="s">
@@ -13189,15 +13333,9 @@
       <c r="F61" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="G61" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="H61" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="I61" s="21" t="s">
-        <v>126</v>
-      </c>
+      <c r="G61" s="21"/>
+      <c r="H61" s="21"/>
+      <c r="I61" s="21"/>
       <c r="J61" s="21" t="s">
         <v>16</v>
       </c>
@@ -13207,16 +13345,12 @@
       <c r="L61" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="M61" s="21" t="s">
-        <v>16</v>
-      </c>
+      <c r="M61" s="21"/>
       <c r="N61" s="21" t="s">
         <v>126</v>
       </c>
       <c r="O61" s="21"/>
-      <c r="P61" s="21" t="s">
-        <v>126</v>
-      </c>
+      <c r="P61" s="21"/>
       <c r="Q61" s="21" t="s">
         <v>16</v>
       </c>
@@ -13226,27 +13360,21 @@
       <c r="S61" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="T61" s="21" t="s">
-        <v>130</v>
-      </c>
-      <c r="U61" s="21" t="s">
-        <v>16</v>
-      </c>
+      <c r="T61" s="21"/>
+      <c r="U61" s="21"/>
       <c r="V61" s="21" t="s">
         <v>130</v>
       </c>
       <c r="W61" s="21"/>
-      <c r="X61" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y61" s="27"/>
+      <c r="X61" s="21"/>
+      <c r="Y61" s="10"/>
     </row>
-    <row r="62" spans="1:25" s="48" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:25" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="26" t="s">
         <v>42</v>
       </c>
       <c r="B62" s="26" t="s">
-        <v>172</v>
+        <v>120</v>
       </c>
       <c r="C62" s="21"/>
       <c r="D62" s="21" t="s">
@@ -13308,14 +13436,14 @@
       <c r="X62" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="Y62" s="47"/>
+      <c r="Y62" s="27"/>
     </row>
-    <row r="63" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:25" s="48" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="26" t="s">
         <v>42</v>
       </c>
       <c r="B63" s="26" t="s">
-        <v>56</v>
+        <v>172</v>
       </c>
       <c r="C63" s="21"/>
       <c r="D63" s="21" t="s">
@@ -13351,9 +13479,7 @@
       <c r="N63" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="O63" s="21" t="s">
-        <v>126</v>
-      </c>
+      <c r="O63" s="21"/>
       <c r="P63" s="21" t="s">
         <v>126</v>
       </c>
@@ -13379,14 +13505,14 @@
       <c r="X63" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="Y63" s="10"/>
+      <c r="Y63" s="47"/>
     </row>
-    <row r="64" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="26" t="s">
         <v>42</v>
       </c>
       <c r="B64" s="26" t="s">
-        <v>124</v>
+        <v>56</v>
       </c>
       <c r="C64" s="21"/>
       <c r="D64" s="21" t="s">
@@ -13447,15 +13573,17 @@
         <v>130</v>
       </c>
       <c r="W64" s="21"/>
-      <c r="X64" s="21"/>
-      <c r="Y64" s="36"/>
+      <c r="X64" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y64" s="10"/>
     </row>
     <row r="65" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="26" t="s">
         <v>42</v>
       </c>
       <c r="B65" s="26" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="C65" s="21"/>
       <c r="D65" s="21" t="s">
@@ -13524,7 +13652,7 @@
         <v>42</v>
       </c>
       <c r="B66" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C66" s="21"/>
       <c r="D66" s="21" t="s">
@@ -13593,7 +13721,7 @@
         <v>42</v>
       </c>
       <c r="B67" s="26" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C67" s="21"/>
       <c r="D67" s="21" t="s">
@@ -13662,7 +13790,7 @@
         <v>42</v>
       </c>
       <c r="B68" s="26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C68" s="21"/>
       <c r="D68" s="21" t="s">
@@ -13726,26 +13854,32 @@
       <c r="X68" s="21"/>
       <c r="Y68" s="36"/>
     </row>
-    <row r="69" spans="1:25" s="34" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:25" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="26" t="s">
         <v>42</v>
       </c>
       <c r="B69" s="26" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C69" s="21"/>
-      <c r="D69" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="E69" s="17" t="s">
+      <c r="D69" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="E69" s="21" t="s">
         <v>126</v>
       </c>
       <c r="F69" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="G69" s="21"/>
-      <c r="H69" s="21"/>
-      <c r="I69" s="21"/>
+      <c r="G69" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="H69" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="I69" s="21" t="s">
+        <v>126</v>
+      </c>
       <c r="J69" s="21" t="s">
         <v>16</v>
       </c>
@@ -13755,12 +13889,18 @@
       <c r="L69" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="M69" s="21"/>
+      <c r="M69" s="21" t="s">
+        <v>16</v>
+      </c>
       <c r="N69" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="O69" s="21"/>
-      <c r="P69" s="21"/>
+      <c r="O69" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="P69" s="21" t="s">
+        <v>126</v>
+      </c>
       <c r="Q69" s="21" t="s">
         <v>16</v>
       </c>
@@ -13770,39 +13910,39 @@
       <c r="S69" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="T69" s="21"/>
-      <c r="U69" s="21"/>
-      <c r="V69" s="21"/>
+      <c r="T69" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="U69" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="V69" s="21" t="s">
+        <v>130</v>
+      </c>
       <c r="W69" s="21"/>
       <c r="X69" s="21"/>
-      <c r="Y69" s="33"/>
+      <c r="Y69" s="36"/>
     </row>
-    <row r="70" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:25" s="34" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="26" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="B70" s="26" t="s">
-        <v>58</v>
+        <v>146</v>
       </c>
       <c r="C70" s="21"/>
-      <c r="D70" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="E70" s="21" t="s">
+      <c r="D70" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="E70" s="17" t="s">
         <v>126</v>
       </c>
       <c r="F70" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="G70" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="H70" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="I70" s="21" t="s">
-        <v>126</v>
-      </c>
+      <c r="G70" s="21"/>
+      <c r="H70" s="21"/>
+      <c r="I70" s="21"/>
       <c r="J70" s="21" t="s">
         <v>16</v>
       </c>
@@ -13812,18 +13952,12 @@
       <c r="L70" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="M70" s="21" t="s">
-        <v>16</v>
-      </c>
+      <c r="M70" s="21"/>
       <c r="N70" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="O70" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="P70" s="21" t="s">
-        <v>126</v>
-      </c>
+      <c r="O70" s="21"/>
+      <c r="P70" s="21"/>
       <c r="Q70" s="21" t="s">
         <v>16</v>
       </c>
@@ -13833,31 +13967,19 @@
       <c r="S70" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="T70" s="21" t="s">
-        <v>130</v>
-      </c>
-      <c r="U70" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="V70" s="21" t="s">
-        <v>130</v>
-      </c>
-      <c r="W70" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="X70" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y70" s="54" t="s">
-        <v>59</v>
-      </c>
+      <c r="T70" s="21"/>
+      <c r="U70" s="21"/>
+      <c r="V70" s="21"/>
+      <c r="W70" s="21"/>
+      <c r="X70" s="21"/>
+      <c r="Y70" s="33"/>
     </row>
     <row r="71" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="26" t="s">
         <v>57</v>
       </c>
       <c r="B71" s="26" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C71" s="21"/>
       <c r="D71" s="21" t="s">
@@ -13923,20 +14045,22 @@
       <c r="X71" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="Y71" s="55"/>
+      <c r="Y71" s="56" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="72" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="26" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B72" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C72" s="21"/>
       <c r="D72" s="21" t="s">
-        <v>125</v>
-      </c>
-      <c r="E72" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="E72" s="21" t="s">
         <v>126</v>
       </c>
       <c r="F72" s="21" t="s">
@@ -13955,7 +14079,7 @@
         <v>16</v>
       </c>
       <c r="K72" s="21" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L72" s="21" t="s">
         <v>126</v>
@@ -13976,129 +14100,170 @@
         <v>16</v>
       </c>
       <c r="R72" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="S72" s="21" t="s">
-        <v>112</v>
+        <v>16</v>
       </c>
       <c r="T72" s="21" t="s">
         <v>130</v>
       </c>
       <c r="U72" s="21" t="s">
-        <v>112</v>
+        <v>16</v>
       </c>
       <c r="V72" s="21" t="s">
         <v>130</v>
       </c>
       <c r="W72" s="21" t="s">
-        <v>112</v>
+        <v>16</v>
       </c>
       <c r="X72" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="Y72" s="10"/>
+        <v>16</v>
+      </c>
+      <c r="Y72" s="57"/>
     </row>
-    <row r="73" spans="1:25" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A73" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="B73" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="C73" s="19"/>
+    <row r="73" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A73" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="B73" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C73" s="21"/>
       <c r="D73" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="E73" s="19"/>
-      <c r="F73" s="19"/>
-      <c r="G73" s="19"/>
-      <c r="H73" s="19"/>
-      <c r="I73" s="19"/>
-      <c r="J73" s="19"/>
-      <c r="K73" s="19"/>
-      <c r="L73" s="19"/>
-      <c r="M73" s="19"/>
-      <c r="N73" s="19"/>
-      <c r="O73" s="19"/>
-      <c r="P73" s="19"/>
-      <c r="Q73" s="19"/>
-      <c r="R73" s="19"/>
-      <c r="S73" s="19"/>
-      <c r="T73" s="19"/>
-      <c r="U73" s="19"/>
-      <c r="V73" s="19"/>
-      <c r="W73" s="19"/>
-      <c r="X73" s="19"/>
-      <c r="Y73" s="14" t="s">
-        <v>64</v>
-      </c>
+      <c r="E73" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="F73" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="G73" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="H73" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="I73" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="J73" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="K73" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="L73" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="M73" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="N73" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="O73" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="P73" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q73" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="R73" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="S73" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="T73" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="U73" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="V73" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="W73" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="X73" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y73" s="10"/>
     </row>
-    <row r="74" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A74" s="16" t="s">
+    <row r="74" spans="1:25" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A74" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B74" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C74" s="17"/>
+      <c r="B74" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C74" s="19"/>
       <c r="D74" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="E74" s="17"/>
-      <c r="F74" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="G74" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="H74" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="I74" s="17"/>
-      <c r="J74" s="21"/>
-      <c r="K74" s="17"/>
-      <c r="L74" s="17"/>
-      <c r="M74" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="N74" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="O74" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="P74" s="17"/>
-      <c r="Q74" s="21"/>
-      <c r="R74" s="17"/>
-      <c r="S74" s="17"/>
-      <c r="T74" s="17"/>
-      <c r="U74" s="17"/>
-      <c r="V74" s="17"/>
-      <c r="W74" s="17"/>
-      <c r="X74" s="17"/>
+      <c r="E74" s="19"/>
+      <c r="F74" s="19"/>
+      <c r="G74" s="19"/>
+      <c r="H74" s="19"/>
+      <c r="I74" s="19"/>
+      <c r="J74" s="19"/>
+      <c r="K74" s="19"/>
+      <c r="L74" s="19"/>
+      <c r="M74" s="19"/>
+      <c r="N74" s="19"/>
+      <c r="O74" s="19"/>
+      <c r="P74" s="19"/>
+      <c r="Q74" s="19"/>
+      <c r="R74" s="19"/>
+      <c r="S74" s="19"/>
+      <c r="T74" s="19"/>
+      <c r="U74" s="19"/>
+      <c r="V74" s="19"/>
+      <c r="W74" s="19"/>
+      <c r="X74" s="19"/>
+      <c r="Y74" s="14" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="75" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="16" t="s">
         <v>62</v>
       </c>
       <c r="B75" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C75" s="17"/>
       <c r="D75" s="21" t="s">
         <v>125</v>
       </c>
       <c r="E75" s="17"/>
-      <c r="F75" s="17"/>
-      <c r="G75" s="17"/>
-      <c r="H75" s="17"/>
+      <c r="F75" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G75" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H75" s="17" t="s">
+        <v>18</v>
+      </c>
       <c r="I75" s="17"/>
       <c r="J75" s="21"/>
       <c r="K75" s="17"/>
       <c r="L75" s="17"/>
-      <c r="M75" s="17"/>
-      <c r="N75" s="17"/>
-      <c r="O75" s="17"/>
+      <c r="M75" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="N75" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="O75" s="17" t="s">
+        <v>18</v>
+      </c>
       <c r="P75" s="17"/>
       <c r="Q75" s="21"/>
       <c r="R75" s="17"/>
@@ -14114,7 +14279,7 @@
         <v>62</v>
       </c>
       <c r="B76" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C76" s="17"/>
       <c r="D76" s="21" t="s">
@@ -14146,7 +14311,7 @@
         <v>62</v>
       </c>
       <c r="B77" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C77" s="17"/>
       <c r="D77" s="21" t="s">
@@ -14173,12 +14338,12 @@
       <c r="W77" s="17"/>
       <c r="X77" s="17"/>
     </row>
-    <row r="78" spans="1:25" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="16" t="s">
         <v>62</v>
       </c>
       <c r="B78" s="16" t="s">
-        <v>165</v>
+        <v>68</v>
       </c>
       <c r="C78" s="17"/>
       <c r="D78" s="21" t="s">
@@ -14205,12 +14370,12 @@
       <c r="W78" s="17"/>
       <c r="X78" s="17"/>
     </row>
-    <row r="79" spans="1:25" s="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:25" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="16" t="s">
         <v>62</v>
       </c>
       <c r="B79" s="16" t="s">
-        <v>32</v>
+        <v>165</v>
       </c>
       <c r="C79" s="17"/>
       <c r="D79" s="21" t="s">
@@ -14237,12 +14402,12 @@
       <c r="W79" s="17"/>
       <c r="X79" s="17"/>
     </row>
-    <row r="80" spans="1:25" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:25" s="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="16" t="s">
         <v>62</v>
       </c>
       <c r="B80" s="16" t="s">
-        <v>180</v>
+        <v>32</v>
       </c>
       <c r="C80" s="17"/>
       <c r="D80" s="21" t="s">
@@ -14269,12 +14434,12 @@
       <c r="W80" s="17"/>
       <c r="X80" s="17"/>
     </row>
-    <row r="81" spans="1:24" s="32" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:24" s="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A81" s="16" t="s">
         <v>62</v>
       </c>
       <c r="B81" s="16" t="s">
-        <v>123</v>
+        <v>180</v>
       </c>
       <c r="C81" s="17"/>
       <c r="D81" s="21" t="s">
@@ -14301,97 +14466,141 @@
       <c r="W81" s="17"/>
       <c r="X81" s="17"/>
     </row>
-    <row r="82" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:24" s="32" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A82" s="16" t="s">
-        <v>108</v>
+        <v>62</v>
       </c>
       <c r="B82" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="C82" s="20"/>
+        <v>123</v>
+      </c>
+      <c r="C82" s="17"/>
       <c r="D82" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="E82" s="20"/>
-      <c r="F82" s="20"/>
-      <c r="G82" s="20"/>
-      <c r="H82" s="20"/>
-      <c r="I82" s="20"/>
-      <c r="J82" s="43"/>
-      <c r="K82" s="20"/>
-      <c r="L82" s="20"/>
-      <c r="M82" s="20"/>
-      <c r="N82" s="20"/>
-      <c r="O82" s="20"/>
-      <c r="P82" s="20"/>
-      <c r="Q82" s="43"/>
-      <c r="R82" s="20"/>
-      <c r="S82" s="20"/>
-      <c r="T82" s="20"/>
-      <c r="U82" s="20"/>
-      <c r="V82" s="20"/>
-      <c r="W82" s="20"/>
-      <c r="X82" s="20"/>
+      <c r="E82" s="17"/>
+      <c r="F82" s="17"/>
+      <c r="G82" s="17"/>
+      <c r="H82" s="17"/>
+      <c r="I82" s="17"/>
+      <c r="J82" s="21"/>
+      <c r="K82" s="17"/>
+      <c r="L82" s="17"/>
+      <c r="M82" s="17"/>
+      <c r="N82" s="17"/>
+      <c r="O82" s="17"/>
+      <c r="P82" s="17"/>
+      <c r="Q82" s="21"/>
+      <c r="R82" s="17"/>
+      <c r="S82" s="17"/>
+      <c r="T82" s="17"/>
+      <c r="U82" s="17"/>
+      <c r="V82" s="17"/>
+      <c r="W82" s="17"/>
+      <c r="X82" s="17"/>
     </row>
     <row r="83" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83" s="16" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B83" s="16" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="C83" s="20"/>
       <c r="D83" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="E83" s="20"/>
+      <c r="F83" s="20"/>
+      <c r="G83" s="20"/>
+      <c r="H83" s="20"/>
+      <c r="I83" s="20"/>
+      <c r="J83" s="43"/>
+      <c r="K83" s="20"/>
+      <c r="L83" s="20"/>
+      <c r="M83" s="20"/>
+      <c r="N83" s="20"/>
+      <c r="O83" s="20"/>
+      <c r="P83" s="20"/>
+      <c r="Q83" s="43"/>
+      <c r="R83" s="20"/>
+      <c r="S83" s="20"/>
+      <c r="T83" s="20"/>
+      <c r="U83" s="20"/>
+      <c r="V83" s="20"/>
+      <c r="W83" s="20"/>
+      <c r="X83" s="20"/>
+    </row>
+    <row r="84" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A84" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B84" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="C84" s="20"/>
+      <c r="D84" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="E83" s="29" t="s">
+      <c r="E84" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="F83" s="29"/>
-      <c r="G83" s="29" t="s">
+      <c r="F84" s="29"/>
+      <c r="G84" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="H83" s="29"/>
-      <c r="I83" s="29"/>
-      <c r="J83" s="44" t="s">
+      <c r="H84" s="29"/>
+      <c r="I84" s="29"/>
+      <c r="J84" s="44" t="s">
         <v>159</v>
       </c>
-      <c r="K83" s="29" t="s">
+      <c r="K84" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="L83" s="29" t="s">
+      <c r="L84" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="M83" s="29" t="s">
+      <c r="M84" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="N83" s="29" t="s">
+      <c r="N84" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="O83" s="29"/>
-      <c r="P83" s="29"/>
-      <c r="Q83" s="44" t="s">
+      <c r="O84" s="29"/>
+      <c r="P84" s="29"/>
+      <c r="Q84" s="44" t="s">
         <v>159</v>
       </c>
-      <c r="R83" s="46" t="s">
+      <c r="R84" s="46" t="s">
         <v>164</v>
       </c>
-      <c r="S83" s="44" t="s">
+      <c r="S84" s="44" t="s">
         <v>159</v>
       </c>
-      <c r="T83" s="29"/>
-      <c r="U83" s="29" t="s">
+      <c r="T84" s="29"/>
+      <c r="U84" s="29" t="s">
         <v>159</v>
       </c>
-      <c r="V83" s="29"/>
-      <c r="W83" s="29"/>
-      <c r="X83" s="29"/>
+      <c r="V84" s="29"/>
+      <c r="W84" s="29"/>
+      <c r="X84" s="29"/>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="H25" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="N31" sqref="N31"/>
+    <customSheetView guid="{E88E7AA2-EE96-CA4C-AB2A-FE73CCE938AC}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="C32" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="B44" sqref="B44"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="C29" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="B48" sqref="B48"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
+      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -14401,21 +14610,15 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
-      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C29" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="B48" sqref="B48"/>
+    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="H25" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="N31" sqref="N31"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="6">
-    <mergeCell ref="Y70:Y71"/>
+    <mergeCell ref="Y71:Y72"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="K5:O5"/>
     <mergeCell ref="R5:X5"/>
@@ -14766,8 +14969,18 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}">
+    <customSheetView guid="{E88E7AA2-EE96-CA4C-AB2A-FE73CCE938AC}">
       <selection activeCell="G36" sqref="G36"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}">
+      <selection activeCell="A22" sqref="A22"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
+      <selection activeCell="B17" sqref="B17"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -14776,13 +14989,8 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
-      <selection activeCell="B17" sqref="B17"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}">
-      <selection activeCell="A22" sqref="A22"/>
+    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}">
+      <selection activeCell="G36" sqref="G36"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>

</xml_diff>

<commit_message>
Lisää oikeudet ELY urakanvalvojalle & ELY rakennuttajakonsultille varusteisiin
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tatuta/projects/harja/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikkoro/Desktop/Sources/harja/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="26440" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="26800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -23,11 +23,11 @@
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Mikko Rönkkömäki - Personal View" guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" mergeInterval="0" personalView="1" windowWidth="2560" windowHeight="1167" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="475" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
+    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="Microsoft Office -käyttäjä - Oma näkymä" guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="1149" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
-    <customWorkbookView name="Mikko Rönkkömäki - Personal View" guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" mergeInterval="0" personalView="1" windowWidth="2560" windowHeight="1263" tabRatio="500" activeSheetId="2"/>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="475" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -1066,183 +1066,183 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="177">
-    <cellStyle name="Avattu hyperlinkki" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="96" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="98" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="100" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="102" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="104" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="106" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="108" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="110" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="112" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="114" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="116" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="118" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="120" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="122" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="124" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="126" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="128" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="130" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="132" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="134" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="136" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="138" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="140" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="142" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="144" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="146" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="148" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="150" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="152" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="154" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="156" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="158" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="160" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="162" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="164" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="166" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="168" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="170" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="172" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="174" builtinId="9" hidden="1"/>
-    <cellStyle name="Avattu hyperlinkki" xfId="176" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="93" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="95" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="97" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="99" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="101" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="103" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="105" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="107" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="109" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="111" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="113" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="115" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="117" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="119" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="121" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="123" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="125" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="127" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="129" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="131" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="133" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="135" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="137" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="139" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="141" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="143" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="145" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="147" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="149" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="151" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="153" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="155" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="157" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="159" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="161" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="163" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="165" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="167" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="169" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="171" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="173" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlinkki" xfId="175" builtinId="8" hidden="1"/>
-    <cellStyle name="Norm." xfId="0" builtinId="0"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1255,7 +1255,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{1E352813-0B26-DB4E-84BE-460845B77133}" diskRevisions="1" revisionId="465">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{1AB7A282-42ED-4740-A9CB-95FF229EC1A0}" diskRevisions="1" revisionId="468" version="2">
   <header guid="{81BBEED1-AE57-644F-AA35-AD2520AD95CE}" dateTime="2016-09-06T09:14:56" maxSheetId="3" userName="Tatu Tarvainen" r:id="rId2" minRId="1" maxRId="3">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1610,6 +1610,12 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{1AB7A282-42ED-4740-A9CB-95FF229EC1A0}" dateTime="2017-06-22T10:46:08" maxSheetId="3" userName="Mikko Rönkkömäki" r:id="rId61" minRId="466" maxRId="467">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -9498,6 +9504,41 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog60.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="466" sId="1">
+    <oc r="L19" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </oc>
+    <nc r="L19" t="inlineStr">
+      <is>
+        <t>R*,W*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="467" sId="1">
+    <oc r="Q19" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </oc>
+    <nc r="Q19" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" action="delete"/>
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_1DD617EE_F308_3E45_A8EF_4713F47FA0DD_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Oikeudet!$A$5:$Y$85</formula>
+    <oldFormula>Oikeudet!$A$5:$Y$85</oldFormula>
+  </rdn>
+  <rcv guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog7.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="59" sId="1">
@@ -9567,8 +9608,9 @@
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="2">
   <userInfo guid="{1E352813-0B26-DB4E-84BE-460845B77133}" name="Microsoft Office -käyttäjä" id="-785751636" dateTime="2017-06-20T12:33:00"/>
+  <userInfo guid="{1AB7A282-42ED-4740-A9CB-95FF229EC1A0}" name="Mikko Rönkkömäki" id="-727946492" dateTime="2017-06-22T10:45:48"/>
 </users>
 </file>
 
@@ -9897,10 +9939,10 @@
   <dimension ref="A1:Y85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C31" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
+      <selection pane="bottomRight" activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -10849,7 +10891,7 @@
         <v>125</v>
       </c>
       <c r="L19" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M19" s="17" t="s">
         <v>16</v>
@@ -10862,7 +10904,7 @@
       </c>
       <c r="P19" s="17"/>
       <c r="Q19" s="21" t="s">
-        <v>16</v>
+        <v>112</v>
       </c>
       <c r="R19" s="17" t="s">
         <v>131</v>
@@ -14650,9 +14692,21 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C31" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
+    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="Q19" sqref="Q19"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="C40" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="C44" sqref="C44"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
+      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -14662,21 +14716,9 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
-      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C29" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="B48" sqref="B48"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C40" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="C44" sqref="C44"/>
+    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="C31" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -14700,7 +14742,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -15033,21 +15075,6 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}">
-      <selection activeCell="G36" sqref="G36"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
-      <selection activeCell="C7" sqref="C7"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
-      <selection activeCell="B17" sqref="B17"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
     <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}">
       <selection activeCell="A22" sqref="A22"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15058,6 +15085,21 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
+      <selection activeCell="B17" sqref="B17"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
+      <selection activeCell="C7" sqref="C7"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}">
+      <selection activeCell="G36" sqref="G36"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Päivitä roolit.excel asiakkaan ohjeistuksen mukaiseksi
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -1317,7 +1317,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{9FC49A30-B185-5F49-BE32-47B376592978}" diskRevisions="1" revisionId="635" version="24">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{94B4A4EA-4B96-F548-A073-1FA97DA62AB9}" diskRevisions="1" revisionId="636" version="25">
   <header guid="{1E352813-0B26-DB4E-84BE-460845B77133}" dateTime="2017-06-20T12:32:37" maxSheetId="3" userName="Microsoft Office -käyttäjä" r:id="rId60" minRId="448" maxRId="464">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1462,6 +1462,12 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{94B4A4EA-4B96-F548-A073-1FA97DA62AB9}" dateTime="2017-07-28T09:44:35" maxSheetId="3" userName="Microsoft Office User" r:id="rId84">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -3231,6 +3237,17 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog22.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="delete"/>
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_7A9649F2_657F_9445_B6E6_FE94C6A09957_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Oikeudet!$A$5:$Y$87</formula>
+    <oldFormula>Oikeudet!$A$5:$Y$87</oldFormula>
+  </rdn>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="497" sId="1">
@@ -3907,10 +3924,9 @@
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="3">
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="2">
   <userInfo guid="{1E352813-0B26-DB4E-84BE-460845B77133}" name="Microsoft Office -käyttäjä" id="-785751636" dateTime="2017-06-20T12:33:00"/>
   <userInfo guid="{1AB7A282-42ED-4740-A9CB-95FF229EC1A0}" name="Mikko Rönkkömäki" id="-727946492" dateTime="2017-06-22T10:45:48"/>
-  <userInfo guid="{9FC49A30-B185-5F49-BE32-47B376592978}" name="Microsoft Office User" id="-296985388" dateTime="2017-07-28T09:20:51"/>
 </users>
 </file>
 
@@ -4239,10 +4255,10 @@
   <dimension ref="A1:Y87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="G33" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="E33" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="J41" sqref="J41"/>
+      <selection pane="bottomRight" activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4254,8 +4270,8 @@
     <col min="5" max="5" width="26.1640625" customWidth="1"/>
     <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" style="6" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.1640625" style="6" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25.33203125" style="20" customWidth="1"/>
     <col min="11" max="11" width="40.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="38.1640625" bestFit="1" customWidth="1"/>
@@ -9194,8 +9210,8 @@
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="G33" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="J41" sqref="J41"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="E33" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="E40" sqref="E40"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>

</xml_diff>

<commit_message>
Päivitä roolit-excel, urakoitsija ei voi irrottaa kiintiöstä
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarihan/Jari/Tyo/Solita/Projektit/Harja/harja/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/teemukau/code/harja/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="24100" yWindow="980" windowWidth="27060" windowHeight="26520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27060" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -23,11 +23,11 @@
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="1353" windowHeight="1153" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="1353" windowHeight="884" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
+    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office -käyttäjä - Oma näkymä" guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="1149" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="Mikko Rönkkömäki - Personal View" guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" mergeInterval="0" personalView="1" windowWidth="2560" windowHeight="1071" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Microsoft Office -käyttäjä - Oma näkymä" guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="1149" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1399" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1399" uniqueCount="204">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -647,9 +647,6 @@
   </si>
   <si>
     <t>R*,W,irrota</t>
-  </si>
-  <si>
-    <t>R+,W+,irrota+</t>
   </si>
   <si>
     <t>R*,W*,siirrä-yksikköhintaisiin*,liitä-kiintiöön*,lisää-liite*</t>
@@ -1317,7 +1314,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{94B4A4EA-4B96-F548-A073-1FA97DA62AB9}" diskRevisions="1" revisionId="636" version="25">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{87D69379-A5DA-5B4B-BD89-C67F53EA7C4C}" diskRevisions="1" revisionId="640" version="26">
   <header guid="{1E352813-0B26-DB4E-84BE-460845B77133}" dateTime="2017-06-20T12:32:37" maxSheetId="3" userName="Microsoft Office -käyttäjä" r:id="rId60" minRId="448" maxRId="464">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1468,6 +1465,12 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{87D69379-A5DA-5B4B-BD89-C67F53EA7C4C}" dateTime="2017-07-31T09:08:11" maxSheetId="3" userName="Microsoft Office User" r:id="rId85" minRId="637" maxRId="639">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -3239,6 +3242,53 @@
 
 <file path=xl/revisions/revisionLog22.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="delete"/>
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_7A9649F2_657F_9445_B6E6_FE94C6A09957_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Oikeudet!$A$5:$Y$87</formula>
+    <oldFormula>Oikeudet!$A$5:$Y$87</oldFormula>
+  </rdn>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog23.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="637" sId="1">
+    <oc r="R43" t="inlineStr">
+      <is>
+        <t>R+,W+,irrota+</t>
+      </is>
+    </oc>
+    <nc r="R43" t="inlineStr">
+      <is>
+        <t>R+,W+</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="638" sId="1">
+    <oc r="S43" t="inlineStr">
+      <is>
+        <t>R,W,irrota</t>
+      </is>
+    </oc>
+    <nc r="S43" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="639" sId="1">
+    <oc r="T43" t="inlineStr">
+      <is>
+        <t>R+,W+,irrota+</t>
+      </is>
+    </oc>
+    <nc r="T43" t="inlineStr">
+      <is>
+        <t>R+,W+</t>
+      </is>
+    </nc>
+  </rcc>
   <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="delete"/>
   <rdn rId="0" localSheetId="1" customView="1" name="Z_7A9649F2_657F_9445_B6E6_FE94C6A09957_.wvu.FilterData" hidden="1" oldHidden="1">
     <formula>Oikeudet!$A$5:$Y$87</formula>
@@ -4255,10 +4305,10 @@
   <dimension ref="A1:Y87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="E33" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="U36" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E40" sqref="E40"/>
+      <selection pane="bottomRight" activeCell="W44" sqref="W44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5723,7 +5773,7 @@
         <v>14</v>
       </c>
       <c r="B27" s="39" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C27" s="37"/>
       <c r="D27" s="36" t="s">
@@ -6511,7 +6561,7 @@
       </c>
       <c r="Y39" s="38"/>
     </row>
-    <row r="40" spans="1:25" s="25" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:25" s="25" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="A40" s="39" t="s">
         <v>14</v>
       </c>
@@ -6520,10 +6570,10 @@
       </c>
       <c r="C40" s="37"/>
       <c r="D40" s="41" t="s">
+        <v>191</v>
+      </c>
+      <c r="E40" s="41" t="s">
         <v>192</v>
-      </c>
-      <c r="E40" s="41" t="s">
-        <v>193</v>
       </c>
       <c r="F40" s="37" t="s">
         <v>126</v>
@@ -6534,7 +6584,7 @@
       </c>
       <c r="I40" s="36"/>
       <c r="J40" s="41" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K40" s="36"/>
       <c r="L40" s="37"/>
@@ -6544,10 +6594,10 @@
       <c r="P40" s="36"/>
       <c r="Q40" s="37"/>
       <c r="R40" s="41" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="S40" s="50" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="T40" s="37" t="s">
         <v>130</v>
@@ -6561,7 +6611,7 @@
       <c r="W40" s="37"/>
       <c r="X40" s="37"/>
       <c r="Y40" s="38" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="41" spans="1:25" s="25" customFormat="1" ht="65" x14ac:dyDescent="0.15">
@@ -6573,10 +6623,10 @@
       </c>
       <c r="C41" s="37"/>
       <c r="D41" s="41" t="s">
+        <v>196</v>
+      </c>
+      <c r="E41" s="41" t="s">
         <v>197</v>
-      </c>
-      <c r="E41" s="41" t="s">
-        <v>198</v>
       </c>
       <c r="F41" s="37" t="s">
         <v>126</v>
@@ -6587,7 +6637,7 @@
       </c>
       <c r="I41" s="37"/>
       <c r="J41" s="41" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K41" s="41"/>
       <c r="L41" s="41"/>
@@ -6597,10 +6647,10 @@
       <c r="P41" s="36"/>
       <c r="Q41" s="37"/>
       <c r="R41" s="41" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="S41" s="50" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="T41" s="37" t="s">
         <v>130</v>
@@ -6614,7 +6664,7 @@
       <c r="W41" s="37"/>
       <c r="X41" s="37"/>
       <c r="Y41" s="38" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="42" spans="1:25" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -6683,13 +6733,13 @@
       <c r="P43" s="36"/>
       <c r="Q43" s="37"/>
       <c r="R43" s="37" t="s">
-        <v>191</v>
+        <v>131</v>
       </c>
       <c r="S43" s="37" t="s">
-        <v>189</v>
+        <v>112</v>
       </c>
       <c r="T43" s="37" t="s">
-        <v>191</v>
+        <v>131</v>
       </c>
       <c r="U43" s="37" t="s">
         <v>16</v>
@@ -6700,7 +6750,7 @@
       <c r="W43" s="37"/>
       <c r="X43" s="37"/>
       <c r="Y43" s="38" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="44" spans="1:25" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -6845,7 +6895,7 @@
         <v>42</v>
       </c>
       <c r="B47" s="39" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C47" s="37"/>
       <c r="D47" s="36" t="s">
@@ -9210,14 +9260,20 @@
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="E33" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="E40" sqref="E40"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="U36" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="W44" sqref="W44"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C48" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="D72" sqref="D72:X72"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
+      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
+      <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -9227,15 +9283,9 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
-      <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
-      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
+    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="C48" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="D72" sqref="D72:X72"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -9597,8 +9647,13 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}">
-      <selection activeCell="A22" sqref="A22"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
+      <selection activeCell="B17" sqref="B17"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
+      <selection activeCell="C7" sqref="C7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -9607,13 +9662,8 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
-      <selection activeCell="C7" sqref="C7"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
-      <selection activeCell="B17" sqref="B17"/>
+    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}">
+      <selection activeCell="A22" sqref="A22"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>

</xml_diff>

<commit_message>
Poista urakoitsijalta mahdollisuus luoda ja poistaa vv-tilauksia
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/teemukau/code/harja/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarihan/Jari/Tyo/Solita/Projektit/Harja/harja/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27060" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="47500" windowHeight="25220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -23,11 +23,11 @@
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="1353" windowHeight="884" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="2375" windowHeight="1088" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Mikko Rönkkömäki - Personal View" guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" mergeInterval="0" personalView="1" windowWidth="2560" windowHeight="1071" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office -käyttäjä - Oma näkymä" guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="1149" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
-    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Microsoft Office -käyttäjä - Oma näkymä" guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="1149" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Mikko Rönkkömäki - Personal View" guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" mergeInterval="0" personalView="1" windowWidth="2560" windowHeight="1071" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1399" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1399" uniqueCount="205">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -670,9 +670,6 @@
     <t>R*,W,siirrä-kokonaishintaisiin,lisää-liite,tilausten-muokkaus,siirrä-tilaukseen,hinnoittele-toimenpide,hinnoittele-tilaus</t>
   </si>
   <si>
-    <t>R+,W+,siirrä-kokonaishintaisiin+,lisää-liite+,tilausten-muokkaus+,siirrä-tilaukseen+,hinnoittele-toimenpide+,hinnoittele-tilaus+</t>
-  </si>
-  <si>
     <t>Erikoisoikeudet: siirrä-kokonaishintaisiin, lisää-liite, tilausten-muokkaus, siirrä-tilaukseen, hinnoittele-toimenpide, hinnoittele-tilaus</t>
   </si>
   <si>
@@ -686,6 +683,12 @@
   </si>
   <si>
     <t>Vesiväylälaskutusyhteenveto</t>
+  </si>
+  <si>
+    <t>R+,W+,siirrä-kokonaishintaisiin+,lisää-liite+,siirrä-tilaukseen+,hinnoittele-toimenpide+,hinnoittele-tilaus+</t>
+  </si>
+  <si>
+    <t>R,W,siirrä-kokonaishintaisiin,lisää-liite,siirrä-tilaukseen,hinnoittele-toimenpide,hinnoittele-tilaus</t>
   </si>
 </sst>
 </file>
@@ -1314,7 +1317,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{87D69379-A5DA-5B4B-BD89-C67F53EA7C4C}" diskRevisions="1" revisionId="640" version="26">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{2DE19633-D9F6-EF4C-B6F2-DE3186C97C8D}" diskRevisions="1" revisionId="643" version="27">
   <header guid="{1E352813-0B26-DB4E-84BE-460845B77133}" dateTime="2017-06-20T12:32:37" maxSheetId="3" userName="Microsoft Office -käyttäjä" r:id="rId60" minRId="448" maxRId="464">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1471,6 +1474,12 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{2DE19633-D9F6-EF4C-B6F2-DE3186C97C8D}" dateTime="2017-08-10T13:24:12" maxSheetId="3" userName="Microsoft Office User" r:id="rId86" minRId="641" maxRId="642">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -3286,6 +3295,41 @@
     <nc r="T43" t="inlineStr">
       <is>
         <t>R+,W+</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="delete"/>
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_7A9649F2_657F_9445_B6E6_FE94C6A09957_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Oikeudet!$A$5:$Y$87</formula>
+    <oldFormula>Oikeudet!$A$5:$Y$87</oldFormula>
+  </rdn>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog24.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="641" sId="1">
+    <oc r="R41" t="inlineStr">
+      <is>
+        <t>R+,W+,siirrä-kokonaishintaisiin+,lisää-liite+,tilausten-muokkaus+,siirrä-tilaukseen+,hinnoittele-toimenpide+,hinnoittele-tilaus+</t>
+      </is>
+    </oc>
+    <nc r="R41" t="inlineStr">
+      <is>
+        <t>R+,W+,siirrä-kokonaishintaisiin+,lisää-liite+,siirrä-tilaukseen+,hinnoittele-toimenpide+,hinnoittele-tilaus+</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="642" sId="1">
+    <oc r="S41" t="inlineStr">
+      <is>
+        <t>R,W,siirrä-kokonaishintaisiin,lisää-liite,tilausten-muokkaus,siirrä-tilaukseen,hinnoittele-toimenpide,hinnoittele-tilaus</t>
+      </is>
+    </oc>
+    <nc r="S41" t="inlineStr">
+      <is>
+        <t>R,W,siirrä-kokonaishintaisiin,lisää-liite,siirrä-tilaukseen,hinnoittele-toimenpide,hinnoittele-tilaus</t>
       </is>
     </nc>
   </rcc>
@@ -4305,10 +4349,10 @@
   <dimension ref="A1:Y87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="U36" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="O28" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="W44" sqref="W44"/>
+      <selection pane="bottomRight" activeCell="S41" sqref="S41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5773,7 +5817,7 @@
         <v>14</v>
       </c>
       <c r="B27" s="39" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C27" s="37"/>
       <c r="D27" s="36" t="s">
@@ -6584,7 +6628,7 @@
       </c>
       <c r="I40" s="36"/>
       <c r="J40" s="41" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K40" s="36"/>
       <c r="L40" s="37"/>
@@ -6597,7 +6641,7 @@
         <v>193</v>
       </c>
       <c r="S40" s="50" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="T40" s="37" t="s">
         <v>130</v>
@@ -6637,7 +6681,7 @@
       </c>
       <c r="I41" s="37"/>
       <c r="J41" s="41" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K41" s="41"/>
       <c r="L41" s="41"/>
@@ -6647,10 +6691,10 @@
       <c r="P41" s="36"/>
       <c r="Q41" s="37"/>
       <c r="R41" s="41" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="S41" s="50" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="T41" s="37" t="s">
         <v>130</v>
@@ -6664,7 +6708,7 @@
       <c r="W41" s="37"/>
       <c r="X41" s="37"/>
       <c r="Y41" s="38" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="42" spans="1:25" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -6895,7 +6939,7 @@
         <v>42</v>
       </c>
       <c r="B47" s="39" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C47" s="37"/>
       <c r="D47" s="36" t="s">
@@ -9260,14 +9304,20 @@
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="U36" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="W44" sqref="W44"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="O28" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="S41" sqref="S41"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
-      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
+    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="C48" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="D72" sqref="D72:X72"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="C31" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -9277,15 +9327,9 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C31" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C48" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="D72" sqref="D72:X72"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
+      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -9647,8 +9691,13 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
-      <selection activeCell="B17" sqref="B17"/>
+    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}">
+      <selection activeCell="A22" sqref="A22"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}">
+      <selection activeCell="G36" sqref="G36"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -9657,13 +9706,8 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}">
-      <selection activeCell="G36" sqref="G36"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}">
-      <selection activeCell="A22" sqref="A22"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
+      <selection activeCell="B17" sqref="B17"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>

</xml_diff>

<commit_message>
Poista oikeudet varustetoteumista muilta kuin järjestelmävastaavalta
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarihan/Jari/Tyo/Solita/Projektit/Harja/harja/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikkoro/Desktop/Sources/harja/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="47500" windowHeight="23300" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -23,11 +23,11 @@
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Mikko Rönkkömäki - Personal View" guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" mergeInterval="0" personalView="1" windowWidth="2560" windowHeight="1267" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office -käyttäjä - Oma näkymä" guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="1149" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
     <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="2375" windowHeight="992" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
-    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Microsoft Office -käyttäjä - Oma näkymä" guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="1149" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Mikko Rönkkömäki - Personal View" guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" mergeInterval="0" personalView="1" windowWidth="2560" windowHeight="1071" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -1324,7 +1324,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{375CDBCC-8E3D-0941-8323-5102D220C5C7}" diskRevisions="1" revisionId="648" version="28">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{D70D34AE-4624-304F-A0C5-E10200940432}" diskRevisions="1" revisionId="649" version="29">
   <header guid="{1E352813-0B26-DB4E-84BE-460845B77133}" dateTime="2017-06-20T12:32:37" maxSheetId="3" userName="Microsoft Office -käyttäjä" r:id="rId60" minRId="448" maxRId="464">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1493,6 +1493,12 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{D70D34AE-4624-304F-A0C5-E10200940432}" dateTime="2017-09-15T15:52:25" maxSheetId="3" userName="Mikko Rönkkömäki" r:id="rId88">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -3388,6 +3394,17 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog26.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcv guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" action="delete"/>
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_1DD617EE_F308_3E45_A8EF_4713F47FA0DD_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Oikeudet!$A$5:$Y$88</formula>
+    <oldFormula>Oikeudet!$A$5:$Y$88</oldFormula>
+  </rdn>
+  <rcv guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="497" sId="1">
@@ -4064,9 +4081,10 @@
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="2">
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="3">
   <userInfo guid="{1E352813-0B26-DB4E-84BE-460845B77133}" name="Microsoft Office -käyttäjä" id="-785751636" dateTime="2017-06-20T12:33:00"/>
   <userInfo guid="{1AB7A282-42ED-4740-A9CB-95FF229EC1A0}" name="Mikko Rönkkömäki" id="-727946492" dateTime="2017-06-22T10:45:48"/>
+  <userInfo guid="{D70D34AE-4624-304F-A0C5-E10200940432}" name="Mikko Rönkkömäki" id="-727973888" dateTime="2017-09-15T12:09:14"/>
 </users>
 </file>
 
@@ -4395,10 +4413,10 @@
   <dimension ref="A1:Y88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C64" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D78" sqref="D78"/>
+      <selection pane="bottomRight" activeCell="E19" sqref="E19:J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9382,9 +9400,21 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C64" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="D78" sqref="D78"/>
+    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="E19" sqref="E19:J19"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="C31" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
+      <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -9394,21 +9424,9 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
-      <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C31" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C48" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="D72" sqref="D72:X72"/>
+    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="C64" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="D78" sqref="D78"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -9431,8 +9449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9765,8 +9783,18 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="150">
+    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}">
+      <selection activeCell="A22" sqref="A22"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}">
       <selection activeCell="G36" sqref="G36"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
+      <selection activeCell="C7" sqref="C7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -9775,18 +9803,8 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
-      <selection activeCell="C7" sqref="C7"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}">
+    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="150">
       <selection activeCell="G36" sqref="G36"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}">
-      <selection activeCell="A22" sqref="A22"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>

</xml_diff>

<commit_message>
HAR-5985: Urakoitsija ei saa muokata kiintiöitä
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarihan/Jari/Tyo/Solita/Projektit/Harja/harja/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/teemukau/code/harja/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="47500" windowHeight="23300" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -23,11 +23,11 @@
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="2375" windowHeight="992" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="1280" windowHeight="600" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Mikko Rönkkömäki - Personal View" guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" mergeInterval="0" personalView="1" windowWidth="2560" windowHeight="1071" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office -käyttäjä - Oma näkymä" guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="1149" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
-    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Microsoft Office -käyttäjä - Oma näkymä" guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="1149" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Mikko Rönkkömäki - Personal View" guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" mergeInterval="0" personalView="1" windowWidth="2560" windowHeight="1071" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1402" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1402" uniqueCount="208">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -692,6 +692,12 @@
   </si>
   <si>
     <t>Häiriöilmoitukset</t>
+  </si>
+  <si>
+    <t>R+,irrota+</t>
+  </si>
+  <si>
+    <t>R,irrota</t>
   </si>
 </sst>
 </file>
@@ -1324,7 +1330,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{375CDBCC-8E3D-0941-8323-5102D220C5C7}" diskRevisions="1" revisionId="648" version="28">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{53E34551-370B-C144-87BF-D6D84A54E372}" diskRevisions="1" revisionId="654" version="29">
   <header guid="{1E352813-0B26-DB4E-84BE-460845B77133}" dateTime="2017-06-20T12:32:37" maxSheetId="3" userName="Microsoft Office -käyttäjä" r:id="rId60" minRId="448" maxRId="464">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1493,6 +1499,12 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{53E34551-370B-C144-87BF-D6D84A54E372}" dateTime="2017-09-21T07:50:07" maxSheetId="3" userName="Microsoft Office User" r:id="rId88" minRId="649" maxRId="653">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -3376,6 +3388,77 @@
     <nc r="D85" t="inlineStr">
       <is>
         <t>R*,W*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="delete"/>
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_7A9649F2_657F_9445_B6E6_FE94C6A09957_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Oikeudet!$A$5:$Y$88</formula>
+    <oldFormula>Oikeudet!$A$5:$Y$88</oldFormula>
+  </rdn>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog26.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="649" sId="1">
+    <oc r="R43" t="inlineStr">
+      <is>
+        <t>R+,W+</t>
+      </is>
+    </oc>
+    <nc r="R43" t="inlineStr">
+      <is>
+        <t>R+,irrota+</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="650" sId="1">
+    <oc r="S43" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </oc>
+    <nc r="S43" t="inlineStr">
+      <is>
+        <t>R,irrota</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="651" sId="1">
+    <oc r="T43" t="inlineStr">
+      <is>
+        <t>R+,W+</t>
+      </is>
+    </oc>
+    <nc r="T43" t="inlineStr">
+      <is>
+        <t>R+,irrota+</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="652" sId="1">
+    <oc r="U43" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </oc>
+    <nc r="U43" t="inlineStr">
+      <is>
+        <t>R,irrota</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="653" sId="1">
+    <oc r="V43" t="inlineStr">
+      <is>
+        <t>R+</t>
+      </is>
+    </oc>
+    <nc r="V43" t="inlineStr">
+      <is>
+        <t>R+,irrota+</t>
       </is>
     </nc>
   </rcc>
@@ -4395,10 +4478,10 @@
   <dimension ref="A1:Y88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C64" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="U41" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D78" sqref="D78"/>
+      <selection pane="bottomRight" activeCell="W48" sqref="W48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6823,19 +6906,19 @@
       <c r="P43" s="36"/>
       <c r="Q43" s="37"/>
       <c r="R43" s="37" t="s">
-        <v>131</v>
+        <v>206</v>
       </c>
       <c r="S43" s="37" t="s">
-        <v>112</v>
+        <v>207</v>
       </c>
       <c r="T43" s="37" t="s">
-        <v>131</v>
+        <v>206</v>
       </c>
       <c r="U43" s="37" t="s">
-        <v>16</v>
+        <v>207</v>
       </c>
       <c r="V43" s="36" t="s">
-        <v>130</v>
+        <v>206</v>
       </c>
       <c r="W43" s="37"/>
       <c r="X43" s="37"/>
@@ -9383,14 +9466,20 @@
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C64" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="D78" sqref="D78"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="U41" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="W48" sqref="W48"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
-      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
+    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="C48" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="D72" sqref="D72:X72"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="C31" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -9400,15 +9489,9 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C31" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C48" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="D72" sqref="D72:X72"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
+      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -9770,8 +9853,13 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
-      <selection activeCell="B17" sqref="B17"/>
+    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}">
+      <selection activeCell="A22" sqref="A22"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}">
+      <selection activeCell="G36" sqref="G36"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -9780,13 +9868,8 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}">
-      <selection activeCell="G36" sqref="G36"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}">
-      <selection activeCell="A22" sqref="A22"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
+      <selection activeCell="B17" sqref="B17"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>

</xml_diff>

<commit_message>
HAR-5974: Liikennevirastolle W-oikeus vesiväylien erilliskustannuksiin
Tiepuolella urakanvalvojia ovat ELY:läiset, mutta vesiväylien puolella
Liikennevirastolaiset. Tämän takia vesipuolella täytyy antaa kirjoitusoikeudet
erilliskustannuksiin Liikenneviraston edustajille.
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -9,25 +9,25 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
     <sheet name="Roolit" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$88</definedName>
-    <definedName name="Z_1DD617EE_F308_3E45_A8EF_4713F47FA0DD_.wvu.FilterData" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$88</definedName>
-    <definedName name="Z_7A9649F2_657F_9445_B6E6_FE94C6A09957_.wvu.FilterData" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$88</definedName>
-    <definedName name="Z_F86DF6F3_8AE5_3A44_B2D2_D623E01AE54F_.wvu.FilterData" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$88</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$89</definedName>
+    <definedName name="Z_1DD617EE_F308_3E45_A8EF_4713F47FA0DD_.wvu.FilterData" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$89</definedName>
+    <definedName name="Z_7A9649F2_657F_9445_B6E6_FE94C6A09957_.wvu.FilterData" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$89</definedName>
+    <definedName name="Z_F86DF6F3_8AE5_3A44_B2D2_D623E01AE54F_.wvu.FilterData" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$89</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
+    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office -käyttäjä - Oma näkymä" guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="1149" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Mikko Rönkkömäki - Personal View" guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" mergeInterval="0" personalView="1" windowWidth="2560" windowHeight="1071" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="1280" windowHeight="600" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Mikko Rönkkömäki - Personal View" guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" mergeInterval="0" personalView="1" windowWidth="2560" windowHeight="1071" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Microsoft Office -käyttäjä - Oma näkymä" guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="1149" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -46,7 +46,7 @@
     <author>Tatu Tarvainen</author>
   </authors>
   <commentList>
-    <comment ref="N28" authorId="0" guid="{DB5603A0-3291-7849-94B2-B86D15FBE193}">
+    <comment ref="N29" authorId="0" guid="{DB5603A0-3291-7849-94B2-B86D15FBE193}">
       <text>
         <r>
           <rPr>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1402" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1419" uniqueCount="209">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -698,6 +698,9 @@
   </si>
   <si>
     <t>R,irrota</t>
+  </si>
+  <si>
+    <t>Toteumat / Vesiväyläerilliskustannukset</t>
   </si>
 </sst>
 </file>
@@ -1018,7 +1021,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -1115,6 +1118,10 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1330,7 +1337,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{53E34551-370B-C144-87BF-D6D84A54E372}" diskRevisions="1" revisionId="654" version="29">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{4A189F6B-10A0-794F-AE26-98E1292E0A90}" diskRevisions="1" revisionId="675" version="30">
   <header guid="{1E352813-0B26-DB4E-84BE-460845B77133}" dateTime="2017-06-20T12:32:37" maxSheetId="3" userName="Microsoft Office -käyttäjä" r:id="rId60" minRId="448" maxRId="464">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1500,6 +1507,12 @@
     </sheetIdMap>
   </header>
   <header guid="{53E34551-370B-C144-87BF-D6D84A54E372}" dateTime="2017-09-21T07:50:07" maxSheetId="3" userName="Microsoft Office User" r:id="rId88" minRId="649" maxRId="653">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{4A189F6B-10A0-794F-AE26-98E1292E0A90}" dateTime="2017-09-21T08:13:09" maxSheetId="3" userName="Microsoft Office User" r:id="rId89" minRId="655" maxRId="675">
     <sheetIdMap count="2">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -3471,6 +3484,176 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog27.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="655" sId="1" ref="A18:XFD18" action="insertRow"/>
+  <rcc rId="656" sId="1">
+    <nc r="A18" t="inlineStr">
+      <is>
+        <t>Urakat</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="657" sId="1">
+    <nc r="B18" t="inlineStr">
+      <is>
+        <t>Toteumat / Erilliskustannukset</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="658" sId="1">
+    <nc r="D18" t="inlineStr">
+      <is>
+        <t>R*,W*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="659" sId="1">
+    <nc r="E18" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="660" sId="1">
+    <nc r="F18" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="G18" start="0" length="0">
+    <dxf/>
+  </rfmt>
+  <rfmt sheetId="1" sqref="H18" start="0" length="0">
+    <dxf/>
+  </rfmt>
+  <rfmt sheetId="1" sqref="I18" start="0" length="0">
+    <dxf/>
+  </rfmt>
+  <rcc rId="661" sId="1">
+    <nc r="J18" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="662" sId="1">
+    <nc r="K18" t="inlineStr">
+      <is>
+        <t>R*,W*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="663" sId="1">
+    <nc r="L18" t="inlineStr">
+      <is>
+        <t>R*,W</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="664" sId="1">
+    <nc r="N18" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="665" sId="1">
+    <nc r="Q18" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="666" sId="1">
+    <nc r="R18" t="inlineStr">
+      <is>
+        <t>R+</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="667" sId="1">
+    <nc r="S18" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="668" sId="1">
+    <nc r="U18" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="669" sId="1">
+    <nc r="V18" t="inlineStr">
+      <is>
+        <t>R+</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="670" sId="1">
+    <oc r="B19" t="inlineStr">
+      <is>
+        <t>Toteumat / Erilliskustannukset</t>
+      </is>
+    </oc>
+    <nc r="B19" t="inlineStr">
+      <is>
+        <t>Toteumat / Vesiväyläerilliskustannukset</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="671" sId="1">
+    <oc r="E19" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </oc>
+    <nc r="E19" t="inlineStr">
+      <is>
+        <t>R*,W</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="672" sId="1">
+    <oc r="F19" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </oc>
+    <nc r="F19" t="inlineStr">
+      <is>
+        <t>R*,W</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="673" sId="1">
+    <nc r="H19" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="674" sId="1">
+    <nc r="I19" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="675" sId="1">
+    <nc r="G19" t="inlineStr">
+      <is>
+        <t>R*,W</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="497" sId="1">
@@ -4147,9 +4330,10 @@
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="2">
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="3">
   <userInfo guid="{1E352813-0B26-DB4E-84BE-460845B77133}" name="Microsoft Office -käyttäjä" id="-785751636" dateTime="2017-06-20T12:33:00"/>
   <userInfo guid="{1AB7A282-42ED-4740-A9CB-95FF229EC1A0}" name="Mikko Rönkkömäki" id="-727946492" dateTime="2017-06-22T10:45:48"/>
+  <userInfo guid="{4A189F6B-10A0-794F-AE26-98E1292E0A90}" name="Microsoft Office User" id="-296987972" dateTime="2017-09-21T08:10:21"/>
 </users>
 </file>
 
@@ -4475,13 +4659,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y88"/>
+  <dimension ref="A1:Y89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="U41" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C14" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="W48" sqref="W48"/>
+      <selection pane="bottomRight" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4518,40 +4702,40 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="56" t="s">
+      <c r="C1" s="58" t="s">
         <v>150</v>
       </c>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="57"/>
-      <c r="O1" s="57"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="58" t="s">
+      <c r="C2" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="59"/>
-      <c r="M2" s="59"/>
-      <c r="N2" s="59"/>
-      <c r="O2" s="59"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="61"/>
+      <c r="N2" s="61"/>
+      <c r="O2" s="61"/>
     </row>
     <row r="3" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
@@ -4574,34 +4758,34 @@
     <row r="5" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="30"/>
       <c r="B5" s="30"/>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="54"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="56"/>
+      <c r="H5" s="56"/>
       <c r="I5" s="30"/>
       <c r="J5" s="30"/>
-      <c r="K5" s="55" t="s">
+      <c r="K5" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="L5" s="54"/>
-      <c r="M5" s="54"/>
-      <c r="N5" s="54"/>
-      <c r="O5" s="54"/>
+      <c r="L5" s="56"/>
+      <c r="M5" s="56"/>
+      <c r="N5" s="56"/>
+      <c r="O5" s="56"/>
       <c r="P5" s="30"/>
       <c r="Q5" s="30"/>
-      <c r="R5" s="55" t="s">
+      <c r="R5" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="S5" s="54"/>
-      <c r="T5" s="54"/>
-      <c r="U5" s="54"/>
-      <c r="V5" s="54"/>
-      <c r="W5" s="54"/>
-      <c r="X5" s="54"/>
+      <c r="S5" s="56"/>
+      <c r="T5" s="56"/>
+      <c r="U5" s="56"/>
+      <c r="V5" s="56"/>
+      <c r="W5" s="56"/>
+      <c r="X5" s="56"/>
       <c r="Y5" s="31" t="s">
         <v>13</v>
       </c>
@@ -5350,7 +5534,7 @@
       <c r="X17" s="36"/>
       <c r="Y17" s="38"/>
     </row>
-    <row r="18" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:25" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="35" t="s">
         <v>14</v>
       </c>
@@ -5403,65 +5587,59 @@
       </c>
       <c r="W18" s="36"/>
       <c r="X18" s="36"/>
-      <c r="Y18" s="38"/>
+      <c r="Y18" s="53"/>
     </row>
     <row r="19" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="35" t="s">
         <v>14</v>
       </c>
       <c r="B19" s="35" t="s">
-        <v>27</v>
+        <v>208</v>
       </c>
       <c r="C19" s="36"/>
       <c r="D19" s="36" t="s">
         <v>125</v>
       </c>
       <c r="E19" s="36" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="F19" s="36" t="s">
-        <v>126</v>
-      </c>
-      <c r="G19" s="36" t="s">
-        <v>126</v>
-      </c>
-      <c r="H19" s="36" t="s">
-        <v>126</v>
-      </c>
-      <c r="I19" s="36" t="s">
+        <v>129</v>
+      </c>
+      <c r="G19" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="H19" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="I19" s="37" t="s">
         <v>126</v>
       </c>
       <c r="J19" s="37" t="s">
-        <v>16</v>
+        <v>112</v>
       </c>
       <c r="K19" s="36" t="s">
         <v>125</v>
       </c>
       <c r="L19" s="36" t="s">
-        <v>125</v>
-      </c>
-      <c r="M19" s="36" t="s">
-        <v>16</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="M19" s="36"/>
       <c r="N19" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="O19" s="37" t="s">
-        <v>126</v>
-      </c>
+      <c r="O19" s="37"/>
       <c r="P19" s="36"/>
       <c r="Q19" s="37" t="s">
         <v>112</v>
       </c>
       <c r="R19" s="36" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="S19" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="T19" s="37" t="s">
-        <v>130</v>
-      </c>
+      <c r="T19" s="37"/>
       <c r="U19" s="37" t="s">
         <v>112</v>
       </c>
@@ -5477,20 +5655,20 @@
         <v>14</v>
       </c>
       <c r="B20" s="35" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20" s="36"/>
       <c r="D20" s="36" t="s">
         <v>125</v>
       </c>
       <c r="E20" s="36" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F20" s="36" t="s">
         <v>126</v>
       </c>
       <c r="G20" s="36" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H20" s="36" t="s">
         <v>126</v>
@@ -5499,16 +5677,16 @@
         <v>126</v>
       </c>
       <c r="J20" s="37" t="s">
-        <v>112</v>
+        <v>16</v>
       </c>
       <c r="K20" s="36" t="s">
         <v>125</v>
       </c>
       <c r="L20" s="36" t="s">
-        <v>129</v>
-      </c>
-      <c r="M20" s="37" t="s">
-        <v>112</v>
+        <v>125</v>
+      </c>
+      <c r="M20" s="36" t="s">
+        <v>16</v>
       </c>
       <c r="N20" s="37" t="s">
         <v>126</v>
@@ -5516,9 +5694,7 @@
       <c r="O20" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="P20" s="37" t="s">
-        <v>126</v>
-      </c>
+      <c r="P20" s="36"/>
       <c r="Q20" s="37" t="s">
         <v>112</v>
       </c>
@@ -5537,22 +5713,18 @@
       <c r="V20" s="36" t="s">
         <v>130</v>
       </c>
-      <c r="W20" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="X20" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="W20" s="36"/>
+      <c r="X20" s="36"/>
       <c r="Y20" s="38"/>
     </row>
     <row r="21" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="37"/>
+      <c r="B21" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="36"/>
       <c r="D21" s="36" t="s">
         <v>125</v>
       </c>
@@ -5598,7 +5770,7 @@
       <c r="R21" s="36" t="s">
         <v>131</v>
       </c>
-      <c r="S21" s="37" t="s">
+      <c r="S21" s="36" t="s">
         <v>112</v>
       </c>
       <c r="T21" s="37" t="s">
@@ -5610,7 +5782,7 @@
       <c r="V21" s="36" t="s">
         <v>130</v>
       </c>
-      <c r="W21" s="37" t="s">
+      <c r="W21" s="36" t="s">
         <v>16</v>
       </c>
       <c r="X21" s="37" t="s">
@@ -5623,11 +5795,11 @@
         <v>14</v>
       </c>
       <c r="B22" s="39" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C22" s="37"/>
       <c r="D22" s="36" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E22" s="36" t="s">
         <v>129</v>
@@ -5635,8 +5807,8 @@
       <c r="F22" s="36" t="s">
         <v>126</v>
       </c>
-      <c r="G22" s="37" t="s">
-        <v>126</v>
+      <c r="G22" s="36" t="s">
+        <v>128</v>
       </c>
       <c r="H22" s="36" t="s">
         <v>126</v>
@@ -5645,16 +5817,16 @@
         <v>126</v>
       </c>
       <c r="J22" s="37" t="s">
-        <v>157</v>
+        <v>112</v>
       </c>
       <c r="K22" s="36" t="s">
         <v>125</v>
       </c>
-      <c r="L22" s="37" t="s">
-        <v>132</v>
+      <c r="L22" s="36" t="s">
+        <v>129</v>
       </c>
       <c r="M22" s="37" t="s">
-        <v>16</v>
+        <v>112</v>
       </c>
       <c r="N22" s="37" t="s">
         <v>126</v>
@@ -5666,39 +5838,41 @@
         <v>126</v>
       </c>
       <c r="Q22" s="37" t="s">
-        <v>157</v>
-      </c>
-      <c r="R22" s="37" t="s">
-        <v>130</v>
+        <v>112</v>
+      </c>
+      <c r="R22" s="36" t="s">
+        <v>131</v>
       </c>
       <c r="S22" s="37" t="s">
-        <v>16</v>
+        <v>112</v>
       </c>
       <c r="T22" s="37" t="s">
         <v>130</v>
       </c>
       <c r="U22" s="37" t="s">
-        <v>16</v>
+        <v>112</v>
       </c>
       <c r="V22" s="36" t="s">
         <v>130</v>
       </c>
-      <c r="W22" s="37"/>
-      <c r="X22" s="37"/>
-      <c r="Y22" s="38" t="s">
-        <v>116</v>
-      </c>
+      <c r="W22" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="X22" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y22" s="38"/>
     </row>
     <row r="23" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="39" t="s">
         <v>14</v>
       </c>
       <c r="B23" s="39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" s="37"/>
       <c r="D23" s="36" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="E23" s="36" t="s">
         <v>129</v>
@@ -5716,13 +5890,13 @@
         <v>126</v>
       </c>
       <c r="J23" s="37" t="s">
-        <v>112</v>
+        <v>157</v>
       </c>
       <c r="K23" s="36" t="s">
         <v>125</v>
       </c>
       <c r="L23" s="37" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="M23" s="37" t="s">
         <v>16</v>
@@ -5737,40 +5911,42 @@
         <v>126</v>
       </c>
       <c r="Q23" s="37" t="s">
-        <v>112</v>
-      </c>
-      <c r="R23" s="36" t="s">
-        <v>131</v>
+        <v>157</v>
+      </c>
+      <c r="R23" s="37" t="s">
+        <v>130</v>
       </c>
       <c r="S23" s="37" t="s">
-        <v>112</v>
+        <v>16</v>
       </c>
       <c r="T23" s="37" t="s">
         <v>130</v>
       </c>
       <c r="U23" s="37" t="s">
-        <v>112</v>
+        <v>16</v>
       </c>
       <c r="V23" s="36" t="s">
         <v>130</v>
       </c>
       <c r="W23" s="37"/>
       <c r="X23" s="37"/>
-      <c r="Y23" s="38"/>
+      <c r="Y23" s="38" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="24" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="39" t="s">
         <v>14</v>
       </c>
       <c r="B24" s="39" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C24" s="37"/>
       <c r="D24" s="36" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="E24" s="36" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="F24" s="36" t="s">
         <v>126</v>
@@ -5785,13 +5961,13 @@
         <v>126</v>
       </c>
       <c r="J24" s="37" t="s">
-        <v>149</v>
+        <v>112</v>
       </c>
       <c r="K24" s="36" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="L24" s="37" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="M24" s="37" t="s">
         <v>16</v>
@@ -5802,151 +5978,167 @@
       <c r="O24" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="P24" s="37"/>
+      <c r="P24" s="37" t="s">
+        <v>126</v>
+      </c>
       <c r="Q24" s="37" t="s">
-        <v>149</v>
-      </c>
-      <c r="R24" s="37" t="s">
-        <v>148</v>
+        <v>112</v>
+      </c>
+      <c r="R24" s="36" t="s">
+        <v>131</v>
       </c>
       <c r="S24" s="37" t="s">
-        <v>149</v>
+        <v>112</v>
       </c>
       <c r="T24" s="37" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="U24" s="37" t="s">
-        <v>149</v>
+        <v>112</v>
       </c>
       <c r="V24" s="36" t="s">
         <v>130</v>
       </c>
       <c r="W24" s="37"/>
       <c r="X24" s="37"/>
-      <c r="Y24" s="38" t="s">
-        <v>138</v>
-      </c>
+      <c r="Y24" s="38"/>
     </row>
     <row r="25" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="39" t="s">
         <v>14</v>
       </c>
       <c r="B25" s="39" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C25" s="37"/>
       <c r="D25" s="36" t="s">
-        <v>125</v>
+        <v>139</v>
       </c>
       <c r="E25" s="36" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="F25" s="36" t="s">
         <v>126</v>
       </c>
-      <c r="G25" s="37"/>
-      <c r="H25" s="37"/>
-      <c r="I25" s="37" t="s">
-        <v>125</v>
+      <c r="G25" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="H25" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="I25" s="36" t="s">
+        <v>126</v>
       </c>
       <c r="J25" s="37" t="s">
-        <v>112</v>
+        <v>149</v>
       </c>
       <c r="K25" s="36" t="s">
-        <v>125</v>
+        <v>139</v>
       </c>
       <c r="L25" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="M25" s="37"/>
+        <v>140</v>
+      </c>
+      <c r="M25" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="N25" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="O25" s="37"/>
-      <c r="P25" s="37" t="s">
-        <v>128</v>
-      </c>
+      <c r="O25" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="P25" s="37"/>
       <c r="Q25" s="37" t="s">
-        <v>112</v>
-      </c>
-      <c r="R25" s="36" t="s">
-        <v>131</v>
+        <v>149</v>
+      </c>
+      <c r="R25" s="37" t="s">
+        <v>148</v>
       </c>
       <c r="S25" s="37" t="s">
-        <v>112</v>
+        <v>149</v>
       </c>
       <c r="T25" s="37" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="U25" s="37" t="s">
-        <v>112</v>
-      </c>
-      <c r="V25" s="37" t="s">
+        <v>149</v>
+      </c>
+      <c r="V25" s="36" t="s">
         <v>130</v>
       </c>
       <c r="W25" s="37"/>
       <c r="X25" s="37"/>
-      <c r="Y25" s="38"/>
+      <c r="Y25" s="38" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="26" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="39" t="s">
         <v>14</v>
       </c>
       <c r="B26" s="39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C26" s="37"/>
       <c r="D26" s="36" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E26" s="36" t="s">
-        <v>126</v>
-      </c>
-      <c r="F26" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="F26" s="36" t="s">
         <v>126</v>
       </c>
       <c r="G26" s="37"/>
       <c r="H26" s="37"/>
-      <c r="I26" s="37"/>
+      <c r="I26" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="J26" s="37" t="s">
-        <v>16</v>
+        <v>112</v>
       </c>
       <c r="K26" s="36" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L26" s="37" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="M26" s="37"/>
       <c r="N26" s="37" t="s">
         <v>126</v>
       </c>
       <c r="O26" s="37"/>
-      <c r="P26" s="37"/>
+      <c r="P26" s="37" t="s">
+        <v>128</v>
+      </c>
       <c r="Q26" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="R26" s="37" t="s">
-        <v>130</v>
+        <v>112</v>
+      </c>
+      <c r="R26" s="36" t="s">
+        <v>131</v>
       </c>
       <c r="S26" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="T26" s="37"/>
-      <c r="U26" s="37"/>
-      <c r="V26" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="T26" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="U26" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="V26" s="37" t="s">
         <v>130</v>
       </c>
       <c r="W26" s="37"/>
       <c r="X26" s="37"/>
       <c r="Y26" s="38"/>
     </row>
-    <row r="27" spans="1:25" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="39" t="s">
         <v>14</v>
       </c>
       <c r="B27" s="39" t="s">
-        <v>201</v>
+        <v>34</v>
       </c>
       <c r="C27" s="37"/>
       <c r="D27" s="36" t="s">
@@ -5964,13 +6156,21 @@
       <c r="J27" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="K27" s="36"/>
-      <c r="L27" s="37"/>
+      <c r="K27" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="L27" s="37" t="s">
+        <v>126</v>
+      </c>
       <c r="M27" s="37"/>
-      <c r="N27" s="37"/>
+      <c r="N27" s="37" t="s">
+        <v>126</v>
+      </c>
       <c r="O27" s="37"/>
       <c r="P27" s="37"/>
-      <c r="Q27" s="37"/>
+      <c r="Q27" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="R27" s="37" t="s">
         <v>130</v>
       </c>
@@ -5986,81 +6186,77 @@
       <c r="X27" s="37"/>
       <c r="Y27" s="38"/>
     </row>
-    <row r="28" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:25" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="39" t="s">
         <v>14</v>
       </c>
       <c r="B28" s="39" t="s">
-        <v>35</v>
+        <v>201</v>
       </c>
       <c r="C28" s="37"/>
       <c r="D28" s="36" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E28" s="36" t="s">
-        <v>129</v>
-      </c>
-      <c r="F28" s="37"/>
+        <v>126</v>
+      </c>
+      <c r="F28" s="37" t="s">
+        <v>126</v>
+      </c>
       <c r="G28" s="37"/>
       <c r="H28" s="37"/>
       <c r="I28" s="37"/>
       <c r="J28" s="37" t="s">
-        <v>112</v>
-      </c>
-      <c r="K28" s="36" t="s">
-        <v>125</v>
-      </c>
-      <c r="L28" s="37" t="s">
-        <v>129</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="K28" s="36"/>
+      <c r="L28" s="37"/>
       <c r="M28" s="37"/>
-      <c r="N28" s="37" t="s">
-        <v>126</v>
-      </c>
+      <c r="N28" s="37"/>
       <c r="O28" s="37"/>
       <c r="P28" s="37"/>
-      <c r="Q28" s="37" t="s">
-        <v>112</v>
-      </c>
-      <c r="R28" s="37"/>
-      <c r="S28" s="37"/>
+      <c r="Q28" s="37"/>
+      <c r="R28" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="S28" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="T28" s="37"/>
       <c r="U28" s="37"/>
-      <c r="V28" s="37"/>
+      <c r="V28" s="36" t="s">
+        <v>130</v>
+      </c>
       <c r="W28" s="37"/>
       <c r="X28" s="37"/>
-      <c r="Y28" s="38" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="29" spans="1:25" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="Y28" s="38"/>
+    </row>
+    <row r="29" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="39" t="s">
         <v>14</v>
       </c>
       <c r="B29" s="39" t="s">
-        <v>170</v>
+        <v>35</v>
       </c>
       <c r="C29" s="37"/>
       <c r="D29" s="36" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E29" s="36" t="s">
-        <v>126</v>
-      </c>
-      <c r="F29" s="37" t="s">
-        <v>126</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="F29" s="37"/>
       <c r="G29" s="37"/>
       <c r="H29" s="37"/>
       <c r="I29" s="37"/>
       <c r="J29" s="37" t="s">
-        <v>16</v>
+        <v>112</v>
       </c>
       <c r="K29" s="36" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L29" s="37" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="M29" s="37"/>
       <c r="N29" s="37" t="s">
@@ -6069,126 +6265,110 @@
       <c r="O29" s="37"/>
       <c r="P29" s="37"/>
       <c r="Q29" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="R29" s="37" t="s">
-        <v>130</v>
-      </c>
-      <c r="S29" s="37" t="s">
-        <v>16</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="R29" s="37"/>
+      <c r="S29" s="37"/>
       <c r="T29" s="37"/>
       <c r="U29" s="37"/>
-      <c r="V29" s="36" t="s">
-        <v>130</v>
-      </c>
+      <c r="V29" s="37"/>
       <c r="W29" s="37"/>
       <c r="X29" s="37"/>
-      <c r="Y29" s="38"/>
-    </row>
-    <row r="30" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="Y29" s="38" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="39" t="s">
         <v>14</v>
       </c>
       <c r="B30" s="39" t="s">
-        <v>37</v>
+        <v>170</v>
       </c>
       <c r="C30" s="37"/>
       <c r="D30" s="36" t="s">
-        <v>151</v>
+        <v>126</v>
       </c>
       <c r="E30" s="36" t="s">
-        <v>156</v>
+        <v>126</v>
       </c>
       <c r="F30" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="G30" s="36" t="s">
-        <v>129</v>
-      </c>
-      <c r="H30" s="37" t="s">
-        <v>126</v>
-      </c>
-      <c r="I30" s="37" t="s">
-        <v>126</v>
-      </c>
-      <c r="J30" s="40" t="s">
-        <v>158</v>
+      <c r="G30" s="37"/>
+      <c r="H30" s="37"/>
+      <c r="I30" s="37"/>
+      <c r="J30" s="37" t="s">
+        <v>16</v>
       </c>
       <c r="K30" s="36" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L30" s="37" t="s">
-        <v>156</v>
-      </c>
-      <c r="M30" s="37" t="s">
-        <v>112</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="M30" s="37"/>
       <c r="N30" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="O30" s="36" t="s">
-        <v>126</v>
-      </c>
+      <c r="O30" s="37"/>
       <c r="P30" s="37"/>
-      <c r="Q30" s="40" t="s">
-        <v>158</v>
+      <c r="Q30" s="37" t="s">
+        <v>16</v>
       </c>
       <c r="R30" s="37" t="s">
-        <v>167</v>
+        <v>130</v>
       </c>
       <c r="S30" s="37" t="s">
-        <v>166</v>
-      </c>
-      <c r="T30" s="37" t="s">
-        <v>130</v>
-      </c>
-      <c r="U30" s="37" t="s">
-        <v>16</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="T30" s="37"/>
+      <c r="U30" s="37"/>
       <c r="V30" s="36" t="s">
         <v>130</v>
       </c>
       <c r="W30" s="37"/>
       <c r="X30" s="37"/>
-      <c r="Y30" s="38" t="s">
-        <v>117</v>
-      </c>
+      <c r="Y30" s="38"/>
     </row>
     <row r="31" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="39" t="s">
         <v>14</v>
       </c>
       <c r="B31" s="39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C31" s="37"/>
-      <c r="D31" s="37" t="s">
-        <v>136</v>
-      </c>
-      <c r="E31" s="37" t="s">
-        <v>133</v>
+      <c r="D31" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="E31" s="36" t="s">
+        <v>156</v>
       </c>
       <c r="F31" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="G31" s="37"/>
+      <c r="G31" s="36" t="s">
+        <v>129</v>
+      </c>
       <c r="H31" s="37" t="s">
         <v>126</v>
       </c>
       <c r="I31" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="J31" s="37" t="s">
+      <c r="J31" s="40" t="s">
+        <v>158</v>
+      </c>
+      <c r="K31" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="L31" s="37" t="s">
+        <v>156</v>
+      </c>
+      <c r="M31" s="37" t="s">
         <v>112</v>
       </c>
-      <c r="K31" s="36" t="s">
-        <v>168</v>
-      </c>
-      <c r="L31" s="37" t="s">
-        <v>133</v>
-      </c>
-      <c r="M31" s="37"/>
       <c r="N31" s="37" t="s">
         <v>126</v>
       </c>
@@ -6196,14 +6376,14 @@
         <v>126</v>
       </c>
       <c r="P31" s="37"/>
-      <c r="Q31" s="37" t="s">
-        <v>169</v>
+      <c r="Q31" s="40" t="s">
+        <v>158</v>
       </c>
       <c r="R31" s="37" t="s">
-        <v>131</v>
+        <v>167</v>
       </c>
       <c r="S31" s="37" t="s">
-        <v>112</v>
+        <v>166</v>
       </c>
       <c r="T31" s="37" t="s">
         <v>130</v>
@@ -6216,28 +6396,28 @@
       </c>
       <c r="W31" s="37"/>
       <c r="X31" s="37"/>
-      <c r="Y31" s="38"/>
+      <c r="Y31" s="38" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="32" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="39" t="s">
         <v>14</v>
       </c>
       <c r="B32" s="39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C32" s="37"/>
-      <c r="D32" s="36" t="s">
-        <v>141</v>
-      </c>
-      <c r="E32" s="36" t="s">
-        <v>129</v>
+      <c r="D32" s="37" t="s">
+        <v>136</v>
+      </c>
+      <c r="E32" s="37" t="s">
+        <v>133</v>
       </c>
       <c r="F32" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="G32" s="37" t="s">
-        <v>134</v>
-      </c>
+      <c r="G32" s="37"/>
       <c r="H32" s="37" t="s">
         <v>126</v>
       </c>
@@ -6245,13 +6425,13 @@
         <v>126</v>
       </c>
       <c r="J32" s="37" t="s">
-        <v>157</v>
+        <v>112</v>
       </c>
       <c r="K32" s="36" t="s">
-        <v>125</v>
+        <v>168</v>
       </c>
       <c r="L32" s="37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="M32" s="37"/>
       <c r="N32" s="37" t="s">
@@ -6262,7 +6442,7 @@
       </c>
       <c r="P32" s="37"/>
       <c r="Q32" s="37" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="R32" s="37" t="s">
         <v>131</v>
@@ -6288,19 +6468,21 @@
         <v>14</v>
       </c>
       <c r="B33" s="39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C33" s="37"/>
-      <c r="D33" s="37" t="s">
-        <v>136</v>
-      </c>
-      <c r="E33" s="37" t="s">
-        <v>133</v>
+      <c r="D33" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="E33" s="36" t="s">
+        <v>129</v>
       </c>
       <c r="F33" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="G33" s="37"/>
+      <c r="G33" s="37" t="s">
+        <v>134</v>
+      </c>
       <c r="H33" s="37" t="s">
         <v>126</v>
       </c>
@@ -6308,13 +6490,13 @@
         <v>126</v>
       </c>
       <c r="J33" s="37" t="s">
-        <v>112</v>
+        <v>157</v>
       </c>
       <c r="K33" s="36" t="s">
-        <v>168</v>
+        <v>125</v>
       </c>
       <c r="L33" s="37" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M33" s="37"/>
       <c r="N33" s="37" t="s">
@@ -6325,7 +6507,7 @@
       </c>
       <c r="P33" s="37"/>
       <c r="Q33" s="37" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="R33" s="37" t="s">
         <v>131</v>
@@ -6351,14 +6533,14 @@
         <v>14</v>
       </c>
       <c r="B34" s="39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C34" s="37"/>
-      <c r="D34" s="36" t="s">
-        <v>135</v>
-      </c>
-      <c r="E34" s="36" t="s">
-        <v>129</v>
+      <c r="D34" s="37" t="s">
+        <v>136</v>
+      </c>
+      <c r="E34" s="37" t="s">
+        <v>133</v>
       </c>
       <c r="F34" s="37" t="s">
         <v>126</v>
@@ -6374,10 +6556,10 @@
         <v>112</v>
       </c>
       <c r="K34" s="36" t="s">
-        <v>125</v>
+        <v>168</v>
       </c>
       <c r="L34" s="37" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="M34" s="37"/>
       <c r="N34" s="37" t="s">
@@ -6388,7 +6570,7 @@
       </c>
       <c r="P34" s="37"/>
       <c r="Q34" s="37" t="s">
-        <v>112</v>
+        <v>169</v>
       </c>
       <c r="R34" s="37" t="s">
         <v>131</v>
@@ -6409,19 +6591,19 @@
       <c r="X34" s="37"/>
       <c r="Y34" s="38"/>
     </row>
-    <row r="35" spans="1:25" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="39" t="s">
         <v>14</v>
       </c>
       <c r="B35" s="39" t="s">
-        <v>174</v>
+        <v>41</v>
       </c>
       <c r="C35" s="37"/>
       <c r="D35" s="36" t="s">
-        <v>179</v>
+        <v>135</v>
       </c>
       <c r="E35" s="36" t="s">
-        <v>175</v>
+        <v>129</v>
       </c>
       <c r="F35" s="37" t="s">
         <v>126</v>
@@ -6437,10 +6619,10 @@
         <v>112</v>
       </c>
       <c r="K35" s="36" t="s">
-        <v>176</v>
+        <v>125</v>
       </c>
       <c r="L35" s="37" t="s">
-        <v>175</v>
+        <v>129</v>
       </c>
       <c r="M35" s="37"/>
       <c r="N35" s="37" t="s">
@@ -6454,10 +6636,10 @@
         <v>112</v>
       </c>
       <c r="R35" s="37" t="s">
-        <v>177</v>
+        <v>131</v>
       </c>
       <c r="S35" s="37" t="s">
-        <v>178</v>
+        <v>112</v>
       </c>
       <c r="T35" s="37" t="s">
         <v>130</v>
@@ -6472,19 +6654,19 @@
       <c r="X35" s="37"/>
       <c r="Y35" s="38"/>
     </row>
-    <row r="36" spans="1:25" s="18" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:25" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="39" t="s">
         <v>14</v>
       </c>
       <c r="B36" s="39" t="s">
-        <v>152</v>
+        <v>174</v>
       </c>
       <c r="C36" s="37"/>
       <c r="D36" s="36" t="s">
-        <v>125</v>
+        <v>179</v>
       </c>
       <c r="E36" s="36" t="s">
-        <v>129</v>
+        <v>175</v>
       </c>
       <c r="F36" s="37" t="s">
         <v>126</v>
@@ -6500,10 +6682,10 @@
         <v>112</v>
       </c>
       <c r="K36" s="36" t="s">
-        <v>125</v>
+        <v>176</v>
       </c>
       <c r="L36" s="37" t="s">
-        <v>129</v>
+        <v>175</v>
       </c>
       <c r="M36" s="37"/>
       <c r="N36" s="37" t="s">
@@ -6512,15 +6694,15 @@
       <c r="O36" s="36" t="s">
         <v>126</v>
       </c>
-      <c r="P36" s="36"/>
+      <c r="P36" s="37"/>
       <c r="Q36" s="37" t="s">
         <v>112</v>
       </c>
       <c r="R36" s="37" t="s">
-        <v>131</v>
+        <v>177</v>
       </c>
       <c r="S36" s="37" t="s">
-        <v>112</v>
+        <v>178</v>
       </c>
       <c r="T36" s="37" t="s">
         <v>130</v>
@@ -6533,14 +6715,14 @@
       </c>
       <c r="W36" s="37"/>
       <c r="X36" s="37"/>
-      <c r="Y36" s="30"/>
+      <c r="Y36" s="38"/>
     </row>
     <row r="37" spans="1:25" s="18" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="39" t="s">
         <v>14</v>
       </c>
       <c r="B37" s="39" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C37" s="37"/>
       <c r="D37" s="36" t="s">
@@ -6603,7 +6785,7 @@
         <v>14</v>
       </c>
       <c r="B38" s="39" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="C38" s="37"/>
       <c r="D38" s="36" t="s">
@@ -6661,12 +6843,12 @@
       <c r="X38" s="37"/>
       <c r="Y38" s="30"/>
     </row>
-    <row r="39" spans="1:25" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:25" s="18" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="39" t="s">
         <v>14</v>
       </c>
       <c r="B39" s="39" t="s">
-        <v>115</v>
+        <v>173</v>
       </c>
       <c r="C39" s="37"/>
       <c r="D39" s="36" t="s">
@@ -6678,14 +6860,12 @@
       <c r="F39" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="G39" s="37" t="s">
-        <v>128</v>
-      </c>
+      <c r="G39" s="37"/>
       <c r="H39" s="37" t="s">
         <v>126</v>
       </c>
       <c r="I39" s="37" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="J39" s="37" t="s">
         <v>112</v>
@@ -6694,20 +6874,16 @@
         <v>125</v>
       </c>
       <c r="L39" s="37" t="s">
-        <v>132</v>
-      </c>
-      <c r="M39" s="37" t="s">
-        <v>112</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="M39" s="37"/>
       <c r="N39" s="37" t="s">
         <v>126</v>
       </c>
       <c r="O39" s="36" t="s">
         <v>126</v>
       </c>
-      <c r="P39" s="36" t="s">
-        <v>126</v>
-      </c>
+      <c r="P39" s="36"/>
       <c r="Q39" s="37" t="s">
         <v>112</v>
       </c>
@@ -6721,85 +6897,101 @@
         <v>130</v>
       </c>
       <c r="U39" s="37" t="s">
-        <v>112</v>
+        <v>16</v>
       </c>
       <c r="V39" s="36" t="s">
         <v>130</v>
       </c>
-      <c r="W39" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="X39" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y39" s="38"/>
-    </row>
-    <row r="40" spans="1:25" s="25" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+      <c r="W39" s="37"/>
+      <c r="X39" s="37"/>
+      <c r="Y39" s="30"/>
+    </row>
+    <row r="40" spans="1:25" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="39" t="s">
         <v>14</v>
       </c>
       <c r="B40" s="39" t="s">
-        <v>181</v>
+        <v>115</v>
       </c>
       <c r="C40" s="37"/>
-      <c r="D40" s="41" t="s">
-        <v>191</v>
-      </c>
-      <c r="E40" s="41" t="s">
-        <v>192</v>
+      <c r="D40" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="E40" s="36" t="s">
+        <v>129</v>
       </c>
       <c r="F40" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="G40" s="37"/>
+      <c r="G40" s="37" t="s">
+        <v>128</v>
+      </c>
       <c r="H40" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="I40" s="36"/>
-      <c r="J40" s="41" t="s">
-        <v>199</v>
-      </c>
-      <c r="K40" s="36"/>
-      <c r="L40" s="37"/>
-      <c r="M40" s="37"/>
-      <c r="N40" s="37"/>
-      <c r="O40" s="36"/>
-      <c r="P40" s="36"/>
-      <c r="Q40" s="37"/>
-      <c r="R40" s="41" t="s">
-        <v>193</v>
-      </c>
-      <c r="S40" s="50" t="s">
-        <v>199</v>
+      <c r="I40" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="J40" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="K40" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="L40" s="37" t="s">
+        <v>132</v>
+      </c>
+      <c r="M40" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="N40" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="O40" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="P40" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q40" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="R40" s="37" t="s">
+        <v>131</v>
+      </c>
+      <c r="S40" s="37" t="s">
+        <v>112</v>
       </c>
       <c r="T40" s="37" t="s">
         <v>130</v>
       </c>
       <c r="U40" s="37" t="s">
-        <v>16</v>
+        <v>112</v>
       </c>
       <c r="V40" s="36" t="s">
         <v>130</v>
       </c>
-      <c r="W40" s="37"/>
-      <c r="X40" s="37"/>
-      <c r="Y40" s="38" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="41" spans="1:25" s="25" customFormat="1" ht="65" x14ac:dyDescent="0.15">
+      <c r="W40" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="X40" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y40" s="38"/>
+    </row>
+    <row r="41" spans="1:25" s="25" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="A41" s="39" t="s">
         <v>14</v>
       </c>
       <c r="B41" s="39" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C41" s="37"/>
       <c r="D41" s="41" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="E41" s="41" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="F41" s="37" t="s">
         <v>126</v>
@@ -6808,22 +7000,22 @@
       <c r="H41" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="I41" s="37"/>
+      <c r="I41" s="36"/>
       <c r="J41" s="41" t="s">
-        <v>200</v>
-      </c>
-      <c r="K41" s="41"/>
-      <c r="L41" s="41"/>
+        <v>199</v>
+      </c>
+      <c r="K41" s="36"/>
+      <c r="L41" s="37"/>
       <c r="M41" s="37"/>
       <c r="N41" s="37"/>
       <c r="O41" s="36"/>
       <c r="P41" s="36"/>
       <c r="Q41" s="37"/>
       <c r="R41" s="41" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="S41" s="50" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="T41" s="37" t="s">
         <v>130</v>
@@ -6837,153 +7029,165 @@
       <c r="W41" s="37"/>
       <c r="X41" s="37"/>
       <c r="Y41" s="38" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="42" spans="1:25" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" s="25" customFormat="1" ht="65" x14ac:dyDescent="0.15">
       <c r="A42" s="39" t="s">
         <v>14</v>
       </c>
       <c r="B42" s="39" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C42" s="37"/>
-      <c r="D42" s="36" t="s">
-        <v>125</v>
-      </c>
-      <c r="E42" s="36"/>
-      <c r="F42" s="37"/>
+      <c r="D42" s="41" t="s">
+        <v>196</v>
+      </c>
+      <c r="E42" s="41" t="s">
+        <v>197</v>
+      </c>
+      <c r="F42" s="37" t="s">
+        <v>126</v>
+      </c>
       <c r="G42" s="37"/>
-      <c r="H42" s="37"/>
+      <c r="H42" s="37" t="s">
+        <v>126</v>
+      </c>
       <c r="I42" s="37"/>
-      <c r="J42" s="37"/>
-      <c r="K42" s="36"/>
-      <c r="L42" s="37"/>
+      <c r="J42" s="41" t="s">
+        <v>200</v>
+      </c>
+      <c r="K42" s="41"/>
+      <c r="L42" s="41"/>
       <c r="M42" s="37"/>
       <c r="N42" s="37"/>
       <c r="O42" s="36"/>
       <c r="P42" s="36"/>
       <c r="Q42" s="37"/>
-      <c r="R42" s="37"/>
-      <c r="S42" s="37"/>
-      <c r="T42" s="37"/>
-      <c r="U42" s="37"/>
-      <c r="V42" s="36"/>
+      <c r="R42" s="41" t="s">
+        <v>203</v>
+      </c>
+      <c r="S42" s="50" t="s">
+        <v>204</v>
+      </c>
+      <c r="T42" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="U42" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="V42" s="36" t="s">
+        <v>130</v>
+      </c>
       <c r="W42" s="37"/>
       <c r="X42" s="37"/>
-      <c r="Y42" s="38"/>
-    </row>
-    <row r="43" spans="1:25" s="26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="Y42" s="38" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="39" t="s">
         <v>14</v>
       </c>
       <c r="B43" s="39" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C43" s="37"/>
       <c r="D43" s="36" t="s">
-        <v>188</v>
-      </c>
-      <c r="E43" s="30" t="s">
-        <v>190</v>
-      </c>
-      <c r="F43" s="37" t="s">
-        <v>126</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="E43" s="36"/>
+      <c r="F43" s="37"/>
       <c r="G43" s="37"/>
-      <c r="H43" s="37" t="s">
-        <v>126</v>
-      </c>
+      <c r="H43" s="37"/>
       <c r="I43" s="37"/>
-      <c r="J43" s="37" t="s">
-        <v>189</v>
-      </c>
+      <c r="J43" s="37"/>
       <c r="K43" s="36"/>
-      <c r="L43" s="36"/>
+      <c r="L43" s="37"/>
       <c r="M43" s="37"/>
       <c r="N43" s="37"/>
       <c r="O43" s="36"/>
       <c r="P43" s="36"/>
       <c r="Q43" s="37"/>
-      <c r="R43" s="37" t="s">
-        <v>206</v>
-      </c>
-      <c r="S43" s="37" t="s">
-        <v>207</v>
-      </c>
-      <c r="T43" s="37" t="s">
-        <v>206</v>
-      </c>
-      <c r="U43" s="37" t="s">
-        <v>207</v>
-      </c>
-      <c r="V43" s="36" t="s">
-        <v>206</v>
-      </c>
+      <c r="R43" s="37"/>
+      <c r="S43" s="37"/>
+      <c r="T43" s="37"/>
+      <c r="U43" s="37"/>
+      <c r="V43" s="36"/>
       <c r="W43" s="37"/>
       <c r="X43" s="37"/>
-      <c r="Y43" s="38" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="44" spans="1:25" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="Y43" s="38"/>
+    </row>
+    <row r="44" spans="1:25" s="26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="39" t="s">
         <v>14</v>
       </c>
       <c r="B44" s="39" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C44" s="37"/>
       <c r="D44" s="36" t="s">
-        <v>125</v>
-      </c>
-      <c r="E44" s="36"/>
-      <c r="F44" s="37"/>
+        <v>188</v>
+      </c>
+      <c r="E44" s="30" t="s">
+        <v>190</v>
+      </c>
+      <c r="F44" s="37" t="s">
+        <v>126</v>
+      </c>
       <c r="G44" s="37"/>
-      <c r="H44" s="37"/>
+      <c r="H44" s="37" t="s">
+        <v>126</v>
+      </c>
       <c r="I44" s="37"/>
-      <c r="J44" s="37"/>
+      <c r="J44" s="37" t="s">
+        <v>189</v>
+      </c>
       <c r="K44" s="36"/>
-      <c r="L44" s="37"/>
+      <c r="L44" s="36"/>
       <c r="M44" s="37"/>
       <c r="N44" s="37"/>
       <c r="O44" s="36"/>
       <c r="P44" s="36"/>
       <c r="Q44" s="37"/>
-      <c r="R44" s="37"/>
-      <c r="S44" s="37"/>
-      <c r="T44" s="37"/>
-      <c r="U44" s="37"/>
-      <c r="V44" s="36"/>
+      <c r="R44" s="37" t="s">
+        <v>206</v>
+      </c>
+      <c r="S44" s="37" t="s">
+        <v>207</v>
+      </c>
+      <c r="T44" s="37" t="s">
+        <v>206</v>
+      </c>
+      <c r="U44" s="37" t="s">
+        <v>207</v>
+      </c>
+      <c r="V44" s="36" t="s">
+        <v>206</v>
+      </c>
       <c r="W44" s="37"/>
       <c r="X44" s="37"/>
-      <c r="Y44" s="38"/>
-    </row>
-    <row r="45" spans="1:25" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="Y44" s="38" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="39" t="s">
         <v>14</v>
       </c>
       <c r="B45" s="39" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C45" s="37"/>
       <c r="D45" s="36" t="s">
         <v>125</v>
       </c>
-      <c r="E45" s="36" t="s">
-        <v>129</v>
-      </c>
-      <c r="F45" s="37" t="s">
-        <v>126</v>
-      </c>
+      <c r="E45" s="36"/>
+      <c r="F45" s="37"/>
       <c r="G45" s="37"/>
-      <c r="H45" s="37" t="s">
-        <v>126</v>
-      </c>
+      <c r="H45" s="37"/>
       <c r="I45" s="37"/>
-      <c r="J45" s="37" t="s">
-        <v>112</v>
-      </c>
+      <c r="J45" s="37"/>
       <c r="K45" s="36"/>
       <c r="L45" s="37"/>
       <c r="M45" s="37"/>
@@ -6991,84 +7195,72 @@
       <c r="O45" s="36"/>
       <c r="P45" s="36"/>
       <c r="Q45" s="37"/>
-      <c r="R45" s="37" t="s">
-        <v>131</v>
-      </c>
-      <c r="S45" s="37" t="s">
-        <v>112</v>
-      </c>
-      <c r="T45" s="37" t="s">
-        <v>130</v>
-      </c>
-      <c r="U45" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="V45" s="36" t="s">
-        <v>130</v>
-      </c>
+      <c r="R45" s="37"/>
+      <c r="S45" s="37"/>
+      <c r="T45" s="37"/>
+      <c r="U45" s="37"/>
+      <c r="V45" s="36"/>
       <c r="W45" s="37"/>
       <c r="X45" s="37"/>
       <c r="Y45" s="38"/>
     </row>
-    <row r="46" spans="1:25" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:25" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="39" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="B46" s="39" t="s">
-        <v>122</v>
+        <v>186</v>
       </c>
       <c r="C46" s="37"/>
       <c r="D46" s="36" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E46" s="36" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="F46" s="37" t="s">
         <v>126</v>
       </c>
       <c r="G46" s="37"/>
-      <c r="H46" s="37"/>
+      <c r="H46" s="37" t="s">
+        <v>126</v>
+      </c>
       <c r="I46" s="37"/>
       <c r="J46" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="K46" s="37" t="s">
-        <v>126</v>
-      </c>
-      <c r="L46" s="37" t="s">
-        <v>126</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="K46" s="36"/>
+      <c r="L46" s="37"/>
       <c r="M46" s="37"/>
-      <c r="N46" s="37" t="s">
-        <v>126</v>
-      </c>
-      <c r="O46" s="37"/>
-      <c r="P46" s="37"/>
-      <c r="Q46" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="N46" s="37"/>
+      <c r="O46" s="36"/>
+      <c r="P46" s="36"/>
+      <c r="Q46" s="37"/>
       <c r="R46" s="37" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="S46" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="T46" s="37"/>
-      <c r="U46" s="37"/>
-      <c r="V46" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="T46" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="U46" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="V46" s="36" t="s">
         <v>130</v>
       </c>
       <c r="W46" s="37"/>
       <c r="X46" s="37"/>
       <c r="Y46" s="38"/>
     </row>
-    <row r="47" spans="1:25" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:25" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B47" s="39" t="s">
-        <v>202</v>
+        <v>122</v>
       </c>
       <c r="C47" s="37"/>
       <c r="D47" s="36" t="s">
@@ -7089,12 +7281,18 @@
       <c r="K47" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="L47" s="37"/>
+      <c r="L47" s="37" t="s">
+        <v>126</v>
+      </c>
       <c r="M47" s="37"/>
-      <c r="N47" s="37"/>
+      <c r="N47" s="37" t="s">
+        <v>126</v>
+      </c>
       <c r="O47" s="37"/>
       <c r="P47" s="37"/>
-      <c r="Q47" s="37"/>
+      <c r="Q47" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="R47" s="37" t="s">
         <v>130</v>
       </c>
@@ -7110,12 +7308,12 @@
       <c r="X47" s="37"/>
       <c r="Y47" s="38"/>
     </row>
-    <row r="48" spans="1:25" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:25" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B48" s="39" t="s">
-        <v>171</v>
+        <v>202</v>
       </c>
       <c r="C48" s="37"/>
       <c r="D48" s="36" t="s">
@@ -7136,18 +7334,12 @@
       <c r="K48" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="L48" s="37" t="s">
-        <v>126</v>
-      </c>
+      <c r="L48" s="37"/>
       <c r="M48" s="37"/>
-      <c r="N48" s="37" t="s">
-        <v>126</v>
-      </c>
+      <c r="N48" s="37"/>
       <c r="O48" s="37"/>
       <c r="P48" s="37"/>
-      <c r="Q48" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="Q48" s="37"/>
       <c r="R48" s="37" t="s">
         <v>130</v>
       </c>
@@ -7163,26 +7355,24 @@
       <c r="X48" s="37"/>
       <c r="Y48" s="38"/>
     </row>
-    <row r="49" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:25" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B49" s="39" t="s">
-        <v>43</v>
+        <v>171</v>
       </c>
       <c r="C49" s="37"/>
-      <c r="D49" s="37" t="s">
-        <v>126</v>
-      </c>
-      <c r="E49" s="37" t="s">
+      <c r="D49" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="E49" s="36" t="s">
         <v>126</v>
       </c>
       <c r="F49" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="G49" s="37" t="s">
-        <v>18</v>
-      </c>
+      <c r="G49" s="37"/>
       <c r="H49" s="37"/>
       <c r="I49" s="37"/>
       <c r="J49" s="37" t="s">
@@ -7223,7 +7413,7 @@
         <v>42</v>
       </c>
       <c r="B50" s="39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C50" s="37"/>
       <c r="D50" s="37" t="s">
@@ -7236,14 +7426,10 @@
         <v>126</v>
       </c>
       <c r="G50" s="37" t="s">
-        <v>126</v>
-      </c>
-      <c r="H50" s="37" t="s">
-        <v>126</v>
-      </c>
-      <c r="I50" s="37" t="s">
-        <v>126</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="H50" s="37"/>
+      <c r="I50" s="37"/>
       <c r="J50" s="37" t="s">
         <v>16</v>
       </c>
@@ -7253,18 +7439,12 @@
       <c r="L50" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="M50" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="M50" s="37"/>
       <c r="N50" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="O50" s="37" t="s">
-        <v>126</v>
-      </c>
-      <c r="P50" s="37" t="s">
-        <v>126</v>
-      </c>
+      <c r="O50" s="37"/>
+      <c r="P50" s="37"/>
       <c r="Q50" s="37" t="s">
         <v>16</v>
       </c>
@@ -7274,27 +7454,21 @@
       <c r="S50" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="T50" s="37" t="s">
-        <v>130</v>
-      </c>
-      <c r="U50" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="T50" s="37"/>
+      <c r="U50" s="37"/>
       <c r="V50" s="37" t="s">
         <v>130</v>
       </c>
       <c r="W50" s="37"/>
-      <c r="X50" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="X50" s="37"/>
       <c r="Y50" s="38"/>
     </row>
-    <row r="51" spans="1:25" s="17" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B51" s="39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C51" s="37"/>
       <c r="D51" s="37" t="s">
@@ -7354,20 +7528,18 @@
       <c r="V51" s="37" t="s">
         <v>130</v>
       </c>
-      <c r="W51" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="W51" s="37"/>
       <c r="X51" s="37" t="s">
         <v>16</v>
       </c>
       <c r="Y51" s="38"/>
     </row>
-    <row r="52" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:25" s="17" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B52" s="39" t="s">
-        <v>147</v>
+        <v>45</v>
       </c>
       <c r="C52" s="37"/>
       <c r="D52" s="37" t="s">
@@ -7427,7 +7599,9 @@
       <c r="V52" s="37" t="s">
         <v>130</v>
       </c>
-      <c r="W52" s="37"/>
+      <c r="W52" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="X52" s="37" t="s">
         <v>16</v>
       </c>
@@ -7438,7 +7612,7 @@
         <v>42</v>
       </c>
       <c r="B53" s="39" t="s">
-        <v>46</v>
+        <v>147</v>
       </c>
       <c r="C53" s="37"/>
       <c r="D53" s="37" t="s">
@@ -7509,7 +7683,7 @@
         <v>42</v>
       </c>
       <c r="B54" s="39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C54" s="37"/>
       <c r="D54" s="37" t="s">
@@ -7575,12 +7749,12 @@
       </c>
       <c r="Y54" s="38"/>
     </row>
-    <row r="55" spans="1:25" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B55" s="39" t="s">
-        <v>154</v>
+        <v>47</v>
       </c>
       <c r="C55" s="37"/>
       <c r="D55" s="37" t="s">
@@ -7646,12 +7820,12 @@
       </c>
       <c r="Y55" s="38"/>
     </row>
-    <row r="56" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:25" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B56" s="39" t="s">
-        <v>48</v>
+        <v>154</v>
       </c>
       <c r="C56" s="37"/>
       <c r="D56" s="37" t="s">
@@ -7722,7 +7896,7 @@
         <v>42</v>
       </c>
       <c r="B57" s="39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C57" s="37"/>
       <c r="D57" s="37" t="s">
@@ -7758,7 +7932,9 @@
       <c r="N57" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="O57" s="37"/>
+      <c r="O57" s="37" t="s">
+        <v>126</v>
+      </c>
       <c r="P57" s="37" t="s">
         <v>126</v>
       </c>
@@ -7791,7 +7967,7 @@
         <v>42</v>
       </c>
       <c r="B58" s="39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C58" s="37"/>
       <c r="D58" s="37" t="s">
@@ -7827,9 +8003,7 @@
       <c r="N58" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="O58" s="37" t="s">
-        <v>126</v>
-      </c>
+      <c r="O58" s="37"/>
       <c r="P58" s="37" t="s">
         <v>126</v>
       </c>
@@ -7862,7 +8036,7 @@
         <v>42</v>
       </c>
       <c r="B59" s="39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C59" s="37"/>
       <c r="D59" s="37" t="s">
@@ -7874,8 +8048,12 @@
       <c r="F59" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="G59" s="37"/>
-      <c r="H59" s="37"/>
+      <c r="G59" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="H59" s="37" t="s">
+        <v>126</v>
+      </c>
       <c r="I59" s="37" t="s">
         <v>126</v>
       </c>
@@ -7888,11 +8066,15 @@
       <c r="L59" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="M59" s="37"/>
+      <c r="M59" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="N59" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="O59" s="37"/>
+      <c r="O59" s="37" t="s">
+        <v>126</v>
+      </c>
       <c r="P59" s="37" t="s">
         <v>126</v>
       </c>
@@ -7925,7 +8107,7 @@
         <v>42</v>
       </c>
       <c r="B60" s="39" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C60" s="37"/>
       <c r="D60" s="37" t="s">
@@ -7938,10 +8120,10 @@
         <v>126</v>
       </c>
       <c r="G60" s="37"/>
-      <c r="H60" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="I60" s="37"/>
+      <c r="H60" s="37"/>
+      <c r="I60" s="37" t="s">
+        <v>126</v>
+      </c>
       <c r="J60" s="37" t="s">
         <v>16</v>
       </c>
@@ -7955,10 +8137,10 @@
       <c r="N60" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="O60" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="P60" s="37"/>
+      <c r="O60" s="37"/>
+      <c r="P60" s="37" t="s">
+        <v>126</v>
+      </c>
       <c r="Q60" s="37" t="s">
         <v>16</v>
       </c>
@@ -7968,13 +8150,19 @@
       <c r="S60" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="T60" s="37"/>
-      <c r="U60" s="37"/>
+      <c r="T60" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="U60" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="V60" s="37" t="s">
         <v>130</v>
       </c>
       <c r="W60" s="37"/>
-      <c r="X60" s="37"/>
+      <c r="X60" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="Y60" s="38"/>
     </row>
     <row r="61" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7982,7 +8170,7 @@
         <v>42</v>
       </c>
       <c r="B61" s="39" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C61" s="37"/>
       <c r="D61" s="37" t="s">
@@ -7995,7 +8183,9 @@
         <v>126</v>
       </c>
       <c r="G61" s="37"/>
-      <c r="H61" s="37"/>
+      <c r="H61" s="37" t="s">
+        <v>18</v>
+      </c>
       <c r="I61" s="37"/>
       <c r="J61" s="37" t="s">
         <v>16</v>
@@ -8010,7 +8200,9 @@
       <c r="N61" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="O61" s="37"/>
+      <c r="O61" s="37" t="s">
+        <v>18</v>
+      </c>
       <c r="P61" s="37"/>
       <c r="Q61" s="37" t="s">
         <v>16</v>
@@ -8035,7 +8227,7 @@
         <v>42</v>
       </c>
       <c r="B62" s="39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C62" s="37"/>
       <c r="D62" s="37" t="s">
@@ -8088,7 +8280,7 @@
         <v>42</v>
       </c>
       <c r="B63" s="39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C63" s="37"/>
       <c r="D63" s="37" t="s">
@@ -8136,12 +8328,12 @@
       <c r="X63" s="37"/>
       <c r="Y63" s="38"/>
     </row>
-    <row r="64" spans="1:25" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B64" s="39" t="s">
-        <v>120</v>
+        <v>55</v>
       </c>
       <c r="C64" s="37"/>
       <c r="D64" s="37" t="s">
@@ -8153,15 +8345,9 @@
       <c r="F64" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="G64" s="37" t="s">
-        <v>126</v>
-      </c>
-      <c r="H64" s="37" t="s">
-        <v>126</v>
-      </c>
-      <c r="I64" s="37" t="s">
-        <v>126</v>
-      </c>
+      <c r="G64" s="37"/>
+      <c r="H64" s="37"/>
+      <c r="I64" s="37"/>
       <c r="J64" s="37" t="s">
         <v>16</v>
       </c>
@@ -8171,16 +8357,12 @@
       <c r="L64" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="M64" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="M64" s="37"/>
       <c r="N64" s="37" t="s">
         <v>126</v>
       </c>
       <c r="O64" s="37"/>
-      <c r="P64" s="37" t="s">
-        <v>126</v>
-      </c>
+      <c r="P64" s="37"/>
       <c r="Q64" s="37" t="s">
         <v>16</v>
       </c>
@@ -8190,27 +8372,21 @@
       <c r="S64" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="T64" s="37" t="s">
-        <v>130</v>
-      </c>
-      <c r="U64" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="T64" s="37"/>
+      <c r="U64" s="37"/>
       <c r="V64" s="37" t="s">
         <v>130</v>
       </c>
       <c r="W64" s="37"/>
-      <c r="X64" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="X64" s="37"/>
       <c r="Y64" s="38"/>
     </row>
-    <row r="65" spans="1:25" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:25" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B65" s="39" t="s">
-        <v>172</v>
+        <v>120</v>
       </c>
       <c r="C65" s="37"/>
       <c r="D65" s="37" t="s">
@@ -8274,12 +8450,12 @@
       </c>
       <c r="Y65" s="38"/>
     </row>
-    <row r="66" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:25" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B66" s="39" t="s">
-        <v>56</v>
+        <v>172</v>
       </c>
       <c r="C66" s="37"/>
       <c r="D66" s="37" t="s">
@@ -8315,9 +8491,7 @@
       <c r="N66" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="O66" s="37" t="s">
-        <v>126</v>
-      </c>
+      <c r="O66" s="37"/>
       <c r="P66" s="37" t="s">
         <v>126</v>
       </c>
@@ -8345,12 +8519,12 @@
       </c>
       <c r="Y66" s="38"/>
     </row>
-    <row r="67" spans="1:25" s="17" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B67" s="39" t="s">
-        <v>124</v>
+        <v>56</v>
       </c>
       <c r="C67" s="37"/>
       <c r="D67" s="37" t="s">
@@ -8411,7 +8585,9 @@
         <v>130</v>
       </c>
       <c r="W67" s="37"/>
-      <c r="X67" s="37"/>
+      <c r="X67" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="Y67" s="38"/>
     </row>
     <row r="68" spans="1:25" s="17" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8419,7 +8595,7 @@
         <v>42</v>
       </c>
       <c r="B68" s="39" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="C68" s="37"/>
       <c r="D68" s="37" t="s">
@@ -8488,7 +8664,7 @@
         <v>42</v>
       </c>
       <c r="B69" s="39" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C69" s="37"/>
       <c r="D69" s="37" t="s">
@@ -8557,7 +8733,7 @@
         <v>42</v>
       </c>
       <c r="B70" s="39" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C70" s="37"/>
       <c r="D70" s="37" t="s">
@@ -8626,7 +8802,7 @@
         <v>42</v>
       </c>
       <c r="B71" s="39" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C71" s="37"/>
       <c r="D71" s="37" t="s">
@@ -8690,26 +8866,32 @@
       <c r="X71" s="37"/>
       <c r="Y71" s="38"/>
     </row>
-    <row r="72" spans="1:25" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:25" s="17" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B72" s="39" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C72" s="37"/>
-      <c r="D72" s="36" t="s">
-        <v>126</v>
-      </c>
-      <c r="E72" s="36" t="s">
+      <c r="D72" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="E72" s="37" t="s">
         <v>126</v>
       </c>
       <c r="F72" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="G72" s="37"/>
-      <c r="H72" s="37"/>
-      <c r="I72" s="37"/>
+      <c r="G72" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="H72" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="I72" s="37" t="s">
+        <v>126</v>
+      </c>
       <c r="J72" s="37" t="s">
         <v>16</v>
       </c>
@@ -8719,12 +8901,18 @@
       <c r="L72" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="M72" s="37"/>
+      <c r="M72" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="N72" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="O72" s="37"/>
-      <c r="P72" s="37"/>
+      <c r="O72" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="P72" s="37" t="s">
+        <v>126</v>
+      </c>
       <c r="Q72" s="37" t="s">
         <v>16</v>
       </c>
@@ -8734,39 +8922,39 @@
       <c r="S72" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="T72" s="37"/>
-      <c r="U72" s="37"/>
-      <c r="V72" s="37"/>
+      <c r="T72" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="U72" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="V72" s="37" t="s">
+        <v>130</v>
+      </c>
       <c r="W72" s="37"/>
       <c r="X72" s="37"/>
       <c r="Y72" s="38"/>
     </row>
-    <row r="73" spans="1:25" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:25" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B73" s="39" t="s">
-        <v>187</v>
+        <v>146</v>
       </c>
       <c r="C73" s="37"/>
-      <c r="D73" s="37" t="s">
-        <v>126</v>
-      </c>
-      <c r="E73" s="37" t="s">
+      <c r="D73" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="E73" s="36" t="s">
         <v>126</v>
       </c>
       <c r="F73" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="G73" s="37" t="s">
-        <v>126</v>
-      </c>
-      <c r="H73" s="37" t="s">
-        <v>126</v>
-      </c>
-      <c r="I73" s="37" t="s">
-        <v>126</v>
-      </c>
+      <c r="G73" s="37"/>
+      <c r="H73" s="37"/>
+      <c r="I73" s="37"/>
       <c r="J73" s="37" t="s">
         <v>16</v>
       </c>
@@ -8776,18 +8964,12 @@
       <c r="L73" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="M73" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="M73" s="37"/>
       <c r="N73" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="O73" s="37" t="s">
-        <v>126</v>
-      </c>
-      <c r="P73" s="37" t="s">
-        <v>126</v>
-      </c>
+      <c r="O73" s="37"/>
+      <c r="P73" s="37"/>
       <c r="Q73" s="37" t="s">
         <v>16</v>
       </c>
@@ -8797,25 +8979,19 @@
       <c r="S73" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="T73" s="37" t="s">
-        <v>130</v>
-      </c>
-      <c r="U73" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="V73" s="37" t="s">
-        <v>130</v>
-      </c>
+      <c r="T73" s="37"/>
+      <c r="U73" s="37"/>
+      <c r="V73" s="37"/>
       <c r="W73" s="37"/>
       <c r="X73" s="37"/>
       <c r="Y73" s="38"/>
     </row>
-    <row r="74" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:25" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="39" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="B74" s="39" t="s">
-        <v>58</v>
+        <v>187</v>
       </c>
       <c r="C74" s="37"/>
       <c r="D74" s="37" t="s">
@@ -8875,22 +9051,16 @@
       <c r="V74" s="37" t="s">
         <v>130</v>
       </c>
-      <c r="W74" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="X74" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y74" s="53" t="s">
-        <v>59</v>
-      </c>
+      <c r="W74" s="37"/>
+      <c r="X74" s="37"/>
+      <c r="Y74" s="38"/>
     </row>
     <row r="75" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="39" t="s">
         <v>57</v>
       </c>
       <c r="B75" s="39" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C75" s="37"/>
       <c r="D75" s="37" t="s">
@@ -8956,20 +9126,22 @@
       <c r="X75" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="Y75" s="54"/>
+      <c r="Y75" s="55" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="76" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="39" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B76" s="39" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C76" s="37"/>
       <c r="D76" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="E76" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="E76" s="37" t="s">
         <v>126</v>
       </c>
       <c r="F76" s="37" t="s">
@@ -8988,7 +9160,7 @@
         <v>16</v>
       </c>
       <c r="K76" s="37" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L76" s="37" t="s">
         <v>126</v>
@@ -9009,130 +9181,170 @@
         <v>16</v>
       </c>
       <c r="R76" s="37" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="S76" s="37" t="s">
-        <v>112</v>
+        <v>16</v>
       </c>
       <c r="T76" s="37" t="s">
         <v>130</v>
       </c>
       <c r="U76" s="37" t="s">
-        <v>112</v>
+        <v>16</v>
       </c>
       <c r="V76" s="37" t="s">
         <v>130</v>
       </c>
       <c r="W76" s="37" t="s">
-        <v>112</v>
+        <v>16</v>
       </c>
       <c r="X76" s="37" t="s">
-        <v>112</v>
-      </c>
-      <c r="Y76" s="38"/>
-    </row>
-    <row r="77" spans="1:25" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A77" s="42" t="s">
-        <v>62</v>
-      </c>
-      <c r="B77" s="42" t="s">
-        <v>63</v>
-      </c>
-      <c r="C77" s="43"/>
+        <v>16</v>
+      </c>
+      <c r="Y76" s="56"/>
+    </row>
+    <row r="77" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A77" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="B77" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="C77" s="37"/>
       <c r="D77" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="E77" s="43"/>
-      <c r="F77" s="43"/>
-      <c r="G77" s="43"/>
-      <c r="H77" s="43"/>
-      <c r="I77" s="43"/>
-      <c r="J77" s="43"/>
-      <c r="K77" s="43"/>
-      <c r="L77" s="43"/>
-      <c r="M77" s="43"/>
-      <c r="N77" s="43"/>
-      <c r="O77" s="43"/>
-      <c r="P77" s="43"/>
-      <c r="Q77" s="43"/>
-      <c r="R77" s="43"/>
-      <c r="S77" s="43"/>
-      <c r="T77" s="43"/>
-      <c r="U77" s="43"/>
-      <c r="V77" s="43"/>
-      <c r="W77" s="43"/>
-      <c r="X77" s="43"/>
-      <c r="Y77" s="44" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="78" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A78" s="35" t="s">
+      <c r="E77" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="F77" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="G77" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="H77" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="I77" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="J77" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="K77" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="L77" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="M77" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="N77" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="O77" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="P77" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q77" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="R77" s="37" t="s">
+        <v>131</v>
+      </c>
+      <c r="S77" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="T77" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="U77" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="V77" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="W77" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="X77" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y77" s="38"/>
+    </row>
+    <row r="78" spans="1:25" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A78" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="B78" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="C78" s="36"/>
+      <c r="B78" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="C78" s="43"/>
       <c r="D78" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="E78" s="36"/>
-      <c r="F78" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="G78" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="H78" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="I78" s="36"/>
-      <c r="J78" s="37"/>
-      <c r="K78" s="36"/>
-      <c r="L78" s="36"/>
-      <c r="M78" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="N78" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="O78" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="P78" s="36"/>
-      <c r="Q78" s="37"/>
-      <c r="R78" s="36"/>
-      <c r="S78" s="36"/>
-      <c r="T78" s="36"/>
-      <c r="U78" s="36"/>
-      <c r="V78" s="36"/>
-      <c r="W78" s="36"/>
-      <c r="X78" s="36"/>
-      <c r="Y78" s="30"/>
+      <c r="E78" s="43"/>
+      <c r="F78" s="43"/>
+      <c r="G78" s="43"/>
+      <c r="H78" s="43"/>
+      <c r="I78" s="43"/>
+      <c r="J78" s="43"/>
+      <c r="K78" s="43"/>
+      <c r="L78" s="43"/>
+      <c r="M78" s="43"/>
+      <c r="N78" s="43"/>
+      <c r="O78" s="43"/>
+      <c r="P78" s="43"/>
+      <c r="Q78" s="43"/>
+      <c r="R78" s="43"/>
+      <c r="S78" s="43"/>
+      <c r="T78" s="43"/>
+      <c r="U78" s="43"/>
+      <c r="V78" s="43"/>
+      <c r="W78" s="43"/>
+      <c r="X78" s="43"/>
+      <c r="Y78" s="44" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="79" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="35" t="s">
         <v>62</v>
       </c>
       <c r="B79" s="35" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C79" s="36"/>
       <c r="D79" s="37" t="s">
         <v>125</v>
       </c>
       <c r="E79" s="36"/>
-      <c r="F79" s="36"/>
-      <c r="G79" s="36"/>
-      <c r="H79" s="36"/>
+      <c r="F79" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="G79" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="H79" s="36" t="s">
+        <v>18</v>
+      </c>
       <c r="I79" s="36"/>
       <c r="J79" s="37"/>
       <c r="K79" s="36"/>
       <c r="L79" s="36"/>
-      <c r="M79" s="36"/>
-      <c r="N79" s="36"/>
-      <c r="O79" s="36"/>
+      <c r="M79" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="N79" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="O79" s="36" t="s">
+        <v>18</v>
+      </c>
       <c r="P79" s="36"/>
       <c r="Q79" s="37"/>
       <c r="R79" s="36"/>
@@ -9149,7 +9361,7 @@
         <v>62</v>
       </c>
       <c r="B80" s="35" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C80" s="36"/>
       <c r="D80" s="37" t="s">
@@ -9182,7 +9394,7 @@
         <v>62</v>
       </c>
       <c r="B81" s="35" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C81" s="36"/>
       <c r="D81" s="37" t="s">
@@ -9210,12 +9422,12 @@
       <c r="X81" s="36"/>
       <c r="Y81" s="30"/>
     </row>
-    <row r="82" spans="1:25" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A82" s="35" t="s">
         <v>62</v>
       </c>
       <c r="B82" s="35" t="s">
-        <v>165</v>
+        <v>68</v>
       </c>
       <c r="C82" s="36"/>
       <c r="D82" s="37" t="s">
@@ -9243,12 +9455,12 @@
       <c r="X82" s="36"/>
       <c r="Y82" s="30"/>
     </row>
-    <row r="83" spans="1:25" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:25" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83" s="35" t="s">
         <v>62</v>
       </c>
       <c r="B83" s="35" t="s">
-        <v>32</v>
+        <v>165</v>
       </c>
       <c r="C83" s="36"/>
       <c r="D83" s="37" t="s">
@@ -9276,12 +9488,12 @@
       <c r="X83" s="36"/>
       <c r="Y83" s="30"/>
     </row>
-    <row r="84" spans="1:25" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:25" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A84" s="35" t="s">
         <v>62</v>
       </c>
       <c r="B84" s="35" t="s">
-        <v>180</v>
+        <v>32</v>
       </c>
       <c r="C84" s="36"/>
       <c r="D84" s="37" t="s">
@@ -9309,12 +9521,12 @@
       <c r="X84" s="36"/>
       <c r="Y84" s="30"/>
     </row>
-    <row r="85" spans="1:25" s="52" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:25" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A85" s="35" t="s">
         <v>62</v>
       </c>
       <c r="B85" s="35" t="s">
-        <v>205</v>
+        <v>180</v>
       </c>
       <c r="C85" s="36"/>
       <c r="D85" s="37" t="s">
@@ -9340,14 +9552,14 @@
       <c r="V85" s="36"/>
       <c r="W85" s="36"/>
       <c r="X85" s="36"/>
-      <c r="Y85" s="51"/>
-    </row>
-    <row r="86" spans="1:25" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="Y85" s="30"/>
+    </row>
+    <row r="86" spans="1:25" s="52" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A86" s="35" t="s">
         <v>62</v>
       </c>
       <c r="B86" s="35" t="s">
-        <v>123</v>
+        <v>205</v>
       </c>
       <c r="C86" s="36"/>
       <c r="D86" s="37" t="s">
@@ -9373,101 +9585,146 @@
       <c r="V86" s="36"/>
       <c r="W86" s="36"/>
       <c r="X86" s="36"/>
-      <c r="Y86" s="30"/>
-    </row>
-    <row r="87" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="Y86" s="51"/>
+    </row>
+    <row r="87" spans="1:25" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A87" s="35" t="s">
-        <v>108</v>
+        <v>62</v>
       </c>
       <c r="B87" s="35" t="s">
-        <v>109</v>
-      </c>
-      <c r="C87" s="45"/>
+        <v>123</v>
+      </c>
+      <c r="C87" s="36"/>
       <c r="D87" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="E87" s="45"/>
-      <c r="F87" s="45"/>
-      <c r="G87" s="45"/>
-      <c r="H87" s="45"/>
-      <c r="I87" s="45"/>
-      <c r="J87" s="46"/>
-      <c r="K87" s="45"/>
-      <c r="L87" s="45"/>
-      <c r="M87" s="45"/>
-      <c r="N87" s="45"/>
-      <c r="O87" s="45"/>
-      <c r="P87" s="45"/>
-      <c r="Q87" s="46"/>
-      <c r="R87" s="45"/>
-      <c r="S87" s="45"/>
-      <c r="T87" s="45"/>
-      <c r="U87" s="45"/>
-      <c r="V87" s="45"/>
-      <c r="W87" s="45"/>
-      <c r="X87" s="45"/>
+      <c r="E87" s="36"/>
+      <c r="F87" s="36"/>
+      <c r="G87" s="36"/>
+      <c r="H87" s="36"/>
+      <c r="I87" s="36"/>
+      <c r="J87" s="37"/>
+      <c r="K87" s="36"/>
+      <c r="L87" s="36"/>
+      <c r="M87" s="36"/>
+      <c r="N87" s="36"/>
+      <c r="O87" s="36"/>
+      <c r="P87" s="36"/>
+      <c r="Q87" s="37"/>
+      <c r="R87" s="36"/>
+      <c r="S87" s="36"/>
+      <c r="T87" s="36"/>
+      <c r="U87" s="36"/>
+      <c r="V87" s="36"/>
+      <c r="W87" s="36"/>
+      <c r="X87" s="36"/>
       <c r="Y87" s="30"/>
     </row>
     <row r="88" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A88" s="35" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B88" s="35" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="C88" s="45"/>
       <c r="D88" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="E88" s="45"/>
+      <c r="F88" s="45"/>
+      <c r="G88" s="45"/>
+      <c r="H88" s="45"/>
+      <c r="I88" s="45"/>
+      <c r="J88" s="46"/>
+      <c r="K88" s="45"/>
+      <c r="L88" s="45"/>
+      <c r="M88" s="45"/>
+      <c r="N88" s="45"/>
+      <c r="O88" s="45"/>
+      <c r="P88" s="45"/>
+      <c r="Q88" s="46"/>
+      <c r="R88" s="45"/>
+      <c r="S88" s="45"/>
+      <c r="T88" s="45"/>
+      <c r="U88" s="45"/>
+      <c r="V88" s="45"/>
+      <c r="W88" s="45"/>
+      <c r="X88" s="45"/>
+      <c r="Y88" s="30"/>
+    </row>
+    <row r="89" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A89" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="B89" s="35" t="s">
+        <v>119</v>
+      </c>
+      <c r="C89" s="45"/>
+      <c r="D89" s="37" t="s">
         <v>127</v>
       </c>
-      <c r="E88" s="47" t="s">
+      <c r="E89" s="47" t="s">
         <v>127</v>
       </c>
-      <c r="F88" s="47"/>
-      <c r="G88" s="47" t="s">
+      <c r="F89" s="47"/>
+      <c r="G89" s="47" t="s">
         <v>127</v>
       </c>
-      <c r="H88" s="47"/>
-      <c r="I88" s="47"/>
-      <c r="J88" s="48" t="s">
+      <c r="H89" s="47"/>
+      <c r="I89" s="47"/>
+      <c r="J89" s="48" t="s">
         <v>159</v>
       </c>
-      <c r="K88" s="47" t="s">
+      <c r="K89" s="47" t="s">
         <v>127</v>
       </c>
-      <c r="L88" s="47" t="s">
+      <c r="L89" s="47" t="s">
         <v>127</v>
       </c>
-      <c r="M88" s="47" t="s">
+      <c r="M89" s="47" t="s">
         <v>127</v>
       </c>
-      <c r="N88" s="47" t="s">
+      <c r="N89" s="47" t="s">
         <v>127</v>
       </c>
-      <c r="O88" s="47"/>
-      <c r="P88" s="47"/>
-      <c r="Q88" s="48" t="s">
+      <c r="O89" s="47"/>
+      <c r="P89" s="47"/>
+      <c r="Q89" s="48" t="s">
         <v>159</v>
       </c>
-      <c r="R88" s="49" t="s">
+      <c r="R89" s="49" t="s">
         <v>164</v>
       </c>
-      <c r="S88" s="48" t="s">
+      <c r="S89" s="48" t="s">
         <v>159</v>
       </c>
-      <c r="T88" s="47"/>
-      <c r="U88" s="47" t="s">
+      <c r="T89" s="47"/>
+      <c r="U89" s="47" t="s">
         <v>159</v>
       </c>
-      <c r="V88" s="47"/>
-      <c r="W88" s="47"/>
-      <c r="X88" s="47"/>
-      <c r="Y88" s="30"/>
+      <c r="V89" s="47"/>
+      <c r="W89" s="47"/>
+      <c r="X89" s="47"/>
+      <c r="Y89" s="30"/>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="U41" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="W48" sqref="W48"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
+      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
+      <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="C31" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -9477,27 +9734,15 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C31" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
-      <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
-      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
+    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="U41" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="W48" sqref="W48"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="6">
-    <mergeCell ref="Y74:Y75"/>
+    <mergeCell ref="Y75:Y76"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="K5:O5"/>
     <mergeCell ref="R5:X5"/>
@@ -9848,7 +10093,17 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="150">
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
+      <selection activeCell="B17" sqref="B17"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
+      <selection activeCell="C7" sqref="C7"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}">
       <selection activeCell="G36" sqref="G36"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -9858,18 +10113,8 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}">
+    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="150">
       <selection activeCell="G36" sqref="G36"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
-      <selection activeCell="C7" sqref="C7"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
-      <selection activeCell="B17" sqref="B17"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>

</xml_diff>

<commit_message>
Aseta urakoitsijalle näytön oikeustarkistukset kuntoon
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/teemukau/code/harja/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarihan/Jari/Tyo/Solita/Projektit/Harja/harja/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="4460" yWindow="2960" windowWidth="42420" windowHeight="22540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -23,11 +23,11 @@
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="2121" windowHeight="954" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Mikko Rönkkömäki - Personal View" guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" mergeInterval="0" personalView="1" windowWidth="2560" windowHeight="1071" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office -käyttäjä - Oma näkymä" guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="1149" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
-    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Microsoft Office -käyttäjä - Oma näkymä" guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="1149" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Mikko Rönkkömäki - Personal View" guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" mergeInterval="0" personalView="1" windowWidth="2560" windowHeight="1071" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="1280" windowHeight="600" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1419" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1419" uniqueCount="213">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -701,6 +701,18 @@
   </si>
   <si>
     <t>Toteumat / Vesiväyläerilliskustannukset</t>
+  </si>
+  <si>
+    <t>R*,W*,aseta-näkyviin-urakoitsijalle*</t>
+  </si>
+  <si>
+    <t>R*,W,aseta-näkyviin-urakoitsijalle</t>
+  </si>
+  <si>
+    <t>R*,W+,aseta-näkyviin-urakoitsijalle+</t>
+  </si>
+  <si>
+    <t>R,W,aseta-näkyviin-urakoitsijalle</t>
   </si>
 </sst>
 </file>
@@ -1337,7 +1349,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{4A189F6B-10A0-794F-AE26-98E1292E0A90}" diskRevisions="1" revisionId="675" version="30">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{6BC78FCF-55A6-204A-B897-B2B98ECA17AE}" diskRevisions="1" revisionId="684" version="31">
   <header guid="{1E352813-0B26-DB4E-84BE-460845B77133}" dateTime="2017-06-20T12:32:37" maxSheetId="3" userName="Microsoft Office -käyttäjä" r:id="rId60" minRId="448" maxRId="464">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1513,6 +1525,12 @@
     </sheetIdMap>
   </header>
   <header guid="{4A189F6B-10A0-794F-AE26-98E1292E0A90}" dateTime="2017-09-21T08:13:09" maxSheetId="3" userName="Microsoft Office User" r:id="rId89" minRId="655" maxRId="675">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{6BC78FCF-55A6-204A-B897-B2B98ECA17AE}" dateTime="2017-09-28T10:38:14" maxSheetId="3" userName="Microsoft Office User" r:id="rId90" minRId="676" maxRId="683">
     <sheetIdMap count="2">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -3654,6 +3672,113 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog28.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="676" sId="1">
+    <oc r="D21" t="inlineStr">
+      <is>
+        <t>R*,W*</t>
+      </is>
+    </oc>
+    <nc r="D21" t="inlineStr">
+      <is>
+        <t>R*,W*,aseta-näkyviin-urakoitsijalle*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="677" sId="1">
+    <oc r="E21" t="inlineStr">
+      <is>
+        <t>R*,W</t>
+      </is>
+    </oc>
+    <nc r="E21" t="inlineStr">
+      <is>
+        <t>R*,W,aseta-näkyviin-urakoitsijalle</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="678" sId="1">
+    <oc r="G21" t="inlineStr">
+      <is>
+        <t>R*,W+</t>
+      </is>
+    </oc>
+    <nc r="G21" t="inlineStr">
+      <is>
+        <t>R*,W+,aseta-näkyviin-urakoitsijalle+</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="679" sId="1">
+    <oc r="J21" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </oc>
+    <nc r="J21" t="inlineStr">
+      <is>
+        <t>R,W,aseta-näkyviin-urakoitsijalle</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="680" sId="1">
+    <oc r="K21" t="inlineStr">
+      <is>
+        <t>R*,W*</t>
+      </is>
+    </oc>
+    <nc r="K21" t="inlineStr">
+      <is>
+        <t>R*,W*,aseta-näkyviin-urakoitsijalle*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="681" sId="1">
+    <oc r="L21" t="inlineStr">
+      <is>
+        <t>R*,W</t>
+      </is>
+    </oc>
+    <nc r="L21" t="inlineStr">
+      <is>
+        <t>R*,W,aseta-näkyviin-urakoitsijalle</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="682" sId="1">
+    <oc r="M21" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </oc>
+    <nc r="M21" t="inlineStr">
+      <is>
+        <t>R,W,aseta-näkyviin-urakoitsijalle</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="683" sId="1">
+    <oc r="Q21" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </oc>
+    <nc r="Q21" t="inlineStr">
+      <is>
+        <t>R,W,aseta-näkyviin-urakoitsijalle</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="delete"/>
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_7A9649F2_657F_9445_B6E6_FE94C6A09957_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Oikeudet!$A$5:$Y$89</formula>
+    <oldFormula>Oikeudet!$A$5:$Y$89</oldFormula>
+  </rdn>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="497" sId="1">
@@ -4329,7 +4454,7 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="3">
   <userInfo guid="{1E352813-0B26-DB4E-84BE-460845B77133}" name="Microsoft Office -käyttäjä" id="-785751636" dateTime="2017-06-20T12:33:00"/>
   <userInfo guid="{1AB7A282-42ED-4740-A9CB-95FF229EC1A0}" name="Mikko Rönkkömäki" id="-727946492" dateTime="2017-06-22T10:45:48"/>
@@ -4662,10 +4787,10 @@
   <dimension ref="A1:Y89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C14" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="K7" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E21" sqref="E21"/>
+      <selection pane="bottomRight" activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5726,16 +5851,16 @@
       </c>
       <c r="C21" s="36"/>
       <c r="D21" s="36" t="s">
-        <v>125</v>
+        <v>209</v>
       </c>
       <c r="E21" s="36" t="s">
-        <v>129</v>
+        <v>210</v>
       </c>
       <c r="F21" s="36" t="s">
         <v>126</v>
       </c>
       <c r="G21" s="36" t="s">
-        <v>128</v>
+        <v>211</v>
       </c>
       <c r="H21" s="36" t="s">
         <v>126</v>
@@ -5744,16 +5869,16 @@
         <v>126</v>
       </c>
       <c r="J21" s="37" t="s">
-        <v>112</v>
+        <v>212</v>
       </c>
       <c r="K21" s="36" t="s">
-        <v>125</v>
+        <v>209</v>
       </c>
       <c r="L21" s="36" t="s">
-        <v>129</v>
+        <v>210</v>
       </c>
       <c r="M21" s="37" t="s">
-        <v>112</v>
+        <v>212</v>
       </c>
       <c r="N21" s="37" t="s">
         <v>126</v>
@@ -5765,7 +5890,7 @@
         <v>126</v>
       </c>
       <c r="Q21" s="37" t="s">
-        <v>112</v>
+        <v>212</v>
       </c>
       <c r="R21" s="36" t="s">
         <v>131</v>
@@ -9710,9 +9835,21 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
-      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
+    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="J21" sqref="J21"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="C48" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="D72" sqref="D72:X72"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="C31" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -9722,21 +9859,9 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C31" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C48" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="D72" sqref="D72:X72"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="U41" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="W48" sqref="W48"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
+      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -10093,17 +10218,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
-      <selection activeCell="B17" sqref="B17"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
-      <selection activeCell="C7" sqref="C7"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}">
+    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="150">
       <selection activeCell="G36" sqref="G36"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -10113,8 +10228,18 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="150">
+    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}">
       <selection activeCell="G36" sqref="G36"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
+      <selection activeCell="C7" sqref="C7"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
+      <selection activeCell="B17" sqref="B17"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>

</xml_diff>

<commit_message>
Päivitä Roolit-excel, lisää erikoisoikeus nähdä tilannekuvassa urakan ely-alueen tiedot
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/teemukau/code/harja/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarihan/Jari/Tyo/Solita/Projektit/Harja/harja/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12840" yWindow="0" windowWidth="12760" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="32100" windowHeight="20380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -23,11 +23,11 @@
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="638" windowHeight="614" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="1605" windowHeight="846" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
+    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office -käyttäjä - Oma näkymä" guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="1149" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="Mikko Rönkkömäki - Personal View" guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" mergeInterval="0" personalView="1" windowWidth="2560" windowHeight="1071" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Microsoft Office -käyttäjä - Oma näkymä" guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="1149" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1446" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1446" uniqueCount="217">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -719,6 +719,12 @@
   </si>
   <si>
     <t>Kanavat / Lisätyöt</t>
+  </si>
+  <si>
+    <t>R,urakan-ely</t>
+  </si>
+  <si>
+    <t>R+,urakan-ely</t>
   </si>
 </sst>
 </file>
@@ -1178,6 +1184,18 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1195,18 +1213,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="185">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1406,7 +1412,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{6E4CA5A8-8365-3A42-8AB2-5AE7527F63CD}" diskRevisions="1" revisionId="710" version="31">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{FE05E342-1832-0F4A-90B6-5A7BDC307B68}" diskRevisions="1" revisionId="717" version="32">
   <header guid="{1E352813-0B26-DB4E-84BE-460845B77133}" dateTime="2017-06-20T12:32:37" maxSheetId="3" userName="Microsoft Office -käyttäjä" r:id="rId60" minRId="448" maxRId="464">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1593,6 +1599,12 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{FE05E342-1832-0F4A-90B6-5A7BDC307B68}" dateTime="2017-09-28T14:42:27" maxSheetId="3" userName="Microsoft Office User" r:id="rId91" minRId="711" maxRId="716">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -7807,6 +7819,89 @@
     <nc r="B46" t="inlineStr">
       <is>
         <t>Kanavat / Lisätyöt</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="delete"/>
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_7A9649F2_657F_9445_B6E6_FE94C6A09957_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Oikeudet!$A$5:$Y$95</formula>
+    <oldFormula>Oikeudet!$A$5:$Y$95</oldFormula>
+  </rdn>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog29.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="711" sId="1">
+    <oc r="Q80" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </oc>
+    <nc r="Q80" t="inlineStr">
+      <is>
+        <t>R,urakan-ely</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="712" sId="1">
+    <oc r="R80" t="inlineStr">
+      <is>
+        <t>R+</t>
+      </is>
+    </oc>
+    <nc r="R80" t="inlineStr">
+      <is>
+        <t>R+,urakan-ely</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="713" sId="1">
+    <oc r="S80" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </oc>
+    <nc r="S80" t="inlineStr">
+      <is>
+        <t>R,urakan-ely</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="714" sId="1">
+    <oc r="Q81" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </oc>
+    <nc r="Q81" t="inlineStr">
+      <is>
+        <t>R,urakan-ely</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="715" sId="1">
+    <oc r="R81" t="inlineStr">
+      <is>
+        <t>R+</t>
+      </is>
+    </oc>
+    <nc r="R81" t="inlineStr">
+      <is>
+        <t>R+,urakan-ely</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="716" sId="1">
+    <oc r="S81" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </oc>
+    <nc r="S81" t="inlineStr">
+      <is>
+        <t>R,urakan-ely</t>
       </is>
     </nc>
   </rcc>
@@ -8827,10 +8922,10 @@
   <dimension ref="A1:Y95"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C42" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="P70" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B43" sqref="B43"/>
+      <selection pane="bottomRight" activeCell="R80" sqref="R80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8867,40 +8962,40 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="61" t="s">
+      <c r="C1" s="65" t="s">
         <v>150</v>
       </c>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-      <c r="N1" s="62"/>
-      <c r="O1" s="62"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
+      <c r="L1" s="66"/>
+      <c r="M1" s="66"/>
+      <c r="N1" s="66"/>
+      <c r="O1" s="66"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="64"/>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64"/>
-      <c r="O2" s="64"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="68"/>
+      <c r="N2" s="68"/>
+      <c r="O2" s="68"/>
     </row>
     <row r="3" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
@@ -8923,34 +9018,34 @@
     <row r="5" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="30"/>
       <c r="B5" s="30"/>
-      <c r="C5" s="60" t="s">
+      <c r="C5" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="59"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
       <c r="I5" s="30"/>
       <c r="J5" s="30"/>
-      <c r="K5" s="60" t="s">
+      <c r="K5" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="L5" s="59"/>
-      <c r="M5" s="59"/>
-      <c r="N5" s="59"/>
-      <c r="O5" s="59"/>
+      <c r="L5" s="63"/>
+      <c r="M5" s="63"/>
+      <c r="N5" s="63"/>
+      <c r="O5" s="63"/>
       <c r="P5" s="30"/>
       <c r="Q5" s="30"/>
-      <c r="R5" s="60" t="s">
+      <c r="R5" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="S5" s="59"/>
-      <c r="T5" s="59"/>
-      <c r="U5" s="59"/>
-      <c r="V5" s="59"/>
-      <c r="W5" s="59"/>
-      <c r="X5" s="59"/>
+      <c r="S5" s="63"/>
+      <c r="T5" s="63"/>
+      <c r="U5" s="63"/>
+      <c r="V5" s="63"/>
+      <c r="W5" s="63"/>
+      <c r="X5" s="63"/>
       <c r="Y5" s="31" t="s">
         <v>13</v>
       </c>
@@ -10172,51 +10267,51 @@
       <c r="A25" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="67" t="s">
+      <c r="B25" s="60" t="s">
         <v>211</v>
       </c>
-      <c r="C25" s="68"/>
-      <c r="D25" s="68" t="s">
+      <c r="C25" s="61"/>
+      <c r="D25" s="61" t="s">
         <v>125</v>
       </c>
-      <c r="E25" s="68" t="s">
+      <c r="E25" s="61" t="s">
         <v>129</v>
       </c>
-      <c r="F25" s="68" t="s">
-        <v>126</v>
-      </c>
-      <c r="G25" s="68"/>
-      <c r="H25" s="68" t="s">
-        <v>126</v>
-      </c>
-      <c r="I25" s="68"/>
-      <c r="J25" s="68" t="s">
+      <c r="F25" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="G25" s="61"/>
+      <c r="H25" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="I25" s="61"/>
+      <c r="J25" s="61" t="s">
         <v>112</v>
       </c>
-      <c r="K25" s="68"/>
-      <c r="L25" s="68"/>
-      <c r="M25" s="68"/>
-      <c r="N25" s="68"/>
-      <c r="O25" s="68"/>
-      <c r="P25" s="68"/>
-      <c r="Q25" s="68"/>
-      <c r="R25" s="68" t="s">
+      <c r="K25" s="61"/>
+      <c r="L25" s="61"/>
+      <c r="M25" s="61"/>
+      <c r="N25" s="61"/>
+      <c r="O25" s="61"/>
+      <c r="P25" s="61"/>
+      <c r="Q25" s="61"/>
+      <c r="R25" s="61" t="s">
         <v>131</v>
       </c>
-      <c r="S25" s="68" t="s">
+      <c r="S25" s="61" t="s">
         <v>112</v>
       </c>
-      <c r="T25" s="68" t="s">
-        <v>130</v>
-      </c>
-      <c r="U25" s="68" t="s">
-        <v>16</v>
-      </c>
-      <c r="V25" s="68" t="s">
-        <v>130</v>
-      </c>
-      <c r="W25" s="68"/>
-      <c r="X25" s="68"/>
+      <c r="T25" s="61" t="s">
+        <v>130</v>
+      </c>
+      <c r="U25" s="61" t="s">
+        <v>16</v>
+      </c>
+      <c r="V25" s="61" t="s">
+        <v>130</v>
+      </c>
+      <c r="W25" s="61"/>
+      <c r="X25" s="61"/>
       <c r="Y25" s="55"/>
     </row>
     <row r="26" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10448,13 +10543,13 @@
       <c r="Y29" s="38"/>
     </row>
     <row r="30" spans="1:25" s="57" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="65" t="s">
+      <c r="A30" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="B30" s="65" t="s">
+      <c r="B30" s="58" t="s">
         <v>210</v>
       </c>
-      <c r="D30" s="66" t="s">
+      <c r="D30" s="59" t="s">
         <v>125</v>
       </c>
     </row>
@@ -11316,66 +11411,66 @@
       <c r="A45" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B45" s="67" t="s">
+      <c r="B45" s="60" t="s">
         <v>213</v>
       </c>
-      <c r="C45" s="68"/>
-      <c r="D45" s="68" t="s">
+      <c r="C45" s="61"/>
+      <c r="D45" s="61" t="s">
         <v>125</v>
       </c>
-      <c r="E45" s="68"/>
-      <c r="F45" s="68"/>
-      <c r="G45" s="68"/>
-      <c r="H45" s="68"/>
-      <c r="I45" s="68"/>
-      <c r="J45" s="68"/>
-      <c r="K45" s="68"/>
-      <c r="L45" s="68"/>
-      <c r="M45" s="68"/>
-      <c r="N45" s="68"/>
-      <c r="O45" s="68"/>
-      <c r="P45" s="68"/>
-      <c r="Q45" s="68"/>
-      <c r="R45" s="68"/>
-      <c r="S45" s="68"/>
-      <c r="T45" s="68"/>
-      <c r="U45" s="68"/>
-      <c r="V45" s="68"/>
-      <c r="W45" s="68"/>
-      <c r="X45" s="68"/>
+      <c r="E45" s="61"/>
+      <c r="F45" s="61"/>
+      <c r="G45" s="61"/>
+      <c r="H45" s="61"/>
+      <c r="I45" s="61"/>
+      <c r="J45" s="61"/>
+      <c r="K45" s="61"/>
+      <c r="L45" s="61"/>
+      <c r="M45" s="61"/>
+      <c r="N45" s="61"/>
+      <c r="O45" s="61"/>
+      <c r="P45" s="61"/>
+      <c r="Q45" s="61"/>
+      <c r="R45" s="61"/>
+      <c r="S45" s="61"/>
+      <c r="T45" s="61"/>
+      <c r="U45" s="61"/>
+      <c r="V45" s="61"/>
+      <c r="W45" s="61"/>
+      <c r="X45" s="61"/>
       <c r="Y45" s="56"/>
     </row>
     <row r="46" spans="1:25" s="57" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="67" t="s">
+      <c r="B46" s="60" t="s">
         <v>214</v>
       </c>
-      <c r="C46" s="68"/>
-      <c r="D46" s="68" t="s">
+      <c r="C46" s="61"/>
+      <c r="D46" s="61" t="s">
         <v>125</v>
       </c>
-      <c r="E46" s="68"/>
-      <c r="F46" s="68"/>
-      <c r="G46" s="68"/>
-      <c r="H46" s="68"/>
-      <c r="I46" s="68"/>
-      <c r="J46" s="68"/>
-      <c r="K46" s="68"/>
-      <c r="L46" s="68"/>
-      <c r="M46" s="68"/>
-      <c r="N46" s="68"/>
-      <c r="O46" s="68"/>
-      <c r="P46" s="68"/>
-      <c r="Q46" s="68"/>
-      <c r="R46" s="68"/>
-      <c r="S46" s="68"/>
-      <c r="T46" s="68"/>
-      <c r="U46" s="68"/>
-      <c r="V46" s="68"/>
-      <c r="W46" s="68"/>
-      <c r="X46" s="68"/>
+      <c r="E46" s="61"/>
+      <c r="F46" s="61"/>
+      <c r="G46" s="61"/>
+      <c r="H46" s="61"/>
+      <c r="I46" s="61"/>
+      <c r="J46" s="61"/>
+      <c r="K46" s="61"/>
+      <c r="L46" s="61"/>
+      <c r="M46" s="61"/>
+      <c r="N46" s="61"/>
+      <c r="O46" s="61"/>
+      <c r="P46" s="61"/>
+      <c r="Q46" s="61"/>
+      <c r="R46" s="61"/>
+      <c r="S46" s="61"/>
+      <c r="T46" s="61"/>
+      <c r="U46" s="61"/>
+      <c r="V46" s="61"/>
+      <c r="W46" s="61"/>
+      <c r="X46" s="61"/>
       <c r="Y46" s="55"/>
     </row>
     <row r="47" spans="1:25" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -11549,13 +11644,13 @@
       <c r="Y50" s="38"/>
     </row>
     <row r="51" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="65" t="s">
+      <c r="A51" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="B51" s="65" t="s">
+      <c r="B51" s="58" t="s">
         <v>209</v>
       </c>
-      <c r="D51" s="66" t="s">
+      <c r="D51" s="59" t="s">
         <v>125</v>
       </c>
     </row>
@@ -13407,13 +13502,13 @@
         <v>126</v>
       </c>
       <c r="Q80" s="37" t="s">
-        <v>16</v>
+        <v>215</v>
       </c>
       <c r="R80" s="37" t="s">
-        <v>130</v>
+        <v>216</v>
       </c>
       <c r="S80" s="37" t="s">
-        <v>16</v>
+        <v>215</v>
       </c>
       <c r="T80" s="37" t="s">
         <v>130</v>
@@ -13430,7 +13525,7 @@
       <c r="X80" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="Y80" s="58" t="s">
+      <c r="Y80" s="62" t="s">
         <v>59</v>
       </c>
     </row>
@@ -13482,13 +13577,13 @@
         <v>126</v>
       </c>
       <c r="Q81" s="37" t="s">
-        <v>16</v>
+        <v>215</v>
       </c>
       <c r="R81" s="37" t="s">
-        <v>130</v>
+        <v>216</v>
       </c>
       <c r="S81" s="37" t="s">
-        <v>16</v>
+        <v>215</v>
       </c>
       <c r="T81" s="37" t="s">
         <v>130</v>
@@ -13505,7 +13600,7 @@
       <c r="X81" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="Y81" s="59"/>
+      <c r="Y81" s="63"/>
     </row>
     <row r="82" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A82" s="39" t="s">
@@ -13862,33 +13957,33 @@
       <c r="A91" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="B91" s="67" t="s">
+      <c r="B91" s="60" t="s">
         <v>212</v>
       </c>
-      <c r="C91" s="68"/>
-      <c r="D91" s="68" t="s">
+      <c r="C91" s="61"/>
+      <c r="D91" s="61" t="s">
         <v>125</v>
       </c>
-      <c r="E91" s="68"/>
-      <c r="F91" s="68"/>
-      <c r="G91" s="68"/>
-      <c r="H91" s="68"/>
-      <c r="I91" s="68"/>
-      <c r="J91" s="68"/>
-      <c r="K91" s="68"/>
-      <c r="L91" s="68"/>
-      <c r="M91" s="68"/>
-      <c r="N91" s="68"/>
-      <c r="O91" s="68"/>
-      <c r="P91" s="68"/>
-      <c r="Q91" s="68"/>
-      <c r="R91" s="68"/>
-      <c r="S91" s="68"/>
-      <c r="T91" s="68"/>
-      <c r="U91" s="68"/>
-      <c r="V91" s="68"/>
-      <c r="W91" s="68"/>
-      <c r="X91" s="68"/>
+      <c r="E91" s="61"/>
+      <c r="F91" s="61"/>
+      <c r="G91" s="61"/>
+      <c r="H91" s="61"/>
+      <c r="I91" s="61"/>
+      <c r="J91" s="61"/>
+      <c r="K91" s="61"/>
+      <c r="L91" s="61"/>
+      <c r="M91" s="61"/>
+      <c r="N91" s="61"/>
+      <c r="O91" s="61"/>
+      <c r="P91" s="61"/>
+      <c r="Q91" s="61"/>
+      <c r="R91" s="61"/>
+      <c r="S91" s="61"/>
+      <c r="T91" s="61"/>
+      <c r="U91" s="61"/>
+      <c r="V91" s="61"/>
+      <c r="W91" s="61"/>
+      <c r="X91" s="61"/>
       <c r="Y91" s="55"/>
     </row>
     <row r="92" spans="1:25" s="52" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -14048,14 +14143,20 @@
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C42" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="B43" sqref="B43"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="P70" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="R80" sqref="R80"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C48" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="D72" sqref="D72:X72"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
+      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
+      <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -14065,15 +14166,9 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
-      <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
-      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
+    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="C48" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="D72" sqref="D72:X72"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -14435,8 +14530,13 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}">
-      <selection activeCell="A22" sqref="A22"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
+      <selection activeCell="B17" sqref="B17"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
+      <selection activeCell="C7" sqref="C7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -14445,13 +14545,8 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
-      <selection activeCell="C7" sqref="C7"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
-      <selection activeCell="B17" sqref="B17"/>
+    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}">
+      <selection activeCell="A22" sqref="A22"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>

</xml_diff>

<commit_message>
Tarkista käyttäjän urakoiden haussa lisäoikeus oman urakan elyihin
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="32100" windowHeight="18460" tabRatio="500"/>
+    <workbookView xWindow="5880" yWindow="3560" windowWidth="42240" windowHeight="16540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -23,11 +23,11 @@
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="1605" windowHeight="750" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="2112" windowHeight="654" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
+    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office -käyttäjä - Oma näkymä" guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="1149" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="Mikko Rönkkömäki - Personal View" guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" mergeInterval="0" personalView="1" windowWidth="2560" windowHeight="1071" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Microsoft Office -käyttäjä - Oma näkymä" guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="1149" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -718,13 +718,13 @@
     <t>Kanavat / Lisätyöt</t>
   </si>
   <si>
-    <t>R,urakan-ely</t>
-  </si>
-  <si>
-    <t>R+,urakan-ely</t>
-  </si>
-  <si>
-    <t>Urakoitsija näkee vain oman urakkansa tiedot, ellei ole erikoisoikeutta urakan-ely, joka antaa näkyvyyden oman urakan ELY:n urakoihin.</t>
+    <t>R,oman-urakan-ely</t>
+  </si>
+  <si>
+    <t>R+,oman-urakan-ely</t>
+  </si>
+  <si>
+    <t>Urakoitsija näkee vain oman urakkansa tiedot, ellei ole erikoisoikeutta oman-urakan-ely, joka antaa näkyvyyden oman urakan ELY:n urakoihin.</t>
   </si>
 </sst>
 </file>
@@ -1196,10 +1196,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1210,12 +1216,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="185">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1415,7 +1415,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{5F66B6B9-B96F-DE4A-A457-5D2CA755059D}" diskRevisions="1" revisionId="719" version="33">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{12DFED72-64B6-AF46-A249-33E0D13E4C58}" diskRevisions="1" revisionId="727" version="34">
   <header guid="{1E352813-0B26-DB4E-84BE-460845B77133}" dateTime="2017-06-20T12:32:37" maxSheetId="3" userName="Microsoft Office -käyttäjä" r:id="rId60" minRId="448" maxRId="464">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1614,6 +1614,12 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{12DFED72-64B6-AF46-A249-33E0D13E4C58}" dateTime="2017-09-29T12:33:28" maxSheetId="3" userName="Microsoft Office User" r:id="rId93" minRId="720" maxRId="726">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -7966,6 +7972,101 @@
       <alignment wrapText="1"/>
     </dxf>
   </rfmt>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="delete"/>
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_7A9649F2_657F_9445_B6E6_FE94C6A09957_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Oikeudet!$A$5:$Y$95</formula>
+    <oldFormula>Oikeudet!$A$5:$Y$95</oldFormula>
+  </rdn>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog31.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="720" sId="1">
+    <oc r="Q80" t="inlineStr">
+      <is>
+        <t>R,urakan-ely</t>
+      </is>
+    </oc>
+    <nc r="Q80" t="inlineStr">
+      <is>
+        <t>R,oman-urakan-ely</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="721" sId="1">
+    <oc r="R80" t="inlineStr">
+      <is>
+        <t>R+,urakan-ely</t>
+      </is>
+    </oc>
+    <nc r="R80" t="inlineStr">
+      <is>
+        <t>R+,oman-urakan-ely</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="722" sId="1">
+    <oc r="S80" t="inlineStr">
+      <is>
+        <t>R,urakan-ely</t>
+      </is>
+    </oc>
+    <nc r="S80" t="inlineStr">
+      <is>
+        <t>R,oman-urakan-ely</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="723" sId="1">
+    <oc r="Y80" t="inlineStr">
+      <is>
+        <t>Urakoitsija näkee vain oman urakkansa tiedot, ellei ole erikoisoikeutta urakan-ely, joka antaa näkyvyyden oman urakan ELY:n urakoihin.</t>
+      </is>
+    </oc>
+    <nc r="Y80" t="inlineStr">
+      <is>
+        <t>Urakoitsija näkee vain oman urakkansa tiedot, ellei ole erikoisoikeutta oman-urakan-ely, joka antaa näkyvyyden oman urakan ELY:n urakoihin.</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="724" sId="1">
+    <oc r="Q81" t="inlineStr">
+      <is>
+        <t>R,urakan-ely</t>
+      </is>
+    </oc>
+    <nc r="Q81" t="inlineStr">
+      <is>
+        <t>R,oman-urakan-ely</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="725" sId="1">
+    <oc r="R81" t="inlineStr">
+      <is>
+        <t>R+,urakan-ely</t>
+      </is>
+    </oc>
+    <nc r="R81" t="inlineStr">
+      <is>
+        <t>R+,oman-urakan-ely</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="726" sId="1">
+    <oc r="S81" t="inlineStr">
+      <is>
+        <t>R,urakan-ely</t>
+      </is>
+    </oc>
+    <nc r="S81" t="inlineStr">
+      <is>
+        <t>R,oman-urakan-ely</t>
+      </is>
+    </nc>
+  </rcc>
   <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="delete"/>
   <rdn rId="0" localSheetId="1" customView="1" name="Z_7A9649F2_657F_9445_B6E6_FE94C6A09957_.wvu.FilterData" hidden="1" oldHidden="1">
     <formula>Oikeudet!$A$5:$Y$95</formula>
@@ -8959,10 +9060,10 @@
   <dimension ref="A1:Y95"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="U70" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="S70" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="Y72" sqref="Y72"/>
+      <selection pane="bottomRight" activeCell="Y73" sqref="Y73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8991,7 +9092,7 @@
     <col min="22" max="22" width="11.5" customWidth="1"/>
     <col min="23" max="23" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="11.1640625" customWidth="1"/>
-    <col min="25" max="25" width="53.83203125" customWidth="1"/>
+    <col min="25" max="25" width="59" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="24" customHeight="1" x14ac:dyDescent="0.15">
@@ -8999,40 +9100,40 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="64" t="s">
+      <c r="C1" s="66" t="s">
         <v>149</v>
       </c>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="67"/>
+      <c r="M1" s="67"/>
+      <c r="N1" s="67"/>
+      <c r="O1" s="67"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="66" t="s">
+      <c r="C2" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="67"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="67"/>
-      <c r="O2" s="67"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="69"/>
+      <c r="M2" s="69"/>
+      <c r="N2" s="69"/>
+      <c r="O2" s="69"/>
     </row>
     <row r="3" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
@@ -9055,34 +9156,34 @@
     <row r="5" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="30"/>
       <c r="B5" s="30"/>
-      <c r="C5" s="63" t="s">
+      <c r="C5" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="62"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65"/>
       <c r="I5" s="30"/>
       <c r="J5" s="30"/>
-      <c r="K5" s="63" t="s">
+      <c r="K5" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="L5" s="62"/>
-      <c r="M5" s="62"/>
-      <c r="N5" s="62"/>
-      <c r="O5" s="62"/>
+      <c r="L5" s="65"/>
+      <c r="M5" s="65"/>
+      <c r="N5" s="65"/>
+      <c r="O5" s="65"/>
       <c r="P5" s="30"/>
       <c r="Q5" s="30"/>
-      <c r="R5" s="63" t="s">
+      <c r="R5" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="S5" s="62"/>
-      <c r="T5" s="62"/>
-      <c r="U5" s="62"/>
-      <c r="V5" s="62"/>
-      <c r="W5" s="62"/>
-      <c r="X5" s="62"/>
+      <c r="S5" s="65"/>
+      <c r="T5" s="65"/>
+      <c r="U5" s="65"/>
+      <c r="V5" s="65"/>
+      <c r="W5" s="65"/>
+      <c r="X5" s="65"/>
       <c r="Y5" s="31" t="s">
         <v>13</v>
       </c>
@@ -13562,7 +13663,7 @@
       <c r="X80" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="Y80" s="68" t="s">
+      <c r="Y80" s="62" t="s">
         <v>216</v>
       </c>
     </row>
@@ -13637,7 +13738,7 @@
       <c r="X81" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="Y81" s="69"/>
+      <c r="Y81" s="63"/>
     </row>
     <row r="82" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A82" s="39" t="s">
@@ -14180,14 +14281,20 @@
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="U70" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="Y72" sqref="Y72"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="S70" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="Y73" sqref="Y73"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C48" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="D72" sqref="D72:X72"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
+      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
+      <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -14197,15 +14304,9 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
-      <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
-      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
+    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="C48" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="D72" sqref="D72:X72"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -14567,8 +14668,13 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}">
-      <selection activeCell="A22" sqref="A22"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
+      <selection activeCell="B17" sqref="B17"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
+      <selection activeCell="C7" sqref="C7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -14577,13 +14683,8 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
-      <selection activeCell="C7" sqref="C7"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
-      <selection activeCell="B17" sqref="B17"/>
+    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}">
+      <selection activeCell="A22" sqref="A22"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>

</xml_diff>

<commit_message>
Lisää oman-urakan-ely erikoisoikeus roolille Tilaajan rakennuttajakonsultti
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5880" yWindow="3560" windowWidth="42240" windowHeight="16540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="42240" windowHeight="14620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -23,11 +23,11 @@
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="2112" windowHeight="654" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="2112" windowHeight="558" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Mikko Rönkkömäki - Personal View" guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" mergeInterval="0" personalView="1" windowWidth="2560" windowHeight="1071" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office -käyttäjä - Oma näkymä" guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="1149" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
-    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Microsoft Office -käyttäjä - Oma näkymä" guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="1149" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Mikko Rönkkömäki - Personal View" guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" mergeInterval="0" personalView="1" windowWidth="2560" windowHeight="1071" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -1415,7 +1415,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{12DFED72-64B6-AF46-A249-33E0D13E4C58}" diskRevisions="1" revisionId="727" version="34">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{58BA8950-DC2E-E64B-8D55-A1BA526CF2D2}" diskRevisions="1" revisionId="730" version="35">
   <header guid="{1E352813-0B26-DB4E-84BE-460845B77133}" dateTime="2017-06-20T12:32:37" maxSheetId="3" userName="Microsoft Office -käyttäjä" r:id="rId60" minRId="448" maxRId="464">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1620,6 +1620,12 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{58BA8950-DC2E-E64B-8D55-A1BA526CF2D2}" dateTime="2017-09-29T13:50:27" maxSheetId="3" userName="Microsoft Office User" r:id="rId94" minRId="728" maxRId="729">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -8062,6 +8068,63 @@
       </is>
     </oc>
     <nc r="S81" t="inlineStr">
+      <is>
+        <t>R,oman-urakan-ely</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="delete"/>
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_7A9649F2_657F_9445_B6E6_FE94C6A09957_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Oikeudet!$A$5:$Y$95</formula>
+    <oldFormula>Oikeudet!$A$5:$Y$95</oldFormula>
+  </rdn>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog32.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" xfDxf="1" sqref="J80" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rcc rId="728" sId="1">
+    <oc r="J80" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </oc>
+    <nc r="J80" t="inlineStr">
+      <is>
+        <t>R,oman-urakan-ely</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="729" sId="1">
+    <oc r="J81" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </oc>
+    <nc r="J81" t="inlineStr">
       <is>
         <t>R,oman-urakan-ely</t>
       </is>
@@ -9060,10 +9123,10 @@
   <dimension ref="A1:Y95"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="S70" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C72" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="Y73" sqref="Y73"/>
+      <selection pane="bottomRight" activeCell="J80" sqref="J80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -13619,7 +13682,7 @@
         <v>125</v>
       </c>
       <c r="J80" s="37" t="s">
-        <v>16</v>
+        <v>214</v>
       </c>
       <c r="K80" s="37" t="s">
         <v>125</v>
@@ -13694,7 +13757,7 @@
         <v>125</v>
       </c>
       <c r="J81" s="37" t="s">
-        <v>16</v>
+        <v>214</v>
       </c>
       <c r="K81" s="37" t="s">
         <v>125</v>
@@ -14281,14 +14344,20 @@
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="S70" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="Y73" sqref="Y73"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C72" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="J80" sqref="J80"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
-      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
+    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="C48" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="D72" sqref="D72:X72"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="C31" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -14298,15 +14367,9 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C31" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C48" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="D72" sqref="D72:X72"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
+      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -14668,8 +14731,13 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
-      <selection activeCell="B17" sqref="B17"/>
+    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}">
+      <selection activeCell="A22" sqref="A22"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}">
+      <selection activeCell="G36" sqref="G36"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -14678,13 +14746,8 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}">
-      <selection activeCell="G36" sqref="G36"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}">
-      <selection activeCell="A22" sqref="A22"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
+      <selection activeCell="B17" sqref="B17"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>

</xml_diff>

<commit_message>
Lisää oikeustarkistus alusten muokkaukselle
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="3340" windowWidth="46340" windowHeight="22940" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="46340" windowHeight="19240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -23,11 +23,11 @@
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="2317" windowHeight="974" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="2317" windowHeight="789" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Mikko Rönkkömäki - Personal View" guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" mergeInterval="0" personalView="1" windowWidth="2560" windowHeight="1071" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office -käyttäjä - Oma näkymä" guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="1149" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
-    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Microsoft Office -käyttäjä - Oma näkymä" guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="1149" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Mikko Rönkkömäki - Personal View" guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" mergeInterval="0" personalView="1" windowWidth="2560" windowHeight="1071" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1446" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1446" uniqueCount="222">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -737,6 +737,9 @@
   </si>
   <si>
     <t>R,W,aseta-näkyviin-urakoitsijalle</t>
+  </si>
+  <si>
+    <t>R,W,alusten-muokkaus</t>
   </si>
 </sst>
 </file>
@@ -1428,7 +1431,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{CFAAB58E-5CF4-9746-AF6D-FBD3E192F34E}" diskRevisions="1" revisionId="739" version="36">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{0BEF1B45-C0BB-CB40-A91E-FC4F2671A39B}" diskRevisions="1" revisionId="741" version="37">
   <header guid="{1E352813-0B26-DB4E-84BE-460845B77133}" dateTime="2017-06-20T12:32:37" maxSheetId="3" userName="Microsoft Office -käyttäjä" r:id="rId60" minRId="448" maxRId="464">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1645,6 +1648,12 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{0BEF1B45-C0BB-CB40-A91E-FC4F2671A39B}" dateTime="2017-10-25T11:03:22" maxSheetId="3" userName="Microsoft Office User" r:id="rId96" minRId="740">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -8265,6 +8274,29 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog34.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="740" sId="1">
+    <oc r="S7" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </oc>
+    <nc r="S7" t="inlineStr">
+      <is>
+        <t>R,W,alusten-muokkaus</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="delete"/>
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_7A9649F2_657F_9445_B6E6_FE94C6A09957_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Oikeudet!$A$5:$Y$95</formula>
+    <oldFormula>Oikeudet!$A$5:$Y$95</oldFormula>
+  </rdn>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="499" sId="1">
@@ -8916,7 +8948,7 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="3">
   <userInfo guid="{1E352813-0B26-DB4E-84BE-460845B77133}" name="Microsoft Office -käyttäjä" id="-785751636" dateTime="2017-06-20T12:33:00"/>
   <userInfo guid="{1AB7A282-42ED-4740-A9CB-95FF229EC1A0}" name="Mikko Rönkkömäki" id="-727946492" dateTime="2017-06-22T10:45:48"/>
@@ -9249,10 +9281,10 @@
   <dimension ref="A1:Y95"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C13" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="Q7" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D21" sqref="D21"/>
+      <selection pane="bottomRight" activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9504,7 +9536,7 @@
         <v>130</v>
       </c>
       <c r="S7" s="36" t="s">
-        <v>111</v>
+        <v>221</v>
       </c>
       <c r="T7" s="37" t="s">
         <v>129</v>
@@ -14470,14 +14502,20 @@
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C13" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="D21" sqref="D21"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="Q7" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="S7" sqref="S7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
-      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
+    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="C48" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="D72" sqref="D72:X72"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="C31" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -14487,15 +14525,9 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C31" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C48" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="D72" sqref="D72:X72"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
+      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -14857,8 +14889,13 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
-      <selection activeCell="B17" sqref="B17"/>
+    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}">
+      <selection activeCell="A22" sqref="A22"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}">
+      <selection activeCell="G36" sqref="G36"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -14867,13 +14904,8 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}">
-      <selection activeCell="G36" sqref="G36"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}">
-      <selection activeCell="A22" sqref="A22"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
+      <selection activeCell="B17" sqref="B17"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>

</xml_diff>

<commit_message>
Lisää oikeus muokaya aluksia myös JVH:lle
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="46340" windowHeight="19240" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="46340" windowHeight="17320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -23,11 +23,11 @@
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="2317" windowHeight="789" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="2317" windowHeight="693" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
+    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office -käyttäjä - Oma näkymä" guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="1149" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="Mikko Rönkkömäki - Personal View" guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" mergeInterval="0" personalView="1" windowWidth="2560" windowHeight="1071" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Microsoft Office -käyttäjä - Oma näkymä" guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="1149" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1446" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1446" uniqueCount="223">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -740,6 +740,9 @@
   </si>
   <si>
     <t>R,W,alusten-muokkaus</t>
+  </si>
+  <si>
+    <t>R*,W*,alusten-muokkaus*</t>
   </si>
 </sst>
 </file>
@@ -1431,7 +1434,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{0BEF1B45-C0BB-CB40-A91E-FC4F2671A39B}" diskRevisions="1" revisionId="741" version="37">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{72187562-2E05-9542-A596-E87B0EC7A6D4}" diskRevisions="1" revisionId="743" version="38">
   <header guid="{1E352813-0B26-DB4E-84BE-460845B77133}" dateTime="2017-06-20T12:32:37" maxSheetId="3" userName="Microsoft Office -käyttäjä" r:id="rId60" minRId="448" maxRId="464">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1654,6 +1657,12 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{72187562-2E05-9542-A596-E87B0EC7A6D4}" dateTime="2017-10-25T11:07:50" maxSheetId="3" userName="Microsoft Office User" r:id="rId97" minRId="742">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -8297,6 +8306,29 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog35.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="742" sId="1">
+    <oc r="D7" t="inlineStr">
+      <is>
+        <t>R*,W*</t>
+      </is>
+    </oc>
+    <nc r="D7" t="inlineStr">
+      <is>
+        <t>R*,W*,alusten-muokkaus*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="delete"/>
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_7A9649F2_657F_9445_B6E6_FE94C6A09957_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Oikeudet!$A$5:$Y$95</formula>
+    <oldFormula>Oikeudet!$A$5:$Y$95</oldFormula>
+  </rdn>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="499" sId="1">
@@ -8948,7 +8980,7 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="3">
   <userInfo guid="{1E352813-0B26-DB4E-84BE-460845B77133}" name="Microsoft Office -käyttäjä" id="-785751636" dateTime="2017-06-20T12:33:00"/>
   <userInfo guid="{1AB7A282-42ED-4740-A9CB-95FF229EC1A0}" name="Mikko Rönkkömäki" id="-727946492" dateTime="2017-06-22T10:45:48"/>
@@ -9281,10 +9313,10 @@
   <dimension ref="A1:Y95"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="Q7" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="S7" sqref="S7"/>
+      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9491,7 +9523,7 @@
       </c>
       <c r="C7" s="36"/>
       <c r="D7" s="36" t="s">
-        <v>124</v>
+        <v>222</v>
       </c>
       <c r="E7" s="36" t="s">
         <v>128</v>
@@ -14502,14 +14534,20 @@
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="Q7" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="S7" sqref="S7"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C48" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="D72" sqref="D72:X72"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
+      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
+      <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -14519,15 +14557,9 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
-      <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
-      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
+    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="C48" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="D72" sqref="D72:X72"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -14889,8 +14921,13 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}">
-      <selection activeCell="A22" sqref="A22"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
+      <selection activeCell="B17" sqref="B17"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
+      <selection activeCell="C7" sqref="C7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -14899,13 +14936,8 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
-      <selection activeCell="C7" sqref="C7"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
-      <selection activeCell="B17" sqref="B17"/>
+    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}">
+      <selection activeCell="A22" sqref="A22"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>

</xml_diff>

<commit_message>
Lisää oikeustarkistus ja sille testi.
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarihan/Jari/Tyo/Solita/Projektit/Harja/harja/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joonasmi/projects/harja/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="46340" windowHeight="17320" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="46340" windowHeight="15400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -23,11 +23,11 @@
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="2317" windowHeight="693" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="2317" windowHeight="597" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Mikko Rönkkömäki - Personal View" guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" mergeInterval="0" personalView="1" windowWidth="2560" windowHeight="1071" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office -käyttäjä - Oma näkymä" guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="1149" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
-    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Microsoft Office -käyttäjä - Oma näkymä" guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="1149" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Mikko Rönkkömäki - Personal View" guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" mergeInterval="0" personalView="1" windowWidth="2560" windowHeight="1071" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1446" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1446" uniqueCount="225">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -743,6 +743,12 @@
   </si>
   <si>
     <t>R*,W*,alusten-muokkaus*</t>
+  </si>
+  <si>
+    <t>R*,W*,siirrä-kokonaishintaisiin*</t>
+  </si>
+  <si>
+    <t>R*,W*,siirrä-muutos-ja-lisätöihin*</t>
   </si>
 </sst>
 </file>
@@ -1434,7 +1440,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{72187562-2E05-9542-A596-E87B0EC7A6D4}" diskRevisions="1" revisionId="743" version="38">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{7DE0565B-D0D5-DF45-A2A1-25AA2C726E19}" diskRevisions="1" revisionId="747" version="40">
   <header guid="{1E352813-0B26-DB4E-84BE-460845B77133}" dateTime="2017-06-20T12:32:37" maxSheetId="3" userName="Microsoft Office -käyttäjä" r:id="rId60" minRId="448" maxRId="464">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1663,6 +1669,18 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{BE47CF9D-4E1C-F649-96CB-C204CD8DEBF8}" dateTime="2017-11-20T14:55:15" maxSheetId="3" userName="Microsoft Office User" r:id="rId98" minRId="744">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{7DE0565B-D0D5-DF45-A2A1-25AA2C726E19}" dateTime="2017-11-20T15:19:18" maxSheetId="3" userName="Microsoft Office User" r:id="rId99" minRId="746" maxRId="747">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -8329,6 +8347,58 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog36.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="744" sId="1">
+    <oc r="D45" t="inlineStr">
+      <is>
+        <t>R*,W*</t>
+      </is>
+    </oc>
+    <nc r="D45" t="inlineStr">
+      <is>
+        <t>R*,W*,siirrä-kokonaishintaisiin*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="delete"/>
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_7A9649F2_657F_9445_B6E6_FE94C6A09957_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Oikeudet!$A$5:$Y$95</formula>
+    <oldFormula>Oikeudet!$A$5:$Y$95</oldFormula>
+  </rdn>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog37.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="746" sId="1">
+    <oc r="D45" t="inlineStr">
+      <is>
+        <t>R*,W*,siirrä-kokonaishintaisiin*</t>
+      </is>
+    </oc>
+    <nc r="D45" t="inlineStr">
+      <is>
+        <t>R*,W*,siirrä-muutos-ja-lisätöihin*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="747" sId="1">
+    <oc r="D46" t="inlineStr">
+      <is>
+        <t>R*,W*</t>
+      </is>
+    </oc>
+    <nc r="D46" t="inlineStr">
+      <is>
+        <t>R*,W*,siirrä-kokonaishintaisiin*</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="499" sId="1">
@@ -8981,11 +9051,12 @@
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="4">
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="5">
   <userInfo guid="{1E352813-0B26-DB4E-84BE-460845B77133}" name="Microsoft Office -käyttäjä" id="-785751636" dateTime="2017-06-20T12:33:00"/>
   <userInfo guid="{1AB7A282-42ED-4740-A9CB-95FF229EC1A0}" name="Mikko Rönkkömäki" id="-727946492" dateTime="2017-06-22T10:45:48"/>
   <userInfo guid="{4A189F6B-10A0-794F-AE26-98E1292E0A90}" name="Microsoft Office User" id="-296987972" dateTime="2017-09-21T08:10:21"/>
   <userInfo guid="{72187562-2E05-9542-A596-E87B0EC7A6D4}" name="Microsoft Office User" id="-296946728" dateTime="2017-11-06T12:39:34"/>
+  <userInfo guid="{7DE0565B-D0D5-DF45-A2A1-25AA2C726E19}" name="Microsoft Office User" id="-296947028" dateTime="2017-11-20T14:54:25"/>
 </users>
 </file>
 
@@ -9314,10 +9385,10 @@
   <dimension ref="A1:Y95"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C41" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -11808,7 +11879,7 @@
       </c>
       <c r="C45" s="61"/>
       <c r="D45" s="61" t="s">
-        <v>124</v>
+        <v>224</v>
       </c>
       <c r="E45" s="61"/>
       <c r="F45" s="61"/>
@@ -11841,7 +11912,7 @@
       </c>
       <c r="C46" s="61"/>
       <c r="D46" s="61" t="s">
-        <v>124</v>
+        <v>223</v>
       </c>
       <c r="E46" s="61"/>
       <c r="F46" s="61"/>
@@ -14535,14 +14606,20 @@
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C41" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="D46" sqref="D46"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
-      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
+    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="C48" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="D72" sqref="D72:X72"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="C31" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -14552,15 +14629,9 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C31" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C48" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="D72" sqref="D72:X72"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
+      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -14922,8 +14993,13 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
-      <selection activeCell="B17" sqref="B17"/>
+    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}">
+      <selection activeCell="A22" sqref="A22"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}">
+      <selection activeCell="G36" sqref="G36"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -14932,13 +15008,8 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}">
-      <selection activeCell="G36" sqref="G36"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}">
-      <selection activeCell="A22" sqref="A22"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
+      <selection activeCell="B17" sqref="B17"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>

</xml_diff>

<commit_message>
Tee oikeustarkastukset, muokkaa lomakeen ulkoasua, muuta kan_hairio taulukon pvm sarake timestampiksi
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -9,25 +9,25 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="46340" windowHeight="15400" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
     <sheet name="Roolit" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$95</definedName>
-    <definedName name="Z_1DD617EE_F308_3E45_A8EF_4713F47FA0DD_.wvu.FilterData" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$95</definedName>
-    <definedName name="Z_7A9649F2_657F_9445_B6E6_FE94C6A09957_.wvu.FilterData" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$95</definedName>
-    <definedName name="Z_F86DF6F3_8AE5_3A44_B2D2_D623E01AE54F_.wvu.FilterData" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$95</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$96</definedName>
+    <definedName name="Z_1DD617EE_F308_3E45_A8EF_4713F47FA0DD_.wvu.FilterData" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$96</definedName>
+    <definedName name="Z_7A9649F2_657F_9445_B6E6_FE94C6A09957_.wvu.FilterData" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$96</definedName>
+    <definedName name="Z_F86DF6F3_8AE5_3A44_B2D2_D623E01AE54F_.wvu.FilterData" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$96</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="2317" windowHeight="597" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="2560" windowHeight="1254" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
+    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office -käyttäjä - Oma näkymä" guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="1149" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="Mikko Rönkkömäki - Personal View" guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" mergeInterval="0" personalView="1" windowWidth="2560" windowHeight="1071" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Microsoft Office -käyttäjä - Oma näkymä" guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="1149" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1446" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1449" uniqueCount="226">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -749,6 +749,9 @@
   </si>
   <si>
     <t>R*,W*,siirrä-muutos-ja-lisätöihin*</t>
+  </si>
+  <si>
+    <t>Kanavat / Laadunseuranta / Häiriötilanteet</t>
   </si>
 </sst>
 </file>
@@ -1097,7 +1100,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -1221,6 +1224,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1241,6 +1245,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="185">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1440,7 +1456,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{7DE0565B-D0D5-DF45-A2A1-25AA2C726E19}" diskRevisions="1" revisionId="747" version="40">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{0602C519-A1BE-AE48-B457-EFC7185CD0F1}" diskRevisions="1" revisionId="757" version="41">
   <header guid="{1E352813-0B26-DB4E-84BE-460845B77133}" dateTime="2017-06-20T12:32:37" maxSheetId="3" userName="Microsoft Office -käyttäjä" r:id="rId60" minRId="448" maxRId="464">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1681,6 +1697,12 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{0602C519-A1BE-AE48-B457-EFC7185CD0F1}" dateTime="2017-11-30T10:32:34" maxSheetId="3" userName="Microsoft Office User" r:id="rId100" minRId="748" maxRId="756">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -8399,6 +8421,1108 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog38.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="748" sId="1" ref="A46:XFD46" action="insertRow"/>
+  <rrc rId="749" sId="1" ref="A46:XFD46" action="insertRow"/>
+  <rm rId="750" sheetId="1" source="A53:XFD53" destination="A46:XFD46" sourceSheetId="1">
+    <rfmt sheetId="1" xfDxf="1" sqref="A46:XFD46" start="0" length="0"/>
+    <rfmt sheetId="1" sqref="A46" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <border outline="0">
+          <left style="thin">
+            <color auto="1"/>
+          </left>
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="B46" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="C46" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="D46" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="E46" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="F46" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="G46" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="H46" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="I46" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="J46" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="K46" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="L46" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="M46" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="N46" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="O46" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="P46" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="Q46" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="R46" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="S46" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="T46" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="U46" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="V46" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="W46" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="X46" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+  </rm>
+  <rrc rId="751" sId="1" ref="A53:XFD53" action="deleteRow">
+    <rfmt sheetId="1" xfDxf="1" sqref="A53:XFD53" start="0" length="0"/>
+  </rrc>
+  <rrc rId="752" sId="1" ref="A47:XFD47" action="deleteRow">
+    <rfmt sheetId="1" xfDxf="1" sqref="A47:XFD47" start="0" length="0"/>
+    <rfmt sheetId="1" sqref="A47" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <border outline="0">
+          <left style="thin">
+            <color auto="1"/>
+          </left>
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="B47" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="C47" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="D47" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="E47" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="F47" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="G47" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="H47" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="I47" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="J47" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="K47" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="L47" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="M47" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="N47" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="O47" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="P47" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="Q47" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="R47" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="S47" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="T47" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="U47" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="V47" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="W47" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="X47" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+  </rrc>
+  <rrc rId="753" sId="1" ref="A45:XFD45" action="insertRow"/>
+  <rcc rId="754" sId="1">
+    <nc r="A45" t="inlineStr">
+      <is>
+        <t>Urakat</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="755" sId="1">
+    <nc r="B45" t="inlineStr">
+      <is>
+        <t>Kanavat / Laadunseuranta / Häiriötilanteet</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="756" sId="1">
+    <nc r="D45" t="inlineStr">
+      <is>
+        <t>R*,W*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="delete"/>
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_7A9649F2_657F_9445_B6E6_FE94C6A09957_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Oikeudet!$A$5:$Y$96</formula>
+    <oldFormula>Oikeudet!$A$5:$Y$96</oldFormula>
+  </rdn>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="499" sId="1">
@@ -9050,7 +10174,7 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="5">
   <userInfo guid="{1E352813-0B26-DB4E-84BE-460845B77133}" name="Microsoft Office -käyttäjä" id="-785751636" dateTime="2017-06-20T12:33:00"/>
   <userInfo guid="{1AB7A282-42ED-4740-A9CB-95FF229EC1A0}" name="Mikko Rönkkömäki" id="-727946492" dateTime="2017-06-22T10:45:48"/>
@@ -9382,13 +10506,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y95"/>
+  <dimension ref="A1:Y96"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C41" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C18" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D47" sqref="D47"/>
+      <selection pane="bottomRight" activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9425,40 +10549,40 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="67" t="s">
+      <c r="C1" s="68" t="s">
         <v>149</v>
       </c>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
+      <c r="M1" s="69"/>
+      <c r="N1" s="69"/>
+      <c r="O1" s="69"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="69" t="s">
+      <c r="C2" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
-      <c r="O2" s="70"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
+      <c r="O2" s="71"/>
     </row>
     <row r="3" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
@@ -9481,34 +10605,34 @@
     <row r="5" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="30"/>
       <c r="B5" s="30"/>
-      <c r="C5" s="65" t="s">
+      <c r="C5" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
       <c r="I5" s="30"/>
       <c r="J5" s="30"/>
-      <c r="K5" s="65" t="s">
+      <c r="K5" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="L5" s="66"/>
-      <c r="M5" s="66"/>
-      <c r="N5" s="66"/>
-      <c r="O5" s="66"/>
+      <c r="L5" s="67"/>
+      <c r="M5" s="67"/>
+      <c r="N5" s="67"/>
+      <c r="O5" s="67"/>
       <c r="P5" s="30"/>
       <c r="Q5" s="30"/>
-      <c r="R5" s="65" t="s">
+      <c r="R5" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="S5" s="66"/>
-      <c r="T5" s="66"/>
-      <c r="U5" s="66"/>
-      <c r="V5" s="66"/>
-      <c r="W5" s="66"/>
-      <c r="X5" s="66"/>
+      <c r="S5" s="67"/>
+      <c r="T5" s="67"/>
+      <c r="U5" s="67"/>
+      <c r="V5" s="67"/>
+      <c r="W5" s="67"/>
+      <c r="X5" s="67"/>
       <c r="Y5" s="31" t="s">
         <v>13</v>
       </c>
@@ -11870,49 +12994,49 @@
         <v>197</v>
       </c>
     </row>
-    <row r="45" spans="1:25" s="57" customFormat="1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A45" s="35" t="s">
+    <row r="45" spans="1:25" s="63" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A45" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="B45" s="60" t="s">
-        <v>212</v>
-      </c>
-      <c r="C45" s="61"/>
-      <c r="D45" s="61" t="s">
-        <v>224</v>
-      </c>
-      <c r="E45" s="61"/>
-      <c r="F45" s="61"/>
-      <c r="G45" s="61"/>
-      <c r="H45" s="61"/>
-      <c r="I45" s="61"/>
-      <c r="J45" s="61"/>
-      <c r="K45" s="61"/>
-      <c r="L45" s="61"/>
-      <c r="M45" s="61"/>
-      <c r="N45" s="61"/>
+      <c r="B45" s="72" t="s">
+        <v>225</v>
+      </c>
+      <c r="C45" s="73"/>
+      <c r="D45" s="74" t="s">
+        <v>124</v>
+      </c>
+      <c r="E45" s="74"/>
+      <c r="F45" s="73"/>
+      <c r="G45" s="73"/>
+      <c r="H45" s="73"/>
+      <c r="I45" s="73"/>
+      <c r="J45" s="74"/>
+      <c r="K45" s="74"/>
+      <c r="L45" s="74"/>
+      <c r="M45" s="73"/>
+      <c r="N45" s="73"/>
       <c r="O45" s="61"/>
       <c r="P45" s="61"/>
-      <c r="Q45" s="61"/>
-      <c r="R45" s="61"/>
-      <c r="S45" s="61"/>
-      <c r="T45" s="61"/>
-      <c r="U45" s="61"/>
+      <c r="Q45" s="73"/>
+      <c r="R45" s="74"/>
+      <c r="S45" s="75"/>
+      <c r="T45" s="73"/>
+      <c r="U45" s="73"/>
       <c r="V45" s="61"/>
-      <c r="W45" s="61"/>
-      <c r="X45" s="61"/>
-      <c r="Y45" s="56"/>
+      <c r="W45" s="73"/>
+      <c r="X45" s="73"/>
+      <c r="Y45" s="55"/>
     </row>
-    <row r="46" spans="1:25" s="57" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:25" s="57" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A46" s="35" t="s">
         <v>14</v>
       </c>
       <c r="B46" s="60" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C46" s="61"/>
       <c r="D46" s="61" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E46" s="61"/>
       <c r="F46" s="61"/>
@@ -11934,100 +13058,58 @@
       <c r="V46" s="61"/>
       <c r="W46" s="61"/>
       <c r="X46" s="61"/>
-      <c r="Y46" s="55"/>
+      <c r="Y46" s="56"/>
     </row>
-    <row r="47" spans="1:25" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="39" t="s">
+    <row r="47" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="B47" s="39" t="s">
-        <v>183</v>
-      </c>
-      <c r="C47" s="37"/>
-      <c r="D47" s="36" t="s">
+      <c r="B47" s="58" t="s">
+        <v>208</v>
+      </c>
+      <c r="D47" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="E47" s="36"/>
-      <c r="F47" s="37"/>
-      <c r="G47" s="37"/>
-      <c r="H47" s="37"/>
-      <c r="I47" s="37"/>
-      <c r="J47" s="37"/>
-      <c r="K47" s="36"/>
-      <c r="L47" s="37"/>
-      <c r="M47" s="37"/>
-      <c r="N47" s="37"/>
-      <c r="O47" s="36"/>
-      <c r="P47" s="36"/>
-      <c r="Q47" s="37"/>
-      <c r="R47" s="37"/>
-      <c r="S47" s="37"/>
-      <c r="T47" s="37"/>
-      <c r="U47" s="37"/>
-      <c r="V47" s="36"/>
-      <c r="W47" s="37"/>
-      <c r="X47" s="37"/>
-      <c r="Y47" s="38"/>
     </row>
-    <row r="48" spans="1:25" s="26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="39" t="s">
+    <row r="48" spans="1:25" s="57" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B48" s="39" t="s">
-        <v>184</v>
-      </c>
-      <c r="C48" s="37"/>
-      <c r="D48" s="36" t="s">
-        <v>187</v>
-      </c>
-      <c r="E48" s="30" t="s">
-        <v>189</v>
-      </c>
-      <c r="F48" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="G48" s="37"/>
-      <c r="H48" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="I48" s="37"/>
-      <c r="J48" s="37" t="s">
-        <v>188</v>
-      </c>
-      <c r="K48" s="36"/>
-      <c r="L48" s="36"/>
-      <c r="M48" s="37"/>
-      <c r="N48" s="37"/>
-      <c r="O48" s="36"/>
-      <c r="P48" s="36"/>
-      <c r="Q48" s="37"/>
-      <c r="R48" s="37" t="s">
-        <v>205</v>
-      </c>
-      <c r="S48" s="37" t="s">
-        <v>206</v>
-      </c>
-      <c r="T48" s="37" t="s">
-        <v>205</v>
-      </c>
-      <c r="U48" s="37" t="s">
-        <v>206</v>
-      </c>
-      <c r="V48" s="36" t="s">
-        <v>205</v>
-      </c>
-      <c r="W48" s="37"/>
-      <c r="X48" s="37"/>
-      <c r="Y48" s="38" t="s">
-        <v>193</v>
-      </c>
+      <c r="B48" s="60" t="s">
+        <v>213</v>
+      </c>
+      <c r="C48" s="61"/>
+      <c r="D48" s="61" t="s">
+        <v>223</v>
+      </c>
+      <c r="E48" s="61"/>
+      <c r="F48" s="61"/>
+      <c r="G48" s="61"/>
+      <c r="H48" s="61"/>
+      <c r="I48" s="61"/>
+      <c r="J48" s="61"/>
+      <c r="K48" s="61"/>
+      <c r="L48" s="61"/>
+      <c r="M48" s="61"/>
+      <c r="N48" s="61"/>
+      <c r="O48" s="61"/>
+      <c r="P48" s="61"/>
+      <c r="Q48" s="61"/>
+      <c r="R48" s="61"/>
+      <c r="S48" s="61"/>
+      <c r="T48" s="61"/>
+      <c r="U48" s="61"/>
+      <c r="V48" s="61"/>
+      <c r="W48" s="61"/>
+      <c r="X48" s="61"/>
+      <c r="Y48" s="55"/>
     </row>
     <row r="49" spans="1:25" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="39" t="s">
         <v>14</v>
       </c>
       <c r="B49" s="39" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C49" s="37"/>
       <c r="D49" s="36" t="s">
@@ -12055,19 +13137,19 @@
       <c r="X49" s="37"/>
       <c r="Y49" s="38"/>
     </row>
-    <row r="50" spans="1:25" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:25" s="26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="39" t="s">
         <v>14</v>
       </c>
       <c r="B50" s="39" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C50" s="37"/>
       <c r="D50" s="36" t="s">
-        <v>124</v>
-      </c>
-      <c r="E50" s="36" t="s">
-        <v>128</v>
+        <v>187</v>
+      </c>
+      <c r="E50" s="30" t="s">
+        <v>189</v>
       </c>
       <c r="F50" s="37" t="s">
         <v>125</v>
@@ -12078,104 +13160,126 @@
       </c>
       <c r="I50" s="37"/>
       <c r="J50" s="37" t="s">
-        <v>111</v>
+        <v>188</v>
       </c>
       <c r="K50" s="36"/>
-      <c r="L50" s="37"/>
+      <c r="L50" s="36"/>
       <c r="M50" s="37"/>
       <c r="N50" s="37"/>
       <c r="O50" s="36"/>
       <c r="P50" s="36"/>
       <c r="Q50" s="37"/>
       <c r="R50" s="37" t="s">
-        <v>130</v>
+        <v>205</v>
       </c>
       <c r="S50" s="37" t="s">
-        <v>111</v>
+        <v>206</v>
       </c>
       <c r="T50" s="37" t="s">
-        <v>129</v>
+        <v>205</v>
       </c>
       <c r="U50" s="37" t="s">
-        <v>16</v>
+        <v>206</v>
       </c>
       <c r="V50" s="36" t="s">
-        <v>129</v>
+        <v>205</v>
       </c>
       <c r="W50" s="37"/>
       <c r="X50" s="37"/>
-      <c r="Y50" s="38"/>
+      <c r="Y50" s="38" t="s">
+        <v>193</v>
+      </c>
     </row>
-    <row r="51" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="58" t="s">
+    <row r="51" spans="1:25" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A51" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="B51" s="58" t="s">
-        <v>208</v>
-      </c>
-      <c r="D51" s="59" t="s">
+      <c r="B51" s="39" t="s">
+        <v>182</v>
+      </c>
+      <c r="C51" s="37"/>
+      <c r="D51" s="36" t="s">
         <v>124</v>
       </c>
+      <c r="E51" s="36"/>
+      <c r="F51" s="37"/>
+      <c r="G51" s="37"/>
+      <c r="H51" s="37"/>
+      <c r="I51" s="37"/>
+      <c r="J51" s="37"/>
+      <c r="K51" s="36"/>
+      <c r="L51" s="37"/>
+      <c r="M51" s="37"/>
+      <c r="N51" s="37"/>
+      <c r="O51" s="36"/>
+      <c r="P51" s="36"/>
+      <c r="Q51" s="37"/>
+      <c r="R51" s="37"/>
+      <c r="S51" s="37"/>
+      <c r="T51" s="37"/>
+      <c r="U51" s="37"/>
+      <c r="V51" s="36"/>
+      <c r="W51" s="37"/>
+      <c r="X51" s="37"/>
+      <c r="Y51" s="38"/>
     </row>
-    <row r="52" spans="1:25" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:25" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="39" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="B52" s="39" t="s">
-        <v>121</v>
+        <v>185</v>
       </c>
       <c r="C52" s="37"/>
       <c r="D52" s="36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E52" s="36" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="F52" s="37" t="s">
         <v>125</v>
       </c>
       <c r="G52" s="37"/>
-      <c r="H52" s="37"/>
+      <c r="H52" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="I52" s="37"/>
       <c r="J52" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="K52" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="L52" s="37" t="s">
-        <v>125</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="K52" s="36"/>
+      <c r="L52" s="37"/>
       <c r="M52" s="37"/>
-      <c r="N52" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="O52" s="37"/>
-      <c r="P52" s="37"/>
-      <c r="Q52" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="N52" s="37"/>
+      <c r="O52" s="36"/>
+      <c r="P52" s="36"/>
+      <c r="Q52" s="37"/>
       <c r="R52" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="S52" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="T52" s="37" t="s">
         <v>129</v>
       </c>
-      <c r="S52" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="T52" s="37"/>
-      <c r="U52" s="37"/>
-      <c r="V52" s="37" t="s">
+      <c r="U52" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="V52" s="36" t="s">
         <v>129</v>
       </c>
       <c r="W52" s="37"/>
       <c r="X52" s="37"/>
       <c r="Y52" s="38"/>
     </row>
-    <row r="53" spans="1:25" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:25" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B53" s="39" t="s">
-        <v>201</v>
+        <v>121</v>
       </c>
       <c r="C53" s="37"/>
       <c r="D53" s="36" t="s">
@@ -12196,12 +13300,18 @@
       <c r="K53" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="L53" s="37"/>
+      <c r="L53" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="M53" s="37"/>
-      <c r="N53" s="37"/>
+      <c r="N53" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="O53" s="37"/>
       <c r="P53" s="37"/>
-      <c r="Q53" s="37"/>
+      <c r="Q53" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="R53" s="37" t="s">
         <v>129</v>
       </c>
@@ -12217,12 +13327,12 @@
       <c r="X53" s="37"/>
       <c r="Y53" s="38"/>
     </row>
-    <row r="54" spans="1:25" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:25" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B54" s="39" t="s">
-        <v>170</v>
+        <v>201</v>
       </c>
       <c r="C54" s="37"/>
       <c r="D54" s="36" t="s">
@@ -12243,18 +13353,12 @@
       <c r="K54" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="L54" s="37" t="s">
-        <v>125</v>
-      </c>
+      <c r="L54" s="37"/>
       <c r="M54" s="37"/>
-      <c r="N54" s="37" t="s">
-        <v>125</v>
-      </c>
+      <c r="N54" s="37"/>
       <c r="O54" s="37"/>
       <c r="P54" s="37"/>
-      <c r="Q54" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="Q54" s="37"/>
       <c r="R54" s="37" t="s">
         <v>129</v>
       </c>
@@ -12270,26 +13374,24 @@
       <c r="X54" s="37"/>
       <c r="Y54" s="38"/>
     </row>
-    <row r="55" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:25" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B55" s="39" t="s">
-        <v>43</v>
+        <v>170</v>
       </c>
       <c r="C55" s="37"/>
-      <c r="D55" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="E55" s="37" t="s">
+      <c r="D55" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="E55" s="36" t="s">
         <v>125</v>
       </c>
       <c r="F55" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="G55" s="37" t="s">
-        <v>18</v>
-      </c>
+      <c r="G55" s="37"/>
       <c r="H55" s="37"/>
       <c r="I55" s="37"/>
       <c r="J55" s="37" t="s">
@@ -12330,7 +13432,7 @@
         <v>42</v>
       </c>
       <c r="B56" s="39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C56" s="37"/>
       <c r="D56" s="37" t="s">
@@ -12343,14 +13445,10 @@
         <v>125</v>
       </c>
       <c r="G56" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="H56" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="I56" s="37" t="s">
-        <v>125</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="H56" s="37"/>
+      <c r="I56" s="37"/>
       <c r="J56" s="37" t="s">
         <v>16</v>
       </c>
@@ -12360,18 +13458,12 @@
       <c r="L56" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="M56" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="M56" s="37"/>
       <c r="N56" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="O56" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="P56" s="37" t="s">
-        <v>125</v>
-      </c>
+      <c r="O56" s="37"/>
+      <c r="P56" s="37"/>
       <c r="Q56" s="37" t="s">
         <v>16</v>
       </c>
@@ -12381,27 +13473,21 @@
       <c r="S56" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="T56" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="U56" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="T56" s="37"/>
+      <c r="U56" s="37"/>
       <c r="V56" s="37" t="s">
         <v>129</v>
       </c>
       <c r="W56" s="37"/>
-      <c r="X56" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="X56" s="37"/>
       <c r="Y56" s="38"/>
     </row>
-    <row r="57" spans="1:25" s="17" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B57" s="39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C57" s="37"/>
       <c r="D57" s="37" t="s">
@@ -12461,20 +13547,18 @@
       <c r="V57" s="37" t="s">
         <v>129</v>
       </c>
-      <c r="W57" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="W57" s="37"/>
       <c r="X57" s="37" t="s">
         <v>16</v>
       </c>
       <c r="Y57" s="38"/>
     </row>
-    <row r="58" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:25" s="17" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B58" s="39" t="s">
-        <v>146</v>
+        <v>45</v>
       </c>
       <c r="C58" s="37"/>
       <c r="D58" s="37" t="s">
@@ -12534,7 +13618,9 @@
       <c r="V58" s="37" t="s">
         <v>129</v>
       </c>
-      <c r="W58" s="37"/>
+      <c r="W58" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="X58" s="37" t="s">
         <v>16</v>
       </c>
@@ -12545,7 +13631,7 @@
         <v>42</v>
       </c>
       <c r="B59" s="39" t="s">
-        <v>46</v>
+        <v>146</v>
       </c>
       <c r="C59" s="37"/>
       <c r="D59" s="37" t="s">
@@ -12616,7 +13702,7 @@
         <v>42</v>
       </c>
       <c r="B60" s="39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C60" s="37"/>
       <c r="D60" s="37" t="s">
@@ -12682,12 +13768,12 @@
       </c>
       <c r="Y60" s="38"/>
     </row>
-    <row r="61" spans="1:25" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B61" s="39" t="s">
-        <v>153</v>
+        <v>47</v>
       </c>
       <c r="C61" s="37"/>
       <c r="D61" s="37" t="s">
@@ -12753,12 +13839,12 @@
       </c>
       <c r="Y61" s="38"/>
     </row>
-    <row r="62" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:25" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B62" s="39" t="s">
-        <v>48</v>
+        <v>153</v>
       </c>
       <c r="C62" s="37"/>
       <c r="D62" s="37" t="s">
@@ -12829,7 +13915,7 @@
         <v>42</v>
       </c>
       <c r="B63" s="39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C63" s="37"/>
       <c r="D63" s="37" t="s">
@@ -12865,7 +13951,9 @@
       <c r="N63" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="O63" s="37"/>
+      <c r="O63" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="P63" s="37" t="s">
         <v>125</v>
       </c>
@@ -12898,7 +13986,7 @@
         <v>42</v>
       </c>
       <c r="B64" s="39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C64" s="37"/>
       <c r="D64" s="37" t="s">
@@ -12934,9 +14022,7 @@
       <c r="N64" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="O64" s="37" t="s">
-        <v>125</v>
-      </c>
+      <c r="O64" s="37"/>
       <c r="P64" s="37" t="s">
         <v>125</v>
       </c>
@@ -12969,7 +14055,7 @@
         <v>42</v>
       </c>
       <c r="B65" s="39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C65" s="37"/>
       <c r="D65" s="37" t="s">
@@ -12981,8 +14067,12 @@
       <c r="F65" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="G65" s="37"/>
-      <c r="H65" s="37"/>
+      <c r="G65" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="H65" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="I65" s="37" t="s">
         <v>125</v>
       </c>
@@ -12995,11 +14085,15 @@
       <c r="L65" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="M65" s="37"/>
+      <c r="M65" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="N65" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="O65" s="37"/>
+      <c r="O65" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="P65" s="37" t="s">
         <v>125</v>
       </c>
@@ -13032,7 +14126,7 @@
         <v>42</v>
       </c>
       <c r="B66" s="39" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C66" s="37"/>
       <c r="D66" s="37" t="s">
@@ -13045,10 +14139,10 @@
         <v>125</v>
       </c>
       <c r="G66" s="37"/>
-      <c r="H66" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="I66" s="37"/>
+      <c r="H66" s="37"/>
+      <c r="I66" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="J66" s="37" t="s">
         <v>16</v>
       </c>
@@ -13062,10 +14156,10 @@
       <c r="N66" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="O66" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="P66" s="37"/>
+      <c r="O66" s="37"/>
+      <c r="P66" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="Q66" s="37" t="s">
         <v>16</v>
       </c>
@@ -13075,13 +14169,19 @@
       <c r="S66" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="T66" s="37"/>
-      <c r="U66" s="37"/>
+      <c r="T66" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="U66" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="V66" s="37" t="s">
         <v>129</v>
       </c>
       <c r="W66" s="37"/>
-      <c r="X66" s="37"/>
+      <c r="X66" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="Y66" s="38"/>
     </row>
     <row r="67" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -13089,7 +14189,7 @@
         <v>42</v>
       </c>
       <c r="B67" s="39" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C67" s="37"/>
       <c r="D67" s="37" t="s">
@@ -13102,7 +14202,9 @@
         <v>125</v>
       </c>
       <c r="G67" s="37"/>
-      <c r="H67" s="37"/>
+      <c r="H67" s="37" t="s">
+        <v>18</v>
+      </c>
       <c r="I67" s="37"/>
       <c r="J67" s="37" t="s">
         <v>16</v>
@@ -13117,7 +14219,9 @@
       <c r="N67" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="O67" s="37"/>
+      <c r="O67" s="37" t="s">
+        <v>18</v>
+      </c>
       <c r="P67" s="37"/>
       <c r="Q67" s="37" t="s">
         <v>16</v>
@@ -13142,7 +14246,7 @@
         <v>42</v>
       </c>
       <c r="B68" s="39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C68" s="37"/>
       <c r="D68" s="37" t="s">
@@ -13195,7 +14299,7 @@
         <v>42</v>
       </c>
       <c r="B69" s="39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C69" s="37"/>
       <c r="D69" s="37" t="s">
@@ -13243,12 +14347,12 @@
       <c r="X69" s="37"/>
       <c r="Y69" s="38"/>
     </row>
-    <row r="70" spans="1:25" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B70" s="39" t="s">
-        <v>119</v>
+        <v>55</v>
       </c>
       <c r="C70" s="37"/>
       <c r="D70" s="37" t="s">
@@ -13260,15 +14364,9 @@
       <c r="F70" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="G70" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="H70" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="I70" s="37" t="s">
-        <v>125</v>
-      </c>
+      <c r="G70" s="37"/>
+      <c r="H70" s="37"/>
+      <c r="I70" s="37"/>
       <c r="J70" s="37" t="s">
         <v>16</v>
       </c>
@@ -13278,16 +14376,12 @@
       <c r="L70" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="M70" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="M70" s="37"/>
       <c r="N70" s="37" t="s">
         <v>125</v>
       </c>
       <c r="O70" s="37"/>
-      <c r="P70" s="37" t="s">
-        <v>125</v>
-      </c>
+      <c r="P70" s="37"/>
       <c r="Q70" s="37" t="s">
         <v>16</v>
       </c>
@@ -13297,27 +14391,21 @@
       <c r="S70" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="T70" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="U70" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="T70" s="37"/>
+      <c r="U70" s="37"/>
       <c r="V70" s="37" t="s">
         <v>129</v>
       </c>
       <c r="W70" s="37"/>
-      <c r="X70" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="X70" s="37"/>
       <c r="Y70" s="38"/>
     </row>
-    <row r="71" spans="1:25" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:25" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B71" s="39" t="s">
-        <v>171</v>
+        <v>119</v>
       </c>
       <c r="C71" s="37"/>
       <c r="D71" s="37" t="s">
@@ -13381,12 +14469,12 @@
       </c>
       <c r="Y71" s="38"/>
     </row>
-    <row r="72" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:25" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B72" s="39" t="s">
-        <v>56</v>
+        <v>171</v>
       </c>
       <c r="C72" s="37"/>
       <c r="D72" s="37" t="s">
@@ -13422,9 +14510,7 @@
       <c r="N72" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="O72" s="37" t="s">
-        <v>125</v>
-      </c>
+      <c r="O72" s="37"/>
       <c r="P72" s="37" t="s">
         <v>125</v>
       </c>
@@ -13452,12 +14538,12 @@
       </c>
       <c r="Y72" s="38"/>
     </row>
-    <row r="73" spans="1:25" s="17" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B73" s="39" t="s">
-        <v>123</v>
+        <v>56</v>
       </c>
       <c r="C73" s="37"/>
       <c r="D73" s="37" t="s">
@@ -13518,7 +14604,9 @@
         <v>129</v>
       </c>
       <c r="W73" s="37"/>
-      <c r="X73" s="37"/>
+      <c r="X73" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="Y73" s="38"/>
     </row>
     <row r="74" spans="1:25" s="17" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -13526,7 +14614,7 @@
         <v>42</v>
       </c>
       <c r="B74" s="39" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="C74" s="37"/>
       <c r="D74" s="37" t="s">
@@ -13595,7 +14683,7 @@
         <v>42</v>
       </c>
       <c r="B75" s="39" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C75" s="37"/>
       <c r="D75" s="37" t="s">
@@ -13664,7 +14752,7 @@
         <v>42</v>
       </c>
       <c r="B76" s="39" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C76" s="37"/>
       <c r="D76" s="37" t="s">
@@ -13733,7 +14821,7 @@
         <v>42</v>
       </c>
       <c r="B77" s="39" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C77" s="37"/>
       <c r="D77" s="37" t="s">
@@ -13797,26 +14885,32 @@
       <c r="X77" s="37"/>
       <c r="Y77" s="38"/>
     </row>
-    <row r="78" spans="1:25" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:25" s="17" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B78" s="39" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C78" s="37"/>
-      <c r="D78" s="36" t="s">
-        <v>125</v>
-      </c>
-      <c r="E78" s="36" t="s">
+      <c r="D78" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="E78" s="37" t="s">
         <v>125</v>
       </c>
       <c r="F78" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="G78" s="37"/>
-      <c r="H78" s="37"/>
-      <c r="I78" s="37"/>
+      <c r="G78" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="H78" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="I78" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="J78" s="37" t="s">
         <v>16</v>
       </c>
@@ -13826,12 +14920,18 @@
       <c r="L78" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="M78" s="37"/>
+      <c r="M78" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="N78" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="O78" s="37"/>
-      <c r="P78" s="37"/>
+      <c r="O78" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="P78" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="Q78" s="37" t="s">
         <v>16</v>
       </c>
@@ -13841,39 +14941,39 @@
       <c r="S78" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="T78" s="37"/>
-      <c r="U78" s="37"/>
-      <c r="V78" s="37"/>
+      <c r="T78" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="U78" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="V78" s="37" t="s">
+        <v>129</v>
+      </c>
       <c r="W78" s="37"/>
       <c r="X78" s="37"/>
       <c r="Y78" s="38"/>
     </row>
-    <row r="79" spans="1:25" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:25" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B79" s="39" t="s">
-        <v>186</v>
+        <v>145</v>
       </c>
       <c r="C79" s="37"/>
-      <c r="D79" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="E79" s="37" t="s">
+      <c r="D79" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="E79" s="36" t="s">
         <v>125</v>
       </c>
       <c r="F79" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="G79" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="H79" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="I79" s="37" t="s">
-        <v>125</v>
-      </c>
+      <c r="G79" s="37"/>
+      <c r="H79" s="37"/>
+      <c r="I79" s="37"/>
       <c r="J79" s="37" t="s">
         <v>16</v>
       </c>
@@ -13883,18 +14983,12 @@
       <c r="L79" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="M79" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="M79" s="37"/>
       <c r="N79" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="O79" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="P79" s="37" t="s">
-        <v>125</v>
-      </c>
+      <c r="O79" s="37"/>
+      <c r="P79" s="37"/>
       <c r="Q79" s="37" t="s">
         <v>16</v>
       </c>
@@ -13904,25 +14998,19 @@
       <c r="S79" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="T79" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="U79" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="V79" s="37" t="s">
-        <v>129</v>
-      </c>
+      <c r="T79" s="37"/>
+      <c r="U79" s="37"/>
+      <c r="V79" s="37"/>
       <c r="W79" s="37"/>
       <c r="X79" s="37"/>
       <c r="Y79" s="38"/>
     </row>
-    <row r="80" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:25" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="39" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="B80" s="39" t="s">
-        <v>58</v>
+        <v>186</v>
       </c>
       <c r="C80" s="37"/>
       <c r="D80" s="37" t="s">
@@ -13944,7 +15032,7 @@
         <v>125</v>
       </c>
       <c r="J80" s="37" t="s">
-        <v>214</v>
+        <v>16</v>
       </c>
       <c r="K80" s="37" t="s">
         <v>125</v>
@@ -13965,13 +15053,13 @@
         <v>125</v>
       </c>
       <c r="Q80" s="37" t="s">
-        <v>214</v>
+        <v>16</v>
       </c>
       <c r="R80" s="37" t="s">
-        <v>215</v>
+        <v>129</v>
       </c>
       <c r="S80" s="37" t="s">
-        <v>214</v>
+        <v>16</v>
       </c>
       <c r="T80" s="37" t="s">
         <v>129</v>
@@ -13982,22 +15070,16 @@
       <c r="V80" s="37" t="s">
         <v>129</v>
       </c>
-      <c r="W80" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="X80" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y80" s="63" t="s">
-        <v>216</v>
-      </c>
+      <c r="W80" s="37"/>
+      <c r="X80" s="37"/>
+      <c r="Y80" s="38"/>
     </row>
     <row r="81" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A81" s="39" t="s">
         <v>57</v>
       </c>
       <c r="B81" s="39" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C81" s="37"/>
       <c r="D81" s="37" t="s">
@@ -14063,20 +15145,22 @@
       <c r="X81" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="Y81" s="64"/>
+      <c r="Y81" s="64" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="82" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A82" s="39" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B82" s="39" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C82" s="37"/>
       <c r="D82" s="37" t="s">
-        <v>124</v>
-      </c>
-      <c r="E82" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="E82" s="37" t="s">
         <v>125</v>
       </c>
       <c r="F82" s="37" t="s">
@@ -14092,10 +15176,10 @@
         <v>125</v>
       </c>
       <c r="J82" s="37" t="s">
-        <v>16</v>
+        <v>214</v>
       </c>
       <c r="K82" s="37" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="L82" s="37" t="s">
         <v>125</v>
@@ -14113,133 +15197,173 @@
         <v>125</v>
       </c>
       <c r="Q82" s="37" t="s">
-        <v>16</v>
+        <v>214</v>
       </c>
       <c r="R82" s="37" t="s">
-        <v>130</v>
+        <v>215</v>
       </c>
       <c r="S82" s="37" t="s">
-        <v>111</v>
+        <v>214</v>
       </c>
       <c r="T82" s="37" t="s">
         <v>129</v>
       </c>
       <c r="U82" s="37" t="s">
-        <v>111</v>
+        <v>16</v>
       </c>
       <c r="V82" s="37" t="s">
         <v>129</v>
       </c>
       <c r="W82" s="37" t="s">
-        <v>111</v>
+        <v>16</v>
       </c>
       <c r="X82" s="37" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y82" s="38"/>
+        <v>16</v>
+      </c>
+      <c r="Y82" s="65"/>
     </row>
-    <row r="83" spans="1:25" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A83" s="42" t="s">
-        <v>61</v>
-      </c>
-      <c r="B83" s="42" t="s">
-        <v>62</v>
-      </c>
-      <c r="C83" s="43"/>
+    <row r="83" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A83" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="B83" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="C83" s="37"/>
       <c r="D83" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="E83" s="43"/>
-      <c r="F83" s="43"/>
-      <c r="G83" s="43"/>
-      <c r="H83" s="43"/>
-      <c r="I83" s="43"/>
-      <c r="J83" s="43"/>
-      <c r="K83" s="43"/>
-      <c r="L83" s="43"/>
-      <c r="M83" s="43"/>
-      <c r="N83" s="43"/>
-      <c r="O83" s="43"/>
-      <c r="P83" s="43"/>
-      <c r="Q83" s="43"/>
-      <c r="R83" s="43"/>
-      <c r="S83" s="43"/>
-      <c r="T83" s="43"/>
-      <c r="U83" s="43"/>
-      <c r="V83" s="43"/>
-      <c r="W83" s="43"/>
-      <c r="X83" s="43"/>
-      <c r="Y83" s="44" t="s">
-        <v>63</v>
-      </c>
+      <c r="E83" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="F83" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="G83" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="H83" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="I83" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="J83" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="K83" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="L83" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="M83" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="N83" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="O83" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="P83" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q83" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="R83" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="S83" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="T83" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="U83" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="V83" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="W83" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="X83" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="Y83" s="38"/>
     </row>
-    <row r="84" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A84" s="35" t="s">
+    <row r="84" spans="1:25" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A84" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="B84" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="C84" s="36"/>
+      <c r="B84" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="C84" s="43"/>
       <c r="D84" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="E84" s="36"/>
-      <c r="F84" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="G84" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="H84" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="I84" s="36"/>
-      <c r="J84" s="37"/>
-      <c r="K84" s="36"/>
-      <c r="L84" s="36"/>
-      <c r="M84" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="N84" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="O84" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="P84" s="36"/>
-      <c r="Q84" s="37"/>
-      <c r="R84" s="36"/>
-      <c r="S84" s="36"/>
-      <c r="T84" s="36"/>
-      <c r="U84" s="36"/>
-      <c r="V84" s="36"/>
-      <c r="W84" s="36"/>
-      <c r="X84" s="36"/>
-      <c r="Y84" s="30"/>
+      <c r="E84" s="43"/>
+      <c r="F84" s="43"/>
+      <c r="G84" s="43"/>
+      <c r="H84" s="43"/>
+      <c r="I84" s="43"/>
+      <c r="J84" s="43"/>
+      <c r="K84" s="43"/>
+      <c r="L84" s="43"/>
+      <c r="M84" s="43"/>
+      <c r="N84" s="43"/>
+      <c r="O84" s="43"/>
+      <c r="P84" s="43"/>
+      <c r="Q84" s="43"/>
+      <c r="R84" s="43"/>
+      <c r="S84" s="43"/>
+      <c r="T84" s="43"/>
+      <c r="U84" s="43"/>
+      <c r="V84" s="43"/>
+      <c r="W84" s="43"/>
+      <c r="X84" s="43"/>
+      <c r="Y84" s="44" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="85" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A85" s="35" t="s">
         <v>61</v>
       </c>
       <c r="B85" s="35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C85" s="36"/>
       <c r="D85" s="37" t="s">
         <v>124</v>
       </c>
       <c r="E85" s="36"/>
-      <c r="F85" s="36"/>
-      <c r="G85" s="36"/>
-      <c r="H85" s="36"/>
+      <c r="F85" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="G85" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="H85" s="36" t="s">
+        <v>18</v>
+      </c>
       <c r="I85" s="36"/>
       <c r="J85" s="37"/>
       <c r="K85" s="36"/>
       <c r="L85" s="36"/>
-      <c r="M85" s="36"/>
-      <c r="N85" s="36"/>
-      <c r="O85" s="36"/>
+      <c r="M85" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="N85" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="O85" s="36" t="s">
+        <v>18</v>
+      </c>
       <c r="P85" s="36"/>
       <c r="Q85" s="37"/>
       <c r="R85" s="36"/>
@@ -14256,7 +15380,7 @@
         <v>61</v>
       </c>
       <c r="B86" s="35" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C86" s="36"/>
       <c r="D86" s="37" t="s">
@@ -14289,7 +15413,7 @@
         <v>61</v>
       </c>
       <c r="B87" s="35" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C87" s="36"/>
       <c r="D87" s="37" t="s">
@@ -14317,12 +15441,12 @@
       <c r="X87" s="36"/>
       <c r="Y87" s="30"/>
     </row>
-    <row r="88" spans="1:25" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A88" s="35" t="s">
         <v>61</v>
       </c>
       <c r="B88" s="35" t="s">
-        <v>164</v>
+        <v>67</v>
       </c>
       <c r="C88" s="36"/>
       <c r="D88" s="37" t="s">
@@ -14350,12 +15474,12 @@
       <c r="X88" s="36"/>
       <c r="Y88" s="30"/>
     </row>
-    <row r="89" spans="1:25" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:25" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A89" s="35" t="s">
         <v>61</v>
       </c>
       <c r="B89" s="35" t="s">
-        <v>32</v>
+        <v>164</v>
       </c>
       <c r="C89" s="36"/>
       <c r="D89" s="37" t="s">
@@ -14383,12 +15507,12 @@
       <c r="X89" s="36"/>
       <c r="Y89" s="30"/>
     </row>
-    <row r="90" spans="1:25" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:25" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A90" s="35" t="s">
         <v>61</v>
       </c>
       <c r="B90" s="35" t="s">
-        <v>179</v>
+        <v>32</v>
       </c>
       <c r="C90" s="36"/>
       <c r="D90" s="37" t="s">
@@ -14416,78 +15540,78 @@
       <c r="X90" s="36"/>
       <c r="Y90" s="30"/>
     </row>
-    <row r="91" spans="1:25" s="57" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:25" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A91" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="B91" s="60" t="s">
-        <v>211</v>
-      </c>
-      <c r="C91" s="61"/>
-      <c r="D91" s="61" t="s">
+      <c r="B91" s="35" t="s">
+        <v>179</v>
+      </c>
+      <c r="C91" s="36"/>
+      <c r="D91" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="E91" s="61"/>
-      <c r="F91" s="61"/>
-      <c r="G91" s="61"/>
-      <c r="H91" s="61"/>
-      <c r="I91" s="61"/>
-      <c r="J91" s="61"/>
-      <c r="K91" s="61"/>
-      <c r="L91" s="61"/>
-      <c r="M91" s="61"/>
-      <c r="N91" s="61"/>
-      <c r="O91" s="61"/>
-      <c r="P91" s="61"/>
-      <c r="Q91" s="61"/>
-      <c r="R91" s="61"/>
-      <c r="S91" s="61"/>
-      <c r="T91" s="61"/>
-      <c r="U91" s="61"/>
-      <c r="V91" s="61"/>
-      <c r="W91" s="61"/>
-      <c r="X91" s="61"/>
-      <c r="Y91" s="55"/>
+      <c r="E91" s="36"/>
+      <c r="F91" s="36"/>
+      <c r="G91" s="36"/>
+      <c r="H91" s="36"/>
+      <c r="I91" s="36"/>
+      <c r="J91" s="37"/>
+      <c r="K91" s="36"/>
+      <c r="L91" s="36"/>
+      <c r="M91" s="36"/>
+      <c r="N91" s="36"/>
+      <c r="O91" s="36"/>
+      <c r="P91" s="36"/>
+      <c r="Q91" s="37"/>
+      <c r="R91" s="36"/>
+      <c r="S91" s="36"/>
+      <c r="T91" s="36"/>
+      <c r="U91" s="36"/>
+      <c r="V91" s="36"/>
+      <c r="W91" s="36"/>
+      <c r="X91" s="36"/>
+      <c r="Y91" s="30"/>
     </row>
-    <row r="92" spans="1:25" s="52" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:25" s="57" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A92" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="B92" s="35" t="s">
-        <v>204</v>
-      </c>
-      <c r="C92" s="36"/>
-      <c r="D92" s="37" t="s">
+      <c r="B92" s="60" t="s">
+        <v>211</v>
+      </c>
+      <c r="C92" s="61"/>
+      <c r="D92" s="61" t="s">
         <v>124</v>
       </c>
-      <c r="E92" s="36"/>
-      <c r="F92" s="36"/>
-      <c r="G92" s="36"/>
-      <c r="H92" s="36"/>
-      <c r="I92" s="36"/>
-      <c r="J92" s="37"/>
-      <c r="K92" s="36"/>
-      <c r="L92" s="36"/>
-      <c r="M92" s="36"/>
-      <c r="N92" s="36"/>
-      <c r="O92" s="36"/>
-      <c r="P92" s="36"/>
-      <c r="Q92" s="37"/>
-      <c r="R92" s="36"/>
-      <c r="S92" s="36"/>
-      <c r="T92" s="36"/>
-      <c r="U92" s="36"/>
-      <c r="V92" s="36"/>
-      <c r="W92" s="36"/>
-      <c r="X92" s="36"/>
-      <c r="Y92" s="51"/>
+      <c r="E92" s="61"/>
+      <c r="F92" s="61"/>
+      <c r="G92" s="61"/>
+      <c r="H92" s="61"/>
+      <c r="I92" s="61"/>
+      <c r="J92" s="61"/>
+      <c r="K92" s="61"/>
+      <c r="L92" s="61"/>
+      <c r="M92" s="61"/>
+      <c r="N92" s="61"/>
+      <c r="O92" s="61"/>
+      <c r="P92" s="61"/>
+      <c r="Q92" s="61"/>
+      <c r="R92" s="61"/>
+      <c r="S92" s="61"/>
+      <c r="T92" s="61"/>
+      <c r="U92" s="61"/>
+      <c r="V92" s="61"/>
+      <c r="W92" s="61"/>
+      <c r="X92" s="61"/>
+      <c r="Y92" s="55"/>
     </row>
-    <row r="93" spans="1:25" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:25" s="52" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A93" s="35" t="s">
         <v>61</v>
       </c>
       <c r="B93" s="35" t="s">
-        <v>122</v>
+        <v>204</v>
       </c>
       <c r="C93" s="36"/>
       <c r="D93" s="37" t="s">
@@ -14513,101 +15637,152 @@
       <c r="V93" s="36"/>
       <c r="W93" s="36"/>
       <c r="X93" s="36"/>
-      <c r="Y93" s="30"/>
+      <c r="Y93" s="51"/>
     </row>
-    <row r="94" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:25" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A94" s="35" t="s">
-        <v>107</v>
+        <v>61</v>
       </c>
       <c r="B94" s="35" t="s">
-        <v>108</v>
-      </c>
-      <c r="C94" s="45"/>
+        <v>122</v>
+      </c>
+      <c r="C94" s="36"/>
       <c r="D94" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="E94" s="45"/>
-      <c r="F94" s="45"/>
-      <c r="G94" s="45"/>
-      <c r="H94" s="45"/>
-      <c r="I94" s="45"/>
-      <c r="J94" s="46"/>
-      <c r="K94" s="45"/>
-      <c r="L94" s="45"/>
-      <c r="M94" s="45"/>
-      <c r="N94" s="45"/>
-      <c r="O94" s="45"/>
-      <c r="P94" s="45"/>
-      <c r="Q94" s="46"/>
-      <c r="R94" s="45"/>
-      <c r="S94" s="45"/>
-      <c r="T94" s="45"/>
-      <c r="U94" s="45"/>
-      <c r="V94" s="45"/>
-      <c r="W94" s="45"/>
-      <c r="X94" s="45"/>
+      <c r="E94" s="36"/>
+      <c r="F94" s="36"/>
+      <c r="G94" s="36"/>
+      <c r="H94" s="36"/>
+      <c r="I94" s="36"/>
+      <c r="J94" s="37"/>
+      <c r="K94" s="36"/>
+      <c r="L94" s="36"/>
+      <c r="M94" s="36"/>
+      <c r="N94" s="36"/>
+      <c r="O94" s="36"/>
+      <c r="P94" s="36"/>
+      <c r="Q94" s="37"/>
+      <c r="R94" s="36"/>
+      <c r="S94" s="36"/>
+      <c r="T94" s="36"/>
+      <c r="U94" s="36"/>
+      <c r="V94" s="36"/>
+      <c r="W94" s="36"/>
+      <c r="X94" s="36"/>
       <c r="Y94" s="30"/>
     </row>
     <row r="95" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A95" s="35" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="B95" s="35" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C95" s="45"/>
       <c r="D95" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="E95" s="45"/>
+      <c r="F95" s="45"/>
+      <c r="G95" s="45"/>
+      <c r="H95" s="45"/>
+      <c r="I95" s="45"/>
+      <c r="J95" s="46"/>
+      <c r="K95" s="45"/>
+      <c r="L95" s="45"/>
+      <c r="M95" s="45"/>
+      <c r="N95" s="45"/>
+      <c r="O95" s="45"/>
+      <c r="P95" s="45"/>
+      <c r="Q95" s="46"/>
+      <c r="R95" s="45"/>
+      <c r="S95" s="45"/>
+      <c r="T95" s="45"/>
+      <c r="U95" s="45"/>
+      <c r="V95" s="45"/>
+      <c r="W95" s="45"/>
+      <c r="X95" s="45"/>
+      <c r="Y95" s="30"/>
+    </row>
+    <row r="96" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A96" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="B96" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="C96" s="45"/>
+      <c r="D96" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="E95" s="47" t="s">
+      <c r="E96" s="47" t="s">
         <v>126</v>
       </c>
-      <c r="F95" s="47"/>
-      <c r="G95" s="47" t="s">
+      <c r="F96" s="47"/>
+      <c r="G96" s="47" t="s">
         <v>126</v>
       </c>
-      <c r="H95" s="47"/>
-      <c r="I95" s="47"/>
-      <c r="J95" s="48" t="s">
+      <c r="H96" s="47"/>
+      <c r="I96" s="47"/>
+      <c r="J96" s="48" t="s">
         <v>158</v>
       </c>
-      <c r="K95" s="47" t="s">
+      <c r="K96" s="47" t="s">
         <v>126</v>
       </c>
-      <c r="L95" s="47" t="s">
+      <c r="L96" s="47" t="s">
         <v>126</v>
       </c>
-      <c r="M95" s="47" t="s">
+      <c r="M96" s="47" t="s">
         <v>126</v>
       </c>
-      <c r="N95" s="47" t="s">
+      <c r="N96" s="47" t="s">
         <v>126</v>
       </c>
-      <c r="O95" s="47"/>
-      <c r="P95" s="47"/>
-      <c r="Q95" s="48" t="s">
+      <c r="O96" s="47"/>
+      <c r="P96" s="47"/>
+      <c r="Q96" s="48" t="s">
         <v>158</v>
       </c>
-      <c r="R95" s="49" t="s">
+      <c r="R96" s="49" t="s">
         <v>163</v>
       </c>
-      <c r="S95" s="48" t="s">
+      <c r="S96" s="48" t="s">
         <v>158</v>
       </c>
-      <c r="T95" s="47"/>
-      <c r="U95" s="47" t="s">
+      <c r="T96" s="47"/>
+      <c r="U96" s="47" t="s">
         <v>158</v>
       </c>
-      <c r="V95" s="47"/>
-      <c r="W95" s="47"/>
-      <c r="X95" s="47"/>
-      <c r="Y95" s="30"/>
+      <c r="V96" s="47"/>
+      <c r="W96" s="47"/>
+      <c r="X96" s="47"/>
+      <c r="Y96" s="30"/>
     </row>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C41" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="D46" sqref="D46"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C29" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="E46" sqref="E46"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
+      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
+      <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="C31" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -14617,27 +15792,9 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C31" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
-      <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
-      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
   </customSheetViews>
   <mergeCells count="6">
-    <mergeCell ref="Y80:Y81"/>
+    <mergeCell ref="Y81:Y82"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="K5:O5"/>
     <mergeCell ref="R5:X5"/>
@@ -14993,8 +16150,13 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}">
-      <selection activeCell="A22" sqref="A22"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
+      <selection activeCell="B17" sqref="B17"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
+      <selection activeCell="C7" sqref="C7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -15003,13 +16165,8 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
-      <selection activeCell="C7" sqref="C7"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
-      <selection activeCell="B17" sqref="B17"/>
+    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}">
+      <selection activeCell="A22" sqref="A22"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>

</xml_diff>

<commit_message>
Lisää ELY laadunvalvojalle lukuoikeudet
Toteumat / Kokonaishintaiset työt
Toteumat / Yksikköhintaiset työt
Toteumat / Muutos- ja-lisätyöt
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joonasmi/projects/harja/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikkoro/Documents/Sources/harja/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="28700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -23,11 +23,11 @@
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="2560" windowHeight="1254" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="1280" windowHeight="1262" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Mikko Rönkkömäki - Personal View" guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" mergeInterval="0" personalView="1" windowWidth="2560" windowHeight="1071" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office -käyttäjä - Oma näkymä" guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="1149" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
-    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Microsoft Office -käyttäjä - Oma näkymä" guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="1149" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Mikko Rönkkömäki - Personal View" guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" mergeInterval="0" personalView="1" windowWidth="2560" windowHeight="1071" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1449" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1452" uniqueCount="226">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -1225,6 +1225,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1245,18 +1257,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="185">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1456,7 +1456,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{0602C519-A1BE-AE48-B457-EFC7185CD0F1}" diskRevisions="1" revisionId="757" version="41">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{AB41DA79-7B74-0C42-BA09-18D919672E74}" diskRevisions="1" revisionId="761" version="42">
   <header guid="{1E352813-0B26-DB4E-84BE-460845B77133}" dateTime="2017-06-20T12:32:37" maxSheetId="3" userName="Microsoft Office -käyttäjä" r:id="rId60" minRId="448" maxRId="464">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1703,6 +1703,12 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{AB41DA79-7B74-0C42-BA09-18D919672E74}" dateTime="2017-12-12T08:15:52" maxSheetId="3" userName="Microsoft Office User" r:id="rId101" minRId="758" maxRId="760">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -9511,6 +9517,38 @@
     <nc r="D45" t="inlineStr">
       <is>
         <t>R*,W*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="delete"/>
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_7A9649F2_657F_9445_B6E6_FE94C6A09957_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Oikeudet!$A$5:$Y$96</formula>
+    <oldFormula>Oikeudet!$A$5:$Y$96</oldFormula>
+  </rdn>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog39.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="758" sId="1">
+    <nc r="M13" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="759" sId="1">
+    <nc r="M14" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="760" sId="1">
+    <nc r="M15" t="inlineStr">
+      <is>
+        <t>R</t>
       </is>
     </nc>
   </rcc>
@@ -10509,10 +10547,10 @@
   <dimension ref="A1:Y96"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C18" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="L13" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E46" sqref="E46"/>
+      <selection pane="bottomRight" activeCell="B13" sqref="B13:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -10549,40 +10587,40 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="68" t="s">
+      <c r="C1" s="72" t="s">
         <v>149</v>
       </c>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
-      <c r="L1" s="69"/>
-      <c r="M1" s="69"/>
-      <c r="N1" s="69"/>
-      <c r="O1" s="69"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="73"/>
+      <c r="O1" s="73"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="70" t="s">
+      <c r="C2" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="75"/>
+      <c r="N2" s="75"/>
+      <c r="O2" s="75"/>
     </row>
     <row r="3" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
@@ -10605,34 +10643,34 @@
     <row r="5" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="30"/>
       <c r="B5" s="30"/>
-      <c r="C5" s="66" t="s">
+      <c r="C5" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="67"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="71"/>
       <c r="I5" s="30"/>
       <c r="J5" s="30"/>
-      <c r="K5" s="66" t="s">
+      <c r="K5" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="L5" s="67"/>
-      <c r="M5" s="67"/>
-      <c r="N5" s="67"/>
-      <c r="O5" s="67"/>
+      <c r="L5" s="71"/>
+      <c r="M5" s="71"/>
+      <c r="N5" s="71"/>
+      <c r="O5" s="71"/>
       <c r="P5" s="30"/>
       <c r="Q5" s="30"/>
-      <c r="R5" s="66" t="s">
+      <c r="R5" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="S5" s="67"/>
-      <c r="T5" s="67"/>
-      <c r="U5" s="67"/>
-      <c r="V5" s="67"/>
-      <c r="W5" s="67"/>
-      <c r="X5" s="67"/>
+      <c r="S5" s="71"/>
+      <c r="T5" s="71"/>
+      <c r="U5" s="71"/>
+      <c r="V5" s="71"/>
+      <c r="W5" s="71"/>
+      <c r="X5" s="71"/>
       <c r="Y5" s="31" t="s">
         <v>13</v>
       </c>
@@ -11111,7 +11149,9 @@
       <c r="L13" s="36" t="s">
         <v>125</v>
       </c>
-      <c r="M13" s="36"/>
+      <c r="M13" s="36" t="s">
+        <v>16</v>
+      </c>
       <c r="N13" s="37" t="s">
         <v>125</v>
       </c>
@@ -11166,7 +11206,9 @@
       <c r="L14" s="36" t="s">
         <v>125</v>
       </c>
-      <c r="M14" s="36"/>
+      <c r="M14" s="36" t="s">
+        <v>16</v>
+      </c>
       <c r="N14" s="37" t="s">
         <v>125</v>
       </c>
@@ -11221,7 +11263,9 @@
       <c r="L15" s="36" t="s">
         <v>125</v>
       </c>
-      <c r="M15" s="36"/>
+      <c r="M15" s="36" t="s">
+        <v>16</v>
+      </c>
       <c r="N15" s="37" t="s">
         <v>125</v>
       </c>
@@ -12998,33 +13042,33 @@
       <c r="A45" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="B45" s="72" t="s">
+      <c r="B45" s="64" t="s">
         <v>225</v>
       </c>
-      <c r="C45" s="73"/>
-      <c r="D45" s="74" t="s">
+      <c r="C45" s="65"/>
+      <c r="D45" s="66" t="s">
         <v>124</v>
       </c>
-      <c r="E45" s="74"/>
-      <c r="F45" s="73"/>
-      <c r="G45" s="73"/>
-      <c r="H45" s="73"/>
-      <c r="I45" s="73"/>
-      <c r="J45" s="74"/>
-      <c r="K45" s="74"/>
-      <c r="L45" s="74"/>
-      <c r="M45" s="73"/>
-      <c r="N45" s="73"/>
+      <c r="E45" s="66"/>
+      <c r="F45" s="65"/>
+      <c r="G45" s="65"/>
+      <c r="H45" s="65"/>
+      <c r="I45" s="65"/>
+      <c r="J45" s="66"/>
+      <c r="K45" s="66"/>
+      <c r="L45" s="66"/>
+      <c r="M45" s="65"/>
+      <c r="N45" s="65"/>
       <c r="O45" s="61"/>
       <c r="P45" s="61"/>
-      <c r="Q45" s="73"/>
-      <c r="R45" s="74"/>
-      <c r="S45" s="75"/>
-      <c r="T45" s="73"/>
-      <c r="U45" s="73"/>
+      <c r="Q45" s="65"/>
+      <c r="R45" s="66"/>
+      <c r="S45" s="67"/>
+      <c r="T45" s="65"/>
+      <c r="U45" s="65"/>
       <c r="V45" s="61"/>
-      <c r="W45" s="73"/>
-      <c r="X45" s="73"/>
+      <c r="W45" s="65"/>
+      <c r="X45" s="65"/>
       <c r="Y45" s="55"/>
     </row>
     <row r="46" spans="1:25" s="57" customFormat="1" ht="13" x14ac:dyDescent="0.15">
@@ -15145,7 +15189,7 @@
       <c r="X81" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="Y81" s="64" t="s">
+      <c r="Y81" s="68" t="s">
         <v>216</v>
       </c>
     </row>
@@ -15220,7 +15264,7 @@
       <c r="X82" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="Y82" s="65"/>
+      <c r="Y82" s="69"/>
     </row>
     <row r="83" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83" s="39" t="s">
@@ -15763,14 +15807,20 @@
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C29" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="E46" sqref="E46"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="L13" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="M15" sqref="M15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
-      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
+    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="C48" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="D72" sqref="D72:X72"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="C31" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -15780,15 +15830,9 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C31" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C48" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="D72" sqref="D72:X72"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
+      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -16150,8 +16194,13 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
-      <selection activeCell="B17" sqref="B17"/>
+    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}">
+      <selection activeCell="A22" sqref="A22"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}">
+      <selection activeCell="G36" sqref="G36"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -16160,13 +16209,8 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}">
-      <selection activeCell="G36" sqref="G36"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}">
-      <selection activeCell="A22" sqref="A22"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
+      <selection activeCell="B17" sqref="B17"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>

</xml_diff>

<commit_message>
Lisää oma oikeustarkistus kohdehaulle
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -1,33 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikkoro/Documents/Sources/harja/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarihan/Jari/Tyo/Solita/Projektit/Harja/harja/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="20920" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="27240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
     <sheet name="Roolit" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$97</definedName>
-    <definedName name="Z_1DD617EE_F308_3E45_A8EF_4713F47FA0DD_.wvu.FilterData" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$97</definedName>
-    <definedName name="Z_7A9649F2_657F_9445_B6E6_FE94C6A09957_.wvu.FilterData" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$97</definedName>
-    <definedName name="Z_F86DF6F3_8AE5_3A44_B2D2_D623E01AE54F_.wvu.FilterData" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$97</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$98</definedName>
+    <definedName name="Z_1DD617EE_F308_3E45_A8EF_4713F47FA0DD_.wvu.FilterData" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$98</definedName>
+    <definedName name="Z_7A9649F2_657F_9445_B6E6_FE94C6A09957_.wvu.FilterData" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$98</definedName>
+    <definedName name="Z_F86DF6F3_8AE5_3A44_B2D2_D623E01AE54F_.wvu.FilterData" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$98</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" windowWidth="1280" windowHeight="873" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2560" windowHeight="1189" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Mikko Rönkkömäki - Personal View" guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" mergeInterval="0" personalView="1" windowWidth="2560" windowHeight="1071" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office -käyttäjä - Oma näkymä" guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="1149" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
-    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Microsoft Office -käyttäjä - Oma näkymä" guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="1149" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Mikko Rönkkömäki - Personal View" guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" mergeInterval="0" personalView="1" windowWidth="2560" windowHeight="1071" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1455" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1459" uniqueCount="229">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -755,6 +755,12 @@
   </si>
   <si>
     <t>Järjestelmäasetukset</t>
+  </si>
+  <si>
+    <t>Kanavat / Kanavakohteet</t>
+  </si>
+  <si>
+    <t>Tällä oikeudella voi hakea urakan kanavakohteet (tarvitaan mm. lomakkeissa)</t>
   </si>
 </sst>
 </file>
@@ -916,7 +922,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="185">
+  <cellStyleXfs count="189">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1102,8 +1108,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -1244,6 +1254,10 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1265,7 +1279,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="185">
+  <cellStyles count="189">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1358,6 +1372,8 @@
     <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1450,6 +1466,8 @@
     <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1463,7 +1481,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{1279139B-9DED-9E4B-A706-20C773B5D568}" diskRevisions="1" revisionId="766" version="43">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{CBA5289A-5B9B-984A-BEA7-1AD0AA9EDC22}" diskRevisions="1" revisionId="772" version="44">
   <header guid="{1E352813-0B26-DB4E-84BE-460845B77133}" dateTime="2017-06-20T12:32:37" maxSheetId="3" userName="Microsoft Office -käyttäjä" r:id="rId60" minRId="448" maxRId="464">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1722,6 +1740,12 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{CBA5289A-5B9B-984A-BEA7-1AD0AA9EDC22}" dateTime="2017-12-21T10:21:09" maxSheetId="3" userName="Microsoft Office User" r:id="rId103" minRId="767" maxRId="771">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -9717,6 +9741,132 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog41.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="767" sId="1" ref="A46:XFD46" action="insertRow"/>
+  <rcc rId="768" sId="1" odxf="1" dxf="1">
+    <nc r="A46" t="inlineStr">
+      <is>
+        <t>Urakat</t>
+      </is>
+    </nc>
+    <odxf/>
+    <ndxf/>
+  </rcc>
+  <rfmt sheetId="1" sqref="B46" start="0" length="0">
+    <dxf/>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C46" start="0" length="0">
+    <dxf/>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D46" start="0" length="0">
+    <dxf>
+      <alignment wrapText="0" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="E46" start="0" length="0">
+    <dxf>
+      <alignment wrapText="0" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="F46" start="0" length="0">
+    <dxf/>
+  </rfmt>
+  <rfmt sheetId="1" sqref="G46" start="0" length="0">
+    <dxf/>
+  </rfmt>
+  <rfmt sheetId="1" sqref="H46" start="0" length="0">
+    <dxf/>
+  </rfmt>
+  <rfmt sheetId="1" sqref="I46" start="0" length="0">
+    <dxf/>
+  </rfmt>
+  <rfmt sheetId="1" sqref="J46" start="0" length="0">
+    <dxf>
+      <alignment wrapText="0" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="K46" start="0" length="0">
+    <dxf>
+      <alignment wrapText="0" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="L46" start="0" length="0">
+    <dxf>
+      <alignment wrapText="0" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="M46" start="0" length="0">
+    <dxf/>
+  </rfmt>
+  <rfmt sheetId="1" sqref="N46" start="0" length="0">
+    <dxf/>
+  </rfmt>
+  <rfmt sheetId="1" sqref="Q46" start="0" length="0">
+    <dxf/>
+  </rfmt>
+  <rfmt sheetId="1" sqref="R46" start="0" length="0">
+    <dxf>
+      <alignment wrapText="0" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="S46" start="0" length="0">
+    <dxf>
+      <alignment wrapText="0" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="T46" start="0" length="0">
+    <dxf/>
+  </rfmt>
+  <rfmt sheetId="1" sqref="U46" start="0" length="0">
+    <dxf/>
+  </rfmt>
+  <rfmt sheetId="1" sqref="W46" start="0" length="0">
+    <dxf/>
+  </rfmt>
+  <rfmt sheetId="1" sqref="X46" start="0" length="0">
+    <dxf/>
+  </rfmt>
+  <rfmt sheetId="1" sqref="Y46" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="769" sId="1">
+    <nc r="B46" t="inlineStr">
+      <is>
+        <t>Kanavat / Kanavakohteet</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="770" sId="1">
+    <nc r="D46" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="771" sId="1">
+    <nc r="Y46" t="inlineStr">
+      <is>
+        <t>Tällä oikeudella voi hakea urakan kanavakohteet (tarvitaan mm. lomakkeissa)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="delete"/>
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_7A9649F2_657F_9445_B6E6_FE94C6A09957_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Oikeudet!$A$5:$Y$98</formula>
+    <oldFormula>Oikeudet!$A$5:$Y$98</oldFormula>
+  </rdn>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog5.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="514" sId="1">
@@ -10258,13 +10408,14 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="5">
+<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="6">
   <userInfo guid="{1E352813-0B26-DB4E-84BE-460845B77133}" name="Microsoft Office -käyttäjä" id="-785751636" dateTime="2017-06-20T12:33:00"/>
   <userInfo guid="{1AB7A282-42ED-4740-A9CB-95FF229EC1A0}" name="Mikko Rönkkömäki" id="-727946492" dateTime="2017-06-22T10:45:48"/>
   <userInfo guid="{4A189F6B-10A0-794F-AE26-98E1292E0A90}" name="Microsoft Office User" id="-296987972" dateTime="2017-09-21T08:10:21"/>
   <userInfo guid="{72187562-2E05-9542-A596-E87B0EC7A6D4}" name="Microsoft Office User" id="-296946728" dateTime="2017-11-06T12:39:34"/>
   <userInfo guid="{7DE0565B-D0D5-DF45-A2A1-25AA2C726E19}" name="Microsoft Office User" id="-296947028" dateTime="2017-11-20T14:54:25"/>
+  <userInfo guid="{CBA5289A-5B9B-984A-BEA7-1AD0AA9EDC22}" name="Microsoft Office User" id="-296966720" dateTime="2017-12-21T10:14:22"/>
 </users>
 </file>
 
@@ -10590,13 +10741,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y97"/>
+  <dimension ref="A1:Y98"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C77" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C34" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B95" sqref="B95"/>
+      <selection pane="bottomRight" activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -10633,40 +10784,40 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="74" t="s">
+      <c r="C1" s="76" t="s">
         <v>149</v>
       </c>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
-      <c r="K1" s="75"/>
-      <c r="L1" s="75"/>
-      <c r="M1" s="75"/>
-      <c r="N1" s="75"/>
-      <c r="O1" s="75"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="76" t="s">
+      <c r="C2" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
-      <c r="J2" s="77"/>
-      <c r="K2" s="77"/>
-      <c r="L2" s="77"/>
-      <c r="M2" s="77"/>
-      <c r="N2" s="77"/>
-      <c r="O2" s="77"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="79"/>
+      <c r="L2" s="79"/>
+      <c r="M2" s="79"/>
+      <c r="N2" s="79"/>
+      <c r="O2" s="79"/>
     </row>
     <row r="3" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
@@ -10689,34 +10840,34 @@
     <row r="5" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="30"/>
       <c r="B5" s="30"/>
-      <c r="C5" s="72" t="s">
+      <c r="C5" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="73"/>
-      <c r="H5" s="73"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="75"/>
       <c r="I5" s="30"/>
       <c r="J5" s="30"/>
-      <c r="K5" s="72" t="s">
+      <c r="K5" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="L5" s="73"/>
-      <c r="M5" s="73"/>
-      <c r="N5" s="73"/>
-      <c r="O5" s="73"/>
+      <c r="L5" s="75"/>
+      <c r="M5" s="75"/>
+      <c r="N5" s="75"/>
+      <c r="O5" s="75"/>
       <c r="P5" s="30"/>
       <c r="Q5" s="30"/>
-      <c r="R5" s="72" t="s">
+      <c r="R5" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="S5" s="73"/>
-      <c r="T5" s="73"/>
-      <c r="U5" s="73"/>
-      <c r="V5" s="73"/>
-      <c r="W5" s="73"/>
-      <c r="X5" s="73"/>
+      <c r="S5" s="75"/>
+      <c r="T5" s="75"/>
+      <c r="U5" s="75"/>
+      <c r="V5" s="75"/>
+      <c r="W5" s="75"/>
+      <c r="X5" s="75"/>
       <c r="Y5" s="31" t="s">
         <v>13</v>
       </c>
@@ -13117,16 +13268,16 @@
       <c r="X45" s="65"/>
       <c r="Y45" s="55"/>
     </row>
-    <row r="46" spans="1:25" s="57" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:25" s="71" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A46" s="35" t="s">
         <v>14</v>
       </c>
       <c r="B46" s="60" t="s">
-        <v>212</v>
+        <v>227</v>
       </c>
       <c r="C46" s="61"/>
       <c r="D46" s="61" t="s">
-        <v>224</v>
+        <v>125</v>
       </c>
       <c r="E46" s="61"/>
       <c r="F46" s="61"/>
@@ -13148,196 +13299,190 @@
       <c r="V46" s="61"/>
       <c r="W46" s="61"/>
       <c r="X46" s="61"/>
-      <c r="Y46" s="56"/>
+      <c r="Y46" s="70" t="s">
+        <v>228</v>
+      </c>
     </row>
-    <row r="47" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="58" t="s">
+    <row r="47" spans="1:25" s="57" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A47" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B47" s="58" t="s">
+      <c r="B47" s="60" t="s">
+        <v>212</v>
+      </c>
+      <c r="C47" s="61"/>
+      <c r="D47" s="61" t="s">
+        <v>224</v>
+      </c>
+      <c r="E47" s="61"/>
+      <c r="F47" s="61"/>
+      <c r="G47" s="61"/>
+      <c r="H47" s="61"/>
+      <c r="I47" s="61"/>
+      <c r="J47" s="61"/>
+      <c r="K47" s="61"/>
+      <c r="L47" s="61"/>
+      <c r="M47" s="61"/>
+      <c r="N47" s="61"/>
+      <c r="O47" s="61"/>
+      <c r="P47" s="61"/>
+      <c r="Q47" s="61"/>
+      <c r="R47" s="61"/>
+      <c r="S47" s="61"/>
+      <c r="T47" s="61"/>
+      <c r="U47" s="61"/>
+      <c r="V47" s="61"/>
+      <c r="W47" s="61"/>
+      <c r="X47" s="61"/>
+      <c r="Y47" s="56"/>
+    </row>
+    <row r="48" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="58" t="s">
+        <v>14</v>
+      </c>
+      <c r="B48" s="58" t="s">
         <v>208</v>
       </c>
-      <c r="D47" s="59" t="s">
+      <c r="D48" s="59" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="48" spans="1:25" s="57" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="35" t="s">
+    <row r="49" spans="1:25" s="57" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B48" s="60" t="s">
+      <c r="B49" s="60" t="s">
         <v>213</v>
       </c>
-      <c r="C48" s="61"/>
-      <c r="D48" s="61" t="s">
+      <c r="C49" s="61"/>
+      <c r="D49" s="61" t="s">
         <v>223</v>
       </c>
-      <c r="E48" s="61"/>
-      <c r="F48" s="61"/>
-      <c r="G48" s="61"/>
-      <c r="H48" s="61"/>
-      <c r="I48" s="61"/>
-      <c r="J48" s="61"/>
-      <c r="K48" s="61"/>
-      <c r="L48" s="61"/>
-      <c r="M48" s="61"/>
-      <c r="N48" s="61"/>
-      <c r="O48" s="61"/>
-      <c r="P48" s="61"/>
-      <c r="Q48" s="61"/>
-      <c r="R48" s="61"/>
-      <c r="S48" s="61"/>
-      <c r="T48" s="61"/>
-      <c r="U48" s="61"/>
-      <c r="V48" s="61"/>
-      <c r="W48" s="61"/>
-      <c r="X48" s="61"/>
-      <c r="Y48" s="55"/>
+      <c r="E49" s="61"/>
+      <c r="F49" s="61"/>
+      <c r="G49" s="61"/>
+      <c r="H49" s="61"/>
+      <c r="I49" s="61"/>
+      <c r="J49" s="61"/>
+      <c r="K49" s="61"/>
+      <c r="L49" s="61"/>
+      <c r="M49" s="61"/>
+      <c r="N49" s="61"/>
+      <c r="O49" s="61"/>
+      <c r="P49" s="61"/>
+      <c r="Q49" s="61"/>
+      <c r="R49" s="61"/>
+      <c r="S49" s="61"/>
+      <c r="T49" s="61"/>
+      <c r="U49" s="61"/>
+      <c r="V49" s="61"/>
+      <c r="W49" s="61"/>
+      <c r="X49" s="61"/>
+      <c r="Y49" s="55"/>
     </row>
-    <row r="49" spans="1:25" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="B49" s="39" t="s">
-        <v>183</v>
-      </c>
-      <c r="C49" s="37"/>
-      <c r="D49" s="36" t="s">
-        <v>124</v>
-      </c>
-      <c r="E49" s="36"/>
-      <c r="F49" s="37"/>
-      <c r="G49" s="37"/>
-      <c r="H49" s="37"/>
-      <c r="I49" s="37"/>
-      <c r="J49" s="37"/>
-      <c r="K49" s="36"/>
-      <c r="L49" s="37"/>
-      <c r="M49" s="37"/>
-      <c r="N49" s="37"/>
-      <c r="O49" s="36"/>
-      <c r="P49" s="36"/>
-      <c r="Q49" s="37"/>
-      <c r="R49" s="37"/>
-      <c r="S49" s="37"/>
-      <c r="T49" s="37"/>
-      <c r="U49" s="37"/>
-      <c r="V49" s="36"/>
-      <c r="W49" s="37"/>
-      <c r="X49" s="37"/>
-      <c r="Y49" s="38"/>
-    </row>
-    <row r="50" spans="1:25" s="26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:25" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="39" t="s">
         <v>14</v>
       </c>
       <c r="B50" s="39" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C50" s="37"/>
       <c r="D50" s="36" t="s">
-        <v>187</v>
-      </c>
-      <c r="E50" s="30" t="s">
-        <v>189</v>
-      </c>
-      <c r="F50" s="37" t="s">
-        <v>125</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="E50" s="36"/>
+      <c r="F50" s="37"/>
       <c r="G50" s="37"/>
-      <c r="H50" s="37" t="s">
-        <v>125</v>
-      </c>
+      <c r="H50" s="37"/>
       <c r="I50" s="37"/>
-      <c r="J50" s="37" t="s">
-        <v>188</v>
-      </c>
+      <c r="J50" s="37"/>
       <c r="K50" s="36"/>
-      <c r="L50" s="36"/>
+      <c r="L50" s="37"/>
       <c r="M50" s="37"/>
       <c r="N50" s="37"/>
       <c r="O50" s="36"/>
       <c r="P50" s="36"/>
       <c r="Q50" s="37"/>
-      <c r="R50" s="37" t="s">
-        <v>205</v>
-      </c>
-      <c r="S50" s="37" t="s">
-        <v>206</v>
-      </c>
-      <c r="T50" s="37" t="s">
-        <v>205</v>
-      </c>
-      <c r="U50" s="37" t="s">
-        <v>206</v>
-      </c>
-      <c r="V50" s="36" t="s">
-        <v>205</v>
-      </c>
+      <c r="R50" s="37"/>
+      <c r="S50" s="37"/>
+      <c r="T50" s="37"/>
+      <c r="U50" s="37"/>
+      <c r="V50" s="36"/>
       <c r="W50" s="37"/>
       <c r="X50" s="37"/>
-      <c r="Y50" s="38" t="s">
-        <v>193</v>
-      </c>
+      <c r="Y50" s="38"/>
     </row>
-    <row r="51" spans="1:25" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:25" s="26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="39" t="s">
         <v>14</v>
       </c>
       <c r="B51" s="39" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C51" s="37"/>
       <c r="D51" s="36" t="s">
-        <v>124</v>
-      </c>
-      <c r="E51" s="36"/>
-      <c r="F51" s="37"/>
+        <v>187</v>
+      </c>
+      <c r="E51" s="30" t="s">
+        <v>189</v>
+      </c>
+      <c r="F51" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="G51" s="37"/>
-      <c r="H51" s="37"/>
+      <c r="H51" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="I51" s="37"/>
-      <c r="J51" s="37"/>
+      <c r="J51" s="37" t="s">
+        <v>188</v>
+      </c>
       <c r="K51" s="36"/>
-      <c r="L51" s="37"/>
+      <c r="L51" s="36"/>
       <c r="M51" s="37"/>
       <c r="N51" s="37"/>
       <c r="O51" s="36"/>
       <c r="P51" s="36"/>
       <c r="Q51" s="37"/>
-      <c r="R51" s="37"/>
-      <c r="S51" s="37"/>
-      <c r="T51" s="37"/>
-      <c r="U51" s="37"/>
-      <c r="V51" s="36"/>
+      <c r="R51" s="37" t="s">
+        <v>205</v>
+      </c>
+      <c r="S51" s="37" t="s">
+        <v>206</v>
+      </c>
+      <c r="T51" s="37" t="s">
+        <v>205</v>
+      </c>
+      <c r="U51" s="37" t="s">
+        <v>206</v>
+      </c>
+      <c r="V51" s="36" t="s">
+        <v>205</v>
+      </c>
       <c r="W51" s="37"/>
       <c r="X51" s="37"/>
-      <c r="Y51" s="38"/>
+      <c r="Y51" s="38" t="s">
+        <v>193</v>
+      </c>
     </row>
-    <row r="52" spans="1:25" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:25" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="39" t="s">
         <v>14</v>
       </c>
       <c r="B52" s="39" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C52" s="37"/>
       <c r="D52" s="36" t="s">
         <v>124</v>
       </c>
-      <c r="E52" s="36" t="s">
-        <v>128</v>
-      </c>
-      <c r="F52" s="37" t="s">
-        <v>125</v>
-      </c>
+      <c r="E52" s="36"/>
+      <c r="F52" s="37"/>
       <c r="G52" s="37"/>
-      <c r="H52" s="37" t="s">
-        <v>125</v>
-      </c>
+      <c r="H52" s="37"/>
       <c r="I52" s="37"/>
-      <c r="J52" s="37" t="s">
-        <v>111</v>
-      </c>
+      <c r="J52" s="37"/>
       <c r="K52" s="36"/>
       <c r="L52" s="37"/>
       <c r="M52" s="37"/>
@@ -13345,84 +13490,72 @@
       <c r="O52" s="36"/>
       <c r="P52" s="36"/>
       <c r="Q52" s="37"/>
-      <c r="R52" s="37" t="s">
-        <v>130</v>
-      </c>
-      <c r="S52" s="37" t="s">
-        <v>111</v>
-      </c>
-      <c r="T52" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="U52" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="V52" s="36" t="s">
-        <v>129</v>
-      </c>
+      <c r="R52" s="37"/>
+      <c r="S52" s="37"/>
+      <c r="T52" s="37"/>
+      <c r="U52" s="37"/>
+      <c r="V52" s="36"/>
       <c r="W52" s="37"/>
       <c r="X52" s="37"/>
       <c r="Y52" s="38"/>
     </row>
-    <row r="53" spans="1:25" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:25" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="39" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="B53" s="39" t="s">
-        <v>121</v>
+        <v>185</v>
       </c>
       <c r="C53" s="37"/>
       <c r="D53" s="36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E53" s="36" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="F53" s="37" t="s">
         <v>125</v>
       </c>
       <c r="G53" s="37"/>
-      <c r="H53" s="37"/>
+      <c r="H53" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="I53" s="37"/>
       <c r="J53" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="K53" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="L53" s="37" t="s">
-        <v>125</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="K53" s="36"/>
+      <c r="L53" s="37"/>
       <c r="M53" s="37"/>
-      <c r="N53" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="O53" s="37"/>
-      <c r="P53" s="37"/>
-      <c r="Q53" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="N53" s="37"/>
+      <c r="O53" s="36"/>
+      <c r="P53" s="36"/>
+      <c r="Q53" s="37"/>
       <c r="R53" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="S53" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="T53" s="37" t="s">
         <v>129</v>
       </c>
-      <c r="S53" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="T53" s="37"/>
-      <c r="U53" s="37"/>
-      <c r="V53" s="37" t="s">
+      <c r="U53" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="V53" s="36" t="s">
         <v>129</v>
       </c>
       <c r="W53" s="37"/>
       <c r="X53" s="37"/>
       <c r="Y53" s="38"/>
     </row>
-    <row r="54" spans="1:25" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:25" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B54" s="39" t="s">
-        <v>201</v>
+        <v>121</v>
       </c>
       <c r="C54" s="37"/>
       <c r="D54" s="36" t="s">
@@ -13443,12 +13576,18 @@
       <c r="K54" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="L54" s="37"/>
+      <c r="L54" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="M54" s="37"/>
-      <c r="N54" s="37"/>
+      <c r="N54" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="O54" s="37"/>
       <c r="P54" s="37"/>
-      <c r="Q54" s="37"/>
+      <c r="Q54" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="R54" s="37" t="s">
         <v>129</v>
       </c>
@@ -13464,12 +13603,12 @@
       <c r="X54" s="37"/>
       <c r="Y54" s="38"/>
     </row>
-    <row r="55" spans="1:25" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:25" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B55" s="39" t="s">
-        <v>170</v>
+        <v>201</v>
       </c>
       <c r="C55" s="37"/>
       <c r="D55" s="36" t="s">
@@ -13490,18 +13629,12 @@
       <c r="K55" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="L55" s="37" t="s">
-        <v>125</v>
-      </c>
+      <c r="L55" s="37"/>
       <c r="M55" s="37"/>
-      <c r="N55" s="37" t="s">
-        <v>125</v>
-      </c>
+      <c r="N55" s="37"/>
       <c r="O55" s="37"/>
       <c r="P55" s="37"/>
-      <c r="Q55" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="Q55" s="37"/>
       <c r="R55" s="37" t="s">
         <v>129</v>
       </c>
@@ -13517,26 +13650,24 @@
       <c r="X55" s="37"/>
       <c r="Y55" s="38"/>
     </row>
-    <row r="56" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:25" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B56" s="39" t="s">
-        <v>43</v>
+        <v>170</v>
       </c>
       <c r="C56" s="37"/>
-      <c r="D56" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="E56" s="37" t="s">
+      <c r="D56" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="E56" s="36" t="s">
         <v>125</v>
       </c>
       <c r="F56" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="G56" s="37" t="s">
-        <v>18</v>
-      </c>
+      <c r="G56" s="37"/>
       <c r="H56" s="37"/>
       <c r="I56" s="37"/>
       <c r="J56" s="37" t="s">
@@ -13577,7 +13708,7 @@
         <v>42</v>
       </c>
       <c r="B57" s="39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C57" s="37"/>
       <c r="D57" s="37" t="s">
@@ -13590,14 +13721,10 @@
         <v>125</v>
       </c>
       <c r="G57" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="H57" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="I57" s="37" t="s">
-        <v>125</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="H57" s="37"/>
+      <c r="I57" s="37"/>
       <c r="J57" s="37" t="s">
         <v>16</v>
       </c>
@@ -13607,18 +13734,12 @@
       <c r="L57" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="M57" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="M57" s="37"/>
       <c r="N57" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="O57" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="P57" s="37" t="s">
-        <v>125</v>
-      </c>
+      <c r="O57" s="37"/>
+      <c r="P57" s="37"/>
       <c r="Q57" s="37" t="s">
         <v>16</v>
       </c>
@@ -13628,27 +13749,21 @@
       <c r="S57" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="T57" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="U57" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="T57" s="37"/>
+      <c r="U57" s="37"/>
       <c r="V57" s="37" t="s">
         <v>129</v>
       </c>
       <c r="W57" s="37"/>
-      <c r="X57" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="X57" s="37"/>
       <c r="Y57" s="38"/>
     </row>
-    <row r="58" spans="1:25" s="17" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B58" s="39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C58" s="37"/>
       <c r="D58" s="37" t="s">
@@ -13708,20 +13823,18 @@
       <c r="V58" s="37" t="s">
         <v>129</v>
       </c>
-      <c r="W58" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="W58" s="37"/>
       <c r="X58" s="37" t="s">
         <v>16</v>
       </c>
       <c r="Y58" s="38"/>
     </row>
-    <row r="59" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:25" s="17" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B59" s="39" t="s">
-        <v>146</v>
+        <v>45</v>
       </c>
       <c r="C59" s="37"/>
       <c r="D59" s="37" t="s">
@@ -13781,7 +13894,9 @@
       <c r="V59" s="37" t="s">
         <v>129</v>
       </c>
-      <c r="W59" s="37"/>
+      <c r="W59" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="X59" s="37" t="s">
         <v>16</v>
       </c>
@@ -13792,7 +13907,7 @@
         <v>42</v>
       </c>
       <c r="B60" s="39" t="s">
-        <v>46</v>
+        <v>146</v>
       </c>
       <c r="C60" s="37"/>
       <c r="D60" s="37" t="s">
@@ -13863,7 +13978,7 @@
         <v>42</v>
       </c>
       <c r="B61" s="39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C61" s="37"/>
       <c r="D61" s="37" t="s">
@@ -13929,12 +14044,12 @@
       </c>
       <c r="Y61" s="38"/>
     </row>
-    <row r="62" spans="1:25" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B62" s="39" t="s">
-        <v>153</v>
+        <v>47</v>
       </c>
       <c r="C62" s="37"/>
       <c r="D62" s="37" t="s">
@@ -14000,12 +14115,12 @@
       </c>
       <c r="Y62" s="38"/>
     </row>
-    <row r="63" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:25" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B63" s="39" t="s">
-        <v>48</v>
+        <v>153</v>
       </c>
       <c r="C63" s="37"/>
       <c r="D63" s="37" t="s">
@@ -14076,7 +14191,7 @@
         <v>42</v>
       </c>
       <c r="B64" s="39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C64" s="37"/>
       <c r="D64" s="37" t="s">
@@ -14112,7 +14227,9 @@
       <c r="N64" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="O64" s="37"/>
+      <c r="O64" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="P64" s="37" t="s">
         <v>125</v>
       </c>
@@ -14145,7 +14262,7 @@
         <v>42</v>
       </c>
       <c r="B65" s="39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C65" s="37"/>
       <c r="D65" s="37" t="s">
@@ -14181,9 +14298,7 @@
       <c r="N65" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="O65" s="37" t="s">
-        <v>125</v>
-      </c>
+      <c r="O65" s="37"/>
       <c r="P65" s="37" t="s">
         <v>125</v>
       </c>
@@ -14216,7 +14331,7 @@
         <v>42</v>
       </c>
       <c r="B66" s="39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C66" s="37"/>
       <c r="D66" s="37" t="s">
@@ -14228,8 +14343,12 @@
       <c r="F66" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="G66" s="37"/>
-      <c r="H66" s="37"/>
+      <c r="G66" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="H66" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="I66" s="37" t="s">
         <v>125</v>
       </c>
@@ -14242,11 +14361,15 @@
       <c r="L66" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="M66" s="37"/>
+      <c r="M66" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="N66" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="O66" s="37"/>
+      <c r="O66" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="P66" s="37" t="s">
         <v>125</v>
       </c>
@@ -14279,7 +14402,7 @@
         <v>42</v>
       </c>
       <c r="B67" s="39" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C67" s="37"/>
       <c r="D67" s="37" t="s">
@@ -14292,10 +14415,10 @@
         <v>125</v>
       </c>
       <c r="G67" s="37"/>
-      <c r="H67" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="I67" s="37"/>
+      <c r="H67" s="37"/>
+      <c r="I67" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="J67" s="37" t="s">
         <v>16</v>
       </c>
@@ -14309,10 +14432,10 @@
       <c r="N67" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="O67" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="P67" s="37"/>
+      <c r="O67" s="37"/>
+      <c r="P67" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="Q67" s="37" t="s">
         <v>16</v>
       </c>
@@ -14322,13 +14445,19 @@
       <c r="S67" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="T67" s="37"/>
-      <c r="U67" s="37"/>
+      <c r="T67" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="U67" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="V67" s="37" t="s">
         <v>129</v>
       </c>
       <c r="W67" s="37"/>
-      <c r="X67" s="37"/>
+      <c r="X67" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="Y67" s="38"/>
     </row>
     <row r="68" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -14336,7 +14465,7 @@
         <v>42</v>
       </c>
       <c r="B68" s="39" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C68" s="37"/>
       <c r="D68" s="37" t="s">
@@ -14349,7 +14478,9 @@
         <v>125</v>
       </c>
       <c r="G68" s="37"/>
-      <c r="H68" s="37"/>
+      <c r="H68" s="37" t="s">
+        <v>18</v>
+      </c>
       <c r="I68" s="37"/>
       <c r="J68" s="37" t="s">
         <v>16</v>
@@ -14364,7 +14495,9 @@
       <c r="N68" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="O68" s="37"/>
+      <c r="O68" s="37" t="s">
+        <v>18</v>
+      </c>
       <c r="P68" s="37"/>
       <c r="Q68" s="37" t="s">
         <v>16</v>
@@ -14389,7 +14522,7 @@
         <v>42</v>
       </c>
       <c r="B69" s="39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C69" s="37"/>
       <c r="D69" s="37" t="s">
@@ -14442,7 +14575,7 @@
         <v>42</v>
       </c>
       <c r="B70" s="39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C70" s="37"/>
       <c r="D70" s="37" t="s">
@@ -14490,12 +14623,12 @@
       <c r="X70" s="37"/>
       <c r="Y70" s="38"/>
     </row>
-    <row r="71" spans="1:25" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B71" s="39" t="s">
-        <v>119</v>
+        <v>55</v>
       </c>
       <c r="C71" s="37"/>
       <c r="D71" s="37" t="s">
@@ -14507,15 +14640,9 @@
       <c r="F71" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="G71" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="H71" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="I71" s="37" t="s">
-        <v>125</v>
-      </c>
+      <c r="G71" s="37"/>
+      <c r="H71" s="37"/>
+      <c r="I71" s="37"/>
       <c r="J71" s="37" t="s">
         <v>16</v>
       </c>
@@ -14525,16 +14652,12 @@
       <c r="L71" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="M71" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="M71" s="37"/>
       <c r="N71" s="37" t="s">
         <v>125</v>
       </c>
       <c r="O71" s="37"/>
-      <c r="P71" s="37" t="s">
-        <v>125</v>
-      </c>
+      <c r="P71" s="37"/>
       <c r="Q71" s="37" t="s">
         <v>16</v>
       </c>
@@ -14544,27 +14667,21 @@
       <c r="S71" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="T71" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="U71" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="T71" s="37"/>
+      <c r="U71" s="37"/>
       <c r="V71" s="37" t="s">
         <v>129</v>
       </c>
       <c r="W71" s="37"/>
-      <c r="X71" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="X71" s="37"/>
       <c r="Y71" s="38"/>
     </row>
-    <row r="72" spans="1:25" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:25" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B72" s="39" t="s">
-        <v>171</v>
+        <v>119</v>
       </c>
       <c r="C72" s="37"/>
       <c r="D72" s="37" t="s">
@@ -14628,12 +14745,12 @@
       </c>
       <c r="Y72" s="38"/>
     </row>
-    <row r="73" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:25" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B73" s="39" t="s">
-        <v>56</v>
+        <v>171</v>
       </c>
       <c r="C73" s="37"/>
       <c r="D73" s="37" t="s">
@@ -14669,9 +14786,7 @@
       <c r="N73" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="O73" s="37" t="s">
-        <v>125</v>
-      </c>
+      <c r="O73" s="37"/>
       <c r="P73" s="37" t="s">
         <v>125</v>
       </c>
@@ -14699,12 +14814,12 @@
       </c>
       <c r="Y73" s="38"/>
     </row>
-    <row r="74" spans="1:25" s="17" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B74" s="39" t="s">
-        <v>123</v>
+        <v>56</v>
       </c>
       <c r="C74" s="37"/>
       <c r="D74" s="37" t="s">
@@ -14765,7 +14880,9 @@
         <v>129</v>
       </c>
       <c r="W74" s="37"/>
-      <c r="X74" s="37"/>
+      <c r="X74" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="Y74" s="38"/>
     </row>
     <row r="75" spans="1:25" s="17" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -14773,7 +14890,7 @@
         <v>42</v>
       </c>
       <c r="B75" s="39" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="C75" s="37"/>
       <c r="D75" s="37" t="s">
@@ -14842,7 +14959,7 @@
         <v>42</v>
       </c>
       <c r="B76" s="39" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C76" s="37"/>
       <c r="D76" s="37" t="s">
@@ -14911,7 +15028,7 @@
         <v>42</v>
       </c>
       <c r="B77" s="39" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C77" s="37"/>
       <c r="D77" s="37" t="s">
@@ -14980,7 +15097,7 @@
         <v>42</v>
       </c>
       <c r="B78" s="39" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C78" s="37"/>
       <c r="D78" s="37" t="s">
@@ -15044,26 +15161,32 @@
       <c r="X78" s="37"/>
       <c r="Y78" s="38"/>
     </row>
-    <row r="79" spans="1:25" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:25" s="17" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B79" s="39" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C79" s="37"/>
-      <c r="D79" s="36" t="s">
-        <v>125</v>
-      </c>
-      <c r="E79" s="36" t="s">
+      <c r="D79" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="E79" s="37" t="s">
         <v>125</v>
       </c>
       <c r="F79" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="G79" s="37"/>
-      <c r="H79" s="37"/>
-      <c r="I79" s="37"/>
+      <c r="G79" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="H79" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="I79" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="J79" s="37" t="s">
         <v>16</v>
       </c>
@@ -15073,12 +15196,18 @@
       <c r="L79" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="M79" s="37"/>
+      <c r="M79" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="N79" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="O79" s="37"/>
-      <c r="P79" s="37"/>
+      <c r="O79" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="P79" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="Q79" s="37" t="s">
         <v>16</v>
       </c>
@@ -15088,39 +15217,39 @@
       <c r="S79" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="T79" s="37"/>
-      <c r="U79" s="37"/>
-      <c r="V79" s="37"/>
+      <c r="T79" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="U79" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="V79" s="37" t="s">
+        <v>129</v>
+      </c>
       <c r="W79" s="37"/>
       <c r="X79" s="37"/>
       <c r="Y79" s="38"/>
     </row>
-    <row r="80" spans="1:25" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:25" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B80" s="39" t="s">
-        <v>186</v>
+        <v>145</v>
       </c>
       <c r="C80" s="37"/>
-      <c r="D80" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="E80" s="37" t="s">
+      <c r="D80" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="E80" s="36" t="s">
         <v>125</v>
       </c>
       <c r="F80" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="G80" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="H80" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="I80" s="37" t="s">
-        <v>125</v>
-      </c>
+      <c r="G80" s="37"/>
+      <c r="H80" s="37"/>
+      <c r="I80" s="37"/>
       <c r="J80" s="37" t="s">
         <v>16</v>
       </c>
@@ -15130,18 +15259,12 @@
       <c r="L80" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="M80" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="M80" s="37"/>
       <c r="N80" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="O80" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="P80" s="37" t="s">
-        <v>125</v>
-      </c>
+      <c r="O80" s="37"/>
+      <c r="P80" s="37"/>
       <c r="Q80" s="37" t="s">
         <v>16</v>
       </c>
@@ -15151,25 +15274,19 @@
       <c r="S80" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="T80" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="U80" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="V80" s="37" t="s">
-        <v>129</v>
-      </c>
+      <c r="T80" s="37"/>
+      <c r="U80" s="37"/>
+      <c r="V80" s="37"/>
       <c r="W80" s="37"/>
       <c r="X80" s="37"/>
       <c r="Y80" s="38"/>
     </row>
-    <row r="81" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:25" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A81" s="39" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="B81" s="39" t="s">
-        <v>58</v>
+        <v>186</v>
       </c>
       <c r="C81" s="37"/>
       <c r="D81" s="37" t="s">
@@ -15191,7 +15308,7 @@
         <v>125</v>
       </c>
       <c r="J81" s="37" t="s">
-        <v>214</v>
+        <v>16</v>
       </c>
       <c r="K81" s="37" t="s">
         <v>125</v>
@@ -15212,13 +15329,13 @@
         <v>125</v>
       </c>
       <c r="Q81" s="37" t="s">
-        <v>214</v>
+        <v>16</v>
       </c>
       <c r="R81" s="37" t="s">
-        <v>215</v>
+        <v>129</v>
       </c>
       <c r="S81" s="37" t="s">
-        <v>214</v>
+        <v>16</v>
       </c>
       <c r="T81" s="37" t="s">
         <v>129</v>
@@ -15229,22 +15346,16 @@
       <c r="V81" s="37" t="s">
         <v>129</v>
       </c>
-      <c r="W81" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="X81" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y81" s="70" t="s">
-        <v>216</v>
-      </c>
+      <c r="W81" s="37"/>
+      <c r="X81" s="37"/>
+      <c r="Y81" s="38"/>
     </row>
     <row r="82" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A82" s="39" t="s">
         <v>57</v>
       </c>
       <c r="B82" s="39" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C82" s="37"/>
       <c r="D82" s="37" t="s">
@@ -15310,20 +15421,22 @@
       <c r="X82" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="Y82" s="71"/>
+      <c r="Y82" s="72" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="83" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83" s="39" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B83" s="39" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C83" s="37"/>
       <c r="D83" s="37" t="s">
-        <v>124</v>
-      </c>
-      <c r="E83" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="E83" s="37" t="s">
         <v>125</v>
       </c>
       <c r="F83" s="37" t="s">
@@ -15339,10 +15452,10 @@
         <v>125</v>
       </c>
       <c r="J83" s="37" t="s">
-        <v>16</v>
+        <v>214</v>
       </c>
       <c r="K83" s="37" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="L83" s="37" t="s">
         <v>125</v>
@@ -15360,133 +15473,173 @@
         <v>125</v>
       </c>
       <c r="Q83" s="37" t="s">
-        <v>16</v>
+        <v>214</v>
       </c>
       <c r="R83" s="37" t="s">
-        <v>130</v>
+        <v>215</v>
       </c>
       <c r="S83" s="37" t="s">
-        <v>111</v>
+        <v>214</v>
       </c>
       <c r="T83" s="37" t="s">
         <v>129</v>
       </c>
       <c r="U83" s="37" t="s">
-        <v>111</v>
+        <v>16</v>
       </c>
       <c r="V83" s="37" t="s">
         <v>129</v>
       </c>
       <c r="W83" s="37" t="s">
-        <v>111</v>
+        <v>16</v>
       </c>
       <c r="X83" s="37" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y83" s="38"/>
+        <v>16</v>
+      </c>
+      <c r="Y83" s="73"/>
     </row>
-    <row r="84" spans="1:25" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A84" s="42" t="s">
-        <v>61</v>
-      </c>
-      <c r="B84" s="42" t="s">
-        <v>62</v>
-      </c>
-      <c r="C84" s="43"/>
+    <row r="84" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A84" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="B84" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="C84" s="37"/>
       <c r="D84" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="E84" s="43"/>
-      <c r="F84" s="43"/>
-      <c r="G84" s="43"/>
-      <c r="H84" s="43"/>
-      <c r="I84" s="43"/>
-      <c r="J84" s="43"/>
-      <c r="K84" s="43"/>
-      <c r="L84" s="43"/>
-      <c r="M84" s="43"/>
-      <c r="N84" s="43"/>
-      <c r="O84" s="43"/>
-      <c r="P84" s="43"/>
-      <c r="Q84" s="43"/>
-      <c r="R84" s="43"/>
-      <c r="S84" s="43"/>
-      <c r="T84" s="43"/>
-      <c r="U84" s="43"/>
-      <c r="V84" s="43"/>
-      <c r="W84" s="43"/>
-      <c r="X84" s="43"/>
-      <c r="Y84" s="44" t="s">
-        <v>63</v>
-      </c>
+      <c r="E84" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="F84" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="G84" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="H84" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="I84" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="J84" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="K84" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="L84" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="M84" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="N84" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="O84" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="P84" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q84" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="R84" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="S84" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="T84" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="U84" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="V84" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="W84" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="X84" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="Y84" s="38"/>
     </row>
-    <row r="85" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A85" s="35" t="s">
+    <row r="85" spans="1:25" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A85" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="B85" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="C85" s="36"/>
+      <c r="B85" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="C85" s="43"/>
       <c r="D85" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="E85" s="36"/>
-      <c r="F85" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="G85" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="H85" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="I85" s="36"/>
-      <c r="J85" s="37"/>
-      <c r="K85" s="36"/>
-      <c r="L85" s="36"/>
-      <c r="M85" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="N85" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="O85" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="P85" s="36"/>
-      <c r="Q85" s="37"/>
-      <c r="R85" s="36"/>
-      <c r="S85" s="36"/>
-      <c r="T85" s="36"/>
-      <c r="U85" s="36"/>
-      <c r="V85" s="36"/>
-      <c r="W85" s="36"/>
-      <c r="X85" s="36"/>
-      <c r="Y85" s="30"/>
+      <c r="E85" s="43"/>
+      <c r="F85" s="43"/>
+      <c r="G85" s="43"/>
+      <c r="H85" s="43"/>
+      <c r="I85" s="43"/>
+      <c r="J85" s="43"/>
+      <c r="K85" s="43"/>
+      <c r="L85" s="43"/>
+      <c r="M85" s="43"/>
+      <c r="N85" s="43"/>
+      <c r="O85" s="43"/>
+      <c r="P85" s="43"/>
+      <c r="Q85" s="43"/>
+      <c r="R85" s="43"/>
+      <c r="S85" s="43"/>
+      <c r="T85" s="43"/>
+      <c r="U85" s="43"/>
+      <c r="V85" s="43"/>
+      <c r="W85" s="43"/>
+      <c r="X85" s="43"/>
+      <c r="Y85" s="44" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="86" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A86" s="35" t="s">
         <v>61</v>
       </c>
       <c r="B86" s="35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C86" s="36"/>
       <c r="D86" s="37" t="s">
         <v>124</v>
       </c>
       <c r="E86" s="36"/>
-      <c r="F86" s="36"/>
-      <c r="G86" s="36"/>
-      <c r="H86" s="36"/>
+      <c r="F86" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="G86" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="H86" s="36" t="s">
+        <v>18</v>
+      </c>
       <c r="I86" s="36"/>
       <c r="J86" s="37"/>
       <c r="K86" s="36"/>
       <c r="L86" s="36"/>
-      <c r="M86" s="36"/>
-      <c r="N86" s="36"/>
-      <c r="O86" s="36"/>
+      <c r="M86" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="N86" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="O86" s="36" t="s">
+        <v>18</v>
+      </c>
       <c r="P86" s="36"/>
       <c r="Q86" s="37"/>
       <c r="R86" s="36"/>
@@ -15503,7 +15656,7 @@
         <v>61</v>
       </c>
       <c r="B87" s="35" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C87" s="36"/>
       <c r="D87" s="37" t="s">
@@ -15536,7 +15689,7 @@
         <v>61</v>
       </c>
       <c r="B88" s="35" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C88" s="36"/>
       <c r="D88" s="37" t="s">
@@ -15564,12 +15717,12 @@
       <c r="X88" s="36"/>
       <c r="Y88" s="30"/>
     </row>
-    <row r="89" spans="1:25" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A89" s="35" t="s">
         <v>61</v>
       </c>
       <c r="B89" s="35" t="s">
-        <v>164</v>
+        <v>67</v>
       </c>
       <c r="C89" s="36"/>
       <c r="D89" s="37" t="s">
@@ -15597,12 +15750,12 @@
       <c r="X89" s="36"/>
       <c r="Y89" s="30"/>
     </row>
-    <row r="90" spans="1:25" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:25" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A90" s="35" t="s">
         <v>61</v>
       </c>
       <c r="B90" s="35" t="s">
-        <v>32</v>
+        <v>164</v>
       </c>
       <c r="C90" s="36"/>
       <c r="D90" s="37" t="s">
@@ -15630,12 +15783,12 @@
       <c r="X90" s="36"/>
       <c r="Y90" s="30"/>
     </row>
-    <row r="91" spans="1:25" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:25" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A91" s="35" t="s">
         <v>61</v>
       </c>
       <c r="B91" s="35" t="s">
-        <v>179</v>
+        <v>32</v>
       </c>
       <c r="C91" s="36"/>
       <c r="D91" s="37" t="s">
@@ -15663,78 +15816,78 @@
       <c r="X91" s="36"/>
       <c r="Y91" s="30"/>
     </row>
-    <row r="92" spans="1:25" s="57" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:25" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A92" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="B92" s="60" t="s">
-        <v>211</v>
-      </c>
-      <c r="C92" s="61"/>
-      <c r="D92" s="61" t="s">
+      <c r="B92" s="35" t="s">
+        <v>179</v>
+      </c>
+      <c r="C92" s="36"/>
+      <c r="D92" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="E92" s="61"/>
-      <c r="F92" s="61"/>
-      <c r="G92" s="61"/>
-      <c r="H92" s="61"/>
-      <c r="I92" s="61"/>
-      <c r="J92" s="61"/>
-      <c r="K92" s="61"/>
-      <c r="L92" s="61"/>
-      <c r="M92" s="61"/>
-      <c r="N92" s="61"/>
-      <c r="O92" s="61"/>
-      <c r="P92" s="61"/>
-      <c r="Q92" s="61"/>
-      <c r="R92" s="61"/>
-      <c r="S92" s="61"/>
-      <c r="T92" s="61"/>
-      <c r="U92" s="61"/>
-      <c r="V92" s="61"/>
-      <c r="W92" s="61"/>
-      <c r="X92" s="61"/>
-      <c r="Y92" s="55"/>
+      <c r="E92" s="36"/>
+      <c r="F92" s="36"/>
+      <c r="G92" s="36"/>
+      <c r="H92" s="36"/>
+      <c r="I92" s="36"/>
+      <c r="J92" s="37"/>
+      <c r="K92" s="36"/>
+      <c r="L92" s="36"/>
+      <c r="M92" s="36"/>
+      <c r="N92" s="36"/>
+      <c r="O92" s="36"/>
+      <c r="P92" s="36"/>
+      <c r="Q92" s="37"/>
+      <c r="R92" s="36"/>
+      <c r="S92" s="36"/>
+      <c r="T92" s="36"/>
+      <c r="U92" s="36"/>
+      <c r="V92" s="36"/>
+      <c r="W92" s="36"/>
+      <c r="X92" s="36"/>
+      <c r="Y92" s="30"/>
     </row>
-    <row r="93" spans="1:25" s="52" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:25" s="57" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A93" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="B93" s="35" t="s">
-        <v>204</v>
-      </c>
-      <c r="C93" s="36"/>
-      <c r="D93" s="37" t="s">
+      <c r="B93" s="60" t="s">
+        <v>211</v>
+      </c>
+      <c r="C93" s="61"/>
+      <c r="D93" s="61" t="s">
         <v>124</v>
       </c>
-      <c r="E93" s="36"/>
-      <c r="F93" s="36"/>
-      <c r="G93" s="36"/>
-      <c r="H93" s="36"/>
-      <c r="I93" s="36"/>
-      <c r="J93" s="37"/>
-      <c r="K93" s="36"/>
-      <c r="L93" s="36"/>
-      <c r="M93" s="36"/>
-      <c r="N93" s="36"/>
-      <c r="O93" s="36"/>
-      <c r="P93" s="36"/>
-      <c r="Q93" s="37"/>
-      <c r="R93" s="36"/>
-      <c r="S93" s="36"/>
-      <c r="T93" s="36"/>
-      <c r="U93" s="36"/>
-      <c r="V93" s="36"/>
-      <c r="W93" s="36"/>
-      <c r="X93" s="36"/>
-      <c r="Y93" s="51"/>
+      <c r="E93" s="61"/>
+      <c r="F93" s="61"/>
+      <c r="G93" s="61"/>
+      <c r="H93" s="61"/>
+      <c r="I93" s="61"/>
+      <c r="J93" s="61"/>
+      <c r="K93" s="61"/>
+      <c r="L93" s="61"/>
+      <c r="M93" s="61"/>
+      <c r="N93" s="61"/>
+      <c r="O93" s="61"/>
+      <c r="P93" s="61"/>
+      <c r="Q93" s="61"/>
+      <c r="R93" s="61"/>
+      <c r="S93" s="61"/>
+      <c r="T93" s="61"/>
+      <c r="U93" s="61"/>
+      <c r="V93" s="61"/>
+      <c r="W93" s="61"/>
+      <c r="X93" s="61"/>
+      <c r="Y93" s="55"/>
     </row>
-    <row r="94" spans="1:25" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:25" s="52" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A94" s="35" t="s">
         <v>61</v>
       </c>
       <c r="B94" s="35" t="s">
-        <v>122</v>
+        <v>204</v>
       </c>
       <c r="C94" s="36"/>
       <c r="D94" s="37" t="s">
@@ -15760,14 +15913,14 @@
       <c r="V94" s="36"/>
       <c r="W94" s="36"/>
       <c r="X94" s="36"/>
-      <c r="Y94" s="30"/>
+      <c r="Y94" s="51"/>
     </row>
-    <row r="95" spans="1:25" s="69" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:25" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A95" s="35" t="s">
         <v>61</v>
       </c>
       <c r="B95" s="35" t="s">
-        <v>226</v>
+        <v>122</v>
       </c>
       <c r="C95" s="36"/>
       <c r="D95" s="37" t="s">
@@ -15793,101 +15946,152 @@
       <c r="V95" s="36"/>
       <c r="W95" s="36"/>
       <c r="X95" s="36"/>
-      <c r="Y95" s="68"/>
+      <c r="Y95" s="30"/>
     </row>
-    <row r="96" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:25" s="69" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A96" s="35" t="s">
-        <v>107</v>
+        <v>61</v>
       </c>
       <c r="B96" s="35" t="s">
-        <v>108</v>
-      </c>
-      <c r="C96" s="45"/>
+        <v>226</v>
+      </c>
+      <c r="C96" s="36"/>
       <c r="D96" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="E96" s="45"/>
-      <c r="F96" s="45"/>
-      <c r="G96" s="45"/>
-      <c r="H96" s="45"/>
-      <c r="I96" s="45"/>
-      <c r="J96" s="46"/>
-      <c r="K96" s="45"/>
-      <c r="L96" s="45"/>
-      <c r="M96" s="45"/>
-      <c r="N96" s="45"/>
-      <c r="O96" s="45"/>
-      <c r="P96" s="45"/>
-      <c r="Q96" s="46"/>
-      <c r="R96" s="45"/>
-      <c r="S96" s="45"/>
-      <c r="T96" s="45"/>
-      <c r="U96" s="45"/>
-      <c r="V96" s="45"/>
-      <c r="W96" s="45"/>
-      <c r="X96" s="45"/>
-      <c r="Y96" s="30"/>
+      <c r="E96" s="36"/>
+      <c r="F96" s="36"/>
+      <c r="G96" s="36"/>
+      <c r="H96" s="36"/>
+      <c r="I96" s="36"/>
+      <c r="J96" s="37"/>
+      <c r="K96" s="36"/>
+      <c r="L96" s="36"/>
+      <c r="M96" s="36"/>
+      <c r="N96" s="36"/>
+      <c r="O96" s="36"/>
+      <c r="P96" s="36"/>
+      <c r="Q96" s="37"/>
+      <c r="R96" s="36"/>
+      <c r="S96" s="36"/>
+      <c r="T96" s="36"/>
+      <c r="U96" s="36"/>
+      <c r="V96" s="36"/>
+      <c r="W96" s="36"/>
+      <c r="X96" s="36"/>
+      <c r="Y96" s="68"/>
     </row>
     <row r="97" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A97" s="35" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="B97" s="35" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C97" s="45"/>
       <c r="D97" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="E97" s="45"/>
+      <c r="F97" s="45"/>
+      <c r="G97" s="45"/>
+      <c r="H97" s="45"/>
+      <c r="I97" s="45"/>
+      <c r="J97" s="46"/>
+      <c r="K97" s="45"/>
+      <c r="L97" s="45"/>
+      <c r="M97" s="45"/>
+      <c r="N97" s="45"/>
+      <c r="O97" s="45"/>
+      <c r="P97" s="45"/>
+      <c r="Q97" s="46"/>
+      <c r="R97" s="45"/>
+      <c r="S97" s="45"/>
+      <c r="T97" s="45"/>
+      <c r="U97" s="45"/>
+      <c r="V97" s="45"/>
+      <c r="W97" s="45"/>
+      <c r="X97" s="45"/>
+      <c r="Y97" s="30"/>
+    </row>
+    <row r="98" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A98" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="B98" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="C98" s="45"/>
+      <c r="D98" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="E97" s="47" t="s">
+      <c r="E98" s="47" t="s">
         <v>126</v>
       </c>
-      <c r="F97" s="47"/>
-      <c r="G97" s="47" t="s">
+      <c r="F98" s="47"/>
+      <c r="G98" s="47" t="s">
         <v>126</v>
       </c>
-      <c r="H97" s="47"/>
-      <c r="I97" s="47"/>
-      <c r="J97" s="48" t="s">
+      <c r="H98" s="47"/>
+      <c r="I98" s="47"/>
+      <c r="J98" s="48" t="s">
         <v>158</v>
       </c>
-      <c r="K97" s="47" t="s">
+      <c r="K98" s="47" t="s">
         <v>126</v>
       </c>
-      <c r="L97" s="47" t="s">
+      <c r="L98" s="47" t="s">
         <v>126</v>
       </c>
-      <c r="M97" s="47" t="s">
+      <c r="M98" s="47" t="s">
         <v>126</v>
       </c>
-      <c r="N97" s="47" t="s">
+      <c r="N98" s="47" t="s">
         <v>126</v>
       </c>
-      <c r="O97" s="47"/>
-      <c r="P97" s="47"/>
-      <c r="Q97" s="48" t="s">
+      <c r="O98" s="47"/>
+      <c r="P98" s="47"/>
+      <c r="Q98" s="48" t="s">
         <v>158</v>
       </c>
-      <c r="R97" s="49" t="s">
+      <c r="R98" s="49" t="s">
         <v>163</v>
       </c>
-      <c r="S97" s="48" t="s">
+      <c r="S98" s="48" t="s">
         <v>158</v>
       </c>
-      <c r="T97" s="47"/>
-      <c r="U97" s="47" t="s">
+      <c r="T98" s="47"/>
+      <c r="U98" s="47" t="s">
         <v>158</v>
       </c>
-      <c r="V97" s="47"/>
-      <c r="W97" s="47"/>
-      <c r="X97" s="47"/>
-      <c r="Y97" s="30"/>
+      <c r="V98" s="47"/>
+      <c r="W98" s="47"/>
+      <c r="X98" s="47"/>
+      <c r="Y98" s="30"/>
     </row>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C77" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="B95" sqref="B95"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C34" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="D46" sqref="D46"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="C48" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="D72" sqref="D72:X72"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="C31" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
+      <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -15897,27 +16101,9 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
-      <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C31" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C48" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="D72" sqref="D72:X72"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
   </customSheetViews>
   <mergeCells count="6">
-    <mergeCell ref="Y81:Y82"/>
+    <mergeCell ref="Y82:Y83"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="K5:O5"/>
     <mergeCell ref="R5:X5"/>
@@ -16273,8 +16459,13 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
-      <selection activeCell="B17" sqref="B17"/>
+    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}">
+      <selection activeCell="A22" sqref="A22"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}">
+      <selection activeCell="G36" sqref="G36"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -16283,13 +16474,8 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}">
-      <selection activeCell="G36" sqref="G36"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}">
-      <selection activeCell="A22" sqref="A22"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
+      <selection activeCell="B17" sqref="B17"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>

</xml_diff>

<commit_message>
Poista turha duplikaattioikeusrivi Excelistä (kanavat / laadunseuranta / häiriötilanteet)
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -9,25 +9,25 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="27240" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="13020" windowWidth="51200" windowHeight="14660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
     <sheet name="Roolit" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$98</definedName>
-    <definedName name="Z_1DD617EE_F308_3E45_A8EF_4713F47FA0DD_.wvu.FilterData" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$98</definedName>
-    <definedName name="Z_7A9649F2_657F_9445_B6E6_FE94C6A09957_.wvu.FilterData" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$98</definedName>
-    <definedName name="Z_F86DF6F3_8AE5_3A44_B2D2_D623E01AE54F_.wvu.FilterData" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$98</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$97</definedName>
+    <definedName name="Z_1DD617EE_F308_3E45_A8EF_4713F47FA0DD_.wvu.FilterData" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$97</definedName>
+    <definedName name="Z_7A9649F2_657F_9445_B6E6_FE94C6A09957_.wvu.FilterData" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$97</definedName>
+    <definedName name="Z_F86DF6F3_8AE5_3A44_B2D2_D623E01AE54F_.wvu.FilterData" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$97</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2560" windowHeight="1189" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2560" windowHeight="560" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
+    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office -käyttäjä - Oma näkymä" guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="1149" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="Mikko Rönkkömäki - Personal View" guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" mergeInterval="0" personalView="1" windowWidth="2560" windowHeight="1071" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Microsoft Office -käyttäjä - Oma näkymä" guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="1149" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1459" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1456" uniqueCount="228">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -749,9 +749,6 @@
   </si>
   <si>
     <t>R*,W*,siirrä-muutos-ja-lisätöihin*</t>
-  </si>
-  <si>
-    <t>Kanavat / Laadunseuranta / Häiriötilanteet</t>
   </si>
   <si>
     <t>Järjestelmäasetukset</t>
@@ -1113,7 +1110,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -1237,19 +1234,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1481,7 +1465,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{CBA5289A-5B9B-984A-BEA7-1AD0AA9EDC22}" diskRevisions="1" revisionId="772" version="44">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{59381CD3-9619-064B-BFE6-F97D1F318E9C}" diskRevisions="1" revisionId="774" version="45">
   <header guid="{1E352813-0B26-DB4E-84BE-460845B77133}" dateTime="2017-06-20T12:32:37" maxSheetId="3" userName="Microsoft Office -käyttäjä" r:id="rId60" minRId="448" maxRId="464">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1746,6 +1730,12 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{59381CD3-9619-064B-BFE6-F97D1F318E9C}" dateTime="2017-12-21T15:05:29" maxSheetId="3" userName="Microsoft Office User" r:id="rId104" minRId="773">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -9867,6 +9857,574 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog42.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="773" sId="1" ref="A45:XFD45" action="deleteRow">
+    <rfmt sheetId="1" xfDxf="1" sqref="A45:XFD45" start="0" length="0"/>
+    <rcc rId="0" sId="1" dxf="1">
+      <nc r="A45" t="inlineStr">
+        <is>
+          <t>Urakat</t>
+        </is>
+      </nc>
+      <ndxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <border outline="0">
+          <left style="thin">
+            <color auto="1"/>
+          </left>
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </ndxf>
+    </rcc>
+    <rcc rId="0" sId="1" dxf="1">
+      <nc r="B45" t="inlineStr">
+        <is>
+          <t>Kanavat / Laadunseuranta / Häiriötilanteet</t>
+        </is>
+      </nc>
+      <ndxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </ndxf>
+    </rcc>
+    <rfmt sheetId="1" sqref="C45" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rcc rId="0" sId="1" dxf="1">
+      <nc r="D45" t="inlineStr">
+        <is>
+          <t>R*,W*</t>
+        </is>
+      </nc>
+      <ndxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" wrapText="1" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </ndxf>
+    </rcc>
+    <rfmt sheetId="1" sqref="E45" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" wrapText="1" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="F45" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="G45" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="H45" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="I45" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="J45" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" wrapText="1" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="K45" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" wrapText="1" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="L45" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" wrapText="1" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="M45" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="N45" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="O45" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="P45" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="Q45" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="R45" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" wrapText="1" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="S45" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" wrapText="1" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="T45" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="U45" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="V45" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="W45" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="X45" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="center" readingOrder="0"/>
+        <border outline="0">
+          <right style="thin">
+            <color auto="1"/>
+          </right>
+          <top style="thin">
+            <color auto="1"/>
+          </top>
+          <bottom style="thin">
+            <color auto="1"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="Y45" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color auto="1"/>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+      </dxf>
+    </rfmt>
+  </rrc>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="delete"/>
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_7A9649F2_657F_9445_B6E6_FE94C6A09957_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Oikeudet!$A$5:$Y$97</formula>
+    <oldFormula>Oikeudet!$A$5:$Y$97</oldFormula>
+  </rdn>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog5.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="514" sId="1">
@@ -10408,13 +10966,14 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="5">
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="6">
   <userInfo guid="{1E352813-0B26-DB4E-84BE-460845B77133}" name="Microsoft Office -käyttäjä" id="-785751636" dateTime="2017-06-20T12:33:00"/>
   <userInfo guid="{1AB7A282-42ED-4740-A9CB-95FF229EC1A0}" name="Mikko Rönkkömäki" id="-727946492" dateTime="2017-06-22T10:45:48"/>
   <userInfo guid="{4A189F6B-10A0-794F-AE26-98E1292E0A90}" name="Microsoft Office User" id="-296987972" dateTime="2017-09-21T08:10:21"/>
   <userInfo guid="{72187562-2E05-9542-A596-E87B0EC7A6D4}" name="Microsoft Office User" id="-296946728" dateTime="2017-11-06T12:39:34"/>
   <userInfo guid="{7DE0565B-D0D5-DF45-A2A1-25AA2C726E19}" name="Microsoft Office User" id="-296947028" dateTime="2017-11-20T14:54:25"/>
+  <userInfo guid="{59381CD3-9619-064B-BFE6-F97D1F318E9C}" name="Microsoft Office User" id="-296969556" dateTime="2017-12-21T15:04:51"/>
 </users>
 </file>
 
@@ -10740,13 +11299,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y98"/>
+  <dimension ref="A1:Y97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C34" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C19" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D46" sqref="D46"/>
+      <selection pane="bottomRight" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -10783,40 +11342,40 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="76" t="s">
+      <c r="C1" s="71" t="s">
         <v>149</v>
       </c>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-      <c r="L1" s="77"/>
-      <c r="M1" s="77"/>
-      <c r="N1" s="77"/>
-      <c r="O1" s="77"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="72"/>
+      <c r="M1" s="72"/>
+      <c r="N1" s="72"/>
+      <c r="O1" s="72"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="78" t="s">
+      <c r="C2" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="79"/>
-      <c r="K2" s="79"/>
-      <c r="L2" s="79"/>
-      <c r="M2" s="79"/>
-      <c r="N2" s="79"/>
-      <c r="O2" s="79"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+      <c r="M2" s="74"/>
+      <c r="N2" s="74"/>
+      <c r="O2" s="74"/>
     </row>
     <row r="3" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
@@ -10839,34 +11398,34 @@
     <row r="5" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="30"/>
       <c r="B5" s="30"/>
-      <c r="C5" s="74" t="s">
+      <c r="C5" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="75"/>
-      <c r="E5" s="75"/>
-      <c r="F5" s="75"/>
-      <c r="G5" s="75"/>
-      <c r="H5" s="75"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="70"/>
       <c r="I5" s="30"/>
       <c r="J5" s="30"/>
-      <c r="K5" s="74" t="s">
+      <c r="K5" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="L5" s="75"/>
-      <c r="M5" s="75"/>
-      <c r="N5" s="75"/>
-      <c r="O5" s="75"/>
+      <c r="L5" s="70"/>
+      <c r="M5" s="70"/>
+      <c r="N5" s="70"/>
+      <c r="O5" s="70"/>
       <c r="P5" s="30"/>
       <c r="Q5" s="30"/>
-      <c r="R5" s="74" t="s">
+      <c r="R5" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="S5" s="75"/>
-      <c r="T5" s="75"/>
-      <c r="U5" s="75"/>
-      <c r="V5" s="75"/>
-      <c r="W5" s="75"/>
-      <c r="X5" s="75"/>
+      <c r="S5" s="70"/>
+      <c r="T5" s="70"/>
+      <c r="U5" s="70"/>
+      <c r="V5" s="70"/>
+      <c r="W5" s="70"/>
+      <c r="X5" s="70"/>
       <c r="Y5" s="31" t="s">
         <v>13</v>
       </c>
@@ -13234,49 +13793,51 @@
         <v>197</v>
       </c>
     </row>
-    <row r="45" spans="1:25" s="63" customFormat="1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A45" s="39" t="s">
+    <row r="45" spans="1:25" s="66" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A45" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B45" s="64" t="s">
-        <v>225</v>
-      </c>
-      <c r="C45" s="65"/>
-      <c r="D45" s="66" t="s">
-        <v>124</v>
-      </c>
-      <c r="E45" s="66"/>
-      <c r="F45" s="65"/>
-      <c r="G45" s="65"/>
-      <c r="H45" s="65"/>
-      <c r="I45" s="65"/>
-      <c r="J45" s="66"/>
-      <c r="K45" s="66"/>
-      <c r="L45" s="66"/>
-      <c r="M45" s="65"/>
-      <c r="N45" s="65"/>
+      <c r="B45" s="60" t="s">
+        <v>226</v>
+      </c>
+      <c r="C45" s="61"/>
+      <c r="D45" s="61" t="s">
+        <v>125</v>
+      </c>
+      <c r="E45" s="61"/>
+      <c r="F45" s="61"/>
+      <c r="G45" s="61"/>
+      <c r="H45" s="61"/>
+      <c r="I45" s="61"/>
+      <c r="J45" s="61"/>
+      <c r="K45" s="61"/>
+      <c r="L45" s="61"/>
+      <c r="M45" s="61"/>
+      <c r="N45" s="61"/>
       <c r="O45" s="61"/>
       <c r="P45" s="61"/>
-      <c r="Q45" s="65"/>
-      <c r="R45" s="66"/>
-      <c r="S45" s="67"/>
-      <c r="T45" s="65"/>
-      <c r="U45" s="65"/>
+      <c r="Q45" s="61"/>
+      <c r="R45" s="61"/>
+      <c r="S45" s="61"/>
+      <c r="T45" s="61"/>
+      <c r="U45" s="61"/>
       <c r="V45" s="61"/>
-      <c r="W45" s="65"/>
-      <c r="X45" s="65"/>
-      <c r="Y45" s="55"/>
+      <c r="W45" s="61"/>
+      <c r="X45" s="61"/>
+      <c r="Y45" s="65" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="46" spans="1:25" s="71" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:25" s="57" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A46" s="35" t="s">
         <v>14</v>
       </c>
       <c r="B46" s="60" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="C46" s="61"/>
       <c r="D46" s="61" t="s">
-        <v>125</v>
+        <v>224</v>
       </c>
       <c r="E46" s="61"/>
       <c r="F46" s="61"/>
@@ -13298,190 +13859,196 @@
       <c r="V46" s="61"/>
       <c r="W46" s="61"/>
       <c r="X46" s="61"/>
-      <c r="Y46" s="70" t="s">
-        <v>228</v>
-      </c>
+      <c r="Y46" s="56"/>
     </row>
-    <row r="47" spans="1:25" s="57" customFormat="1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A47" s="35" t="s">
+    <row r="47" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="B47" s="60" t="s">
-        <v>212</v>
-      </c>
-      <c r="C47" s="61"/>
-      <c r="D47" s="61" t="s">
-        <v>224</v>
-      </c>
-      <c r="E47" s="61"/>
-      <c r="F47" s="61"/>
-      <c r="G47" s="61"/>
-      <c r="H47" s="61"/>
-      <c r="I47" s="61"/>
-      <c r="J47" s="61"/>
-      <c r="K47" s="61"/>
-      <c r="L47" s="61"/>
-      <c r="M47" s="61"/>
-      <c r="N47" s="61"/>
-      <c r="O47" s="61"/>
-      <c r="P47" s="61"/>
-      <c r="Q47" s="61"/>
-      <c r="R47" s="61"/>
-      <c r="S47" s="61"/>
-      <c r="T47" s="61"/>
-      <c r="U47" s="61"/>
-      <c r="V47" s="61"/>
-      <c r="W47" s="61"/>
-      <c r="X47" s="61"/>
-      <c r="Y47" s="56"/>
+      <c r="B47" s="58" t="s">
+        <v>208</v>
+      </c>
+      <c r="D47" s="59" t="s">
+        <v>124</v>
+      </c>
     </row>
-    <row r="48" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="58" t="s">
+    <row r="48" spans="1:25" s="57" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B48" s="58" t="s">
-        <v>208</v>
-      </c>
-      <c r="D48" s="59" t="s">
+      <c r="B48" s="60" t="s">
+        <v>213</v>
+      </c>
+      <c r="C48" s="61"/>
+      <c r="D48" s="61" t="s">
+        <v>223</v>
+      </c>
+      <c r="E48" s="61"/>
+      <c r="F48" s="61"/>
+      <c r="G48" s="61"/>
+      <c r="H48" s="61"/>
+      <c r="I48" s="61"/>
+      <c r="J48" s="61"/>
+      <c r="K48" s="61"/>
+      <c r="L48" s="61"/>
+      <c r="M48" s="61"/>
+      <c r="N48" s="61"/>
+      <c r="O48" s="61"/>
+      <c r="P48" s="61"/>
+      <c r="Q48" s="61"/>
+      <c r="R48" s="61"/>
+      <c r="S48" s="61"/>
+      <c r="T48" s="61"/>
+      <c r="U48" s="61"/>
+      <c r="V48" s="61"/>
+      <c r="W48" s="61"/>
+      <c r="X48" s="61"/>
+      <c r="Y48" s="55"/>
+    </row>
+    <row r="49" spans="1:25" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B49" s="39" t="s">
+        <v>183</v>
+      </c>
+      <c r="C49" s="37"/>
+      <c r="D49" s="36" t="s">
         <v>124</v>
       </c>
+      <c r="E49" s="36"/>
+      <c r="F49" s="37"/>
+      <c r="G49" s="37"/>
+      <c r="H49" s="37"/>
+      <c r="I49" s="37"/>
+      <c r="J49" s="37"/>
+      <c r="K49" s="36"/>
+      <c r="L49" s="37"/>
+      <c r="M49" s="37"/>
+      <c r="N49" s="37"/>
+      <c r="O49" s="36"/>
+      <c r="P49" s="36"/>
+      <c r="Q49" s="37"/>
+      <c r="R49" s="37"/>
+      <c r="S49" s="37"/>
+      <c r="T49" s="37"/>
+      <c r="U49" s="37"/>
+      <c r="V49" s="36"/>
+      <c r="W49" s="37"/>
+      <c r="X49" s="37"/>
+      <c r="Y49" s="38"/>
     </row>
-    <row r="49" spans="1:25" s="57" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="B49" s="60" t="s">
-        <v>213</v>
-      </c>
-      <c r="C49" s="61"/>
-      <c r="D49" s="61" t="s">
-        <v>223</v>
-      </c>
-      <c r="E49" s="61"/>
-      <c r="F49" s="61"/>
-      <c r="G49" s="61"/>
-      <c r="H49" s="61"/>
-      <c r="I49" s="61"/>
-      <c r="J49" s="61"/>
-      <c r="K49" s="61"/>
-      <c r="L49" s="61"/>
-      <c r="M49" s="61"/>
-      <c r="N49" s="61"/>
-      <c r="O49" s="61"/>
-      <c r="P49" s="61"/>
-      <c r="Q49" s="61"/>
-      <c r="R49" s="61"/>
-      <c r="S49" s="61"/>
-      <c r="T49" s="61"/>
-      <c r="U49" s="61"/>
-      <c r="V49" s="61"/>
-      <c r="W49" s="61"/>
-      <c r="X49" s="61"/>
-      <c r="Y49" s="55"/>
-    </row>
-    <row r="50" spans="1:25" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:25" s="26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="39" t="s">
         <v>14</v>
       </c>
       <c r="B50" s="39" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C50" s="37"/>
       <c r="D50" s="36" t="s">
-        <v>124</v>
-      </c>
-      <c r="E50" s="36"/>
-      <c r="F50" s="37"/>
+        <v>187</v>
+      </c>
+      <c r="E50" s="30" t="s">
+        <v>189</v>
+      </c>
+      <c r="F50" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="G50" s="37"/>
-      <c r="H50" s="37"/>
+      <c r="H50" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="I50" s="37"/>
-      <c r="J50" s="37"/>
+      <c r="J50" s="37" t="s">
+        <v>188</v>
+      </c>
       <c r="K50" s="36"/>
-      <c r="L50" s="37"/>
+      <c r="L50" s="36"/>
       <c r="M50" s="37"/>
       <c r="N50" s="37"/>
       <c r="O50" s="36"/>
       <c r="P50" s="36"/>
       <c r="Q50" s="37"/>
-      <c r="R50" s="37"/>
-      <c r="S50" s="37"/>
-      <c r="T50" s="37"/>
-      <c r="U50" s="37"/>
-      <c r="V50" s="36"/>
+      <c r="R50" s="37" t="s">
+        <v>205</v>
+      </c>
+      <c r="S50" s="37" t="s">
+        <v>206</v>
+      </c>
+      <c r="T50" s="37" t="s">
+        <v>205</v>
+      </c>
+      <c r="U50" s="37" t="s">
+        <v>206</v>
+      </c>
+      <c r="V50" s="36" t="s">
+        <v>205</v>
+      </c>
       <c r="W50" s="37"/>
       <c r="X50" s="37"/>
-      <c r="Y50" s="38"/>
+      <c r="Y50" s="38" t="s">
+        <v>193</v>
+      </c>
     </row>
-    <row r="51" spans="1:25" s="26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:25" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="39" t="s">
         <v>14</v>
       </c>
       <c r="B51" s="39" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C51" s="37"/>
       <c r="D51" s="36" t="s">
-        <v>187</v>
-      </c>
-      <c r="E51" s="30" t="s">
-        <v>189</v>
-      </c>
-      <c r="F51" s="37" t="s">
-        <v>125</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="E51" s="36"/>
+      <c r="F51" s="37"/>
       <c r="G51" s="37"/>
-      <c r="H51" s="37" t="s">
-        <v>125</v>
-      </c>
+      <c r="H51" s="37"/>
       <c r="I51" s="37"/>
-      <c r="J51" s="37" t="s">
-        <v>188</v>
-      </c>
+      <c r="J51" s="37"/>
       <c r="K51" s="36"/>
-      <c r="L51" s="36"/>
+      <c r="L51" s="37"/>
       <c r="M51" s="37"/>
       <c r="N51" s="37"/>
       <c r="O51" s="36"/>
       <c r="P51" s="36"/>
       <c r="Q51" s="37"/>
-      <c r="R51" s="37" t="s">
-        <v>205</v>
-      </c>
-      <c r="S51" s="37" t="s">
-        <v>206</v>
-      </c>
-      <c r="T51" s="37" t="s">
-        <v>205</v>
-      </c>
-      <c r="U51" s="37" t="s">
-        <v>206</v>
-      </c>
-      <c r="V51" s="36" t="s">
-        <v>205</v>
-      </c>
+      <c r="R51" s="37"/>
+      <c r="S51" s="37"/>
+      <c r="T51" s="37"/>
+      <c r="U51" s="37"/>
+      <c r="V51" s="36"/>
       <c r="W51" s="37"/>
       <c r="X51" s="37"/>
-      <c r="Y51" s="38" t="s">
-        <v>193</v>
-      </c>
+      <c r="Y51" s="38"/>
     </row>
-    <row r="52" spans="1:25" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:25" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="39" t="s">
         <v>14</v>
       </c>
       <c r="B52" s="39" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C52" s="37"/>
       <c r="D52" s="36" t="s">
         <v>124</v>
       </c>
-      <c r="E52" s="36"/>
-      <c r="F52" s="37"/>
+      <c r="E52" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="F52" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="G52" s="37"/>
-      <c r="H52" s="37"/>
+      <c r="H52" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="I52" s="37"/>
-      <c r="J52" s="37"/>
+      <c r="J52" s="37" t="s">
+        <v>111</v>
+      </c>
       <c r="K52" s="36"/>
       <c r="L52" s="37"/>
       <c r="M52" s="37"/>
@@ -13489,72 +14056,84 @@
       <c r="O52" s="36"/>
       <c r="P52" s="36"/>
       <c r="Q52" s="37"/>
-      <c r="R52" s="37"/>
-      <c r="S52" s="37"/>
-      <c r="T52" s="37"/>
-      <c r="U52" s="37"/>
-      <c r="V52" s="36"/>
+      <c r="R52" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="S52" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="T52" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="U52" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="V52" s="36" t="s">
+        <v>129</v>
+      </c>
       <c r="W52" s="37"/>
       <c r="X52" s="37"/>
       <c r="Y52" s="38"/>
     </row>
-    <row r="53" spans="1:25" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:25" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="39" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="B53" s="39" t="s">
-        <v>185</v>
+        <v>121</v>
       </c>
       <c r="C53" s="37"/>
       <c r="D53" s="36" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E53" s="36" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F53" s="37" t="s">
         <v>125</v>
       </c>
       <c r="G53" s="37"/>
-      <c r="H53" s="37" t="s">
-        <v>125</v>
-      </c>
+      <c r="H53" s="37"/>
       <c r="I53" s="37"/>
       <c r="J53" s="37" t="s">
-        <v>111</v>
-      </c>
-      <c r="K53" s="36"/>
-      <c r="L53" s="37"/>
+        <v>16</v>
+      </c>
+      <c r="K53" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="L53" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="M53" s="37"/>
-      <c r="N53" s="37"/>
-      <c r="O53" s="36"/>
-      <c r="P53" s="36"/>
-      <c r="Q53" s="37"/>
+      <c r="N53" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="O53" s="37"/>
+      <c r="P53" s="37"/>
+      <c r="Q53" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="R53" s="37" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="S53" s="37" t="s">
-        <v>111</v>
-      </c>
-      <c r="T53" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="U53" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="V53" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="T53" s="37"/>
+      <c r="U53" s="37"/>
+      <c r="V53" s="37" t="s">
         <v>129</v>
       </c>
       <c r="W53" s="37"/>
       <c r="X53" s="37"/>
       <c r="Y53" s="38"/>
     </row>
-    <row r="54" spans="1:25" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:25" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B54" s="39" t="s">
-        <v>121</v>
+        <v>201</v>
       </c>
       <c r="C54" s="37"/>
       <c r="D54" s="36" t="s">
@@ -13575,18 +14154,12 @@
       <c r="K54" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="L54" s="37" t="s">
-        <v>125</v>
-      </c>
+      <c r="L54" s="37"/>
       <c r="M54" s="37"/>
-      <c r="N54" s="37" t="s">
-        <v>125</v>
-      </c>
+      <c r="N54" s="37"/>
       <c r="O54" s="37"/>
       <c r="P54" s="37"/>
-      <c r="Q54" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="Q54" s="37"/>
       <c r="R54" s="37" t="s">
         <v>129</v>
       </c>
@@ -13602,12 +14175,12 @@
       <c r="X54" s="37"/>
       <c r="Y54" s="38"/>
     </row>
-    <row r="55" spans="1:25" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:25" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B55" s="39" t="s">
-        <v>201</v>
+        <v>170</v>
       </c>
       <c r="C55" s="37"/>
       <c r="D55" s="36" t="s">
@@ -13628,12 +14201,18 @@
       <c r="K55" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="L55" s="37"/>
+      <c r="L55" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="M55" s="37"/>
-      <c r="N55" s="37"/>
+      <c r="N55" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="O55" s="37"/>
       <c r="P55" s="37"/>
-      <c r="Q55" s="37"/>
+      <c r="Q55" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="R55" s="37" t="s">
         <v>129</v>
       </c>
@@ -13649,24 +14228,26 @@
       <c r="X55" s="37"/>
       <c r="Y55" s="38"/>
     </row>
-    <row r="56" spans="1:25" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B56" s="39" t="s">
-        <v>170</v>
+        <v>43</v>
       </c>
       <c r="C56" s="37"/>
-      <c r="D56" s="36" t="s">
-        <v>125</v>
-      </c>
-      <c r="E56" s="36" t="s">
+      <c r="D56" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="E56" s="37" t="s">
         <v>125</v>
       </c>
       <c r="F56" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="G56" s="37"/>
+      <c r="G56" s="37" t="s">
+        <v>18</v>
+      </c>
       <c r="H56" s="37"/>
       <c r="I56" s="37"/>
       <c r="J56" s="37" t="s">
@@ -13707,7 +14288,7 @@
         <v>42</v>
       </c>
       <c r="B57" s="39" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C57" s="37"/>
       <c r="D57" s="37" t="s">
@@ -13720,10 +14301,14 @@
         <v>125</v>
       </c>
       <c r="G57" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="H57" s="37"/>
-      <c r="I57" s="37"/>
+        <v>125</v>
+      </c>
+      <c r="H57" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="I57" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="J57" s="37" t="s">
         <v>16</v>
       </c>
@@ -13733,12 +14318,18 @@
       <c r="L57" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="M57" s="37"/>
+      <c r="M57" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="N57" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="O57" s="37"/>
-      <c r="P57" s="37"/>
+      <c r="O57" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="P57" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="Q57" s="37" t="s">
         <v>16</v>
       </c>
@@ -13748,21 +14339,27 @@
       <c r="S57" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="T57" s="37"/>
-      <c r="U57" s="37"/>
+      <c r="T57" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="U57" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="V57" s="37" t="s">
         <v>129</v>
       </c>
       <c r="W57" s="37"/>
-      <c r="X57" s="37"/>
+      <c r="X57" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="Y57" s="38"/>
     </row>
-    <row r="58" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:25" s="17" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B58" s="39" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C58" s="37"/>
       <c r="D58" s="37" t="s">
@@ -13822,18 +14419,20 @@
       <c r="V58" s="37" t="s">
         <v>129</v>
       </c>
-      <c r="W58" s="37"/>
+      <c r="W58" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="X58" s="37" t="s">
         <v>16</v>
       </c>
       <c r="Y58" s="38"/>
     </row>
-    <row r="59" spans="1:25" s="17" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B59" s="39" t="s">
-        <v>45</v>
+        <v>146</v>
       </c>
       <c r="C59" s="37"/>
       <c r="D59" s="37" t="s">
@@ -13893,9 +14492,7 @@
       <c r="V59" s="37" t="s">
         <v>129</v>
       </c>
-      <c r="W59" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="W59" s="37"/>
       <c r="X59" s="37" t="s">
         <v>16</v>
       </c>
@@ -13906,7 +14503,7 @@
         <v>42</v>
       </c>
       <c r="B60" s="39" t="s">
-        <v>146</v>
+        <v>46</v>
       </c>
       <c r="C60" s="37"/>
       <c r="D60" s="37" t="s">
@@ -13977,7 +14574,7 @@
         <v>42</v>
       </c>
       <c r="B61" s="39" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C61" s="37"/>
       <c r="D61" s="37" t="s">
@@ -14043,12 +14640,12 @@
       </c>
       <c r="Y61" s="38"/>
     </row>
-    <row r="62" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:25" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B62" s="39" t="s">
-        <v>47</v>
+        <v>153</v>
       </c>
       <c r="C62" s="37"/>
       <c r="D62" s="37" t="s">
@@ -14114,12 +14711,12 @@
       </c>
       <c r="Y62" s="38"/>
     </row>
-    <row r="63" spans="1:25" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B63" s="39" t="s">
-        <v>153</v>
+        <v>48</v>
       </c>
       <c r="C63" s="37"/>
       <c r="D63" s="37" t="s">
@@ -14190,7 +14787,7 @@
         <v>42</v>
       </c>
       <c r="B64" s="39" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C64" s="37"/>
       <c r="D64" s="37" t="s">
@@ -14226,9 +14823,7 @@
       <c r="N64" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="O64" s="37" t="s">
-        <v>125</v>
-      </c>
+      <c r="O64" s="37"/>
       <c r="P64" s="37" t="s">
         <v>125</v>
       </c>
@@ -14261,7 +14856,7 @@
         <v>42</v>
       </c>
       <c r="B65" s="39" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C65" s="37"/>
       <c r="D65" s="37" t="s">
@@ -14297,7 +14892,9 @@
       <c r="N65" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="O65" s="37"/>
+      <c r="O65" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="P65" s="37" t="s">
         <v>125</v>
       </c>
@@ -14330,7 +14927,7 @@
         <v>42</v>
       </c>
       <c r="B66" s="39" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C66" s="37"/>
       <c r="D66" s="37" t="s">
@@ -14342,12 +14939,8 @@
       <c r="F66" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="G66" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="H66" s="37" t="s">
-        <v>125</v>
-      </c>
+      <c r="G66" s="37"/>
+      <c r="H66" s="37"/>
       <c r="I66" s="37" t="s">
         <v>125</v>
       </c>
@@ -14360,15 +14953,11 @@
       <c r="L66" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="M66" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="M66" s="37"/>
       <c r="N66" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="O66" s="37" t="s">
-        <v>125</v>
-      </c>
+      <c r="O66" s="37"/>
       <c r="P66" s="37" t="s">
         <v>125</v>
       </c>
@@ -14401,7 +14990,7 @@
         <v>42</v>
       </c>
       <c r="B67" s="39" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C67" s="37"/>
       <c r="D67" s="37" t="s">
@@ -14414,10 +15003,10 @@
         <v>125</v>
       </c>
       <c r="G67" s="37"/>
-      <c r="H67" s="37"/>
-      <c r="I67" s="37" t="s">
-        <v>125</v>
-      </c>
+      <c r="H67" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="I67" s="37"/>
       <c r="J67" s="37" t="s">
         <v>16</v>
       </c>
@@ -14431,10 +15020,10 @@
       <c r="N67" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="O67" s="37"/>
-      <c r="P67" s="37" t="s">
-        <v>125</v>
-      </c>
+      <c r="O67" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="P67" s="37"/>
       <c r="Q67" s="37" t="s">
         <v>16</v>
       </c>
@@ -14444,19 +15033,13 @@
       <c r="S67" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="T67" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="U67" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="T67" s="37"/>
+      <c r="U67" s="37"/>
       <c r="V67" s="37" t="s">
         <v>129</v>
       </c>
       <c r="W67" s="37"/>
-      <c r="X67" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="X67" s="37"/>
       <c r="Y67" s="38"/>
     </row>
     <row r="68" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -14464,7 +15047,7 @@
         <v>42</v>
       </c>
       <c r="B68" s="39" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C68" s="37"/>
       <c r="D68" s="37" t="s">
@@ -14477,9 +15060,7 @@
         <v>125</v>
       </c>
       <c r="G68" s="37"/>
-      <c r="H68" s="37" t="s">
-        <v>18</v>
-      </c>
+      <c r="H68" s="37"/>
       <c r="I68" s="37"/>
       <c r="J68" s="37" t="s">
         <v>16</v>
@@ -14494,9 +15075,7 @@
       <c r="N68" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="O68" s="37" t="s">
-        <v>18</v>
-      </c>
+      <c r="O68" s="37"/>
       <c r="P68" s="37"/>
       <c r="Q68" s="37" t="s">
         <v>16</v>
@@ -14521,7 +15100,7 @@
         <v>42</v>
       </c>
       <c r="B69" s="39" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C69" s="37"/>
       <c r="D69" s="37" t="s">
@@ -14574,7 +15153,7 @@
         <v>42</v>
       </c>
       <c r="B70" s="39" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C70" s="37"/>
       <c r="D70" s="37" t="s">
@@ -14622,12 +15201,12 @@
       <c r="X70" s="37"/>
       <c r="Y70" s="38"/>
     </row>
-    <row r="71" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:25" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B71" s="39" t="s">
-        <v>55</v>
+        <v>119</v>
       </c>
       <c r="C71" s="37"/>
       <c r="D71" s="37" t="s">
@@ -14639,9 +15218,15 @@
       <c r="F71" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="G71" s="37"/>
-      <c r="H71" s="37"/>
-      <c r="I71" s="37"/>
+      <c r="G71" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="H71" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="I71" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="J71" s="37" t="s">
         <v>16</v>
       </c>
@@ -14651,12 +15236,16 @@
       <c r="L71" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="M71" s="37"/>
+      <c r="M71" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="N71" s="37" t="s">
         <v>125</v>
       </c>
       <c r="O71" s="37"/>
-      <c r="P71" s="37"/>
+      <c r="P71" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="Q71" s="37" t="s">
         <v>16</v>
       </c>
@@ -14666,21 +15255,27 @@
       <c r="S71" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="T71" s="37"/>
-      <c r="U71" s="37"/>
+      <c r="T71" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="U71" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="V71" s="37" t="s">
         <v>129</v>
       </c>
       <c r="W71" s="37"/>
-      <c r="X71" s="37"/>
+      <c r="X71" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="Y71" s="38"/>
     </row>
-    <row r="72" spans="1:25" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:25" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B72" s="39" t="s">
-        <v>119</v>
+        <v>171</v>
       </c>
       <c r="C72" s="37"/>
       <c r="D72" s="37" t="s">
@@ -14744,12 +15339,12 @@
       </c>
       <c r="Y72" s="38"/>
     </row>
-    <row r="73" spans="1:25" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B73" s="39" t="s">
-        <v>171</v>
+        <v>56</v>
       </c>
       <c r="C73" s="37"/>
       <c r="D73" s="37" t="s">
@@ -14785,7 +15380,9 @@
       <c r="N73" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="O73" s="37"/>
+      <c r="O73" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="P73" s="37" t="s">
         <v>125</v>
       </c>
@@ -14813,12 +15410,12 @@
       </c>
       <c r="Y73" s="38"/>
     </row>
-    <row r="74" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:25" s="17" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B74" s="39" t="s">
-        <v>56</v>
+        <v>123</v>
       </c>
       <c r="C74" s="37"/>
       <c r="D74" s="37" t="s">
@@ -14879,9 +15476,7 @@
         <v>129</v>
       </c>
       <c r="W74" s="37"/>
-      <c r="X74" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="X74" s="37"/>
       <c r="Y74" s="38"/>
     </row>
     <row r="75" spans="1:25" s="17" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -14889,7 +15484,7 @@
         <v>42</v>
       </c>
       <c r="B75" s="39" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="C75" s="37"/>
       <c r="D75" s="37" t="s">
@@ -14958,7 +15553,7 @@
         <v>42</v>
       </c>
       <c r="B76" s="39" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C76" s="37"/>
       <c r="D76" s="37" t="s">
@@ -15027,7 +15622,7 @@
         <v>42</v>
       </c>
       <c r="B77" s="39" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C77" s="37"/>
       <c r="D77" s="37" t="s">
@@ -15096,7 +15691,7 @@
         <v>42</v>
       </c>
       <c r="B78" s="39" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C78" s="37"/>
       <c r="D78" s="37" t="s">
@@ -15160,32 +15755,26 @@
       <c r="X78" s="37"/>
       <c r="Y78" s="38"/>
     </row>
-    <row r="79" spans="1:25" s="17" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:25" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B79" s="39" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C79" s="37"/>
-      <c r="D79" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="E79" s="37" t="s">
+      <c r="D79" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="E79" s="36" t="s">
         <v>125</v>
       </c>
       <c r="F79" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="G79" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="H79" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="I79" s="37" t="s">
-        <v>125</v>
-      </c>
+      <c r="G79" s="37"/>
+      <c r="H79" s="37"/>
+      <c r="I79" s="37"/>
       <c r="J79" s="37" t="s">
         <v>16</v>
       </c>
@@ -15195,18 +15784,12 @@
       <c r="L79" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="M79" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="M79" s="37"/>
       <c r="N79" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="O79" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="P79" s="37" t="s">
-        <v>125</v>
-      </c>
+      <c r="O79" s="37"/>
+      <c r="P79" s="37"/>
       <c r="Q79" s="37" t="s">
         <v>16</v>
       </c>
@@ -15216,39 +15799,39 @@
       <c r="S79" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="T79" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="U79" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="V79" s="37" t="s">
-        <v>129</v>
-      </c>
+      <c r="T79" s="37"/>
+      <c r="U79" s="37"/>
+      <c r="V79" s="37"/>
       <c r="W79" s="37"/>
       <c r="X79" s="37"/>
       <c r="Y79" s="38"/>
     </row>
-    <row r="80" spans="1:25" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:25" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B80" s="39" t="s">
-        <v>145</v>
+        <v>186</v>
       </c>
       <c r="C80" s="37"/>
-      <c r="D80" s="36" t="s">
-        <v>125</v>
-      </c>
-      <c r="E80" s="36" t="s">
+      <c r="D80" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="E80" s="37" t="s">
         <v>125</v>
       </c>
       <c r="F80" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="G80" s="37"/>
-      <c r="H80" s="37"/>
-      <c r="I80" s="37"/>
+      <c r="G80" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="H80" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="I80" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="J80" s="37" t="s">
         <v>16</v>
       </c>
@@ -15258,12 +15841,18 @@
       <c r="L80" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="M80" s="37"/>
+      <c r="M80" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="N80" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="O80" s="37"/>
-      <c r="P80" s="37"/>
+      <c r="O80" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="P80" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="Q80" s="37" t="s">
         <v>16</v>
       </c>
@@ -15273,19 +15862,25 @@
       <c r="S80" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="T80" s="37"/>
-      <c r="U80" s="37"/>
-      <c r="V80" s="37"/>
+      <c r="T80" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="U80" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="V80" s="37" t="s">
+        <v>129</v>
+      </c>
       <c r="W80" s="37"/>
       <c r="X80" s="37"/>
       <c r="Y80" s="38"/>
     </row>
-    <row r="81" spans="1:25" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A81" s="39" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="B81" s="39" t="s">
-        <v>186</v>
+        <v>58</v>
       </c>
       <c r="C81" s="37"/>
       <c r="D81" s="37" t="s">
@@ -15307,7 +15902,7 @@
         <v>125</v>
       </c>
       <c r="J81" s="37" t="s">
-        <v>16</v>
+        <v>214</v>
       </c>
       <c r="K81" s="37" t="s">
         <v>125</v>
@@ -15328,13 +15923,13 @@
         <v>125</v>
       </c>
       <c r="Q81" s="37" t="s">
-        <v>16</v>
+        <v>214</v>
       </c>
       <c r="R81" s="37" t="s">
-        <v>129</v>
+        <v>215</v>
       </c>
       <c r="S81" s="37" t="s">
-        <v>16</v>
+        <v>214</v>
       </c>
       <c r="T81" s="37" t="s">
         <v>129</v>
@@ -15345,16 +15940,22 @@
       <c r="V81" s="37" t="s">
         <v>129</v>
       </c>
-      <c r="W81" s="37"/>
-      <c r="X81" s="37"/>
-      <c r="Y81" s="38"/>
+      <c r="W81" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="X81" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y81" s="67" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="82" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A82" s="39" t="s">
         <v>57</v>
       </c>
       <c r="B82" s="39" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C82" s="37"/>
       <c r="D82" s="37" t="s">
@@ -15420,22 +16021,20 @@
       <c r="X82" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="Y82" s="72" t="s">
-        <v>216</v>
-      </c>
+      <c r="Y82" s="68"/>
     </row>
     <row r="83" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83" s="39" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B83" s="39" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C83" s="37"/>
       <c r="D83" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="E83" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="E83" s="36" t="s">
         <v>125</v>
       </c>
       <c r="F83" s="37" t="s">
@@ -15451,10 +16050,10 @@
         <v>125</v>
       </c>
       <c r="J83" s="37" t="s">
-        <v>214</v>
+        <v>16</v>
       </c>
       <c r="K83" s="37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L83" s="37" t="s">
         <v>125</v>
@@ -15472,173 +16071,133 @@
         <v>125</v>
       </c>
       <c r="Q83" s="37" t="s">
-        <v>214</v>
+        <v>16</v>
       </c>
       <c r="R83" s="37" t="s">
-        <v>215</v>
+        <v>130</v>
       </c>
       <c r="S83" s="37" t="s">
-        <v>214</v>
+        <v>111</v>
       </c>
       <c r="T83" s="37" t="s">
         <v>129</v>
       </c>
       <c r="U83" s="37" t="s">
-        <v>16</v>
+        <v>111</v>
       </c>
       <c r="V83" s="37" t="s">
         <v>129</v>
       </c>
       <c r="W83" s="37" t="s">
-        <v>16</v>
+        <v>111</v>
       </c>
       <c r="X83" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y83" s="73"/>
+        <v>111</v>
+      </c>
+      <c r="Y83" s="38"/>
     </row>
-    <row r="84" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A84" s="39" t="s">
-        <v>60</v>
-      </c>
-      <c r="B84" s="39" t="s">
-        <v>60</v>
-      </c>
-      <c r="C84" s="37"/>
+    <row r="84" spans="1:25" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A84" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="B84" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="C84" s="43"/>
       <c r="D84" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="E84" s="36" t="s">
-        <v>125</v>
-      </c>
-      <c r="F84" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="G84" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="H84" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="I84" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="J84" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="K84" s="37" t="s">
-        <v>124</v>
-      </c>
-      <c r="L84" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="M84" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="N84" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="O84" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="P84" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="Q84" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="R84" s="37" t="s">
-        <v>130</v>
-      </c>
-      <c r="S84" s="37" t="s">
-        <v>111</v>
-      </c>
-      <c r="T84" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="U84" s="37" t="s">
-        <v>111</v>
-      </c>
-      <c r="V84" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="W84" s="37" t="s">
-        <v>111</v>
-      </c>
-      <c r="X84" s="37" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y84" s="38"/>
+      <c r="E84" s="43"/>
+      <c r="F84" s="43"/>
+      <c r="G84" s="43"/>
+      <c r="H84" s="43"/>
+      <c r="I84" s="43"/>
+      <c r="J84" s="43"/>
+      <c r="K84" s="43"/>
+      <c r="L84" s="43"/>
+      <c r="M84" s="43"/>
+      <c r="N84" s="43"/>
+      <c r="O84" s="43"/>
+      <c r="P84" s="43"/>
+      <c r="Q84" s="43"/>
+      <c r="R84" s="43"/>
+      <c r="S84" s="43"/>
+      <c r="T84" s="43"/>
+      <c r="U84" s="43"/>
+      <c r="V84" s="43"/>
+      <c r="W84" s="43"/>
+      <c r="X84" s="43"/>
+      <c r="Y84" s="44" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="85" spans="1:25" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A85" s="42" t="s">
+    <row r="85" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A85" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="B85" s="42" t="s">
-        <v>62</v>
-      </c>
-      <c r="C85" s="43"/>
+      <c r="B85" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C85" s="36"/>
       <c r="D85" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="E85" s="43"/>
-      <c r="F85" s="43"/>
-      <c r="G85" s="43"/>
-      <c r="H85" s="43"/>
-      <c r="I85" s="43"/>
-      <c r="J85" s="43"/>
-      <c r="K85" s="43"/>
-      <c r="L85" s="43"/>
-      <c r="M85" s="43"/>
-      <c r="N85" s="43"/>
-      <c r="O85" s="43"/>
-      <c r="P85" s="43"/>
-      <c r="Q85" s="43"/>
-      <c r="R85" s="43"/>
-      <c r="S85" s="43"/>
-      <c r="T85" s="43"/>
-      <c r="U85" s="43"/>
-      <c r="V85" s="43"/>
-      <c r="W85" s="43"/>
-      <c r="X85" s="43"/>
-      <c r="Y85" s="44" t="s">
-        <v>63</v>
-      </c>
+      <c r="E85" s="36"/>
+      <c r="F85" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="G85" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="H85" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="I85" s="36"/>
+      <c r="J85" s="37"/>
+      <c r="K85" s="36"/>
+      <c r="L85" s="36"/>
+      <c r="M85" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="N85" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="O85" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="P85" s="36"/>
+      <c r="Q85" s="37"/>
+      <c r="R85" s="36"/>
+      <c r="S85" s="36"/>
+      <c r="T85" s="36"/>
+      <c r="U85" s="36"/>
+      <c r="V85" s="36"/>
+      <c r="W85" s="36"/>
+      <c r="X85" s="36"/>
+      <c r="Y85" s="30"/>
     </row>
     <row r="86" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A86" s="35" t="s">
         <v>61</v>
       </c>
       <c r="B86" s="35" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C86" s="36"/>
       <c r="D86" s="37" t="s">
         <v>124</v>
       </c>
       <c r="E86" s="36"/>
-      <c r="F86" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="G86" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="H86" s="36" t="s">
-        <v>18</v>
-      </c>
+      <c r="F86" s="36"/>
+      <c r="G86" s="36"/>
+      <c r="H86" s="36"/>
       <c r="I86" s="36"/>
       <c r="J86" s="37"/>
       <c r="K86" s="36"/>
       <c r="L86" s="36"/>
-      <c r="M86" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="N86" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="O86" s="36" t="s">
-        <v>18</v>
-      </c>
+      <c r="M86" s="36"/>
+      <c r="N86" s="36"/>
+      <c r="O86" s="36"/>
       <c r="P86" s="36"/>
       <c r="Q86" s="37"/>
       <c r="R86" s="36"/>
@@ -15655,7 +16214,7 @@
         <v>61</v>
       </c>
       <c r="B87" s="35" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C87" s="36"/>
       <c r="D87" s="37" t="s">
@@ -15688,7 +16247,7 @@
         <v>61</v>
       </c>
       <c r="B88" s="35" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C88" s="36"/>
       <c r="D88" s="37" t="s">
@@ -15716,12 +16275,12 @@
       <c r="X88" s="36"/>
       <c r="Y88" s="30"/>
     </row>
-    <row r="89" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:25" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A89" s="35" t="s">
         <v>61</v>
       </c>
       <c r="B89" s="35" t="s">
-        <v>67</v>
+        <v>164</v>
       </c>
       <c r="C89" s="36"/>
       <c r="D89" s="37" t="s">
@@ -15749,12 +16308,12 @@
       <c r="X89" s="36"/>
       <c r="Y89" s="30"/>
     </row>
-    <row r="90" spans="1:25" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:25" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A90" s="35" t="s">
         <v>61</v>
       </c>
       <c r="B90" s="35" t="s">
-        <v>164</v>
+        <v>32</v>
       </c>
       <c r="C90" s="36"/>
       <c r="D90" s="37" t="s">
@@ -15782,12 +16341,12 @@
       <c r="X90" s="36"/>
       <c r="Y90" s="30"/>
     </row>
-    <row r="91" spans="1:25" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:25" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A91" s="35" t="s">
         <v>61</v>
       </c>
       <c r="B91" s="35" t="s">
-        <v>32</v>
+        <v>179</v>
       </c>
       <c r="C91" s="36"/>
       <c r="D91" s="37" t="s">
@@ -15815,78 +16374,78 @@
       <c r="X91" s="36"/>
       <c r="Y91" s="30"/>
     </row>
-    <row r="92" spans="1:25" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:25" s="57" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A92" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="B92" s="35" t="s">
-        <v>179</v>
-      </c>
-      <c r="C92" s="36"/>
-      <c r="D92" s="37" t="s">
+      <c r="B92" s="60" t="s">
+        <v>211</v>
+      </c>
+      <c r="C92" s="61"/>
+      <c r="D92" s="61" t="s">
         <v>124</v>
       </c>
-      <c r="E92" s="36"/>
-      <c r="F92" s="36"/>
-      <c r="G92" s="36"/>
-      <c r="H92" s="36"/>
-      <c r="I92" s="36"/>
-      <c r="J92" s="37"/>
-      <c r="K92" s="36"/>
-      <c r="L92" s="36"/>
-      <c r="M92" s="36"/>
-      <c r="N92" s="36"/>
-      <c r="O92" s="36"/>
-      <c r="P92" s="36"/>
-      <c r="Q92" s="37"/>
-      <c r="R92" s="36"/>
-      <c r="S92" s="36"/>
-      <c r="T92" s="36"/>
-      <c r="U92" s="36"/>
-      <c r="V92" s="36"/>
-      <c r="W92" s="36"/>
-      <c r="X92" s="36"/>
-      <c r="Y92" s="30"/>
+      <c r="E92" s="61"/>
+      <c r="F92" s="61"/>
+      <c r="G92" s="61"/>
+      <c r="H92" s="61"/>
+      <c r="I92" s="61"/>
+      <c r="J92" s="61"/>
+      <c r="K92" s="61"/>
+      <c r="L92" s="61"/>
+      <c r="M92" s="61"/>
+      <c r="N92" s="61"/>
+      <c r="O92" s="61"/>
+      <c r="P92" s="61"/>
+      <c r="Q92" s="61"/>
+      <c r="R92" s="61"/>
+      <c r="S92" s="61"/>
+      <c r="T92" s="61"/>
+      <c r="U92" s="61"/>
+      <c r="V92" s="61"/>
+      <c r="W92" s="61"/>
+      <c r="X92" s="61"/>
+      <c r="Y92" s="55"/>
     </row>
-    <row r="93" spans="1:25" s="57" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:25" s="52" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A93" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="B93" s="60" t="s">
-        <v>211</v>
-      </c>
-      <c r="C93" s="61"/>
-      <c r="D93" s="61" t="s">
+      <c r="B93" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="C93" s="36"/>
+      <c r="D93" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="E93" s="61"/>
-      <c r="F93" s="61"/>
-      <c r="G93" s="61"/>
-      <c r="H93" s="61"/>
-      <c r="I93" s="61"/>
-      <c r="J93" s="61"/>
-      <c r="K93" s="61"/>
-      <c r="L93" s="61"/>
-      <c r="M93" s="61"/>
-      <c r="N93" s="61"/>
-      <c r="O93" s="61"/>
-      <c r="P93" s="61"/>
-      <c r="Q93" s="61"/>
-      <c r="R93" s="61"/>
-      <c r="S93" s="61"/>
-      <c r="T93" s="61"/>
-      <c r="U93" s="61"/>
-      <c r="V93" s="61"/>
-      <c r="W93" s="61"/>
-      <c r="X93" s="61"/>
-      <c r="Y93" s="55"/>
+      <c r="E93" s="36"/>
+      <c r="F93" s="36"/>
+      <c r="G93" s="36"/>
+      <c r="H93" s="36"/>
+      <c r="I93" s="36"/>
+      <c r="J93" s="37"/>
+      <c r="K93" s="36"/>
+      <c r="L93" s="36"/>
+      <c r="M93" s="36"/>
+      <c r="N93" s="36"/>
+      <c r="O93" s="36"/>
+      <c r="P93" s="36"/>
+      <c r="Q93" s="37"/>
+      <c r="R93" s="36"/>
+      <c r="S93" s="36"/>
+      <c r="T93" s="36"/>
+      <c r="U93" s="36"/>
+      <c r="V93" s="36"/>
+      <c r="W93" s="36"/>
+      <c r="X93" s="36"/>
+      <c r="Y93" s="51"/>
     </row>
-    <row r="94" spans="1:25" s="52" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:25" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A94" s="35" t="s">
         <v>61</v>
       </c>
       <c r="B94" s="35" t="s">
-        <v>204</v>
+        <v>122</v>
       </c>
       <c r="C94" s="36"/>
       <c r="D94" s="37" t="s">
@@ -15912,14 +16471,14 @@
       <c r="V94" s="36"/>
       <c r="W94" s="36"/>
       <c r="X94" s="36"/>
-      <c r="Y94" s="51"/>
+      <c r="Y94" s="30"/>
     </row>
-    <row r="95" spans="1:25" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:25" s="64" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A95" s="35" t="s">
         <v>61</v>
       </c>
       <c r="B95" s="35" t="s">
-        <v>122</v>
+        <v>225</v>
       </c>
       <c r="C95" s="36"/>
       <c r="D95" s="37" t="s">
@@ -15945,134 +16504,119 @@
       <c r="V95" s="36"/>
       <c r="W95" s="36"/>
       <c r="X95" s="36"/>
-      <c r="Y95" s="30"/>
+      <c r="Y95" s="63"/>
     </row>
-    <row r="96" spans="1:25" s="69" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A96" s="35" t="s">
-        <v>61</v>
+        <v>107</v>
       </c>
       <c r="B96" s="35" t="s">
-        <v>226</v>
-      </c>
-      <c r="C96" s="36"/>
+        <v>108</v>
+      </c>
+      <c r="C96" s="45"/>
       <c r="D96" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="E96" s="36"/>
-      <c r="F96" s="36"/>
-      <c r="G96" s="36"/>
-      <c r="H96" s="36"/>
-      <c r="I96" s="36"/>
-      <c r="J96" s="37"/>
-      <c r="K96" s="36"/>
-      <c r="L96" s="36"/>
-      <c r="M96" s="36"/>
-      <c r="N96" s="36"/>
-      <c r="O96" s="36"/>
-      <c r="P96" s="36"/>
-      <c r="Q96" s="37"/>
-      <c r="R96" s="36"/>
-      <c r="S96" s="36"/>
-      <c r="T96" s="36"/>
-      <c r="U96" s="36"/>
-      <c r="V96" s="36"/>
-      <c r="W96" s="36"/>
-      <c r="X96" s="36"/>
-      <c r="Y96" s="68"/>
+      <c r="E96" s="45"/>
+      <c r="F96" s="45"/>
+      <c r="G96" s="45"/>
+      <c r="H96" s="45"/>
+      <c r="I96" s="45"/>
+      <c r="J96" s="46"/>
+      <c r="K96" s="45"/>
+      <c r="L96" s="45"/>
+      <c r="M96" s="45"/>
+      <c r="N96" s="45"/>
+      <c r="O96" s="45"/>
+      <c r="P96" s="45"/>
+      <c r="Q96" s="46"/>
+      <c r="R96" s="45"/>
+      <c r="S96" s="45"/>
+      <c r="T96" s="45"/>
+      <c r="U96" s="45"/>
+      <c r="V96" s="45"/>
+      <c r="W96" s="45"/>
+      <c r="X96" s="45"/>
+      <c r="Y96" s="30"/>
     </row>
     <row r="97" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A97" s="35" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="B97" s="35" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="C97" s="45"/>
       <c r="D97" s="37" t="s">
-        <v>124</v>
-      </c>
-      <c r="E97" s="45"/>
-      <c r="F97" s="45"/>
-      <c r="G97" s="45"/>
-      <c r="H97" s="45"/>
-      <c r="I97" s="45"/>
-      <c r="J97" s="46"/>
-      <c r="K97" s="45"/>
-      <c r="L97" s="45"/>
-      <c r="M97" s="45"/>
-      <c r="N97" s="45"/>
-      <c r="O97" s="45"/>
-      <c r="P97" s="45"/>
-      <c r="Q97" s="46"/>
-      <c r="R97" s="45"/>
-      <c r="S97" s="45"/>
-      <c r="T97" s="45"/>
-      <c r="U97" s="45"/>
-      <c r="V97" s="45"/>
-      <c r="W97" s="45"/>
-      <c r="X97" s="45"/>
+        <v>126</v>
+      </c>
+      <c r="E97" s="47" t="s">
+        <v>126</v>
+      </c>
+      <c r="F97" s="47"/>
+      <c r="G97" s="47" t="s">
+        <v>126</v>
+      </c>
+      <c r="H97" s="47"/>
+      <c r="I97" s="47"/>
+      <c r="J97" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="K97" s="47" t="s">
+        <v>126</v>
+      </c>
+      <c r="L97" s="47" t="s">
+        <v>126</v>
+      </c>
+      <c r="M97" s="47" t="s">
+        <v>126</v>
+      </c>
+      <c r="N97" s="47" t="s">
+        <v>126</v>
+      </c>
+      <c r="O97" s="47"/>
+      <c r="P97" s="47"/>
+      <c r="Q97" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="R97" s="49" t="s">
+        <v>163</v>
+      </c>
+      <c r="S97" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="T97" s="47"/>
+      <c r="U97" s="47" t="s">
+        <v>158</v>
+      </c>
+      <c r="V97" s="47"/>
+      <c r="W97" s="47"/>
+      <c r="X97" s="47"/>
       <c r="Y97" s="30"/>
-    </row>
-    <row r="98" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A98" s="35" t="s">
-        <v>117</v>
-      </c>
-      <c r="B98" s="35" t="s">
-        <v>118</v>
-      </c>
-      <c r="C98" s="45"/>
-      <c r="D98" s="37" t="s">
-        <v>126</v>
-      </c>
-      <c r="E98" s="47" t="s">
-        <v>126</v>
-      </c>
-      <c r="F98" s="47"/>
-      <c r="G98" s="47" t="s">
-        <v>126</v>
-      </c>
-      <c r="H98" s="47"/>
-      <c r="I98" s="47"/>
-      <c r="J98" s="48" t="s">
-        <v>158</v>
-      </c>
-      <c r="K98" s="47" t="s">
-        <v>126</v>
-      </c>
-      <c r="L98" s="47" t="s">
-        <v>126</v>
-      </c>
-      <c r="M98" s="47" t="s">
-        <v>126</v>
-      </c>
-      <c r="N98" s="47" t="s">
-        <v>126</v>
-      </c>
-      <c r="O98" s="47"/>
-      <c r="P98" s="47"/>
-      <c r="Q98" s="48" t="s">
-        <v>158</v>
-      </c>
-      <c r="R98" s="49" t="s">
-        <v>163</v>
-      </c>
-      <c r="S98" s="48" t="s">
-        <v>158</v>
-      </c>
-      <c r="T98" s="47"/>
-      <c r="U98" s="47" t="s">
-        <v>158</v>
-      </c>
-      <c r="V98" s="47"/>
-      <c r="W98" s="47"/>
-      <c r="X98" s="47"/>
-      <c r="Y98" s="30"/>
     </row>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C34" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="D46" sqref="D46"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C19" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="B25" sqref="B25"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
+      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
+      <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="C31" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -16082,27 +16626,9 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C31" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
-      <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" scale="125">
-      <pane xSplit="2" ySplit="6.0526315789473681" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
   </customSheetViews>
   <mergeCells count="6">
-    <mergeCell ref="Y82:Y83"/>
+    <mergeCell ref="Y81:Y82"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="K5:O5"/>
     <mergeCell ref="R5:X5"/>
@@ -16458,8 +16984,13 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}">
-      <selection activeCell="A22" sqref="A22"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
+      <selection activeCell="B17" sqref="B17"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
+      <selection activeCell="C7" sqref="C7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -16468,13 +16999,8 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}">
-      <selection activeCell="C7" sqref="C7"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
-      <selection activeCell="B17" sqref="B17"/>
+    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}">
+      <selection activeCell="A22" sqref="A22"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>

</xml_diff>

<commit_message>
Päivitä kanavaoikeusrivit Kaukon Excelin pohjalta
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="13020" windowWidth="51200" windowHeight="14660" tabRatio="500"/>
+    <workbookView xWindow="-260" yWindow="2920" windowWidth="51200" windowHeight="24660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2560" windowHeight="560" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2560" windowHeight="1060" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
     <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="Microsoft Office -käyttäjä - Oma näkymä" guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="1149" tabRatio="500" activeSheetId="1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1456" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1498" uniqueCount="234">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -748,16 +748,34 @@
     <t>R*,W*,siirrä-kokonaishintaisiin*</t>
   </si>
   <si>
-    <t>R*,W*,siirrä-muutos-ja-lisätöihin*</t>
-  </si>
-  <si>
     <t>Järjestelmäasetukset</t>
   </si>
   <si>
     <t>Kanavat / Kanavakohteet</t>
   </si>
   <si>
-    <t>Tällä oikeudella voi hakea urakan kanavakohteet (tarvitaan mm. lomakkeissa)</t>
+    <t>R*,W*,siirrä-muutos- ja lisätöihin*</t>
+  </si>
+  <si>
+    <t>R*,W,siirrä-muutos- ja lisätöihin</t>
+  </si>
+  <si>
+    <t>R,W,siirrä-muutos- ja lisätöihin</t>
+  </si>
+  <si>
+    <t>R+,W+,siirrä-muutos- ja lisätöihin+</t>
+  </si>
+  <si>
+    <t>R*,W,siirrä-kokonaishintaisiin</t>
+  </si>
+  <si>
+    <t>R,W,siirrä-kokonaishintaisiin</t>
+  </si>
+  <si>
+    <t>R+,W+,siirrä-kokonaishintaisiin+</t>
+  </si>
+  <si>
+    <t>Tällä oikeudella voi hakea urakan kanavakohteet (tarvitaan mm. lomakkeissa). Kohteiden muokkaamiseen on oma oikeus hallintapuolella.</t>
   </si>
 </sst>
 </file>
@@ -871,7 +889,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -918,8 +936,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="189">
+  <cellStyleXfs count="201">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1109,8 +1136,20 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -1224,9 +1263,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1262,8 +1298,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="189">
+  <cellStyles count="201">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1358,6 +1398,12 @@
     <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1452,6 +1498,12 @@
     <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1465,7 +1517,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{59381CD3-9619-064B-BFE6-F97D1F318E9C}" diskRevisions="1" revisionId="774" version="45">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{66013A6B-07DA-FA4E-96DD-EE8248ECB42D}" diskRevisions="1" revisionId="823" version="51">
   <header guid="{1E352813-0B26-DB4E-84BE-460845B77133}" dateTime="2017-06-20T12:32:37" maxSheetId="3" userName="Microsoft Office -käyttäjä" r:id="rId60" minRId="448" maxRId="464">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1736,6 +1788,42 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{F9196CAE-B095-044E-808F-62217660B09D}" dateTime="2017-12-21T15:10:51" maxSheetId="3" userName="Microsoft Office User" r:id="rId105" minRId="775" maxRId="782">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{CDBC26EE-0BE6-DA47-BFBF-2DEAC01C6312}" dateTime="2017-12-21T15:12:38" maxSheetId="3" userName="Microsoft Office User" r:id="rId106" minRId="784" maxRId="786">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{D99D0248-35B6-8A43-9165-2B060F027799}" dateTime="2017-12-21T15:18:05" maxSheetId="3" userName="Microsoft Office User" r:id="rId107" minRId="787" maxRId="795">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{98FC5DE7-78A9-154D-B562-8B1E09DA9D7A}" dateTime="2017-12-21T15:19:01" maxSheetId="3" userName="Microsoft Office User" r:id="rId108" minRId="796" maxRId="803">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{507B86D1-857C-5D44-9A93-5145CCF7DFBA}" dateTime="2017-12-21T15:19:35" maxSheetId="3" userName="Microsoft Office User" r:id="rId109" minRId="804" maxRId="813">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{66013A6B-07DA-FA4E-96DD-EE8248ECB42D}" dateTime="2017-12-21T15:20:31" maxSheetId="3" userName="Microsoft Office User" r:id="rId110" minRId="814" maxRId="822">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -10425,6 +10513,2446 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog43.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="775" sId="1">
+    <oc r="U25" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </oc>
+    <nc r="U25" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="D30:X30" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D30" start="0" length="0">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="E30" start="0" length="0">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="F30" start="0" length="0">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="G30" start="0" length="0">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="H30" start="0" length="0">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="I30" start="0" length="0">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="J30" start="0" length="0">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="K30" start="0" length="0">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="L30" start="0" length="0">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="M30" start="0" length="0">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="N30" start="0" length="0">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="O30" start="0" length="0">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="P30" start="0" length="0">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="Q30" start="0" length="0">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="R30" start="0" length="0">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="S30" start="0" length="0">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="T30" start="0" length="0">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="U30" start="0" length="0">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="V30" start="0" length="0">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="W30" start="0" length="0">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="X30" start="0" length="0">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="D30" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="E30" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="F30" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="G30" start="0" length="0"/>
+  <rfmt sheetId="1" xfDxf="1" sqref="H30" start="0" length="0"/>
+  <rfmt sheetId="1" xfDxf="1" sqref="I30" start="0" length="0"/>
+  <rfmt sheetId="1" xfDxf="1" sqref="J30" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="K30" start="0" length="0"/>
+  <rfmt sheetId="1" xfDxf="1" sqref="L30" start="0" length="0"/>
+  <rfmt sheetId="1" xfDxf="1" sqref="M30" start="0" length="0"/>
+  <rfmt sheetId="1" xfDxf="1" sqref="N30" start="0" length="0"/>
+  <rfmt sheetId="1" xfDxf="1" sqref="O30" start="0" length="0"/>
+  <rfmt sheetId="1" xfDxf="1" sqref="P30" start="0" length="0"/>
+  <rfmt sheetId="1" xfDxf="1" sqref="Q30" start="0" length="0"/>
+  <rfmt sheetId="1" xfDxf="1" sqref="R30" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="S30" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="T30" start="0" length="0"/>
+  <rfmt sheetId="1" xfDxf="1" sqref="U30" start="0" length="0"/>
+  <rfmt sheetId="1" xfDxf="1" sqref="V30" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="W30" start="0" length="0"/>
+  <rfmt sheetId="1" xfDxf="1" sqref="X30" start="0" length="0"/>
+  <rfmt sheetId="1" sqref="D30" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <right/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="E30" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <right/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="F30" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="J30" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="R30" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="S30" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="V30" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rcc rId="776" sId="1" xfDxf="1" dxf="1">
+    <oc r="D30" t="inlineStr">
+      <is>
+        <t>R*,W*</t>
+      </is>
+    </oc>
+    <nc r="D30" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+    <ndxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+      </border>
+    </ndxf>
+  </rcc>
+  <rcc rId="777" sId="1" xfDxf="1" dxf="1">
+    <nc r="E30" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+    <ndxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+      </border>
+    </ndxf>
+  </rcc>
+  <rcc rId="778" sId="1" xfDxf="1" dxf="1">
+    <nc r="F30" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+    <ndxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rfmt sheetId="1" xfDxf="1" sqref="G30" start="0" length="0"/>
+  <rfmt sheetId="1" xfDxf="1" sqref="H30" start="0" length="0"/>
+  <rfmt sheetId="1" xfDxf="1" sqref="I30" start="0" length="0"/>
+  <rcc rId="779" sId="1" xfDxf="1" dxf="1">
+    <nc r="J30" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+    <ndxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rfmt sheetId="1" xfDxf="1" sqref="K30" start="0" length="0"/>
+  <rfmt sheetId="1" xfDxf="1" sqref="L30" start="0" length="0"/>
+  <rfmt sheetId="1" xfDxf="1" sqref="M30" start="0" length="0"/>
+  <rfmt sheetId="1" xfDxf="1" sqref="N30" start="0" length="0"/>
+  <rfmt sheetId="1" xfDxf="1" sqref="O30" start="0" length="0"/>
+  <rfmt sheetId="1" xfDxf="1" sqref="P30" start="0" length="0"/>
+  <rfmt sheetId="1" xfDxf="1" sqref="Q30" start="0" length="0"/>
+  <rcc rId="780" sId="1" xfDxf="1" dxf="1">
+    <nc r="R30" t="inlineStr">
+      <is>
+        <t>R+</t>
+      </is>
+    </nc>
+    <ndxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rcc rId="781" sId="1" xfDxf="1" dxf="1">
+    <nc r="S30" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+    <ndxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rfmt sheetId="1" xfDxf="1" sqref="T30" start="0" length="0"/>
+  <rfmt sheetId="1" xfDxf="1" sqref="U30" start="0" length="0"/>
+  <rcc rId="782" sId="1" xfDxf="1" dxf="1">
+    <nc r="V30" t="inlineStr">
+      <is>
+        <t>R+</t>
+      </is>
+    </nc>
+    <ndxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rfmt sheetId="1" xfDxf="1" sqref="W30" start="0" length="0"/>
+  <rfmt sheetId="1" xfDxf="1" sqref="X30" start="0" length="0"/>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="delete"/>
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_7A9649F2_657F_9445_B6E6_FE94C6A09957_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Oikeudet!$A$5:$Y$97</formula>
+    <oldFormula>Oikeudet!$A$5:$Y$97</oldFormula>
+  </rdn>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog44.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="D25" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="E25" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="F25" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="G25" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="H25" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="I25" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="J25" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="K25" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="L25" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="M25" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="N25" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="O25" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="P25" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="Q25" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="R25" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="S25" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="T25" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="U25" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="V25" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="W25" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="X25" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="D25" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="E25" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="F25" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rcc rId="784" sId="1" xfDxf="1" dxf="1">
+    <nc r="G25" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+    <ndxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rfmt sheetId="1" xfDxf="1" sqref="H25" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rcc rId="785" sId="1" xfDxf="1" dxf="1">
+    <nc r="I25" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+    <ndxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rcc rId="786" sId="1" xfDxf="1" dxf="1">
+    <oc r="J25" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </oc>
+    <nc r="J25" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+    <ndxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rfmt sheetId="1" xfDxf="1" sqref="K25" start="0" length="0"/>
+  <rfmt sheetId="1" xfDxf="1" sqref="L25" start="0" length="0"/>
+  <rfmt sheetId="1" xfDxf="1" sqref="M25" start="0" length="0"/>
+  <rfmt sheetId="1" xfDxf="1" sqref="N25" start="0" length="0"/>
+  <rfmt sheetId="1" xfDxf="1" sqref="O25" start="0" length="0"/>
+  <rfmt sheetId="1" xfDxf="1" sqref="P25" start="0" length="0"/>
+  <rfmt sheetId="1" xfDxf="1" sqref="Q25" start="0" length="0"/>
+  <rfmt sheetId="1" xfDxf="1" sqref="R25" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="S25" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="T25" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="U25" start="0" length="0">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="V25" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="W25" start="0" length="0"/>
+  <rfmt sheetId="1" xfDxf="1" sqref="X25" start="0" length="0"/>
+  <rfmt sheetId="1" sqref="U25" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog45.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="D46" start="0" length="0">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <alignment wrapText="1" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="E46" start="0" length="0">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <alignment wrapText="1" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+      </border>
+    </dxf>
+  </rfmt>
+  <rcc rId="787" sId="1" odxf="1" dxf="1">
+    <nc r="F46" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+    <odxf>
+      <border outline="0">
+        <left/>
+      </border>
+    </odxf>
+    <ndxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+      </border>
+    </ndxf>
+  </rcc>
+  <rfmt sheetId="1" sqref="H46" start="0" length="0">
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="J46" start="0" length="0">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <alignment wrapText="1" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="R46" start="0" length="0">
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="S46" start="0" length="0">
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+      </border>
+    </dxf>
+  </rfmt>
+  <rcc rId="788" sId="1" odxf="1" dxf="1">
+    <nc r="T46" t="inlineStr">
+      <is>
+        <t>R+</t>
+      </is>
+    </nc>
+    <odxf>
+      <border outline="0">
+        <left/>
+      </border>
+    </odxf>
+    <ndxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+      </border>
+    </ndxf>
+  </rcc>
+  <rfmt sheetId="1" sqref="U46" start="0" length="0">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+      </border>
+    </dxf>
+  </rfmt>
+  <rcc rId="789" sId="1" odxf="1" dxf="1">
+    <nc r="V46" t="inlineStr">
+      <is>
+        <t>R+</t>
+      </is>
+    </nc>
+    <odxf>
+      <border outline="0">
+        <left/>
+      </border>
+    </odxf>
+    <ndxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+      </border>
+    </ndxf>
+  </rcc>
+  <rcc rId="790" sId="1" odxf="1" dxf="1">
+    <nc r="U46" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </nc>
+    <ndxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment wrapText="1" readingOrder="0"/>
+    </ndxf>
+  </rcc>
+  <rfmt sheetId="1" sqref="D46" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment wrapText="0" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="E46" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment wrapText="0" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="G46" start="0" length="0">
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="I46" start="0" length="0">
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="J46" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment wrapText="0" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D46:J46">
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+  </rfmt>
+  <rcc rId="791" sId="1">
+    <oc r="D46" t="inlineStr">
+      <is>
+        <t>R*,W*,siirrä-muutos-ja-lisätöihin*</t>
+      </is>
+    </oc>
+    <nc r="D46" t="inlineStr">
+      <is>
+        <t>R*,W*,siirrä-muutos- ja lisätöihin*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="792" sId="1">
+    <nc r="E46" t="inlineStr">
+      <is>
+        <t>R*,W,siirrä-muutos- ja lisätöihin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="793" sId="1">
+    <nc r="J46" t="inlineStr">
+      <is>
+        <t>R,W,siirrä-muutos- ja lisätöihin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="794" sId="1">
+    <nc r="R46" t="inlineStr">
+      <is>
+        <t>R+,W+,siirrä-muutos- ja lisätöihin+</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="S46" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" wrapText="0" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rcc rId="795" sId="1" xfDxf="1" dxf="1">
+    <nc r="S46" t="inlineStr">
+      <is>
+        <t>R,W,siirrä-muutos- ja lisätöihin</t>
+      </is>
+    </nc>
+    <ndxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog46.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="796" sId="1">
+    <nc r="E48" t="inlineStr">
+      <is>
+        <t>R*,W,siirrä-kokonaishintaisiin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="797" sId="1">
+    <nc r="F48" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="798" sId="1">
+    <nc r="J48" t="inlineStr">
+      <is>
+        <t>R,W,siirrä-kokonaishintaisiin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="799" sId="1">
+    <nc r="R48" t="inlineStr">
+      <is>
+        <t>R+,W+,siirrä-kokonaishintaisiin+</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="S48" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rcc rId="800" sId="1" xfDxf="1" dxf="1">
+    <nc r="S48" t="inlineStr">
+      <is>
+        <t>R,W,siirrä-kokonaishintaisiin</t>
+      </is>
+    </nc>
+    <ndxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rcc rId="801" sId="1">
+    <nc r="T48" t="inlineStr">
+      <is>
+        <t>R+</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="802" sId="1">
+    <nc r="U48" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="803" sId="1">
+    <nc r="V48" t="inlineStr">
+      <is>
+        <t>R+</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog47.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="D47" start="0" length="0">
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rcc rId="804" sId="1" odxf="1" dxf="1">
+    <nc r="E47" t="inlineStr">
+      <is>
+        <t>R*,W</t>
+      </is>
+    </nc>
+    <odxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </odxf>
+    <ndxf>
+      <font>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rcc rId="805" sId="1" odxf="1" dxf="1">
+    <nc r="F47" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+    <odxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </odxf>
+    <ndxf>
+      <font>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rfmt sheetId="1" sqref="G47" start="0" length="0">
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rcc rId="806" sId="1" odxf="1" dxf="1">
+    <nc r="H47" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+    <odxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </odxf>
+    <ndxf>
+      <font>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rcc rId="807" sId="1" odxf="1" dxf="1">
+    <nc r="I47" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+    <odxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </odxf>
+    <ndxf>
+      <font>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rcc rId="808" sId="1" odxf="1" dxf="1">
+    <nc r="J47" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </nc>
+    <odxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </odxf>
+    <ndxf>
+      <font>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rfmt sheetId="1" sqref="K47" start="0" length="0">
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="L47" start="0" length="0">
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="M47" start="0" length="0">
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="N47" start="0" length="0">
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="O47" start="0" length="0">
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="P47" start="0" length="0">
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="Q47" start="0" length="0">
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rcc rId="809" sId="1" odxf="1" dxf="1">
+    <nc r="R47" t="inlineStr">
+      <is>
+        <t>R+,W+</t>
+      </is>
+    </nc>
+    <odxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </odxf>
+    <ndxf>
+      <font>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rcc rId="810" sId="1" odxf="1" dxf="1">
+    <nc r="S47" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </nc>
+    <odxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </odxf>
+    <ndxf>
+      <font>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rcc rId="811" sId="1" odxf="1" dxf="1">
+    <nc r="T47" t="inlineStr">
+      <is>
+        <t>R+</t>
+      </is>
+    </nc>
+    <odxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </odxf>
+    <ndxf>
+      <font>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rfmt sheetId="1" sqref="U47" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rcc rId="812" sId="1" odxf="1" dxf="1">
+    <nc r="V47" t="inlineStr">
+      <is>
+        <t>R+</t>
+      </is>
+    </nc>
+    <odxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </odxf>
+    <ndxf>
+      <font>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rfmt sheetId="1" sqref="W47" start="0" length="0">
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="X47" start="0" length="0">
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rcc rId="813" sId="1" odxf="1" dxf="1">
+    <nc r="U47" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </nc>
+    <ndxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </ndxf>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog48.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="814" sId="1">
+    <nc r="E45" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="815" sId="1">
+    <nc r="F45" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="816" sId="1">
+    <nc r="J45" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="817" sId="1">
+    <nc r="R45" t="inlineStr">
+      <is>
+        <t>R+</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="818" sId="1">
+    <nc r="S45" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="T45" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rcc rId="819" sId="1" xfDxf="1" dxf="1">
+    <nc r="T45" t="inlineStr">
+      <is>
+        <t>R+</t>
+      </is>
+    </nc>
+    <ndxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rcc rId="820" sId="1">
+    <nc r="U45" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="821" sId="1">
+    <nc r="V45" t="inlineStr">
+      <is>
+        <t>R+</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="822" sId="1">
+    <oc r="Y45" t="inlineStr">
+      <is>
+        <t>Tällä oikeudella voi hakea urakan kanavakohteet (tarvitaan mm. lomakkeissa)</t>
+      </is>
+    </oc>
+    <nc r="Y45" t="inlineStr">
+      <is>
+        <t>Tällä oikeudella voi hakea urakan kanavakohteet (tarvitaan mm. lomakkeissa). Kohteiden muokkaamiseen on oma oikeus hallintapuolella.</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="delete"/>
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_7A9649F2_657F_9445_B6E6_FE94C6A09957_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Oikeudet!$A$5:$Y$97</formula>
+    <oldFormula>Oikeudet!$A$5:$Y$97</oldFormula>
+  </rdn>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog5.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="514" sId="1">
@@ -10966,14 +13494,13 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="6">
+<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="5">
   <userInfo guid="{1E352813-0B26-DB4E-84BE-460845B77133}" name="Microsoft Office -käyttäjä" id="-785751636" dateTime="2017-06-20T12:33:00"/>
   <userInfo guid="{1AB7A282-42ED-4740-A9CB-95FF229EC1A0}" name="Mikko Rönkkömäki" id="-727946492" dateTime="2017-06-22T10:45:48"/>
   <userInfo guid="{4A189F6B-10A0-794F-AE26-98E1292E0A90}" name="Microsoft Office User" id="-296987972" dateTime="2017-09-21T08:10:21"/>
   <userInfo guid="{72187562-2E05-9542-A596-E87B0EC7A6D4}" name="Microsoft Office User" id="-296946728" dateTime="2017-11-06T12:39:34"/>
   <userInfo guid="{7DE0565B-D0D5-DF45-A2A1-25AA2C726E19}" name="Microsoft Office User" id="-296947028" dateTime="2017-11-20T14:54:25"/>
-  <userInfo guid="{59381CD3-9619-064B-BFE6-F97D1F318E9C}" name="Microsoft Office User" id="-296969556" dateTime="2017-12-21T15:04:51"/>
 </users>
 </file>
 
@@ -11302,10 +13829,10 @@
   <dimension ref="A1:Y97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C19" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="R10" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B25" sqref="B25"/>
+      <selection pane="bottomRight" activeCell="Y30" sqref="Y30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -11342,40 +13869,40 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="71" t="s">
+      <c r="C1" s="70" t="s">
         <v>149</v>
       </c>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
-      <c r="K1" s="72"/>
-      <c r="L1" s="72"/>
-      <c r="M1" s="72"/>
-      <c r="N1" s="72"/>
-      <c r="O1" s="72"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
+      <c r="M1" s="71"/>
+      <c r="N1" s="71"/>
+      <c r="O1" s="71"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="73" t="s">
+      <c r="C2" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
-      <c r="J2" s="74"/>
-      <c r="K2" s="74"/>
-      <c r="L2" s="74"/>
-      <c r="M2" s="74"/>
-      <c r="N2" s="74"/>
-      <c r="O2" s="74"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
+      <c r="M2" s="73"/>
+      <c r="N2" s="73"/>
+      <c r="O2" s="73"/>
     </row>
     <row r="3" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
@@ -11398,34 +13925,34 @@
     <row r="5" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="30"/>
       <c r="B5" s="30"/>
-      <c r="C5" s="69" t="s">
+      <c r="C5" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="70"/>
-      <c r="E5" s="70"/>
-      <c r="F5" s="70"/>
-      <c r="G5" s="70"/>
-      <c r="H5" s="70"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
+      <c r="G5" s="69"/>
+      <c r="H5" s="69"/>
       <c r="I5" s="30"/>
       <c r="J5" s="30"/>
-      <c r="K5" s="69" t="s">
+      <c r="K5" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="L5" s="70"/>
-      <c r="M5" s="70"/>
-      <c r="N5" s="70"/>
-      <c r="O5" s="70"/>
+      <c r="L5" s="69"/>
+      <c r="M5" s="69"/>
+      <c r="N5" s="69"/>
+      <c r="O5" s="69"/>
       <c r="P5" s="30"/>
       <c r="Q5" s="30"/>
-      <c r="R5" s="69" t="s">
+      <c r="R5" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="S5" s="70"/>
-      <c r="T5" s="70"/>
-      <c r="U5" s="70"/>
-      <c r="V5" s="70"/>
-      <c r="W5" s="70"/>
-      <c r="X5" s="70"/>
+      <c r="S5" s="69"/>
+      <c r="T5" s="69"/>
+      <c r="U5" s="69"/>
+      <c r="V5" s="69"/>
+      <c r="W5" s="69"/>
+      <c r="X5" s="69"/>
       <c r="Y5" s="31" t="s">
         <v>13</v>
       </c>
@@ -12363,7 +14890,7 @@
       <c r="X20" s="36"/>
       <c r="Y20" s="38"/>
     </row>
-    <row r="21" spans="1:25" s="62" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:25" s="61" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="35" t="s">
         <v>14</v>
       </c>
@@ -12653,51 +15180,55 @@
       <c r="A25" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="60" t="s">
+      <c r="B25" s="59" t="s">
         <v>210</v>
       </c>
-      <c r="C25" s="61"/>
-      <c r="D25" s="61" t="s">
+      <c r="C25" s="60"/>
+      <c r="D25" s="36" t="s">
         <v>124</v>
       </c>
-      <c r="E25" s="61" t="s">
+      <c r="E25" s="60" t="s">
         <v>128</v>
       </c>
-      <c r="F25" s="61" t="s">
-        <v>125</v>
-      </c>
-      <c r="G25" s="61"/>
-      <c r="H25" s="61" t="s">
-        <v>125</v>
-      </c>
-      <c r="I25" s="61"/>
-      <c r="J25" s="61" t="s">
+      <c r="F25" s="60" t="s">
+        <v>125</v>
+      </c>
+      <c r="G25" s="60" t="s">
+        <v>125</v>
+      </c>
+      <c r="H25" s="60" t="s">
+        <v>125</v>
+      </c>
+      <c r="I25" s="60" t="s">
+        <v>125</v>
+      </c>
+      <c r="J25" s="60" t="s">
+        <v>125</v>
+      </c>
+      <c r="K25"/>
+      <c r="L25"/>
+      <c r="M25"/>
+      <c r="N25"/>
+      <c r="O25"/>
+      <c r="P25"/>
+      <c r="Q25"/>
+      <c r="R25" s="36" t="s">
+        <v>130</v>
+      </c>
+      <c r="S25" s="60" t="s">
         <v>111</v>
       </c>
-      <c r="K25" s="61"/>
-      <c r="L25" s="61"/>
-      <c r="M25" s="61"/>
-      <c r="N25" s="61"/>
-      <c r="O25" s="61"/>
-      <c r="P25" s="61"/>
-      <c r="Q25" s="61"/>
-      <c r="R25" s="61" t="s">
-        <v>130</v>
-      </c>
-      <c r="S25" s="61" t="s">
+      <c r="T25" s="60" t="s">
+        <v>129</v>
+      </c>
+      <c r="U25" s="60" t="s">
         <v>111</v>
       </c>
-      <c r="T25" s="61" t="s">
+      <c r="V25" s="60" t="s">
         <v>129</v>
       </c>
-      <c r="U25" s="61" t="s">
-        <v>16</v>
-      </c>
-      <c r="V25" s="61" t="s">
-        <v>129</v>
-      </c>
-      <c r="W25" s="61"/>
-      <c r="X25" s="61"/>
+      <c r="W25"/>
+      <c r="X25"/>
       <c r="Y25" s="55"/>
     </row>
     <row r="26" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -12935,9 +15466,41 @@
       <c r="B30" s="58" t="s">
         <v>209</v>
       </c>
-      <c r="D30" s="59" t="s">
-        <v>124</v>
-      </c>
+      <c r="D30" s="74" t="s">
+        <v>125</v>
+      </c>
+      <c r="E30" s="74" t="s">
+        <v>125</v>
+      </c>
+      <c r="F30" s="60" t="s">
+        <v>125</v>
+      </c>
+      <c r="G30"/>
+      <c r="H30"/>
+      <c r="I30"/>
+      <c r="J30" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="K30"/>
+      <c r="L30"/>
+      <c r="M30"/>
+      <c r="N30"/>
+      <c r="O30"/>
+      <c r="P30"/>
+      <c r="Q30"/>
+      <c r="R30" s="36" t="s">
+        <v>129</v>
+      </c>
+      <c r="S30" s="60" t="s">
+        <v>16</v>
+      </c>
+      <c r="T30"/>
+      <c r="U30"/>
+      <c r="V30" s="36" t="s">
+        <v>129</v>
+      </c>
+      <c r="W30"/>
+      <c r="X30"/>
     </row>
     <row r="31" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="39" t="s">
@@ -13793,72 +16356,104 @@
         <v>197</v>
       </c>
     </row>
-    <row r="45" spans="1:25" s="66" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:25" s="65" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A45" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B45" s="60" t="s">
-        <v>226</v>
-      </c>
-      <c r="C45" s="61"/>
-      <c r="D45" s="61" t="s">
-        <v>125</v>
-      </c>
-      <c r="E45" s="61"/>
-      <c r="F45" s="61"/>
-      <c r="G45" s="61"/>
-      <c r="H45" s="61"/>
-      <c r="I45" s="61"/>
-      <c r="J45" s="61"/>
-      <c r="K45" s="61"/>
-      <c r="L45" s="61"/>
-      <c r="M45" s="61"/>
-      <c r="N45" s="61"/>
-      <c r="O45" s="61"/>
-      <c r="P45" s="61"/>
-      <c r="Q45" s="61"/>
-      <c r="R45" s="61"/>
-      <c r="S45" s="61"/>
-      <c r="T45" s="61"/>
-      <c r="U45" s="61"/>
-      <c r="V45" s="61"/>
-      <c r="W45" s="61"/>
-      <c r="X45" s="61"/>
-      <c r="Y45" s="65" t="s">
-        <v>227</v>
+      <c r="B45" s="59" t="s">
+        <v>225</v>
+      </c>
+      <c r="C45" s="60"/>
+      <c r="D45" s="60" t="s">
+        <v>125</v>
+      </c>
+      <c r="E45" s="60" t="s">
+        <v>125</v>
+      </c>
+      <c r="F45" s="60" t="s">
+        <v>125</v>
+      </c>
+      <c r="G45" s="60"/>
+      <c r="H45" s="60"/>
+      <c r="I45" s="60"/>
+      <c r="J45" s="60" t="s">
+        <v>16</v>
+      </c>
+      <c r="K45" s="60"/>
+      <c r="L45" s="60"/>
+      <c r="M45" s="60"/>
+      <c r="N45" s="60"/>
+      <c r="O45" s="60"/>
+      <c r="P45" s="60"/>
+      <c r="Q45" s="60"/>
+      <c r="R45" s="60" t="s">
+        <v>129</v>
+      </c>
+      <c r="S45" s="60" t="s">
+        <v>16</v>
+      </c>
+      <c r="T45" s="60" t="s">
+        <v>129</v>
+      </c>
+      <c r="U45" s="60" t="s">
+        <v>16</v>
+      </c>
+      <c r="V45" s="60" t="s">
+        <v>129</v>
+      </c>
+      <c r="W45" s="60"/>
+      <c r="X45" s="60"/>
+      <c r="Y45" s="64" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="46" spans="1:25" s="57" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A46" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="60" t="s">
+      <c r="B46" s="59" t="s">
         <v>212</v>
       </c>
-      <c r="C46" s="61"/>
-      <c r="D46" s="61" t="s">
-        <v>224</v>
-      </c>
-      <c r="E46" s="61"/>
-      <c r="F46" s="61"/>
-      <c r="G46" s="61"/>
-      <c r="H46" s="61"/>
-      <c r="I46" s="61"/>
-      <c r="J46" s="61"/>
-      <c r="K46" s="61"/>
-      <c r="L46" s="61"/>
-      <c r="M46" s="61"/>
-      <c r="N46" s="61"/>
-      <c r="O46" s="61"/>
-      <c r="P46" s="61"/>
-      <c r="Q46" s="61"/>
-      <c r="R46" s="61"/>
-      <c r="S46" s="61"/>
-      <c r="T46" s="61"/>
-      <c r="U46" s="61"/>
-      <c r="V46" s="61"/>
-      <c r="W46" s="61"/>
-      <c r="X46" s="61"/>
+      <c r="C46" s="60"/>
+      <c r="D46" s="41" t="s">
+        <v>226</v>
+      </c>
+      <c r="E46" s="41" t="s">
+        <v>227</v>
+      </c>
+      <c r="F46" s="41" t="s">
+        <v>125</v>
+      </c>
+      <c r="G46" s="41"/>
+      <c r="H46" s="41"/>
+      <c r="I46" s="41"/>
+      <c r="J46" s="41" t="s">
+        <v>228</v>
+      </c>
+      <c r="K46" s="60"/>
+      <c r="L46" s="60"/>
+      <c r="M46" s="60"/>
+      <c r="N46" s="60"/>
+      <c r="O46" s="60"/>
+      <c r="P46" s="60"/>
+      <c r="Q46" s="60"/>
+      <c r="R46" s="41" t="s">
+        <v>229</v>
+      </c>
+      <c r="S46" s="41" t="s">
+        <v>228</v>
+      </c>
+      <c r="T46" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="U46" s="50" t="s">
+        <v>111</v>
+      </c>
+      <c r="V46" s="36" t="s">
+        <v>129</v>
+      </c>
+      <c r="W46" s="60"/>
+      <c r="X46" s="60"/>
       <c r="Y46" s="56"/>
     </row>
     <row r="47" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -13868,41 +16463,97 @@
       <c r="B47" s="58" t="s">
         <v>208</v>
       </c>
-      <c r="D47" s="59" t="s">
+      <c r="D47" s="37" t="s">
         <v>124</v>
       </c>
+      <c r="E47" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="F47" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="G47" s="75"/>
+      <c r="H47" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="I47" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="J47" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="K47" s="75"/>
+      <c r="L47" s="75"/>
+      <c r="M47" s="75"/>
+      <c r="N47" s="75"/>
+      <c r="O47" s="75"/>
+      <c r="P47" s="75"/>
+      <c r="Q47" s="75"/>
+      <c r="R47" s="36" t="s">
+        <v>130</v>
+      </c>
+      <c r="S47" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="T47" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="U47" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="V47" s="36" t="s">
+        <v>129</v>
+      </c>
+      <c r="W47" s="75"/>
+      <c r="X47" s="75"/>
     </row>
     <row r="48" spans="1:25" s="57" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B48" s="60" t="s">
+      <c r="B48" s="59" t="s">
         <v>213</v>
       </c>
-      <c r="C48" s="61"/>
-      <c r="D48" s="61" t="s">
+      <c r="C48" s="60"/>
+      <c r="D48" s="60" t="s">
         <v>223</v>
       </c>
-      <c r="E48" s="61"/>
-      <c r="F48" s="61"/>
-      <c r="G48" s="61"/>
-      <c r="H48" s="61"/>
-      <c r="I48" s="61"/>
-      <c r="J48" s="61"/>
-      <c r="K48" s="61"/>
-      <c r="L48" s="61"/>
-      <c r="M48" s="61"/>
-      <c r="N48" s="61"/>
-      <c r="O48" s="61"/>
-      <c r="P48" s="61"/>
-      <c r="Q48" s="61"/>
-      <c r="R48" s="61"/>
-      <c r="S48" s="61"/>
-      <c r="T48" s="61"/>
-      <c r="U48" s="61"/>
-      <c r="V48" s="61"/>
-      <c r="W48" s="61"/>
-      <c r="X48" s="61"/>
+      <c r="E48" s="60" t="s">
+        <v>230</v>
+      </c>
+      <c r="F48" s="60" t="s">
+        <v>125</v>
+      </c>
+      <c r="G48" s="60"/>
+      <c r="H48" s="60"/>
+      <c r="I48" s="60"/>
+      <c r="J48" s="60" t="s">
+        <v>231</v>
+      </c>
+      <c r="K48" s="60"/>
+      <c r="L48" s="60"/>
+      <c r="M48" s="60"/>
+      <c r="N48" s="60"/>
+      <c r="O48" s="60"/>
+      <c r="P48" s="60"/>
+      <c r="Q48" s="60"/>
+      <c r="R48" s="60" t="s">
+        <v>232</v>
+      </c>
+      <c r="S48" s="60" t="s">
+        <v>231</v>
+      </c>
+      <c r="T48" s="60" t="s">
+        <v>129</v>
+      </c>
+      <c r="U48" s="60" t="s">
+        <v>111</v>
+      </c>
+      <c r="V48" s="60" t="s">
+        <v>129</v>
+      </c>
+      <c r="W48" s="60"/>
+      <c r="X48" s="60"/>
       <c r="Y48" s="55"/>
     </row>
     <row r="49" spans="1:25" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -15946,7 +18597,7 @@
       <c r="X81" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="Y81" s="67" t="s">
+      <c r="Y81" s="66" t="s">
         <v>216</v>
       </c>
     </row>
@@ -16021,7 +18672,7 @@
       <c r="X82" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="Y82" s="68"/>
+      <c r="Y82" s="67"/>
     </row>
     <row r="83" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83" s="39" t="s">
@@ -16378,33 +19029,33 @@
       <c r="A92" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="B92" s="60" t="s">
+      <c r="B92" s="59" t="s">
         <v>211</v>
       </c>
-      <c r="C92" s="61"/>
-      <c r="D92" s="61" t="s">
+      <c r="C92" s="60"/>
+      <c r="D92" s="60" t="s">
         <v>124</v>
       </c>
-      <c r="E92" s="61"/>
-      <c r="F92" s="61"/>
-      <c r="G92" s="61"/>
-      <c r="H92" s="61"/>
-      <c r="I92" s="61"/>
-      <c r="J92" s="61"/>
-      <c r="K92" s="61"/>
-      <c r="L92" s="61"/>
-      <c r="M92" s="61"/>
-      <c r="N92" s="61"/>
-      <c r="O92" s="61"/>
-      <c r="P92" s="61"/>
-      <c r="Q92" s="61"/>
-      <c r="R92" s="61"/>
-      <c r="S92" s="61"/>
-      <c r="T92" s="61"/>
-      <c r="U92" s="61"/>
-      <c r="V92" s="61"/>
-      <c r="W92" s="61"/>
-      <c r="X92" s="61"/>
+      <c r="E92" s="60"/>
+      <c r="F92" s="60"/>
+      <c r="G92" s="60"/>
+      <c r="H92" s="60"/>
+      <c r="I92" s="60"/>
+      <c r="J92" s="60"/>
+      <c r="K92" s="60"/>
+      <c r="L92" s="60"/>
+      <c r="M92" s="60"/>
+      <c r="N92" s="60"/>
+      <c r="O92" s="60"/>
+      <c r="P92" s="60"/>
+      <c r="Q92" s="60"/>
+      <c r="R92" s="60"/>
+      <c r="S92" s="60"/>
+      <c r="T92" s="60"/>
+      <c r="U92" s="60"/>
+      <c r="V92" s="60"/>
+      <c r="W92" s="60"/>
+      <c r="X92" s="60"/>
       <c r="Y92" s="55"/>
     </row>
     <row r="93" spans="1:25" s="52" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -16473,12 +19124,12 @@
       <c r="X94" s="36"/>
       <c r="Y94" s="30"/>
     </row>
-    <row r="95" spans="1:25" s="64" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:25" s="63" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A95" s="35" t="s">
         <v>61</v>
       </c>
       <c r="B95" s="35" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C95" s="36"/>
       <c r="D95" s="37" t="s">
@@ -16504,7 +19155,7 @@
       <c r="V95" s="36"/>
       <c r="W95" s="36"/>
       <c r="X95" s="36"/>
-      <c r="Y95" s="63"/>
+      <c r="Y95" s="62"/>
     </row>
     <row r="96" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A96" s="35" t="s">
@@ -16597,8 +19248,8 @@
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C19" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="B25" sqref="B25"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C37" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="D45" sqref="D45"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>

</xml_diff>

<commit_message>
Lisää oikeudet paikkausnäkymiin ja nosta excelistä luettavien rivien määrää 100 -> 1000
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -1,33 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarihan/Jari/Tyo/Solita/Projektit/Harja/harja/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joonasmi/projects/harja/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="27200" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="26980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
     <sheet name="Roolit" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$98</definedName>
-    <definedName name="Z_1DD617EE_F308_3E45_A8EF_4713F47FA0DD_.wvu.FilterData" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$98</definedName>
-    <definedName name="Z_7A9649F2_657F_9445_B6E6_FE94C6A09957_.wvu.FilterData" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$98</definedName>
-    <definedName name="Z_F86DF6F3_8AE5_3A44_B2D2_D623E01AE54F_.wvu.FilterData" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$98</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$100</definedName>
+    <definedName name="Z_1DD617EE_F308_3E45_A8EF_4713F47FA0DD_.wvu.FilterData" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$100</definedName>
+    <definedName name="Z_7A9649F2_657F_9445_B6E6_FE94C6A09957_.wvu.FilterData" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$100</definedName>
+    <definedName name="Z_F86DF6F3_8AE5_3A44_B2D2_D623E01AE54F_.wvu.FilterData" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$100</definedName>
   </definedNames>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" yWindow="22" windowWidth="2560" windowHeight="1360" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2560" windowHeight="1176" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Mikko Rönkkömäki - Personal View" guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" mergeInterval="0" personalView="1" windowWidth="2560" windowHeight="1071" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office -käyttäjä - Oma näkymä" guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="1149" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
-    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Microsoft Office -käyttäjä - Oma näkymä" guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="1149" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Mikko Rönkkömäki - Personal View" guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" mergeInterval="0" personalView="1" windowWidth="2560" windowHeight="1071" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -46,7 +46,7 @@
     <author>Tatu Tarvainen</author>
   </authors>
   <commentList>
-    <comment ref="N31" authorId="0" guid="{DB5603A0-3291-7849-94B2-B86D15FBE193}" shapeId="0">
+    <comment ref="N31" authorId="0" guid="{DB5603A0-3291-7849-94B2-B86D15FBE193}">
       <text>
         <r>
           <rPr>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1511" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1517" uniqueCount="237">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -779,12 +779,18 @@
   </si>
   <si>
     <t>Vastaanottotarkastusraportti</t>
+  </si>
+  <si>
+    <t>Paikkaukset / Toteumat</t>
+  </si>
+  <si>
+    <t>Paikkaukset / Kustannukset</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -897,7 +903,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -951,6 +957,30 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1157,7 +1187,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -1291,6 +1321,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1311,8 +1345,14 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="201">
@@ -1532,7 +1572,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{23AC25BB-AA9F-4242-ACBB-939A4FE9E51A}" diskRevisions="1" revisionId="844" version="53">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{CBB67C01-AFBA-E149-B685-A2E5778AB3B4}" diskRevisions="1" revisionId="853" version="54">
   <header guid="{1E352813-0B26-DB4E-84BE-460845B77133}" dateTime="2017-06-20T12:32:37" maxSheetId="3" userName="Microsoft Office -käyttäjä" r:id="rId60" minRId="448" maxRId="464">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1851,6 +1891,12 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{CBB67C01-AFBA-E149-B685-A2E5778AB3B4}" dateTime="2018-03-21T16:46:29" maxSheetId="3" userName="Microsoft Office User" r:id="rId113" minRId="845" maxRId="852">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -13174,6 +13220,1743 @@
   <rdn rId="0" localSheetId="1" customView="1" name="Z_7A9649F2_657F_9445_B6E6_FE94C6A09957_.wvu.FilterData" hidden="1" oldHidden="1">
     <formula>Oikeudet!$A$5:$Y$98</formula>
     <oldFormula>Oikeudet!$A$5:$Y$98</oldFormula>
+  </rdn>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog51.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="845" sId="1" ref="A53:XFD53" action="insertRow"/>
+  <rrc rId="846" sId="1" ref="A53:XFD53" action="insertRow"/>
+  <rfmt sheetId="1" sqref="A53" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="B53" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C53" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D53" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="E53" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="F53" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="G53" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="H53" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="I53" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="J53" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="K53" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="L53" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="M53" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="N53" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="O53" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="P53" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="Q53" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="R53" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="S53" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="T53" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="U53" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="V53" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="W53" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="X53" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="Y53" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="A54" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="B54" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="C54" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="D54" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="E54" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="F54" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="G54" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="H54" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="I54" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="J54" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="K54" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="L54" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="M54" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="N54" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="O54" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="P54" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="Q54" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="R54" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="S54" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="T54" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="U54" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="V54" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="W54" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="X54" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="Y54" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="847" sId="1" xfDxf="1" dxf="1">
+    <nc r="A53" t="inlineStr">
+      <is>
+        <t>Urakat</t>
+      </is>
+    </nc>
+    <ndxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rcc rId="848" sId="1" xfDxf="1" dxf="1">
+    <nc r="B53" t="inlineStr">
+      <is>
+        <t>Paikkaukset / Toteumat</t>
+      </is>
+    </nc>
+    <ndxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rfmt sheetId="1" xfDxf="1" sqref="C53" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rcc rId="849" sId="1" xfDxf="1" dxf="1">
+    <nc r="D53" t="inlineStr">
+      <is>
+        <t>R*,W*</t>
+      </is>
+    </nc>
+    <ndxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rfmt sheetId="1" xfDxf="1" sqref="E53" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="F53" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="G53" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="H53" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="I53" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="J53" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="K53" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="L53" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="M53" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="N53" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="O53" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="P53" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="Q53" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="R53" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="S53" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="T53" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="U53" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="V53" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="W53" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="X53" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="Y53" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment vertical="top" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rcc rId="850" sId="1" xfDxf="1" dxf="1">
+    <nc r="A54" t="inlineStr">
+      <is>
+        <t>Urakat</t>
+      </is>
+    </nc>
+    <ndxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rcc rId="851" sId="1" xfDxf="1" dxf="1">
+    <nc r="B54" t="inlineStr">
+      <is>
+        <t>Paikkaukset / Kustannukset</t>
+      </is>
+    </nc>
+    <ndxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rfmt sheetId="1" xfDxf="1" sqref="C54" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rcc rId="852" sId="1" xfDxf="1" dxf="1">
+    <nc r="D54" t="inlineStr">
+      <is>
+        <t>R*,W*</t>
+      </is>
+    </nc>
+    <ndxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rfmt sheetId="1" xfDxf="1" sqref="E54" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="F54" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="G54" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="H54" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="I54" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="J54" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="K54" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="L54" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="M54" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="N54" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="O54" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="P54" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="Q54" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="R54" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="S54" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="T54" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="U54" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="V54" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="W54" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="X54" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment horizontal="center" vertical="top" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" xfDxf="1" sqref="Y54" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <alignment vertical="top" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="delete"/>
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_7A9649F2_657F_9445_B6E6_FE94C6A09957_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Oikeudet!$A$5:$Y$100</formula>
+    <oldFormula>Oikeudet!$A$5:$Y$100</oldFormula>
   </rdn>
   <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="add"/>
 </revisions>
@@ -14037,13 +15820,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y98"/>
+  <dimension ref="A1:Y100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C57" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C35" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B82" sqref="B82"/>
+      <selection pane="bottomRight" activeCell="A53" sqref="A53:Y54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -14080,40 +15863,40 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="73" t="s">
+      <c r="C1" s="75" t="s">
         <v>149</v>
       </c>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
-      <c r="L1" s="74"/>
-      <c r="M1" s="74"/>
-      <c r="N1" s="74"/>
-      <c r="O1" s="74"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="75" t="s">
+      <c r="C2" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="76"/>
-      <c r="L2" s="76"/>
-      <c r="M2" s="76"/>
-      <c r="N2" s="76"/>
-      <c r="O2" s="76"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
+      <c r="N2" s="78"/>
+      <c r="O2" s="78"/>
     </row>
     <row r="3" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
@@ -14136,34 +15919,34 @@
     <row r="5" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="30"/>
       <c r="B5" s="30"/>
-      <c r="C5" s="71" t="s">
+      <c r="C5" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="72"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="74"/>
       <c r="I5" s="30"/>
       <c r="J5" s="30"/>
-      <c r="K5" s="71" t="s">
+      <c r="K5" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="L5" s="72"/>
-      <c r="M5" s="72"/>
-      <c r="N5" s="72"/>
-      <c r="O5" s="72"/>
+      <c r="L5" s="74"/>
+      <c r="M5" s="74"/>
+      <c r="N5" s="74"/>
+      <c r="O5" s="74"/>
       <c r="P5" s="30"/>
       <c r="Q5" s="30"/>
-      <c r="R5" s="71" t="s">
+      <c r="R5" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="S5" s="72"/>
-      <c r="T5" s="72"/>
-      <c r="U5" s="72"/>
-      <c r="V5" s="72"/>
-      <c r="W5" s="72"/>
-      <c r="X5" s="72"/>
+      <c r="S5" s="74"/>
+      <c r="T5" s="74"/>
+      <c r="U5" s="74"/>
+      <c r="V5" s="74"/>
+      <c r="W5" s="74"/>
+      <c r="X5" s="74"/>
       <c r="Y5" s="31" t="s">
         <v>13</v>
       </c>
@@ -16937,112 +18720,78 @@
       <c r="X52" s="37"/>
       <c r="Y52" s="38"/>
     </row>
-    <row r="53" spans="1:25" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="B53" s="39" t="s">
-        <v>121</v>
-      </c>
-      <c r="C53" s="37"/>
-      <c r="D53" s="36" t="s">
-        <v>125</v>
-      </c>
-      <c r="E53" s="36" t="s">
-        <v>125</v>
-      </c>
-      <c r="F53" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="G53" s="37"/>
-      <c r="H53" s="37"/>
-      <c r="I53" s="37"/>
-      <c r="J53" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="K53" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="L53" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="M53" s="37"/>
-      <c r="N53" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="O53" s="37"/>
-      <c r="P53" s="37"/>
-      <c r="Q53" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="R53" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="S53" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="T53" s="37"/>
-      <c r="U53" s="37"/>
-      <c r="V53" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="W53" s="37"/>
-      <c r="X53" s="37"/>
-      <c r="Y53" s="38"/>
+    <row r="53" spans="1:25" s="69" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A53" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="B53" s="59" t="s">
+        <v>235</v>
+      </c>
+      <c r="C53" s="60"/>
+      <c r="D53" s="60" t="s">
+        <v>124</v>
+      </c>
+      <c r="E53" s="60"/>
+      <c r="F53" s="60"/>
+      <c r="G53" s="60"/>
+      <c r="H53" s="60"/>
+      <c r="I53" s="60"/>
+      <c r="J53" s="60"/>
+      <c r="K53" s="60"/>
+      <c r="L53" s="60"/>
+      <c r="M53" s="60"/>
+      <c r="N53" s="60"/>
+      <c r="O53" s="60"/>
+      <c r="P53" s="60"/>
+      <c r="Q53" s="60"/>
+      <c r="R53" s="60"/>
+      <c r="S53" s="60"/>
+      <c r="T53" s="60"/>
+      <c r="U53" s="60"/>
+      <c r="V53" s="60"/>
+      <c r="W53" s="60"/>
+      <c r="X53" s="60"/>
+      <c r="Y53" s="55"/>
     </row>
-    <row r="54" spans="1:25" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="B54" s="39" t="s">
-        <v>201</v>
-      </c>
-      <c r="C54" s="37"/>
-      <c r="D54" s="36" t="s">
-        <v>125</v>
-      </c>
-      <c r="E54" s="36" t="s">
-        <v>125</v>
-      </c>
-      <c r="F54" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="G54" s="37"/>
-      <c r="H54" s="37"/>
-      <c r="I54" s="37"/>
-      <c r="J54" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="K54" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="L54" s="37"/>
-      <c r="M54" s="37"/>
-      <c r="N54" s="37"/>
-      <c r="O54" s="37"/>
-      <c r="P54" s="37"/>
-      <c r="Q54" s="37"/>
-      <c r="R54" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="S54" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="T54" s="37"/>
-      <c r="U54" s="37"/>
-      <c r="V54" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="W54" s="37"/>
-      <c r="X54" s="37"/>
-      <c r="Y54" s="38"/>
+    <row r="54" spans="1:25" s="69" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A54" s="79" t="s">
+        <v>14</v>
+      </c>
+      <c r="B54" s="80" t="s">
+        <v>236</v>
+      </c>
+      <c r="C54" s="81"/>
+      <c r="D54" s="81" t="s">
+        <v>124</v>
+      </c>
+      <c r="E54" s="81"/>
+      <c r="F54" s="81"/>
+      <c r="G54" s="81"/>
+      <c r="H54" s="81"/>
+      <c r="I54" s="81"/>
+      <c r="J54" s="81"/>
+      <c r="K54" s="81"/>
+      <c r="L54" s="81"/>
+      <c r="M54" s="81"/>
+      <c r="N54" s="81"/>
+      <c r="O54" s="81"/>
+      <c r="P54" s="81"/>
+      <c r="Q54" s="81"/>
+      <c r="R54" s="81"/>
+      <c r="S54" s="81"/>
+      <c r="T54" s="81"/>
+      <c r="U54" s="81"/>
+      <c r="V54" s="81"/>
+      <c r="W54" s="81"/>
+      <c r="X54" s="81"/>
+      <c r="Y54" s="55"/>
     </row>
-    <row r="55" spans="1:25" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:25" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B55" s="39" t="s">
-        <v>170</v>
+        <v>121</v>
       </c>
       <c r="C55" s="37"/>
       <c r="D55" s="36" t="s">
@@ -17090,26 +18839,24 @@
       <c r="X55" s="37"/>
       <c r="Y55" s="38"/>
     </row>
-    <row r="56" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:25" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B56" s="39" t="s">
-        <v>43</v>
+        <v>201</v>
       </c>
       <c r="C56" s="37"/>
-      <c r="D56" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="E56" s="37" t="s">
+      <c r="D56" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="E56" s="36" t="s">
         <v>125</v>
       </c>
       <c r="F56" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="G56" s="37" t="s">
-        <v>18</v>
-      </c>
+      <c r="G56" s="37"/>
       <c r="H56" s="37"/>
       <c r="I56" s="37"/>
       <c r="J56" s="37" t="s">
@@ -17118,18 +18865,12 @@
       <c r="K56" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="L56" s="37" t="s">
-        <v>125</v>
-      </c>
+      <c r="L56" s="37"/>
       <c r="M56" s="37"/>
-      <c r="N56" s="37" t="s">
-        <v>125</v>
-      </c>
+      <c r="N56" s="37"/>
       <c r="O56" s="37"/>
       <c r="P56" s="37"/>
-      <c r="Q56" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="Q56" s="37"/>
       <c r="R56" s="37" t="s">
         <v>129</v>
       </c>
@@ -17145,32 +18886,26 @@
       <c r="X56" s="37"/>
       <c r="Y56" s="38"/>
     </row>
-    <row r="57" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:25" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B57" s="39" t="s">
-        <v>44</v>
+        <v>170</v>
       </c>
       <c r="C57" s="37"/>
-      <c r="D57" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="E57" s="37" t="s">
+      <c r="D57" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="E57" s="36" t="s">
         <v>125</v>
       </c>
       <c r="F57" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="G57" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="H57" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="I57" s="37" t="s">
-        <v>125</v>
-      </c>
+      <c r="G57" s="37"/>
+      <c r="H57" s="37"/>
+      <c r="I57" s="37"/>
       <c r="J57" s="37" t="s">
         <v>16</v>
       </c>
@@ -17180,18 +18915,12 @@
       <c r="L57" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="M57" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="M57" s="37"/>
       <c r="N57" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="O57" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="P57" s="37" t="s">
-        <v>125</v>
-      </c>
+      <c r="O57" s="37"/>
+      <c r="P57" s="37"/>
       <c r="Q57" s="37" t="s">
         <v>16</v>
       </c>
@@ -17201,27 +18930,21 @@
       <c r="S57" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="T57" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="U57" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="T57" s="37"/>
+      <c r="U57" s="37"/>
       <c r="V57" s="37" t="s">
         <v>129</v>
       </c>
       <c r="W57" s="37"/>
-      <c r="X57" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="X57" s="37"/>
       <c r="Y57" s="38"/>
     </row>
-    <row r="58" spans="1:25" s="17" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B58" s="39" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C58" s="37"/>
       <c r="D58" s="37" t="s">
@@ -17234,14 +18957,10 @@
         <v>125</v>
       </c>
       <c r="G58" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="H58" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="I58" s="37" t="s">
-        <v>125</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="H58" s="37"/>
+      <c r="I58" s="37"/>
       <c r="J58" s="37" t="s">
         <v>16</v>
       </c>
@@ -17251,18 +18970,12 @@
       <c r="L58" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="M58" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="M58" s="37"/>
       <c r="N58" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="O58" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="P58" s="37" t="s">
-        <v>125</v>
-      </c>
+      <c r="O58" s="37"/>
+      <c r="P58" s="37"/>
       <c r="Q58" s="37" t="s">
         <v>16</v>
       </c>
@@ -17272,21 +18985,13 @@
       <c r="S58" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="T58" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="U58" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="T58" s="37"/>
+      <c r="U58" s="37"/>
       <c r="V58" s="37" t="s">
         <v>129</v>
       </c>
-      <c r="W58" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="X58" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="W58" s="37"/>
+      <c r="X58" s="37"/>
       <c r="Y58" s="38"/>
     </row>
     <row r="59" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -17294,7 +18999,7 @@
         <v>42</v>
       </c>
       <c r="B59" s="39" t="s">
-        <v>146</v>
+        <v>44</v>
       </c>
       <c r="C59" s="37"/>
       <c r="D59" s="37" t="s">
@@ -17360,12 +19065,12 @@
       </c>
       <c r="Y59" s="38"/>
     </row>
-    <row r="60" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:25" s="17" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B60" s="39" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C60" s="37"/>
       <c r="D60" s="37" t="s">
@@ -17425,7 +19130,9 @@
       <c r="V60" s="37" t="s">
         <v>129</v>
       </c>
-      <c r="W60" s="37"/>
+      <c r="W60" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="X60" s="37" t="s">
         <v>16</v>
       </c>
@@ -17436,7 +19143,7 @@
         <v>42</v>
       </c>
       <c r="B61" s="39" t="s">
-        <v>47</v>
+        <v>146</v>
       </c>
       <c r="C61" s="37"/>
       <c r="D61" s="37" t="s">
@@ -17502,12 +19209,12 @@
       </c>
       <c r="Y61" s="38"/>
     </row>
-    <row r="62" spans="1:25" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B62" s="39" t="s">
-        <v>153</v>
+        <v>46</v>
       </c>
       <c r="C62" s="37"/>
       <c r="D62" s="37" t="s">
@@ -17578,7 +19285,7 @@
         <v>42</v>
       </c>
       <c r="B63" s="39" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C63" s="37"/>
       <c r="D63" s="37" t="s">
@@ -17644,12 +19351,12 @@
       </c>
       <c r="Y63" s="38"/>
     </row>
-    <row r="64" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:25" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B64" s="39" t="s">
-        <v>49</v>
+        <v>153</v>
       </c>
       <c r="C64" s="37"/>
       <c r="D64" s="37" t="s">
@@ -17685,7 +19392,9 @@
       <c r="N64" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="O64" s="37"/>
+      <c r="O64" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="P64" s="37" t="s">
         <v>125</v>
       </c>
@@ -17718,7 +19427,7 @@
         <v>42</v>
       </c>
       <c r="B65" s="39" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C65" s="37"/>
       <c r="D65" s="37" t="s">
@@ -17789,7 +19498,7 @@
         <v>42</v>
       </c>
       <c r="B66" s="39" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C66" s="37"/>
       <c r="D66" s="37" t="s">
@@ -17801,8 +19510,12 @@
       <c r="F66" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="G66" s="37"/>
-      <c r="H66" s="37"/>
+      <c r="G66" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="H66" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="I66" s="37" t="s">
         <v>125</v>
       </c>
@@ -17815,7 +19528,9 @@
       <c r="L66" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="M66" s="37"/>
+      <c r="M66" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="N66" s="37" t="s">
         <v>125</v>
       </c>
@@ -17852,7 +19567,7 @@
         <v>42</v>
       </c>
       <c r="B67" s="39" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C67" s="37"/>
       <c r="D67" s="37" t="s">
@@ -17864,11 +19579,15 @@
       <c r="F67" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="G67" s="37"/>
+      <c r="G67" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="H67" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="I67" s="37"/>
+        <v>125</v>
+      </c>
+      <c r="I67" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="J67" s="37" t="s">
         <v>16</v>
       </c>
@@ -17878,14 +19597,18 @@
       <c r="L67" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="M67" s="37"/>
+      <c r="M67" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="N67" s="37" t="s">
         <v>125</v>
       </c>
       <c r="O67" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="P67" s="37"/>
+        <v>125</v>
+      </c>
+      <c r="P67" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="Q67" s="37" t="s">
         <v>16</v>
       </c>
@@ -17895,13 +19618,19 @@
       <c r="S67" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="T67" s="37"/>
-      <c r="U67" s="37"/>
+      <c r="T67" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="U67" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="V67" s="37" t="s">
         <v>129</v>
       </c>
       <c r="W67" s="37"/>
-      <c r="X67" s="37"/>
+      <c r="X67" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="Y67" s="38"/>
     </row>
     <row r="68" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -17909,7 +19638,7 @@
         <v>42</v>
       </c>
       <c r="B68" s="39" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C68" s="37"/>
       <c r="D68" s="37" t="s">
@@ -17923,7 +19652,9 @@
       </c>
       <c r="G68" s="37"/>
       <c r="H68" s="37"/>
-      <c r="I68" s="37"/>
+      <c r="I68" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="J68" s="37" t="s">
         <v>16</v>
       </c>
@@ -17938,7 +19669,9 @@
         <v>125</v>
       </c>
       <c r="O68" s="37"/>
-      <c r="P68" s="37"/>
+      <c r="P68" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="Q68" s="37" t="s">
         <v>16</v>
       </c>
@@ -17948,13 +19681,19 @@
       <c r="S68" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="T68" s="37"/>
-      <c r="U68" s="37"/>
+      <c r="T68" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="U68" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="V68" s="37" t="s">
         <v>129</v>
       </c>
       <c r="W68" s="37"/>
-      <c r="X68" s="37"/>
+      <c r="X68" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="Y68" s="38"/>
     </row>
     <row r="69" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -17962,7 +19701,7 @@
         <v>42</v>
       </c>
       <c r="B69" s="39" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C69" s="37"/>
       <c r="D69" s="37" t="s">
@@ -17975,7 +19714,9 @@
         <v>125</v>
       </c>
       <c r="G69" s="37"/>
-      <c r="H69" s="37"/>
+      <c r="H69" s="37" t="s">
+        <v>18</v>
+      </c>
       <c r="I69" s="37"/>
       <c r="J69" s="37" t="s">
         <v>16</v>
@@ -17990,7 +19731,9 @@
       <c r="N69" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="O69" s="37"/>
+      <c r="O69" s="37" t="s">
+        <v>18</v>
+      </c>
       <c r="P69" s="37"/>
       <c r="Q69" s="37" t="s">
         <v>16</v>
@@ -18015,7 +19758,7 @@
         <v>42</v>
       </c>
       <c r="B70" s="39" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C70" s="37"/>
       <c r="D70" s="37" t="s">
@@ -18063,12 +19806,12 @@
       <c r="X70" s="37"/>
       <c r="Y70" s="38"/>
     </row>
-    <row r="71" spans="1:25" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B71" s="39" t="s">
-        <v>119</v>
+        <v>54</v>
       </c>
       <c r="C71" s="37"/>
       <c r="D71" s="37" t="s">
@@ -18080,15 +19823,9 @@
       <c r="F71" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="G71" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="H71" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="I71" s="37" t="s">
-        <v>125</v>
-      </c>
+      <c r="G71" s="37"/>
+      <c r="H71" s="37"/>
+      <c r="I71" s="37"/>
       <c r="J71" s="37" t="s">
         <v>16</v>
       </c>
@@ -18098,16 +19835,12 @@
       <c r="L71" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="M71" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="M71" s="37"/>
       <c r="N71" s="37" t="s">
         <v>125</v>
       </c>
       <c r="O71" s="37"/>
-      <c r="P71" s="37" t="s">
-        <v>125</v>
-      </c>
+      <c r="P71" s="37"/>
       <c r="Q71" s="37" t="s">
         <v>16</v>
       </c>
@@ -18117,27 +19850,21 @@
       <c r="S71" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="T71" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="U71" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="T71" s="37"/>
+      <c r="U71" s="37"/>
       <c r="V71" s="37" t="s">
         <v>129</v>
       </c>
       <c r="W71" s="37"/>
-      <c r="X71" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="X71" s="37"/>
       <c r="Y71" s="38"/>
     </row>
-    <row r="72" spans="1:25" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B72" s="39" t="s">
-        <v>171</v>
+        <v>55</v>
       </c>
       <c r="C72" s="37"/>
       <c r="D72" s="37" t="s">
@@ -18149,15 +19876,9 @@
       <c r="F72" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="G72" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="H72" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="I72" s="37" t="s">
-        <v>125</v>
-      </c>
+      <c r="G72" s="37"/>
+      <c r="H72" s="37"/>
+      <c r="I72" s="37"/>
       <c r="J72" s="37" t="s">
         <v>16</v>
       </c>
@@ -18167,16 +19888,12 @@
       <c r="L72" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="M72" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="M72" s="37"/>
       <c r="N72" s="37" t="s">
         <v>125</v>
       </c>
       <c r="O72" s="37"/>
-      <c r="P72" s="37" t="s">
-        <v>125</v>
-      </c>
+      <c r="P72" s="37"/>
       <c r="Q72" s="37" t="s">
         <v>16</v>
       </c>
@@ -18186,27 +19903,21 @@
       <c r="S72" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="T72" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="U72" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="T72" s="37"/>
+      <c r="U72" s="37"/>
       <c r="V72" s="37" t="s">
         <v>129</v>
       </c>
       <c r="W72" s="37"/>
-      <c r="X72" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="X72" s="37"/>
       <c r="Y72" s="38"/>
     </row>
-    <row r="73" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:25" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B73" s="39" t="s">
-        <v>56</v>
+        <v>119</v>
       </c>
       <c r="C73" s="37"/>
       <c r="D73" s="37" t="s">
@@ -18242,9 +19953,7 @@
       <c r="N73" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="O73" s="37" t="s">
-        <v>125</v>
-      </c>
+      <c r="O73" s="37"/>
       <c r="P73" s="37" t="s">
         <v>125</v>
       </c>
@@ -18272,12 +19981,12 @@
       </c>
       <c r="Y73" s="38"/>
     </row>
-    <row r="74" spans="1:25" s="17" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:25" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B74" s="39" t="s">
-        <v>123</v>
+        <v>171</v>
       </c>
       <c r="C74" s="37"/>
       <c r="D74" s="37" t="s">
@@ -18313,9 +20022,7 @@
       <c r="N74" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="O74" s="37" t="s">
-        <v>125</v>
-      </c>
+      <c r="O74" s="37"/>
       <c r="P74" s="37" t="s">
         <v>125</v>
       </c>
@@ -18338,15 +20045,17 @@
         <v>129</v>
       </c>
       <c r="W74" s="37"/>
-      <c r="X74" s="37"/>
+      <c r="X74" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="Y74" s="38"/>
     </row>
-    <row r="75" spans="1:25" s="17" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B75" s="39" t="s">
-        <v>141</v>
+        <v>56</v>
       </c>
       <c r="C75" s="37"/>
       <c r="D75" s="37" t="s">
@@ -18407,7 +20116,9 @@
         <v>129</v>
       </c>
       <c r="W75" s="37"/>
-      <c r="X75" s="37"/>
+      <c r="X75" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="Y75" s="38"/>
     </row>
     <row r="76" spans="1:25" s="17" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -18415,7 +20126,7 @@
         <v>42</v>
       </c>
       <c r="B76" s="39" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="C76" s="37"/>
       <c r="D76" s="37" t="s">
@@ -18484,7 +20195,7 @@
         <v>42</v>
       </c>
       <c r="B77" s="39" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C77" s="37"/>
       <c r="D77" s="37" t="s">
@@ -18553,7 +20264,7 @@
         <v>42</v>
       </c>
       <c r="B78" s="39" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C78" s="37"/>
       <c r="D78" s="37" t="s">
@@ -18617,26 +20328,32 @@
       <c r="X78" s="37"/>
       <c r="Y78" s="38"/>
     </row>
-    <row r="79" spans="1:25" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:25" s="17" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B79" s="39" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C79" s="37"/>
-      <c r="D79" s="36" t="s">
-        <v>125</v>
-      </c>
-      <c r="E79" s="36" t="s">
+      <c r="D79" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="E79" s="37" t="s">
         <v>125</v>
       </c>
       <c r="F79" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="G79" s="37"/>
-      <c r="H79" s="37"/>
-      <c r="I79" s="37"/>
+      <c r="G79" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="H79" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="I79" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="J79" s="37" t="s">
         <v>16</v>
       </c>
@@ -18646,12 +20363,18 @@
       <c r="L79" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="M79" s="37"/>
+      <c r="M79" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="N79" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="O79" s="37"/>
-      <c r="P79" s="37"/>
+      <c r="O79" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="P79" s="37" t="s">
+        <v>125</v>
+      </c>
       <c r="Q79" s="37" t="s">
         <v>16</v>
       </c>
@@ -18661,19 +20384,25 @@
       <c r="S79" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="T79" s="37"/>
-      <c r="U79" s="37"/>
-      <c r="V79" s="37"/>
+      <c r="T79" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="U79" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="V79" s="37" t="s">
+        <v>129</v>
+      </c>
       <c r="W79" s="37"/>
       <c r="X79" s="37"/>
       <c r="Y79" s="38"/>
     </row>
-    <row r="80" spans="1:25" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:25" s="17" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B80" s="39" t="s">
-        <v>186</v>
+        <v>144</v>
       </c>
       <c r="C80" s="37"/>
       <c r="D80" s="37" t="s">
@@ -18737,12 +20466,12 @@
       <c r="X80" s="37"/>
       <c r="Y80" s="38"/>
     </row>
-    <row r="81" spans="1:25" s="68" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:25" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A81" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="B81" s="77" t="s">
-        <v>234</v>
+      <c r="B81" s="39" t="s">
+        <v>145</v>
       </c>
       <c r="C81" s="37"/>
       <c r="D81" s="36" t="s">
@@ -18783,19 +20512,17 @@
       </c>
       <c r="T81" s="37"/>
       <c r="U81" s="37"/>
-      <c r="V81" s="37" t="s">
-        <v>129</v>
-      </c>
+      <c r="V81" s="37"/>
       <c r="W81" s="37"/>
       <c r="X81" s="37"/>
-      <c r="Y81" s="55"/>
+      <c r="Y81" s="38"/>
     </row>
-    <row r="82" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:25" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A82" s="39" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="B82" s="39" t="s">
-        <v>58</v>
+        <v>186</v>
       </c>
       <c r="C82" s="37"/>
       <c r="D82" s="37" t="s">
@@ -18817,7 +20544,7 @@
         <v>125</v>
       </c>
       <c r="J82" s="37" t="s">
-        <v>214</v>
+        <v>16</v>
       </c>
       <c r="K82" s="37" t="s">
         <v>125</v>
@@ -18838,13 +20565,13 @@
         <v>125</v>
       </c>
       <c r="Q82" s="37" t="s">
-        <v>214</v>
+        <v>16</v>
       </c>
       <c r="R82" s="37" t="s">
-        <v>215</v>
+        <v>129</v>
       </c>
       <c r="S82" s="37" t="s">
-        <v>214</v>
+        <v>16</v>
       </c>
       <c r="T82" s="37" t="s">
         <v>129</v>
@@ -18855,101 +20582,75 @@
       <c r="V82" s="37" t="s">
         <v>129</v>
       </c>
-      <c r="W82" s="37" t="s">
+      <c r="W82" s="37"/>
+      <c r="X82" s="37"/>
+      <c r="Y82" s="38"/>
+    </row>
+    <row r="83" spans="1:25" s="68" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A83" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B83" s="70" t="s">
+        <v>234</v>
+      </c>
+      <c r="C83" s="37"/>
+      <c r="D83" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="E83" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="F83" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="G83" s="37"/>
+      <c r="H83" s="37"/>
+      <c r="I83" s="37"/>
+      <c r="J83" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="X82" s="37" t="s">
+      <c r="K83" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="L83" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="M83" s="37"/>
+      <c r="N83" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="O83" s="37"/>
+      <c r="P83" s="37"/>
+      <c r="Q83" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="Y82" s="69" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="83" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A83" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="B83" s="39" t="s">
-        <v>59</v>
-      </c>
-      <c r="C83" s="37"/>
-      <c r="D83" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="E83" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="F83" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="G83" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="H83" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="I83" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="J83" s="37" t="s">
-        <v>214</v>
-      </c>
-      <c r="K83" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="L83" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="M83" s="37" t="s">
+      <c r="R83" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="S83" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="N83" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="O83" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="P83" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="Q83" s="37" t="s">
-        <v>214</v>
-      </c>
-      <c r="R83" s="37" t="s">
-        <v>215</v>
-      </c>
-      <c r="S83" s="37" t="s">
-        <v>214</v>
-      </c>
-      <c r="T83" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="U83" s="37" t="s">
-        <v>16</v>
-      </c>
+      <c r="T83" s="37"/>
+      <c r="U83" s="37"/>
       <c r="V83" s="37" t="s">
         <v>129</v>
       </c>
-      <c r="W83" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="X83" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y83" s="70"/>
+      <c r="W83" s="37"/>
+      <c r="X83" s="37"/>
+      <c r="Y83" s="55"/>
     </row>
     <row r="84" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A84" s="39" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B84" s="39" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C84" s="37"/>
       <c r="D84" s="37" t="s">
-        <v>124</v>
-      </c>
-      <c r="E84" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="E84" s="37" t="s">
         <v>125</v>
       </c>
       <c r="F84" s="37" t="s">
@@ -18965,10 +20666,10 @@
         <v>125</v>
       </c>
       <c r="J84" s="37" t="s">
-        <v>16</v>
+        <v>214</v>
       </c>
       <c r="K84" s="37" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="L84" s="37" t="s">
         <v>125</v>
@@ -18986,166 +20687,248 @@
         <v>125</v>
       </c>
       <c r="Q84" s="37" t="s">
-        <v>16</v>
+        <v>214</v>
       </c>
       <c r="R84" s="37" t="s">
-        <v>130</v>
+        <v>215</v>
       </c>
       <c r="S84" s="37" t="s">
-        <v>111</v>
+        <v>214</v>
       </c>
       <c r="T84" s="37" t="s">
         <v>129</v>
       </c>
       <c r="U84" s="37" t="s">
-        <v>111</v>
+        <v>16</v>
       </c>
       <c r="V84" s="37" t="s">
         <v>129</v>
       </c>
       <c r="W84" s="37" t="s">
-        <v>111</v>
+        <v>16</v>
       </c>
       <c r="X84" s="37" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y84" s="38"/>
+        <v>16</v>
+      </c>
+      <c r="Y84" s="71" t="s">
+        <v>216</v>
+      </c>
     </row>
-    <row r="85" spans="1:25" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A85" s="42" t="s">
-        <v>61</v>
-      </c>
-      <c r="B85" s="42" t="s">
-        <v>62</v>
-      </c>
-      <c r="C85" s="43"/>
+    <row r="85" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A85" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="B85" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="C85" s="37"/>
       <c r="D85" s="37" t="s">
-        <v>124</v>
-      </c>
-      <c r="E85" s="43"/>
-      <c r="F85" s="43"/>
-      <c r="G85" s="43"/>
-      <c r="H85" s="43"/>
-      <c r="I85" s="43"/>
-      <c r="J85" s="43"/>
-      <c r="K85" s="43"/>
-      <c r="L85" s="43"/>
-      <c r="M85" s="43"/>
-      <c r="N85" s="43"/>
-      <c r="O85" s="43"/>
-      <c r="P85" s="43"/>
-      <c r="Q85" s="43"/>
-      <c r="R85" s="43"/>
-      <c r="S85" s="43"/>
-      <c r="T85" s="43"/>
-      <c r="U85" s="43"/>
-      <c r="V85" s="43"/>
-      <c r="W85" s="43"/>
-      <c r="X85" s="43"/>
-      <c r="Y85" s="44" t="s">
-        <v>63</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="E85" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="F85" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="G85" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="H85" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="I85" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="J85" s="37" t="s">
+        <v>214</v>
+      </c>
+      <c r="K85" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="L85" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="M85" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="N85" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="O85" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="P85" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q85" s="37" t="s">
+        <v>214</v>
+      </c>
+      <c r="R85" s="37" t="s">
+        <v>215</v>
+      </c>
+      <c r="S85" s="37" t="s">
+        <v>214</v>
+      </c>
+      <c r="T85" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="U85" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="V85" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="W85" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="X85" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y85" s="72"/>
     </row>
     <row r="86" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A86" s="35" t="s">
-        <v>61</v>
-      </c>
-      <c r="B86" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="C86" s="36"/>
+      <c r="A86" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="B86" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="C86" s="37"/>
       <c r="D86" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="E86" s="36"/>
-      <c r="F86" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="G86" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="H86" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="I86" s="36"/>
-      <c r="J86" s="37"/>
-      <c r="K86" s="36"/>
-      <c r="L86" s="36"/>
-      <c r="M86" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="N86" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="O86" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="P86" s="36"/>
-      <c r="Q86" s="37"/>
-      <c r="R86" s="36"/>
-      <c r="S86" s="36"/>
-      <c r="T86" s="36"/>
-      <c r="U86" s="36"/>
-      <c r="V86" s="36"/>
-      <c r="W86" s="36"/>
-      <c r="X86" s="36"/>
-      <c r="Y86" s="30"/>
+      <c r="E86" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="F86" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="G86" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="H86" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="I86" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="J86" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="K86" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="L86" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="M86" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="N86" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="O86" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="P86" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q86" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="R86" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="S86" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="T86" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="U86" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="V86" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="W86" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="X86" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="Y86" s="38"/>
     </row>
-    <row r="87" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A87" s="35" t="s">
+    <row r="87" spans="1:25" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A87" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="B87" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="C87" s="36"/>
+      <c r="B87" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="C87" s="43"/>
       <c r="D87" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="E87" s="36"/>
-      <c r="F87" s="36"/>
-      <c r="G87" s="36"/>
-      <c r="H87" s="36"/>
-      <c r="I87" s="36"/>
-      <c r="J87" s="37"/>
-      <c r="K87" s="36"/>
-      <c r="L87" s="36"/>
-      <c r="M87" s="36"/>
-      <c r="N87" s="36"/>
-      <c r="O87" s="36"/>
-      <c r="P87" s="36"/>
-      <c r="Q87" s="37"/>
-      <c r="R87" s="36"/>
-      <c r="S87" s="36"/>
-      <c r="T87" s="36"/>
-      <c r="U87" s="36"/>
-      <c r="V87" s="36"/>
-      <c r="W87" s="36"/>
-      <c r="X87" s="36"/>
-      <c r="Y87" s="30"/>
+      <c r="E87" s="43"/>
+      <c r="F87" s="43"/>
+      <c r="G87" s="43"/>
+      <c r="H87" s="43"/>
+      <c r="I87" s="43"/>
+      <c r="J87" s="43"/>
+      <c r="K87" s="43"/>
+      <c r="L87" s="43"/>
+      <c r="M87" s="43"/>
+      <c r="N87" s="43"/>
+      <c r="O87" s="43"/>
+      <c r="P87" s="43"/>
+      <c r="Q87" s="43"/>
+      <c r="R87" s="43"/>
+      <c r="S87" s="43"/>
+      <c r="T87" s="43"/>
+      <c r="U87" s="43"/>
+      <c r="V87" s="43"/>
+      <c r="W87" s="43"/>
+      <c r="X87" s="43"/>
+      <c r="Y87" s="44" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="88" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A88" s="35" t="s">
         <v>61</v>
       </c>
       <c r="B88" s="35" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C88" s="36"/>
       <c r="D88" s="37" t="s">
         <v>124</v>
       </c>
       <c r="E88" s="36"/>
-      <c r="F88" s="36"/>
-      <c r="G88" s="36"/>
-      <c r="H88" s="36"/>
+      <c r="F88" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="G88" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="H88" s="36" t="s">
+        <v>18</v>
+      </c>
       <c r="I88" s="36"/>
       <c r="J88" s="37"/>
       <c r="K88" s="36"/>
       <c r="L88" s="36"/>
-      <c r="M88" s="36"/>
-      <c r="N88" s="36"/>
-      <c r="O88" s="36"/>
+      <c r="M88" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="N88" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="O88" s="36" t="s">
+        <v>18</v>
+      </c>
       <c r="P88" s="36"/>
       <c r="Q88" s="37"/>
       <c r="R88" s="36"/>
@@ -19162,7 +20945,7 @@
         <v>61</v>
       </c>
       <c r="B89" s="35" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C89" s="36"/>
       <c r="D89" s="37" t="s">
@@ -19190,12 +20973,12 @@
       <c r="X89" s="36"/>
       <c r="Y89" s="30"/>
     </row>
-    <row r="90" spans="1:25" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A90" s="35" t="s">
         <v>61</v>
       </c>
       <c r="B90" s="35" t="s">
-        <v>164</v>
+        <v>66</v>
       </c>
       <c r="C90" s="36"/>
       <c r="D90" s="37" t="s">
@@ -19223,12 +21006,12 @@
       <c r="X90" s="36"/>
       <c r="Y90" s="30"/>
     </row>
-    <row r="91" spans="1:25" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A91" s="35" t="s">
         <v>61</v>
       </c>
       <c r="B91" s="35" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
       <c r="C91" s="36"/>
       <c r="D91" s="37" t="s">
@@ -19256,12 +21039,12 @@
       <c r="X91" s="36"/>
       <c r="Y91" s="30"/>
     </row>
-    <row r="92" spans="1:25" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:25" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A92" s="35" t="s">
         <v>61</v>
       </c>
       <c r="B92" s="35" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="C92" s="36"/>
       <c r="D92" s="37" t="s">
@@ -19289,45 +21072,45 @@
       <c r="X92" s="36"/>
       <c r="Y92" s="30"/>
     </row>
-    <row r="93" spans="1:25" s="57" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:25" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A93" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="B93" s="59" t="s">
-        <v>211</v>
-      </c>
-      <c r="C93" s="60"/>
-      <c r="D93" s="60" t="s">
+      <c r="B93" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="C93" s="36"/>
+      <c r="D93" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="E93" s="60"/>
-      <c r="F93" s="60"/>
-      <c r="G93" s="60"/>
-      <c r="H93" s="60"/>
-      <c r="I93" s="60"/>
-      <c r="J93" s="60"/>
-      <c r="K93" s="60"/>
-      <c r="L93" s="60"/>
-      <c r="M93" s="60"/>
-      <c r="N93" s="60"/>
-      <c r="O93" s="60"/>
-      <c r="P93" s="60"/>
-      <c r="Q93" s="60"/>
-      <c r="R93" s="60"/>
-      <c r="S93" s="60"/>
-      <c r="T93" s="60"/>
-      <c r="U93" s="60"/>
-      <c r="V93" s="60"/>
-      <c r="W93" s="60"/>
-      <c r="X93" s="60"/>
-      <c r="Y93" s="55"/>
+      <c r="E93" s="36"/>
+      <c r="F93" s="36"/>
+      <c r="G93" s="36"/>
+      <c r="H93" s="36"/>
+      <c r="I93" s="36"/>
+      <c r="J93" s="37"/>
+      <c r="K93" s="36"/>
+      <c r="L93" s="36"/>
+      <c r="M93" s="36"/>
+      <c r="N93" s="36"/>
+      <c r="O93" s="36"/>
+      <c r="P93" s="36"/>
+      <c r="Q93" s="37"/>
+      <c r="R93" s="36"/>
+      <c r="S93" s="36"/>
+      <c r="T93" s="36"/>
+      <c r="U93" s="36"/>
+      <c r="V93" s="36"/>
+      <c r="W93" s="36"/>
+      <c r="X93" s="36"/>
+      <c r="Y93" s="30"/>
     </row>
-    <row r="94" spans="1:25" s="52" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:25" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A94" s="35" t="s">
         <v>61</v>
       </c>
       <c r="B94" s="35" t="s">
-        <v>204</v>
+        <v>179</v>
       </c>
       <c r="C94" s="36"/>
       <c r="D94" s="37" t="s">
@@ -19353,47 +21136,47 @@
       <c r="V94" s="36"/>
       <c r="W94" s="36"/>
       <c r="X94" s="36"/>
-      <c r="Y94" s="51"/>
+      <c r="Y94" s="30"/>
     </row>
-    <row r="95" spans="1:25" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:25" s="57" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A95" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="B95" s="35" t="s">
-        <v>122</v>
-      </c>
-      <c r="C95" s="36"/>
-      <c r="D95" s="37" t="s">
+      <c r="B95" s="59" t="s">
+        <v>211</v>
+      </c>
+      <c r="C95" s="60"/>
+      <c r="D95" s="60" t="s">
         <v>124</v>
       </c>
-      <c r="E95" s="36"/>
-      <c r="F95" s="36"/>
-      <c r="G95" s="36"/>
-      <c r="H95" s="36"/>
-      <c r="I95" s="36"/>
-      <c r="J95" s="37"/>
-      <c r="K95" s="36"/>
-      <c r="L95" s="36"/>
-      <c r="M95" s="36"/>
-      <c r="N95" s="36"/>
-      <c r="O95" s="36"/>
-      <c r="P95" s="36"/>
-      <c r="Q95" s="37"/>
-      <c r="R95" s="36"/>
-      <c r="S95" s="36"/>
-      <c r="T95" s="36"/>
-      <c r="U95" s="36"/>
-      <c r="V95" s="36"/>
-      <c r="W95" s="36"/>
-      <c r="X95" s="36"/>
-      <c r="Y95" s="30"/>
+      <c r="E95" s="60"/>
+      <c r="F95" s="60"/>
+      <c r="G95" s="60"/>
+      <c r="H95" s="60"/>
+      <c r="I95" s="60"/>
+      <c r="J95" s="60"/>
+      <c r="K95" s="60"/>
+      <c r="L95" s="60"/>
+      <c r="M95" s="60"/>
+      <c r="N95" s="60"/>
+      <c r="O95" s="60"/>
+      <c r="P95" s="60"/>
+      <c r="Q95" s="60"/>
+      <c r="R95" s="60"/>
+      <c r="S95" s="60"/>
+      <c r="T95" s="60"/>
+      <c r="U95" s="60"/>
+      <c r="V95" s="60"/>
+      <c r="W95" s="60"/>
+      <c r="X95" s="60"/>
+      <c r="Y95" s="55"/>
     </row>
-    <row r="96" spans="1:25" s="63" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:25" s="52" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A96" s="35" t="s">
         <v>61</v>
       </c>
       <c r="B96" s="35" t="s">
-        <v>224</v>
+        <v>204</v>
       </c>
       <c r="C96" s="36"/>
       <c r="D96" s="37" t="s">
@@ -19419,101 +21202,185 @@
       <c r="V96" s="36"/>
       <c r="W96" s="36"/>
       <c r="X96" s="36"/>
-      <c r="Y96" s="62"/>
+      <c r="Y96" s="51"/>
     </row>
-    <row r="97" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:25" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A97" s="35" t="s">
-        <v>107</v>
+        <v>61</v>
       </c>
       <c r="B97" s="35" t="s">
-        <v>108</v>
-      </c>
-      <c r="C97" s="45"/>
+        <v>122</v>
+      </c>
+      <c r="C97" s="36"/>
       <c r="D97" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="E97" s="45"/>
-      <c r="F97" s="45"/>
-      <c r="G97" s="45"/>
-      <c r="H97" s="45"/>
-      <c r="I97" s="45"/>
-      <c r="J97" s="46"/>
-      <c r="K97" s="45"/>
-      <c r="L97" s="45"/>
-      <c r="M97" s="45"/>
-      <c r="N97" s="45"/>
-      <c r="O97" s="45"/>
-      <c r="P97" s="45"/>
-      <c r="Q97" s="46"/>
-      <c r="R97" s="45"/>
-      <c r="S97" s="45"/>
-      <c r="T97" s="45"/>
-      <c r="U97" s="45"/>
-      <c r="V97" s="45"/>
-      <c r="W97" s="45"/>
-      <c r="X97" s="45"/>
+      <c r="E97" s="36"/>
+      <c r="F97" s="36"/>
+      <c r="G97" s="36"/>
+      <c r="H97" s="36"/>
+      <c r="I97" s="36"/>
+      <c r="J97" s="37"/>
+      <c r="K97" s="36"/>
+      <c r="L97" s="36"/>
+      <c r="M97" s="36"/>
+      <c r="N97" s="36"/>
+      <c r="O97" s="36"/>
+      <c r="P97" s="36"/>
+      <c r="Q97" s="37"/>
+      <c r="R97" s="36"/>
+      <c r="S97" s="36"/>
+      <c r="T97" s="36"/>
+      <c r="U97" s="36"/>
+      <c r="V97" s="36"/>
+      <c r="W97" s="36"/>
+      <c r="X97" s="36"/>
       <c r="Y97" s="30"/>
     </row>
-    <row r="98" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:25" s="63" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A98" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="B98" s="35" t="s">
+        <v>224</v>
+      </c>
+      <c r="C98" s="36"/>
+      <c r="D98" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="E98" s="36"/>
+      <c r="F98" s="36"/>
+      <c r="G98" s="36"/>
+      <c r="H98" s="36"/>
+      <c r="I98" s="36"/>
+      <c r="J98" s="37"/>
+      <c r="K98" s="36"/>
+      <c r="L98" s="36"/>
+      <c r="M98" s="36"/>
+      <c r="N98" s="36"/>
+      <c r="O98" s="36"/>
+      <c r="P98" s="36"/>
+      <c r="Q98" s="37"/>
+      <c r="R98" s="36"/>
+      <c r="S98" s="36"/>
+      <c r="T98" s="36"/>
+      <c r="U98" s="36"/>
+      <c r="V98" s="36"/>
+      <c r="W98" s="36"/>
+      <c r="X98" s="36"/>
+      <c r="Y98" s="62"/>
+    </row>
+    <row r="99" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A99" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="B99" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="C99" s="45"/>
+      <c r="D99" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="E99" s="45"/>
+      <c r="F99" s="45"/>
+      <c r="G99" s="45"/>
+      <c r="H99" s="45"/>
+      <c r="I99" s="45"/>
+      <c r="J99" s="46"/>
+      <c r="K99" s="45"/>
+      <c r="L99" s="45"/>
+      <c r="M99" s="45"/>
+      <c r="N99" s="45"/>
+      <c r="O99" s="45"/>
+      <c r="P99" s="45"/>
+      <c r="Q99" s="46"/>
+      <c r="R99" s="45"/>
+      <c r="S99" s="45"/>
+      <c r="T99" s="45"/>
+      <c r="U99" s="45"/>
+      <c r="V99" s="45"/>
+      <c r="W99" s="45"/>
+      <c r="X99" s="45"/>
+      <c r="Y99" s="30"/>
+    </row>
+    <row r="100" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A100" s="35" t="s">
         <v>117</v>
       </c>
-      <c r="B98" s="35" t="s">
+      <c r="B100" s="35" t="s">
         <v>118</v>
       </c>
-      <c r="C98" s="45"/>
-      <c r="D98" s="37" t="s">
+      <c r="C100" s="45"/>
+      <c r="D100" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="E98" s="47" t="s">
+      <c r="E100" s="47" t="s">
         <v>126</v>
       </c>
-      <c r="F98" s="47"/>
-      <c r="G98" s="47" t="s">
+      <c r="F100" s="47"/>
+      <c r="G100" s="47" t="s">
         <v>126</v>
       </c>
-      <c r="H98" s="47"/>
-      <c r="I98" s="47"/>
-      <c r="J98" s="48" t="s">
+      <c r="H100" s="47"/>
+      <c r="I100" s="47"/>
+      <c r="J100" s="48" t="s">
         <v>158</v>
       </c>
-      <c r="K98" s="47" t="s">
+      <c r="K100" s="47" t="s">
         <v>126</v>
       </c>
-      <c r="L98" s="47" t="s">
+      <c r="L100" s="47" t="s">
         <v>126</v>
       </c>
-      <c r="M98" s="47" t="s">
+      <c r="M100" s="47" t="s">
         <v>126</v>
       </c>
-      <c r="N98" s="47" t="s">
+      <c r="N100" s="47" t="s">
         <v>126</v>
       </c>
-      <c r="O98" s="47"/>
-      <c r="P98" s="47"/>
-      <c r="Q98" s="48" t="s">
+      <c r="O100" s="47"/>
+      <c r="P100" s="47"/>
+      <c r="Q100" s="48" t="s">
         <v>158</v>
       </c>
-      <c r="R98" s="49" t="s">
+      <c r="R100" s="49" t="s">
         <v>163</v>
       </c>
-      <c r="S98" s="48" t="s">
+      <c r="S100" s="48" t="s">
         <v>158</v>
       </c>
-      <c r="T98" s="47"/>
-      <c r="U98" s="47" t="s">
+      <c r="T100" s="47"/>
+      <c r="U100" s="47" t="s">
         <v>158</v>
       </c>
-      <c r="V98" s="47"/>
-      <c r="W98" s="47"/>
-      <c r="X98" s="47"/>
-      <c r="Y98" s="30"/>
+      <c r="V100" s="47"/>
+      <c r="W100" s="47"/>
+      <c r="X100" s="47"/>
+      <c r="Y100" s="30"/>
     </row>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C57" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="B82" sqref="B82"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C35" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="A53" sqref="A53:Y54"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="C48" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="D72" sqref="D72:X72"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" scale="170">
+      <pane xSplit="2" ySplit="6" topLeftCell="C31" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
+      <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -19523,27 +21390,9 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{41779DD2-B938-0C4D-877B-9108B2018222}" scale="170">
-      <pane xSplit="2" ySplit="6.0384615384615383" topLeftCell="C24" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C31" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" scale="170">
-      <pane xSplit="2" ySplit="6" topLeftCell="C48" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="D72" sqref="D72:X72"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
   </customSheetViews>
   <mergeCells count="6">
-    <mergeCell ref="Y82:Y83"/>
+    <mergeCell ref="Y84:Y85"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="K5:O5"/>
     <mergeCell ref="R5:X5"/>
@@ -19899,8 +21748,13 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
-      <selection activeCell="B17" sqref="B17"/>
+    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}">
+      <selection activeCell="A22" sqref="A22"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}">
+      <selection activeCell="G36" sqref="G36"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -19909,13 +21763,8 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}">
-      <selection activeCell="G36" sqref="G36"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}">
-      <selection activeCell="A22" sqref="A22"/>
+    <customSheetView guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}">
+      <selection activeCell="B17" sqref="B17"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>

</xml_diff>

<commit_message>
Lisää Tielupien haku roolit-exceliin
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -1,33 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarihan/Jari/Tyo/Solita/Projektit/Harja/harja/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/teemukau/code/harja/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="27200" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
     <sheet name="Roolit" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$98</definedName>
-    <definedName name="Z_1DD617EE_F308_3E45_A8EF_4713F47FA0DD_.wvu.FilterData" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$98</definedName>
-    <definedName name="Z_7A9649F2_657F_9445_B6E6_FE94C6A09957_.wvu.FilterData" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$98</definedName>
-    <definedName name="Z_F86DF6F3_8AE5_3A44_B2D2_D623E01AE54F_.wvu.FilterData" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$98</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$99</definedName>
+    <definedName name="Z_1DD617EE_F308_3E45_A8EF_4713F47FA0DD_.wvu.FilterData" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$99</definedName>
+    <definedName name="Z_7A9649F2_657F_9445_B6E6_FE94C6A09957_.wvu.FilterData" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$99</definedName>
+    <definedName name="Z_F86DF6F3_8AE5_3A44_B2D2_D623E01AE54F_.wvu.FilterData" localSheetId="0" hidden="1">Oikeudet!$A$5:$Y$99</definedName>
   </definedNames>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" yWindow="22" windowWidth="2560" windowHeight="1360" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1680" windowHeight="823" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Mikko Rönkkömäki - Personal View" guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" mergeInterval="0" personalView="1" windowWidth="2560" windowHeight="1071" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office -käyttäjä - Oma näkymä" guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="1149" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="Jarno Väyrynen - Personal View" guid="{C10F9F10-1A4D-7B47-A88E-9424D9FB3197}" mergeInterval="0" personalView="1" yWindow="9" windowWidth="1920" windowHeight="1048" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
-    <customWorkbookView name="Tatu Tarvainen - Personal View" guid="{41779DD2-B938-0C4D-877B-9108B2018222}" mergeInterval="0" personalView="1" xWindow="38" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Microsoft Office -käyttäjä - Oma näkymä" guid="{F86DF6F3-8AE5-3A44-B2D2-D623E01AE54F}" mergeInterval="0" personalView="1" windowWidth="1920" windowHeight="1149" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Mikko Rönkkömäki - Personal View" guid="{1DD617EE-F308-3E45-A8EF-4713F47FA0DD}" mergeInterval="0" personalView="1" windowWidth="2560" windowHeight="1071" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -46,7 +46,7 @@
     <author>Tatu Tarvainen</author>
   </authors>
   <commentList>
-    <comment ref="N31" authorId="0" guid="{DB5603A0-3291-7849-94B2-B86D15FBE193}" shapeId="0">
+    <comment ref="N31" authorId="0" guid="{DB5603A0-3291-7849-94B2-B86D15FBE193}">
       <text>
         <r>
           <rPr>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1511" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1534" uniqueCount="237">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -779,12 +779,18 @@
   </si>
   <si>
     <t>Vastaanottotarkastusraportti</t>
+  </si>
+  <si>
+    <t>Tieluvat</t>
+  </si>
+  <si>
+    <t>Tielupien haku</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1157,7 +1163,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -1291,6 +1297,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1311,9 +1324,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="201">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1532,7 +1542,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{23AC25BB-AA9F-4242-ACBB-939A4FE9E51A}" diskRevisions="1" revisionId="844" version="53">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{F1DB029F-312C-004C-A5D1-DBC9372C29F7}" diskRevisions="1" revisionId="869" version="54">
   <header guid="{1E352813-0B26-DB4E-84BE-460845B77133}" dateTime="2017-06-20T12:32:37" maxSheetId="3" userName="Microsoft Office -käyttäjä" r:id="rId60" minRId="448" maxRId="464">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1851,6 +1861,12 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{F1DB029F-312C-004C-A5D1-DBC9372C29F7}" dateTime="2018-03-26T11:23:02" maxSheetId="3" userName="Microsoft Office User" r:id="rId113" minRId="845" maxRId="868">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -13174,6 +13190,181 @@
   <rdn rId="0" localSheetId="1" customView="1" name="Z_7A9649F2_657F_9445_B6E6_FE94C6A09957_.wvu.FilterData" hidden="1" oldHidden="1">
     <formula>Oikeudet!$A$5:$Y$98</formula>
     <oldFormula>Oikeudet!$A$5:$Y$98</oldFormula>
+  </rdn>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog51.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="845" sId="1" ref="A84:XFD84" action="insertRow"/>
+  <rcc rId="846" sId="1">
+    <nc r="A84" t="inlineStr">
+      <is>
+        <t>Tieluvat</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="847" sId="1">
+    <nc r="B84" t="inlineStr">
+      <is>
+        <t>Tielupien haku</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="848" sId="1">
+    <nc r="D84" t="inlineStr">
+      <is>
+        <t>R*,W*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="849" sId="1" odxf="1" dxf="1">
+    <nc r="E84" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+    <odxf/>
+    <ndxf/>
+  </rcc>
+  <rcc rId="850" sId="1">
+    <nc r="F84" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="851" sId="1">
+    <nc r="G84" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="852" sId="1">
+    <nc r="H84" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="853" sId="1">
+    <nc r="I84" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="854" sId="1">
+    <nc r="J84" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="855" sId="1">
+    <nc r="K84" t="inlineStr">
+      <is>
+        <t>R*,W*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="856" sId="1">
+    <nc r="L84" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="857" sId="1">
+    <nc r="M84" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="858" sId="1">
+    <nc r="N84" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="859" sId="1">
+    <nc r="O84" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="860" sId="1">
+    <nc r="P84" t="inlineStr">
+      <is>
+        <t>R*</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="861" sId="1">
+    <nc r="Q84" t="inlineStr">
+      <is>
+        <t>R</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="862" sId="1">
+    <nc r="R84" t="inlineStr">
+      <is>
+        <t>R+,W+</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="863" sId="1">
+    <nc r="S84" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="864" sId="1">
+    <nc r="T84" t="inlineStr">
+      <is>
+        <t>R+</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="865" sId="1">
+    <nc r="U84" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="866" sId="1">
+    <nc r="V84" t="inlineStr">
+      <is>
+        <t>R+</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="867" sId="1">
+    <nc r="W84" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="868" sId="1">
+    <nc r="X84" t="inlineStr">
+      <is>
+        <t>R,W</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="delete"/>
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_7A9649F2_657F_9445_B6E6_FE94C6A09957_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Oikeudet!$A$5:$Y$99</formula>
+    <oldFormula>Oikeudet!$A$5:$Y$99</oldFormula>
   </rdn>
   <rcv guid="{7A9649F2-657F-9445-B6E6-FE94C6A09957}" action="add"/>
 </revisions>
@@ -14037,13 +14228,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y98"/>
+  <dimension ref="A1:Y99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C57" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C73" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B82" sqref="B82"/>
+      <selection pane="bottomRight" activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -14080,40 +14271,40 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="73" t="s">
+      <c r="C1" s="76" t="s">
         <v>149</v>
       </c>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
-      <c r="L1" s="74"/>
-      <c r="M1" s="74"/>
-      <c r="N1" s="74"/>
-      <c r="O1" s="74"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="75" t="s">
+      <c r="C2" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="76"/>
-      <c r="L2" s="76"/>
-      <c r="M2" s="76"/>
-      <c r="N2" s="76"/>
-      <c r="O2" s="76"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="79"/>
+      <c r="L2" s="79"/>
+      <c r="M2" s="79"/>
+      <c r="N2" s="79"/>
+      <c r="O2" s="79"/>
     </row>
     <row r="3" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
@@ -14136,34 +14327,34 @@
     <row r="5" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="30"/>
       <c r="B5" s="30"/>
-      <c r="C5" s="71" t="s">
+      <c r="C5" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="72"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="75"/>
       <c r="I5" s="30"/>
       <c r="J5" s="30"/>
-      <c r="K5" s="71" t="s">
+      <c r="K5" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="L5" s="72"/>
-      <c r="M5" s="72"/>
-      <c r="N5" s="72"/>
-      <c r="O5" s="72"/>
+      <c r="L5" s="75"/>
+      <c r="M5" s="75"/>
+      <c r="N5" s="75"/>
+      <c r="O5" s="75"/>
       <c r="P5" s="30"/>
       <c r="Q5" s="30"/>
-      <c r="R5" s="71" t="s">
+      <c r="R5" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="S5" s="72"/>
-      <c r="T5" s="72"/>
-      <c r="U5" s="72"/>
-      <c r="V5" s="72"/>
-      <c r="W5" s="72"/>
-      <c r="X5" s="72"/>
+      <c r="S5" s="75"/>
+      <c r="T5" s="75"/>
+      <c r="U5" s="75"/>
+      <c r="V5" s="75"/>
+      <c r="W5" s="75"/>
+      <c r="X5" s="75"/>
       <c r="Y5" s="31" t="s">
         <v>13</v>
       </c>
@@ -18741,7 +18932,7 @@
       <c r="A81" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="B81" s="77" t="s">
+      <c r="B81" s="71" t="s">
         <v>234</v>
       </c>
       <c r="C81" s="37"/>
@@ -18861,7 +19052,7 @@
       <c r="X82" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="Y82" s="69" t="s">
+      <c r="Y82" s="72" t="s">
         <v>216</v>
       </c>
     </row>
@@ -18936,14 +19127,14 @@
       <c r="X83" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="Y83" s="70"/>
+      <c r="Y83" s="73"/>
     </row>
-    <row r="84" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:25" s="70" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A84" s="39" t="s">
-        <v>60</v>
+        <v>235</v>
       </c>
       <c r="B84" s="39" t="s">
-        <v>60</v>
+        <v>236</v>
       </c>
       <c r="C84" s="37"/>
       <c r="D84" s="37" t="s">
@@ -19009,110 +19200,150 @@
       <c r="X84" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="Y84" s="38"/>
+      <c r="Y84" s="69"/>
     </row>
-    <row r="85" spans="1:25" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A85" s="42" t="s">
-        <v>61</v>
-      </c>
-      <c r="B85" s="42" t="s">
-        <v>62</v>
-      </c>
-      <c r="C85" s="43"/>
+    <row r="85" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A85" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="B85" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="C85" s="37"/>
       <c r=